<commit_message>
Add a possibility to expand existing building stock
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_RSD.xlsx
+++ b/SubRES_TMPL/SubRes_RSD.xlsx
@@ -8,23 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26FD81B5-419A-494C-9CCC-C7583E5F428B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B17290-87C3-41E8-9DA2-B9999F194721}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="646" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="646" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RSD" sheetId="22" r:id="rId1"/>
+    <sheet name="RSD_buildings" sheetId="23" r:id="rId2"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId2"/>
     <externalReference r:id="rId3"/>
     <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
   </externalReferences>
   <definedNames>
     <definedName name="_.DMD.">#REF!</definedName>
+    <definedName name="__123Graph_AEUMILKPN" hidden="1">#REF!</definedName>
+    <definedName name="_Regression_Y" hidden="1">#REF!</definedName>
+    <definedName name="aa" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="Cars_12">'[1]TechRep-Doc'!#REF!</definedName>
     <definedName name="ddddd">[2]AGR_Fuels!$A$2</definedName>
     <definedName name="DISCRATE">'[1]TechRep-Doc'!#REF!</definedName>
+    <definedName name="elec" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec2" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec3" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elecc" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="FID_1" localSheetId="0">[1]AGR_Fuels!$A$2</definedName>
     <definedName name="FID_1">[3]AGR_Fuels!$A$2</definedName>
     <definedName name="GROWTH">'[1]TechRep-Doc'!#REF!</definedName>
@@ -33,10 +42,12 @@
     <definedName name="LIFE">'[1]TechRep-Doc'!#REF!</definedName>
     <definedName name="NAs_CCAR">'[1]TechRep-Doc'!#REF!</definedName>
     <definedName name="SETS">'[1]TechRep-Doc'!#REF!</definedName>
+    <definedName name="table6" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="TRTGAB005">'[1]TechRep-Doc'!#REF!</definedName>
     <definedName name="TRTGAC005">'[1]TechRep-Doc'!#REF!</definedName>
     <definedName name="Trucks_15">'[1]TechRep-Doc'!#REF!</definedName>
     <definedName name="TSUB_COST">'[1]TechRep-Doc'!#REF!</definedName>
+    <definedName name="wrn.Electricity._.Questionnaire." hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="x">[1]AGR_Fuels!$A$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -55,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="70">
   <si>
     <t>~FI_T</t>
   </si>
@@ -217,6 +228,54 @@
   </si>
   <si>
     <t>Residential Other Applications - New</t>
+  </si>
+  <si>
+    <t>LIFE</t>
+  </si>
+  <si>
+    <t>000units</t>
+  </si>
+  <si>
+    <t>RSD_Apt</t>
+  </si>
+  <si>
+    <t>Residential Apartment demand</t>
+  </si>
+  <si>
+    <t>RSH_Apt,RSC_Apt,RWH_Apt,RLT_Apt,RPF_Apt</t>
+  </si>
+  <si>
+    <t>RSD_Att</t>
+  </si>
+  <si>
+    <t>RSH_Att,RSC_Att,RWH_Att,RLT_Att,RPF_Att</t>
+  </si>
+  <si>
+    <t>RSD_Det</t>
+  </si>
+  <si>
+    <t>RSH_Det,RSC_Det,RWH_Det,RLT_Det,RPF_Det</t>
+  </si>
+  <si>
+    <t>RSD_Det-NEW</t>
+  </si>
+  <si>
+    <t>RSD_Att-NEW</t>
+  </si>
+  <si>
+    <t>RSD_Apt-NEW</t>
+  </si>
+  <si>
+    <t>NCAP_COST</t>
+  </si>
+  <si>
+    <t>Dummy cost</t>
+  </si>
+  <si>
+    <t>Residential Attached demand - New</t>
+  </si>
+  <si>
+    <t>Residential Detached demand - New</t>
   </si>
 </sst>
 </file>
@@ -224,7 +283,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -440,8 +499,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -738,6 +797,59 @@
       <sheetData sheetId="48" refreshError="1"/>
       <sheetData sheetId="49" refreshError="1"/>
       <sheetData sheetId="50" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Cover"/>
+      <sheetName val="Intro"/>
+      <sheetName val="Regions"/>
+      <sheetName val="RES"/>
+      <sheetName val="SETUP"/>
+      <sheetName val="EnergyBalance"/>
+      <sheetName val="RSD_Balance"/>
+      <sheetName val="Fuel-Age_Adj"/>
+      <sheetName val="COMM"/>
+      <sheetName val="EMIS"/>
+      <sheetName val="DIST"/>
+      <sheetName val="Sector_Fuels"/>
+      <sheetName val="Heating Drivers"/>
+      <sheetName val="Non-Heat Drivers"/>
+      <sheetName val="DwellingStocks"/>
+      <sheetName val="SHWLP-Apt"/>
+      <sheetName val="SHWLP-Att"/>
+      <sheetName val="SHWLP-Det"/>
+      <sheetName val="ApartmentEnergyData"/>
+      <sheetName val="AttachedEnergyData"/>
+      <sheetName val="DettachedEnergyData"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1067,8 +1179,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B4:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1277,11 +1389,11 @@
     </row>
     <row r="11" spans="2:12" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="10" t="str">
-        <f>C22</f>
+        <f t="shared" ref="B11:C15" si="0">C22</f>
         <v>RSDRCW_N1</v>
       </c>
       <c r="C11" s="11" t="str">
-        <f>D22</f>
+        <f t="shared" si="0"/>
         <v>Residential Cloth Washing demand - New</v>
       </c>
       <c r="D11" s="11" t="s">
@@ -1308,11 +1420,11 @@
     </row>
     <row r="12" spans="2:12" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="7" t="str">
-        <f>C23</f>
+        <f t="shared" si="0"/>
         <v>RSDRCD_N1</v>
       </c>
       <c r="C12" s="8" t="str">
-        <f>D23</f>
+        <f t="shared" si="0"/>
         <v>Residential Cloth Drying demand - New</v>
       </c>
       <c r="D12" s="8" t="s">
@@ -1339,11 +1451,11 @@
     </row>
     <row r="13" spans="2:12" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="10" t="str">
-        <f>C24</f>
+        <f t="shared" si="0"/>
         <v>RSDRDW_N1</v>
       </c>
       <c r="C13" s="11" t="str">
-        <f>D24</f>
+        <f t="shared" si="0"/>
         <v>Residential Dish Washing demand - New</v>
       </c>
       <c r="D13" s="11" t="s">
@@ -1370,11 +1482,11 @@
     </row>
     <row r="14" spans="2:12" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="7" t="str">
-        <f>C25</f>
+        <f t="shared" si="0"/>
         <v>RSDROE_N1</v>
       </c>
       <c r="C14" s="8" t="str">
-        <f>D25</f>
+        <f t="shared" si="0"/>
         <v>Residential ELC Appliances - New</v>
       </c>
       <c r="D14" s="8" t="s">
@@ -1401,11 +1513,11 @@
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="str">
-        <f>C26</f>
+        <f t="shared" si="0"/>
         <v>RSDROA_N1</v>
       </c>
       <c r="C15" s="2" t="str">
-        <f>D26</f>
+        <f t="shared" si="0"/>
         <v>Residential Other Applications - New</v>
       </c>
       <c r="D15" s="2" t="s">
@@ -1644,4 +1756,222 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C2D43F6-97F6-4E25-A1BC-F561B5C1DF16}">
+  <dimension ref="C4:I21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="F4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H5" t="s">
+        <v>54</v>
+      </c>
+      <c r="I5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C7" t="str">
+        <f>D19</f>
+        <v>RSD_Apt-NEW</v>
+      </c>
+      <c r="D7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G7">
+        <v>0.01</v>
+      </c>
+      <c r="H7">
+        <v>100</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C8" t="str">
+        <f t="shared" ref="C8:C9" si="0">D20</f>
+        <v>RSD_Att-NEW</v>
+      </c>
+      <c r="D8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G8">
+        <v>0.01</v>
+      </c>
+      <c r="H8">
+        <v>100</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>RSD_Det-NEW</v>
+      </c>
+      <c r="D9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" t="s">
+        <v>62</v>
+      </c>
+      <c r="F9" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9">
+        <v>0.01</v>
+      </c>
+      <c r="H9">
+        <v>100</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" t="s">
+        <v>11</v>
+      </c>
+      <c r="I18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19" t="str">
+        <f>D7</f>
+        <v>Residential Apartment demand</v>
+      </c>
+      <c r="F19" t="s">
+        <v>55</v>
+      </c>
+      <c r="G19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" t="s">
+        <v>68</v>
+      </c>
+      <c r="F20" t="s">
+        <v>55</v>
+      </c>
+      <c r="G20" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" t="s">
+        <v>63</v>
+      </c>
+      <c r="E21" t="s">
+        <v>69</v>
+      </c>
+      <c r="F21" t="s">
+        <v>55</v>
+      </c>
+      <c r="G21" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Activate RSDOA and update RSD names in SubRES
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_RSD.xlsx
+++ b/SubRES_TMPL/SubRes_RSD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B17290-87C3-41E8-9DA2-B9999F194721}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B7C0D6-CA3F-4BCE-BB9C-D513B6059F98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="646" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="646" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RSD" sheetId="22" r:id="rId1"/>
@@ -20,7 +20,6 @@
     <externalReference r:id="rId3"/>
     <externalReference r:id="rId4"/>
     <externalReference r:id="rId5"/>
-    <externalReference r:id="rId6"/>
   </externalReferences>
   <definedNames>
     <definedName name="_.DMD.">#REF!</definedName>
@@ -66,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="81">
   <si>
     <t>~FI_T</t>
   </si>
@@ -158,57 +157,15 @@
     <t>RSDELC</t>
   </si>
   <si>
-    <t>RSDRRF</t>
-  </si>
-  <si>
     <t>DMD</t>
   </si>
   <si>
-    <t>RSDRCK</t>
-  </si>
-  <si>
     <t>RSDGASNAT</t>
   </si>
   <si>
     <t>RSDOILLPG</t>
   </si>
   <si>
-    <t>RSDRCW</t>
-  </si>
-  <si>
-    <t>RSDRCD</t>
-  </si>
-  <si>
-    <t>RSDRDW</t>
-  </si>
-  <si>
-    <t>RSDROE</t>
-  </si>
-  <si>
-    <t>RSDROA</t>
-  </si>
-  <si>
-    <t>RSDRRF_N1</t>
-  </si>
-  <si>
-    <t>RSDRCK_N1</t>
-  </si>
-  <si>
-    <t>RSDRCW_N1</t>
-  </si>
-  <si>
-    <t>RSDRCD_N1</t>
-  </si>
-  <si>
-    <t>RSDRDW_N1</t>
-  </si>
-  <si>
-    <t>RSDROE_N1</t>
-  </si>
-  <si>
-    <t>RSDROA_N1</t>
-  </si>
-  <si>
     <t>Residential Refrigeration - New</t>
   </si>
   <si>
@@ -239,43 +196,118 @@
     <t>RSD_Apt</t>
   </si>
   <si>
-    <t>Residential Apartment demand</t>
-  </si>
-  <si>
-    <t>RSH_Apt,RSC_Apt,RWH_Apt,RLT_Apt,RPF_Apt</t>
-  </si>
-  <si>
     <t>RSD_Att</t>
   </si>
   <si>
-    <t>RSH_Att,RSC_Att,RWH_Att,RLT_Att,RPF_Att</t>
-  </si>
-  <si>
     <t>RSD_Det</t>
   </si>
   <si>
-    <t>RSH_Det,RSC_Det,RWH_Det,RLT_Det,RPF_Det</t>
-  </si>
-  <si>
-    <t>RSD_Det-NEW</t>
-  </si>
-  <si>
-    <t>RSD_Att-NEW</t>
-  </si>
-  <si>
-    <t>RSD_Apt-NEW</t>
-  </si>
-  <si>
-    <t>NCAP_COST</t>
-  </si>
-  <si>
-    <t>Dummy cost</t>
-  </si>
-  <si>
-    <t>Residential Attached demand - New</t>
-  </si>
-  <si>
-    <t>Residential Detached demand - New</t>
+    <t>R-BLD_Det-NEW</t>
+  </si>
+  <si>
+    <t>R-BLD_Att-NEW</t>
+  </si>
+  <si>
+    <t>R-BLD_Apt-NEW</t>
+  </si>
+  <si>
+    <t>Residential Building Detached - New</t>
+  </si>
+  <si>
+    <t>Residential Building Apartment - New</t>
+  </si>
+  <si>
+    <t>Residential Building Attached - New</t>
+  </si>
+  <si>
+    <t>RSDSH_Apt</t>
+  </si>
+  <si>
+    <t>RSDSC_Apt</t>
+  </si>
+  <si>
+    <t>RSDWH_Apt</t>
+  </si>
+  <si>
+    <t>RSDLT_Apt</t>
+  </si>
+  <si>
+    <t>RSDPF_Apt</t>
+  </si>
+  <si>
+    <t>RSDSH_Att</t>
+  </si>
+  <si>
+    <t>RSDSC_Att</t>
+  </si>
+  <si>
+    <t>RSDWH_Att</t>
+  </si>
+  <si>
+    <t>RSDLT_Att</t>
+  </si>
+  <si>
+    <t>RSDPF_Att</t>
+  </si>
+  <si>
+    <t>RSDSH_Det</t>
+  </si>
+  <si>
+    <t>RSDSC_Det</t>
+  </si>
+  <si>
+    <t>RSDWH_Det</t>
+  </si>
+  <si>
+    <t>RSDLT_Det</t>
+  </si>
+  <si>
+    <t>RSDPF_Det</t>
+  </si>
+  <si>
+    <t>INPUT</t>
+  </si>
+  <si>
+    <t>R-RSDRF_NEW</t>
+  </si>
+  <si>
+    <t>R-RSDCK_NEW</t>
+  </si>
+  <si>
+    <t>R-RSDCW_NEW</t>
+  </si>
+  <si>
+    <t>R-RSDCD_NEW</t>
+  </si>
+  <si>
+    <t>R-RSDDW_NEW</t>
+  </si>
+  <si>
+    <t>R-RSDOE_NEW</t>
+  </si>
+  <si>
+    <t>R-RSDOA_NEW</t>
+  </si>
+  <si>
+    <t>RSDRF</t>
+  </si>
+  <si>
+    <t>RSDCK</t>
+  </si>
+  <si>
+    <t>RSDCW</t>
+  </si>
+  <si>
+    <t>RSDCD</t>
+  </si>
+  <si>
+    <t>RSDDW</t>
+  </si>
+  <si>
+    <t>RSDOE</t>
+  </si>
+  <si>
+    <t>RSDOA</t>
   </si>
 </sst>
 </file>
@@ -302,7 +334,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -327,8 +359,14 @@
         <bgColor theme="5"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor theme="6" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -472,11 +510,146 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </right>
+      <top style="thick">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -501,6 +674,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -797,59 +984,6 @@
       <sheetData sheetId="48" refreshError="1"/>
       <sheetData sheetId="49" refreshError="1"/>
       <sheetData sheetId="50" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Cover"/>
-      <sheetName val="Intro"/>
-      <sheetName val="Regions"/>
-      <sheetName val="RES"/>
-      <sheetName val="SETUP"/>
-      <sheetName val="EnergyBalance"/>
-      <sheetName val="RSD_Balance"/>
-      <sheetName val="Fuel-Age_Adj"/>
-      <sheetName val="COMM"/>
-      <sheetName val="EMIS"/>
-      <sheetName val="DIST"/>
-      <sheetName val="Sector_Fuels"/>
-      <sheetName val="Heating Drivers"/>
-      <sheetName val="Non-Heat Drivers"/>
-      <sheetName val="DwellingStocks"/>
-      <sheetName val="SHWLP-Apt"/>
-      <sheetName val="SHWLP-Att"/>
-      <sheetName val="SHWLP-Det"/>
-      <sheetName val="ApartmentEnergyData"/>
-      <sheetName val="AttachedEnergyData"/>
-      <sheetName val="DettachedEnergyData"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1179,8 +1313,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B4:L26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1282,7 +1416,7 @@
     <row r="7" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B7" s="10" t="str">
         <f>C20</f>
-        <v>RSDRRF_N1</v>
+        <v>R-RSDRF_NEW</v>
       </c>
       <c r="C7" s="11" t="str">
         <f>D20</f>
@@ -1292,7 +1426,7 @@
         <v>29</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>30</v>
+        <v>74</v>
       </c>
       <c r="F7" s="11">
         <v>0.8</v>
@@ -1313,7 +1447,7 @@
     <row r="8" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B8" s="7" t="str">
         <f>C21</f>
-        <v>RSDRCK_N1</v>
+        <v>R-RSDCK_NEW</v>
       </c>
       <c r="C8" s="8" t="str">
         <f>D21</f>
@@ -1323,7 +1457,7 @@
         <v>29</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>32</v>
+        <v>75</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="8">
@@ -1349,7 +1483,7 @@
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
@@ -1370,7 +1504,7 @@
       <c r="B10" s="7"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
@@ -1390,7 +1524,7 @@
     <row r="11" spans="2:12" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="10" t="str">
         <f t="shared" ref="B11:C15" si="0">C22</f>
-        <v>RSDRCW_N1</v>
+        <v>R-RSDCW_NEW</v>
       </c>
       <c r="C11" s="11" t="str">
         <f t="shared" si="0"/>
@@ -1400,7 +1534,7 @@
         <v>29</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
       <c r="F11" s="11">
         <v>0.7</v>
@@ -1421,7 +1555,7 @@
     <row r="12" spans="2:12" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>RSDRCD_N1</v>
+        <v>R-RSDCD_NEW</v>
       </c>
       <c r="C12" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1431,7 +1565,7 @@
         <v>29</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>36</v>
+        <v>77</v>
       </c>
       <c r="F12" s="8">
         <v>0.6</v>
@@ -1452,7 +1586,7 @@
     <row r="13" spans="2:12" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>RSDRDW_N1</v>
+        <v>R-RSDDW_NEW</v>
       </c>
       <c r="C13" s="11" t="str">
         <f t="shared" si="0"/>
@@ -1462,7 +1596,7 @@
         <v>29</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>37</v>
+        <v>78</v>
       </c>
       <c r="F13" s="11">
         <v>0.7</v>
@@ -1483,7 +1617,7 @@
     <row r="14" spans="2:12" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>RSDROE_N1</v>
+        <v>R-RSDOE_NEW</v>
       </c>
       <c r="C14" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1493,7 +1627,7 @@
         <v>29</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>38</v>
+        <v>79</v>
       </c>
       <c r="F14" s="8">
         <v>0.85</v>
@@ -1514,7 +1648,7 @@
     <row r="15" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>RSDROA_N1</v>
+        <v>R-RSDOA_NEW</v>
       </c>
       <c r="C15" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1524,7 +1658,7 @@
         <v>29</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>39</v>
+        <v>80</v>
       </c>
       <c r="F15" s="2">
         <v>0.85</v>
@@ -1575,13 +1709,13 @@
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B20" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="E20" s="17" t="s">
         <v>17</v>
@@ -1597,13 +1731,13 @@
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B21" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>41</v>
+        <v>68</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="E21" s="17" t="s">
         <v>17</v>
@@ -1619,13 +1753,13 @@
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B22" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="E22" s="17" t="s">
         <v>17</v>
@@ -1641,13 +1775,13 @@
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B23" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="E23" s="17" t="s">
         <v>17</v>
@@ -1663,13 +1797,13 @@
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B24" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="E24" s="17" t="s">
         <v>17</v>
@@ -1685,13 +1819,13 @@
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B25" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E25" s="17" t="s">
         <v>17</v>
@@ -1707,13 +1841,13 @@
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B26" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="E26" s="20" t="s">
         <v>17</v>
@@ -1760,10 +1894,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C2D43F6-97F6-4E25-A1BC-F561B5C1DF16}">
-  <dimension ref="C4:I21"/>
+  <dimension ref="C4:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1772,203 +1906,369 @@
     <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="42.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" customWidth="1"/>
+    <col min="9" max="9" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="F4" t="s">
+    <row r="4" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C5" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C6" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" s="17"/>
+      <c r="I6" s="18"/>
+    </row>
+    <row r="7" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C7" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" s="17"/>
+      <c r="I7" s="18"/>
+    </row>
+    <row r="8" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C8" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" s="20"/>
+      <c r="I8" s="21"/>
+    </row>
+    <row r="13" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="G13" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C5" t="s">
+    <row r="14" spans="3:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D14" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E14" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F14" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G14" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H14" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="I14" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="J14" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="H5" t="s">
+    </row>
+    <row r="15" spans="3:10" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="D15" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="30"/>
+    </row>
+    <row r="16" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="D16" s="31" t="str">
+        <f>D6</f>
+        <v>R-BLD_Apt-NEW</v>
+      </c>
+      <c r="E16" s="25" t="str">
+        <f>E6</f>
+        <v>Residential Building Apartment - New</v>
+      </c>
+      <c r="F16" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="G16" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="H16" s="25">
+        <v>100</v>
+      </c>
+      <c r="I16" s="25">
+        <v>1</v>
+      </c>
+      <c r="J16" s="32">
+        <v>1.4820480670008396E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D17" s="33"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D18" s="31"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="G18" s="25"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="25"/>
+      <c r="J18" s="32">
+        <v>8.2251262129918352E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D19" s="33"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="I5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C7" t="str">
-        <f>D19</f>
-        <v>RSD_Apt-NEW</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="34">
+        <v>4.9822250206190887E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D20" s="31"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="G20" s="25"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="32">
+        <v>1.0266309705907878E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D21" s="33" t="str">
+        <f>D7</f>
+        <v>R-BLD_Att-NEW</v>
+      </c>
+      <c r="E21" s="24" t="str">
+        <f>E7</f>
+        <v>Residential Building Attached - New</v>
+      </c>
+      <c r="F21" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="G21" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="H21" s="24">
+        <v>100</v>
+      </c>
+      <c r="I21" s="24">
+        <v>1</v>
+      </c>
+      <c r="J21" s="34">
+        <v>4.1539609916574856E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D22" s="31"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="E7" t="s">
+      <c r="G22" s="25"/>
+      <c r="H22" s="25"/>
+      <c r="I22" s="25"/>
+      <c r="J22" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D23" s="33"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="F7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G7">
-        <v>0.01</v>
-      </c>
-      <c r="H7">
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="34">
+        <v>1.4064457368099048E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D24" s="31"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="G24" s="25"/>
+      <c r="H24" s="25"/>
+      <c r="I24" s="25"/>
+      <c r="J24" s="32">
+        <v>1.3444460955064912E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D25" s="33"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="G25" s="24"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="24"/>
+      <c r="J25" s="34">
+        <v>2.7703485776427552E-4</v>
+      </c>
+    </row>
+    <row r="26" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D26" s="31" t="str">
+        <f>D8</f>
+        <v>R-BLD_Det-NEW</v>
+      </c>
+      <c r="E26" s="25" t="str">
+        <f>E8</f>
+        <v>Residential Building Detached - New</v>
+      </c>
+      <c r="F26" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="G26" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="H26" s="25">
         <v>100</v>
       </c>
-      <c r="I7">
+      <c r="I26" s="25">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C8" t="str">
-        <f t="shared" ref="C8:C9" si="0">D20</f>
-        <v>RSD_Att-NEW</v>
-      </c>
-      <c r="D8" t="s">
-        <v>57</v>
-      </c>
-      <c r="E8" t="s">
-        <v>60</v>
-      </c>
-      <c r="F8" t="s">
-        <v>59</v>
-      </c>
-      <c r="G8">
-        <v>0.01</v>
-      </c>
-      <c r="H8">
-        <v>100</v>
-      </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C9" t="str">
-        <f t="shared" si="0"/>
-        <v>RSD_Det-NEW</v>
-      </c>
-      <c r="D9" t="s">
-        <v>57</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="J26" s="32">
+        <v>7.5283956459279863E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D27" s="33"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="F9" t="s">
-        <v>61</v>
-      </c>
-      <c r="G9">
-        <v>0.01</v>
-      </c>
-      <c r="H9">
-        <v>100</v>
-      </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C17" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C18" t="s">
-        <v>2</v>
-      </c>
-      <c r="D18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E18" t="s">
-        <v>4</v>
-      </c>
-      <c r="F18" t="s">
-        <v>9</v>
-      </c>
-      <c r="G18" t="s">
-        <v>10</v>
-      </c>
-      <c r="H18" t="s">
-        <v>11</v>
-      </c>
-      <c r="I18" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C19" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D28" s="31"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="32">
+        <v>1.7830953440996895E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D29" s="33"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="G29" s="24"/>
+      <c r="H29" s="24"/>
+      <c r="I29" s="24"/>
+      <c r="J29" s="34">
+        <v>1.1036083669191172E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D30" s="35"/>
+      <c r="E30" s="36"/>
+      <c r="F30" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="E19" t="str">
-        <f>D7</f>
-        <v>Residential Apartment demand</v>
-      </c>
-      <c r="F19" t="s">
-        <v>55</v>
-      </c>
-      <c r="G19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C20" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20" t="s">
-        <v>64</v>
-      </c>
-      <c r="E20" t="s">
-        <v>68</v>
-      </c>
-      <c r="F20" t="s">
-        <v>55</v>
-      </c>
-      <c r="G20" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="21" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C21" t="s">
-        <v>31</v>
-      </c>
-      <c r="D21" t="s">
-        <v>63</v>
-      </c>
-      <c r="E21" t="s">
-        <v>69</v>
-      </c>
-      <c r="F21" t="s">
-        <v>55</v>
-      </c>
-      <c r="G21" t="s">
-        <v>55</v>
+      <c r="G30" s="36"/>
+      <c r="H30" s="36"/>
+      <c r="I30" s="36"/>
+      <c r="J30" s="37">
+        <v>2.2970926283112933E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Expand RSD SubRES with temporary technologies and make corrections to VT
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_RSD.xlsx
+++ b/SubRES_TMPL/SubRes_RSD.xlsx
@@ -8,18 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B7C0D6-CA3F-4BCE-BB9C-D513B6059F98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EE4BBD1-0C6D-4EAE-B19F-8EB239B1224C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="646" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="646" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RSD" sheetId="22" r:id="rId1"/>
     <sheet name="RSD_buildings" sheetId="23" r:id="rId2"/>
+    <sheet name="RSD_Boilers" sheetId="24" r:id="rId3"/>
+    <sheet name="RSD_OTH" sheetId="25" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
-    <externalReference r:id="rId4"/>
     <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
   </externalReferences>
   <definedNames>
     <definedName name="_.DMD.">#REF!</definedName>
@@ -65,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="108">
   <si>
     <t>~FI_T</t>
   </si>
@@ -308,6 +310,87 @@
   </si>
   <si>
     <t>RSDOA</t>
+  </si>
+  <si>
+    <t>START</t>
+  </si>
+  <si>
+    <t>PRE</t>
+  </si>
+  <si>
+    <t>R-SH_Apt_ELC_N1</t>
+  </si>
+  <si>
+    <t>R-SH_Att_ELC_N1</t>
+  </si>
+  <si>
+    <t>R-SH_Det_ELC_N1</t>
+  </si>
+  <si>
+    <t>Residential Space Heating Apartment Electricity to Residential New</t>
+  </si>
+  <si>
+    <t>R-WH_Apt_ELC_N1</t>
+  </si>
+  <si>
+    <t>R-WH_Att_ELC_N1</t>
+  </si>
+  <si>
+    <t>R-WH_Det_ELC_N1</t>
+  </si>
+  <si>
+    <t>Residential Water Heating Apartment Electricity to Residential New</t>
+  </si>
+  <si>
+    <t>NCAP_COST</t>
+  </si>
+  <si>
+    <t>Residential Space Heating Attached Electricity to Residential New</t>
+  </si>
+  <si>
+    <t>Residential Space Heating Detached Electricity to Residential New</t>
+  </si>
+  <si>
+    <t>Residential Water Heating Attached Electricity to Residential New</t>
+  </si>
+  <si>
+    <t>Residential Water Heating Detached Electricity to Residential New</t>
+  </si>
+  <si>
+    <t>R-LT_Apt_N1</t>
+  </si>
+  <si>
+    <t>R-PF_Apt_N1</t>
+  </si>
+  <si>
+    <t>R-LT_Att_N1</t>
+  </si>
+  <si>
+    <t>R-PF_Att_N1</t>
+  </si>
+  <si>
+    <t>R-LT_Det_N1</t>
+  </si>
+  <si>
+    <t>R-PF_Det_N1</t>
+  </si>
+  <si>
+    <t>Residential Lighting Apartment New</t>
+  </si>
+  <si>
+    <t>Residential Pumps &amp; Fans Apartment New</t>
+  </si>
+  <si>
+    <t>Residential Lighting Attached New</t>
+  </si>
+  <si>
+    <t>Residential Pumps &amp; Fans Attached New</t>
+  </si>
+  <si>
+    <t>Residential Lighting Detached New</t>
+  </si>
+  <si>
+    <t>Residential Pumps &amp; Fans Detached New</t>
   </si>
 </sst>
 </file>
@@ -366,7 +449,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -645,11 +728,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -688,6 +780,10 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1311,10 +1407,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B4:L26"/>
+  <dimension ref="B4:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1346,12 +1442,12 @@
     <col min="27" max="27" width="8.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
       <c r="E4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
         <v>3</v>
       </c>
@@ -1385,8 +1481,11 @@
       <c r="L5" s="6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="M5" s="38" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B6" s="7" t="s">
         <v>23</v>
       </c>
@@ -1412,8 +1511,9 @@
       <c r="L6" s="9" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="M6" s="9"/>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B7" s="10" t="str">
         <f>C20</f>
         <v>R-RSDRF_NEW</v>
@@ -1443,8 +1543,11 @@
       </c>
       <c r="K7" s="11"/>
       <c r="L7" s="12"/>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="M7" s="12">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B8" s="7" t="str">
         <f>C21</f>
         <v>R-RSDCK_NEW</v>
@@ -1478,8 +1581,11 @@
       <c r="L8" s="9">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="M8" s="9">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11" t="s">
@@ -1499,8 +1605,9 @@
       <c r="L9" s="12">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="2:12" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M9" s="12"/>
+    </row>
+    <row r="10" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="7"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8" t="s">
@@ -1520,8 +1627,9 @@
       <c r="L10" s="9">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="2:12" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M10" s="9"/>
+    </row>
+    <row r="11" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="10" t="str">
         <f t="shared" ref="B11:C15" si="0">C22</f>
         <v>R-RSDCW_NEW</v>
@@ -1551,8 +1659,11 @@
       </c>
       <c r="K11" s="11"/>
       <c r="L11" s="12"/>
-    </row>
-    <row r="12" spans="2:12" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M11" s="12">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="7" t="str">
         <f t="shared" si="0"/>
         <v>R-RSDCD_NEW</v>
@@ -1582,8 +1693,11 @@
       </c>
       <c r="K12" s="8"/>
       <c r="L12" s="9"/>
-    </row>
-    <row r="13" spans="2:12" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M12" s="9">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="10" t="str">
         <f t="shared" si="0"/>
         <v>R-RSDDW_NEW</v>
@@ -1613,8 +1727,11 @@
       </c>
       <c r="K13" s="11"/>
       <c r="L13" s="12"/>
-    </row>
-    <row r="14" spans="2:12" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M13" s="12">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="7" t="str">
         <f t="shared" si="0"/>
         <v>R-RSDOE_NEW</v>
@@ -1644,8 +1761,11 @@
       </c>
       <c r="K14" s="8"/>
       <c r="L14" s="9"/>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="M14" s="9">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="str">
         <f t="shared" si="0"/>
         <v>R-RSDOA_NEW</v>
@@ -1675,6 +1795,7 @@
       </c>
       <c r="K15" s="2"/>
       <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
@@ -1894,10 +2015,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C2D43F6-97F6-4E25-A1BC-F561B5C1DF16}">
-  <dimension ref="C4:J30"/>
+  <dimension ref="C4:K30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+      <selection activeCell="C4" sqref="C4:K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1910,12 +2031,12 @@
     <col min="9" max="9" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C5" s="13" t="s">
         <v>2</v>
       </c>
@@ -1938,7 +2059,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C6" s="16" t="s">
         <v>30</v>
       </c>
@@ -1957,7 +2078,7 @@
       <c r="H6" s="17"/>
       <c r="I6" s="18"/>
     </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C7" s="16" t="s">
         <v>30</v>
       </c>
@@ -1976,7 +2097,7 @@
       <c r="H7" s="17"/>
       <c r="I7" s="18"/>
     </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C8" s="19" t="s">
         <v>30</v>
       </c>
@@ -1995,12 +2116,12 @@
       <c r="H8" s="20"/>
       <c r="I8" s="21"/>
     </row>
-    <row r="13" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="3:11" x14ac:dyDescent="0.2">
       <c r="G13" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="3:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D14" s="4" t="s">
         <v>3</v>
       </c>
@@ -2022,8 +2143,11 @@
       <c r="J14" s="28" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="15" spans="3:10" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="K14" s="27" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="3:11" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="D15" s="29" t="s">
         <v>23</v>
       </c>
@@ -2039,8 +2163,9 @@
       <c r="H15" s="26"/>
       <c r="I15" s="26"/>
       <c r="J15" s="30"/>
-    </row>
-    <row r="16" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="K15" s="26"/>
+    </row>
+    <row r="16" spans="3:11" x14ac:dyDescent="0.2">
       <c r="D16" s="31" t="str">
         <f>D6</f>
         <v>R-BLD_Apt-NEW</v>
@@ -2064,8 +2189,11 @@
       <c r="J16" s="32">
         <v>1.4820480670008396E-2</v>
       </c>
-    </row>
-    <row r="17" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="K16" s="25">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="17" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D17" s="33"/>
       <c r="E17" s="24"/>
       <c r="F17" s="24" t="s">
@@ -2077,8 +2205,9 @@
       <c r="J17" s="34">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="K17" s="24"/>
+    </row>
+    <row r="18" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D18" s="31"/>
       <c r="E18" s="25"/>
       <c r="F18" s="25" t="s">
@@ -2090,8 +2219,9 @@
       <c r="J18" s="32">
         <v>8.2251262129918352E-3</v>
       </c>
-    </row>
-    <row r="19" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="K18" s="25"/>
+    </row>
+    <row r="19" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D19" s="33"/>
       <c r="E19" s="24"/>
       <c r="F19" s="24" t="s">
@@ -2103,8 +2233,9 @@
       <c r="J19" s="34">
         <v>4.9822250206190887E-3</v>
       </c>
-    </row>
-    <row r="20" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="K19" s="24"/>
+    </row>
+    <row r="20" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D20" s="31"/>
       <c r="E20" s="25"/>
       <c r="F20" s="25" t="s">
@@ -2116,8 +2247,9 @@
       <c r="J20" s="32">
         <v>1.0266309705907878E-3</v>
       </c>
-    </row>
-    <row r="21" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="K20" s="25"/>
+    </row>
+    <row r="21" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D21" s="33" t="str">
         <f>D7</f>
         <v>R-BLD_Att-NEW</v>
@@ -2141,8 +2273,11 @@
       <c r="J21" s="34">
         <v>4.1539609916574856E-2</v>
       </c>
-    </row>
-    <row r="22" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="K21" s="24">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="22" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D22" s="31"/>
       <c r="E22" s="25"/>
       <c r="F22" s="25" t="s">
@@ -2154,8 +2289,9 @@
       <c r="J22" s="32">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="K22" s="25"/>
+    </row>
+    <row r="23" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D23" s="33"/>
       <c r="E23" s="24"/>
       <c r="F23" s="24" t="s">
@@ -2167,8 +2303,9 @@
       <c r="J23" s="34">
         <v>1.4064457368099048E-2</v>
       </c>
-    </row>
-    <row r="24" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="K23" s="24"/>
+    </row>
+    <row r="24" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D24" s="31"/>
       <c r="E24" s="25"/>
       <c r="F24" s="25" t="s">
@@ -2180,8 +2317,9 @@
       <c r="J24" s="32">
         <v>1.3444460955064912E-3</v>
       </c>
-    </row>
-    <row r="25" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="K24" s="25"/>
+    </row>
+    <row r="25" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D25" s="33"/>
       <c r="E25" s="24"/>
       <c r="F25" s="24" t="s">
@@ -2193,8 +2331,9 @@
       <c r="J25" s="34">
         <v>2.7703485776427552E-4</v>
       </c>
-    </row>
-    <row r="26" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="K25" s="24"/>
+    </row>
+    <row r="26" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D26" s="31" t="str">
         <f>D8</f>
         <v>R-BLD_Det-NEW</v>
@@ -2218,8 +2357,11 @@
       <c r="J26" s="32">
         <v>7.5283956459279863E-2</v>
       </c>
-    </row>
-    <row r="27" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="K26" s="25">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="27" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D27" s="33"/>
       <c r="E27" s="24"/>
       <c r="F27" s="24" t="s">
@@ -2231,8 +2373,9 @@
       <c r="J27" s="34">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="K27" s="24"/>
+    </row>
+    <row r="28" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D28" s="31"/>
       <c r="E28" s="25"/>
       <c r="F28" s="25" t="s">
@@ -2244,8 +2387,9 @@
       <c r="J28" s="32">
         <v>1.7830953440996895E-2</v>
       </c>
-    </row>
-    <row r="29" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="K28" s="25"/>
+    </row>
+    <row r="29" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D29" s="33"/>
       <c r="E29" s="24"/>
       <c r="F29" s="24" t="s">
@@ -2257,8 +2401,9 @@
       <c r="J29" s="34">
         <v>1.1036083669191172E-2</v>
       </c>
-    </row>
-    <row r="30" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="K29" s="24"/>
+    </row>
+    <row r="30" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D30" s="35"/>
       <c r="E30" s="36"/>
       <c r="F30" s="36" t="s">
@@ -2270,6 +2415,855 @@
       <c r="J30" s="37">
         <v>2.2970926283112933E-3</v>
       </c>
+      <c r="K30" s="36"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44A2CE90-9318-48DC-AE66-3D2EBD04129C}">
+  <dimension ref="B4:L21"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B5" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B6" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" t="s">
+        <v>86</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="17"/>
+      <c r="H6" s="18"/>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B7" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" t="s">
+        <v>92</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="17"/>
+      <c r="H7" s="18"/>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B8" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" t="s">
+        <v>93</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="20"/>
+      <c r="H8" s="21"/>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B9" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D9" t="s">
+        <v>90</v>
+      </c>
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="17"/>
+      <c r="H9" s="18"/>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B10" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D10" t="s">
+        <v>94</v>
+      </c>
+      <c r="E10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" s="17"/>
+      <c r="H10" s="18"/>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B11" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="20"/>
+      <c r="H11" s="21"/>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="F13" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="H14" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="I14" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="J14" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="K14" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="L14" s="39" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="C15" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="26"/>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C16" s="31" t="str">
+        <f t="shared" ref="C16:D21" si="0">C6</f>
+        <v>R-SH_Apt_ELC_N1</v>
+      </c>
+      <c r="D16" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>Residential Space Heating Apartment Electricity to Residential New</v>
+      </c>
+      <c r="E16" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="G16" s="25">
+        <v>20</v>
+      </c>
+      <c r="H16" s="25">
+        <v>1</v>
+      </c>
+      <c r="I16" s="25">
+        <v>2020</v>
+      </c>
+      <c r="J16" s="25">
+        <v>3.0701960784313722</v>
+      </c>
+      <c r="K16" s="25">
+        <v>2.1013453171159005E-3</v>
+      </c>
+      <c r="L16" s="40">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C17" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v>R-SH_Att_ELC_N1</v>
+      </c>
+      <c r="D17" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>Residential Space Heating Attached Electricity to Residential New</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="G17" s="24">
+        <v>20</v>
+      </c>
+      <c r="H17" s="24">
+        <v>1</v>
+      </c>
+      <c r="I17" s="24">
+        <v>2020</v>
+      </c>
+      <c r="J17" s="24">
+        <v>3.0701960784313722</v>
+      </c>
+      <c r="K17" s="24">
+        <v>2.1013453171159005E-3</v>
+      </c>
+      <c r="L17" s="41">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="18" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C18" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>R-SH_Det_ELC_N1</v>
+      </c>
+      <c r="D18" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>Residential Space Heating Detached Electricity to Residential New</v>
+      </c>
+      <c r="E18" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="G18" s="25">
+        <v>20</v>
+      </c>
+      <c r="H18" s="25">
+        <v>1</v>
+      </c>
+      <c r="I18" s="25">
+        <v>2020</v>
+      </c>
+      <c r="J18" s="25">
+        <v>3.0701960784313722</v>
+      </c>
+      <c r="K18" s="25">
+        <v>2.1013453171159005E-3</v>
+      </c>
+      <c r="L18" s="40">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="19" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C19" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>R-WH_Apt_ELC_N1</v>
+      </c>
+      <c r="D19" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>Residential Water Heating Apartment Electricity to Residential New</v>
+      </c>
+      <c r="E19" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="F19" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="G19" s="25">
+        <v>20</v>
+      </c>
+      <c r="H19" s="25">
+        <v>1</v>
+      </c>
+      <c r="I19" s="25">
+        <v>2020</v>
+      </c>
+      <c r="J19" s="25">
+        <v>3.0701960784313722</v>
+      </c>
+      <c r="K19" s="25">
+        <v>2.1013453171159005E-3</v>
+      </c>
+      <c r="L19" s="40">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C20" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v>R-WH_Att_ELC_N1</v>
+      </c>
+      <c r="D20" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>Residential Water Heating Attached Electricity to Residential New</v>
+      </c>
+      <c r="E20" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="G20" s="24">
+        <v>20</v>
+      </c>
+      <c r="H20" s="24">
+        <v>1</v>
+      </c>
+      <c r="I20" s="24">
+        <v>2020</v>
+      </c>
+      <c r="J20" s="24">
+        <v>3.0701960784313722</v>
+      </c>
+      <c r="K20" s="24">
+        <v>2.1013453171159005E-3</v>
+      </c>
+      <c r="L20" s="41">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C21" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>R-WH_Det_ELC_N1</v>
+      </c>
+      <c r="D21" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>Residential Water Heating Detached Electricity to Residential New</v>
+      </c>
+      <c r="E21" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="G21" s="25">
+        <v>20</v>
+      </c>
+      <c r="H21" s="25">
+        <v>1</v>
+      </c>
+      <c r="I21" s="25">
+        <v>2020</v>
+      </c>
+      <c r="J21" s="25">
+        <v>3.0701960784313722</v>
+      </c>
+      <c r="K21" s="25">
+        <v>2.1013453171159005E-3</v>
+      </c>
+      <c r="L21" s="40">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F882C1B-5853-4411-BE2E-98858752C5D0}">
+  <dimension ref="B2:L19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B3" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B4" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" s="17"/>
+      <c r="H4" s="18"/>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B5" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" s="17"/>
+      <c r="H5" s="18"/>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B6" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D6" t="s">
+        <v>104</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="20"/>
+      <c r="H6" s="21"/>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B7" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D7" t="s">
+        <v>105</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="17"/>
+      <c r="H7" s="18"/>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B8" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D8" t="s">
+        <v>106</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="17"/>
+      <c r="H8" s="18"/>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B9" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D9" t="s">
+        <v>107</v>
+      </c>
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="20"/>
+      <c r="H9" s="21"/>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="F11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="H12" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="I12" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="J12" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="K12" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="L12" s="39" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="C13" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="26"/>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C14" s="31" t="str">
+        <f t="shared" ref="C14:D19" si="0">C4</f>
+        <v>R-LT_Apt_N1</v>
+      </c>
+      <c r="D14" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>Residential Lighting Apartment New</v>
+      </c>
+      <c r="E14" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="G14" s="25">
+        <v>10</v>
+      </c>
+      <c r="H14" s="25">
+        <v>1</v>
+      </c>
+      <c r="I14" s="25">
+        <v>2020</v>
+      </c>
+      <c r="J14" s="25">
+        <v>0.37037039770119351</v>
+      </c>
+      <c r="K14" s="25">
+        <v>4.9822250206190887E-3</v>
+      </c>
+      <c r="L14" s="40">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C15" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v>R-PF_Apt_N1</v>
+      </c>
+      <c r="D15" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>Residential Pumps &amp; Fans Apartment New</v>
+      </c>
+      <c r="E15" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="G15" s="24">
+        <v>10</v>
+      </c>
+      <c r="H15" s="24">
+        <v>1</v>
+      </c>
+      <c r="I15" s="24">
+        <v>2020</v>
+      </c>
+      <c r="J15" s="24">
+        <v>0.37037049989705056</v>
+      </c>
+      <c r="K15" s="24">
+        <v>1.0266309705907878E-3</v>
+      </c>
+      <c r="L15" s="41">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C16" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>R-LT_Att_N1</v>
+      </c>
+      <c r="D16" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>Residential Lighting Attached New</v>
+      </c>
+      <c r="E16" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="G16" s="25">
+        <v>10</v>
+      </c>
+      <c r="H16" s="25">
+        <v>1</v>
+      </c>
+      <c r="I16" s="25">
+        <v>2020</v>
+      </c>
+      <c r="J16" s="25">
+        <v>0.37037039770119351</v>
+      </c>
+      <c r="K16" s="25">
+        <v>4.9822250206190887E-3</v>
+      </c>
+      <c r="L16" s="40">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="17" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C17" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>R-PF_Att_N1</v>
+      </c>
+      <c r="D17" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>Residential Pumps &amp; Fans Attached New</v>
+      </c>
+      <c r="E17" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="G17" s="25">
+        <v>10</v>
+      </c>
+      <c r="H17" s="25">
+        <v>1</v>
+      </c>
+      <c r="I17" s="25">
+        <v>2020</v>
+      </c>
+      <c r="J17" s="25">
+        <v>0.37037049989705056</v>
+      </c>
+      <c r="K17" s="25">
+        <v>1.0266309705907878E-3</v>
+      </c>
+      <c r="L17" s="40">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="18" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C18" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v>R-LT_Det_N1</v>
+      </c>
+      <c r="D18" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>Residential Lighting Detached New</v>
+      </c>
+      <c r="E18" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="G18" s="24">
+        <v>10</v>
+      </c>
+      <c r="H18" s="24">
+        <v>1</v>
+      </c>
+      <c r="I18" s="24">
+        <v>2020</v>
+      </c>
+      <c r="J18" s="24">
+        <v>0.37037039770119351</v>
+      </c>
+      <c r="K18" s="24">
+        <v>4.9822250206190887E-3</v>
+      </c>
+      <c r="L18" s="41">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="19" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C19" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>R-PF_Det_N1</v>
+      </c>
+      <c r="D19" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>Residential Pumps &amp; Fans Detached New</v>
+      </c>
+      <c r="E19" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="F19" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="G19" s="25">
+        <v>10</v>
+      </c>
+      <c r="H19" s="25">
+        <v>1</v>
+      </c>
+      <c r="I19" s="25">
+        <v>2020</v>
+      </c>
+      <c r="J19" s="25">
+        <v>0.37037049989705056</v>
+      </c>
+      <c r="K19" s="25">
+        <v>1.0266309705907878E-3</v>
+      </c>
+      <c r="L19" s="40">
+        <v>0.1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Bring back previous tech names and do related changes
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_RSD.xlsx
+++ b/SubRES_TMPL/SubRes_RSD.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AC8C483-25D5-4F33-9526-EFFFF1D6CB6C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0DBB256-029D-4C2A-82C3-4CAAA7730958}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="4" xr2:uid="{9D5618E0-D2A2-4912-B654-2E39BDAED497}"/>
+    <workbookView xWindow="690" yWindow="2715" windowWidth="14400" windowHeight="6795" firstSheet="4" activeTab="6" xr2:uid="{9D5618E0-D2A2-4912-B654-2E39BDAED497}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="34" r:id="rId1"/>
@@ -98,78 +98,6 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="G6" authorId="0" shapeId="0" xr:uid="{E178D96D-2199-4142-A136-D18CCE9B3BCA}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Alessandro Chiodi:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Wrong calculation of these indexes!t! The index shall be estimated relatively to BY technology. </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="U6" authorId="0" shapeId="0" xr:uid="{A9205C3D-A502-4275-86B1-F52A4D2678E1}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Alessandro Chiodi:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Wrong unit! The chosen capacity unit is 'kunit', not kW!</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="Y6" authorId="0" shapeId="0" xr:uid="{5300CA7A-0ADE-4AC0-96EE-0CDBAA0A3AEB}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Alessandro Chiodi:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Wrong unit! The chosen capacity unit is 'kunit', not kW!</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="AF7" authorId="0" shapeId="0" xr:uid="{374DB055-F5C1-43ED-915B-ECEEEDC762B6}">
       <text>
         <r>
@@ -801,54 +729,6 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="L6" authorId="0" shapeId="0" xr:uid="{C72F7DCB-450D-4644-9E13-D78EAD7F6744}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Alessandro Chiodi:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Wrong unit! The chosen capacity unit is 'kunit', not kW!</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="P6" authorId="0" shapeId="0" xr:uid="{AFD45750-5F08-4529-8BDC-469C169AEBB5}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Alessandro Chiodi:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Wrong unit! The chosen capacity unit is 'kunit', not kW!</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="L7" authorId="0" shapeId="0" xr:uid="{26227E42-266E-4D7E-9CCC-4136610DED2C}">
       <text>
         <r>
@@ -883,30 +763,6 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="H6" authorId="0" shapeId="0" xr:uid="{78EAD3C8-7AFC-4116-9BB3-83D0685AE9BF}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-These efficiencies are completely different (lower) than the ones assumed for the BY (1). Are you assuming here higher efficiency?</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="Q7" authorId="0" shapeId="0" xr:uid="{144293F5-CA78-47DF-9990-9E4B53D88CB1}">
       <text>
         <r>
@@ -1234,7 +1090,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2830" uniqueCount="819">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2830" uniqueCount="815">
   <si>
     <t>Document type:</t>
   </si>
@@ -3297,6 +3153,18 @@
     <t>CEFF~RSDSH_Apt~2050</t>
   </si>
   <si>
+    <t>CEFF~RSDSC_Apt</t>
+  </si>
+  <si>
+    <t>CEFF~RSDSC_Apt~2030</t>
+  </si>
+  <si>
+    <t>CEFF~RSDSC_Apt~2040</t>
+  </si>
+  <si>
+    <t>CEFF~RSDSC_Apt~2050</t>
+  </si>
+  <si>
     <t>CEFF~RSDWH_Apt</t>
   </si>
   <si>
@@ -3321,6 +3189,18 @@
     <t>CEFF~RSDSH_Att~2050</t>
   </si>
   <si>
+    <t>CEFF~RSDSC_Att</t>
+  </si>
+  <si>
+    <t>CEFF~RSDSC_Att~2030</t>
+  </si>
+  <si>
+    <t>CEFF~RSDSC_Att~2040</t>
+  </si>
+  <si>
+    <t>CEFF~RSDSC_Att~2050</t>
+  </si>
+  <si>
     <t>CEFF~RSDWH_Att</t>
   </si>
   <si>
@@ -3345,6 +3225,18 @@
     <t>CEFF~RSDSH_Det~2050</t>
   </si>
   <si>
+    <t>CEFF~RSDSC_Det</t>
+  </si>
+  <si>
+    <t>CEFF~RSDSC_Det~2030</t>
+  </si>
+  <si>
+    <t>CEFF~RSDSC_Det~2040</t>
+  </si>
+  <si>
+    <t>CEFF~RSDSC_Det~2050</t>
+  </si>
+  <si>
     <t>CEFF~RSDWH_Det</t>
   </si>
   <si>
@@ -3480,6 +3372,9 @@
     <t>SpaceCooling</t>
   </si>
   <si>
+    <t>*R-H_Apt_HVO_N1</t>
+  </si>
+  <si>
     <t>Residential  Hydrotreated vegetable oil - New 1 SH</t>
   </si>
   <si>
@@ -3576,6 +3471,9 @@
     <t>RSDBDL</t>
   </si>
   <si>
+    <t>RSDELC,RSDSOL</t>
+  </si>
+  <si>
     <t>RSDELC,RSDGAS</t>
   </si>
   <si>
@@ -3633,85 +3531,31 @@
     <t>Share-I~UP~RSDGAS</t>
   </si>
   <si>
-    <t>*R-SH_Apt_HVO_N1</t>
-  </si>
-  <si>
-    <t>RSDSOL,RSDELC</t>
-  </si>
-  <si>
-    <t>RSDGAS,RSDELC</t>
-  </si>
-  <si>
-    <t>RSDAC_Apt</t>
-  </si>
-  <si>
-    <t>RSDAC_Det</t>
-  </si>
-  <si>
-    <t>RSDAC_Att</t>
-  </si>
-  <si>
-    <t>CEFF~RSDAC_Apt</t>
-  </si>
-  <si>
-    <t>CEFF~RSDAC_Apt~2030</t>
-  </si>
-  <si>
-    <t>CEFF~RSDAC_Apt~2040</t>
-  </si>
-  <si>
-    <t>CEFF~RSDAC_Apt~2050</t>
-  </si>
-  <si>
-    <t>CEFF~RSDAC_Att</t>
-  </si>
-  <si>
-    <t>CEFF~RSDAC_Att~2030</t>
-  </si>
-  <si>
-    <t>CEFF~RSDAC_Att~2040</t>
-  </si>
-  <si>
-    <t>CEFF~RSDAC_Att~2050</t>
-  </si>
-  <si>
-    <t>CEFF~RSDAC_Det</t>
-  </si>
-  <si>
-    <t>CEFF~RSDAC_Det~2030</t>
-  </si>
-  <si>
-    <t>CEFF~RSDAC_Det~2040</t>
-  </si>
-  <si>
-    <t>CEFF~RSDAC_Det~2050</t>
-  </si>
-  <si>
-    <t>R-RF_N1</t>
-  </si>
-  <si>
-    <t>R-CK_N1</t>
-  </si>
-  <si>
-    <t>R-CD_N1</t>
-  </si>
-  <si>
-    <t>R-DW_N1</t>
-  </si>
-  <si>
-    <t>R-OE_N1</t>
-  </si>
-  <si>
-    <t>R-OA_N1</t>
-  </si>
-  <si>
-    <t>R-CW_N1</t>
-  </si>
-  <si>
-    <t>kunit to PJ</t>
-  </si>
-  <si>
-    <t>kunits to PJ</t>
+    <t>kUnit to PJ</t>
+  </si>
+  <si>
+    <t>PJa to PJ</t>
+  </si>
+  <si>
+    <t>R-RSDRF_N1</t>
+  </si>
+  <si>
+    <t>R-RSDCK_N1</t>
+  </si>
+  <si>
+    <t>R-RSDCW_N1</t>
+  </si>
+  <si>
+    <t>R-RSDCD_N1</t>
+  </si>
+  <si>
+    <t>R-RSDDW_N1</t>
+  </si>
+  <si>
+    <t>R-RSDOE_N1</t>
+  </si>
+  <si>
+    <t>R-RSDOA_N1</t>
   </si>
 </sst>
 </file>
@@ -3729,7 +3573,7 @@
     <numFmt numFmtId="170" formatCode="0.00000"/>
     <numFmt numFmtId="171" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="56" x14ac:knownFonts="1">
+  <fonts count="54" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -4085,19 +3929,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="32">
@@ -5087,7 +4918,7 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="39" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="397">
+  <cellXfs count="393">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -5734,10 +5565,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="16" fillId="21" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -7419,14 +7246,14 @@
       <c r="F16" s="217"/>
     </row>
     <row r="17" spans="1:14" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="371" t="s">
+      <c r="A17" s="367" t="s">
         <v>474</v>
       </c>
-      <c r="B17" s="371"/>
-      <c r="C17" s="371"/>
-      <c r="D17" s="371"/>
-      <c r="E17" s="371"/>
-      <c r="F17" s="371"/>
+      <c r="B17" s="367"/>
+      <c r="C17" s="367"/>
+      <c r="D17" s="367"/>
+      <c r="E17" s="367"/>
+      <c r="F17" s="367"/>
       <c r="G17" s="219"/>
       <c r="H17" s="219"/>
       <c r="I17" s="220"/>
@@ -7464,13 +7291,13 @@
       <c r="A20" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="372" t="s">
+      <c r="B20" s="368" t="s">
         <v>476</v>
       </c>
-      <c r="C20" s="372"/>
-      <c r="D20" s="372"/>
-      <c r="E20" s="372"/>
-      <c r="F20" s="372"/>
+      <c r="C20" s="368"/>
+      <c r="D20" s="368"/>
+      <c r="E20" s="368"/>
+      <c r="F20" s="368"/>
       <c r="G20" s="224"/>
       <c r="H20" s="224"/>
       <c r="I20" s="225"/>
@@ -7484,13 +7311,13 @@
       <c r="A21" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B21" s="373" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" s="373"/>
-      <c r="D21" s="373"/>
-      <c r="E21" s="373"/>
-      <c r="F21" s="373"/>
+      <c r="B21" s="369" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="369"/>
+      <c r="D21" s="369"/>
+      <c r="E21" s="369"/>
+      <c r="F21" s="369"/>
       <c r="G21" s="224"/>
       <c r="H21" s="224"/>
       <c r="I21" s="225"/>
@@ -7504,13 +7331,13 @@
       <c r="A22" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="373" t="s">
+      <c r="B22" s="369" t="s">
         <v>59</v>
       </c>
-      <c r="C22" s="373"/>
-      <c r="D22" s="373"/>
-      <c r="E22" s="373"/>
-      <c r="F22" s="373"/>
+      <c r="C22" s="369"/>
+      <c r="D22" s="369"/>
+      <c r="E22" s="369"/>
+      <c r="F22" s="369"/>
     </row>
     <row r="23" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
@@ -7539,22 +7366,22 @@
       <c r="H24" s="3"/>
     </row>
     <row r="25" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="374"/>
-      <c r="B25" s="374"/>
-      <c r="C25" s="374"/>
-      <c r="D25" s="374"/>
-      <c r="E25" s="374"/>
-      <c r="F25" s="374"/>
+      <c r="A25" s="370"/>
+      <c r="B25" s="370"/>
+      <c r="C25" s="370"/>
+      <c r="D25" s="370"/>
+      <c r="E25" s="370"/>
+      <c r="F25" s="370"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
     </row>
     <row r="26" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="370"/>
-      <c r="B26" s="370"/>
-      <c r="C26" s="370"/>
-      <c r="D26" s="370"/>
-      <c r="E26" s="370"/>
-      <c r="F26" s="370"/>
+      <c r="A26" s="366"/>
+      <c r="B26" s="366"/>
+      <c r="C26" s="366"/>
+      <c r="D26" s="366"/>
+      <c r="E26" s="366"/>
+      <c r="F26" s="366"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="217"/>
@@ -7741,16 +7568,16 @@
   <sheetData>
     <row r="1" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:20" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="375" t="s">
+      <c r="B2" s="371" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="376"/>
-      <c r="D2" s="376"/>
-      <c r="E2" s="377"/>
-      <c r="G2" s="375" t="s">
+      <c r="C2" s="372"/>
+      <c r="D2" s="372"/>
+      <c r="E2" s="373"/>
+      <c r="G2" s="371" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="377"/>
+      <c r="H2" s="373"/>
       <c r="I2" s="228"/>
       <c r="J2" s="228"/>
       <c r="K2" s="229"/>
@@ -8092,16 +7919,16 @@
     </row>
     <row r="19" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="2:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="378" t="s">
+      <c r="B20" s="374" t="s">
         <v>81</v>
       </c>
-      <c r="C20" s="379"/>
-      <c r="D20" s="379"/>
-      <c r="E20" s="380"/>
-      <c r="G20" s="375" t="s">
+      <c r="C20" s="375"/>
+      <c r="D20" s="375"/>
+      <c r="E20" s="376"/>
+      <c r="G20" s="371" t="s">
         <v>14</v>
       </c>
-      <c r="H20" s="377"/>
+      <c r="H20" s="373"/>
     </row>
     <row r="21" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="256" t="s">
@@ -8345,16 +8172,16 @@
     </row>
     <row r="37" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="38" spans="2:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="375" t="s">
+      <c r="B38" s="371" t="s">
         <v>89</v>
       </c>
-      <c r="C38" s="376"/>
-      <c r="D38" s="376"/>
-      <c r="E38" s="377"/>
-      <c r="G38" s="381" t="s">
+      <c r="C38" s="372"/>
+      <c r="D38" s="372"/>
+      <c r="E38" s="373"/>
+      <c r="G38" s="377" t="s">
         <v>83</v>
       </c>
-      <c r="H38" s="382"/>
+      <c r="H38" s="378"/>
     </row>
     <row r="39" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B39" s="277" t="s">
@@ -8508,7 +8335,7 @@
         <v>44</v>
       </c>
       <c r="H3" s="64" t="s">
-        <v>704</v>
+        <v>716</v>
       </c>
       <c r="I3" s="64" t="s">
         <v>342</v>
@@ -8523,7 +8350,7 @@
         <v>92</v>
       </c>
       <c r="M3" s="64" t="s">
-        <v>703</v>
+        <v>715</v>
       </c>
       <c r="N3" s="64" t="s">
         <v>332</v>
@@ -8531,13 +8358,13 @@
       <c r="Q3" s="5" t="s">
         <v>424</v>
       </c>
-      <c r="W3" s="383" t="s">
-        <v>723</v>
-      </c>
-      <c r="X3" s="383"/>
-      <c r="Y3" s="383"/>
-      <c r="Z3" s="383"/>
-      <c r="AA3" s="383"/>
+      <c r="W3" s="379" t="s">
+        <v>735</v>
+      </c>
+      <c r="X3" s="379"/>
+      <c r="Y3" s="379"/>
+      <c r="Z3" s="379"/>
+      <c r="AA3" s="379"/>
     </row>
     <row r="4" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C4" s="63" t="s">
@@ -8555,12 +8382,12 @@
       <c r="G4" s="178" t="s">
         <v>339</v>
       </c>
-      <c r="H4" s="387" t="s">
+      <c r="H4" s="383" t="s">
         <v>340</v>
       </c>
-      <c r="I4" s="388"/>
-      <c r="J4" s="388"/>
-      <c r="K4" s="389"/>
+      <c r="I4" s="384"/>
+      <c r="J4" s="384"/>
+      <c r="K4" s="385"/>
       <c r="L4" s="107"/>
       <c r="M4" s="107"/>
       <c r="N4" s="107"/>
@@ -8568,19 +8395,19 @@
         <v>423</v>
       </c>
       <c r="W4" s="309" t="s">
-        <v>724</v>
+        <v>736</v>
       </c>
       <c r="X4" s="310" t="s">
-        <v>725</v>
+        <v>737</v>
       </c>
       <c r="Y4" s="310" t="s">
-        <v>726</v>
+        <v>738</v>
       </c>
       <c r="Z4" s="310" t="s">
-        <v>727</v>
+        <v>739</v>
       </c>
       <c r="AA4" s="311" t="s">
-        <v>728</v>
+        <v>740</v>
       </c>
     </row>
     <row r="5" spans="3:27" ht="25.5" x14ac:dyDescent="0.2">
@@ -8593,17 +8420,17 @@
       <c r="G5" s="84" t="s">
         <v>313</v>
       </c>
-      <c r="H5" s="390" t="s">
-        <v>701</v>
-      </c>
-      <c r="I5" s="391"/>
-      <c r="J5" s="391"/>
-      <c r="K5" s="392"/>
+      <c r="H5" s="386" t="s">
+        <v>713</v>
+      </c>
+      <c r="I5" s="387"/>
+      <c r="J5" s="387"/>
+      <c r="K5" s="388"/>
       <c r="L5" s="108" t="s">
         <v>472</v>
       </c>
       <c r="M5" s="108" t="s">
-        <v>702</v>
+        <v>714</v>
       </c>
       <c r="N5" s="108" t="s">
         <v>349</v>
@@ -8612,7 +8439,7 @@
         <v>422</v>
       </c>
       <c r="W5" s="312" t="s">
-        <v>708</v>
+        <v>720</v>
       </c>
       <c r="X5" s="313">
         <v>9418.8988568067343</v>
@@ -8668,7 +8495,7 @@
         <v>2020</v>
       </c>
       <c r="W6" s="315" t="s">
-        <v>709</v>
+        <v>721</v>
       </c>
       <c r="X6" s="316">
         <v>7459.2913438514906</v>
@@ -8702,7 +8529,7 @@
       </c>
       <c r="N7" s="104"/>
       <c r="W7" s="318" t="s">
-        <v>710</v>
+        <v>722</v>
       </c>
       <c r="X7" s="319">
         <v>14041.847426430093</v>
@@ -8736,7 +8563,7 @@
       </c>
       <c r="N8" s="105"/>
       <c r="W8" s="315" t="s">
-        <v>711</v>
+        <v>723</v>
       </c>
       <c r="X8" s="316">
         <v>19924.480375055824</v>
@@ -8770,7 +8597,7 @@
       </c>
       <c r="N9" s="104"/>
       <c r="W9" s="318" t="s">
-        <v>712</v>
+        <v>724</v>
       </c>
       <c r="X9" s="319">
         <v>58904.8034364337</v>
@@ -8804,7 +8631,7 @@
       </c>
       <c r="N10" s="143"/>
       <c r="W10" s="315" t="s">
-        <v>713</v>
+        <v>725</v>
       </c>
       <c r="X10" s="316">
         <v>43739.341649106158</v>
@@ -8829,19 +8656,19 @@
       <c r="G11" s="84" t="s">
         <v>313</v>
       </c>
-      <c r="H11" s="384" t="s">
-        <v>701</v>
-      </c>
-      <c r="I11" s="385"/>
-      <c r="J11" s="385"/>
-      <c r="K11" s="386"/>
+      <c r="H11" s="380" t="s">
+        <v>713</v>
+      </c>
+      <c r="I11" s="381"/>
+      <c r="J11" s="381"/>
+      <c r="K11" s="382"/>
       <c r="L11" s="202"/>
       <c r="M11" s="202"/>
       <c r="N11" s="108" t="s">
         <v>349</v>
       </c>
       <c r="W11" s="318" t="s">
-        <v>714</v>
+        <v>726</v>
       </c>
       <c r="X11" s="319">
         <v>25767.876472761334</v>
@@ -8897,7 +8724,7 @@
         <v>2020</v>
       </c>
       <c r="W12" s="315" t="s">
-        <v>715</v>
+        <v>727</v>
       </c>
       <c r="X12" s="316">
         <v>12331.173226884033</v>
@@ -8931,7 +8758,7 @@
       </c>
       <c r="N13" s="104"/>
       <c r="W13" s="321" t="s">
-        <v>716</v>
+        <v>728</v>
       </c>
       <c r="X13" s="322">
         <v>15211.172212670604</v>
@@ -8965,7 +8792,7 @@
       </c>
       <c r="N14" s="105"/>
       <c r="W14" s="323" t="s">
-        <v>729</v>
+        <v>741</v>
       </c>
       <c r="X14" s="324">
         <v>206798.88499999998</v>
@@ -8999,7 +8826,7 @@
       </c>
       <c r="N15" s="104"/>
       <c r="W15" s="327" t="s">
-        <v>730</v>
+        <v>742</v>
       </c>
       <c r="X15" s="326">
         <v>0.74286208971025169</v>
@@ -9040,12 +8867,12 @@
       <c r="G17" s="84" t="s">
         <v>313</v>
       </c>
-      <c r="H17" s="384" t="s">
-        <v>701</v>
-      </c>
-      <c r="I17" s="385"/>
-      <c r="J17" s="385"/>
-      <c r="K17" s="386"/>
+      <c r="H17" s="380" t="s">
+        <v>713</v>
+      </c>
+      <c r="I17" s="381"/>
+      <c r="J17" s="381"/>
+      <c r="K17" s="382"/>
       <c r="L17" s="202"/>
       <c r="M17" s="202"/>
       <c r="N17" s="108" t="s">
@@ -9131,49 +8958,49 @@
       </c>
       <c r="N20" s="105"/>
       <c r="W20" s="5" t="s">
-        <v>718</v>
+        <v>730</v>
       </c>
       <c r="X20" s="5" t="s">
-        <v>718</v>
+        <v>730</v>
       </c>
       <c r="Y20" s="5" t="s">
-        <v>718</v>
+        <v>730</v>
       </c>
       <c r="Z20" s="5" t="s">
-        <v>718</v>
+        <v>730</v>
       </c>
       <c r="AA20" s="5" t="s">
-        <v>718</v>
+        <v>730</v>
       </c>
       <c r="AB20" s="5" t="s">
-        <v>718</v>
+        <v>730</v>
       </c>
       <c r="AC20" s="5" t="s">
-        <v>718</v>
+        <v>730</v>
       </c>
       <c r="AD20" s="5" t="s">
-        <v>718</v>
+        <v>730</v>
       </c>
       <c r="AE20" s="5" t="s">
-        <v>718</v>
+        <v>730</v>
       </c>
       <c r="AF20" s="5" t="s">
-        <v>718</v>
+        <v>730</v>
       </c>
       <c r="AH20" s="329" t="s">
-        <v>731</v>
+        <v>743</v>
       </c>
       <c r="AI20" s="330" t="s">
-        <v>738</v>
+        <v>750</v>
       </c>
       <c r="AJ20" s="330" t="s">
-        <v>739</v>
+        <v>751</v>
       </c>
       <c r="AK20" s="5" t="s">
-        <v>734</v>
+        <v>746</v>
       </c>
       <c r="AL20" s="328" t="s">
-        <v>740</v>
+        <v>752</v>
       </c>
     </row>
     <row r="21" spans="2:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -9195,40 +9022,40 @@
       </c>
       <c r="N21" s="104"/>
       <c r="V21" s="5" t="s">
-        <v>717</v>
+        <v>729</v>
       </c>
       <c r="W21" s="5" t="s">
-        <v>719</v>
+        <v>731</v>
       </c>
       <c r="X21" s="5" t="s">
-        <v>720</v>
+        <v>732</v>
       </c>
       <c r="Y21" s="5" t="s">
-        <v>721</v>
+        <v>733</v>
       </c>
       <c r="Z21" s="5" t="s">
-        <v>732</v>
+        <v>744</v>
       </c>
       <c r="AA21" s="5" t="s">
-        <v>733</v>
+        <v>745</v>
       </c>
       <c r="AB21" s="194" t="s">
-        <v>722</v>
+        <v>734</v>
       </c>
       <c r="AC21" s="194" t="s">
-        <v>734</v>
+        <v>746</v>
       </c>
       <c r="AD21" s="5" t="s">
-        <v>735</v>
+        <v>747</v>
       </c>
       <c r="AE21" s="5" t="s">
-        <v>736</v>
+        <v>748</v>
       </c>
       <c r="AF21" s="5" t="s">
-        <v>729</v>
+        <v>741</v>
       </c>
       <c r="AH21" s="328" t="s">
-        <v>737</v>
+        <v>749</v>
       </c>
     </row>
     <row r="22" spans="2:38" ht="15" x14ac:dyDescent="0.2">
@@ -9250,7 +9077,7 @@
       </c>
       <c r="N22" s="143"/>
       <c r="V22" s="5" t="s">
-        <v>708</v>
+        <v>720</v>
       </c>
       <c r="W22" s="185">
         <v>6419</v>
@@ -9307,7 +9134,7 @@
     </row>
     <row r="23" spans="2:38" ht="15" x14ac:dyDescent="0.2">
       <c r="V23" s="5" t="s">
-        <v>709</v>
+        <v>721</v>
       </c>
       <c r="W23" s="185">
         <v>3209</v>
@@ -9361,7 +9188,7 @@
     </row>
     <row r="24" spans="2:38" ht="15" x14ac:dyDescent="0.2">
       <c r="V24" s="5" t="s">
-        <v>710</v>
+        <v>722</v>
       </c>
       <c r="W24" s="185">
         <v>8665</v>
@@ -9425,7 +9252,7 @@
       <c r="H25" s="57"/>
       <c r="I25" s="57"/>
       <c r="V25" s="5" t="s">
-        <v>711</v>
+        <v>723</v>
       </c>
       <c r="W25" s="185">
         <v>13570</v>
@@ -9500,7 +9327,7 @@
         <v>312</v>
       </c>
       <c r="V26" s="5" t="s">
-        <v>712</v>
+        <v>724</v>
       </c>
       <c r="W26" s="185">
         <v>45566</v>
@@ -9575,7 +9402,7 @@
         <v>319</v>
       </c>
       <c r="V27" s="5" t="s">
-        <v>713</v>
+        <v>725</v>
       </c>
       <c r="W27" s="185">
         <v>30979</v>
@@ -9629,7 +9456,7 @@
     </row>
     <row r="28" spans="2:38" ht="15" x14ac:dyDescent="0.2">
       <c r="B28" s="173" t="s">
-        <v>776</v>
+        <v>790</v>
       </c>
       <c r="C28" s="174" t="s">
         <v>397</v>
@@ -9646,7 +9473,7 @@
       <c r="G28" s="174"/>
       <c r="H28" s="175"/>
       <c r="V28" s="5" t="s">
-        <v>714</v>
+        <v>726</v>
       </c>
       <c r="W28" s="185">
         <v>15595</v>
@@ -9700,7 +9527,7 @@
     </row>
     <row r="29" spans="2:38" ht="15" x14ac:dyDescent="0.2">
       <c r="B29" s="173" t="s">
-        <v>776</v>
+        <v>790</v>
       </c>
       <c r="C29" s="174" t="s">
         <v>398</v>
@@ -9717,7 +9544,7 @@
       <c r="G29" s="174"/>
       <c r="H29" s="175"/>
       <c r="V29" s="5" t="s">
-        <v>715</v>
+        <v>727</v>
       </c>
       <c r="W29" s="185">
         <v>5191</v>
@@ -9771,7 +9598,7 @@
     </row>
     <row r="30" spans="2:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B30" s="173" t="s">
-        <v>776</v>
+        <v>790</v>
       </c>
       <c r="C30" s="176" t="s">
         <v>399</v>
@@ -9788,7 +9615,7 @@
       <c r="G30" s="176"/>
       <c r="H30" s="177"/>
       <c r="V30" s="5" t="s">
-        <v>716</v>
+        <v>728</v>
       </c>
       <c r="W30" s="185">
         <v>5603</v>
@@ -9888,49 +9715,49 @@
       <c r="H35" s="8"/>
       <c r="I35" s="8"/>
       <c r="W35" s="5" t="s">
-        <v>726</v>
+        <v>738</v>
       </c>
       <c r="X35" s="5" t="s">
-        <v>726</v>
+        <v>738</v>
       </c>
       <c r="Y35" s="5" t="s">
-        <v>726</v>
+        <v>738</v>
       </c>
       <c r="Z35" s="5" t="s">
-        <v>726</v>
+        <v>738</v>
       </c>
       <c r="AA35" s="5" t="s">
-        <v>726</v>
+        <v>738</v>
       </c>
       <c r="AB35" s="5" t="s">
-        <v>726</v>
+        <v>738</v>
       </c>
       <c r="AC35" s="5" t="s">
-        <v>726</v>
+        <v>738</v>
       </c>
       <c r="AD35" s="5" t="s">
-        <v>726</v>
+        <v>738</v>
       </c>
       <c r="AE35" s="5" t="s">
-        <v>726</v>
+        <v>738</v>
       </c>
       <c r="AF35" s="5" t="s">
-        <v>726</v>
+        <v>738</v>
       </c>
       <c r="AH35" s="329" t="s">
-        <v>731</v>
+        <v>743</v>
       </c>
       <c r="AI35" s="330" t="s">
-        <v>738</v>
+        <v>750</v>
       </c>
       <c r="AJ35" s="330" t="s">
-        <v>739</v>
+        <v>751</v>
       </c>
       <c r="AK35" s="5" t="s">
-        <v>734</v>
+        <v>746</v>
       </c>
       <c r="AL35" s="328" t="s">
-        <v>740</v>
+        <v>752</v>
       </c>
     </row>
     <row r="36" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -9943,40 +9770,40 @@
       <c r="H36" s="8"/>
       <c r="I36" s="8"/>
       <c r="V36" s="5" t="s">
-        <v>717</v>
+        <v>729</v>
       </c>
       <c r="W36" s="5" t="s">
-        <v>719</v>
+        <v>731</v>
       </c>
       <c r="X36" s="5" t="s">
-        <v>720</v>
+        <v>732</v>
       </c>
       <c r="Y36" s="5" t="s">
-        <v>721</v>
+        <v>733</v>
       </c>
       <c r="Z36" s="5" t="s">
-        <v>732</v>
+        <v>744</v>
       </c>
       <c r="AA36" s="5" t="s">
-        <v>733</v>
+        <v>745</v>
       </c>
       <c r="AB36" s="194" t="s">
-        <v>722</v>
+        <v>734</v>
       </c>
       <c r="AC36" s="194" t="s">
-        <v>734</v>
+        <v>746</v>
       </c>
       <c r="AD36" s="5" t="s">
-        <v>735</v>
+        <v>747</v>
       </c>
       <c r="AE36" s="5" t="s">
-        <v>736</v>
+        <v>748</v>
       </c>
       <c r="AF36" s="5" t="s">
-        <v>729</v>
+        <v>741</v>
       </c>
       <c r="AH36" s="328" t="s">
-        <v>737</v>
+        <v>749</v>
       </c>
     </row>
     <row r="37" spans="1:38" ht="15" x14ac:dyDescent="0.2">
@@ -9989,7 +9816,7 @@
       <c r="H37" s="8"/>
       <c r="I37" s="8"/>
       <c r="V37" s="5" t="s">
-        <v>708</v>
+        <v>720</v>
       </c>
       <c r="W37" s="185">
         <v>30917</v>
@@ -10051,7 +9878,7 @@
       <c r="H38" s="8"/>
       <c r="I38" s="8"/>
       <c r="V38" s="5" t="s">
-        <v>709</v>
+        <v>721</v>
       </c>
       <c r="W38" s="185">
         <v>3722</v>
@@ -10113,7 +9940,7 @@
       <c r="H39" s="8"/>
       <c r="I39" s="8"/>
       <c r="V39" s="5" t="s">
-        <v>710</v>
+        <v>722</v>
       </c>
       <c r="W39" s="185">
         <v>7882</v>
@@ -10175,7 +10002,7 @@
       <c r="H40" s="8"/>
       <c r="I40" s="8"/>
       <c r="V40" s="5" t="s">
-        <v>711</v>
+        <v>723</v>
       </c>
       <c r="W40" s="185">
         <v>27081</v>
@@ -10238,7 +10065,7 @@
       <c r="H41" s="8"/>
       <c r="I41" s="8"/>
       <c r="V41" s="5" t="s">
-        <v>712</v>
+        <v>724</v>
       </c>
       <c r="W41" s="185">
         <v>161926</v>
@@ -10301,7 +10128,7 @@
       <c r="H42" s="8"/>
       <c r="I42" s="8"/>
       <c r="V42" s="5" t="s">
-        <v>713</v>
+        <v>725</v>
       </c>
       <c r="W42" s="185">
         <v>95372</v>
@@ -10364,7 +10191,7 @@
       <c r="H43" s="8"/>
       <c r="I43" s="8"/>
       <c r="V43" s="5" t="s">
-        <v>714</v>
+        <v>726</v>
       </c>
       <c r="W43" s="185">
         <v>46130</v>
@@ -10427,7 +10254,7 @@
       <c r="H44" s="8"/>
       <c r="I44" s="8"/>
       <c r="V44" s="5" t="s">
-        <v>715</v>
+        <v>727</v>
       </c>
       <c r="W44" s="185">
         <v>20720</v>
@@ -10493,7 +10320,7 @@
       <c r="L45" s="8"/>
       <c r="M45" s="8"/>
       <c r="V45" s="5" t="s">
-        <v>716</v>
+        <v>728</v>
       </c>
       <c r="W45" s="185">
         <v>21208</v>
@@ -10617,49 +10444,49 @@
       <c r="H49" s="8"/>
       <c r="I49" s="8"/>
       <c r="W49" s="5" t="s">
-        <v>727</v>
+        <v>739</v>
       </c>
       <c r="X49" s="5" t="s">
-        <v>727</v>
+        <v>739</v>
       </c>
       <c r="Y49" s="5" t="s">
-        <v>727</v>
+        <v>739</v>
       </c>
       <c r="Z49" s="5" t="s">
-        <v>727</v>
+        <v>739</v>
       </c>
       <c r="AA49" s="5" t="s">
-        <v>727</v>
+        <v>739</v>
       </c>
       <c r="AB49" s="5" t="s">
-        <v>727</v>
+        <v>739</v>
       </c>
       <c r="AC49" s="5" t="s">
-        <v>727</v>
+        <v>739</v>
       </c>
       <c r="AD49" s="5" t="s">
-        <v>727</v>
+        <v>739</v>
       </c>
       <c r="AE49" s="5" t="s">
-        <v>727</v>
+        <v>739</v>
       </c>
       <c r="AF49" s="5" t="s">
-        <v>727</v>
+        <v>739</v>
       </c>
       <c r="AH49" s="329" t="s">
-        <v>731</v>
+        <v>743</v>
       </c>
       <c r="AI49" s="330" t="s">
-        <v>738</v>
+        <v>750</v>
       </c>
       <c r="AJ49" s="330" t="s">
-        <v>739</v>
+        <v>751</v>
       </c>
       <c r="AK49" s="5" t="s">
-        <v>734</v>
+        <v>746</v>
       </c>
       <c r="AL49" s="328" t="s">
-        <v>740</v>
+        <v>752</v>
       </c>
     </row>
     <row r="50" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -10673,40 +10500,40 @@
       <c r="H50" s="8"/>
       <c r="I50" s="8"/>
       <c r="V50" s="5" t="s">
-        <v>717</v>
+        <v>729</v>
       </c>
       <c r="W50" s="5" t="s">
-        <v>719</v>
+        <v>731</v>
       </c>
       <c r="X50" s="5" t="s">
-        <v>720</v>
+        <v>732</v>
       </c>
       <c r="Y50" s="5" t="s">
-        <v>721</v>
+        <v>733</v>
       </c>
       <c r="Z50" s="5" t="s">
-        <v>732</v>
+        <v>744</v>
       </c>
       <c r="AA50" s="5" t="s">
-        <v>733</v>
+        <v>745</v>
       </c>
       <c r="AB50" s="194" t="s">
-        <v>722</v>
+        <v>734</v>
       </c>
       <c r="AC50" s="194" t="s">
-        <v>734</v>
+        <v>746</v>
       </c>
       <c r="AD50" s="5" t="s">
-        <v>735</v>
+        <v>747</v>
       </c>
       <c r="AE50" s="5" t="s">
-        <v>736</v>
+        <v>748</v>
       </c>
       <c r="AF50" s="5" t="s">
-        <v>729</v>
+        <v>741</v>
       </c>
       <c r="AH50" s="328" t="s">
-        <v>737</v>
+        <v>749</v>
       </c>
     </row>
     <row r="51" spans="1:38" ht="15" x14ac:dyDescent="0.2">
@@ -10720,7 +10547,7 @@
       <c r="H51" s="8"/>
       <c r="I51" s="8"/>
       <c r="V51" s="5" t="s">
-        <v>708</v>
+        <v>720</v>
       </c>
       <c r="W51" s="185">
         <v>9878</v>
@@ -10783,7 +10610,7 @@
       <c r="H52" s="8"/>
       <c r="I52" s="8"/>
       <c r="V52" s="5" t="s">
-        <v>709</v>
+        <v>721</v>
       </c>
       <c r="W52" s="185">
         <v>3037</v>
@@ -10846,7 +10673,7 @@
       <c r="H53" s="8"/>
       <c r="I53" s="8"/>
       <c r="V53" s="5" t="s">
-        <v>710</v>
+        <v>722</v>
       </c>
       <c r="W53" s="185">
         <v>7052</v>
@@ -10909,7 +10736,7 @@
       <c r="H54" s="8"/>
       <c r="I54" s="8"/>
       <c r="V54" s="5" t="s">
-        <v>711</v>
+        <v>723</v>
       </c>
       <c r="W54" s="185">
         <v>20170</v>
@@ -10972,7 +10799,7 @@
       <c r="H55" s="8"/>
       <c r="I55" s="8"/>
       <c r="V55" s="5" t="s">
-        <v>712</v>
+        <v>724</v>
       </c>
       <c r="W55" s="185">
         <v>97809</v>
@@ -11035,7 +10862,7 @@
       <c r="H56" s="8"/>
       <c r="I56" s="8"/>
       <c r="V56" s="5" t="s">
-        <v>713</v>
+        <v>725</v>
       </c>
       <c r="W56" s="185">
         <v>61656</v>
@@ -11098,7 +10925,7 @@
       <c r="H57" s="8"/>
       <c r="I57" s="8"/>
       <c r="V57" s="5" t="s">
-        <v>714</v>
+        <v>726</v>
       </c>
       <c r="W57" s="185">
         <v>27666</v>
@@ -11161,7 +10988,7 @@
       <c r="H58" s="8"/>
       <c r="I58" s="8"/>
       <c r="V58" s="5" t="s">
-        <v>715</v>
+        <v>727</v>
       </c>
       <c r="W58" s="185">
         <v>13787</v>
@@ -11224,7 +11051,7 @@
       <c r="H59" s="8"/>
       <c r="I59" s="8"/>
       <c r="V59" s="5" t="s">
-        <v>716</v>
+        <v>728</v>
       </c>
       <c r="W59" s="185">
         <v>24436</v>
@@ -11559,7 +11386,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C3" s="229" t="s">
-        <v>700</v>
+        <v>712</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="15" x14ac:dyDescent="0.2">
@@ -16371,8 +16198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{104F8057-C735-4662-BAA6-EEDCF7B57273}">
   <dimension ref="A2:AO170"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView topLeftCell="W1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AD1" sqref="AD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -16439,28 +16266,28 @@
         <v>679</v>
       </c>
       <c r="K3" s="64" t="s">
-        <v>798</v>
+        <v>680</v>
       </c>
       <c r="L3" s="64" t="s">
-        <v>799</v>
+        <v>681</v>
       </c>
       <c r="M3" s="64" t="s">
-        <v>800</v>
+        <v>682</v>
       </c>
       <c r="N3" s="64" t="s">
-        <v>801</v>
+        <v>683</v>
       </c>
       <c r="O3" s="64" t="s">
-        <v>680</v>
+        <v>684</v>
       </c>
       <c r="P3" s="64" t="s">
-        <v>681</v>
+        <v>685</v>
       </c>
       <c r="Q3" s="64" t="s">
-        <v>682</v>
+        <v>686</v>
       </c>
       <c r="R3" s="64" t="s">
-        <v>683</v>
+        <v>687</v>
       </c>
       <c r="S3" s="65" t="s">
         <v>44</v>
@@ -16469,7 +16296,7 @@
         <v>330</v>
       </c>
       <c r="U3" s="64" t="s">
-        <v>704</v>
+        <v>716</v>
       </c>
       <c r="V3" s="64" t="s">
         <v>342</v>
@@ -16487,22 +16314,22 @@
         <v>93</v>
       </c>
       <c r="AA3" s="64" t="s">
-        <v>789</v>
+        <v>803</v>
       </c>
       <c r="AB3" s="64" t="s">
-        <v>790</v>
+        <v>804</v>
       </c>
       <c r="AC3" s="64" t="s">
-        <v>791</v>
+        <v>805</v>
       </c>
       <c r="AD3" s="64" t="s">
-        <v>707</v>
+        <v>719</v>
       </c>
       <c r="AE3" s="64" t="s">
         <v>331</v>
       </c>
       <c r="AF3" s="64" t="s">
-        <v>775</v>
+        <v>789</v>
       </c>
       <c r="AG3" s="64" t="s">
         <v>332</v>
@@ -16510,7 +16337,7 @@
     </row>
     <row r="4" spans="3:41" ht="38.25" x14ac:dyDescent="0.2">
       <c r="C4" s="63" t="s">
-        <v>786</v>
+        <v>800</v>
       </c>
       <c r="D4" s="63" t="s">
         <v>53</v>
@@ -16521,34 +16348,34 @@
       <c r="F4" s="63" t="s">
         <v>335</v>
       </c>
-      <c r="G4" s="393" t="s">
-        <v>763</v>
-      </c>
-      <c r="H4" s="394"/>
-      <c r="I4" s="394"/>
-      <c r="J4" s="395"/>
-      <c r="K4" s="393" t="s">
+      <c r="G4" s="389" t="s">
+        <v>776</v>
+      </c>
+      <c r="H4" s="390"/>
+      <c r="I4" s="390"/>
+      <c r="J4" s="391"/>
+      <c r="K4" s="389" t="s">
         <v>337</v>
       </c>
-      <c r="L4" s="394"/>
-      <c r="M4" s="394"/>
-      <c r="N4" s="395"/>
-      <c r="O4" s="393" t="s">
+      <c r="L4" s="390"/>
+      <c r="M4" s="390"/>
+      <c r="N4" s="391"/>
+      <c r="O4" s="389" t="s">
         <v>338</v>
       </c>
-      <c r="P4" s="394"/>
-      <c r="Q4" s="394"/>
-      <c r="R4" s="395"/>
-      <c r="S4" s="393" t="s">
+      <c r="P4" s="390"/>
+      <c r="Q4" s="390"/>
+      <c r="R4" s="391"/>
+      <c r="S4" s="389" t="s">
         <v>339</v>
       </c>
-      <c r="T4" s="395"/>
-      <c r="U4" s="387" t="s">
+      <c r="T4" s="391"/>
+      <c r="U4" s="383" t="s">
         <v>340</v>
       </c>
-      <c r="V4" s="388"/>
-      <c r="W4" s="388"/>
-      <c r="X4" s="389"/>
+      <c r="V4" s="384"/>
+      <c r="W4" s="384"/>
+      <c r="X4" s="385"/>
       <c r="Y4" s="107"/>
       <c r="Z4" s="107"/>
       <c r="AA4" s="115" t="s">
@@ -16561,7 +16388,7 @@
         <v>661</v>
       </c>
       <c r="AD4" s="118" t="s">
-        <v>706</v>
+        <v>718</v>
       </c>
       <c r="AE4" s="107" t="s">
         <v>127</v>
@@ -16582,7 +16409,7 @@
     </row>
     <row r="5" spans="3:41" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C5" s="61" t="s">
-        <v>785</v>
+        <v>799</v>
       </c>
       <c r="D5" s="61"/>
       <c r="E5" s="61"/>
@@ -16638,39 +16465,39 @@
     </row>
     <row r="6" spans="3:41" ht="33.75" x14ac:dyDescent="0.2">
       <c r="C6" s="84" t="s">
-        <v>777</v>
+        <v>791</v>
       </c>
       <c r="D6" s="85"/>
       <c r="E6" s="85"/>
       <c r="F6" s="86"/>
-      <c r="G6" s="390" t="s">
+      <c r="G6" s="386" t="s">
         <v>56</v>
       </c>
-      <c r="H6" s="391"/>
-      <c r="I6" s="391"/>
-      <c r="J6" s="392"/>
-      <c r="K6" s="391" t="s">
+      <c r="H6" s="387"/>
+      <c r="I6" s="387"/>
+      <c r="J6" s="388"/>
+      <c r="K6" s="387" t="s">
         <v>56</v>
       </c>
-      <c r="L6" s="391"/>
-      <c r="M6" s="391"/>
-      <c r="N6" s="392"/>
-      <c r="O6" s="390" t="s">
+      <c r="L6" s="387"/>
+      <c r="M6" s="387"/>
+      <c r="N6" s="388"/>
+      <c r="O6" s="386" t="s">
         <v>56</v>
       </c>
-      <c r="P6" s="391"/>
-      <c r="Q6" s="391"/>
-      <c r="R6" s="392"/>
-      <c r="S6" s="390" t="s">
+      <c r="P6" s="387"/>
+      <c r="Q6" s="387"/>
+      <c r="R6" s="388"/>
+      <c r="S6" s="386" t="s">
         <v>313</v>
       </c>
-      <c r="T6" s="392"/>
-      <c r="U6" s="390" t="s">
+      <c r="T6" s="388"/>
+      <c r="U6" s="386" t="s">
         <v>346</v>
       </c>
-      <c r="V6" s="391"/>
-      <c r="W6" s="391"/>
-      <c r="X6" s="392"/>
+      <c r="V6" s="387"/>
+      <c r="W6" s="387"/>
+      <c r="X6" s="388"/>
       <c r="Y6" s="108" t="s">
         <v>347</v>
       </c>
@@ -16688,7 +16515,7 @@
       </c>
       <c r="AD6" s="108"/>
       <c r="AE6" s="117" t="s">
-        <v>817</v>
+        <v>806</v>
       </c>
       <c r="AF6" s="108" t="s">
         <v>56</v>
@@ -16727,7 +16554,7 @@
         <v>351</v>
       </c>
       <c r="E7" s="137" t="s">
-        <v>764</v>
+        <v>777</v>
       </c>
       <c r="F7" s="103" t="s">
         <v>403</v>
@@ -16814,10 +16641,10 @@
         <v>352</v>
       </c>
       <c r="E8" s="71" t="s">
-        <v>764</v>
+        <v>777</v>
       </c>
       <c r="F8" s="104" t="s">
-        <v>756</v>
+        <v>769</v>
       </c>
       <c r="G8" s="339">
         <v>1</v>
@@ -16911,10 +16738,10 @@
         <v>353</v>
       </c>
       <c r="E9" s="77" t="s">
-        <v>766</v>
+        <v>779</v>
       </c>
       <c r="F9" s="105" t="s">
-        <v>756</v>
+        <v>769</v>
       </c>
       <c r="G9" s="336">
         <v>1</v>
@@ -17012,10 +16839,10 @@
         <v>357</v>
       </c>
       <c r="E10" s="71" t="s">
-        <v>767</v>
+        <v>780</v>
       </c>
       <c r="F10" s="104" t="s">
-        <v>756</v>
+        <v>769</v>
       </c>
       <c r="G10" s="339">
         <v>1</v>
@@ -17111,7 +16938,7 @@
         <v>350</v>
       </c>
       <c r="E11" s="77" t="s">
-        <v>769</v>
+        <v>782</v>
       </c>
       <c r="F11" s="105" t="s">
         <v>403</v>
@@ -17196,10 +17023,10 @@
         <v>354</v>
       </c>
       <c r="E12" s="71" t="s">
+        <v>782</v>
+      </c>
+      <c r="F12" s="104" t="s">
         <v>769</v>
-      </c>
-      <c r="F12" s="104" t="s">
-        <v>756</v>
       </c>
       <c r="G12" s="339">
         <v>1</v>
@@ -17293,10 +17120,10 @@
         <v>355</v>
       </c>
       <c r="E13" s="77" t="s">
-        <v>770</v>
+        <v>783</v>
       </c>
       <c r="F13" s="105" t="s">
-        <v>756</v>
+        <v>769</v>
       </c>
       <c r="G13" s="336">
         <v>1</v>
@@ -17394,10 +17221,10 @@
         <v>356</v>
       </c>
       <c r="E14" s="71" t="s">
-        <v>771</v>
+        <v>784</v>
       </c>
       <c r="F14" s="104" t="s">
-        <v>756</v>
+        <v>769</v>
       </c>
       <c r="G14" s="339">
         <v>1</v>
@@ -17495,7 +17322,7 @@
         <v>358</v>
       </c>
       <c r="E15" s="77" t="s">
-        <v>765</v>
+        <v>778</v>
       </c>
       <c r="F15" s="105" t="s">
         <v>403</v>
@@ -17580,10 +17407,10 @@
         <v>359</v>
       </c>
       <c r="E16" s="71" t="s">
-        <v>765</v>
+        <v>778</v>
       </c>
       <c r="F16" s="104" t="s">
-        <v>756</v>
+        <v>769</v>
       </c>
       <c r="G16" s="339">
         <v>1</v>
@@ -17677,7 +17504,7 @@
         <v>360</v>
       </c>
       <c r="E17" s="77" t="s">
-        <v>768</v>
+        <v>781</v>
       </c>
       <c r="F17" s="105" t="s">
         <v>403</v>
@@ -17762,10 +17589,10 @@
         <v>361</v>
       </c>
       <c r="E18" s="71" t="s">
-        <v>768</v>
+        <v>781</v>
       </c>
       <c r="F18" s="104" t="s">
-        <v>756</v>
+        <v>769</v>
       </c>
       <c r="G18" s="339">
         <v>1</v>
@@ -17852,13 +17679,13 @@
     </row>
     <row r="19" spans="3:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C19" s="335" t="s">
-        <v>792</v>
+        <v>753</v>
       </c>
       <c r="D19" s="350" t="s">
-        <v>741</v>
+        <v>754</v>
       </c>
       <c r="E19" s="170" t="s">
-        <v>772</v>
+        <v>785</v>
       </c>
       <c r="F19" s="143"/>
       <c r="G19" s="345">
@@ -17942,7 +17769,7 @@
     </row>
     <row r="20" spans="3:41" ht="15" x14ac:dyDescent="0.25">
       <c r="C20" s="80" t="s">
-        <v>778</v>
+        <v>792</v>
       </c>
       <c r="D20" s="80"/>
       <c r="E20" s="81"/>
@@ -18062,7 +17889,7 @@
       <c r="AI21" s="154"/>
       <c r="AJ21" s="153" t="str">
         <f t="shared" si="12"/>
-        <v>R-SC_Apt_ELC_HPN1</v>
+        <v>R-HC_Apt_ELC_HPN1</v>
       </c>
       <c r="AK21" s="153" t="str">
         <f t="shared" si="12"/>
@@ -18081,7 +17908,7 @@
     </row>
     <row r="22" spans="3:41" ht="15" x14ac:dyDescent="0.25">
       <c r="C22" s="80" t="s">
-        <v>779</v>
+        <v>793</v>
       </c>
       <c r="D22" s="80"/>
       <c r="E22" s="81"/>
@@ -18220,8 +18047,8 @@
     </row>
     <row r="24" spans="3:41" ht="15" x14ac:dyDescent="0.25">
       <c r="C24" s="69" t="str">
-        <f>"R-SC_Apt"&amp;"_"&amp;RIGHT(E24,3)&amp;"_HPN1"</f>
-        <v>R-SC_Apt_ELC_HPN1</v>
+        <f>"R-HC_Apt"&amp;"_"&amp;RIGHT(E24,3)&amp;"_HPN1"</f>
+        <v>R-HC_Apt_ELC_HPN1</v>
       </c>
       <c r="D24" s="70" t="s">
         <v>365</v>
@@ -18230,7 +18057,7 @@
         <v>441</v>
       </c>
       <c r="F24" s="104" t="s">
-        <v>757</v>
+        <v>770</v>
       </c>
       <c r="G24" s="339">
         <v>1</v>
@@ -18294,7 +18121,7 @@
       <c r="AI24" s="304"/>
       <c r="AJ24" s="153" t="str">
         <f t="shared" si="12"/>
-        <v>R-SW_Apt_ELC_HPN2</v>
+        <v>R-SW_Apt_SOL_HPN2</v>
       </c>
       <c r="AK24" s="153" t="str">
         <f t="shared" si="12"/>
@@ -18408,7 +18235,7 @@
         <v>441</v>
       </c>
       <c r="F26" s="104" t="s">
-        <v>756</v>
+        <v>769</v>
       </c>
       <c r="G26" s="339">
         <v>1</v>
@@ -18496,16 +18323,16 @@
     <row r="27" spans="3:41" ht="15" x14ac:dyDescent="0.25">
       <c r="C27" s="87" t="str">
         <f>"R-SW_Apt"&amp;"_"&amp;RIGHT(E27,3)&amp;"_HPN2"</f>
-        <v>R-SW_Apt_ELC_HPN2</v>
+        <v>R-SW_Apt_SOL_HPN2</v>
       </c>
       <c r="D27" s="76" t="s">
         <v>368</v>
       </c>
       <c r="E27" s="77" t="s">
-        <v>793</v>
+        <v>786</v>
       </c>
       <c r="F27" s="105" t="s">
-        <v>756</v>
+        <v>769</v>
       </c>
       <c r="G27" s="336">
         <v>1</v>
@@ -18691,7 +18518,7 @@
         <v>441</v>
       </c>
       <c r="F29" s="143" t="s">
-        <v>757</v>
+        <v>770</v>
       </c>
       <c r="G29" s="345">
         <v>1</v>
@@ -18755,7 +18582,7 @@
       <c r="AI29" s="306"/>
       <c r="AJ29" s="159" t="str">
         <f>C34</f>
-        <v>R-SW_Apt_ELC_HHPN1</v>
+        <v>R-SW_Apt_GAS_HHPN1</v>
       </c>
       <c r="AK29" s="159" t="str">
         <f>D34</f>
@@ -18774,7 +18601,7 @@
     </row>
     <row r="30" spans="3:41" ht="15" x14ac:dyDescent="0.25">
       <c r="C30" s="80" t="s">
-        <v>780</v>
+        <v>794</v>
       </c>
       <c r="D30" s="80"/>
       <c r="E30" s="81"/>
@@ -18835,10 +18662,10 @@
         <v>372</v>
       </c>
       <c r="E31" s="137" t="s">
+        <v>782</v>
+      </c>
+      <c r="F31" s="137" t="s">
         <v>769</v>
-      </c>
-      <c r="F31" s="137" t="s">
-        <v>756</v>
       </c>
       <c r="G31" s="342">
         <v>1</v>
@@ -18906,7 +18733,7 @@
       <c r="AI31" s="163"/>
       <c r="AJ31" s="156" t="str">
         <f>C37</f>
-        <v>*R-SW_Apt_HET_N2</v>
+        <v>R-SW_Apt_HET_N2</v>
       </c>
       <c r="AK31" s="156" t="str">
         <f>D37</f>
@@ -18932,10 +18759,10 @@
         <v>373</v>
       </c>
       <c r="E32" s="74" t="s">
+        <v>782</v>
+      </c>
+      <c r="F32" s="74" t="s">
         <v>769</v>
-      </c>
-      <c r="F32" s="74" t="s">
-        <v>756</v>
       </c>
       <c r="G32" s="355">
         <v>1</v>
@@ -19022,7 +18849,7 @@
     </row>
     <row r="33" spans="3:41" ht="15" x14ac:dyDescent="0.25">
       <c r="C33" s="80" t="s">
-        <v>781</v>
+        <v>795</v>
       </c>
       <c r="D33" s="80"/>
       <c r="E33" s="81"/>
@@ -19077,16 +18904,16 @@
     <row r="34" spans="3:41" ht="15" x14ac:dyDescent="0.25">
       <c r="C34" s="144" t="str">
         <f>"R-SW_Apt"&amp;"_"&amp;RIGHT(E34,3)&amp;"_HHPN1"</f>
-        <v>R-SW_Apt_ELC_HHPN1</v>
+        <v>R-SW_Apt_GAS_HHPN1</v>
       </c>
       <c r="D34" s="128" t="s">
         <v>395</v>
       </c>
       <c r="E34" s="172" t="s">
-        <v>794</v>
+        <v>787</v>
       </c>
       <c r="F34" s="146" t="s">
-        <v>756</v>
+        <v>769</v>
       </c>
       <c r="G34" s="355">
         <v>1</v>
@@ -19178,7 +19005,7 @@
     </row>
     <row r="35" spans="3:41" ht="15" x14ac:dyDescent="0.25">
       <c r="C35" s="80" t="s">
-        <v>782</v>
+        <v>796</v>
       </c>
       <c r="D35" s="80"/>
       <c r="E35" s="81"/>
@@ -19239,10 +19066,10 @@
         <v>375</v>
       </c>
       <c r="E36" s="137" t="s">
-        <v>755</v>
+        <v>768</v>
       </c>
       <c r="F36" s="68" t="s">
-        <v>756</v>
+        <v>769</v>
       </c>
       <c r="G36" s="342">
         <v>1</v>
@@ -19325,17 +19152,17 @@
     </row>
     <row r="37" spans="3:41" ht="15" x14ac:dyDescent="0.25">
       <c r="C37" s="354" t="str">
-        <f>"*R-SW_Apt"&amp;"_"&amp;RIGHT(E37,3)&amp;"_N2"</f>
-        <v>*R-SW_Apt_HET_N2</v>
+        <f>"R-SW_Apt"&amp;"_"&amp;RIGHT(E37,3)&amp;"_N2"</f>
+        <v>R-SW_Apt_HET_N2</v>
       </c>
       <c r="D37" s="73" t="s">
         <v>376</v>
       </c>
       <c r="E37" s="74" t="s">
-        <v>755</v>
+        <v>768</v>
       </c>
       <c r="F37" s="75" t="s">
-        <v>756</v>
+        <v>769</v>
       </c>
       <c r="G37" s="355">
         <v>1</v>
@@ -19399,7 +19226,7 @@
       <c r="AI37" s="4"/>
       <c r="AJ37" s="153" t="str">
         <f>C45</f>
-        <v>R-AC_Apt_ELC_N1</v>
+        <v>R-SC_Apt_ELC_N1</v>
       </c>
       <c r="AK37" s="153" t="str">
         <f>D45</f>
@@ -19418,7 +19245,7 @@
     </row>
     <row r="38" spans="3:41" x14ac:dyDescent="0.2">
       <c r="C38" s="80" t="s">
-        <v>783</v>
+        <v>797</v>
       </c>
       <c r="D38" s="80"/>
       <c r="E38" s="81"/>
@@ -19526,7 +19353,7 @@
         <v>379</v>
       </c>
       <c r="E40" s="71" t="s">
-        <v>774</v>
+        <v>788</v>
       </c>
       <c r="F40" s="70" t="s">
         <v>405</v>
@@ -19594,7 +19421,7 @@
         <v>381</v>
       </c>
       <c r="E41" s="77" t="s">
-        <v>769</v>
+        <v>782</v>
       </c>
       <c r="F41" s="76" t="s">
         <v>405</v>
@@ -19660,7 +19487,7 @@
         <v>380</v>
       </c>
       <c r="E42" s="71" t="s">
-        <v>768</v>
+        <v>781</v>
       </c>
       <c r="F42" s="70" t="s">
         <v>405</v>
@@ -19726,7 +19553,7 @@
         <v>382</v>
       </c>
       <c r="E43" s="170" t="s">
-        <v>765</v>
+        <v>778</v>
       </c>
       <c r="F43" s="138" t="s">
         <v>405</v>
@@ -19785,7 +19612,7 @@
     </row>
     <row r="44" spans="3:41" x14ac:dyDescent="0.2">
       <c r="C44" s="80" t="s">
-        <v>784</v>
+        <v>798</v>
       </c>
       <c r="D44" s="80"/>
       <c r="E44" s="81"/>
@@ -19820,8 +19647,8 @@
     </row>
     <row r="45" spans="3:41" x14ac:dyDescent="0.2">
       <c r="C45" s="76" t="str">
-        <f>"R-AC_Apt"&amp;"_"&amp;RIGHT(E45,3)&amp;"_N1"</f>
-        <v>R-AC_Apt_ELC_N1</v>
+        <f>"R-SC_Apt"&amp;"_"&amp;RIGHT(E45,3)&amp;"_N1"</f>
+        <v>R-SC_Apt_ELC_N1</v>
       </c>
       <c r="D45" s="145" t="s">
         <v>383</v>
@@ -19830,7 +19657,7 @@
         <v>441</v>
       </c>
       <c r="F45" s="169" t="s">
-        <v>795</v>
+        <v>404</v>
       </c>
       <c r="G45" s="164"/>
       <c r="H45" s="165"/>
@@ -19903,40 +19730,40 @@
         <v>42</v>
       </c>
       <c r="G50" s="64" t="s">
-        <v>684</v>
+        <v>688</v>
       </c>
       <c r="H50" s="64" t="s">
-        <v>685</v>
+        <v>689</v>
       </c>
       <c r="I50" s="64" t="s">
-        <v>686</v>
+        <v>690</v>
       </c>
       <c r="J50" s="64" t="s">
-        <v>687</v>
+        <v>691</v>
       </c>
       <c r="K50" s="64" t="s">
-        <v>802</v>
+        <v>692</v>
       </c>
       <c r="L50" s="64" t="s">
-        <v>803</v>
+        <v>693</v>
       </c>
       <c r="M50" s="64" t="s">
-        <v>804</v>
+        <v>694</v>
       </c>
       <c r="N50" s="64" t="s">
-        <v>805</v>
+        <v>695</v>
       </c>
       <c r="O50" s="64" t="s">
-        <v>688</v>
+        <v>696</v>
       </c>
       <c r="P50" s="64" t="s">
-        <v>689</v>
+        <v>697</v>
       </c>
       <c r="Q50" s="64" t="s">
-        <v>690</v>
+        <v>698</v>
       </c>
       <c r="R50" s="64" t="s">
-        <v>691</v>
+        <v>699</v>
       </c>
       <c r="S50" s="65" t="s">
         <v>44</v>
@@ -19945,7 +19772,7 @@
         <v>330</v>
       </c>
       <c r="U50" s="64" t="s">
-        <v>704</v>
+        <v>716</v>
       </c>
       <c r="V50" s="64" t="s">
         <v>342</v>
@@ -19963,22 +19790,22 @@
         <v>93</v>
       </c>
       <c r="AA50" s="64" t="s">
-        <v>789</v>
+        <v>803</v>
       </c>
       <c r="AB50" s="64" t="s">
-        <v>790</v>
+        <v>804</v>
       </c>
       <c r="AC50" s="64" t="s">
-        <v>791</v>
+        <v>805</v>
       </c>
       <c r="AD50" s="64" t="s">
-        <v>707</v>
+        <v>719</v>
       </c>
       <c r="AE50" s="64" t="s">
         <v>331</v>
       </c>
       <c r="AF50" s="64" t="s">
-        <v>775</v>
+        <v>789</v>
       </c>
       <c r="AG50" s="64" t="s">
         <v>332</v>
@@ -20006,34 +19833,34 @@
       <c r="F51" s="63" t="s">
         <v>335</v>
       </c>
-      <c r="G51" s="393" t="s">
+      <c r="G51" s="389" t="s">
         <v>336</v>
       </c>
-      <c r="H51" s="394"/>
-      <c r="I51" s="394"/>
-      <c r="J51" s="395"/>
-      <c r="K51" s="393" t="s">
+      <c r="H51" s="390"/>
+      <c r="I51" s="390"/>
+      <c r="J51" s="391"/>
+      <c r="K51" s="389" t="s">
         <v>337</v>
       </c>
-      <c r="L51" s="394"/>
-      <c r="M51" s="394"/>
-      <c r="N51" s="395"/>
-      <c r="O51" s="393" t="s">
+      <c r="L51" s="390"/>
+      <c r="M51" s="390"/>
+      <c r="N51" s="391"/>
+      <c r="O51" s="389" t="s">
         <v>338</v>
       </c>
-      <c r="P51" s="394"/>
-      <c r="Q51" s="394"/>
-      <c r="R51" s="395"/>
-      <c r="S51" s="393" t="s">
+      <c r="P51" s="390"/>
+      <c r="Q51" s="390"/>
+      <c r="R51" s="391"/>
+      <c r="S51" s="389" t="s">
         <v>339</v>
       </c>
-      <c r="T51" s="395"/>
-      <c r="U51" s="387" t="s">
+      <c r="T51" s="391"/>
+      <c r="U51" s="383" t="s">
         <v>340</v>
       </c>
-      <c r="V51" s="388"/>
-      <c r="W51" s="388"/>
-      <c r="X51" s="389"/>
+      <c r="V51" s="384"/>
+      <c r="W51" s="384"/>
+      <c r="X51" s="385"/>
       <c r="Y51" s="107"/>
       <c r="Z51" s="107"/>
       <c r="AA51" s="115" t="s">
@@ -20046,7 +19873,7 @@
         <v>661</v>
       </c>
       <c r="AD51" s="118" t="s">
-        <v>706</v>
+        <v>718</v>
       </c>
       <c r="AE51" s="107" t="s">
         <v>127</v>
@@ -20079,7 +19906,7 @@
     </row>
     <row r="52" spans="3:41" ht="34.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C52" s="61" t="s">
-        <v>787</v>
+        <v>801</v>
       </c>
       <c r="D52" s="61"/>
       <c r="E52" s="61"/>
@@ -20135,39 +19962,39 @@
     </row>
     <row r="53" spans="3:41" ht="15" x14ac:dyDescent="0.25">
       <c r="C53" s="84" t="s">
-        <v>777</v>
+        <v>791</v>
       </c>
       <c r="D53" s="85"/>
       <c r="E53" s="85"/>
       <c r="F53" s="86"/>
-      <c r="G53" s="390" t="s">
+      <c r="G53" s="386" t="s">
         <v>56</v>
       </c>
-      <c r="H53" s="391"/>
-      <c r="I53" s="391"/>
-      <c r="J53" s="392"/>
-      <c r="K53" s="391" t="s">
+      <c r="H53" s="387"/>
+      <c r="I53" s="387"/>
+      <c r="J53" s="388"/>
+      <c r="K53" s="387" t="s">
         <v>56</v>
       </c>
-      <c r="L53" s="391"/>
-      <c r="M53" s="391"/>
-      <c r="N53" s="392"/>
-      <c r="O53" s="390" t="s">
+      <c r="L53" s="387"/>
+      <c r="M53" s="387"/>
+      <c r="N53" s="388"/>
+      <c r="O53" s="386" t="s">
         <v>56</v>
       </c>
-      <c r="P53" s="391"/>
-      <c r="Q53" s="391"/>
-      <c r="R53" s="392"/>
-      <c r="S53" s="390" t="s">
+      <c r="P53" s="387"/>
+      <c r="Q53" s="387"/>
+      <c r="R53" s="388"/>
+      <c r="S53" s="386" t="s">
         <v>313</v>
       </c>
-      <c r="T53" s="392"/>
-      <c r="U53" s="390" t="s">
+      <c r="T53" s="388"/>
+      <c r="U53" s="386" t="s">
         <v>346</v>
       </c>
-      <c r="V53" s="391"/>
-      <c r="W53" s="391"/>
-      <c r="X53" s="392"/>
+      <c r="V53" s="387"/>
+      <c r="W53" s="387"/>
+      <c r="X53" s="388"/>
       <c r="Y53" s="108" t="s">
         <v>347</v>
       </c>
@@ -20185,7 +20012,7 @@
       </c>
       <c r="AD53" s="108"/>
       <c r="AE53" s="117" t="s">
-        <v>817</v>
+        <v>806</v>
       </c>
       <c r="AF53" s="108" t="s">
         <v>56</v>
@@ -20224,7 +20051,7 @@
         <v>351</v>
       </c>
       <c r="E54" s="137" t="s">
-        <v>764</v>
+        <v>777</v>
       </c>
       <c r="F54" s="76" t="s">
         <v>426</v>
@@ -20309,10 +20136,10 @@
         <v>352</v>
       </c>
       <c r="E55" s="71" t="s">
-        <v>764</v>
+        <v>777</v>
       </c>
       <c r="F55" s="70" t="s">
-        <v>758</v>
+        <v>771</v>
       </c>
       <c r="G55" s="339">
         <v>1</v>
@@ -20406,10 +20233,10 @@
         <v>353</v>
       </c>
       <c r="E56" s="77" t="s">
-        <v>766</v>
+        <v>779</v>
       </c>
       <c r="F56" s="76" t="s">
-        <v>758</v>
+        <v>771</v>
       </c>
       <c r="G56" s="336">
         <v>1</v>
@@ -20505,10 +20332,10 @@
         <v>357</v>
       </c>
       <c r="E57" s="71" t="s">
-        <v>767</v>
+        <v>780</v>
       </c>
       <c r="F57" s="70" t="s">
-        <v>758</v>
+        <v>771</v>
       </c>
       <c r="G57" s="339">
         <v>1</v>
@@ -20606,7 +20433,7 @@
         <v>350</v>
       </c>
       <c r="E58" s="77" t="s">
-        <v>769</v>
+        <v>782</v>
       </c>
       <c r="F58" s="76" t="s">
         <v>426</v>
@@ -20691,10 +20518,10 @@
         <v>354</v>
       </c>
       <c r="E59" s="71" t="s">
-        <v>769</v>
+        <v>782</v>
       </c>
       <c r="F59" s="70" t="s">
-        <v>758</v>
+        <v>771</v>
       </c>
       <c r="G59" s="339">
         <v>1</v>
@@ -20788,10 +20615,10 @@
         <v>355</v>
       </c>
       <c r="E60" s="77" t="s">
-        <v>770</v>
+        <v>783</v>
       </c>
       <c r="F60" s="76" t="s">
-        <v>758</v>
+        <v>771</v>
       </c>
       <c r="G60" s="336">
         <v>1</v>
@@ -20889,10 +20716,10 @@
         <v>356</v>
       </c>
       <c r="E61" s="71" t="s">
+        <v>784</v>
+      </c>
+      <c r="F61" s="70" t="s">
         <v>771</v>
-      </c>
-      <c r="F61" s="70" t="s">
-        <v>758</v>
       </c>
       <c r="G61" s="339">
         <v>1</v>
@@ -20990,7 +20817,7 @@
         <v>358</v>
       </c>
       <c r="E62" s="77" t="s">
-        <v>765</v>
+        <v>778</v>
       </c>
       <c r="F62" s="76" t="s">
         <v>426</v>
@@ -21075,10 +20902,10 @@
         <v>359</v>
       </c>
       <c r="E63" s="71" t="s">
-        <v>765</v>
+        <v>778</v>
       </c>
       <c r="F63" s="70" t="s">
-        <v>758</v>
+        <v>771</v>
       </c>
       <c r="G63" s="339">
         <v>1</v>
@@ -21172,7 +20999,7 @@
         <v>360</v>
       </c>
       <c r="E64" s="77" t="s">
-        <v>768</v>
+        <v>781</v>
       </c>
       <c r="F64" s="76" t="s">
         <v>426</v>
@@ -21257,10 +21084,10 @@
         <v>361</v>
       </c>
       <c r="E65" s="71" t="s">
-        <v>768</v>
+        <v>781</v>
       </c>
       <c r="F65" s="73" t="s">
-        <v>758</v>
+        <v>771</v>
       </c>
       <c r="G65" s="339">
         <v>1</v>
@@ -21347,7 +21174,7 @@
     </row>
     <row r="66" spans="3:41" ht="15" x14ac:dyDescent="0.25">
       <c r="C66" s="80" t="s">
-        <v>778</v>
+        <v>792</v>
       </c>
       <c r="D66" s="80"/>
       <c r="E66" s="81"/>
@@ -21467,7 +21294,7 @@
       <c r="AI67" s="154"/>
       <c r="AJ67" s="153" t="str">
         <f t="shared" si="31"/>
-        <v>R-SC_Att_ELC_HPN1</v>
+        <v>R-HC_Att_ELC_HPN1</v>
       </c>
       <c r="AK67" s="153" t="str">
         <f t="shared" si="31"/>
@@ -21486,7 +21313,7 @@
     </row>
     <row r="68" spans="3:41" ht="15" x14ac:dyDescent="0.25">
       <c r="C68" s="80" t="s">
-        <v>779</v>
+        <v>793</v>
       </c>
       <c r="D68" s="80"/>
       <c r="E68" s="81"/>
@@ -21625,8 +21452,8 @@
     </row>
     <row r="70" spans="3:41" ht="15" x14ac:dyDescent="0.25">
       <c r="C70" s="69" t="str">
-        <f>"R-SC_Att"&amp;"_"&amp;RIGHT(E70,3)&amp;"_HPN1"</f>
-        <v>R-SC_Att_ELC_HPN1</v>
+        <f>"R-HC_Att"&amp;"_"&amp;RIGHT(E70,3)&amp;"_HPN1"</f>
+        <v>R-HC_Att_ELC_HPN1</v>
       </c>
       <c r="D70" s="70" t="s">
         <v>365</v>
@@ -21635,7 +21462,7 @@
         <v>441</v>
       </c>
       <c r="F70" s="70" t="s">
-        <v>759</v>
+        <v>772</v>
       </c>
       <c r="G70" s="339">
         <v>1</v>
@@ -21699,7 +21526,7 @@
       <c r="AI70" s="304"/>
       <c r="AJ70" s="153" t="str">
         <f t="shared" si="31"/>
-        <v>R-SW_Att_ELC_HPN2</v>
+        <v>R-SW_Att_SOL_HPN2</v>
       </c>
       <c r="AK70" s="153" t="str">
         <f t="shared" si="31"/>
@@ -21813,7 +21640,7 @@
         <v>441</v>
       </c>
       <c r="F72" s="70" t="s">
-        <v>758</v>
+        <v>771</v>
       </c>
       <c r="G72" s="339">
         <v>1</v>
@@ -21901,16 +21728,16 @@
     <row r="73" spans="3:41" ht="15" x14ac:dyDescent="0.25">
       <c r="C73" s="87" t="str">
         <f>"R-SW_Att"&amp;"_"&amp;RIGHT(E73,3)&amp;"_HPN2"</f>
-        <v>R-SW_Att_ELC_HPN2</v>
+        <v>R-SW_Att_SOL_HPN2</v>
       </c>
       <c r="D73" s="76" t="s">
         <v>368</v>
       </c>
       <c r="E73" s="77" t="s">
-        <v>793</v>
+        <v>786</v>
       </c>
       <c r="F73" s="76" t="s">
-        <v>758</v>
+        <v>771</v>
       </c>
       <c r="G73" s="336">
         <v>1</v>
@@ -22096,7 +21923,7 @@
         <v>441</v>
       </c>
       <c r="F75" s="76" t="s">
-        <v>759</v>
+        <v>772</v>
       </c>
       <c r="G75" s="345">
         <v>1</v>
@@ -22179,7 +22006,7 @@
     </row>
     <row r="76" spans="3:41" ht="15" x14ac:dyDescent="0.25">
       <c r="C76" s="80" t="s">
-        <v>780</v>
+        <v>794</v>
       </c>
       <c r="D76" s="80"/>
       <c r="E76" s="81"/>
@@ -22240,10 +22067,10 @@
         <v>372</v>
       </c>
       <c r="E77" s="137" t="s">
-        <v>769</v>
+        <v>782</v>
       </c>
       <c r="F77" s="137" t="s">
-        <v>758</v>
+        <v>771</v>
       </c>
       <c r="G77" s="342">
         <v>1</v>
@@ -22311,7 +22138,7 @@
       <c r="AI77" s="163"/>
       <c r="AJ77" s="156" t="str">
         <f>C83</f>
-        <v>*R-SW_Att_HET_N2</v>
+        <v>R-SW_Att_HET_N2</v>
       </c>
       <c r="AK77" s="156" t="str">
         <f>D83</f>
@@ -22337,10 +22164,10 @@
         <v>373</v>
       </c>
       <c r="E78" s="74" t="s">
-        <v>769</v>
+        <v>782</v>
       </c>
       <c r="F78" s="74" t="s">
-        <v>758</v>
+        <v>771</v>
       </c>
       <c r="G78" s="355">
         <v>1</v>
@@ -22488,10 +22315,10 @@
         <v>395</v>
       </c>
       <c r="E80" s="172" t="s">
-        <v>773</v>
+        <v>787</v>
       </c>
       <c r="F80" s="76" t="s">
-        <v>758</v>
+        <v>771</v>
       </c>
       <c r="G80" s="355">
         <v>1</v>
@@ -22643,10 +22470,10 @@
         <v>375</v>
       </c>
       <c r="E82" s="137" t="s">
-        <v>755</v>
+        <v>768</v>
       </c>
       <c r="F82" s="137" t="s">
-        <v>758</v>
+        <v>771</v>
       </c>
       <c r="G82" s="342">
         <v>1</v>
@@ -22729,17 +22556,17 @@
     </row>
     <row r="83" spans="3:41" ht="15" x14ac:dyDescent="0.25">
       <c r="C83" s="354" t="str">
-        <f>"*R-SW_Att"&amp;"_"&amp;RIGHT(E83,3)&amp;"_N2"</f>
-        <v>*R-SW_Att_HET_N2</v>
+        <f>"R-SW_Att"&amp;"_"&amp;RIGHT(E83,3)&amp;"_N2"</f>
+        <v>R-SW_Att_HET_N2</v>
       </c>
       <c r="D83" s="73" t="s">
         <v>376</v>
       </c>
       <c r="E83" s="74" t="s">
-        <v>755</v>
+        <v>768</v>
       </c>
       <c r="F83" s="74" t="s">
-        <v>758</v>
+        <v>771</v>
       </c>
       <c r="G83" s="355">
         <v>1</v>
@@ -22803,7 +22630,7 @@
       <c r="AI83" s="4"/>
       <c r="AJ83" s="153" t="str">
         <f>C91</f>
-        <v>R-AC_Att_ELC_N1</v>
+        <v>R-SC_Att_ELC_N1</v>
       </c>
       <c r="AK83" s="153" t="str">
         <f>D91</f>
@@ -22930,7 +22757,7 @@
         <v>379</v>
       </c>
       <c r="E86" s="71" t="s">
-        <v>774</v>
+        <v>788</v>
       </c>
       <c r="F86" s="70" t="s">
         <v>429</v>
@@ -22998,7 +22825,7 @@
         <v>381</v>
       </c>
       <c r="E87" s="77" t="s">
-        <v>769</v>
+        <v>782</v>
       </c>
       <c r="F87" s="76" t="s">
         <v>429</v>
@@ -23064,7 +22891,7 @@
         <v>380</v>
       </c>
       <c r="E88" s="71" t="s">
-        <v>768</v>
+        <v>781</v>
       </c>
       <c r="F88" s="70" t="s">
         <v>429</v>
@@ -23130,7 +22957,7 @@
         <v>382</v>
       </c>
       <c r="E89" s="170" t="s">
-        <v>765</v>
+        <v>778</v>
       </c>
       <c r="F89" s="138" t="s">
         <v>429</v>
@@ -23189,7 +23016,7 @@
     </row>
     <row r="90" spans="3:41" x14ac:dyDescent="0.2">
       <c r="C90" s="80" t="s">
-        <v>784</v>
+        <v>798</v>
       </c>
       <c r="D90" s="80"/>
       <c r="E90" s="81"/>
@@ -23224,8 +23051,8 @@
     </row>
     <row r="91" spans="3:41" x14ac:dyDescent="0.2">
       <c r="C91" s="76" t="str">
-        <f>"R-AC_Att"&amp;"_"&amp;RIGHT(E91,3)&amp;"_N1"</f>
-        <v>R-AC_Att_ELC_N1</v>
+        <f>"R-SC_Att"&amp;"_"&amp;RIGHT(E91,3)&amp;"_N1"</f>
+        <v>R-SC_Att_ELC_N1</v>
       </c>
       <c r="D91" s="145" t="s">
         <v>383</v>
@@ -23234,7 +23061,7 @@
         <v>441</v>
       </c>
       <c r="F91" s="169" t="s">
-        <v>797</v>
+        <v>428</v>
       </c>
       <c r="G91" s="164"/>
       <c r="H91" s="165"/>
@@ -23307,40 +23134,40 @@
         <v>42</v>
       </c>
       <c r="G97" s="64" t="s">
-        <v>692</v>
+        <v>700</v>
       </c>
       <c r="H97" s="64" t="s">
-        <v>693</v>
+        <v>701</v>
       </c>
       <c r="I97" s="64" t="s">
-        <v>694</v>
+        <v>702</v>
       </c>
       <c r="J97" s="64" t="s">
-        <v>695</v>
+        <v>703</v>
       </c>
       <c r="K97" s="64" t="s">
-        <v>806</v>
+        <v>704</v>
       </c>
       <c r="L97" s="64" t="s">
-        <v>807</v>
+        <v>705</v>
       </c>
       <c r="M97" s="64" t="s">
-        <v>808</v>
+        <v>706</v>
       </c>
       <c r="N97" s="64" t="s">
-        <v>809</v>
+        <v>707</v>
       </c>
       <c r="O97" s="64" t="s">
-        <v>696</v>
+        <v>708</v>
       </c>
       <c r="P97" s="64" t="s">
-        <v>697</v>
+        <v>709</v>
       </c>
       <c r="Q97" s="64" t="s">
-        <v>698</v>
+        <v>710</v>
       </c>
       <c r="R97" s="64" t="s">
-        <v>699</v>
+        <v>711</v>
       </c>
       <c r="S97" s="65" t="s">
         <v>44</v>
@@ -23349,7 +23176,7 @@
         <v>330</v>
       </c>
       <c r="U97" s="64" t="s">
-        <v>704</v>
+        <v>716</v>
       </c>
       <c r="V97" s="64" t="s">
         <v>342</v>
@@ -23367,22 +23194,22 @@
         <v>93</v>
       </c>
       <c r="AA97" s="64" t="s">
-        <v>789</v>
+        <v>803</v>
       </c>
       <c r="AB97" s="64" t="s">
-        <v>790</v>
+        <v>804</v>
       </c>
       <c r="AC97" s="64" t="s">
-        <v>791</v>
+        <v>805</v>
       </c>
       <c r="AD97" s="64" t="s">
-        <v>707</v>
+        <v>719</v>
       </c>
       <c r="AE97" s="64" t="s">
         <v>331</v>
       </c>
       <c r="AF97" s="64" t="s">
-        <v>775</v>
+        <v>789</v>
       </c>
       <c r="AG97" s="64" t="s">
         <v>332</v>
@@ -23410,34 +23237,34 @@
       <c r="F98" s="63" t="s">
         <v>335</v>
       </c>
-      <c r="G98" s="393" t="s">
+      <c r="G98" s="389" t="s">
         <v>336</v>
       </c>
-      <c r="H98" s="394"/>
-      <c r="I98" s="394"/>
-      <c r="J98" s="395"/>
-      <c r="K98" s="393" t="s">
+      <c r="H98" s="390"/>
+      <c r="I98" s="390"/>
+      <c r="J98" s="391"/>
+      <c r="K98" s="389" t="s">
         <v>337</v>
       </c>
-      <c r="L98" s="394"/>
-      <c r="M98" s="394"/>
-      <c r="N98" s="395"/>
-      <c r="O98" s="393" t="s">
+      <c r="L98" s="390"/>
+      <c r="M98" s="390"/>
+      <c r="N98" s="391"/>
+      <c r="O98" s="389" t="s">
         <v>338</v>
       </c>
-      <c r="P98" s="394"/>
-      <c r="Q98" s="394"/>
-      <c r="R98" s="395"/>
-      <c r="S98" s="393" t="s">
+      <c r="P98" s="390"/>
+      <c r="Q98" s="390"/>
+      <c r="R98" s="391"/>
+      <c r="S98" s="389" t="s">
         <v>339</v>
       </c>
-      <c r="T98" s="395"/>
-      <c r="U98" s="387" t="s">
+      <c r="T98" s="391"/>
+      <c r="U98" s="383" t="s">
         <v>340</v>
       </c>
-      <c r="V98" s="388"/>
-      <c r="W98" s="388"/>
-      <c r="X98" s="389"/>
+      <c r="V98" s="384"/>
+      <c r="W98" s="384"/>
+      <c r="X98" s="385"/>
       <c r="Y98" s="107"/>
       <c r="Z98" s="107"/>
       <c r="AA98" s="115" t="s">
@@ -23450,7 +23277,7 @@
         <v>661</v>
       </c>
       <c r="AD98" s="118" t="s">
-        <v>706</v>
+        <v>718</v>
       </c>
       <c r="AE98" s="107" t="s">
         <v>127</v>
@@ -23483,7 +23310,7 @@
     </row>
     <row r="99" spans="3:41" ht="34.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C99" s="61" t="s">
-        <v>788</v>
+        <v>802</v>
       </c>
       <c r="D99" s="61"/>
       <c r="E99" s="61"/>
@@ -23539,39 +23366,39 @@
     </row>
     <row r="100" spans="3:41" ht="15" x14ac:dyDescent="0.25">
       <c r="C100" s="84" t="s">
-        <v>777</v>
+        <v>791</v>
       </c>
       <c r="D100" s="85"/>
       <c r="E100" s="85"/>
       <c r="F100" s="86"/>
-      <c r="G100" s="390" t="s">
+      <c r="G100" s="386" t="s">
         <v>56</v>
       </c>
-      <c r="H100" s="391"/>
-      <c r="I100" s="391"/>
-      <c r="J100" s="392"/>
-      <c r="K100" s="391" t="s">
+      <c r="H100" s="387"/>
+      <c r="I100" s="387"/>
+      <c r="J100" s="388"/>
+      <c r="K100" s="387" t="s">
         <v>56</v>
       </c>
-      <c r="L100" s="391"/>
-      <c r="M100" s="391"/>
-      <c r="N100" s="392"/>
-      <c r="O100" s="390" t="s">
+      <c r="L100" s="387"/>
+      <c r="M100" s="387"/>
+      <c r="N100" s="388"/>
+      <c r="O100" s="386" t="s">
         <v>56</v>
       </c>
-      <c r="P100" s="391"/>
-      <c r="Q100" s="391"/>
-      <c r="R100" s="392"/>
-      <c r="S100" s="390" t="s">
+      <c r="P100" s="387"/>
+      <c r="Q100" s="387"/>
+      <c r="R100" s="388"/>
+      <c r="S100" s="386" t="s">
         <v>313</v>
       </c>
-      <c r="T100" s="392"/>
-      <c r="U100" s="390" t="s">
+      <c r="T100" s="388"/>
+      <c r="U100" s="386" t="s">
         <v>346</v>
       </c>
-      <c r="V100" s="391"/>
-      <c r="W100" s="391"/>
-      <c r="X100" s="392"/>
+      <c r="V100" s="387"/>
+      <c r="W100" s="387"/>
+      <c r="X100" s="388"/>
       <c r="Y100" s="108" t="s">
         <v>347</v>
       </c>
@@ -23589,7 +23416,7 @@
       </c>
       <c r="AD100" s="108"/>
       <c r="AE100" s="117" t="s">
-        <v>817</v>
+        <v>806</v>
       </c>
       <c r="AF100" s="108" t="s">
         <v>56</v>
@@ -23628,7 +23455,7 @@
         <v>351</v>
       </c>
       <c r="E101" s="137" t="s">
-        <v>764</v>
+        <v>777</v>
       </c>
       <c r="F101" s="76" t="s">
         <v>434</v>
@@ -23713,10 +23540,10 @@
         <v>352</v>
       </c>
       <c r="E102" s="71" t="s">
-        <v>764</v>
+        <v>777</v>
       </c>
       <c r="F102" s="70" t="s">
-        <v>760</v>
+        <v>773</v>
       </c>
       <c r="G102" s="339">
         <v>1</v>
@@ -23810,10 +23637,10 @@
         <v>353</v>
       </c>
       <c r="E103" s="77" t="s">
-        <v>766</v>
+        <v>779</v>
       </c>
       <c r="F103" s="76" t="s">
-        <v>760</v>
+        <v>773</v>
       </c>
       <c r="G103" s="336">
         <v>1</v>
@@ -23909,10 +23736,10 @@
         <v>357</v>
       </c>
       <c r="E104" s="71" t="s">
-        <v>767</v>
+        <v>780</v>
       </c>
       <c r="F104" s="70" t="s">
-        <v>760</v>
+        <v>773</v>
       </c>
       <c r="G104" s="339">
         <v>1</v>
@@ -24010,7 +23837,7 @@
         <v>350</v>
       </c>
       <c r="E105" s="77" t="s">
-        <v>769</v>
+        <v>782</v>
       </c>
       <c r="F105" s="76" t="s">
         <v>434</v>
@@ -24095,10 +23922,10 @@
         <v>354</v>
       </c>
       <c r="E106" s="71" t="s">
-        <v>769</v>
+        <v>782</v>
       </c>
       <c r="F106" s="70" t="s">
-        <v>760</v>
+        <v>773</v>
       </c>
       <c r="G106" s="339">
         <v>1</v>
@@ -24192,10 +24019,10 @@
         <v>355</v>
       </c>
       <c r="E107" s="77" t="s">
-        <v>770</v>
+        <v>783</v>
       </c>
       <c r="F107" s="76" t="s">
-        <v>760</v>
+        <v>773</v>
       </c>
       <c r="G107" s="336">
         <v>1</v>
@@ -24293,10 +24120,10 @@
         <v>356</v>
       </c>
       <c r="E108" s="71" t="s">
-        <v>771</v>
+        <v>784</v>
       </c>
       <c r="F108" s="70" t="s">
-        <v>760</v>
+        <v>773</v>
       </c>
       <c r="G108" s="339">
         <v>1</v>
@@ -24394,7 +24221,7 @@
         <v>358</v>
       </c>
       <c r="E109" s="77" t="s">
-        <v>765</v>
+        <v>778</v>
       </c>
       <c r="F109" s="76" t="s">
         <v>434</v>
@@ -24479,10 +24306,10 @@
         <v>359</v>
       </c>
       <c r="E110" s="71" t="s">
-        <v>765</v>
+        <v>778</v>
       </c>
       <c r="F110" s="70" t="s">
-        <v>760</v>
+        <v>773</v>
       </c>
       <c r="G110" s="339">
         <v>1</v>
@@ -24576,7 +24403,7 @@
         <v>360</v>
       </c>
       <c r="E111" s="77" t="s">
-        <v>768</v>
+        <v>781</v>
       </c>
       <c r="F111" s="76" t="s">
         <v>434</v>
@@ -24661,10 +24488,10 @@
         <v>361</v>
       </c>
       <c r="E112" s="71" t="s">
-        <v>768</v>
+        <v>781</v>
       </c>
       <c r="F112" s="73" t="s">
-        <v>760</v>
+        <v>773</v>
       </c>
       <c r="G112" s="339">
         <v>1</v>
@@ -24751,7 +24578,7 @@
     </row>
     <row r="113" spans="3:41" ht="15" x14ac:dyDescent="0.25">
       <c r="C113" s="80" t="s">
-        <v>778</v>
+        <v>792</v>
       </c>
       <c r="D113" s="80"/>
       <c r="E113" s="81"/>
@@ -24871,7 +24698,7 @@
       <c r="AI114" s="154"/>
       <c r="AJ114" s="153" t="str">
         <f t="shared" si="53"/>
-        <v>R-SC_Det_ELC_HPN1</v>
+        <v>R-HC_Det_ELC_HPN1</v>
       </c>
       <c r="AK114" s="153" t="str">
         <f t="shared" si="53"/>
@@ -24890,7 +24717,7 @@
     </row>
     <row r="115" spans="3:41" ht="15" x14ac:dyDescent="0.25">
       <c r="C115" s="80" t="s">
-        <v>779</v>
+        <v>793</v>
       </c>
       <c r="D115" s="80"/>
       <c r="E115" s="81"/>
@@ -25029,8 +24856,8 @@
     </row>
     <row r="117" spans="3:41" ht="15" x14ac:dyDescent="0.25">
       <c r="C117" s="69" t="str">
-        <f>"R-SC_Det"&amp;"_"&amp;RIGHT(E117,3)&amp;"_HPN1"</f>
-        <v>R-SC_Det_ELC_HPN1</v>
+        <f>"R-HC_Det"&amp;"_"&amp;RIGHT(E117,3)&amp;"_HPN1"</f>
+        <v>R-HC_Det_ELC_HPN1</v>
       </c>
       <c r="D117" s="70" t="s">
         <v>365</v>
@@ -25039,7 +24866,7 @@
         <v>441</v>
       </c>
       <c r="F117" s="70" t="s">
-        <v>761</v>
+        <v>774</v>
       </c>
       <c r="G117" s="339">
         <v>1</v>
@@ -25103,7 +24930,7 @@
       <c r="AI117" s="304"/>
       <c r="AJ117" s="153" t="str">
         <f t="shared" si="53"/>
-        <v>R-SW_Det_ELC_HPN2</v>
+        <v>R-SW_Det_SOL_HPN2</v>
       </c>
       <c r="AK117" s="153" t="str">
         <f t="shared" si="53"/>
@@ -25217,7 +25044,7 @@
         <v>441</v>
       </c>
       <c r="F119" s="70" t="s">
-        <v>760</v>
+        <v>773</v>
       </c>
       <c r="G119" s="339">
         <v>1</v>
@@ -25305,16 +25132,16 @@
     <row r="120" spans="3:41" ht="15" x14ac:dyDescent="0.25">
       <c r="C120" s="87" t="str">
         <f>"R-SW_Det"&amp;"_"&amp;RIGHT(E120,3)&amp;"_HPN2"</f>
-        <v>R-SW_Det_ELC_HPN2</v>
+        <v>R-SW_Det_SOL_HPN2</v>
       </c>
       <c r="D120" s="76" t="s">
         <v>368</v>
       </c>
       <c r="E120" s="77" t="s">
-        <v>793</v>
+        <v>786</v>
       </c>
       <c r="F120" s="76" t="s">
-        <v>760</v>
+        <v>773</v>
       </c>
       <c r="G120" s="336">
         <v>1</v>
@@ -25500,7 +25327,7 @@
         <v>441</v>
       </c>
       <c r="F122" s="76" t="s">
-        <v>761</v>
+        <v>774</v>
       </c>
       <c r="G122" s="345">
         <v>1</v>
@@ -25644,10 +25471,10 @@
         <v>372</v>
       </c>
       <c r="E124" s="137" t="s">
-        <v>769</v>
+        <v>782</v>
       </c>
       <c r="F124" s="137" t="s">
-        <v>760</v>
+        <v>773</v>
       </c>
       <c r="G124" s="342">
         <v>1</v>
@@ -25715,7 +25542,7 @@
       <c r="AI124" s="163"/>
       <c r="AJ124" s="156" t="str">
         <f>C130</f>
-        <v>*R-SW_Det_HET_N2</v>
+        <v>R-SW_Det_HET_N2</v>
       </c>
       <c r="AK124" s="156" t="str">
         <f>D130</f>
@@ -25741,10 +25568,10 @@
         <v>373</v>
       </c>
       <c r="E125" s="74" t="s">
-        <v>769</v>
+        <v>782</v>
       </c>
       <c r="F125" s="74" t="s">
-        <v>760</v>
+        <v>773</v>
       </c>
       <c r="G125" s="355">
         <v>1</v>
@@ -25831,7 +25658,7 @@
     </row>
     <row r="126" spans="3:41" ht="15" x14ac:dyDescent="0.25">
       <c r="C126" s="80" t="s">
-        <v>781</v>
+        <v>795</v>
       </c>
       <c r="D126" s="80"/>
       <c r="E126" s="81"/>
@@ -25892,10 +25719,10 @@
         <v>395</v>
       </c>
       <c r="E127" s="172" t="s">
+        <v>787</v>
+      </c>
+      <c r="F127" s="76" t="s">
         <v>773</v>
-      </c>
-      <c r="F127" s="76" t="s">
-        <v>760</v>
       </c>
       <c r="G127" s="355">
         <v>1</v>
@@ -25986,7 +25813,7 @@
     </row>
     <row r="128" spans="3:41" ht="15" x14ac:dyDescent="0.25">
       <c r="C128" s="80" t="s">
-        <v>782</v>
+        <v>796</v>
       </c>
       <c r="D128" s="80"/>
       <c r="E128" s="81"/>
@@ -26047,10 +25874,10 @@
         <v>375</v>
       </c>
       <c r="E129" s="137" t="s">
-        <v>755</v>
+        <v>768</v>
       </c>
       <c r="F129" s="137" t="s">
-        <v>760</v>
+        <v>773</v>
       </c>
       <c r="G129" s="342">
         <v>1</v>
@@ -26133,17 +25960,17 @@
     </row>
     <row r="130" spans="1:41" ht="15" x14ac:dyDescent="0.25">
       <c r="C130" s="354" t="str">
-        <f>"*R-SW_Det"&amp;"_"&amp;RIGHT(E130,3)&amp;"_N2"</f>
-        <v>*R-SW_Det_HET_N2</v>
+        <f>"R-SW_Det"&amp;"_"&amp;RIGHT(E130,3)&amp;"_N2"</f>
+        <v>R-SW_Det_HET_N2</v>
       </c>
       <c r="D130" s="73" t="s">
         <v>376</v>
       </c>
       <c r="E130" s="74" t="s">
-        <v>755</v>
+        <v>768</v>
       </c>
       <c r="F130" s="74" t="s">
-        <v>760</v>
+        <v>773</v>
       </c>
       <c r="G130" s="355">
         <v>1</v>
@@ -26207,7 +26034,7 @@
       <c r="AI130" s="4"/>
       <c r="AJ130" s="153" t="str">
         <f>C138</f>
-        <v>R-AC_Det_ELC_N1</v>
+        <v>R-SC_Det_ELC_N1</v>
       </c>
       <c r="AK130" s="153" t="str">
         <f>D138</f>
@@ -26226,7 +26053,7 @@
     </row>
     <row r="131" spans="1:41" x14ac:dyDescent="0.2">
       <c r="C131" s="80" t="s">
-        <v>783</v>
+        <v>797</v>
       </c>
       <c r="D131" s="80"/>
       <c r="E131" s="81"/>
@@ -26334,7 +26161,7 @@
         <v>379</v>
       </c>
       <c r="E133" s="71" t="s">
-        <v>774</v>
+        <v>788</v>
       </c>
       <c r="F133" s="70" t="s">
         <v>437</v>
@@ -26402,7 +26229,7 @@
         <v>381</v>
       </c>
       <c r="E134" s="77" t="s">
-        <v>769</v>
+        <v>782</v>
       </c>
       <c r="F134" s="76" t="s">
         <v>437</v>
@@ -26468,7 +26295,7 @@
         <v>380</v>
       </c>
       <c r="E135" s="71" t="s">
-        <v>768</v>
+        <v>781</v>
       </c>
       <c r="F135" s="70" t="s">
         <v>437</v>
@@ -26534,7 +26361,7 @@
         <v>382</v>
       </c>
       <c r="E136" s="170" t="s">
-        <v>765</v>
+        <v>778</v>
       </c>
       <c r="F136" s="138" t="s">
         <v>437</v>
@@ -26593,7 +26420,7 @@
     </row>
     <row r="137" spans="1:41" x14ac:dyDescent="0.2">
       <c r="C137" s="80" t="s">
-        <v>784</v>
+        <v>798</v>
       </c>
       <c r="D137" s="80"/>
       <c r="E137" s="81"/>
@@ -26628,8 +26455,8 @@
     </row>
     <row r="138" spans="1:41" x14ac:dyDescent="0.2">
       <c r="C138" s="76" t="str">
-        <f>"R-AC_Det"&amp;"_"&amp;RIGHT(E138,3)&amp;"_N1"</f>
-        <v>R-AC_Det_ELC_N1</v>
+        <f>"R-SC_Det"&amp;"_"&amp;RIGHT(E138,3)&amp;"_N1"</f>
+        <v>R-SC_Det_ELC_N1</v>
       </c>
       <c r="D138" s="145" t="s">
         <v>383</v>
@@ -26638,7 +26465,7 @@
         <v>441</v>
       </c>
       <c r="F138" s="169" t="s">
-        <v>796</v>
+        <v>436</v>
       </c>
       <c r="G138" s="164"/>
       <c r="H138" s="165"/>
@@ -26809,7 +26636,7 @@
         <v>325</v>
       </c>
       <c r="B148" s="153" t="s">
-        <v>762</v>
+        <v>775</v>
       </c>
       <c r="C148" s="153" t="s">
         <v>384</v>
@@ -26827,7 +26654,7 @@
     <row r="149" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A149" s="4"/>
       <c r="B149" s="153" t="s">
-        <v>762</v>
+        <v>775</v>
       </c>
       <c r="C149" s="153" t="s">
         <v>385</v>
@@ -26846,7 +26673,7 @@
     <row r="150" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A150" s="4"/>
       <c r="B150" s="153" t="s">
-        <v>762</v>
+        <v>775</v>
       </c>
       <c r="C150" s="153" t="s">
         <v>386</v>
@@ -26865,7 +26692,7 @@
     <row r="151" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A151" s="162"/>
       <c r="B151" s="153" t="s">
-        <v>762</v>
+        <v>775</v>
       </c>
       <c r="C151" s="153" t="s">
         <v>387</v>
@@ -26884,7 +26711,7 @@
     <row r="152" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A152" s="4"/>
       <c r="B152" s="153" t="s">
-        <v>762</v>
+        <v>775</v>
       </c>
       <c r="C152" s="153" t="s">
         <v>388</v>
@@ -26903,7 +26730,7 @@
     <row r="153" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A153" s="4"/>
       <c r="B153" s="153" t="s">
-        <v>762</v>
+        <v>775</v>
       </c>
       <c r="C153" s="153" t="s">
         <v>389</v>
@@ -26922,26 +26749,6 @@
     <row r="170" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="G100:J100"/>
-    <mergeCell ref="K100:N100"/>
-    <mergeCell ref="O100:R100"/>
-    <mergeCell ref="S100:T100"/>
-    <mergeCell ref="U100:X100"/>
-    <mergeCell ref="G98:J98"/>
-    <mergeCell ref="K98:N98"/>
-    <mergeCell ref="O98:R98"/>
-    <mergeCell ref="S98:T98"/>
-    <mergeCell ref="U98:X98"/>
-    <mergeCell ref="G53:J53"/>
-    <mergeCell ref="K53:N53"/>
-    <mergeCell ref="O53:R53"/>
-    <mergeCell ref="S53:T53"/>
-    <mergeCell ref="U53:X53"/>
-    <mergeCell ref="G51:J51"/>
-    <mergeCell ref="K51:N51"/>
-    <mergeCell ref="O51:R51"/>
-    <mergeCell ref="S51:T51"/>
-    <mergeCell ref="U51:X51"/>
     <mergeCell ref="U4:X4"/>
     <mergeCell ref="U6:X6"/>
     <mergeCell ref="G4:J4"/>
@@ -26952,6 +26759,26 @@
     <mergeCell ref="O6:R6"/>
     <mergeCell ref="K6:N6"/>
     <mergeCell ref="G6:J6"/>
+    <mergeCell ref="G51:J51"/>
+    <mergeCell ref="K51:N51"/>
+    <mergeCell ref="O51:R51"/>
+    <mergeCell ref="S51:T51"/>
+    <mergeCell ref="U51:X51"/>
+    <mergeCell ref="G53:J53"/>
+    <mergeCell ref="K53:N53"/>
+    <mergeCell ref="O53:R53"/>
+    <mergeCell ref="S53:T53"/>
+    <mergeCell ref="U53:X53"/>
+    <mergeCell ref="G98:J98"/>
+    <mergeCell ref="K98:N98"/>
+    <mergeCell ref="O98:R98"/>
+    <mergeCell ref="S98:T98"/>
+    <mergeCell ref="U98:X98"/>
+    <mergeCell ref="G100:J100"/>
+    <mergeCell ref="K100:N100"/>
+    <mergeCell ref="O100:R100"/>
+    <mergeCell ref="S100:T100"/>
+    <mergeCell ref="U100:X100"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -26965,8 +26792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CED359C-4B42-41C8-A7E8-4F6FC9AE57D2}">
   <dimension ref="C2:W35"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="R31" sqref="R31"/>
+    <sheetView topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -27047,7 +26874,7 @@
         <v>345</v>
       </c>
       <c r="L4" s="64" t="s">
-        <v>704</v>
+        <v>716</v>
       </c>
       <c r="M4" s="64" t="s">
         <v>342</v>
@@ -27062,7 +26889,7 @@
         <v>92</v>
       </c>
       <c r="Q4" s="64" t="s">
-        <v>775</v>
+        <v>789</v>
       </c>
       <c r="R4" s="64" t="s">
         <v>331</v>
@@ -27091,12 +26918,12 @@
       <c r="I5" s="178"/>
       <c r="J5" s="178"/>
       <c r="K5" s="178"/>
-      <c r="L5" s="387" t="s">
+      <c r="L5" s="383" t="s">
         <v>340</v>
       </c>
-      <c r="M5" s="388"/>
-      <c r="N5" s="388"/>
-      <c r="O5" s="389"/>
+      <c r="M5" s="384"/>
+      <c r="N5" s="384"/>
+      <c r="O5" s="385"/>
       <c r="P5" s="107"/>
       <c r="Q5" s="107" t="s">
         <v>341</v>
@@ -27127,12 +26954,12 @@
       <c r="I6" s="84"/>
       <c r="J6" s="84"/>
       <c r="K6" s="84"/>
-      <c r="L6" s="390" t="s">
+      <c r="L6" s="386" t="s">
         <v>346</v>
       </c>
-      <c r="M6" s="391"/>
-      <c r="N6" s="391"/>
-      <c r="O6" s="392"/>
+      <c r="M6" s="387"/>
+      <c r="N6" s="387"/>
+      <c r="O6" s="388"/>
       <c r="P6" s="108" t="s">
         <v>347</v>
       </c>
@@ -27140,7 +26967,7 @@
         <v>56</v>
       </c>
       <c r="R6" s="117" t="s">
-        <v>818</v>
+        <v>807</v>
       </c>
       <c r="S6" s="108" t="s">
         <v>349</v>
@@ -27158,7 +26985,7 @@
     <row r="7" spans="3:23" x14ac:dyDescent="0.2">
       <c r="C7" s="203" t="str">
         <f>D20</f>
-        <v>R-RF_N1</v>
+        <v>R-RSDRF_N1</v>
       </c>
       <c r="D7" s="204" t="str">
         <f>E20</f>
@@ -27220,7 +27047,7 @@
     <row r="8" spans="3:23" x14ac:dyDescent="0.2">
       <c r="C8" s="206" t="str">
         <f>D21</f>
-        <v>R-CK_N1</v>
+        <v>R-RSDCK_N1</v>
       </c>
       <c r="D8" s="196" t="str">
         <f>E21</f>
@@ -27283,7 +27110,7 @@
       <c r="C9" s="208"/>
       <c r="D9" s="197"/>
       <c r="E9" s="197" t="s">
-        <v>769</v>
+        <v>782</v>
       </c>
       <c r="F9" s="209"/>
       <c r="G9" s="215">
@@ -27337,7 +27164,7 @@
       <c r="C10" s="206"/>
       <c r="D10" s="196"/>
       <c r="E10" s="196" t="s">
-        <v>765</v>
+        <v>778</v>
       </c>
       <c r="F10" s="207"/>
       <c r="G10" s="214">
@@ -27390,7 +27217,7 @@
     <row r="11" spans="3:23" x14ac:dyDescent="0.2">
       <c r="C11" s="208" t="str">
         <f>D22</f>
-        <v>R-CW_N1</v>
+        <v>R-RSDCW_N1</v>
       </c>
       <c r="D11" s="197" t="str">
         <f>E22</f>
@@ -27452,7 +27279,7 @@
     <row r="12" spans="3:23" x14ac:dyDescent="0.2">
       <c r="C12" s="206" t="str">
         <f t="shared" ref="C12:D15" si="2">D23</f>
-        <v>R-CD_N1</v>
+        <v>R-RSDCD_N1</v>
       </c>
       <c r="D12" s="196" t="str">
         <f t="shared" si="2"/>
@@ -27514,7 +27341,7 @@
     <row r="13" spans="3:23" x14ac:dyDescent="0.2">
       <c r="C13" s="208" t="str">
         <f t="shared" si="2"/>
-        <v>R-DW_N1</v>
+        <v>R-RSDDW_N1</v>
       </c>
       <c r="D13" s="197" t="str">
         <f t="shared" si="2"/>
@@ -27576,7 +27403,7 @@
     <row r="14" spans="3:23" x14ac:dyDescent="0.2">
       <c r="C14" s="206" t="str">
         <f t="shared" si="2"/>
-        <v>R-OE_N1</v>
+        <v>R-RSDOE_N1</v>
       </c>
       <c r="D14" s="196" t="str">
         <f t="shared" si="2"/>
@@ -27627,7 +27454,7 @@
     <row r="15" spans="3:23" x14ac:dyDescent="0.2">
       <c r="C15" s="210" t="str">
         <f t="shared" si="2"/>
-        <v>R-OA_N1</v>
+        <v>R-RSDOA_N1</v>
       </c>
       <c r="D15" s="211" t="str">
         <f t="shared" si="2"/>
@@ -27674,18 +27501,18 @@
       <c r="S15" s="216">
         <v>2020</v>
       </c>
-      <c r="T15" s="194" t="s">
+      <c r="U15" s="194" t="s">
         <v>662</v>
       </c>
-      <c r="U15" s="287" t="s">
+      <c r="V15" s="287" t="s">
         <v>519</v>
       </c>
     </row>
     <row r="16" spans="3:23" x14ac:dyDescent="0.2">
-      <c r="T16" s="194" t="s">
+      <c r="U16" s="194" t="s">
         <v>663</v>
       </c>
-      <c r="U16" s="5" t="s">
+      <c r="V16" s="5" t="s">
         <v>664</v>
       </c>
     </row>
@@ -27693,10 +27520,10 @@
       <c r="C18" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="R18" s="396" t="s">
-        <v>705</v>
-      </c>
-      <c r="S18" s="396"/>
+      <c r="R18" s="392" t="s">
+        <v>717</v>
+      </c>
+      <c r="S18" s="392"/>
     </row>
     <row r="19" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C19" s="198" t="s">
@@ -27723,15 +27550,15 @@
       <c r="J19" s="200" t="s">
         <v>312</v>
       </c>
-      <c r="R19" s="396"/>
-      <c r="S19" s="396"/>
+      <c r="R19" s="392"/>
+      <c r="S19" s="392"/>
     </row>
     <row r="20" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C20" s="173" t="s">
         <v>49</v>
       </c>
       <c r="D20" s="174" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="E20" s="174" t="s">
         <v>449</v>
@@ -27747,15 +27574,15 @@
       <c r="J20" s="175" t="s">
         <v>451</v>
       </c>
-      <c r="R20" s="396"/>
-      <c r="S20" s="396"/>
+      <c r="R20" s="392"/>
+      <c r="S20" s="392"/>
     </row>
     <row r="21" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C21" s="173" t="s">
         <v>49</v>
       </c>
       <c r="D21" s="174" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="E21" s="174" t="s">
         <v>452</v>
@@ -27771,15 +27598,15 @@
       <c r="J21" s="175" t="s">
         <v>451</v>
       </c>
-      <c r="R21" s="396"/>
-      <c r="S21" s="396"/>
+      <c r="R21" s="392"/>
+      <c r="S21" s="392"/>
     </row>
     <row r="22" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C22" s="173" t="s">
         <v>49</v>
       </c>
       <c r="D22" s="174" t="s">
-        <v>816</v>
+        <v>810</v>
       </c>
       <c r="E22" s="174" t="s">
         <v>453</v>
@@ -27795,15 +27622,15 @@
       <c r="J22" s="175" t="s">
         <v>451</v>
       </c>
-      <c r="R22" s="396"/>
-      <c r="S22" s="396"/>
+      <c r="R22" s="392"/>
+      <c r="S22" s="392"/>
     </row>
     <row r="23" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C23" s="173" t="s">
         <v>49</v>
       </c>
       <c r="D23" s="174" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="E23" s="174" t="s">
         <v>454</v>
@@ -27825,7 +27652,7 @@
         <v>49</v>
       </c>
       <c r="D24" s="174" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="E24" s="174" t="s">
         <v>455</v>
@@ -27847,7 +27674,7 @@
         <v>49</v>
       </c>
       <c r="D25" s="174" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="E25" s="174" t="s">
         <v>456</v>
@@ -27869,7 +27696,7 @@
         <v>49</v>
       </c>
       <c r="D26" s="176" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="E26" s="176" t="s">
         <v>457</v>
@@ -27900,7 +27727,7 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="U15" r:id="rId1" xr:uid="{8872A4E8-1ED1-45C9-9AE2-8045F13A0849}"/>
+    <hyperlink ref="V15" r:id="rId1" xr:uid="{8872A4E8-1ED1-45C9-9AE2-8045F13A0849}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -27912,8 +27739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAFF4867-10C8-4ED5-9BE1-6E89AAC9887A}">
   <dimension ref="C2:W347"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -27964,7 +27791,7 @@
         <v>345</v>
       </c>
       <c r="L3" s="64" t="s">
-        <v>704</v>
+        <v>716</v>
       </c>
       <c r="M3" s="64" t="s">
         <v>342</v>
@@ -27979,7 +27806,7 @@
         <v>92</v>
       </c>
       <c r="Q3" s="64" t="s">
-        <v>775</v>
+        <v>789</v>
       </c>
       <c r="R3" s="64" t="s">
         <v>331</v>
@@ -28008,12 +27835,12 @@
       <c r="I4" s="178"/>
       <c r="J4" s="178"/>
       <c r="K4" s="178"/>
-      <c r="L4" s="387" t="s">
+      <c r="L4" s="383" t="s">
         <v>340</v>
       </c>
-      <c r="M4" s="388"/>
-      <c r="N4" s="388"/>
-      <c r="O4" s="389"/>
+      <c r="M4" s="384"/>
+      <c r="N4" s="384"/>
+      <c r="O4" s="385"/>
       <c r="P4" s="107"/>
       <c r="Q4" s="107" t="s">
         <v>341</v>
@@ -28037,12 +27864,12 @@
       <c r="I5" s="84"/>
       <c r="J5" s="84"/>
       <c r="K5" s="84"/>
-      <c r="L5" s="390" t="s">
+      <c r="L5" s="386" t="s">
         <v>346</v>
       </c>
-      <c r="M5" s="391"/>
-      <c r="N5" s="391"/>
-      <c r="O5" s="392"/>
+      <c r="M5" s="387"/>
+      <c r="N5" s="387"/>
+      <c r="O5" s="388"/>
       <c r="P5" s="108" t="s">
         <v>347</v>
       </c>
@@ -28050,7 +27877,7 @@
         <v>56</v>
       </c>
       <c r="R5" s="117" t="s">
-        <v>817</v>
+        <v>807</v>
       </c>
       <c r="S5" s="108" t="s">
         <v>349</v>
@@ -28074,16 +27901,16 @@
       <c r="G6" s="213">
         <v>10</v>
       </c>
-      <c r="H6" s="366">
+      <c r="H6" s="203">
         <v>0.4</v>
       </c>
-      <c r="I6" s="367">
+      <c r="I6" s="204">
         <v>0.4</v>
       </c>
-      <c r="J6" s="366">
+      <c r="J6" s="203">
         <v>0.4</v>
       </c>
-      <c r="K6" s="367">
+      <c r="K6" s="204">
         <v>0.4</v>
       </c>
       <c r="L6" s="203">
@@ -28131,16 +27958,16 @@
       <c r="G7" s="214">
         <v>15</v>
       </c>
-      <c r="H7" s="368">
+      <c r="H7" s="206">
         <v>0.6</v>
       </c>
-      <c r="I7" s="369">
+      <c r="I7" s="196">
         <v>0.6</v>
       </c>
-      <c r="J7" s="368">
+      <c r="J7" s="206">
         <v>0.6</v>
       </c>
-      <c r="K7" s="369">
+      <c r="K7" s="196">
         <v>0.6</v>
       </c>
       <c r="L7" s="206">
@@ -28185,16 +28012,16 @@
       <c r="G8" s="215">
         <v>10</v>
       </c>
-      <c r="H8" s="366">
+      <c r="H8" s="203">
         <v>0.4</v>
       </c>
-      <c r="I8" s="367">
+      <c r="I8" s="204">
         <v>0.4</v>
       </c>
-      <c r="J8" s="366">
+      <c r="J8" s="203">
         <v>0.4</v>
       </c>
-      <c r="K8" s="367">
+      <c r="K8" s="204">
         <v>0.4</v>
       </c>
       <c r="L8" s="203">
@@ -28239,16 +28066,16 @@
       <c r="G9" s="214">
         <v>15</v>
       </c>
-      <c r="H9" s="368">
+      <c r="H9" s="206">
         <v>0.6</v>
       </c>
-      <c r="I9" s="369">
+      <c r="I9" s="196">
         <v>0.6</v>
       </c>
-      <c r="J9" s="368">
+      <c r="J9" s="206">
         <v>0.6</v>
       </c>
-      <c r="K9" s="369">
+      <c r="K9" s="196">
         <v>0.6</v>
       </c>
       <c r="L9" s="206">
@@ -28290,16 +28117,16 @@
       <c r="G10" s="215">
         <v>10</v>
       </c>
-      <c r="H10" s="366">
+      <c r="H10" s="203">
         <v>0.4</v>
       </c>
-      <c r="I10" s="367">
+      <c r="I10" s="204">
         <v>0.4</v>
       </c>
-      <c r="J10" s="366">
+      <c r="J10" s="203">
         <v>0.4</v>
       </c>
-      <c r="K10" s="367">
+      <c r="K10" s="204">
         <v>0.4</v>
       </c>
       <c r="L10" s="203">
@@ -28341,16 +28168,16 @@
       <c r="G11" s="214">
         <v>15</v>
       </c>
-      <c r="H11" s="368">
+      <c r="H11" s="206">
         <v>0.6</v>
       </c>
-      <c r="I11" s="369">
+      <c r="I11" s="196">
         <v>0.6</v>
       </c>
-      <c r="J11" s="368">
+      <c r="J11" s="206">
         <v>0.6</v>
       </c>
-      <c r="K11" s="369">
+      <c r="K11" s="196">
         <v>0.6</v>
       </c>
       <c r="L11" s="206">
@@ -30964,49 +30791,49 @@
         <v>98</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>742</v>
+        <v>755</v>
       </c>
       <c r="I1" s="9"/>
       <c r="J1" s="10"/>
       <c r="K1" s="10"/>
       <c r="L1" s="9" t="s">
-        <v>743</v>
+        <v>756</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>744</v>
+        <v>757</v>
       </c>
       <c r="N1" s="9" t="s">
-        <v>745</v>
+        <v>758</v>
       </c>
       <c r="O1" s="9" t="s">
-        <v>746</v>
+        <v>759</v>
       </c>
       <c r="P1" s="9" t="s">
-        <v>747</v>
+        <v>760</v>
       </c>
       <c r="Q1" s="9" t="s">
-        <v>748</v>
+        <v>761</v>
       </c>
       <c r="R1" s="10"/>
       <c r="S1" s="10"/>
       <c r="T1" s="10"/>
       <c r="U1" s="9" t="s">
-        <v>749</v>
+        <v>762</v>
       </c>
       <c r="V1" s="9" t="s">
-        <v>750</v>
+        <v>763</v>
       </c>
       <c r="W1" s="9" t="s">
-        <v>751</v>
+        <v>764</v>
       </c>
       <c r="X1" s="9" t="s">
-        <v>752</v>
+        <v>765</v>
       </c>
       <c r="Y1" s="9" t="s">
-        <v>753</v>
+        <v>766</v>
       </c>
       <c r="Z1" s="9" t="s">
-        <v>754</v>
+        <v>767</v>
       </c>
       <c r="AA1" s="11"/>
       <c r="AB1" s="9" t="s">

</xml_diff>

<commit_message>
Update names of cookers in the declaration table, as well as fill tables in trans
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_RSD.xlsx
+++ b/SubRES_TMPL/SubRes_RSD.xlsx
@@ -3,10 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF80CAE7-5D88-4B1E-9069-EEB21E60744A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF652C77-F333-44A4-9D61-A75D56752D33}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{9D5618E0-D2A2-4912-B654-2E39BDAED497}"/>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{34F9D92C-266F-476D-89E0-63153305AC39}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{34F9D92C-266F-476D-89E0-63153305AC39}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="34" r:id="rId1"/>
@@ -687,7 +686,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L33" authorId="0" shapeId="0" xr:uid="{26227E42-266E-4D7E-9CCC-4136610DED2C}">
+    <comment ref="L35" authorId="0" shapeId="0" xr:uid="{26227E42-266E-4D7E-9CCC-4136610DED2C}">
       <text>
         <r>
           <rPr>
@@ -8420,7 +8419,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3452" uniqueCount="1032">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3461" uniqueCount="1035">
   <si>
     <t>Document type:</t>
   </si>
@@ -11537,6 +11536,15 @@
   </si>
   <si>
     <t>Residential  Hydrotreated vegetable oil - New 1 SH + WH</t>
+  </si>
+  <si>
+    <t>Residential Cooking - Electricity - New</t>
+  </si>
+  <si>
+    <t>Residential Cooking - GAS - New</t>
+  </si>
+  <si>
+    <t>Residential Cooking - LPG - New</t>
   </si>
 </sst>
 </file>
@@ -15646,10 +15654,7 @@
   </sheetPr>
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:F17"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -16101,10 +16106,7 @@
   </sheetPr>
   <dimension ref="B1:T45"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -16835,10 +16837,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4660B878-9B9C-4131-8EFF-29EF25ED69C5}">
   <dimension ref="A2:AL103"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -19861,10 +19860,7 @@
   </sheetPr>
   <dimension ref="A1:Q202"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -24713,10 +24709,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{104F8057-C735-4662-BAA6-EEDCF7B57273}">
   <dimension ref="A2:AO162"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D96" sqref="D96"/>
-    </sheetView>
-    <sheetView topLeftCell="D23" workbookViewId="1">
+    <sheetView topLeftCell="D23" workbookViewId="0">
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
@@ -35192,21 +35185,20 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CED359C-4B42-41C8-A7E8-4F6FC9AE57D2}">
-  <dimension ref="C2:W41"/>
+  <dimension ref="C2:W43"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="5"/>
     <col min="2" max="2" width="10.7109375" style="5" customWidth="1"/>
     <col min="3" max="3" width="20.85546875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="59.140625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="38.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="39.28515625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="63.140625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="17" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.85546875" style="5" customWidth="1"/>
     <col min="8" max="15" width="10.7109375" style="5" customWidth="1"/>
     <col min="16" max="18" width="12.28515625" style="5" customWidth="1"/>
@@ -35416,19 +35408,19 @@
         <v>0.85</v>
       </c>
       <c r="L7" s="358">
-        <f>L33/$V7/1000</f>
+        <f>L35/$V7/1000</f>
         <v>0.432</v>
       </c>
       <c r="M7" s="358">
-        <f>M33/$V7/1000</f>
+        <f>M35/$V7/1000</f>
         <v>0.432</v>
       </c>
       <c r="N7" s="358">
-        <f t="shared" ref="L7:O13" si="0">N33/$V7/1000</f>
+        <f>N35/$V7/1000</f>
         <v>0.432</v>
       </c>
       <c r="O7" s="358">
-        <f t="shared" si="0"/>
+        <f>O35/$V7/1000</f>
         <v>0.432</v>
       </c>
       <c r="P7" s="212"/>
@@ -35447,13 +35439,13 @@
         <v>5.5555555555555554</v>
       </c>
       <c r="W7" s="287">
-        <f t="shared" ref="W7:W13" si="1">L33/V7</f>
+        <f>L35/V7</f>
         <v>432</v>
       </c>
     </row>
     <row r="8" spans="3:23" x14ac:dyDescent="0.2">
       <c r="C8" s="205" t="str">
-        <f>LEFT($D$21,7)&amp;"_"&amp;RIGHT(E8,3)&amp;"_N1"</f>
+        <f>D21</f>
         <v>R-RSDCK_ELC_N1</v>
       </c>
       <c r="D8" s="195" t="str">
@@ -35482,19 +35474,19 @@
         <v>0.8</v>
       </c>
       <c r="L8" s="359">
-        <f t="shared" si="0"/>
+        <f>L36/$V8/1000</f>
         <v>0.61250000000000004</v>
       </c>
       <c r="M8" s="359">
-        <f t="shared" si="0"/>
+        <f>M36/$V8/1000</f>
         <v>0.61250000000000004</v>
       </c>
       <c r="N8" s="359">
-        <f t="shared" si="0"/>
+        <f>N36/$V8/1000</f>
         <v>0.61250000000000004</v>
       </c>
       <c r="O8" s="359">
-        <f t="shared" si="0"/>
+        <f>O36/$V8/1000</f>
         <v>0.61250000000000004</v>
       </c>
       <c r="P8" s="213"/>
@@ -35509,21 +35501,21 @@
         <v>3.5</v>
       </c>
       <c r="V8" s="287">
-        <f t="shared" ref="V8:V13" si="2">1/U8</f>
+        <f t="shared" ref="V8:V13" si="0">1/U8</f>
         <v>0.2857142857142857</v>
       </c>
       <c r="W8" s="287">
-        <f t="shared" si="1"/>
+        <f>L36/V8</f>
         <v>612.5</v>
       </c>
     </row>
     <row r="9" spans="3:23" x14ac:dyDescent="0.2">
-      <c r="C9" s="207" t="str">
-        <f t="shared" ref="C9:C10" si="3">LEFT($D$21,7)&amp;"_"&amp;RIGHT(E9,3)&amp;"_N1"</f>
+      <c r="C9" s="205" t="str">
+        <f t="shared" ref="C9:C10" si="1">D22</f>
         <v>R-RSDCK_GAS_N1</v>
       </c>
       <c r="D9" s="196" t="str">
-        <f t="shared" ref="D9:D10" si="4">LEFT($E$21,20)&amp;"_"&amp;RIGHT(E9,3)&amp;" - New"</f>
+        <f t="shared" ref="D9:D10" si="2">LEFT($E$21,20)&amp;"_"&amp;RIGHT(E9,3)&amp;" - New"</f>
         <v>Residential Cooking _GAS - New</v>
       </c>
       <c r="E9" s="196" t="s">
@@ -35548,19 +35540,19 @@
         <v>0.68</v>
       </c>
       <c r="L9" s="360">
-        <f t="shared" si="0"/>
+        <f>L37/$V9/1000</f>
         <v>0.61250000000000004</v>
       </c>
       <c r="M9" s="360">
-        <f t="shared" si="0"/>
+        <f>M37/$V9/1000</f>
         <v>0.61250000000000004</v>
       </c>
       <c r="N9" s="360">
-        <f t="shared" si="0"/>
+        <f>N37/$V9/1000</f>
         <v>0.61250000000000004</v>
       </c>
       <c r="O9" s="360">
-        <f t="shared" si="0"/>
+        <f>O37/$V9/1000</f>
         <v>0.61250000000000004</v>
       </c>
       <c r="P9" s="214"/>
@@ -35575,21 +35567,21 @@
         <v>3.5</v>
       </c>
       <c r="V9" s="287">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.2857142857142857</v>
       </c>
       <c r="W9" s="287">
-        <f t="shared" si="1"/>
+        <f>L37/V9</f>
         <v>612.5</v>
       </c>
     </row>
     <row r="10" spans="3:23" x14ac:dyDescent="0.2">
       <c r="C10" s="205" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>R-RSDCK_LPG_N1</v>
       </c>
       <c r="D10" s="195" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>Residential Cooking _LPG - New</v>
       </c>
       <c r="E10" s="195" t="s">
@@ -35614,19 +35606,19 @@
         <v>0.68</v>
       </c>
       <c r="L10" s="359">
-        <f t="shared" si="0"/>
+        <f>L38/$V10/1000</f>
         <v>0.61250000000000004</v>
       </c>
       <c r="M10" s="359">
-        <f t="shared" si="0"/>
+        <f>M38/$V10/1000</f>
         <v>0.61250000000000004</v>
       </c>
       <c r="N10" s="359">
-        <f t="shared" si="0"/>
+        <f>N38/$V10/1000</f>
         <v>0.61250000000000004</v>
       </c>
       <c r="O10" s="359">
-        <f t="shared" si="0"/>
+        <f>O38/$V10/1000</f>
         <v>0.61250000000000004</v>
       </c>
       <c r="P10" s="213"/>
@@ -35641,21 +35633,21 @@
         <v>3.5</v>
       </c>
       <c r="V10" s="287">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.2857142857142857</v>
       </c>
       <c r="W10" s="287">
-        <f t="shared" si="1"/>
+        <f>L38/V10</f>
         <v>612.5</v>
       </c>
     </row>
     <row r="11" spans="3:23" x14ac:dyDescent="0.2">
       <c r="C11" s="207" t="str">
-        <f>D22</f>
+        <f>D24</f>
         <v>R-RSDCW_N1</v>
       </c>
       <c r="D11" s="196" t="str">
-        <f>E22</f>
+        <f>E24</f>
         <v>Residential Cloth Washing demand - New</v>
       </c>
       <c r="E11" s="196" t="s">
@@ -35680,19 +35672,19 @@
         <v>0.7</v>
       </c>
       <c r="L11" s="360">
-        <f t="shared" si="0"/>
+        <f>L39/$V11/1000</f>
         <v>0.55220000000000002</v>
       </c>
       <c r="M11" s="360">
-        <f t="shared" si="0"/>
+        <f>M39/$V11/1000</f>
         <v>0.55220000000000002</v>
       </c>
       <c r="N11" s="360">
-        <f t="shared" si="0"/>
+        <f>N39/$V11/1000</f>
         <v>0.55220000000000002</v>
       </c>
       <c r="O11" s="360">
-        <f t="shared" si="0"/>
+        <f>O39/$V11/1000</f>
         <v>0.55220000000000002</v>
       </c>
       <c r="P11" s="214"/>
@@ -35707,21 +35699,21 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="V11" s="287">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.45454545454545453</v>
       </c>
       <c r="W11" s="287">
-        <f t="shared" si="1"/>
+        <f>L39/V11</f>
         <v>552.20000000000005</v>
       </c>
     </row>
     <row r="12" spans="3:23" x14ac:dyDescent="0.2">
       <c r="C12" s="205" t="str">
-        <f t="shared" ref="C12:D15" si="5">D23</f>
+        <f>D25</f>
         <v>R-RSDCD_N1</v>
       </c>
       <c r="D12" s="195" t="str">
-        <f t="shared" si="5"/>
+        <f>E25</f>
         <v>Residential Cloth Drying demand - New</v>
       </c>
       <c r="E12" s="195" t="s">
@@ -35746,19 +35738,19 @@
         <v>0.6</v>
       </c>
       <c r="L12" s="359">
-        <f t="shared" si="0"/>
+        <f>L40/$V12/1000</f>
         <v>0.53500000000000003</v>
       </c>
       <c r="M12" s="359">
-        <f t="shared" si="0"/>
+        <f>M40/$V12/1000</f>
         <v>0.53500000000000003</v>
       </c>
       <c r="N12" s="359">
-        <f t="shared" si="0"/>
+        <f>N40/$V12/1000</f>
         <v>0.53500000000000003</v>
       </c>
       <c r="O12" s="359">
-        <f t="shared" si="0"/>
+        <f>O40/$V12/1000</f>
         <v>0.53500000000000003</v>
       </c>
       <c r="P12" s="213"/>
@@ -35773,21 +35765,21 @@
         <v>2.5</v>
       </c>
       <c r="V12" s="287">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
       <c r="W12" s="287">
-        <f t="shared" si="1"/>
+        <f>L40/V12</f>
         <v>535</v>
       </c>
     </row>
     <row r="13" spans="3:23" x14ac:dyDescent="0.2">
       <c r="C13" s="207" t="str">
-        <f t="shared" si="5"/>
+        <f>D26</f>
         <v>R-RSDDW_N1</v>
       </c>
       <c r="D13" s="196" t="str">
-        <f t="shared" si="5"/>
+        <f>E26</f>
         <v>Residential Dish Washing demand - New</v>
       </c>
       <c r="E13" s="196" t="s">
@@ -35812,19 +35804,19 @@
         <v>0.7</v>
       </c>
       <c r="L13" s="360">
-        <f t="shared" ref="L13" si="6">L39/$V13/1000</f>
+        <f>L41/$V13/1000</f>
         <v>0.42019999999999996</v>
       </c>
       <c r="M13" s="360">
-        <f t="shared" ref="M13" si="7">M39/$V13/1000</f>
+        <f>M41/$V13/1000</f>
         <v>0.42019999999999996</v>
       </c>
       <c r="N13" s="360">
-        <f t="shared" si="0"/>
+        <f>N41/$V13/1000</f>
         <v>0.42019999999999996</v>
       </c>
       <c r="O13" s="360">
-        <f t="shared" si="0"/>
+        <f>O41/$V13/1000</f>
         <v>0.42019999999999996</v>
       </c>
       <c r="P13" s="214"/>
@@ -35839,21 +35831,21 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="V13" s="287">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.45454545454545453</v>
       </c>
       <c r="W13" s="287">
-        <f t="shared" si="1"/>
+        <f>L41/V13</f>
         <v>420.2</v>
       </c>
     </row>
     <row r="14" spans="3:23" x14ac:dyDescent="0.2">
       <c r="C14" s="205" t="str">
-        <f t="shared" si="5"/>
+        <f>D27</f>
         <v>R-RSDOE_N1</v>
       </c>
       <c r="D14" s="195" t="str">
-        <f t="shared" si="5"/>
+        <f>E27</f>
         <v>Residential ELC Appliances - New</v>
       </c>
       <c r="E14" s="195" t="s">
@@ -35878,19 +35870,19 @@
         <v>0.85</v>
       </c>
       <c r="L14" s="368">
-        <f>L40/$V7/1000</f>
+        <f>L42/$V7/1000</f>
         <v>0.9</v>
       </c>
       <c r="M14" s="368">
-        <f t="shared" ref="M14:O14" si="8">M40/$V7/1000</f>
+        <f>M42/$V7/1000</f>
         <v>0.9</v>
       </c>
       <c r="N14" s="368">
-        <f t="shared" si="8"/>
+        <f>N42/$V7/1000</f>
         <v>0.9</v>
       </c>
       <c r="O14" s="368">
-        <f t="shared" si="8"/>
+        <f>O42/$V7/1000</f>
         <v>0.9</v>
       </c>
       <c r="P14" s="213"/>
@@ -35904,11 +35896,11 @@
     </row>
     <row r="15" spans="3:23" x14ac:dyDescent="0.2">
       <c r="C15" s="207" t="str">
-        <f t="shared" si="5"/>
+        <f>D28</f>
         <v>R-RSDOA_N1</v>
       </c>
       <c r="D15" s="196" t="str">
-        <f t="shared" si="5"/>
+        <f>E28</f>
         <v>Residential Other Applications - New</v>
       </c>
       <c r="E15" s="196" t="s">
@@ -35933,19 +35925,19 @@
         <v>0.85</v>
       </c>
       <c r="L15" s="369">
-        <f>L41/$V7/1000</f>
+        <f>L43/$V7/1000</f>
         <v>0.9</v>
       </c>
       <c r="M15" s="369">
-        <f t="shared" ref="M15:O15" si="9">M41/$V7/1000</f>
+        <f>M43/$V7/1000</f>
         <v>0.9</v>
       </c>
       <c r="N15" s="369">
-        <f t="shared" si="9"/>
+        <f>N43/$V7/1000</f>
         <v>0.9</v>
       </c>
       <c r="O15" s="369">
-        <f t="shared" si="9"/>
+        <f>O43/$V7/1000</f>
         <v>0.9</v>
       </c>
       <c r="P15" s="215"/>
@@ -36036,11 +36028,12 @@
       <c r="C21" s="172" t="s">
         <v>48</v>
       </c>
-      <c r="D21" s="173" t="s">
-        <v>789</v>
+      <c r="D21" s="173" t="str">
+        <f>_xlfn.TEXTJOIN("_",TRUE,"R-RSDCK",RIGHT(E8,3),"N1")</f>
+        <v>R-RSDCK_ELC_N1</v>
       </c>
       <c r="E21" s="173" t="s">
-        <v>446</v>
+        <v>1032</v>
       </c>
       <c r="F21" s="173" t="s">
         <v>16</v>
@@ -36060,11 +36053,12 @@
       <c r="C22" s="172" t="s">
         <v>48</v>
       </c>
-      <c r="D22" s="173" t="s">
-        <v>790</v>
+      <c r="D22" s="173" t="str">
+        <f t="shared" ref="D22:D23" si="3">_xlfn.TEXTJOIN("_",TRUE,"R-RSDCK",RIGHT(E9,3),"N1")</f>
+        <v>R-RSDCK_GAS_N1</v>
       </c>
       <c r="E22" s="173" t="s">
-        <v>447</v>
+        <v>1033</v>
       </c>
       <c r="F22" s="173" t="s">
         <v>16</v>
@@ -36084,11 +36078,12 @@
       <c r="C23" s="172" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="173" t="s">
-        <v>791</v>
+      <c r="D23" s="173" t="str">
+        <f t="shared" si="3"/>
+        <v>R-RSDCK_LPG_N1</v>
       </c>
       <c r="E23" s="173" t="s">
-        <v>448</v>
+        <v>1034</v>
       </c>
       <c r="F23" s="173" t="s">
         <v>16</v>
@@ -36107,10 +36102,10 @@
         <v>48</v>
       </c>
       <c r="D24" s="173" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="E24" s="173" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="F24" s="173" t="s">
         <v>16</v>
@@ -36129,10 +36124,10 @@
         <v>48</v>
       </c>
       <c r="D25" s="173" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="E25" s="173" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="F25" s="173" t="s">
         <v>16</v>
@@ -36150,153 +36145,163 @@
       <c r="C26" s="172" t="s">
         <v>48</v>
       </c>
-      <c r="D26" s="175" t="s">
-        <v>794</v>
-      </c>
-      <c r="E26" s="175" t="s">
-        <v>451</v>
-      </c>
-      <c r="F26" s="175" t="s">
+      <c r="D26" s="173" t="s">
+        <v>792</v>
+      </c>
+      <c r="E26" s="173" t="s">
+        <v>449</v>
+      </c>
+      <c r="F26" s="173" t="s">
         <v>16</v>
       </c>
       <c r="G26" s="173" t="s">
         <v>391</v>
       </c>
-      <c r="H26" s="175"/>
-      <c r="I26" s="175"/>
-      <c r="J26" s="176" t="s">
+      <c r="H26" s="173"/>
+      <c r="I26" s="173"/>
+      <c r="J26" s="174" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="30" spans="3:19" ht="30" x14ac:dyDescent="0.2">
-      <c r="H30" s="5" t="s">
+    <row r="27" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C27" s="172" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27" s="173" t="s">
+        <v>793</v>
+      </c>
+      <c r="E27" s="173" t="s">
+        <v>450</v>
+      </c>
+      <c r="F27" s="173" t="s">
+        <v>16</v>
+      </c>
+      <c r="G27" s="173" t="s">
+        <v>391</v>
+      </c>
+      <c r="H27" s="173"/>
+      <c r="I27" s="173"/>
+      <c r="J27" s="174" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="28" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C28" s="172" t="s">
+        <v>48</v>
+      </c>
+      <c r="D28" s="175" t="s">
+        <v>794</v>
+      </c>
+      <c r="E28" s="175" t="s">
+        <v>451</v>
+      </c>
+      <c r="F28" s="175" t="s">
+        <v>16</v>
+      </c>
+      <c r="G28" s="173" t="s">
+        <v>391</v>
+      </c>
+      <c r="H28" s="175"/>
+      <c r="I28" s="175"/>
+      <c r="J28" s="176" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="32" spans="3:19" ht="30" x14ac:dyDescent="0.2">
+      <c r="H32" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="I30" s="5" t="s">
+      <c r="I32" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="J30" s="5" t="s">
+      <c r="J32" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="K30" s="5" t="s">
+      <c r="K32" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="L30" s="64" t="s">
+      <c r="L32" s="64" t="s">
         <v>698</v>
       </c>
-      <c r="M30" s="64" t="s">
+      <c r="M32" s="64" t="s">
         <v>341</v>
       </c>
-      <c r="N30" s="64" t="s">
+      <c r="N32" s="64" t="s">
         <v>342</v>
       </c>
-      <c r="O30" s="64" t="s">
+      <c r="O32" s="64" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="31" spans="3:19" x14ac:dyDescent="0.2">
-      <c r="H31" s="5" t="s">
-        <v>332</v>
-      </c>
-      <c r="I31" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="J31" s="5" t="s">
-        <v>333</v>
-      </c>
-      <c r="K31" s="5" t="s">
-        <v>334</v>
-      </c>
-      <c r="L31" s="498" t="s">
-        <v>339</v>
-      </c>
-      <c r="M31" s="499"/>
-      <c r="N31" s="499"/>
-      <c r="O31" s="500"/>
-    </row>
-    <row r="32" spans="3:19" x14ac:dyDescent="0.2">
-      <c r="H32" s="5" t="s">
-        <v>404</v>
-      </c>
-      <c r="L32" s="501" t="s">
-        <v>345</v>
-      </c>
-      <c r="M32" s="502"/>
-      <c r="N32" s="502"/>
-      <c r="O32" s="503"/>
     </row>
     <row r="33" spans="8:15" x14ac:dyDescent="0.2">
       <c r="H33" s="5" t="s">
-        <v>788</v>
+        <v>332</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>444</v>
+        <v>52</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>436</v>
+        <v>333</v>
       </c>
       <c r="K33" s="5" t="s">
-        <v>437</v>
-      </c>
-      <c r="L33" s="202">
-        <v>2400</v>
-      </c>
-      <c r="M33" s="202">
-        <v>2400</v>
-      </c>
-      <c r="N33" s="202">
-        <v>2400</v>
-      </c>
-      <c r="O33" s="202">
-        <v>2400</v>
-      </c>
+        <v>334</v>
+      </c>
+      <c r="L33" s="498" t="s">
+        <v>339</v>
+      </c>
+      <c r="M33" s="499"/>
+      <c r="N33" s="499"/>
+      <c r="O33" s="500"/>
     </row>
     <row r="34" spans="8:15" x14ac:dyDescent="0.2">
       <c r="H34" s="5" t="s">
+        <v>404</v>
+      </c>
+      <c r="L34" s="501" t="s">
+        <v>345</v>
+      </c>
+      <c r="M34" s="502"/>
+      <c r="N34" s="502"/>
+      <c r="O34" s="503"/>
+    </row>
+    <row r="35" spans="8:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H35" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="I35" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="J35" s="5" t="s">
+        <v>436</v>
+      </c>
+      <c r="K35" s="5" t="s">
+        <v>437</v>
+      </c>
+      <c r="L35" s="202">
+        <v>2400</v>
+      </c>
+      <c r="M35" s="202">
+        <v>2400</v>
+      </c>
+      <c r="N35" s="202">
+        <v>2400</v>
+      </c>
+      <c r="O35" s="202">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="36" spans="8:15" x14ac:dyDescent="0.2">
+      <c r="H36" s="5" t="s">
         <v>789</v>
       </c>
-      <c r="I34" s="5" t="s">
+      <c r="I36" s="5" t="s">
         <v>446</v>
       </c>
-      <c r="J34" s="5" t="s">
+      <c r="J36" s="5" t="s">
         <v>436</v>
       </c>
-      <c r="K34" s="5" t="s">
+      <c r="K36" s="5" t="s">
         <v>438</v>
-      </c>
-      <c r="L34" s="205">
-        <v>175</v>
-      </c>
-      <c r="M34" s="205">
-        <v>175</v>
-      </c>
-      <c r="N34" s="205">
-        <v>175</v>
-      </c>
-      <c r="O34" s="205">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="35" spans="8:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J35" s="5" t="s">
-        <v>764</v>
-      </c>
-      <c r="L35" s="207">
-        <v>175</v>
-      </c>
-      <c r="M35" s="207">
-        <v>175</v>
-      </c>
-      <c r="N35" s="207">
-        <v>175</v>
-      </c>
-      <c r="O35" s="207">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="36" spans="8:15" x14ac:dyDescent="0.2">
-      <c r="J36" s="5" t="s">
-        <v>760</v>
       </c>
       <c r="L36" s="205">
         <v>175</v>
@@ -36312,144 +36317,178 @@
       </c>
     </row>
     <row r="37" spans="8:15" x14ac:dyDescent="0.2">
-      <c r="H37" s="5" t="s">
-        <v>790</v>
-      </c>
-      <c r="I37" s="5" t="s">
-        <v>447</v>
-      </c>
       <c r="J37" s="5" t="s">
-        <v>436</v>
-      </c>
-      <c r="K37" s="5" t="s">
-        <v>439</v>
+        <v>764</v>
       </c>
       <c r="L37" s="207">
-        <v>251</v>
+        <v>175</v>
       </c>
       <c r="M37" s="207">
-        <v>251</v>
+        <v>175</v>
       </c>
       <c r="N37" s="207">
-        <v>251</v>
+        <v>175</v>
       </c>
       <c r="O37" s="207">
-        <v>251</v>
+        <v>175</v>
       </c>
     </row>
     <row r="38" spans="8:15" x14ac:dyDescent="0.2">
-      <c r="H38" s="5" t="s">
-        <v>791</v>
-      </c>
-      <c r="I38" s="5" t="s">
-        <v>448</v>
-      </c>
       <c r="J38" s="5" t="s">
-        <v>436</v>
-      </c>
-      <c r="K38" s="5" t="s">
-        <v>440</v>
+        <v>760</v>
       </c>
       <c r="L38" s="205">
-        <v>214</v>
+        <v>175</v>
       </c>
       <c r="M38" s="205">
-        <v>214</v>
+        <v>175</v>
       </c>
       <c r="N38" s="205">
-        <v>214</v>
+        <v>175</v>
       </c>
       <c r="O38" s="205">
-        <v>214</v>
+        <v>175</v>
       </c>
     </row>
     <row r="39" spans="8:15" x14ac:dyDescent="0.2">
       <c r="H39" s="5" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="I39" s="5" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="J39" s="5" t="s">
         <v>436</v>
       </c>
       <c r="K39" s="5" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="L39" s="207">
-        <v>191</v>
+        <v>251</v>
       </c>
       <c r="M39" s="207">
-        <v>191</v>
+        <v>251</v>
       </c>
       <c r="N39" s="207">
-        <v>191</v>
+        <v>251</v>
       </c>
       <c r="O39" s="207">
-        <v>191</v>
+        <v>251</v>
       </c>
     </row>
     <row r="40" spans="8:15" x14ac:dyDescent="0.2">
       <c r="H40" s="5" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="J40" s="5" t="s">
         <v>436</v>
       </c>
       <c r="K40" s="5" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="L40" s="205">
-        <v>5000</v>
+        <v>214</v>
       </c>
       <c r="M40" s="205">
-        <v>5000</v>
+        <v>214</v>
       </c>
       <c r="N40" s="205">
-        <v>5000</v>
+        <v>214</v>
       </c>
       <c r="O40" s="205">
-        <v>5000</v>
+        <v>214</v>
       </c>
     </row>
     <row r="41" spans="8:15" x14ac:dyDescent="0.2">
       <c r="H41" s="5" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="I41" s="5" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="J41" s="5" t="s">
         <v>436</v>
       </c>
       <c r="K41" s="5" t="s">
+        <v>441</v>
+      </c>
+      <c r="L41" s="207">
+        <v>191</v>
+      </c>
+      <c r="M41" s="207">
+        <v>191</v>
+      </c>
+      <c r="N41" s="207">
+        <v>191</v>
+      </c>
+      <c r="O41" s="207">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="42" spans="8:15" x14ac:dyDescent="0.2">
+      <c r="H42" s="5" t="s">
+        <v>793</v>
+      </c>
+      <c r="I42" s="5" t="s">
+        <v>450</v>
+      </c>
+      <c r="J42" s="5" t="s">
+        <v>436</v>
+      </c>
+      <c r="K42" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="L42" s="205">
+        <v>5000</v>
+      </c>
+      <c r="M42" s="205">
+        <v>5000</v>
+      </c>
+      <c r="N42" s="205">
+        <v>5000</v>
+      </c>
+      <c r="O42" s="205">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="43" spans="8:15" x14ac:dyDescent="0.2">
+      <c r="H43" s="5" t="s">
+        <v>794</v>
+      </c>
+      <c r="I43" s="5" t="s">
+        <v>451</v>
+      </c>
+      <c r="J43" s="5" t="s">
+        <v>436</v>
+      </c>
+      <c r="K43" s="5" t="s">
         <v>443</v>
       </c>
-      <c r="L41" s="209">
+      <c r="L43" s="209">
         <v>5000</v>
       </c>
-      <c r="M41" s="209">
+      <c r="M43" s="209">
         <v>5000</v>
       </c>
-      <c r="N41" s="209">
+      <c r="N43" s="209">
         <v>5000</v>
       </c>
-      <c r="O41" s="209">
+      <c r="O43" s="209">
         <v>5000</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="L32:O32"/>
-    <mergeCell ref="L31:O31"/>
+    <mergeCell ref="L34:O34"/>
+    <mergeCell ref="L33:O33"/>
     <mergeCell ref="R18:S22"/>
     <mergeCell ref="L5:O5"/>
     <mergeCell ref="L6:O6"/>
   </mergeCells>
-  <conditionalFormatting sqref="I19:I26">
+  <conditionalFormatting sqref="I19:I28">
     <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="between">
       <formula>0.000000001</formula>
       <formula>1</formula>
@@ -36468,10 +36507,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAFF4867-10C8-4ED5-9BE1-6E89AAC9887A}">
   <dimension ref="C2:Z347"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Q19" sqref="Q19"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -38596,10 +38632,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E2D0172-8312-40B1-9B5A-8DF7E42AC88D}">
   <dimension ref="A1:AS91"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -47200,9 +47233,6 @@
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="1">
-      <selection activeCell="C30" sqref="C30"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
Use Det commodities instead of Att in the input table with detached technologies
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_RSD.xlsx
+++ b/SubRES_TMPL/SubRes_RSD.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF652C77-F333-44A4-9D61-A75D56752D33}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83529AB5-6210-4925-9568-D4A6A371E194}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{34F9D92C-266F-476D-89E0-63153305AC39}"/>
+    <workbookView xWindow="-3233" yWindow="8002" windowWidth="20716" windowHeight="13276" activeTab="4" xr2:uid="{34F9D92C-266F-476D-89E0-63153305AC39}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="34" r:id="rId1"/>
@@ -8419,7 +8419,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3461" uniqueCount="1035">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3461" uniqueCount="1047">
   <si>
     <t>Document type:</t>
   </si>
@@ -11545,6 +11545,42 @@
   </si>
   <si>
     <t>Residential Cooking - LPG - New</t>
+  </si>
+  <si>
+    <t>CEFF~RSDSH_Det</t>
+  </si>
+  <si>
+    <t>CEFF~RSDSH_Det~2030</t>
+  </si>
+  <si>
+    <t>CEFF~RSDSH_Det~2040</t>
+  </si>
+  <si>
+    <t>CEFF~RSDSH_Det~2050</t>
+  </si>
+  <si>
+    <t>CEFF~RSDSC_Det</t>
+  </si>
+  <si>
+    <t>CEFF~RSDSC_Det~2030</t>
+  </si>
+  <si>
+    <t>CEFF~RSDSC_Det~2040</t>
+  </si>
+  <si>
+    <t>CEFF~RSDSC_Det~2050</t>
+  </si>
+  <si>
+    <t>CEFF~RSDWH_Det</t>
+  </si>
+  <si>
+    <t>CEFF~RSDWH_Det~2030</t>
+  </si>
+  <si>
+    <t>CEFF~RSDWH_Det~2040</t>
+  </si>
+  <si>
+    <t>CEFF~RSDWH_Det~2050</t>
   </si>
 </sst>
 </file>
@@ -14048,6 +14084,15 @@
     <xf numFmtId="0" fontId="16" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -14057,22 +14102,13 @@
     <xf numFmtId="0" fontId="16" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="62" fillId="31" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="62" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="62" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="62" fillId="31" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="62" fillId="31" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -24709,8 +24745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{104F8057-C735-4662-BAA6-EEDCF7B57273}">
   <dimension ref="A2:AO162"/>
   <sheetViews>
-    <sheetView topLeftCell="D23" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -24865,28 +24901,28 @@
       <c r="F4" s="63" t="s">
         <v>334</v>
       </c>
-      <c r="G4" s="504" t="s">
+      <c r="G4" s="507" t="s">
         <v>758</v>
       </c>
-      <c r="H4" s="505"/>
-      <c r="I4" s="505"/>
-      <c r="J4" s="506"/>
-      <c r="K4" s="504" t="s">
+      <c r="H4" s="508"/>
+      <c r="I4" s="508"/>
+      <c r="J4" s="509"/>
+      <c r="K4" s="507" t="s">
         <v>336</v>
       </c>
-      <c r="L4" s="505"/>
-      <c r="M4" s="505"/>
-      <c r="N4" s="506"/>
-      <c r="O4" s="504" t="s">
+      <c r="L4" s="508"/>
+      <c r="M4" s="508"/>
+      <c r="N4" s="509"/>
+      <c r="O4" s="507" t="s">
         <v>337</v>
       </c>
-      <c r="P4" s="505"/>
-      <c r="Q4" s="505"/>
-      <c r="R4" s="506"/>
-      <c r="S4" s="504" t="s">
+      <c r="P4" s="508"/>
+      <c r="Q4" s="508"/>
+      <c r="R4" s="509"/>
+      <c r="S4" s="507" t="s">
         <v>338</v>
       </c>
-      <c r="T4" s="506"/>
+      <c r="T4" s="509"/>
       <c r="U4" s="498" t="s">
         <v>339</v>
       </c>
@@ -24924,7 +24960,7 @@
       <c r="AN4" s="57"/>
       <c r="AO4" s="57"/>
     </row>
-    <row r="5" spans="3:41" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C5" s="61" t="s">
         <v>781</v>
       </c>
@@ -27758,28 +27794,28 @@
       <c r="F42" s="63" t="s">
         <v>334</v>
       </c>
-      <c r="G42" s="504" t="s">
+      <c r="G42" s="507" t="s">
         <v>335</v>
       </c>
-      <c r="H42" s="505"/>
-      <c r="I42" s="505"/>
-      <c r="J42" s="506"/>
-      <c r="K42" s="504" t="s">
+      <c r="H42" s="508"/>
+      <c r="I42" s="508"/>
+      <c r="J42" s="509"/>
+      <c r="K42" s="507" t="s">
         <v>336</v>
       </c>
-      <c r="L42" s="505"/>
-      <c r="M42" s="505"/>
-      <c r="N42" s="506"/>
-      <c r="O42" s="504" t="s">
+      <c r="L42" s="508"/>
+      <c r="M42" s="508"/>
+      <c r="N42" s="509"/>
+      <c r="O42" s="507" t="s">
         <v>337</v>
       </c>
-      <c r="P42" s="505"/>
-      <c r="Q42" s="505"/>
-      <c r="R42" s="506"/>
-      <c r="S42" s="504" t="s">
+      <c r="P42" s="508"/>
+      <c r="Q42" s="508"/>
+      <c r="R42" s="509"/>
+      <c r="S42" s="507" t="s">
         <v>338</v>
       </c>
-      <c r="T42" s="506"/>
+      <c r="T42" s="509"/>
       <c r="U42" s="498" t="s">
         <v>339</v>
       </c>
@@ -27817,7 +27853,7 @@
       <c r="AN42" s="57"/>
       <c r="AO42" s="57"/>
     </row>
-    <row r="43" spans="3:41" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C43" s="61" t="s">
         <v>783</v>
       </c>
@@ -27898,16 +27934,16 @@
       <c r="P44" s="502"/>
       <c r="Q44" s="502"/>
       <c r="R44" s="503"/>
-      <c r="S44" s="507" t="s">
+      <c r="S44" s="504" t="s">
         <v>312</v>
       </c>
-      <c r="T44" s="508"/>
-      <c r="U44" s="507" t="s">
+      <c r="T44" s="505"/>
+      <c r="U44" s="504" t="s">
         <v>1007</v>
       </c>
-      <c r="V44" s="509"/>
-      <c r="W44" s="509"/>
-      <c r="X44" s="508"/>
+      <c r="V44" s="506"/>
+      <c r="W44" s="506"/>
+      <c r="X44" s="505"/>
       <c r="Y44" s="475" t="s">
         <v>1019</v>
       </c>
@@ -31199,40 +31235,40 @@
         <v>41</v>
       </c>
       <c r="G87" s="64" t="s">
-        <v>682</v>
+        <v>1035</v>
       </c>
       <c r="H87" s="64" t="s">
-        <v>683</v>
+        <v>1036</v>
       </c>
       <c r="I87" s="64" t="s">
-        <v>684</v>
+        <v>1037</v>
       </c>
       <c r="J87" s="64" t="s">
-        <v>685</v>
+        <v>1038</v>
       </c>
       <c r="K87" s="64" t="s">
-        <v>686</v>
+        <v>1039</v>
       </c>
       <c r="L87" s="64" t="s">
-        <v>687</v>
+        <v>1040</v>
       </c>
       <c r="M87" s="64" t="s">
-        <v>688</v>
+        <v>1041</v>
       </c>
       <c r="N87" s="64" t="s">
-        <v>689</v>
+        <v>1042</v>
       </c>
       <c r="O87" s="64" t="s">
-        <v>690</v>
+        <v>1043</v>
       </c>
       <c r="P87" s="64" t="s">
-        <v>691</v>
+        <v>1044</v>
       </c>
       <c r="Q87" s="64" t="s">
-        <v>692</v>
+        <v>1045</v>
       </c>
       <c r="R87" s="64" t="s">
-        <v>693</v>
+        <v>1046</v>
       </c>
       <c r="S87" s="65" t="s">
         <v>43</v>
@@ -31293,28 +31329,28 @@
       <c r="F88" s="63" t="s">
         <v>334</v>
       </c>
-      <c r="G88" s="504" t="s">
+      <c r="G88" s="507" t="s">
         <v>335</v>
       </c>
-      <c r="H88" s="505"/>
-      <c r="I88" s="505"/>
-      <c r="J88" s="506"/>
-      <c r="K88" s="504" t="s">
+      <c r="H88" s="508"/>
+      <c r="I88" s="508"/>
+      <c r="J88" s="509"/>
+      <c r="K88" s="507" t="s">
         <v>336</v>
       </c>
-      <c r="L88" s="505"/>
-      <c r="M88" s="505"/>
-      <c r="N88" s="506"/>
-      <c r="O88" s="504" t="s">
+      <c r="L88" s="508"/>
+      <c r="M88" s="508"/>
+      <c r="N88" s="509"/>
+      <c r="O88" s="507" t="s">
         <v>337</v>
       </c>
-      <c r="P88" s="505"/>
-      <c r="Q88" s="505"/>
-      <c r="R88" s="506"/>
-      <c r="S88" s="504" t="s">
+      <c r="P88" s="508"/>
+      <c r="Q88" s="508"/>
+      <c r="R88" s="509"/>
+      <c r="S88" s="507" t="s">
         <v>338</v>
       </c>
-      <c r="T88" s="506"/>
+      <c r="T88" s="509"/>
       <c r="U88" s="498" t="s">
         <v>339</v>
       </c>
@@ -31352,7 +31388,7 @@
       <c r="AN88" s="57"/>
       <c r="AO88" s="57"/>
     </row>
-    <row r="89" spans="3:41" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="3:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C89" s="61" t="s">
         <v>783</v>
       </c>
@@ -31433,16 +31469,16 @@
       <c r="P90" s="502"/>
       <c r="Q90" s="502"/>
       <c r="R90" s="503"/>
-      <c r="S90" s="507" t="s">
+      <c r="S90" s="504" t="s">
         <v>312</v>
       </c>
-      <c r="T90" s="508"/>
-      <c r="U90" s="507" t="s">
+      <c r="T90" s="505"/>
+      <c r="U90" s="504" t="s">
         <v>1007</v>
       </c>
-      <c r="V90" s="509"/>
-      <c r="W90" s="509"/>
-      <c r="X90" s="508"/>
+      <c r="V90" s="506"/>
+      <c r="W90" s="506"/>
+      <c r="X90" s="505"/>
       <c r="Y90" s="475" t="s">
         <v>1019</v>
       </c>
@@ -35144,26 +35180,6 @@
     <row r="162" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="G90:J90"/>
-    <mergeCell ref="K90:N90"/>
-    <mergeCell ref="O90:R90"/>
-    <mergeCell ref="S90:T90"/>
-    <mergeCell ref="U90:X90"/>
-    <mergeCell ref="G88:J88"/>
-    <mergeCell ref="K88:N88"/>
-    <mergeCell ref="O88:R88"/>
-    <mergeCell ref="S88:T88"/>
-    <mergeCell ref="U88:X88"/>
-    <mergeCell ref="G44:J44"/>
-    <mergeCell ref="K44:N44"/>
-    <mergeCell ref="O44:R44"/>
-    <mergeCell ref="S44:T44"/>
-    <mergeCell ref="U44:X44"/>
-    <mergeCell ref="G42:J42"/>
-    <mergeCell ref="K42:N42"/>
-    <mergeCell ref="O42:R42"/>
-    <mergeCell ref="S42:T42"/>
-    <mergeCell ref="U42:X42"/>
     <mergeCell ref="U4:X4"/>
     <mergeCell ref="U6:X6"/>
     <mergeCell ref="G4:J4"/>
@@ -35174,6 +35190,26 @@
     <mergeCell ref="O6:R6"/>
     <mergeCell ref="K6:N6"/>
     <mergeCell ref="G6:J6"/>
+    <mergeCell ref="G42:J42"/>
+    <mergeCell ref="K42:N42"/>
+    <mergeCell ref="O42:R42"/>
+    <mergeCell ref="S42:T42"/>
+    <mergeCell ref="U42:X42"/>
+    <mergeCell ref="G44:J44"/>
+    <mergeCell ref="K44:N44"/>
+    <mergeCell ref="O44:R44"/>
+    <mergeCell ref="S44:T44"/>
+    <mergeCell ref="U44:X44"/>
+    <mergeCell ref="G88:J88"/>
+    <mergeCell ref="K88:N88"/>
+    <mergeCell ref="O88:R88"/>
+    <mergeCell ref="S88:T88"/>
+    <mergeCell ref="U88:X88"/>
+    <mergeCell ref="G90:J90"/>
+    <mergeCell ref="K90:N90"/>
+    <mergeCell ref="O90:R90"/>
+    <mergeCell ref="S90:T90"/>
+    <mergeCell ref="U90:X90"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -35187,7 +35223,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CED359C-4B42-41C8-A7E8-4F6FC9AE57D2}">
   <dimension ref="C2:W43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
@@ -35349,12 +35385,12 @@
       <c r="I6" s="84"/>
       <c r="J6" s="84"/>
       <c r="K6" s="84"/>
-      <c r="L6" s="507" t="s">
+      <c r="L6" s="504" t="s">
         <v>1007</v>
       </c>
-      <c r="M6" s="509"/>
-      <c r="N6" s="509"/>
-      <c r="O6" s="508"/>
+      <c r="M6" s="506"/>
+      <c r="N6" s="506"/>
+      <c r="O6" s="505"/>
       <c r="P6" s="475" t="s">
         <v>1019</v>
       </c>
@@ -35408,19 +35444,19 @@
         <v>0.85</v>
       </c>
       <c r="L7" s="358">
-        <f>L35/$V7/1000</f>
+        <f t="shared" ref="L7:O13" si="0">L35/$V7/1000</f>
         <v>0.432</v>
       </c>
       <c r="M7" s="358">
-        <f>M35/$V7/1000</f>
+        <f t="shared" si="0"/>
         <v>0.432</v>
       </c>
       <c r="N7" s="358">
-        <f>N35/$V7/1000</f>
+        <f t="shared" si="0"/>
         <v>0.432</v>
       </c>
       <c r="O7" s="358">
-        <f>O35/$V7/1000</f>
+        <f t="shared" si="0"/>
         <v>0.432</v>
       </c>
       <c r="P7" s="212"/>
@@ -35439,7 +35475,7 @@
         <v>5.5555555555555554</v>
       </c>
       <c r="W7" s="287">
-        <f>L35/V7</f>
+        <f t="shared" ref="W7:W13" si="1">L35/V7</f>
         <v>432</v>
       </c>
     </row>
@@ -35474,19 +35510,19 @@
         <v>0.8</v>
       </c>
       <c r="L8" s="359">
-        <f>L36/$V8/1000</f>
+        <f t="shared" si="0"/>
         <v>0.61250000000000004</v>
       </c>
       <c r="M8" s="359">
-        <f>M36/$V8/1000</f>
+        <f t="shared" si="0"/>
         <v>0.61250000000000004</v>
       </c>
       <c r="N8" s="359">
-        <f>N36/$V8/1000</f>
+        <f t="shared" si="0"/>
         <v>0.61250000000000004</v>
       </c>
       <c r="O8" s="359">
-        <f>O36/$V8/1000</f>
+        <f t="shared" si="0"/>
         <v>0.61250000000000004</v>
       </c>
       <c r="P8" s="213"/>
@@ -35501,21 +35537,21 @@
         <v>3.5</v>
       </c>
       <c r="V8" s="287">
-        <f t="shared" ref="V8:V13" si="0">1/U8</f>
+        <f t="shared" ref="V8:V13" si="2">1/U8</f>
         <v>0.2857142857142857</v>
       </c>
       <c r="W8" s="287">
-        <f>L36/V8</f>
+        <f t="shared" si="1"/>
         <v>612.5</v>
       </c>
     </row>
     <row r="9" spans="3:23" x14ac:dyDescent="0.2">
       <c r="C9" s="205" t="str">
-        <f t="shared" ref="C9:C10" si="1">D22</f>
+        <f t="shared" ref="C9:C10" si="3">D22</f>
         <v>R-RSDCK_GAS_N1</v>
       </c>
       <c r="D9" s="196" t="str">
-        <f t="shared" ref="D9:D10" si="2">LEFT($E$21,20)&amp;"_"&amp;RIGHT(E9,3)&amp;" - New"</f>
+        <f t="shared" ref="D9:D10" si="4">LEFT($E$21,20)&amp;"_"&amp;RIGHT(E9,3)&amp;" - New"</f>
         <v>Residential Cooking _GAS - New</v>
       </c>
       <c r="E9" s="196" t="s">
@@ -35540,19 +35576,19 @@
         <v>0.68</v>
       </c>
       <c r="L9" s="360">
-        <f>L37/$V9/1000</f>
+        <f t="shared" si="0"/>
         <v>0.61250000000000004</v>
       </c>
       <c r="M9" s="360">
-        <f>M37/$V9/1000</f>
+        <f t="shared" si="0"/>
         <v>0.61250000000000004</v>
       </c>
       <c r="N9" s="360">
-        <f>N37/$V9/1000</f>
+        <f t="shared" si="0"/>
         <v>0.61250000000000004</v>
       </c>
       <c r="O9" s="360">
-        <f>O37/$V9/1000</f>
+        <f t="shared" si="0"/>
         <v>0.61250000000000004</v>
       </c>
       <c r="P9" s="214"/>
@@ -35567,21 +35603,21 @@
         <v>3.5</v>
       </c>
       <c r="V9" s="287">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.2857142857142857</v>
       </c>
       <c r="W9" s="287">
-        <f>L37/V9</f>
+        <f t="shared" si="1"/>
         <v>612.5</v>
       </c>
     </row>
     <row r="10" spans="3:23" x14ac:dyDescent="0.2">
       <c r="C10" s="205" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>R-RSDCK_LPG_N1</v>
       </c>
       <c r="D10" s="195" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>Residential Cooking _LPG - New</v>
       </c>
       <c r="E10" s="195" t="s">
@@ -35606,19 +35642,19 @@
         <v>0.68</v>
       </c>
       <c r="L10" s="359">
-        <f>L38/$V10/1000</f>
+        <f t="shared" si="0"/>
         <v>0.61250000000000004</v>
       </c>
       <c r="M10" s="359">
-        <f>M38/$V10/1000</f>
+        <f t="shared" si="0"/>
         <v>0.61250000000000004</v>
       </c>
       <c r="N10" s="359">
-        <f>N38/$V10/1000</f>
+        <f t="shared" si="0"/>
         <v>0.61250000000000004</v>
       </c>
       <c r="O10" s="359">
-        <f>O38/$V10/1000</f>
+        <f t="shared" si="0"/>
         <v>0.61250000000000004</v>
       </c>
       <c r="P10" s="213"/>
@@ -35633,21 +35669,21 @@
         <v>3.5</v>
       </c>
       <c r="V10" s="287">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.2857142857142857</v>
       </c>
       <c r="W10" s="287">
-        <f>L38/V10</f>
+        <f t="shared" si="1"/>
         <v>612.5</v>
       </c>
     </row>
     <row r="11" spans="3:23" x14ac:dyDescent="0.2">
       <c r="C11" s="207" t="str">
-        <f>D24</f>
+        <f t="shared" ref="C11:D15" si="5">D24</f>
         <v>R-RSDCW_N1</v>
       </c>
       <c r="D11" s="196" t="str">
-        <f>E24</f>
+        <f t="shared" si="5"/>
         <v>Residential Cloth Washing demand - New</v>
       </c>
       <c r="E11" s="196" t="s">
@@ -35672,19 +35708,19 @@
         <v>0.7</v>
       </c>
       <c r="L11" s="360">
-        <f>L39/$V11/1000</f>
+        <f t="shared" si="0"/>
         <v>0.55220000000000002</v>
       </c>
       <c r="M11" s="360">
-        <f>M39/$V11/1000</f>
+        <f t="shared" si="0"/>
         <v>0.55220000000000002</v>
       </c>
       <c r="N11" s="360">
-        <f>N39/$V11/1000</f>
+        <f t="shared" si="0"/>
         <v>0.55220000000000002</v>
       </c>
       <c r="O11" s="360">
-        <f>O39/$V11/1000</f>
+        <f t="shared" si="0"/>
         <v>0.55220000000000002</v>
       </c>
       <c r="P11" s="214"/>
@@ -35699,21 +35735,21 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="V11" s="287">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.45454545454545453</v>
       </c>
       <c r="W11" s="287">
-        <f>L39/V11</f>
+        <f t="shared" si="1"/>
         <v>552.20000000000005</v>
       </c>
     </row>
     <row r="12" spans="3:23" x14ac:dyDescent="0.2">
       <c r="C12" s="205" t="str">
-        <f>D25</f>
+        <f t="shared" si="5"/>
         <v>R-RSDCD_N1</v>
       </c>
       <c r="D12" s="195" t="str">
-        <f>E25</f>
+        <f t="shared" si="5"/>
         <v>Residential Cloth Drying demand - New</v>
       </c>
       <c r="E12" s="195" t="s">
@@ -35738,19 +35774,19 @@
         <v>0.6</v>
       </c>
       <c r="L12" s="359">
-        <f>L40/$V12/1000</f>
+        <f t="shared" si="0"/>
         <v>0.53500000000000003</v>
       </c>
       <c r="M12" s="359">
-        <f>M40/$V12/1000</f>
+        <f t="shared" si="0"/>
         <v>0.53500000000000003</v>
       </c>
       <c r="N12" s="359">
-        <f>N40/$V12/1000</f>
+        <f t="shared" si="0"/>
         <v>0.53500000000000003</v>
       </c>
       <c r="O12" s="359">
-        <f>O40/$V12/1000</f>
+        <f t="shared" si="0"/>
         <v>0.53500000000000003</v>
       </c>
       <c r="P12" s="213"/>
@@ -35765,21 +35801,21 @@
         <v>2.5</v>
       </c>
       <c r="V12" s="287">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.4</v>
       </c>
       <c r="W12" s="287">
-        <f>L40/V12</f>
+        <f t="shared" si="1"/>
         <v>535</v>
       </c>
     </row>
     <row r="13" spans="3:23" x14ac:dyDescent="0.2">
       <c r="C13" s="207" t="str">
-        <f>D26</f>
+        <f t="shared" si="5"/>
         <v>R-RSDDW_N1</v>
       </c>
       <c r="D13" s="196" t="str">
-        <f>E26</f>
+        <f t="shared" si="5"/>
         <v>Residential Dish Washing demand - New</v>
       </c>
       <c r="E13" s="196" t="s">
@@ -35804,19 +35840,19 @@
         <v>0.7</v>
       </c>
       <c r="L13" s="360">
-        <f>L41/$V13/1000</f>
+        <f t="shared" si="0"/>
         <v>0.42019999999999996</v>
       </c>
       <c r="M13" s="360">
-        <f>M41/$V13/1000</f>
+        <f t="shared" si="0"/>
         <v>0.42019999999999996</v>
       </c>
       <c r="N13" s="360">
-        <f>N41/$V13/1000</f>
+        <f t="shared" si="0"/>
         <v>0.42019999999999996</v>
       </c>
       <c r="O13" s="360">
-        <f>O41/$V13/1000</f>
+        <f t="shared" si="0"/>
         <v>0.42019999999999996</v>
       </c>
       <c r="P13" s="214"/>
@@ -35831,21 +35867,21 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="V13" s="287">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.45454545454545453</v>
       </c>
       <c r="W13" s="287">
-        <f>L41/V13</f>
+        <f t="shared" si="1"/>
         <v>420.2</v>
       </c>
     </row>
     <row r="14" spans="3:23" x14ac:dyDescent="0.2">
       <c r="C14" s="205" t="str">
-        <f>D27</f>
+        <f t="shared" si="5"/>
         <v>R-RSDOE_N1</v>
       </c>
       <c r="D14" s="195" t="str">
-        <f>E27</f>
+        <f t="shared" si="5"/>
         <v>Residential ELC Appliances - New</v>
       </c>
       <c r="E14" s="195" t="s">
@@ -35896,11 +35932,11 @@
     </row>
     <row r="15" spans="3:23" x14ac:dyDescent="0.2">
       <c r="C15" s="207" t="str">
-        <f>D28</f>
+        <f t="shared" si="5"/>
         <v>R-RSDOA_N1</v>
       </c>
       <c r="D15" s="196" t="str">
-        <f>E28</f>
+        <f t="shared" si="5"/>
         <v>Residential Other Applications - New</v>
       </c>
       <c r="E15" s="196" t="s">
@@ -36054,7 +36090,7 @@
         <v>48</v>
       </c>
       <c r="D22" s="173" t="str">
-        <f t="shared" ref="D22:D23" si="3">_xlfn.TEXTJOIN("_",TRUE,"R-RSDCK",RIGHT(E9,3),"N1")</f>
+        <f t="shared" ref="D22:D23" si="6">_xlfn.TEXTJOIN("_",TRUE,"R-RSDCK",RIGHT(E9,3),"N1")</f>
         <v>R-RSDCK_GAS_N1</v>
       </c>
       <c r="E22" s="173" t="s">
@@ -36079,7 +36115,7 @@
         <v>48</v>
       </c>
       <c r="D23" s="173" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>R-RSDCK_LPG_N1</v>
       </c>
       <c r="E23" s="173" t="s">
@@ -47644,103 +47680,103 @@
       <c r="C4" s="381" t="s">
         <v>805</v>
       </c>
-      <c r="D4" s="511" t="s">
+      <c r="D4" s="512" t="s">
         <v>806</v>
       </c>
-      <c r="E4" s="512"/>
-      <c r="F4" s="512"/>
-      <c r="G4" s="512"/>
+      <c r="E4" s="511"/>
+      <c r="F4" s="511"/>
+      <c r="G4" s="511"/>
       <c r="H4" s="513"/>
-      <c r="I4" s="512" t="s">
+      <c r="I4" s="511" t="s">
         <v>807</v>
       </c>
-      <c r="J4" s="512"/>
-      <c r="K4" s="512"/>
-      <c r="L4" s="512"/>
+      <c r="J4" s="511"/>
+      <c r="K4" s="511"/>
+      <c r="L4" s="511"/>
       <c r="M4" s="513"/>
-      <c r="N4" s="512" t="s">
+      <c r="N4" s="511" t="s">
         <v>808</v>
       </c>
-      <c r="O4" s="512"/>
-      <c r="P4" s="512"/>
-      <c r="Q4" s="512"/>
+      <c r="O4" s="511"/>
+      <c r="P4" s="511"/>
+      <c r="Q4" s="511"/>
       <c r="R4" s="513"/>
-      <c r="S4" s="512" t="s">
+      <c r="S4" s="511" t="s">
         <v>809</v>
       </c>
-      <c r="T4" s="512"/>
-      <c r="U4" s="512"/>
-      <c r="V4" s="512"/>
+      <c r="T4" s="511"/>
+      <c r="U4" s="511"/>
+      <c r="V4" s="511"/>
       <c r="W4" s="513"/>
-      <c r="X4" s="512" t="s">
+      <c r="X4" s="511" t="s">
         <v>810</v>
       </c>
-      <c r="Y4" s="512"/>
-      <c r="Z4" s="512"/>
-      <c r="AA4" s="512"/>
+      <c r="Y4" s="511"/>
+      <c r="Z4" s="511"/>
+      <c r="AA4" s="511"/>
       <c r="AB4" s="513"/>
-      <c r="AC4" s="512" t="s">
+      <c r="AC4" s="511" t="s">
         <v>811</v>
       </c>
-      <c r="AD4" s="512"/>
-      <c r="AE4" s="512"/>
-      <c r="AF4" s="512"/>
+      <c r="AD4" s="511"/>
+      <c r="AE4" s="511"/>
+      <c r="AF4" s="511"/>
       <c r="AG4" s="513"/>
-      <c r="AH4" s="512" t="s">
+      <c r="AH4" s="511" t="s">
         <v>812</v>
       </c>
-      <c r="AI4" s="512"/>
-      <c r="AJ4" s="512"/>
-      <c r="AK4" s="512"/>
+      <c r="AI4" s="511"/>
+      <c r="AJ4" s="511"/>
+      <c r="AK4" s="511"/>
       <c r="AL4" s="513"/>
-      <c r="AM4" s="512" t="s">
+      <c r="AM4" s="511" t="s">
         <v>813</v>
       </c>
-      <c r="AN4" s="512"/>
-      <c r="AO4" s="512"/>
-      <c r="AP4" s="512"/>
+      <c r="AN4" s="511"/>
+      <c r="AO4" s="511"/>
+      <c r="AP4" s="511"/>
       <c r="AQ4" s="513"/>
-      <c r="AR4" s="512" t="s">
+      <c r="AR4" s="511" t="s">
         <v>814</v>
       </c>
-      <c r="AS4" s="512"/>
-      <c r="AT4" s="512"/>
-      <c r="AU4" s="512"/>
+      <c r="AS4" s="511"/>
+      <c r="AT4" s="511"/>
+      <c r="AU4" s="511"/>
       <c r="AV4" s="513"/>
-      <c r="AW4" s="512" t="s">
+      <c r="AW4" s="511" t="s">
         <v>815</v>
       </c>
-      <c r="AX4" s="512"/>
-      <c r="AY4" s="512"/>
-      <c r="AZ4" s="512"/>
-      <c r="BA4" s="512"/>
-      <c r="BB4" s="511" t="s">
+      <c r="AX4" s="511"/>
+      <c r="AY4" s="511"/>
+      <c r="AZ4" s="511"/>
+      <c r="BA4" s="511"/>
+      <c r="BB4" s="512" t="s">
         <v>816</v>
       </c>
-      <c r="BC4" s="512"/>
-      <c r="BD4" s="512"/>
-      <c r="BE4" s="512"/>
+      <c r="BC4" s="511"/>
+      <c r="BD4" s="511"/>
+      <c r="BE4" s="511"/>
       <c r="BF4" s="513"/>
-      <c r="BG4" s="512" t="s">
+      <c r="BG4" s="511" t="s">
         <v>817</v>
       </c>
-      <c r="BH4" s="512"/>
-      <c r="BI4" s="512"/>
-      <c r="BJ4" s="512"/>
-      <c r="BK4" s="512"/>
-      <c r="BL4" s="511" t="s">
+      <c r="BH4" s="511"/>
+      <c r="BI4" s="511"/>
+      <c r="BJ4" s="511"/>
+      <c r="BK4" s="511"/>
+      <c r="BL4" s="512" t="s">
         <v>818</v>
       </c>
-      <c r="BM4" s="512"/>
-      <c r="BN4" s="512"/>
-      <c r="BO4" s="512"/>
-      <c r="BP4" s="512"/>
-      <c r="BQ4" s="511" t="s">
+      <c r="BM4" s="511"/>
+      <c r="BN4" s="511"/>
+      <c r="BO4" s="511"/>
+      <c r="BP4" s="511"/>
+      <c r="BQ4" s="512" t="s">
         <v>819</v>
       </c>
-      <c r="BR4" s="512"/>
-      <c r="BS4" s="512"/>
-      <c r="BT4" s="512"/>
+      <c r="BR4" s="511"/>
+      <c r="BS4" s="511"/>
+      <c r="BT4" s="511"/>
       <c r="BU4" s="513"/>
       <c r="BV4" s="382" t="s">
         <v>820</v>
@@ -61334,6 +61370,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="BL4:BP4"/>
+    <mergeCell ref="BQ4:BU4"/>
+    <mergeCell ref="BW4:CA4"/>
+    <mergeCell ref="CB4:CF4"/>
+    <mergeCell ref="CG4:CK4"/>
     <mergeCell ref="BG4:BK4"/>
     <mergeCell ref="D4:H4"/>
     <mergeCell ref="I4:M4"/>
@@ -61346,11 +61387,6 @@
     <mergeCell ref="AR4:AV4"/>
     <mergeCell ref="AW4:BA4"/>
     <mergeCell ref="BB4:BF4"/>
-    <mergeCell ref="BL4:BP4"/>
-    <mergeCell ref="BQ4:BU4"/>
-    <mergeCell ref="BW4:CA4"/>
-    <mergeCell ref="CB4:CF4"/>
-    <mergeCell ref="CG4:CK4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
Update User Constraints and Debug
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_RSD.xlsx
+++ b/SubRES_TMPL/SubRes_RSD.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83529AB5-6210-4925-9568-D4A6A371E194}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{368500FC-3941-49B5-921B-DC1190A35F03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3233" yWindow="8002" windowWidth="20716" windowHeight="13276" activeTab="4" xr2:uid="{34F9D92C-266F-476D-89E0-63153305AC39}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{34F9D92C-266F-476D-89E0-63153305AC39}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="34" r:id="rId1"/>
@@ -645,7 +645,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Author:</t>
         </r>
@@ -654,7 +654,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Used units/kW of a fridge just to have something
@@ -11599,7 +11599,7 @@
     <numFmt numFmtId="171" formatCode="#,##0.000"/>
     <numFmt numFmtId="172" formatCode="0.000"/>
   </numFmts>
-  <fonts count="71" x14ac:knownFonts="1">
+  <fonts count="69" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -11957,21 +11957,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -13053,7 +13041,7 @@
     <xf numFmtId="168" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="39" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="56" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="54" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="517">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -13706,8 +13694,20 @@
     <xf numFmtId="0" fontId="32" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="32" fillId="21" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="32" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -13718,112 +13718,121 @@
     <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="59" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="60" fillId="31" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="31" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="31" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="62" fillId="31" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="62" fillId="31" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="62" fillId="31" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="63" fillId="31" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="61" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="63" fillId="31" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="62" fillId="31" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="63" fillId="31" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="62" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="62" fillId="31" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="62" fillId="31" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="64" fillId="31" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="62" fillId="31" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="64" fillId="31" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="63" fillId="32" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="63" fillId="32" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="63" fillId="32" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="64" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="64" fillId="31" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="64" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="65" fillId="31" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="64" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="64" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="65" fillId="31" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="64" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="65" fillId="31" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="64" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="64" fillId="31" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="64" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="65" fillId="32" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="65" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="65" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="65" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="65" fillId="32" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="65" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="65" fillId="32" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="65" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="66" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="65" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="65" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="65" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="65" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="65" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="66" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="66" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="66" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="66" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="66" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="66" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="66" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="66" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="67" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="67" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="67" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="67" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="67" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="67" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="67" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="67" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="66" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="67" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -13832,171 +13841,150 @@
     <xf numFmtId="3" fontId="67" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="67" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="67" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="3" fontId="68" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="68" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="68" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="66" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="69" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="66" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="69" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="64" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="70" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="64" fillId="9" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="70" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="66" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="68" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="66" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="66" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="66" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="68" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="65" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="66" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="66" fillId="0" borderId="0" xfId="15" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="66" fillId="0" borderId="10" xfId="15" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="66" fillId="0" borderId="25" xfId="15" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="65" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="66" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="66" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="66" fillId="9" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="66" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="68" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="66" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="68" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="68" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="68" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="59" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="67" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="65" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="65" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="66" fillId="0" borderId="0" xfId="15" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="68" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="66" fillId="0" borderId="0" xfId="15" applyFont="1"/>
+    <xf numFmtId="164" fontId="65" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="68" fillId="0" borderId="0" xfId="15" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="68" fillId="0" borderId="10" xfId="15" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="68" fillId="0" borderId="25" xfId="15" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="67" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="65" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="65" fillId="12" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="65" fillId="12" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="68" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="65" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="68" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="65" fillId="12" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="68" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="65" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="61" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="65" fillId="12" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="67" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="65" fillId="12" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="67" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="65" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="68" fillId="0" borderId="0" xfId="15" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="65" fillId="12" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="68" fillId="0" borderId="0" xfId="15" applyFont="1"/>
-    <xf numFmtId="164" fontId="67" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="65" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="65" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="65" fillId="12" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="65" fillId="12" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="67" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="65" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="65" fillId="12" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="65" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="65" fillId="12" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="67" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="67" fillId="12" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="67" fillId="12" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="65" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="67" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="65" fillId="12" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="67" fillId="12" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="67" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="67" fillId="12" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="67" fillId="12" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="67" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="67" fillId="12" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="67" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="67" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="67" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="67" fillId="12" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="67" fillId="12" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="67" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="67" fillId="12" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="67" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="67" fillId="12" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="67" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="67" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="67" fillId="12" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="58" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="56" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="15" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="67" fillId="0" borderId="0" xfId="15" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="65" fillId="0" borderId="0" xfId="15" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="67" fillId="0" borderId="10" xfId="15" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="65" fillId="0" borderId="10" xfId="15" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="68" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="66" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -14084,6 +14072,15 @@
     <xf numFmtId="0" fontId="16" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="23" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -14093,34 +14090,25 @@
     <xf numFmtId="0" fontId="16" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="62" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="60" fillId="31" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="62" fillId="31" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="60" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="62" fillId="31" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="60" fillId="31" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="62" fillId="32" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="60" fillId="32" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="62" fillId="32" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="60" fillId="32" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="62" fillId="32" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="60" fillId="32" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -24745,7 +24733,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{104F8057-C735-4662-BAA6-EEDCF7B57273}">
   <dimension ref="A2:AO162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
@@ -24901,28 +24889,28 @@
       <c r="F4" s="63" t="s">
         <v>334</v>
       </c>
-      <c r="G4" s="507" t="s">
+      <c r="G4" s="504" t="s">
         <v>758</v>
       </c>
-      <c r="H4" s="508"/>
-      <c r="I4" s="508"/>
-      <c r="J4" s="509"/>
-      <c r="K4" s="507" t="s">
+      <c r="H4" s="505"/>
+      <c r="I4" s="505"/>
+      <c r="J4" s="506"/>
+      <c r="K4" s="504" t="s">
         <v>336</v>
       </c>
-      <c r="L4" s="508"/>
-      <c r="M4" s="508"/>
-      <c r="N4" s="509"/>
-      <c r="O4" s="507" t="s">
+      <c r="L4" s="505"/>
+      <c r="M4" s="505"/>
+      <c r="N4" s="506"/>
+      <c r="O4" s="504" t="s">
         <v>337</v>
       </c>
-      <c r="P4" s="508"/>
-      <c r="Q4" s="508"/>
-      <c r="R4" s="509"/>
-      <c r="S4" s="507" t="s">
+      <c r="P4" s="505"/>
+      <c r="Q4" s="505"/>
+      <c r="R4" s="506"/>
+      <c r="S4" s="504" t="s">
         <v>338</v>
       </c>
-      <c r="T4" s="509"/>
+      <c r="T4" s="506"/>
       <c r="U4" s="498" t="s">
         <v>339</v>
       </c>
@@ -27794,28 +27782,28 @@
       <c r="F42" s="63" t="s">
         <v>334</v>
       </c>
-      <c r="G42" s="507" t="s">
+      <c r="G42" s="504" t="s">
         <v>335</v>
       </c>
-      <c r="H42" s="508"/>
-      <c r="I42" s="508"/>
-      <c r="J42" s="509"/>
-      <c r="K42" s="507" t="s">
+      <c r="H42" s="505"/>
+      <c r="I42" s="505"/>
+      <c r="J42" s="506"/>
+      <c r="K42" s="504" t="s">
         <v>336</v>
       </c>
-      <c r="L42" s="508"/>
-      <c r="M42" s="508"/>
-      <c r="N42" s="509"/>
-      <c r="O42" s="507" t="s">
+      <c r="L42" s="505"/>
+      <c r="M42" s="505"/>
+      <c r="N42" s="506"/>
+      <c r="O42" s="504" t="s">
         <v>337</v>
       </c>
-      <c r="P42" s="508"/>
-      <c r="Q42" s="508"/>
-      <c r="R42" s="509"/>
-      <c r="S42" s="507" t="s">
+      <c r="P42" s="505"/>
+      <c r="Q42" s="505"/>
+      <c r="R42" s="506"/>
+      <c r="S42" s="504" t="s">
         <v>338</v>
       </c>
-      <c r="T42" s="509"/>
+      <c r="T42" s="506"/>
       <c r="U42" s="498" t="s">
         <v>339</v>
       </c>
@@ -27934,16 +27922,16 @@
       <c r="P44" s="502"/>
       <c r="Q44" s="502"/>
       <c r="R44" s="503"/>
-      <c r="S44" s="504" t="s">
+      <c r="S44" s="507" t="s">
         <v>312</v>
       </c>
-      <c r="T44" s="505"/>
-      <c r="U44" s="504" t="s">
+      <c r="T44" s="508"/>
+      <c r="U44" s="507" t="s">
         <v>1007</v>
       </c>
-      <c r="V44" s="506"/>
-      <c r="W44" s="506"/>
-      <c r="X44" s="505"/>
+      <c r="V44" s="509"/>
+      <c r="W44" s="509"/>
+      <c r="X44" s="508"/>
       <c r="Y44" s="475" t="s">
         <v>1019</v>
       </c>
@@ -31329,28 +31317,28 @@
       <c r="F88" s="63" t="s">
         <v>334</v>
       </c>
-      <c r="G88" s="507" t="s">
+      <c r="G88" s="504" t="s">
         <v>335</v>
       </c>
-      <c r="H88" s="508"/>
-      <c r="I88" s="508"/>
-      <c r="J88" s="509"/>
-      <c r="K88" s="507" t="s">
+      <c r="H88" s="505"/>
+      <c r="I88" s="505"/>
+      <c r="J88" s="506"/>
+      <c r="K88" s="504" t="s">
         <v>336</v>
       </c>
-      <c r="L88" s="508"/>
-      <c r="M88" s="508"/>
-      <c r="N88" s="509"/>
-      <c r="O88" s="507" t="s">
+      <c r="L88" s="505"/>
+      <c r="M88" s="505"/>
+      <c r="N88" s="506"/>
+      <c r="O88" s="504" t="s">
         <v>337</v>
       </c>
-      <c r="P88" s="508"/>
-      <c r="Q88" s="508"/>
-      <c r="R88" s="509"/>
-      <c r="S88" s="507" t="s">
+      <c r="P88" s="505"/>
+      <c r="Q88" s="505"/>
+      <c r="R88" s="506"/>
+      <c r="S88" s="504" t="s">
         <v>338</v>
       </c>
-      <c r="T88" s="509"/>
+      <c r="T88" s="506"/>
       <c r="U88" s="498" t="s">
         <v>339</v>
       </c>
@@ -31469,16 +31457,16 @@
       <c r="P90" s="502"/>
       <c r="Q90" s="502"/>
       <c r="R90" s="503"/>
-      <c r="S90" s="504" t="s">
+      <c r="S90" s="507" t="s">
         <v>312</v>
       </c>
-      <c r="T90" s="505"/>
-      <c r="U90" s="504" t="s">
+      <c r="T90" s="508"/>
+      <c r="U90" s="507" t="s">
         <v>1007</v>
       </c>
-      <c r="V90" s="506"/>
-      <c r="W90" s="506"/>
-      <c r="X90" s="505"/>
+      <c r="V90" s="509"/>
+      <c r="W90" s="509"/>
+      <c r="X90" s="508"/>
       <c r="Y90" s="475" t="s">
         <v>1019</v>
       </c>
@@ -35180,6 +35168,26 @@
     <row r="162" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="G90:J90"/>
+    <mergeCell ref="K90:N90"/>
+    <mergeCell ref="O90:R90"/>
+    <mergeCell ref="S90:T90"/>
+    <mergeCell ref="U90:X90"/>
+    <mergeCell ref="G88:J88"/>
+    <mergeCell ref="K88:N88"/>
+    <mergeCell ref="O88:R88"/>
+    <mergeCell ref="S88:T88"/>
+    <mergeCell ref="U88:X88"/>
+    <mergeCell ref="G44:J44"/>
+    <mergeCell ref="K44:N44"/>
+    <mergeCell ref="O44:R44"/>
+    <mergeCell ref="S44:T44"/>
+    <mergeCell ref="U44:X44"/>
+    <mergeCell ref="G42:J42"/>
+    <mergeCell ref="K42:N42"/>
+    <mergeCell ref="O42:R42"/>
+    <mergeCell ref="S42:T42"/>
+    <mergeCell ref="U42:X42"/>
     <mergeCell ref="U4:X4"/>
     <mergeCell ref="U6:X6"/>
     <mergeCell ref="G4:J4"/>
@@ -35190,26 +35198,6 @@
     <mergeCell ref="O6:R6"/>
     <mergeCell ref="K6:N6"/>
     <mergeCell ref="G6:J6"/>
-    <mergeCell ref="G42:J42"/>
-    <mergeCell ref="K42:N42"/>
-    <mergeCell ref="O42:R42"/>
-    <mergeCell ref="S42:T42"/>
-    <mergeCell ref="U42:X42"/>
-    <mergeCell ref="G44:J44"/>
-    <mergeCell ref="K44:N44"/>
-    <mergeCell ref="O44:R44"/>
-    <mergeCell ref="S44:T44"/>
-    <mergeCell ref="U44:X44"/>
-    <mergeCell ref="G88:J88"/>
-    <mergeCell ref="K88:N88"/>
-    <mergeCell ref="O88:R88"/>
-    <mergeCell ref="S88:T88"/>
-    <mergeCell ref="U88:X88"/>
-    <mergeCell ref="G90:J90"/>
-    <mergeCell ref="K90:N90"/>
-    <mergeCell ref="O90:R90"/>
-    <mergeCell ref="S90:T90"/>
-    <mergeCell ref="U90:X90"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -35385,12 +35373,12 @@
       <c r="I6" s="84"/>
       <c r="J6" s="84"/>
       <c r="K6" s="84"/>
-      <c r="L6" s="504" t="s">
+      <c r="L6" s="507" t="s">
         <v>1007</v>
       </c>
-      <c r="M6" s="506"/>
-      <c r="N6" s="506"/>
-      <c r="O6" s="505"/>
+      <c r="M6" s="509"/>
+      <c r="N6" s="509"/>
+      <c r="O6" s="508"/>
       <c r="P6" s="475" t="s">
         <v>1019</v>
       </c>
@@ -47680,103 +47668,103 @@
       <c r="C4" s="381" t="s">
         <v>805</v>
       </c>
-      <c r="D4" s="512" t="s">
+      <c r="D4" s="511" t="s">
         <v>806</v>
       </c>
-      <c r="E4" s="511"/>
-      <c r="F4" s="511"/>
-      <c r="G4" s="511"/>
+      <c r="E4" s="512"/>
+      <c r="F4" s="512"/>
+      <c r="G4" s="512"/>
       <c r="H4" s="513"/>
-      <c r="I4" s="511" t="s">
+      <c r="I4" s="512" t="s">
         <v>807</v>
       </c>
-      <c r="J4" s="511"/>
-      <c r="K4" s="511"/>
-      <c r="L4" s="511"/>
+      <c r="J4" s="512"/>
+      <c r="K4" s="512"/>
+      <c r="L4" s="512"/>
       <c r="M4" s="513"/>
-      <c r="N4" s="511" t="s">
+      <c r="N4" s="512" t="s">
         <v>808</v>
       </c>
-      <c r="O4" s="511"/>
-      <c r="P4" s="511"/>
-      <c r="Q4" s="511"/>
+      <c r="O4" s="512"/>
+      <c r="P4" s="512"/>
+      <c r="Q4" s="512"/>
       <c r="R4" s="513"/>
-      <c r="S4" s="511" t="s">
+      <c r="S4" s="512" t="s">
         <v>809</v>
       </c>
-      <c r="T4" s="511"/>
-      <c r="U4" s="511"/>
-      <c r="V4" s="511"/>
+      <c r="T4" s="512"/>
+      <c r="U4" s="512"/>
+      <c r="V4" s="512"/>
       <c r="W4" s="513"/>
-      <c r="X4" s="511" t="s">
+      <c r="X4" s="512" t="s">
         <v>810</v>
       </c>
-      <c r="Y4" s="511"/>
-      <c r="Z4" s="511"/>
-      <c r="AA4" s="511"/>
+      <c r="Y4" s="512"/>
+      <c r="Z4" s="512"/>
+      <c r="AA4" s="512"/>
       <c r="AB4" s="513"/>
-      <c r="AC4" s="511" t="s">
+      <c r="AC4" s="512" t="s">
         <v>811</v>
       </c>
-      <c r="AD4" s="511"/>
-      <c r="AE4" s="511"/>
-      <c r="AF4" s="511"/>
+      <c r="AD4" s="512"/>
+      <c r="AE4" s="512"/>
+      <c r="AF4" s="512"/>
       <c r="AG4" s="513"/>
-      <c r="AH4" s="511" t="s">
+      <c r="AH4" s="512" t="s">
         <v>812</v>
       </c>
-      <c r="AI4" s="511"/>
-      <c r="AJ4" s="511"/>
-      <c r="AK4" s="511"/>
+      <c r="AI4" s="512"/>
+      <c r="AJ4" s="512"/>
+      <c r="AK4" s="512"/>
       <c r="AL4" s="513"/>
-      <c r="AM4" s="511" t="s">
+      <c r="AM4" s="512" t="s">
         <v>813</v>
       </c>
-      <c r="AN4" s="511"/>
-      <c r="AO4" s="511"/>
-      <c r="AP4" s="511"/>
+      <c r="AN4" s="512"/>
+      <c r="AO4" s="512"/>
+      <c r="AP4" s="512"/>
       <c r="AQ4" s="513"/>
-      <c r="AR4" s="511" t="s">
+      <c r="AR4" s="512" t="s">
         <v>814</v>
       </c>
-      <c r="AS4" s="511"/>
-      <c r="AT4" s="511"/>
-      <c r="AU4" s="511"/>
+      <c r="AS4" s="512"/>
+      <c r="AT4" s="512"/>
+      <c r="AU4" s="512"/>
       <c r="AV4" s="513"/>
-      <c r="AW4" s="511" t="s">
+      <c r="AW4" s="512" t="s">
         <v>815</v>
       </c>
-      <c r="AX4" s="511"/>
-      <c r="AY4" s="511"/>
-      <c r="AZ4" s="511"/>
-      <c r="BA4" s="511"/>
-      <c r="BB4" s="512" t="s">
+      <c r="AX4" s="512"/>
+      <c r="AY4" s="512"/>
+      <c r="AZ4" s="512"/>
+      <c r="BA4" s="512"/>
+      <c r="BB4" s="511" t="s">
         <v>816</v>
       </c>
-      <c r="BC4" s="511"/>
-      <c r="BD4" s="511"/>
-      <c r="BE4" s="511"/>
+      <c r="BC4" s="512"/>
+      <c r="BD4" s="512"/>
+      <c r="BE4" s="512"/>
       <c r="BF4" s="513"/>
-      <c r="BG4" s="511" t="s">
+      <c r="BG4" s="512" t="s">
         <v>817</v>
       </c>
-      <c r="BH4" s="511"/>
-      <c r="BI4" s="511"/>
-      <c r="BJ4" s="511"/>
-      <c r="BK4" s="511"/>
-      <c r="BL4" s="512" t="s">
+      <c r="BH4" s="512"/>
+      <c r="BI4" s="512"/>
+      <c r="BJ4" s="512"/>
+      <c r="BK4" s="512"/>
+      <c r="BL4" s="511" t="s">
         <v>818</v>
       </c>
-      <c r="BM4" s="511"/>
-      <c r="BN4" s="511"/>
-      <c r="BO4" s="511"/>
-      <c r="BP4" s="511"/>
-      <c r="BQ4" s="512" t="s">
+      <c r="BM4" s="512"/>
+      <c r="BN4" s="512"/>
+      <c r="BO4" s="512"/>
+      <c r="BP4" s="512"/>
+      <c r="BQ4" s="511" t="s">
         <v>819</v>
       </c>
-      <c r="BR4" s="511"/>
-      <c r="BS4" s="511"/>
-      <c r="BT4" s="511"/>
+      <c r="BR4" s="512"/>
+      <c r="BS4" s="512"/>
+      <c r="BT4" s="512"/>
       <c r="BU4" s="513"/>
       <c r="BV4" s="382" t="s">
         <v>820</v>
@@ -61370,11 +61358,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="BL4:BP4"/>
-    <mergeCell ref="BQ4:BU4"/>
-    <mergeCell ref="BW4:CA4"/>
-    <mergeCell ref="CB4:CF4"/>
-    <mergeCell ref="CG4:CK4"/>
     <mergeCell ref="BG4:BK4"/>
     <mergeCell ref="D4:H4"/>
     <mergeCell ref="I4:M4"/>
@@ -61387,6 +61370,11 @@
     <mergeCell ref="AR4:AV4"/>
     <mergeCell ref="AW4:BA4"/>
     <mergeCell ref="BB4:BF4"/>
+    <mergeCell ref="BL4:BP4"/>
+    <mergeCell ref="BQ4:BU4"/>
+    <mergeCell ref="BW4:CA4"/>
+    <mergeCell ref="CB4:CF4"/>
+    <mergeCell ref="CG4:CK4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
Update Apt Cost - Oil and Gas
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_RSD.xlsx
+++ b/SubRES_TMPL/SubRes_RSD.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AEEAD6E-7D5C-4AC6-9978-1B5F78804ACD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B193C012-B9E2-4909-B4B2-8E7C76B0D935}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{34F9D92C-266F-476D-89E0-63153305AC39}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{34F9D92C-266F-476D-89E0-63153305AC39}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="34" r:id="rId1"/>
@@ -102,6 +102,30 @@
     <author>Author</author>
   </authors>
   <commentList>
+    <comment ref="U7" authorId="0" shapeId="0" xr:uid="{1D79DD36-FBC1-4D60-949F-8162AF9F30B1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Oil Boilers approx 30%higher cost than  gas boilers</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="AF7" authorId="0" shapeId="0" xr:uid="{374DB055-F5C1-43ED-915B-ECEEEDC762B6}">
       <text>
         <r>
@@ -149,7 +173,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Author:</t>
         </r>
@@ -158,10 +182,58 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Data from AECOM report - https://www.gov.ie/en/publication/8b915-cost-optimal-residential-report-ireland-2018/</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U11" authorId="0" shapeId="0" xr:uid="{820FF72B-D99E-45E4-8E70-1F46B28DB178}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Data from AECOM report - https://www.gov.ie/en/publication/8b915-cost-optimal-residential-report-ireland-2018/</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U13" authorId="0" shapeId="0" xr:uid="{D457C9FD-B271-4510-A505-DA905A86AC68}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Cost based on AECOM document,price increas based upon JRC data</t>
         </r>
       </text>
     </comment>
@@ -8443,7 +8515,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3461" uniqueCount="1047">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3463" uniqueCount="1049">
   <si>
     <t>Document type:</t>
   </si>
@@ -11606,6 +11678,12 @@
   <si>
     <t>CEFF~RSDWH_Det~2050</t>
   </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>What about extra cost of LPG storage tankscompared to gas boiler cost?</t>
+  </si>
 </sst>
 </file>
 
@@ -11623,7 +11701,7 @@
     <numFmt numFmtId="171" formatCode="#,##0.000"/>
     <numFmt numFmtId="172" formatCode="0.000"/>
   </numFmts>
-  <fonts count="71" x14ac:knownFonts="1">
+  <fonts count="69" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -12071,19 +12149,6 @@
       <color theme="8"/>
       <name val="Cambria"/>
       <family val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="35">
@@ -14052,6 +14117,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="16" fillId="33" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="16" fillId="34" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -14121,6 +14188,15 @@
     <xf numFmtId="0" fontId="16" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="23" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -14130,22 +14206,13 @@
     <xf numFmtId="0" fontId="16" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="60" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="60" fillId="31" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="60" fillId="31" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="60" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="60" fillId="31" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -14160,8 +14227,6 @@
     <xf numFmtId="0" fontId="60" fillId="32" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="16" fillId="33" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="16" fillId="34" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="20% - Colore 2" xfId="11" xr:uid="{3E3DAF22-4D86-48A9-B6EE-8D230C1E993C}"/>
@@ -15878,14 +15943,14 @@
       <c r="F16" s="216"/>
     </row>
     <row r="17" spans="1:14" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="482" t="s">
+      <c r="A17" s="484" t="s">
         <v>468</v>
       </c>
-      <c r="B17" s="482"/>
-      <c r="C17" s="482"/>
-      <c r="D17" s="482"/>
-      <c r="E17" s="482"/>
-      <c r="F17" s="482"/>
+      <c r="B17" s="484"/>
+      <c r="C17" s="484"/>
+      <c r="D17" s="484"/>
+      <c r="E17" s="484"/>
+      <c r="F17" s="484"/>
       <c r="G17" s="218"/>
       <c r="H17" s="218"/>
       <c r="I17" s="219"/>
@@ -15923,13 +15988,13 @@
       <c r="A20" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="483" t="s">
+      <c r="B20" s="485" t="s">
         <v>470</v>
       </c>
-      <c r="C20" s="483"/>
-      <c r="D20" s="483"/>
-      <c r="E20" s="483"/>
-      <c r="F20" s="483"/>
+      <c r="C20" s="485"/>
+      <c r="D20" s="485"/>
+      <c r="E20" s="485"/>
+      <c r="F20" s="485"/>
       <c r="G20" s="223"/>
       <c r="H20" s="223"/>
       <c r="I20" s="224"/>
@@ -15943,13 +16008,13 @@
       <c r="A21" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="484" t="s">
+      <c r="B21" s="486" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="484"/>
-      <c r="D21" s="484"/>
-      <c r="E21" s="484"/>
-      <c r="F21" s="484"/>
+      <c r="C21" s="486"/>
+      <c r="D21" s="486"/>
+      <c r="E21" s="486"/>
+      <c r="F21" s="486"/>
       <c r="G21" s="223"/>
       <c r="H21" s="223"/>
       <c r="I21" s="224"/>
@@ -15963,13 +16028,13 @@
       <c r="A22" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="484" t="s">
+      <c r="B22" s="486" t="s">
         <v>58</v>
       </c>
-      <c r="C22" s="484"/>
-      <c r="D22" s="484"/>
-      <c r="E22" s="484"/>
-      <c r="F22" s="484"/>
+      <c r="C22" s="486"/>
+      <c r="D22" s="486"/>
+      <c r="E22" s="486"/>
+      <c r="F22" s="486"/>
     </row>
     <row r="23" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
@@ -15998,22 +16063,22 @@
       <c r="H24" s="3"/>
     </row>
     <row r="25" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="485"/>
-      <c r="B25" s="485"/>
-      <c r="C25" s="485"/>
-      <c r="D25" s="485"/>
-      <c r="E25" s="485"/>
-      <c r="F25" s="485"/>
+      <c r="A25" s="487"/>
+      <c r="B25" s="487"/>
+      <c r="C25" s="487"/>
+      <c r="D25" s="487"/>
+      <c r="E25" s="487"/>
+      <c r="F25" s="487"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
     </row>
     <row r="26" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="481"/>
-      <c r="B26" s="481"/>
-      <c r="C26" s="481"/>
-      <c r="D26" s="481"/>
-      <c r="E26" s="481"/>
-      <c r="F26" s="481"/>
+      <c r="A26" s="483"/>
+      <c r="B26" s="483"/>
+      <c r="C26" s="483"/>
+      <c r="D26" s="483"/>
+      <c r="E26" s="483"/>
+      <c r="F26" s="483"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="216"/>
@@ -16181,7 +16246,9 @@
   </sheetPr>
   <dimension ref="B1:T45"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -16198,16 +16265,16 @@
   <sheetData>
     <row r="1" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:20" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="486" t="s">
+      <c r="B2" s="488" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="487"/>
-      <c r="D2" s="487"/>
-      <c r="E2" s="488"/>
-      <c r="G2" s="486" t="s">
+      <c r="C2" s="489"/>
+      <c r="D2" s="489"/>
+      <c r="E2" s="490"/>
+      <c r="G2" s="488" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="488"/>
+      <c r="H2" s="490"/>
       <c r="I2" s="227"/>
       <c r="J2" s="227"/>
       <c r="K2" s="228"/>
@@ -16549,16 +16616,16 @@
     </row>
     <row r="19" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="2:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="489" t="s">
+      <c r="B20" s="491" t="s">
         <v>80</v>
       </c>
-      <c r="C20" s="490"/>
-      <c r="D20" s="490"/>
-      <c r="E20" s="491"/>
-      <c r="G20" s="486" t="s">
+      <c r="C20" s="492"/>
+      <c r="D20" s="492"/>
+      <c r="E20" s="493"/>
+      <c r="G20" s="488" t="s">
         <v>14</v>
       </c>
-      <c r="H20" s="488"/>
+      <c r="H20" s="490"/>
     </row>
     <row r="21" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="255" t="s">
@@ -16802,16 +16869,16 @@
     </row>
     <row r="37" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="38" spans="2:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="486" t="s">
+      <c r="B38" s="488" t="s">
         <v>88</v>
       </c>
-      <c r="C38" s="487"/>
-      <c r="D38" s="487"/>
-      <c r="E38" s="488"/>
-      <c r="G38" s="492" t="s">
+      <c r="C38" s="489"/>
+      <c r="D38" s="489"/>
+      <c r="E38" s="490"/>
+      <c r="G38" s="494" t="s">
         <v>82</v>
       </c>
-      <c r="H38" s="493"/>
+      <c r="H38" s="495"/>
     </row>
     <row r="39" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B39" s="276" t="s">
@@ -16846,8 +16913,12 @@
       <c r="E40" s="281" t="s">
         <v>475</v>
       </c>
-      <c r="G40" s="266"/>
-      <c r="H40" s="266"/>
+      <c r="G40" s="266" t="s">
+        <v>1047</v>
+      </c>
+      <c r="H40" s="266" t="s">
+        <v>1048</v>
+      </c>
     </row>
     <row r="41" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B41" s="279"/>
@@ -16986,13 +17057,13 @@
       <c r="Q3" s="5" t="s">
         <v>419</v>
       </c>
-      <c r="W3" s="494" t="s">
+      <c r="W3" s="496" t="s">
         <v>717</v>
       </c>
-      <c r="X3" s="494"/>
-      <c r="Y3" s="494"/>
-      <c r="Z3" s="494"/>
-      <c r="AA3" s="494"/>
+      <c r="X3" s="496"/>
+      <c r="Y3" s="496"/>
+      <c r="Z3" s="496"/>
+      <c r="AA3" s="496"/>
     </row>
     <row r="4" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C4" s="63" t="s">
@@ -17010,12 +17081,12 @@
       <c r="G4" s="177" t="s">
         <v>338</v>
       </c>
-      <c r="H4" s="498" t="s">
+      <c r="H4" s="500" t="s">
         <v>339</v>
       </c>
-      <c r="I4" s="499"/>
-      <c r="J4" s="499"/>
-      <c r="K4" s="500"/>
+      <c r="I4" s="501"/>
+      <c r="J4" s="501"/>
+      <c r="K4" s="502"/>
       <c r="L4" s="107"/>
       <c r="M4" s="107"/>
       <c r="N4" s="107"/>
@@ -17048,12 +17119,12 @@
       <c r="G5" s="84" t="s">
         <v>312</v>
       </c>
-      <c r="H5" s="501" t="s">
+      <c r="H5" s="503" t="s">
         <v>695</v>
       </c>
-      <c r="I5" s="502"/>
-      <c r="J5" s="502"/>
-      <c r="K5" s="503"/>
+      <c r="I5" s="504"/>
+      <c r="J5" s="504"/>
+      <c r="K5" s="505"/>
       <c r="L5" s="108" t="s">
         <v>466</v>
       </c>
@@ -17284,12 +17355,12 @@
       <c r="G11" s="84" t="s">
         <v>312</v>
       </c>
-      <c r="H11" s="495" t="s">
+      <c r="H11" s="497" t="s">
         <v>695</v>
       </c>
-      <c r="I11" s="496"/>
-      <c r="J11" s="496"/>
-      <c r="K11" s="497"/>
+      <c r="I11" s="498"/>
+      <c r="J11" s="498"/>
+      <c r="K11" s="499"/>
       <c r="L11" s="201"/>
       <c r="M11" s="201"/>
       <c r="N11" s="108" t="s">
@@ -17495,12 +17566,12 @@
       <c r="G17" s="84" t="s">
         <v>312</v>
       </c>
-      <c r="H17" s="495" t="s">
+      <c r="H17" s="497" t="s">
         <v>695</v>
       </c>
-      <c r="I17" s="496"/>
-      <c r="J17" s="496"/>
-      <c r="K17" s="497"/>
+      <c r="I17" s="498"/>
+      <c r="J17" s="498"/>
+      <c r="K17" s="499"/>
       <c r="L17" s="201"/>
       <c r="M17" s="201"/>
       <c r="N17" s="108" t="s">
@@ -24784,8 +24855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{104F8057-C735-4662-BAA6-EEDCF7B57273}">
   <dimension ref="A2:AO162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W8" sqref="W8"/>
+    <sheetView tabSelected="1" topLeftCell="E3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="U16" sqref="U16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -24940,34 +25011,34 @@
       <c r="F4" s="63" t="s">
         <v>334</v>
       </c>
-      <c r="G4" s="507" t="s">
+      <c r="G4" s="506" t="s">
         <v>758</v>
       </c>
-      <c r="H4" s="508"/>
-      <c r="I4" s="508"/>
-      <c r="J4" s="509"/>
-      <c r="K4" s="507" t="s">
+      <c r="H4" s="507"/>
+      <c r="I4" s="507"/>
+      <c r="J4" s="508"/>
+      <c r="K4" s="506" t="s">
         <v>336</v>
       </c>
-      <c r="L4" s="508"/>
-      <c r="M4" s="508"/>
-      <c r="N4" s="509"/>
-      <c r="O4" s="507" t="s">
+      <c r="L4" s="507"/>
+      <c r="M4" s="507"/>
+      <c r="N4" s="508"/>
+      <c r="O4" s="506" t="s">
         <v>337</v>
       </c>
-      <c r="P4" s="508"/>
-      <c r="Q4" s="508"/>
-      <c r="R4" s="509"/>
-      <c r="S4" s="507" t="s">
+      <c r="P4" s="507"/>
+      <c r="Q4" s="507"/>
+      <c r="R4" s="508"/>
+      <c r="S4" s="506" t="s">
         <v>338</v>
       </c>
-      <c r="T4" s="509"/>
-      <c r="U4" s="498" t="s">
+      <c r="T4" s="508"/>
+      <c r="U4" s="500" t="s">
         <v>339</v>
       </c>
-      <c r="V4" s="499"/>
-      <c r="W4" s="499"/>
-      <c r="X4" s="500"/>
+      <c r="V4" s="501"/>
+      <c r="W4" s="501"/>
+      <c r="X4" s="502"/>
       <c r="Y4" s="107"/>
       <c r="Z4" s="107"/>
       <c r="AA4" s="115" t="s">
@@ -25062,34 +25133,34 @@
       <c r="D6" s="85"/>
       <c r="E6" s="85"/>
       <c r="F6" s="86"/>
-      <c r="G6" s="501" t="s">
+      <c r="G6" s="503" t="s">
         <v>55</v>
       </c>
-      <c r="H6" s="502"/>
-      <c r="I6" s="502"/>
-      <c r="J6" s="503"/>
-      <c r="K6" s="502" t="s">
+      <c r="H6" s="504"/>
+      <c r="I6" s="504"/>
+      <c r="J6" s="505"/>
+      <c r="K6" s="504" t="s">
         <v>55</v>
       </c>
-      <c r="L6" s="502"/>
-      <c r="M6" s="502"/>
-      <c r="N6" s="503"/>
-      <c r="O6" s="501" t="s">
+      <c r="L6" s="504"/>
+      <c r="M6" s="504"/>
+      <c r="N6" s="505"/>
+      <c r="O6" s="503" t="s">
         <v>55</v>
       </c>
-      <c r="P6" s="502"/>
-      <c r="Q6" s="502"/>
-      <c r="R6" s="503"/>
-      <c r="S6" s="501" t="s">
+      <c r="P6" s="504"/>
+      <c r="Q6" s="504"/>
+      <c r="R6" s="505"/>
+      <c r="S6" s="503" t="s">
         <v>312</v>
       </c>
-      <c r="T6" s="503"/>
-      <c r="U6" s="501" t="s">
+      <c r="T6" s="505"/>
+      <c r="U6" s="503" t="s">
         <v>1007</v>
       </c>
-      <c r="V6" s="502"/>
-      <c r="W6" s="502"/>
-      <c r="X6" s="503"/>
+      <c r="V6" s="504"/>
+      <c r="W6" s="504"/>
+      <c r="X6" s="505"/>
       <c r="Y6" s="108" t="s">
         <v>1019</v>
       </c>
@@ -25175,25 +25246,24 @@
         <v>20</v>
       </c>
       <c r="T7" s="136"/>
-      <c r="U7" s="87">
-        <f>(JRC_Data!BB7/1000)*$T$145</f>
-        <v>6.0393822393822383</v>
-      </c>
-      <c r="V7" s="87">
-        <f>(JRC_Data!BC7/1000)*$T$145</f>
-        <v>6.0393822393822383</v>
-      </c>
-      <c r="W7" s="87">
-        <f>(JRC_Data!BD7/1000)*$T$145</f>
-        <v>6.0393822393822383</v>
-      </c>
-      <c r="X7" s="87">
-        <f>(JRC_Data!BE7/1000)*$T$145</f>
-        <v>6.0393822393822383</v>
-      </c>
-      <c r="Y7" s="87">
-        <f>JRC_Data!BL7/1000</f>
-        <v>0.27</v>
+      <c r="U7" s="481">
+        <f>U9*1.3</f>
+        <v>3.6270000000000002</v>
+      </c>
+      <c r="V7" s="481">
+        <f t="shared" ref="V7:X7" si="0">V9*1.3</f>
+        <v>3.6270000000000002</v>
+      </c>
+      <c r="W7" s="481">
+        <f t="shared" si="0"/>
+        <v>3.6270000000000002</v>
+      </c>
+      <c r="X7" s="481">
+        <f t="shared" si="0"/>
+        <v>3.6270000000000002</v>
+      </c>
+      <c r="Y7" s="481">
+        <v>0.12</v>
       </c>
       <c r="Z7" s="135"/>
       <c r="AA7" s="354"/>
@@ -25264,40 +25334,39 @@
         <v>0.7</v>
       </c>
       <c r="P8" s="338">
-        <f t="shared" ref="P8" si="0">H8*0.7</f>
+        <f t="shared" ref="P8" si="1">H8*0.7</f>
         <v>0.7</v>
       </c>
       <c r="Q8" s="338">
-        <f t="shared" ref="Q8" si="1">I8*0.7</f>
+        <f t="shared" ref="Q8" si="2">I8*0.7</f>
         <v>0.7</v>
       </c>
       <c r="R8" s="339">
-        <f t="shared" ref="R8" si="2">J8*0.7</f>
+        <f t="shared" ref="R8" si="3">J8*0.7</f>
         <v>0.7</v>
       </c>
       <c r="S8" s="100">
         <v>20</v>
       </c>
       <c r="T8" s="71"/>
-      <c r="U8" s="69">
-        <f>(JRC_Data!BB7/1000)*$T$146</f>
-        <v>6.0903474903474901</v>
-      </c>
-      <c r="V8" s="69">
-        <f>(JRC_Data!BC7/1000)*$T$146</f>
-        <v>6.0903474903474901</v>
-      </c>
-      <c r="W8" s="69">
-        <f>(JRC_Data!BD7/1000)*$T$146</f>
-        <v>6.0903474903474901</v>
-      </c>
-      <c r="X8" s="69">
-        <f>(JRC_Data!BE7/1000)*$T$146</f>
-        <v>6.0903474903474901</v>
-      </c>
-      <c r="Y8" s="69">
-        <f>JRC_Data!BL7/1000</f>
-        <v>0.27</v>
+      <c r="U8" s="482">
+        <f>U10*1.3</f>
+        <v>3.6576075949367097</v>
+      </c>
+      <c r="V8" s="482">
+        <f t="shared" ref="V8:X8" si="4">V10*1.3</f>
+        <v>3.6576075949367097</v>
+      </c>
+      <c r="W8" s="482">
+        <f t="shared" si="4"/>
+        <v>3.6576075949367097</v>
+      </c>
+      <c r="X8" s="482">
+        <f t="shared" si="4"/>
+        <v>3.6576075949367097</v>
+      </c>
+      <c r="Y8" s="482">
+        <v>0.12</v>
       </c>
       <c r="Z8" s="113"/>
       <c r="AA8" s="120"/>
@@ -25313,11 +25382,11 @@
       </c>
       <c r="AI8" s="153"/>
       <c r="AJ8" s="152" t="str">
-        <f t="shared" ref="AJ8:AJ13" si="3">C8</f>
+        <f t="shared" ref="AJ8:AJ13" si="5">C8</f>
         <v>R-SW_Apt_KER_N1</v>
       </c>
       <c r="AK8" s="152" t="str">
-        <f t="shared" ref="AK8:AK13" si="4">D8</f>
+        <f t="shared" ref="AK8:AK13" si="6">D8</f>
         <v>Residential Kerosene Heating Oil - New 2 SH + WH</v>
       </c>
       <c r="AL8" s="153" t="s">
@@ -25369,25 +25438,24 @@
         <v>22</v>
       </c>
       <c r="T9" s="77"/>
-      <c r="U9" s="517">
+      <c r="U9" s="481">
         <f>2.79</f>
         <v>2.79</v>
       </c>
-      <c r="V9" s="517">
-        <f t="shared" ref="V9:X9" si="5">2.79</f>
+      <c r="V9" s="481">
+        <f t="shared" ref="V9:X11" si="7">2.79</f>
         <v>2.79</v>
       </c>
-      <c r="W9" s="517">
-        <f t="shared" si="5"/>
+      <c r="W9" s="481">
+        <f t="shared" si="7"/>
         <v>2.79</v>
       </c>
-      <c r="X9" s="517">
-        <f t="shared" si="5"/>
+      <c r="X9" s="481">
+        <f t="shared" si="7"/>
         <v>2.79</v>
       </c>
-      <c r="Y9" s="87">
-        <f>JRC_Data!BL9/1000</f>
-        <v>0.23499999999999999</v>
+      <c r="Y9" s="481">
+        <v>0.12</v>
       </c>
       <c r="Z9" s="112"/>
       <c r="AA9" s="119"/>
@@ -25403,11 +25471,11 @@
       </c>
       <c r="AI9" s="153"/>
       <c r="AJ9" s="152" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>R-SH_Apt_GAS_N1</v>
       </c>
       <c r="AK9" s="152" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>Residential Natural Gas Heating - New 1 SH</v>
       </c>
       <c r="AL9" s="153" t="s">
@@ -25456,40 +25524,39 @@
         <v>0.7</v>
       </c>
       <c r="P10" s="338">
-        <f t="shared" ref="P10" si="6">H10*0.7</f>
+        <f t="shared" ref="P10" si="8">H10*0.7</f>
         <v>0.7</v>
       </c>
       <c r="Q10" s="338">
-        <f t="shared" ref="Q10" si="7">I10*0.7</f>
+        <f t="shared" ref="Q10" si="9">I10*0.7</f>
         <v>0.7</v>
       </c>
       <c r="R10" s="339">
-        <f t="shared" ref="R10" si="8">J10*0.7</f>
+        <f t="shared" ref="R10" si="10">J10*0.7</f>
         <v>0.7</v>
       </c>
       <c r="S10" s="100">
         <v>22</v>
       </c>
       <c r="T10" s="71"/>
-      <c r="U10" s="518">
+      <c r="U10" s="482">
         <f>U9*($T$146/$T$145)</f>
         <v>2.8135443037974688</v>
       </c>
-      <c r="V10" s="518">
-        <f t="shared" ref="V10:X10" si="9">V9*($T$146/$T$145)</f>
+      <c r="V10" s="482">
+        <f t="shared" ref="V10:X10" si="11">V9*($T$146/$T$145)</f>
         <v>2.8135443037974688</v>
       </c>
-      <c r="W10" s="518">
-        <f t="shared" si="9"/>
+      <c r="W10" s="482">
+        <f t="shared" si="11"/>
         <v>2.8135443037974688</v>
       </c>
-      <c r="X10" s="518">
-        <f t="shared" si="9"/>
+      <c r="X10" s="482">
+        <f t="shared" si="11"/>
         <v>2.8135443037974688</v>
       </c>
-      <c r="Y10" s="69">
-        <f>JRC_Data!BL9/1000</f>
-        <v>0.23499999999999999</v>
+      <c r="Y10" s="482">
+        <v>0.12</v>
       </c>
       <c r="Z10" s="113"/>
       <c r="AA10" s="120"/>
@@ -25505,11 +25572,11 @@
       </c>
       <c r="AI10" s="153"/>
       <c r="AJ10" s="152" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>R-SW_Apt_GAS_N1</v>
       </c>
       <c r="AK10" s="152" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>Residential Natural Gas Heating - New 2 SH + WH</v>
       </c>
       <c r="AL10" s="153" t="s">
@@ -25561,25 +25628,24 @@
         <v>22</v>
       </c>
       <c r="T11" s="77"/>
-      <c r="U11" s="87">
-        <f>(JRC_Data!BB9/1000)*($T$145/$T$147)</f>
-        <v>3.9173553719008263</v>
-      </c>
-      <c r="V11" s="87">
-        <f>(JRC_Data!BC9/1000)*($T$145/$T$147)</f>
-        <v>3.9173553719008263</v>
-      </c>
-      <c r="W11" s="87">
-        <f>(JRC_Data!BD9/1000)*($T$145/$T$147)</f>
-        <v>3.9173553719008263</v>
-      </c>
-      <c r="X11" s="87">
-        <f>(JRC_Data!BE9/1000)*($T$145/$T$147)</f>
-        <v>3.9173553719008263</v>
-      </c>
-      <c r="Y11" s="87">
-        <f>JRC_Data!BL9/1000</f>
-        <v>0.23499999999999999</v>
+      <c r="U11" s="481">
+        <f>2.79</f>
+        <v>2.79</v>
+      </c>
+      <c r="V11" s="481">
+        <f t="shared" si="7"/>
+        <v>2.79</v>
+      </c>
+      <c r="W11" s="481">
+        <f t="shared" si="7"/>
+        <v>2.79</v>
+      </c>
+      <c r="X11" s="481">
+        <f t="shared" si="7"/>
+        <v>2.79</v>
+      </c>
+      <c r="Y11" s="481">
+        <v>0.12</v>
       </c>
       <c r="Z11" s="112"/>
       <c r="AA11" s="119"/>
@@ -25595,11 +25661,11 @@
       </c>
       <c r="AI11" s="153"/>
       <c r="AJ11" s="152" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>R-SH_Apt_LPG_N1</v>
       </c>
       <c r="AK11" s="152" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>Residential Liquid Petroleum Gas- New 1 SH</v>
       </c>
       <c r="AL11" s="153" t="s">
@@ -25648,40 +25714,39 @@
         <v>0.7</v>
       </c>
       <c r="P12" s="338">
-        <f t="shared" ref="P12:R12" si="10">H12*0.7</f>
+        <f t="shared" ref="P12:R12" si="12">H12*0.7</f>
         <v>0.7</v>
       </c>
       <c r="Q12" s="338">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.7</v>
       </c>
       <c r="R12" s="339">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.7</v>
       </c>
       <c r="S12" s="100">
         <v>22</v>
       </c>
       <c r="T12" s="71"/>
-      <c r="U12" s="69">
-        <f>(JRC_Data!BB9/1000)*($T$146/$T$147)</f>
-        <v>3.950413223140496</v>
-      </c>
-      <c r="V12" s="69">
-        <f>(JRC_Data!BC9/1000)*($T$146/$T$147)</f>
-        <v>3.950413223140496</v>
-      </c>
-      <c r="W12" s="69">
-        <f>(JRC_Data!BD9/1000)*($T$146/$T$147)</f>
-        <v>3.950413223140496</v>
-      </c>
-      <c r="X12" s="69">
-        <f>(JRC_Data!BE9/1000)*($T$146/$T$147)</f>
-        <v>3.950413223140496</v>
-      </c>
-      <c r="Y12" s="69">
-        <f>JRC_Data!BL9/1000</f>
-        <v>0.23499999999999999</v>
+      <c r="U12" s="482">
+        <f>U11*($T$146/$T$145)</f>
+        <v>2.8135443037974688</v>
+      </c>
+      <c r="V12" s="482">
+        <f t="shared" ref="V12:X12" si="13">V11*($T$146/$T$145)</f>
+        <v>2.8135443037974688</v>
+      </c>
+      <c r="W12" s="482">
+        <f t="shared" si="13"/>
+        <v>2.8135443037974688</v>
+      </c>
+      <c r="X12" s="482">
+        <f t="shared" si="13"/>
+        <v>2.8135443037974688</v>
+      </c>
+      <c r="Y12" s="482">
+        <v>0.12</v>
       </c>
       <c r="Z12" s="113"/>
       <c r="AA12" s="120"/>
@@ -25697,11 +25762,11 @@
       </c>
       <c r="AI12" s="153"/>
       <c r="AJ12" s="152" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>R-SW_Apt_LPG_N1</v>
       </c>
       <c r="AK12" s="152" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>Residential Liquid Petroleum Gas- New 2 SH + WH</v>
       </c>
       <c r="AL12" s="153" t="s">
@@ -25753,25 +25818,22 @@
         <v>20</v>
       </c>
       <c r="T13" s="77"/>
-      <c r="U13" s="87">
-        <f>(JRC_Data!BB11/1000)*($T$145/$T$147)</f>
-        <v>6.6105371900826446</v>
-      </c>
-      <c r="V13" s="87">
-        <f>(JRC_Data!BC11/1000)*($T$145/$T$147)</f>
-        <v>6.6105371900826446</v>
-      </c>
-      <c r="W13" s="87">
-        <f>(JRC_Data!BD11/1000)*($T$145/$T$147)</f>
-        <v>7.3450413223140494</v>
-      </c>
-      <c r="X13" s="87">
-        <f>(JRC_Data!BE11/1000)*($T$145/$T$147)</f>
-        <v>7.3450413223140494</v>
-      </c>
-      <c r="Y13" s="87">
-        <f>JRC_Data!BL11/1000</f>
-        <v>2.5999999999999999E-2</v>
+      <c r="U13" s="481">
+        <v>6.25</v>
+      </c>
+      <c r="V13" s="481">
+        <v>6.25</v>
+      </c>
+      <c r="W13" s="481">
+        <f>V13*1.1</f>
+        <v>6.8750000000000009</v>
+      </c>
+      <c r="X13" s="481">
+        <f>V13*1.1</f>
+        <v>6.8750000000000009</v>
+      </c>
+      <c r="Y13" s="481">
+        <v>0.25</v>
       </c>
       <c r="Z13" s="112"/>
       <c r="AA13" s="119"/>
@@ -25787,11 +25849,11 @@
       </c>
       <c r="AI13" s="153"/>
       <c r="AJ13" s="152" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>R-SH_Apt_WOO_N1</v>
       </c>
       <c r="AK13" s="152" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>Residential Biomass Boiler - New 1 SH</v>
       </c>
       <c r="AL13" s="153" t="s">
@@ -25836,44 +25898,43 @@
       <c r="M14" s="79"/>
       <c r="N14" s="92"/>
       <c r="O14" s="337">
-        <f t="shared" ref="O14:R14" si="11">G14*0.7</f>
+        <f t="shared" ref="O14:R14" si="14">G14*0.7</f>
         <v>0.7</v>
       </c>
       <c r="P14" s="338">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.7</v>
       </c>
       <c r="Q14" s="338">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.7</v>
       </c>
       <c r="R14" s="339">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.7</v>
       </c>
       <c r="S14" s="100">
         <v>20</v>
       </c>
       <c r="T14" s="71"/>
-      <c r="U14" s="69">
+      <c r="U14" s="482">
         <f>(JRC_Data!BB11/1000)*($T$146/$T$147)</f>
         <v>6.6663223140495873</v>
       </c>
-      <c r="V14" s="69">
+      <c r="V14" s="482">
         <f>(JRC_Data!BC11/1000)*($T$146/$T$147)</f>
         <v>6.6663223140495873</v>
       </c>
-      <c r="W14" s="69">
+      <c r="W14" s="482">
         <f>(JRC_Data!BD11/1000)*($T$146/$T$147)</f>
         <v>7.4070247933884303</v>
       </c>
-      <c r="X14" s="69">
+      <c r="X14" s="482">
         <f>(JRC_Data!BE11/1000)*($T$146/$T$147)</f>
         <v>7.4070247933884303</v>
       </c>
-      <c r="Y14" s="69">
-        <f>JRC_Data!BL12/1000</f>
-        <v>3.15E-2</v>
+      <c r="Y14" s="482">
+        <v>0.25</v>
       </c>
       <c r="Z14" s="113"/>
       <c r="AA14" s="120"/>
@@ -26033,11 +26094,11 @@
       </c>
       <c r="AI16" s="151"/>
       <c r="AJ16" s="150" t="str">
-        <f t="shared" ref="AJ16:AK19" si="12">C18</f>
+        <f t="shared" ref="AJ16:AK19" si="15">C18</f>
         <v>R-SH_Apt_ELC_HPN1</v>
       </c>
       <c r="AK16" s="150" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>Residential Electric Heat Pump - Air to Air - SH</v>
       </c>
       <c r="AL16" s="151" t="s">
@@ -26087,11 +26148,11 @@
       <c r="AG17" s="81"/>
       <c r="AI17" s="153"/>
       <c r="AJ17" s="152" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>R-HC_Apt_ELC_HPN1</v>
       </c>
       <c r="AK17" s="152" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>Residential Electric Heat Pump - Air to Air - SH + SC</v>
       </c>
       <c r="AL17" s="153" t="s">
@@ -26180,11 +26241,11 @@
       </c>
       <c r="AI18" s="153"/>
       <c r="AJ18" s="152" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>R-SH_Apt_ELC_HPN2</v>
       </c>
       <c r="AK18" s="152" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>Residential Electric Heat Pump - Air to Water - SH</v>
       </c>
       <c r="AL18" s="153" t="s">
@@ -26284,11 +26345,11 @@
       </c>
       <c r="AI19" s="153"/>
       <c r="AJ19" s="152" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>R-SW_Apt_ELC_HPN1</v>
       </c>
       <c r="AK19" s="152" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>Residential Electric Heat Pump - Air to Water - SH + WH</v>
       </c>
       <c r="AL19" s="153" t="s">
@@ -26435,15 +26496,15 @@
         <v>0.7</v>
       </c>
       <c r="P21" s="70">
-        <f t="shared" ref="P21:R21" si="13">H21*0.7</f>
+        <f t="shared" ref="P21:R21" si="16">H21*0.7</f>
         <v>0.76999999999999991</v>
       </c>
       <c r="Q21" s="70">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0.86333333333333329</v>
       </c>
       <c r="R21" s="104">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0.93333333333333324</v>
       </c>
       <c r="S21" s="100">
@@ -26793,15 +26854,15 @@
         <v>0.7</v>
       </c>
       <c r="P25" s="67">
-        <f t="shared" ref="P25:R25" si="14">H25*0.7</f>
+        <f t="shared" ref="P25:R25" si="17">H25*0.7</f>
         <v>0.75185185185185177</v>
       </c>
       <c r="Q25" s="67">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0.88148148148148131</v>
       </c>
       <c r="R25" s="103">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0.88148148148148131</v>
       </c>
       <c r="S25" s="136">
@@ -26899,15 +26960,15 @@
         <v>0.77777777777777757</v>
       </c>
       <c r="P26" s="73">
-        <f t="shared" ref="P26" si="15">H26*0.7</f>
+        <f t="shared" ref="P26" si="18">H26*0.7</f>
         <v>0.8037037037037037</v>
       </c>
       <c r="Q26" s="73">
-        <f t="shared" ref="Q26" si="16">I26*0.7</f>
+        <f t="shared" ref="Q26" si="19">I26*0.7</f>
         <v>0.8037037037037037</v>
       </c>
       <c r="R26" s="106">
-        <f t="shared" ref="R26" si="17">J26*0.7</f>
+        <f t="shared" ref="R26" si="20">J26*0.7</f>
         <v>0.82962962962962949</v>
       </c>
       <c r="S26" s="74">
@@ -27002,11 +27063,11 @@
       <c r="AG27" s="81"/>
       <c r="AI27" s="306"/>
       <c r="AJ27" s="150" t="str">
-        <f t="shared" ref="AJ27:AK28" si="18">C33</f>
+        <f t="shared" ref="AJ27:AK28" si="21">C33</f>
         <v>R-WH_Apt_ELC_N1</v>
       </c>
       <c r="AK27" s="150" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v xml:space="preserve">Residential Electric Water Heater </v>
       </c>
       <c r="AL27" s="151" t="s">
@@ -27055,15 +27116,15 @@
         <v>0.7</v>
       </c>
       <c r="P28" s="348">
-        <f t="shared" ref="P28:R28" si="19">H28*0.7</f>
+        <f t="shared" ref="P28:R28" si="22">H28*0.7</f>
         <v>0.73360000000000003</v>
       </c>
       <c r="Q28" s="348">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0.76789999999999992</v>
       </c>
       <c r="R28" s="349">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0.81269999999999998</v>
       </c>
       <c r="S28" s="350">
@@ -27108,11 +27169,11 @@
       </c>
       <c r="AI28" s="4"/>
       <c r="AJ28" s="152" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>R-WH_Apt_SOL_N1</v>
       </c>
       <c r="AK28" s="152" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v xml:space="preserve">Residential Solar Water Heater </v>
       </c>
       <c r="AL28" s="153" t="s">
@@ -27833,34 +27894,34 @@
       <c r="F42" s="63" t="s">
         <v>334</v>
       </c>
-      <c r="G42" s="507" t="s">
+      <c r="G42" s="506" t="s">
         <v>335</v>
       </c>
-      <c r="H42" s="508"/>
-      <c r="I42" s="508"/>
-      <c r="J42" s="509"/>
-      <c r="K42" s="507" t="s">
+      <c r="H42" s="507"/>
+      <c r="I42" s="507"/>
+      <c r="J42" s="508"/>
+      <c r="K42" s="506" t="s">
         <v>336</v>
       </c>
-      <c r="L42" s="508"/>
-      <c r="M42" s="508"/>
-      <c r="N42" s="509"/>
-      <c r="O42" s="507" t="s">
+      <c r="L42" s="507"/>
+      <c r="M42" s="507"/>
+      <c r="N42" s="508"/>
+      <c r="O42" s="506" t="s">
         <v>337</v>
       </c>
-      <c r="P42" s="508"/>
-      <c r="Q42" s="508"/>
-      <c r="R42" s="509"/>
-      <c r="S42" s="507" t="s">
+      <c r="P42" s="507"/>
+      <c r="Q42" s="507"/>
+      <c r="R42" s="508"/>
+      <c r="S42" s="506" t="s">
         <v>338</v>
       </c>
-      <c r="T42" s="509"/>
-      <c r="U42" s="498" t="s">
+      <c r="T42" s="508"/>
+      <c r="U42" s="500" t="s">
         <v>339</v>
       </c>
-      <c r="V42" s="499"/>
-      <c r="W42" s="499"/>
-      <c r="X42" s="500"/>
+      <c r="V42" s="501"/>
+      <c r="W42" s="501"/>
+      <c r="X42" s="502"/>
       <c r="Y42" s="107"/>
       <c r="Z42" s="107"/>
       <c r="AA42" s="115" t="s">
@@ -27955,34 +28016,34 @@
       <c r="D44" s="85"/>
       <c r="E44" s="85"/>
       <c r="F44" s="86"/>
-      <c r="G44" s="501" t="s">
+      <c r="G44" s="503" t="s">
         <v>55</v>
       </c>
-      <c r="H44" s="502"/>
-      <c r="I44" s="502"/>
-      <c r="J44" s="503"/>
-      <c r="K44" s="502" t="s">
+      <c r="H44" s="504"/>
+      <c r="I44" s="504"/>
+      <c r="J44" s="505"/>
+      <c r="K44" s="504" t="s">
         <v>55</v>
       </c>
-      <c r="L44" s="502"/>
-      <c r="M44" s="502"/>
-      <c r="N44" s="503"/>
-      <c r="O44" s="501" t="s">
+      <c r="L44" s="504"/>
+      <c r="M44" s="504"/>
+      <c r="N44" s="505"/>
+      <c r="O44" s="503" t="s">
         <v>55</v>
       </c>
-      <c r="P44" s="502"/>
-      <c r="Q44" s="502"/>
-      <c r="R44" s="503"/>
-      <c r="S44" s="504" t="s">
+      <c r="P44" s="504"/>
+      <c r="Q44" s="504"/>
+      <c r="R44" s="505"/>
+      <c r="S44" s="509" t="s">
         <v>312</v>
       </c>
-      <c r="T44" s="505"/>
-      <c r="U44" s="504" t="s">
+      <c r="T44" s="510"/>
+      <c r="U44" s="509" t="s">
         <v>1007</v>
       </c>
-      <c r="V44" s="506"/>
-      <c r="W44" s="506"/>
-      <c r="X44" s="505"/>
+      <c r="V44" s="511"/>
+      <c r="W44" s="511"/>
+      <c r="X44" s="510"/>
       <c r="Y44" s="475" t="s">
         <v>1019</v>
       </c>
@@ -28157,15 +28218,15 @@
         <v>0.7</v>
       </c>
       <c r="P46" s="70">
-        <f t="shared" ref="P46:P48" si="20">H46*0.7</f>
+        <f t="shared" ref="P46:P48" si="23">H46*0.7</f>
         <v>0.7</v>
       </c>
       <c r="Q46" s="70">
-        <f t="shared" ref="Q46:Q48" si="21">I46*0.7</f>
+        <f t="shared" ref="Q46:Q48" si="24">I46*0.7</f>
         <v>0.7</v>
       </c>
       <c r="R46" s="104">
-        <f t="shared" ref="R46:R48" si="22">J46*0.7</f>
+        <f t="shared" ref="R46:R48" si="25">J46*0.7</f>
         <v>0.7</v>
       </c>
       <c r="S46" s="100">
@@ -28206,11 +28267,11 @@
       </c>
       <c r="AI46" s="153"/>
       <c r="AJ46" s="152" t="str">
-        <f t="shared" ref="AJ46:AJ56" si="23">C46</f>
+        <f t="shared" ref="AJ46:AJ56" si="26">C46</f>
         <v>R-SW_Att_KER_N1</v>
       </c>
       <c r="AK46" s="152" t="str">
-        <f t="shared" ref="AK46:AK56" si="24">D46</f>
+        <f t="shared" ref="AK46:AK56" si="27">D46</f>
         <v>Residential Kerosene Heating Oil - New 2 SH + WH</v>
       </c>
       <c r="AL46" s="153" t="s">
@@ -28259,15 +28320,15 @@
         <v>0.7</v>
       </c>
       <c r="P47" s="76">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>0.7</v>
       </c>
       <c r="Q47" s="76">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>0.7</v>
       </c>
       <c r="R47" s="105">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>0.7</v>
       </c>
       <c r="S47" s="101">
@@ -28312,11 +28373,11 @@
       </c>
       <c r="AI47" s="153"/>
       <c r="AJ47" s="152" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>R-SW_Att_KER_N2</v>
       </c>
       <c r="AK47" s="152" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>Residential Kerosene Heating Oil - New 3 SH+WH + Solar</v>
       </c>
       <c r="AL47" s="153" t="s">
@@ -28365,15 +28426,15 @@
         <v>0.7</v>
       </c>
       <c r="P48" s="70">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>0.71749999999999992</v>
       </c>
       <c r="Q48" s="70">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>0.71749999999999992</v>
       </c>
       <c r="R48" s="104">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>0.71749999999999992</v>
       </c>
       <c r="S48" s="100">
@@ -28418,11 +28479,11 @@
       </c>
       <c r="AI48" s="153"/>
       <c r="AJ48" s="152" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>R-SW_Att_KER_N3</v>
       </c>
       <c r="AK48" s="152" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>Residential Kerosene Heating Oil - New 3 SH+WH + Wood Stove</v>
       </c>
       <c r="AL48" s="154" t="s">
@@ -28506,11 +28567,11 @@
       </c>
       <c r="AI49" s="153"/>
       <c r="AJ49" s="152" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>R-SH_Att_GAS_N1</v>
       </c>
       <c r="AK49" s="152" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>Residential Natural Gas Heating - New 1 SH</v>
       </c>
       <c r="AL49" s="153" t="s">
@@ -28559,15 +28620,15 @@
         <v>0.7</v>
       </c>
       <c r="P50" s="70">
-        <f t="shared" ref="P50:P52" si="25">H50*0.7</f>
+        <f t="shared" ref="P50:P52" si="28">H50*0.7</f>
         <v>0.7</v>
       </c>
       <c r="Q50" s="70">
-        <f t="shared" ref="Q50:Q52" si="26">I50*0.7</f>
+        <f t="shared" ref="Q50:Q52" si="29">I50*0.7</f>
         <v>0.7</v>
       </c>
       <c r="R50" s="104">
-        <f t="shared" ref="R50:R52" si="27">J50*0.7</f>
+        <f t="shared" ref="R50:R52" si="30">J50*0.7</f>
         <v>0.7</v>
       </c>
       <c r="S50" s="100">
@@ -28608,11 +28669,11 @@
       </c>
       <c r="AI50" s="153"/>
       <c r="AJ50" s="152" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>R-SW_Att_GAS_N1</v>
       </c>
       <c r="AK50" s="152" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>Residential Natural Gas Heating - New 2 SH + WH</v>
       </c>
       <c r="AL50" s="153" t="s">
@@ -28661,15 +28722,15 @@
         <v>0.7</v>
       </c>
       <c r="P51" s="76">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>0.7</v>
       </c>
       <c r="Q51" s="76">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>0.7</v>
       </c>
       <c r="R51" s="105">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>0.7</v>
       </c>
       <c r="S51" s="101">
@@ -28714,11 +28775,11 @@
       </c>
       <c r="AI51" s="153"/>
       <c r="AJ51" s="152" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>R-SW_Att_GAS_N2</v>
       </c>
       <c r="AK51" s="152" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>Residential Natural Gas Heating - New 3 SH + WH + Solar</v>
       </c>
       <c r="AL51" s="153" t="s">
@@ -28767,15 +28828,15 @@
         <v>0.7</v>
       </c>
       <c r="P52" s="70">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>0.71749999999999992</v>
       </c>
       <c r="Q52" s="70">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>0.71749999999999992</v>
       </c>
       <c r="R52" s="104">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>0.71749999999999992</v>
       </c>
       <c r="S52" s="100">
@@ -28820,11 +28881,11 @@
       </c>
       <c r="AI52" s="153"/>
       <c r="AJ52" s="152" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>R-SW_Att_GAS_N3</v>
       </c>
       <c r="AK52" s="152" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>Residential Natural Gas Heating - New 4 SH + WH + Wood Stove</v>
       </c>
       <c r="AL52" s="153" t="s">
@@ -28910,11 +28971,11 @@
       </c>
       <c r="AI53" s="153"/>
       <c r="AJ53" s="152" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>R-SH_Att_LPG_N1</v>
       </c>
       <c r="AK53" s="152" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>Residential Liquid Petroleum Gas- New 1 SH</v>
       </c>
       <c r="AL53" s="153" t="s">
@@ -28963,15 +29024,15 @@
         <v>0.7</v>
       </c>
       <c r="P54" s="70">
-        <f t="shared" ref="P54" si="28">H54*0.7</f>
+        <f t="shared" ref="P54" si="31">H54*0.7</f>
         <v>0.7</v>
       </c>
       <c r="Q54" s="70">
-        <f t="shared" ref="Q54" si="29">I54*0.7</f>
+        <f t="shared" ref="Q54" si="32">I54*0.7</f>
         <v>0.7</v>
       </c>
       <c r="R54" s="104">
-        <f t="shared" ref="R54" si="30">J54*0.7</f>
+        <f t="shared" ref="R54" si="33">J54*0.7</f>
         <v>0.7</v>
       </c>
       <c r="S54" s="100">
@@ -29012,11 +29073,11 @@
       </c>
       <c r="AI54" s="153"/>
       <c r="AJ54" s="152" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>R-SW_Att_LPG_N1</v>
       </c>
       <c r="AK54" s="152" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>Residential Liquid Petroleum Gas- New 2 SH + WH</v>
       </c>
       <c r="AL54" s="153" t="s">
@@ -29102,11 +29163,11 @@
       </c>
       <c r="AI55" s="153"/>
       <c r="AJ55" s="152" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>R-SH_Att_WOO_N1</v>
       </c>
       <c r="AK55" s="152" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>Residential Biomass Boiler - New 1 SH</v>
       </c>
       <c r="AL55" s="153" t="s">
@@ -29151,19 +29212,19 @@
       <c r="M56" s="79"/>
       <c r="N56" s="92"/>
       <c r="O56" s="69">
-        <f t="shared" ref="O56:R58" si="31">G56*0.7</f>
+        <f t="shared" ref="O56:R58" si="34">G56*0.7</f>
         <v>0.7</v>
       </c>
       <c r="P56" s="70">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>0.7</v>
       </c>
       <c r="Q56" s="70">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>0.7</v>
       </c>
       <c r="R56" s="104">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>0.7</v>
       </c>
       <c r="S56" s="100">
@@ -29204,11 +29265,11 @@
       </c>
       <c r="AI56" s="156"/>
       <c r="AJ56" s="155" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>R-SW_Att_WOO_N1</v>
       </c>
       <c r="AK56" s="155" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>Residential Biomass Boiler - New 2 SH + WH</v>
       </c>
       <c r="AL56" s="156" t="s">
@@ -29252,19 +29313,19 @@
       <c r="M57" s="78"/>
       <c r="N57" s="90"/>
       <c r="O57" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>0.7</v>
       </c>
       <c r="P57" s="76">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>0.7</v>
       </c>
       <c r="Q57" s="76">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>0.7</v>
       </c>
       <c r="R57" s="105">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>0.7</v>
       </c>
       <c r="S57" s="101">
@@ -29305,11 +29366,11 @@
       </c>
       <c r="AI57" s="156"/>
       <c r="AJ57" s="155" t="str">
-        <f t="shared" ref="AJ57:AJ58" si="32">C57</f>
+        <f t="shared" ref="AJ57:AJ58" si="35">C57</f>
         <v>*R-H_Apt_HVO_N1</v>
       </c>
       <c r="AK57" s="155" t="str">
-        <f t="shared" ref="AK57:AK58" si="33">D57</f>
+        <f t="shared" ref="AK57:AK58" si="36">D57</f>
         <v>Residential  Hydrotreated vegetable oil - New 1 SH</v>
       </c>
       <c r="AL57" s="156" t="s">
@@ -29353,19 +29414,19 @@
       <c r="M58" s="97"/>
       <c r="N58" s="98"/>
       <c r="O58" s="346">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>0.7</v>
       </c>
       <c r="P58" s="73">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>0.7</v>
       </c>
       <c r="Q58" s="73">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>0.7</v>
       </c>
       <c r="R58" s="106">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>0.7</v>
       </c>
       <c r="S58" s="102">
@@ -29406,11 +29467,11 @@
       </c>
       <c r="AI58" s="156"/>
       <c r="AJ58" s="155" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="35"/>
         <v>*R-H_Apt_HVO_N2</v>
       </c>
       <c r="AK58" s="155" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="36"/>
         <v>Residential  Hydrotreated vegetable oil - New 1 SH + WH</v>
       </c>
       <c r="AL58" s="156" t="s">
@@ -29550,11 +29611,11 @@
       </c>
       <c r="AI60" s="151"/>
       <c r="AJ60" s="150" t="str">
-        <f t="shared" ref="AJ60:AK66" si="34">C62</f>
+        <f t="shared" ref="AJ60:AK66" si="37">C62</f>
         <v>R-SH_Att_ELC_HPN1</v>
       </c>
       <c r="AK60" s="150" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>Residential Electric Heat Pump - Air to Air - SH</v>
       </c>
       <c r="AL60" s="151" t="s">
@@ -29604,11 +29665,11 @@
       <c r="AG61" s="81"/>
       <c r="AI61" s="153"/>
       <c r="AJ61" s="152" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>R-HC_Att_ELC_HPN1</v>
       </c>
       <c r="AK61" s="152" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>Residential Electric Heat Pump - Air to Air - SH + SC</v>
       </c>
       <c r="AL61" s="153" t="s">
@@ -29697,11 +29758,11 @@
       </c>
       <c r="AI62" s="153"/>
       <c r="AJ62" s="152" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>R-SH_Att_ELC_HPN2</v>
       </c>
       <c r="AK62" s="152" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>Residential Electric Heat Pump - Air to Water - SH</v>
       </c>
       <c r="AL62" s="153" t="s">
@@ -29801,11 +29862,11 @@
       </c>
       <c r="AI63" s="153"/>
       <c r="AJ63" s="152" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>R-SW_Att_ELC_HPN1</v>
       </c>
       <c r="AK63" s="152" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>Residential Electric Heat Pump - Air to Water - SH + WH</v>
       </c>
       <c r="AL63" s="153" t="s">
@@ -29894,11 +29955,11 @@
       </c>
       <c r="AI64" s="303"/>
       <c r="AJ64" s="152" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>R-SW_Att_SOL_HPN2</v>
       </c>
       <c r="AK64" s="152" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>Residential Electric Heat Pump - Air to Water - SH + WH + Solar</v>
       </c>
       <c r="AL64" s="153" t="s">
@@ -29950,15 +30011,15 @@
         <v>0.7</v>
       </c>
       <c r="P65" s="70">
-        <f t="shared" ref="P65:P66" si="35">H65*0.7</f>
+        <f t="shared" ref="P65:P66" si="38">H65*0.7</f>
         <v>0.76999999999999991</v>
       </c>
       <c r="Q65" s="70">
-        <f t="shared" ref="Q65:Q66" si="36">I65*0.7</f>
+        <f t="shared" ref="Q65:Q66" si="39">I65*0.7</f>
         <v>0.86333333333333329</v>
       </c>
       <c r="R65" s="104">
-        <f t="shared" ref="R65:R66" si="37">J65*0.7</f>
+        <f t="shared" ref="R65:R66" si="40">J65*0.7</f>
         <v>0.93333333333333324</v>
       </c>
       <c r="S65" s="100">
@@ -29999,11 +30060,11 @@
       </c>
       <c r="AI65" s="303"/>
       <c r="AJ65" s="152" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>R-SH_Att_ELC_HPN3</v>
       </c>
       <c r="AK65" s="152" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>Residential Electric Heat Pump - Ground to Water - SH</v>
       </c>
       <c r="AL65" s="153" t="s">
@@ -30052,15 +30113,15 @@
         <v>0.7</v>
       </c>
       <c r="P66" s="76">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>0.77700000000000002</v>
       </c>
       <c r="Q66" s="76">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>0.83299999999999996</v>
       </c>
       <c r="R66" s="105">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v>0.83299999999999996</v>
       </c>
       <c r="S66" s="101">
@@ -30105,11 +30166,11 @@
       </c>
       <c r="AI66" s="159"/>
       <c r="AJ66" s="155" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>R-HC_Att_ELC_HPN2</v>
       </c>
       <c r="AK66" s="155" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>Residential Electric Heat Pump - Ground to Water - SH + SC</v>
       </c>
       <c r="AL66" s="156" t="s">
@@ -30415,15 +30476,15 @@
         <v>0.7</v>
       </c>
       <c r="P70" s="341">
-        <f t="shared" ref="P70:P71" si="38">H70*0.7</f>
+        <f t="shared" ref="P70:P71" si="41">H70*0.7</f>
         <v>0.75185185185185177</v>
       </c>
       <c r="Q70" s="341">
-        <f t="shared" ref="Q70:Q71" si="39">I70*0.7</f>
+        <f t="shared" ref="Q70:Q71" si="42">I70*0.7</f>
         <v>0.88148148148148131</v>
       </c>
       <c r="R70" s="342">
-        <f t="shared" ref="R70:R71" si="40">J70*0.7</f>
+        <f t="shared" ref="R70:R71" si="43">J70*0.7</f>
         <v>0.88148148148148131</v>
       </c>
       <c r="S70" s="136">
@@ -30521,15 +30582,15 @@
         <v>0.77777777777777757</v>
       </c>
       <c r="P71" s="348">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>0.8037037037037037</v>
       </c>
       <c r="Q71" s="348">
-        <f t="shared" si="39"/>
+        <f t="shared" si="42"/>
         <v>0.8037037037037037</v>
       </c>
       <c r="R71" s="349">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>0.82962962962962949</v>
       </c>
       <c r="S71" s="74">
@@ -30624,11 +30685,11 @@
       <c r="AG72" s="81"/>
       <c r="AI72" s="306"/>
       <c r="AJ72" s="150" t="str">
-        <f t="shared" ref="AJ72:AK73" si="41">C78</f>
+        <f t="shared" ref="AJ72:AK73" si="44">C78</f>
         <v>R-WH_Att_ELC_N1</v>
       </c>
       <c r="AK72" s="150" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="44"/>
         <v xml:space="preserve">Residential Electric Water Heater </v>
       </c>
       <c r="AL72" s="151" t="s">
@@ -30677,15 +30738,15 @@
         <v>0.7</v>
       </c>
       <c r="P73" s="348">
-        <f t="shared" ref="P73" si="42">H73*0.7</f>
+        <f t="shared" ref="P73" si="45">H73*0.7</f>
         <v>0.73360000000000003</v>
       </c>
       <c r="Q73" s="348">
-        <f t="shared" ref="Q73" si="43">I73*0.7</f>
+        <f t="shared" ref="Q73" si="46">I73*0.7</f>
         <v>0.76789999999999992</v>
       </c>
       <c r="R73" s="349">
-        <f t="shared" ref="R73" si="44">J73*0.7</f>
+        <f t="shared" ref="R73" si="47">J73*0.7</f>
         <v>0.81269999999999998</v>
       </c>
       <c r="S73" s="5">
@@ -30729,11 +30790,11 @@
       </c>
       <c r="AI73" s="4"/>
       <c r="AJ73" s="152" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="44"/>
         <v>R-WH_Att_SOL_N1</v>
       </c>
       <c r="AK73" s="152" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="44"/>
         <v xml:space="preserve">Residential Solar Water Heater </v>
       </c>
       <c r="AL73" s="153" t="s">
@@ -31368,34 +31429,34 @@
       <c r="F88" s="63" t="s">
         <v>334</v>
       </c>
-      <c r="G88" s="507" t="s">
+      <c r="G88" s="506" t="s">
         <v>335</v>
       </c>
-      <c r="H88" s="508"/>
-      <c r="I88" s="508"/>
-      <c r="J88" s="509"/>
-      <c r="K88" s="507" t="s">
+      <c r="H88" s="507"/>
+      <c r="I88" s="507"/>
+      <c r="J88" s="508"/>
+      <c r="K88" s="506" t="s">
         <v>336</v>
       </c>
-      <c r="L88" s="508"/>
-      <c r="M88" s="508"/>
-      <c r="N88" s="509"/>
-      <c r="O88" s="507" t="s">
+      <c r="L88" s="507"/>
+      <c r="M88" s="507"/>
+      <c r="N88" s="508"/>
+      <c r="O88" s="506" t="s">
         <v>337</v>
       </c>
-      <c r="P88" s="508"/>
-      <c r="Q88" s="508"/>
-      <c r="R88" s="509"/>
-      <c r="S88" s="507" t="s">
+      <c r="P88" s="507"/>
+      <c r="Q88" s="507"/>
+      <c r="R88" s="508"/>
+      <c r="S88" s="506" t="s">
         <v>338</v>
       </c>
-      <c r="T88" s="509"/>
-      <c r="U88" s="498" t="s">
+      <c r="T88" s="508"/>
+      <c r="U88" s="500" t="s">
         <v>339</v>
       </c>
-      <c r="V88" s="499"/>
-      <c r="W88" s="499"/>
-      <c r="X88" s="500"/>
+      <c r="V88" s="501"/>
+      <c r="W88" s="501"/>
+      <c r="X88" s="502"/>
       <c r="Y88" s="107"/>
       <c r="Z88" s="107"/>
       <c r="AA88" s="115" t="s">
@@ -31490,34 +31551,34 @@
       <c r="D90" s="85"/>
       <c r="E90" s="85"/>
       <c r="F90" s="86"/>
-      <c r="G90" s="501" t="s">
+      <c r="G90" s="503" t="s">
         <v>55</v>
       </c>
-      <c r="H90" s="502"/>
-      <c r="I90" s="502"/>
-      <c r="J90" s="503"/>
-      <c r="K90" s="502" t="s">
+      <c r="H90" s="504"/>
+      <c r="I90" s="504"/>
+      <c r="J90" s="505"/>
+      <c r="K90" s="504" t="s">
         <v>55</v>
       </c>
-      <c r="L90" s="502"/>
-      <c r="M90" s="502"/>
-      <c r="N90" s="503"/>
-      <c r="O90" s="501" t="s">
+      <c r="L90" s="504"/>
+      <c r="M90" s="504"/>
+      <c r="N90" s="505"/>
+      <c r="O90" s="503" t="s">
         <v>55</v>
       </c>
-      <c r="P90" s="502"/>
-      <c r="Q90" s="502"/>
-      <c r="R90" s="503"/>
-      <c r="S90" s="504" t="s">
+      <c r="P90" s="504"/>
+      <c r="Q90" s="504"/>
+      <c r="R90" s="505"/>
+      <c r="S90" s="509" t="s">
         <v>312</v>
       </c>
-      <c r="T90" s="505"/>
-      <c r="U90" s="504" t="s">
+      <c r="T90" s="510"/>
+      <c r="U90" s="509" t="s">
         <v>1007</v>
       </c>
-      <c r="V90" s="506"/>
-      <c r="W90" s="506"/>
-      <c r="X90" s="505"/>
+      <c r="V90" s="511"/>
+      <c r="W90" s="511"/>
+      <c r="X90" s="510"/>
       <c r="Y90" s="475" t="s">
         <v>1019</v>
       </c>
@@ -31692,15 +31753,15 @@
         <v>0.7</v>
       </c>
       <c r="P92" s="70">
-        <f t="shared" ref="P92:P94" si="45">H92*0.7</f>
+        <f t="shared" ref="P92:P94" si="48">H92*0.7</f>
         <v>0.7</v>
       </c>
       <c r="Q92" s="70">
-        <f t="shared" ref="Q92:Q94" si="46">I92*0.7</f>
+        <f t="shared" ref="Q92:Q94" si="49">I92*0.7</f>
         <v>0.7</v>
       </c>
       <c r="R92" s="104">
-        <f t="shared" ref="R92:R94" si="47">J92*0.7</f>
+        <f t="shared" ref="R92:R94" si="50">J92*0.7</f>
         <v>0.7</v>
       </c>
       <c r="S92" s="100">
@@ -31741,11 +31802,11 @@
       </c>
       <c r="AI92" s="153"/>
       <c r="AJ92" s="152" t="str">
-        <f t="shared" ref="AJ92:AJ104" si="48">C92</f>
+        <f t="shared" ref="AJ92:AJ104" si="51">C92</f>
         <v>R-SW_Det_KER_N1</v>
       </c>
       <c r="AK92" s="152" t="str">
-        <f t="shared" ref="AK92:AK104" si="49">D92</f>
+        <f t="shared" ref="AK92:AK104" si="52">D92</f>
         <v>Residential Kerosene Heating Oil - New 2 SH + WH</v>
       </c>
       <c r="AL92" s="153" t="s">
@@ -31794,15 +31855,15 @@
         <v>0.7</v>
       </c>
       <c r="P93" s="76">
-        <f t="shared" si="45"/>
+        <f t="shared" si="48"/>
         <v>0.7</v>
       </c>
       <c r="Q93" s="76">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>0.7</v>
       </c>
       <c r="R93" s="105">
-        <f t="shared" si="47"/>
+        <f t="shared" si="50"/>
         <v>0.7</v>
       </c>
       <c r="S93" s="101">
@@ -31847,11 +31908,11 @@
       </c>
       <c r="AI93" s="153"/>
       <c r="AJ93" s="152" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>R-SW_Det_KER_N2</v>
       </c>
       <c r="AK93" s="152" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>Residential Kerosene Heating Oil - New 3 SH+WH + Solar</v>
       </c>
       <c r="AL93" s="153" t="s">
@@ -31900,15 +31961,15 @@
         <v>0.7</v>
       </c>
       <c r="P94" s="70">
-        <f t="shared" si="45"/>
+        <f t="shared" si="48"/>
         <v>0.71749999999999992</v>
       </c>
       <c r="Q94" s="70">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>0.71749999999999992</v>
       </c>
       <c r="R94" s="104">
-        <f t="shared" si="47"/>
+        <f t="shared" si="50"/>
         <v>0.71749999999999992</v>
       </c>
       <c r="S94" s="100">
@@ -31953,11 +32014,11 @@
       </c>
       <c r="AI94" s="153"/>
       <c r="AJ94" s="152" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>R-SW_Det_KER_N3</v>
       </c>
       <c r="AK94" s="152" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>Residential Kerosene Heating Oil - New 3 SH+WH + Wood Stove</v>
       </c>
       <c r="AL94" s="154" t="s">
@@ -32041,11 +32102,11 @@
       </c>
       <c r="AI95" s="153"/>
       <c r="AJ95" s="152" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>R-SH_Det_GAS_N1</v>
       </c>
       <c r="AK95" s="152" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>Residential Natural Gas Heating - New 1 SH</v>
       </c>
       <c r="AL95" s="153" t="s">
@@ -32094,15 +32155,15 @@
         <v>0.7</v>
       </c>
       <c r="P96" s="70">
-        <f t="shared" ref="P96:P98" si="50">H96*0.7</f>
+        <f t="shared" ref="P96:P98" si="53">H96*0.7</f>
         <v>0.7</v>
       </c>
       <c r="Q96" s="70">
-        <f t="shared" ref="Q96:Q98" si="51">I96*0.7</f>
+        <f t="shared" ref="Q96:Q98" si="54">I96*0.7</f>
         <v>0.7</v>
       </c>
       <c r="R96" s="104">
-        <f t="shared" ref="R96:R98" si="52">J96*0.7</f>
+        <f t="shared" ref="R96:R98" si="55">J96*0.7</f>
         <v>0.7</v>
       </c>
       <c r="S96" s="100">
@@ -32143,11 +32204,11 @@
       </c>
       <c r="AI96" s="153"/>
       <c r="AJ96" s="152" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>R-SW_Det_GAS_N1</v>
       </c>
       <c r="AK96" s="152" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>Residential Natural Gas Heating - New 2 SH + WH</v>
       </c>
       <c r="AL96" s="153" t="s">
@@ -32196,15 +32257,15 @@
         <v>0.7</v>
       </c>
       <c r="P97" s="76">
-        <f t="shared" si="50"/>
+        <f t="shared" si="53"/>
         <v>0.7</v>
       </c>
       <c r="Q97" s="76">
-        <f t="shared" si="51"/>
+        <f t="shared" si="54"/>
         <v>0.7</v>
       </c>
       <c r="R97" s="105">
-        <f t="shared" si="52"/>
+        <f t="shared" si="55"/>
         <v>0.7</v>
       </c>
       <c r="S97" s="101">
@@ -32249,11 +32310,11 @@
       </c>
       <c r="AI97" s="153"/>
       <c r="AJ97" s="152" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>R-SW_Det_GAS_N2</v>
       </c>
       <c r="AK97" s="152" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>Residential Natural Gas Heating - New 3 SH + WH + Solar</v>
       </c>
       <c r="AL97" s="153" t="s">
@@ -32302,15 +32363,15 @@
         <v>0.7</v>
       </c>
       <c r="P98" s="70">
-        <f t="shared" si="50"/>
+        <f t="shared" si="53"/>
         <v>0.71749999999999992</v>
       </c>
       <c r="Q98" s="70">
-        <f t="shared" si="51"/>
+        <f t="shared" si="54"/>
         <v>0.71749999999999992</v>
       </c>
       <c r="R98" s="104">
-        <f t="shared" si="52"/>
+        <f t="shared" si="55"/>
         <v>0.71749999999999992</v>
       </c>
       <c r="S98" s="100">
@@ -32355,11 +32416,11 @@
       </c>
       <c r="AI98" s="153"/>
       <c r="AJ98" s="152" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>R-SW_Det_GAS_N3</v>
       </c>
       <c r="AK98" s="152" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>Residential Natural Gas Heating - New 4 SH + WH + Wood Stove</v>
       </c>
       <c r="AL98" s="153" t="s">
@@ -32445,11 +32506,11 @@
       </c>
       <c r="AI99" s="153"/>
       <c r="AJ99" s="152" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>R-SH_Det_LPG_N1</v>
       </c>
       <c r="AK99" s="152" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>Residential Liquid Petroleum Gas- New 1 SH</v>
       </c>
       <c r="AL99" s="153" t="s">
@@ -32498,15 +32559,15 @@
         <v>0.7</v>
       </c>
       <c r="P100" s="70">
-        <f t="shared" ref="P100" si="53">H100*0.7</f>
+        <f t="shared" ref="P100" si="56">H100*0.7</f>
         <v>0.7</v>
       </c>
       <c r="Q100" s="70">
-        <f t="shared" ref="Q100" si="54">I100*0.7</f>
+        <f t="shared" ref="Q100" si="57">I100*0.7</f>
         <v>0.7</v>
       </c>
       <c r="R100" s="104">
-        <f t="shared" ref="R100" si="55">J100*0.7</f>
+        <f t="shared" ref="R100" si="58">J100*0.7</f>
         <v>0.7</v>
       </c>
       <c r="S100" s="100">
@@ -32547,11 +32608,11 @@
       </c>
       <c r="AI100" s="153"/>
       <c r="AJ100" s="152" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>R-SW_Det_LPG_N1</v>
       </c>
       <c r="AK100" s="152" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>Residential Liquid Petroleum Gas- New 2 SH + WH</v>
       </c>
       <c r="AL100" s="153" t="s">
@@ -32637,11 +32698,11 @@
       </c>
       <c r="AI101" s="153"/>
       <c r="AJ101" s="152" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>R-SH_Det_WOO_N1</v>
       </c>
       <c r="AK101" s="152" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>Residential Biomass Boiler - New 1 SH</v>
       </c>
       <c r="AL101" s="153" t="s">
@@ -32686,19 +32747,19 @@
       <c r="M102" s="79"/>
       <c r="N102" s="92"/>
       <c r="O102" s="69">
-        <f t="shared" ref="O102:R104" si="56">G102*0.7</f>
+        <f t="shared" ref="O102:R104" si="59">G102*0.7</f>
         <v>0.7</v>
       </c>
       <c r="P102" s="70">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>0.7</v>
       </c>
       <c r="Q102" s="70">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>0.7</v>
       </c>
       <c r="R102" s="104">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>0.7</v>
       </c>
       <c r="S102" s="100">
@@ -32739,11 +32800,11 @@
       </c>
       <c r="AI102" s="156"/>
       <c r="AJ102" s="155" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>R-SW_Det_WOO_N1</v>
       </c>
       <c r="AK102" s="155" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>Residential Biomass Boiler - New 2 SH + WH</v>
       </c>
       <c r="AL102" s="156" t="s">
@@ -32787,19 +32848,19 @@
       <c r="M103" s="78"/>
       <c r="N103" s="90"/>
       <c r="O103" s="87">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>0.7</v>
       </c>
       <c r="P103" s="76">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>0.7</v>
       </c>
       <c r="Q103" s="76">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>0.7</v>
       </c>
       <c r="R103" s="105">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>0.7</v>
       </c>
       <c r="S103" s="101">
@@ -32840,11 +32901,11 @@
       </c>
       <c r="AI103" s="156"/>
       <c r="AJ103" s="155" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>*R-H_Apt_HVO_N1</v>
       </c>
       <c r="AK103" s="155" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>Residential  Hydrotreated vegetable oil - New 1 SH</v>
       </c>
       <c r="AL103" s="156" t="s">
@@ -32888,19 +32949,19 @@
       <c r="M104" s="97"/>
       <c r="N104" s="98"/>
       <c r="O104" s="346">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>0.7</v>
       </c>
       <c r="P104" s="73">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>0.7</v>
       </c>
       <c r="Q104" s="73">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>0.7</v>
       </c>
       <c r="R104" s="106">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>0.7</v>
       </c>
       <c r="S104" s="102">
@@ -32941,11 +33002,11 @@
       </c>
       <c r="AI104" s="156"/>
       <c r="AJ104" s="155" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>*R-H_Apt_HVO_N2</v>
       </c>
       <c r="AK104" s="155" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>Residential  Hydrotreated vegetable oil - New 1 SH + WH</v>
       </c>
       <c r="AL104" s="156" t="s">
@@ -33085,11 +33146,11 @@
       </c>
       <c r="AI106" s="151"/>
       <c r="AJ106" s="150" t="str">
-        <f t="shared" ref="AJ106:AJ112" si="57">C108</f>
+        <f t="shared" ref="AJ106:AJ112" si="60">C108</f>
         <v>R-SH_Det_ELC_HPN1</v>
       </c>
       <c r="AK106" s="150" t="str">
-        <f t="shared" ref="AK106:AK112" si="58">D108</f>
+        <f t="shared" ref="AK106:AK112" si="61">D108</f>
         <v>Residential Electric Heat Pump - Air to Air - SH</v>
       </c>
       <c r="AL106" s="151" t="s">
@@ -33139,11 +33200,11 @@
       <c r="AG107" s="81"/>
       <c r="AI107" s="153"/>
       <c r="AJ107" s="152" t="str">
-        <f t="shared" si="57"/>
+        <f t="shared" si="60"/>
         <v>R-HC_Det_ELC_HPN1</v>
       </c>
       <c r="AK107" s="152" t="str">
-        <f t="shared" si="58"/>
+        <f t="shared" si="61"/>
         <v>Residential Electric Heat Pump - Air to Air - SH + SC</v>
       </c>
       <c r="AL107" s="153" t="s">
@@ -33229,11 +33290,11 @@
       </c>
       <c r="AI108" s="153"/>
       <c r="AJ108" s="152" t="str">
-        <f t="shared" si="57"/>
+        <f t="shared" si="60"/>
         <v>R-SH_Det_ELC_HPN2</v>
       </c>
       <c r="AK108" s="152" t="str">
-        <f t="shared" si="58"/>
+        <f t="shared" si="61"/>
         <v>Residential Electric Heat Pump - Air to Water - SH</v>
       </c>
       <c r="AL108" s="153" t="s">
@@ -33327,11 +33388,11 @@
       </c>
       <c r="AI109" s="153"/>
       <c r="AJ109" s="152" t="str">
-        <f t="shared" si="57"/>
+        <f t="shared" si="60"/>
         <v>R-SW_Det_ELC_HPN1</v>
       </c>
       <c r="AK109" s="152" t="str">
-        <f t="shared" si="58"/>
+        <f t="shared" si="61"/>
         <v>Residential Electric Heat Pump - Air to Water - SH + WH</v>
       </c>
       <c r="AL109" s="153" t="s">
@@ -33417,11 +33478,11 @@
       </c>
       <c r="AI110" s="303"/>
       <c r="AJ110" s="152" t="str">
-        <f t="shared" si="57"/>
+        <f t="shared" si="60"/>
         <v>R-SW_Det_SOL_HPN2</v>
       </c>
       <c r="AK110" s="152" t="str">
-        <f t="shared" si="58"/>
+        <f t="shared" si="61"/>
         <v>Residential Electric Heat Pump - Air to Water - SH + WH + Solar</v>
       </c>
       <c r="AL110" s="153" t="s">
@@ -33470,15 +33531,15 @@
         <v>0.7</v>
       </c>
       <c r="P111" s="70">
-        <f t="shared" ref="P111:P112" si="59">H111*0.7</f>
+        <f t="shared" ref="P111:P112" si="62">H111*0.7</f>
         <v>0.76999999999999991</v>
       </c>
       <c r="Q111" s="70">
-        <f t="shared" ref="Q111:Q112" si="60">I111*0.7</f>
+        <f t="shared" ref="Q111:Q112" si="63">I111*0.7</f>
         <v>0.86333333333333329</v>
       </c>
       <c r="R111" s="104">
-        <f t="shared" ref="R111:R112" si="61">J111*0.7</f>
+        <f t="shared" ref="R111:R112" si="64">J111*0.7</f>
         <v>0.93333333333333324</v>
       </c>
       <c r="S111" s="100">
@@ -33519,11 +33580,11 @@
       </c>
       <c r="AI111" s="303"/>
       <c r="AJ111" s="152" t="str">
-        <f t="shared" si="57"/>
+        <f t="shared" si="60"/>
         <v>R-SH_Det_ELC_HPN3</v>
       </c>
       <c r="AK111" s="152" t="str">
-        <f t="shared" si="58"/>
+        <f t="shared" si="61"/>
         <v>Residential Electric Heat Pump - Ground to Water - SH</v>
       </c>
       <c r="AL111" s="153" t="s">
@@ -33572,15 +33633,15 @@
         <v>0.7</v>
       </c>
       <c r="P112" s="76">
-        <f t="shared" si="59"/>
+        <f t="shared" si="62"/>
         <v>0.77700000000000002</v>
       </c>
       <c r="Q112" s="76">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>0.83299999999999996</v>
       </c>
       <c r="R112" s="105">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>0.83299999999999996</v>
       </c>
       <c r="S112" s="101">
@@ -33625,11 +33686,11 @@
       </c>
       <c r="AI112" s="159"/>
       <c r="AJ112" s="155" t="str">
-        <f t="shared" si="57"/>
+        <f t="shared" si="60"/>
         <v>R-HC_Det_ELC_HPN2</v>
       </c>
       <c r="AK112" s="155" t="str">
-        <f t="shared" si="58"/>
+        <f t="shared" si="61"/>
         <v>Residential Electric Heat Pump - Ground to Water - SH + SC</v>
       </c>
       <c r="AL112" s="156" t="s">
@@ -33920,15 +33981,15 @@
         <v>0.7</v>
       </c>
       <c r="P116" s="341">
-        <f t="shared" ref="P116:P117" si="62">H116*0.7</f>
+        <f t="shared" ref="P116:P117" si="65">H116*0.7</f>
         <v>0.75185185185185177</v>
       </c>
       <c r="Q116" s="341">
-        <f t="shared" ref="Q116:Q117" si="63">I116*0.7</f>
+        <f t="shared" ref="Q116:Q117" si="66">I116*0.7</f>
         <v>0.88148148148148131</v>
       </c>
       <c r="R116" s="342">
-        <f t="shared" ref="R116:R117" si="64">J116*0.7</f>
+        <f t="shared" ref="R116:R117" si="67">J116*0.7</f>
         <v>0.88148148148148131</v>
       </c>
       <c r="S116" s="136">
@@ -34022,15 +34083,15 @@
         <v>0.77777777777777757</v>
       </c>
       <c r="P117" s="348">
-        <f t="shared" si="62"/>
+        <f t="shared" si="65"/>
         <v>0.8037037037037037</v>
       </c>
       <c r="Q117" s="348">
-        <f t="shared" si="63"/>
+        <f t="shared" si="66"/>
         <v>0.8037037037037037</v>
       </c>
       <c r="R117" s="349">
-        <f t="shared" si="64"/>
+        <f t="shared" si="67"/>
         <v>0.82962962962962949</v>
       </c>
       <c r="S117" s="74">
@@ -34125,11 +34186,11 @@
       <c r="AG118" s="81"/>
       <c r="AI118" s="306"/>
       <c r="AJ118" s="150" t="str">
-        <f t="shared" ref="AJ118:AJ119" si="65">C124</f>
+        <f t="shared" ref="AJ118:AJ119" si="68">C124</f>
         <v>R-WH_Det_ELC_N1</v>
       </c>
       <c r="AK118" s="150" t="str">
-        <f t="shared" ref="AK118:AK119" si="66">D124</f>
+        <f t="shared" ref="AK118:AK119" si="69">D124</f>
         <v xml:space="preserve">Residential Electric Water Heater </v>
       </c>
       <c r="AL118" s="151" t="s">
@@ -34178,15 +34239,15 @@
         <v>0.7</v>
       </c>
       <c r="P119" s="348">
-        <f t="shared" ref="P119" si="67">H119*0.7</f>
+        <f t="shared" ref="P119" si="70">H119*0.7</f>
         <v>0.73360000000000003</v>
       </c>
       <c r="Q119" s="348">
-        <f t="shared" ref="Q119" si="68">I119*0.7</f>
+        <f t="shared" ref="Q119" si="71">I119*0.7</f>
         <v>0.76789999999999992</v>
       </c>
       <c r="R119" s="349">
-        <f t="shared" ref="R119" si="69">J119*0.7</f>
+        <f t="shared" ref="R119" si="72">J119*0.7</f>
         <v>0.81269999999999998</v>
       </c>
       <c r="S119" s="5">
@@ -34230,11 +34291,11 @@
       </c>
       <c r="AI119" s="4"/>
       <c r="AJ119" s="152" t="str">
-        <f t="shared" si="65"/>
+        <f t="shared" si="68"/>
         <v>R-WH_Det_SOL_N1</v>
       </c>
       <c r="AK119" s="152" t="str">
-        <f t="shared" si="66"/>
+        <f t="shared" si="69"/>
         <v xml:space="preserve">Residential Solar Water Heater </v>
       </c>
       <c r="AL119" s="153" t="s">
@@ -34951,7 +35012,7 @@
         <v>3</v>
       </c>
       <c r="T141" s="479">
-        <f t="shared" ref="T141:T150" si="70">U141/$U$149</f>
+        <f t="shared" ref="T141:T150" si="73">U141/$U$149</f>
         <v>0.72929037751472525</v>
       </c>
       <c r="U141" s="480">
@@ -34981,7 +35042,7 @@
         <v>5</v>
       </c>
       <c r="T142" s="479">
-        <f t="shared" si="70"/>
+        <f t="shared" si="73"/>
         <v>0.79101166159768732</v>
       </c>
       <c r="U142" s="480">
@@ -34995,7 +35056,7 @@
         <v>8</v>
       </c>
       <c r="T143" s="479">
-        <f t="shared" si="70"/>
+        <f t="shared" si="73"/>
         <v>0.85077698714062355</v>
       </c>
       <c r="U143" s="480">
@@ -35009,7 +35070,7 @@
         <v>10</v>
       </c>
       <c r="T144" s="479">
-        <f t="shared" si="70"/>
+        <f t="shared" si="73"/>
         <v>0.86872586872586877</v>
       </c>
       <c r="U144" s="478">
@@ -35030,7 +35091,7 @@
         <v>15</v>
       </c>
       <c r="T145" s="469">
-        <f t="shared" si="70"/>
+        <f t="shared" si="73"/>
         <v>0.91505791505791501</v>
       </c>
       <c r="U145" s="5">
@@ -35057,7 +35118,7 @@
         <v>18</v>
       </c>
       <c r="T146" s="469">
-        <f t="shared" si="70"/>
+        <f t="shared" si="73"/>
         <v>0.92277992277992282</v>
       </c>
       <c r="U146" s="5">
@@ -35086,7 +35147,7 @@
         <v>20</v>
       </c>
       <c r="T147" s="479">
-        <f t="shared" si="70"/>
+        <f t="shared" si="73"/>
         <v>0.93436293436293438</v>
       </c>
       <c r="U147" s="478">
@@ -35116,7 +35177,7 @@
         <v>24</v>
       </c>
       <c r="T148" s="469">
-        <f t="shared" si="70"/>
+        <f t="shared" si="73"/>
         <v>0.94594594594594594</v>
       </c>
       <c r="U148" s="5">
@@ -35145,7 +35206,7 @@
         <v>30</v>
       </c>
       <c r="T149" s="469">
-        <f t="shared" si="70"/>
+        <f t="shared" si="73"/>
         <v>1</v>
       </c>
       <c r="U149" s="5">
@@ -35174,7 +35235,7 @@
         <v>35</v>
       </c>
       <c r="T150" s="469">
-        <f t="shared" si="70"/>
+        <f t="shared" si="73"/>
         <v>1.0791505791505791</v>
       </c>
       <c r="U150" s="5">
@@ -35207,7 +35268,7 @@
       <c r="P153" s="8"/>
     </row>
     <row r="154" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="L154" s="5" t="s">
+      <c r="L154" s="286" t="s">
         <v>1021</v>
       </c>
     </row>
@@ -35219,6 +35280,26 @@
     <row r="162" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="G90:J90"/>
+    <mergeCell ref="K90:N90"/>
+    <mergeCell ref="O90:R90"/>
+    <mergeCell ref="S90:T90"/>
+    <mergeCell ref="U90:X90"/>
+    <mergeCell ref="G88:J88"/>
+    <mergeCell ref="K88:N88"/>
+    <mergeCell ref="O88:R88"/>
+    <mergeCell ref="S88:T88"/>
+    <mergeCell ref="U88:X88"/>
+    <mergeCell ref="G44:J44"/>
+    <mergeCell ref="K44:N44"/>
+    <mergeCell ref="O44:R44"/>
+    <mergeCell ref="S44:T44"/>
+    <mergeCell ref="U44:X44"/>
+    <mergeCell ref="G42:J42"/>
+    <mergeCell ref="K42:N42"/>
+    <mergeCell ref="O42:R42"/>
+    <mergeCell ref="S42:T42"/>
+    <mergeCell ref="U42:X42"/>
     <mergeCell ref="U4:X4"/>
     <mergeCell ref="U6:X6"/>
     <mergeCell ref="G4:J4"/>
@@ -35229,32 +35310,15 @@
     <mergeCell ref="O6:R6"/>
     <mergeCell ref="K6:N6"/>
     <mergeCell ref="G6:J6"/>
-    <mergeCell ref="G42:J42"/>
-    <mergeCell ref="K42:N42"/>
-    <mergeCell ref="O42:R42"/>
-    <mergeCell ref="S42:T42"/>
-    <mergeCell ref="U42:X42"/>
-    <mergeCell ref="G44:J44"/>
-    <mergeCell ref="K44:N44"/>
-    <mergeCell ref="O44:R44"/>
-    <mergeCell ref="S44:T44"/>
-    <mergeCell ref="U44:X44"/>
-    <mergeCell ref="G88:J88"/>
-    <mergeCell ref="K88:N88"/>
-    <mergeCell ref="O88:R88"/>
-    <mergeCell ref="S88:T88"/>
-    <mergeCell ref="U88:X88"/>
-    <mergeCell ref="G90:J90"/>
-    <mergeCell ref="K90:N90"/>
-    <mergeCell ref="O90:R90"/>
-    <mergeCell ref="S90:T90"/>
-    <mergeCell ref="U90:X90"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="L154" r:id="rId1" xr:uid="{95A20A04-5652-40C1-8115-13257477A004}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -35388,12 +35452,12 @@
       <c r="I5" s="177"/>
       <c r="J5" s="177"/>
       <c r="K5" s="177"/>
-      <c r="L5" s="498" t="s">
+      <c r="L5" s="500" t="s">
         <v>339</v>
       </c>
-      <c r="M5" s="499"/>
-      <c r="N5" s="499"/>
-      <c r="O5" s="500"/>
+      <c r="M5" s="501"/>
+      <c r="N5" s="501"/>
+      <c r="O5" s="502"/>
       <c r="P5" s="107"/>
       <c r="Q5" s="107" t="s">
         <v>340</v>
@@ -35424,12 +35488,12 @@
       <c r="I6" s="84"/>
       <c r="J6" s="84"/>
       <c r="K6" s="84"/>
-      <c r="L6" s="504" t="s">
+      <c r="L6" s="509" t="s">
         <v>1007</v>
       </c>
-      <c r="M6" s="506"/>
-      <c r="N6" s="506"/>
-      <c r="O6" s="505"/>
+      <c r="M6" s="511"/>
+      <c r="N6" s="511"/>
+      <c r="O6" s="510"/>
       <c r="P6" s="475" t="s">
         <v>1019</v>
       </c>
@@ -36042,10 +36106,10 @@
       <c r="C18" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="R18" s="510" t="s">
+      <c r="R18" s="512" t="s">
         <v>699</v>
       </c>
-      <c r="S18" s="510"/>
+      <c r="S18" s="512"/>
     </row>
     <row r="19" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C19" s="197" t="s">
@@ -36072,8 +36136,8 @@
       <c r="J19" s="199" t="s">
         <v>311</v>
       </c>
-      <c r="R19" s="510"/>
-      <c r="S19" s="510"/>
+      <c r="R19" s="512"/>
+      <c r="S19" s="512"/>
     </row>
     <row r="20" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C20" s="172" t="s">
@@ -36096,8 +36160,8 @@
       <c r="J20" s="174" t="s">
         <v>445</v>
       </c>
-      <c r="R20" s="510"/>
-      <c r="S20" s="510"/>
+      <c r="R20" s="512"/>
+      <c r="S20" s="512"/>
     </row>
     <row r="21" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C21" s="172" t="s">
@@ -36121,8 +36185,8 @@
       <c r="J21" s="174" t="s">
         <v>445</v>
       </c>
-      <c r="R21" s="510"/>
-      <c r="S21" s="510"/>
+      <c r="R21" s="512"/>
+      <c r="S21" s="512"/>
     </row>
     <row r="22" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C22" s="172" t="s">
@@ -36146,8 +36210,8 @@
       <c r="J22" s="174" t="s">
         <v>445</v>
       </c>
-      <c r="R22" s="510"/>
-      <c r="S22" s="510"/>
+      <c r="R22" s="512"/>
+      <c r="S22" s="512"/>
     </row>
     <row r="23" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C23" s="172" t="s">
@@ -36321,23 +36385,23 @@
       <c r="K33" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="L33" s="498" t="s">
+      <c r="L33" s="500" t="s">
         <v>339</v>
       </c>
-      <c r="M33" s="499"/>
-      <c r="N33" s="499"/>
-      <c r="O33" s="500"/>
+      <c r="M33" s="501"/>
+      <c r="N33" s="501"/>
+      <c r="O33" s="502"/>
     </row>
     <row r="34" spans="8:15" x14ac:dyDescent="0.2">
       <c r="H34" s="5" t="s">
         <v>404</v>
       </c>
-      <c r="L34" s="501" t="s">
+      <c r="L34" s="503" t="s">
         <v>345</v>
       </c>
-      <c r="M34" s="502"/>
-      <c r="N34" s="502"/>
-      <c r="O34" s="503"/>
+      <c r="M34" s="504"/>
+      <c r="N34" s="504"/>
+      <c r="O34" s="505"/>
     </row>
     <row r="35" spans="8:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H35" s="5" t="s">
@@ -36676,12 +36740,12 @@
       <c r="I4" s="177"/>
       <c r="J4" s="177"/>
       <c r="K4" s="177"/>
-      <c r="L4" s="498" t="s">
+      <c r="L4" s="500" t="s">
         <v>339</v>
       </c>
-      <c r="M4" s="499"/>
-      <c r="N4" s="499"/>
-      <c r="O4" s="500"/>
+      <c r="M4" s="501"/>
+      <c r="N4" s="501"/>
+      <c r="O4" s="502"/>
       <c r="P4" s="107"/>
       <c r="Q4" s="107" t="s">
         <v>340</v>
@@ -36705,12 +36769,12 @@
       <c r="I5" s="84"/>
       <c r="J5" s="84"/>
       <c r="K5" s="84"/>
-      <c r="L5" s="501" t="s">
+      <c r="L5" s="503" t="s">
         <v>796</v>
       </c>
-      <c r="M5" s="502"/>
-      <c r="N5" s="502"/>
-      <c r="O5" s="503"/>
+      <c r="M5" s="504"/>
+      <c r="N5" s="504"/>
+      <c r="O5" s="505"/>
       <c r="P5" s="108" t="s">
         <v>346</v>
       </c>
@@ -37277,12 +37341,12 @@
       <c r="K27" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="L27" s="498" t="s">
+      <c r="L27" s="500" t="s">
         <v>339</v>
       </c>
-      <c r="M27" s="499"/>
-      <c r="N27" s="499"/>
-      <c r="O27" s="500"/>
+      <c r="M27" s="501"/>
+      <c r="N27" s="501"/>
+      <c r="O27" s="502"/>
       <c r="T27" s="288"/>
       <c r="U27" s="288"/>
     </row>
@@ -37290,12 +37354,12 @@
       <c r="J28" s="5" t="s">
         <v>404</v>
       </c>
-      <c r="L28" s="501" t="s">
+      <c r="L28" s="503" t="s">
         <v>345</v>
       </c>
-      <c r="M28" s="502"/>
-      <c r="N28" s="502"/>
-      <c r="O28" s="503"/>
+      <c r="M28" s="504"/>
+      <c r="N28" s="504"/>
+      <c r="O28" s="505"/>
       <c r="T28" s="288"/>
       <c r="U28" s="288"/>
     </row>
@@ -47719,128 +47783,128 @@
       <c r="C4" s="381" t="s">
         <v>805</v>
       </c>
-      <c r="D4" s="512" t="s">
+      <c r="D4" s="513" t="s">
         <v>806</v>
       </c>
-      <c r="E4" s="511"/>
-      <c r="F4" s="511"/>
-      <c r="G4" s="511"/>
-      <c r="H4" s="513"/>
-      <c r="I4" s="511" t="s">
+      <c r="E4" s="514"/>
+      <c r="F4" s="514"/>
+      <c r="G4" s="514"/>
+      <c r="H4" s="515"/>
+      <c r="I4" s="514" t="s">
         <v>807</v>
       </c>
-      <c r="J4" s="511"/>
-      <c r="K4" s="511"/>
-      <c r="L4" s="511"/>
-      <c r="M4" s="513"/>
-      <c r="N4" s="511" t="s">
+      <c r="J4" s="514"/>
+      <c r="K4" s="514"/>
+      <c r="L4" s="514"/>
+      <c r="M4" s="515"/>
+      <c r="N4" s="514" t="s">
         <v>808</v>
       </c>
-      <c r="O4" s="511"/>
-      <c r="P4" s="511"/>
-      <c r="Q4" s="511"/>
-      <c r="R4" s="513"/>
-      <c r="S4" s="511" t="s">
+      <c r="O4" s="514"/>
+      <c r="P4" s="514"/>
+      <c r="Q4" s="514"/>
+      <c r="R4" s="515"/>
+      <c r="S4" s="514" t="s">
         <v>809</v>
       </c>
-      <c r="T4" s="511"/>
-      <c r="U4" s="511"/>
-      <c r="V4" s="511"/>
-      <c r="W4" s="513"/>
-      <c r="X4" s="511" t="s">
+      <c r="T4" s="514"/>
+      <c r="U4" s="514"/>
+      <c r="V4" s="514"/>
+      <c r="W4" s="515"/>
+      <c r="X4" s="514" t="s">
         <v>810</v>
       </c>
-      <c r="Y4" s="511"/>
-      <c r="Z4" s="511"/>
-      <c r="AA4" s="511"/>
-      <c r="AB4" s="513"/>
-      <c r="AC4" s="511" t="s">
+      <c r="Y4" s="514"/>
+      <c r="Z4" s="514"/>
+      <c r="AA4" s="514"/>
+      <c r="AB4" s="515"/>
+      <c r="AC4" s="514" t="s">
         <v>811</v>
       </c>
-      <c r="AD4" s="511"/>
-      <c r="AE4" s="511"/>
-      <c r="AF4" s="511"/>
-      <c r="AG4" s="513"/>
-      <c r="AH4" s="511" t="s">
+      <c r="AD4" s="514"/>
+      <c r="AE4" s="514"/>
+      <c r="AF4" s="514"/>
+      <c r="AG4" s="515"/>
+      <c r="AH4" s="514" t="s">
         <v>812</v>
       </c>
-      <c r="AI4" s="511"/>
-      <c r="AJ4" s="511"/>
-      <c r="AK4" s="511"/>
-      <c r="AL4" s="513"/>
-      <c r="AM4" s="511" t="s">
+      <c r="AI4" s="514"/>
+      <c r="AJ4" s="514"/>
+      <c r="AK4" s="514"/>
+      <c r="AL4" s="515"/>
+      <c r="AM4" s="514" t="s">
         <v>813</v>
       </c>
-      <c r="AN4" s="511"/>
-      <c r="AO4" s="511"/>
-      <c r="AP4" s="511"/>
-      <c r="AQ4" s="513"/>
-      <c r="AR4" s="511" t="s">
+      <c r="AN4" s="514"/>
+      <c r="AO4" s="514"/>
+      <c r="AP4" s="514"/>
+      <c r="AQ4" s="515"/>
+      <c r="AR4" s="514" t="s">
         <v>814</v>
       </c>
-      <c r="AS4" s="511"/>
-      <c r="AT4" s="511"/>
-      <c r="AU4" s="511"/>
-      <c r="AV4" s="513"/>
-      <c r="AW4" s="511" t="s">
+      <c r="AS4" s="514"/>
+      <c r="AT4" s="514"/>
+      <c r="AU4" s="514"/>
+      <c r="AV4" s="515"/>
+      <c r="AW4" s="514" t="s">
         <v>815</v>
       </c>
-      <c r="AX4" s="511"/>
-      <c r="AY4" s="511"/>
-      <c r="AZ4" s="511"/>
-      <c r="BA4" s="511"/>
-      <c r="BB4" s="512" t="s">
+      <c r="AX4" s="514"/>
+      <c r="AY4" s="514"/>
+      <c r="AZ4" s="514"/>
+      <c r="BA4" s="514"/>
+      <c r="BB4" s="513" t="s">
         <v>816</v>
       </c>
-      <c r="BC4" s="511"/>
-      <c r="BD4" s="511"/>
-      <c r="BE4" s="511"/>
-      <c r="BF4" s="513"/>
-      <c r="BG4" s="511" t="s">
+      <c r="BC4" s="514"/>
+      <c r="BD4" s="514"/>
+      <c r="BE4" s="514"/>
+      <c r="BF4" s="515"/>
+      <c r="BG4" s="514" t="s">
         <v>817</v>
       </c>
-      <c r="BH4" s="511"/>
-      <c r="BI4" s="511"/>
-      <c r="BJ4" s="511"/>
-      <c r="BK4" s="511"/>
-      <c r="BL4" s="512" t="s">
+      <c r="BH4" s="514"/>
+      <c r="BI4" s="514"/>
+      <c r="BJ4" s="514"/>
+      <c r="BK4" s="514"/>
+      <c r="BL4" s="513" t="s">
         <v>818</v>
       </c>
-      <c r="BM4" s="511"/>
-      <c r="BN4" s="511"/>
-      <c r="BO4" s="511"/>
-      <c r="BP4" s="511"/>
-      <c r="BQ4" s="512" t="s">
+      <c r="BM4" s="514"/>
+      <c r="BN4" s="514"/>
+      <c r="BO4" s="514"/>
+      <c r="BP4" s="514"/>
+      <c r="BQ4" s="513" t="s">
         <v>819</v>
       </c>
-      <c r="BR4" s="511"/>
-      <c r="BS4" s="511"/>
-      <c r="BT4" s="511"/>
-      <c r="BU4" s="513"/>
+      <c r="BR4" s="514"/>
+      <c r="BS4" s="514"/>
+      <c r="BT4" s="514"/>
+      <c r="BU4" s="515"/>
       <c r="BV4" s="382" t="s">
         <v>820</v>
       </c>
-      <c r="BW4" s="514" t="s">
+      <c r="BW4" s="516" t="s">
         <v>821</v>
       </c>
-      <c r="BX4" s="515"/>
-      <c r="BY4" s="515"/>
-      <c r="BZ4" s="515"/>
-      <c r="CA4" s="516"/>
-      <c r="CB4" s="514" t="s">
+      <c r="BX4" s="517"/>
+      <c r="BY4" s="517"/>
+      <c r="BZ4" s="517"/>
+      <c r="CA4" s="518"/>
+      <c r="CB4" s="516" t="s">
         <v>822</v>
       </c>
-      <c r="CC4" s="515"/>
-      <c r="CD4" s="515"/>
-      <c r="CE4" s="515"/>
-      <c r="CF4" s="516"/>
-      <c r="CG4" s="514" t="s">
+      <c r="CC4" s="517"/>
+      <c r="CD4" s="517"/>
+      <c r="CE4" s="517"/>
+      <c r="CF4" s="518"/>
+      <c r="CG4" s="516" t="s">
         <v>823</v>
       </c>
-      <c r="CH4" s="515"/>
-      <c r="CI4" s="515"/>
-      <c r="CJ4" s="515"/>
-      <c r="CK4" s="516"/>
+      <c r="CH4" s="517"/>
+      <c r="CI4" s="517"/>
+      <c r="CJ4" s="517"/>
+      <c r="CK4" s="518"/>
     </row>
     <row r="5" spans="1:89" x14ac:dyDescent="0.2">
       <c r="A5" s="384"/>
@@ -61409,11 +61473,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="BL4:BP4"/>
-    <mergeCell ref="BQ4:BU4"/>
-    <mergeCell ref="BW4:CA4"/>
-    <mergeCell ref="CB4:CF4"/>
-    <mergeCell ref="CG4:CK4"/>
     <mergeCell ref="BG4:BK4"/>
     <mergeCell ref="D4:H4"/>
     <mergeCell ref="I4:M4"/>
@@ -61426,6 +61485,11 @@
     <mergeCell ref="AR4:AV4"/>
     <mergeCell ref="AW4:BA4"/>
     <mergeCell ref="BB4:BF4"/>
+    <mergeCell ref="BL4:BP4"/>
+    <mergeCell ref="BQ4:BU4"/>
+    <mergeCell ref="BW4:CA4"/>
+    <mergeCell ref="CB4:CF4"/>
+    <mergeCell ref="CG4:CK4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
Debug and Price Update
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_RSD.xlsx
+++ b/SubRES_TMPL/SubRes_RSD.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B193C012-B9E2-4909-B4B2-8E7C76B0D935}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B1BCE6D-564D-48F1-8B0E-3CDF9EC662A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{34F9D92C-266F-476D-89E0-63153305AC39}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{34F9D92C-266F-476D-89E0-63153305AC39}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="34" r:id="rId1"/>
@@ -357,6 +357,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="U45" authorId="0" shapeId="0" xr:uid="{78070B63-6065-4708-ACC8-F2D62C931A27}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Oil Boilers approx 30%higher cost than  gas boilers</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="AF45" authorId="0" shapeId="0" xr:uid="{43FB8299-38F2-46F1-8559-95F979595FFC}">
       <text>
         <r>
@@ -537,6 +561,30 @@
           </rPr>
           <t xml:space="preserve">
 from TIMES-Starter</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U91" authorId="0" shapeId="0" xr:uid="{EC92E8F3-DBAF-44A4-BFBF-45086A40057A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Oil Boilers approx 30%higher cost than  gas boilers</t>
         </r>
       </text>
     </comment>
@@ -14188,6 +14236,15 @@
     <xf numFmtId="0" fontId="16" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -14197,22 +14254,13 @@
     <xf numFmtId="0" fontId="16" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="60" fillId="31" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="60" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="60" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="60" fillId="31" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="60" fillId="31" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -24855,8 +24903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{104F8057-C735-4662-BAA6-EEDCF7B57273}">
   <dimension ref="A2:AO162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="U16" sqref="U16"/>
+    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="AA101" sqref="AA101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -25011,28 +25059,28 @@
       <c r="F4" s="63" t="s">
         <v>334</v>
       </c>
-      <c r="G4" s="506" t="s">
+      <c r="G4" s="509" t="s">
         <v>758</v>
       </c>
-      <c r="H4" s="507"/>
-      <c r="I4" s="507"/>
-      <c r="J4" s="508"/>
-      <c r="K4" s="506" t="s">
+      <c r="H4" s="510"/>
+      <c r="I4" s="510"/>
+      <c r="J4" s="511"/>
+      <c r="K4" s="509" t="s">
         <v>336</v>
       </c>
-      <c r="L4" s="507"/>
-      <c r="M4" s="507"/>
-      <c r="N4" s="508"/>
-      <c r="O4" s="506" t="s">
+      <c r="L4" s="510"/>
+      <c r="M4" s="510"/>
+      <c r="N4" s="511"/>
+      <c r="O4" s="509" t="s">
         <v>337</v>
       </c>
-      <c r="P4" s="507"/>
-      <c r="Q4" s="507"/>
-      <c r="R4" s="508"/>
-      <c r="S4" s="506" t="s">
+      <c r="P4" s="510"/>
+      <c r="Q4" s="510"/>
+      <c r="R4" s="511"/>
+      <c r="S4" s="509" t="s">
         <v>338</v>
       </c>
-      <c r="T4" s="508"/>
+      <c r="T4" s="511"/>
       <c r="U4" s="500" t="s">
         <v>339</v>
       </c>
@@ -26405,29 +26453,27 @@
         <v>20</v>
       </c>
       <c r="T20" s="77"/>
-      <c r="U20" s="87">
-        <f>(JRC_Data!BB18/1000)*($T$145/$T$148)</f>
-        <v>10.640816326530611</v>
-      </c>
-      <c r="V20" s="87">
-        <f>(JRC_Data!BC18/1000)*($T$145/$T$148)</f>
-        <v>9.6734693877551017</v>
-      </c>
-      <c r="W20" s="87">
-        <f>(JRC_Data!BD18/1000)*($T$145/$T$148)</f>
-        <v>9.6734693877551017</v>
-      </c>
-      <c r="X20" s="87">
-        <f>(JRC_Data!BE18/1000)*($T$145/$T$148)</f>
-        <v>8.7061224489795919</v>
-      </c>
-      <c r="Y20" s="87">
-        <f>JRC_Data!BL18/1000</f>
-        <v>0.15</v>
+      <c r="U20" s="481">
+        <v>7.5039999999999996</v>
+      </c>
+      <c r="V20" s="481">
+        <f>U20*0.91</f>
+        <v>6.82864</v>
+      </c>
+      <c r="W20" s="481">
+        <f>V20*0.91</f>
+        <v>6.2140624000000004</v>
+      </c>
+      <c r="X20" s="481">
+        <f>U20*0.82</f>
+        <v>6.1532799999999996</v>
+      </c>
+      <c r="Y20" s="481">
+        <v>0.1</v>
       </c>
       <c r="Z20" s="112"/>
-      <c r="AA20" s="119"/>
-      <c r="AB20" s="119"/>
+      <c r="AA20" s="120"/>
+      <c r="AB20" s="120"/>
       <c r="AC20" s="119"/>
       <c r="AD20" s="119"/>
       <c r="AE20" s="109">
@@ -26511,25 +26557,24 @@
         <v>20</v>
       </c>
       <c r="T21" s="71"/>
-      <c r="U21" s="69">
-        <f>(JRC_Data!BB18/1000)*($T$146/$T$148)</f>
-        <v>10.73061224489796</v>
-      </c>
-      <c r="V21" s="69">
-        <f>(JRC_Data!BC18/1000)*($T$146/$T$148)</f>
-        <v>9.7551020408163271</v>
-      </c>
-      <c r="W21" s="69">
-        <f>(JRC_Data!BD18/1000)*($T$146/$T$148)</f>
-        <v>9.7551020408163271</v>
-      </c>
-      <c r="X21" s="69">
-        <f>(JRC_Data!BE18/1000)*($T$146/$T$148)</f>
-        <v>8.7795918367346939</v>
-      </c>
-      <c r="Y21" s="69">
-        <f>JRC_Data!BL18/1000</f>
-        <v>0.15</v>
+      <c r="U21" s="482">
+        <f>U20*($T$146/$T$145)</f>
+        <v>7.5673248945147682</v>
+      </c>
+      <c r="V21" s="482">
+        <f t="shared" ref="V21:X21" si="17">V20*($T$146/$T$145)</f>
+        <v>6.8862656540084393</v>
+      </c>
+      <c r="W21" s="482">
+        <f t="shared" si="17"/>
+        <v>6.2665017451476803</v>
+      </c>
+      <c r="X21" s="482">
+        <f t="shared" si="17"/>
+        <v>6.2052064135021103</v>
+      </c>
+      <c r="Y21" s="482">
+        <v>0.1</v>
       </c>
       <c r="Z21" s="113"/>
       <c r="AA21" s="120"/>
@@ -26854,15 +26899,15 @@
         <v>0.7</v>
       </c>
       <c r="P25" s="67">
-        <f t="shared" ref="P25:R25" si="17">H25*0.7</f>
+        <f t="shared" ref="P25:R25" si="18">H25*0.7</f>
         <v>0.75185185185185177</v>
       </c>
       <c r="Q25" s="67">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.88148148148148131</v>
       </c>
       <c r="R25" s="103">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.88148148148148131</v>
       </c>
       <c r="S25" s="136">
@@ -26960,15 +27005,15 @@
         <v>0.77777777777777757</v>
       </c>
       <c r="P26" s="73">
-        <f t="shared" ref="P26" si="18">H26*0.7</f>
+        <f t="shared" ref="P26" si="19">H26*0.7</f>
         <v>0.8037037037037037</v>
       </c>
       <c r="Q26" s="73">
-        <f t="shared" ref="Q26" si="19">I26*0.7</f>
+        <f t="shared" ref="Q26" si="20">I26*0.7</f>
         <v>0.8037037037037037</v>
       </c>
       <c r="R26" s="106">
-        <f t="shared" ref="R26" si="20">J26*0.7</f>
+        <f t="shared" ref="R26" si="21">J26*0.7</f>
         <v>0.82962962962962949</v>
       </c>
       <c r="S26" s="74">
@@ -27063,11 +27108,11 @@
       <c r="AG27" s="81"/>
       <c r="AI27" s="306"/>
       <c r="AJ27" s="150" t="str">
-        <f t="shared" ref="AJ27:AK28" si="21">C33</f>
+        <f t="shared" ref="AJ27:AK28" si="22">C33</f>
         <v>R-WH_Apt_ELC_N1</v>
       </c>
       <c r="AK27" s="150" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v xml:space="preserve">Residential Electric Water Heater </v>
       </c>
       <c r="AL27" s="151" t="s">
@@ -27116,15 +27161,15 @@
         <v>0.7</v>
       </c>
       <c r="P28" s="348">
-        <f t="shared" ref="P28:R28" si="22">H28*0.7</f>
+        <f t="shared" ref="P28:R28" si="23">H28*0.7</f>
         <v>0.73360000000000003</v>
       </c>
       <c r="Q28" s="348">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.76789999999999992</v>
       </c>
       <c r="R28" s="349">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.81269999999999998</v>
       </c>
       <c r="S28" s="350">
@@ -27169,11 +27214,11 @@
       </c>
       <c r="AI28" s="4"/>
       <c r="AJ28" s="152" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>R-WH_Apt_SOL_N1</v>
       </c>
       <c r="AK28" s="152" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v xml:space="preserve">Residential Solar Water Heater </v>
       </c>
       <c r="AL28" s="153" t="s">
@@ -27894,28 +27939,28 @@
       <c r="F42" s="63" t="s">
         <v>334</v>
       </c>
-      <c r="G42" s="506" t="s">
+      <c r="G42" s="509" t="s">
         <v>335</v>
       </c>
-      <c r="H42" s="507"/>
-      <c r="I42" s="507"/>
-      <c r="J42" s="508"/>
-      <c r="K42" s="506" t="s">
+      <c r="H42" s="510"/>
+      <c r="I42" s="510"/>
+      <c r="J42" s="511"/>
+      <c r="K42" s="509" t="s">
         <v>336</v>
       </c>
-      <c r="L42" s="507"/>
-      <c r="M42" s="507"/>
-      <c r="N42" s="508"/>
-      <c r="O42" s="506" t="s">
+      <c r="L42" s="510"/>
+      <c r="M42" s="510"/>
+      <c r="N42" s="511"/>
+      <c r="O42" s="509" t="s">
         <v>337</v>
       </c>
-      <c r="P42" s="507"/>
-      <c r="Q42" s="507"/>
-      <c r="R42" s="508"/>
-      <c r="S42" s="506" t="s">
+      <c r="P42" s="510"/>
+      <c r="Q42" s="510"/>
+      <c r="R42" s="511"/>
+      <c r="S42" s="509" t="s">
         <v>338</v>
       </c>
-      <c r="T42" s="508"/>
+      <c r="T42" s="511"/>
       <c r="U42" s="500" t="s">
         <v>339</v>
       </c>
@@ -28034,16 +28079,16 @@
       <c r="P44" s="504"/>
       <c r="Q44" s="504"/>
       <c r="R44" s="505"/>
-      <c r="S44" s="509" t="s">
+      <c r="S44" s="506" t="s">
         <v>312</v>
       </c>
-      <c r="T44" s="510"/>
-      <c r="U44" s="509" t="s">
+      <c r="T44" s="507"/>
+      <c r="U44" s="506" t="s">
         <v>1007</v>
       </c>
-      <c r="V44" s="511"/>
-      <c r="W44" s="511"/>
-      <c r="X44" s="510"/>
+      <c r="V44" s="508"/>
+      <c r="W44" s="508"/>
+      <c r="X44" s="507"/>
       <c r="Y44" s="475" t="s">
         <v>1019</v>
       </c>
@@ -28129,25 +28174,24 @@
         <v>20</v>
       </c>
       <c r="T45" s="88"/>
-      <c r="U45" s="109">
-        <f>(JRC_Data!BB7/1000)*$T$147</f>
-        <v>6.166795366795367</v>
-      </c>
-      <c r="V45" s="109">
-        <f>(JRC_Data!BC7/1000)*$T$147</f>
-        <v>6.166795366795367</v>
-      </c>
-      <c r="W45" s="109">
-        <f>(JRC_Data!BD7/1000)*$T$147</f>
-        <v>6.166795366795367</v>
-      </c>
-      <c r="X45" s="109">
-        <f>(JRC_Data!BE7/1000)*$T$147</f>
-        <v>6.166795366795367</v>
-      </c>
-      <c r="Y45" s="105">
-        <f>JRC_Data!BL7/1000</f>
-        <v>0.27</v>
+      <c r="U45" s="481">
+        <f>U49*1.3</f>
+        <v>4.2250000000000005</v>
+      </c>
+      <c r="V45" s="481">
+        <f t="shared" ref="V45:X45" si="24">V49*1.3</f>
+        <v>4.2250000000000005</v>
+      </c>
+      <c r="W45" s="481">
+        <f t="shared" si="24"/>
+        <v>4.2250000000000005</v>
+      </c>
+      <c r="X45" s="481">
+        <f t="shared" si="24"/>
+        <v>4.2250000000000005</v>
+      </c>
+      <c r="Y45" s="481">
+        <v>0.12</v>
       </c>
       <c r="Z45" s="112"/>
       <c r="AA45" s="89"/>
@@ -28218,40 +28262,39 @@
         <v>0.7</v>
       </c>
       <c r="P46" s="70">
-        <f t="shared" ref="P46:P48" si="23">H46*0.7</f>
+        <f t="shared" ref="P46:P48" si="25">H46*0.7</f>
         <v>0.7</v>
       </c>
       <c r="Q46" s="70">
-        <f t="shared" ref="Q46:Q48" si="24">I46*0.7</f>
+        <f t="shared" ref="Q46:Q48" si="26">I46*0.7</f>
         <v>0.7</v>
       </c>
       <c r="R46" s="104">
-        <f t="shared" ref="R46:R48" si="25">J46*0.7</f>
+        <f t="shared" ref="R46:R48" si="27">J46*0.7</f>
         <v>0.7</v>
       </c>
       <c r="S46" s="100">
         <v>20</v>
       </c>
       <c r="T46" s="72"/>
-      <c r="U46" s="110">
-        <f>(JRC_Data!BB7/1000)*$T$148</f>
-        <v>6.243243243243243</v>
-      </c>
-      <c r="V46" s="110">
-        <f>(JRC_Data!BC7/1000)*$T$148</f>
-        <v>6.243243243243243</v>
-      </c>
-      <c r="W46" s="110">
-        <f>(JRC_Data!BD7/1000)*$T$148</f>
-        <v>6.243243243243243</v>
-      </c>
-      <c r="X46" s="110">
-        <f>(JRC_Data!BE7/1000)*$T$148</f>
-        <v>6.243243243243243</v>
-      </c>
-      <c r="Y46" s="104">
-        <f>JRC_Data!BL7/1000</f>
-        <v>0.27</v>
+      <c r="U46" s="482">
+        <f>U50*1.3</f>
+        <v>4.2773760330578519</v>
+      </c>
+      <c r="V46" s="482">
+        <f t="shared" ref="V46:X46" si="28">V50*1.3</f>
+        <v>4.2773760330578519</v>
+      </c>
+      <c r="W46" s="482">
+        <f t="shared" si="28"/>
+        <v>4.2773760330578519</v>
+      </c>
+      <c r="X46" s="482">
+        <f t="shared" si="28"/>
+        <v>4.2773760330578519</v>
+      </c>
+      <c r="Y46" s="482">
+        <v>0.12</v>
       </c>
       <c r="Z46" s="113"/>
       <c r="AA46" s="91"/>
@@ -28267,11 +28310,11 @@
       </c>
       <c r="AI46" s="153"/>
       <c r="AJ46" s="152" t="str">
-        <f t="shared" ref="AJ46:AJ56" si="26">C46</f>
+        <f t="shared" ref="AJ46:AJ56" si="29">C46</f>
         <v>R-SW_Att_KER_N1</v>
       </c>
       <c r="AK46" s="152" t="str">
-        <f t="shared" ref="AK46:AK56" si="27">D46</f>
+        <f t="shared" ref="AK46:AK56" si="30">D46</f>
         <v>Residential Kerosene Heating Oil - New 2 SH + WH</v>
       </c>
       <c r="AL46" s="153" t="s">
@@ -28320,15 +28363,15 @@
         <v>0.7</v>
       </c>
       <c r="P47" s="76">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>0.7</v>
       </c>
       <c r="Q47" s="76">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>0.7</v>
       </c>
       <c r="R47" s="105">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>0.7</v>
       </c>
       <c r="S47" s="101">
@@ -28373,11 +28416,11 @@
       </c>
       <c r="AI47" s="153"/>
       <c r="AJ47" s="152" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>R-SW_Att_KER_N2</v>
       </c>
       <c r="AK47" s="152" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>Residential Kerosene Heating Oil - New 3 SH+WH + Solar</v>
       </c>
       <c r="AL47" s="153" t="s">
@@ -28426,15 +28469,15 @@
         <v>0.7</v>
       </c>
       <c r="P48" s="70">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>0.71749999999999992</v>
       </c>
       <c r="Q48" s="70">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>0.71749999999999992</v>
       </c>
       <c r="R48" s="104">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>0.71749999999999992</v>
       </c>
       <c r="S48" s="100">
@@ -28479,11 +28522,11 @@
       </c>
       <c r="AI48" s="153"/>
       <c r="AJ48" s="152" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>R-SW_Att_KER_N3</v>
       </c>
       <c r="AK48" s="152" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>Residential Kerosene Heating Oil - New 3 SH+WH + Wood Stove</v>
       </c>
       <c r="AL48" s="154" t="s">
@@ -28533,25 +28576,24 @@
         <v>20</v>
       </c>
       <c r="T49" s="88"/>
-      <c r="U49" s="109">
-        <f>(JRC_Data!BB9/1000)</f>
-        <v>4</v>
-      </c>
-      <c r="V49" s="109">
-        <f>(JRC_Data!BC9/1000)</f>
-        <v>4</v>
-      </c>
-      <c r="W49" s="109">
-        <f>(JRC_Data!BD9/1000)</f>
-        <v>4</v>
-      </c>
-      <c r="X49" s="109">
-        <f>(JRC_Data!BE9/1000)</f>
-        <v>4</v>
-      </c>
-      <c r="Y49" s="105">
-        <f>JRC_Data!BL9/1000</f>
-        <v>0.23499999999999999</v>
+      <c r="U49" s="481">
+        <f>3.25</f>
+        <v>3.25</v>
+      </c>
+      <c r="V49" s="481">
+        <f t="shared" ref="V49:X49" si="31">3.25</f>
+        <v>3.25</v>
+      </c>
+      <c r="W49" s="481">
+        <f t="shared" si="31"/>
+        <v>3.25</v>
+      </c>
+      <c r="X49" s="481">
+        <f t="shared" si="31"/>
+        <v>3.25</v>
+      </c>
+      <c r="Y49" s="481">
+        <v>0.12</v>
       </c>
       <c r="Z49" s="112"/>
       <c r="AA49" s="89"/>
@@ -28567,11 +28609,11 @@
       </c>
       <c r="AI49" s="153"/>
       <c r="AJ49" s="152" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>R-SH_Att_GAS_N1</v>
       </c>
       <c r="AK49" s="152" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>Residential Natural Gas Heating - New 1 SH</v>
       </c>
       <c r="AL49" s="153" t="s">
@@ -28620,40 +28662,39 @@
         <v>0.7</v>
       </c>
       <c r="P50" s="70">
-        <f t="shared" ref="P50:P52" si="28">H50*0.7</f>
+        <f t="shared" ref="P50:P52" si="32">H50*0.7</f>
         <v>0.7</v>
       </c>
       <c r="Q50" s="70">
-        <f t="shared" ref="Q50:Q52" si="29">I50*0.7</f>
+        <f t="shared" ref="Q50:Q52" si="33">I50*0.7</f>
         <v>0.7</v>
       </c>
       <c r="R50" s="104">
-        <f t="shared" ref="R50:R52" si="30">J50*0.7</f>
+        <f t="shared" ref="R50:R52" si="34">J50*0.7</f>
         <v>0.7</v>
       </c>
       <c r="S50" s="100">
         <v>20</v>
       </c>
       <c r="T50" s="72"/>
-      <c r="U50" s="110">
-        <f>(JRC_Data!BB9/1000)*($T$148/$T$147)</f>
-        <v>4.0495867768595044</v>
-      </c>
-      <c r="V50" s="110">
-        <f>(JRC_Data!BC9/1000)*($T$148/$T$147)</f>
-        <v>4.0495867768595044</v>
-      </c>
-      <c r="W50" s="110">
-        <f>(JRC_Data!BD9/1000)*($T$148/$T$147)</f>
-        <v>4.0495867768595044</v>
-      </c>
-      <c r="X50" s="110">
-        <f>(JRC_Data!BE9/1000)*($T$148/$T$147)</f>
-        <v>4.0495867768595044</v>
-      </c>
-      <c r="Y50" s="104">
-        <f>JRC_Data!BL9/1000</f>
-        <v>0.23499999999999999</v>
+      <c r="U50" s="482">
+        <f>U49*($T$148/$T$147)</f>
+        <v>3.2902892561983474</v>
+      </c>
+      <c r="V50" s="482">
+        <f t="shared" ref="V50:X50" si="35">V49*($T$148/$T$147)</f>
+        <v>3.2902892561983474</v>
+      </c>
+      <c r="W50" s="482">
+        <f t="shared" si="35"/>
+        <v>3.2902892561983474</v>
+      </c>
+      <c r="X50" s="482">
+        <f t="shared" si="35"/>
+        <v>3.2902892561983474</v>
+      </c>
+      <c r="Y50" s="482">
+        <v>0.12</v>
       </c>
       <c r="Z50" s="113"/>
       <c r="AA50" s="91"/>
@@ -28669,11 +28710,11 @@
       </c>
       <c r="AI50" s="153"/>
       <c r="AJ50" s="152" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>R-SW_Att_GAS_N1</v>
       </c>
       <c r="AK50" s="152" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>Residential Natural Gas Heating - New 2 SH + WH</v>
       </c>
       <c r="AL50" s="153" t="s">
@@ -28722,40 +28763,38 @@
         <v>0.7</v>
       </c>
       <c r="P51" s="76">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>0.7</v>
       </c>
       <c r="Q51" s="76">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>0.7</v>
       </c>
       <c r="R51" s="105">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>0.7</v>
       </c>
       <c r="S51" s="101">
         <v>20</v>
       </c>
       <c r="T51" s="88"/>
-      <c r="U51" s="109">
-        <f>((JRC_Data!BB9+JRC_Data!BB45)*0.8/1000)*($T$148/$T$147)</f>
-        <v>7.6132231404958679</v>
-      </c>
-      <c r="V51" s="109">
-        <f>((JRC_Data!BC9+JRC_Data!BC45)*0.8/1000)*($T$148/$T$147)</f>
-        <v>7.3702479338842979</v>
-      </c>
-      <c r="W51" s="109">
-        <f>((JRC_Data!BD9+JRC_Data!BD45)*0.8/1000)*($T$148/$T$147)</f>
-        <v>6.9652892561983473</v>
-      </c>
-      <c r="X51" s="109">
-        <f>((JRC_Data!BE9+JRC_Data!BE45)*0.8/1000)*($T$148/$T$147)</f>
-        <v>6.2363636363636372</v>
-      </c>
-      <c r="Y51" s="105">
-        <f>((JRC_Data!BL9+JRC_Data!BL45)*0.8)/1000</f>
-        <v>0.23760000000000003</v>
+      <c r="U51" s="481">
+        <v>12.75</v>
+      </c>
+      <c r="V51" s="481">
+        <f>U51*0.9685</f>
+        <v>12.348375000000001</v>
+      </c>
+      <c r="W51" s="481">
+        <f>U51*0.916</f>
+        <v>11.679</v>
+      </c>
+      <c r="X51" s="481">
+        <f>U51*0.812</f>
+        <v>10.353000000000002</v>
+      </c>
+      <c r="Y51" s="481">
+        <v>0.19</v>
       </c>
       <c r="Z51" s="112"/>
       <c r="AA51" s="89">
@@ -28775,11 +28814,11 @@
       </c>
       <c r="AI51" s="153"/>
       <c r="AJ51" s="152" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>R-SW_Att_GAS_N2</v>
       </c>
       <c r="AK51" s="152" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>Residential Natural Gas Heating - New 3 SH + WH + Solar</v>
       </c>
       <c r="AL51" s="153" t="s">
@@ -28828,15 +28867,15 @@
         <v>0.7</v>
       </c>
       <c r="P52" s="70">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>0.71749999999999992</v>
       </c>
       <c r="Q52" s="70">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>0.71749999999999992</v>
       </c>
       <c r="R52" s="104">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>0.71749999999999992</v>
       </c>
       <c r="S52" s="100">
@@ -28881,11 +28920,11 @@
       </c>
       <c r="AI52" s="153"/>
       <c r="AJ52" s="152" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>R-SW_Att_GAS_N3</v>
       </c>
       <c r="AK52" s="152" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>Residential Natural Gas Heating - New 4 SH + WH + Wood Stove</v>
       </c>
       <c r="AL52" s="153" t="s">
@@ -28937,25 +28976,24 @@
         <v>20</v>
       </c>
       <c r="T53" s="88"/>
-      <c r="U53" s="109">
-        <f>(JRC_Data!BB9/1000)</f>
-        <v>4</v>
-      </c>
-      <c r="V53" s="109">
-        <f>(JRC_Data!BC9/1000)</f>
-        <v>4</v>
-      </c>
-      <c r="W53" s="109">
-        <f>(JRC_Data!BD9/1000)</f>
-        <v>4</v>
-      </c>
-      <c r="X53" s="109">
-        <f>(JRC_Data!BE9/1000)</f>
-        <v>4</v>
-      </c>
-      <c r="Y53" s="105">
-        <f>JRC_Data!BL9/1000</f>
-        <v>0.23499999999999999</v>
+      <c r="U53" s="481">
+        <f>U49</f>
+        <v>3.25</v>
+      </c>
+      <c r="V53" s="481">
+        <f t="shared" ref="V53:X53" si="36">V49</f>
+        <v>3.25</v>
+      </c>
+      <c r="W53" s="481">
+        <f t="shared" si="36"/>
+        <v>3.25</v>
+      </c>
+      <c r="X53" s="481">
+        <f t="shared" si="36"/>
+        <v>3.25</v>
+      </c>
+      <c r="Y53" s="481">
+        <v>0.12</v>
       </c>
       <c r="Z53" s="112"/>
       <c r="AA53" s="89"/>
@@ -28971,11 +29009,11 @@
       </c>
       <c r="AI53" s="153"/>
       <c r="AJ53" s="152" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>R-SH_Att_LPG_N1</v>
       </c>
       <c r="AK53" s="152" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>Residential Liquid Petroleum Gas- New 1 SH</v>
       </c>
       <c r="AL53" s="153" t="s">
@@ -29024,40 +29062,39 @@
         <v>0.7</v>
       </c>
       <c r="P54" s="70">
-        <f t="shared" ref="P54" si="31">H54*0.7</f>
+        <f t="shared" ref="P54" si="37">H54*0.7</f>
         <v>0.7</v>
       </c>
       <c r="Q54" s="70">
-        <f t="shared" ref="Q54" si="32">I54*0.7</f>
+        <f t="shared" ref="Q54" si="38">I54*0.7</f>
         <v>0.7</v>
       </c>
       <c r="R54" s="104">
-        <f t="shared" ref="R54" si="33">J54*0.7</f>
+        <f t="shared" ref="R54" si="39">J54*0.7</f>
         <v>0.7</v>
       </c>
       <c r="S54" s="100">
         <v>20</v>
       </c>
       <c r="T54" s="72"/>
-      <c r="U54" s="110">
-        <f>(JRC_Data!BB9/1000)*($T$148/$T$147)</f>
-        <v>4.0495867768595044</v>
-      </c>
-      <c r="V54" s="110">
-        <f>(JRC_Data!BC9/1000)*($T$148/$T$147)</f>
-        <v>4.0495867768595044</v>
-      </c>
-      <c r="W54" s="110">
-        <f>(JRC_Data!BD9/1000)*($T$148/$T$147)</f>
-        <v>4.0495867768595044</v>
-      </c>
-      <c r="X54" s="110">
-        <f>(JRC_Data!BE9/1000)*($T$148/$T$147)</f>
-        <v>4.0495867768595044</v>
-      </c>
-      <c r="Y54" s="104">
-        <f>JRC_Data!BL9/1000</f>
-        <v>0.23499999999999999</v>
+      <c r="U54" s="482">
+        <f>U50</f>
+        <v>3.2902892561983474</v>
+      </c>
+      <c r="V54" s="482">
+        <f t="shared" ref="V54:X54" si="40">V50</f>
+        <v>3.2902892561983474</v>
+      </c>
+      <c r="W54" s="482">
+        <f t="shared" si="40"/>
+        <v>3.2902892561983474</v>
+      </c>
+      <c r="X54" s="482">
+        <f t="shared" si="40"/>
+        <v>3.2902892561983474</v>
+      </c>
+      <c r="Y54" s="482">
+        <v>0.12</v>
       </c>
       <c r="Z54" s="113"/>
       <c r="AA54" s="91"/>
@@ -29073,11 +29110,11 @@
       </c>
       <c r="AI54" s="153"/>
       <c r="AJ54" s="152" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>R-SW_Att_LPG_N1</v>
       </c>
       <c r="AK54" s="152" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>Residential Liquid Petroleum Gas- New 2 SH + WH</v>
       </c>
       <c r="AL54" s="153" t="s">
@@ -29129,29 +29166,32 @@
         <v>20</v>
       </c>
       <c r="T55" s="88"/>
-      <c r="U55" s="109">
-        <f>((JRC_Data!BB9+JRC_Data!BB45)*0.8/1000)*($T$147/$T$147)</f>
+      <c r="U55" s="481">
+        <v>20.48</v>
+      </c>
+      <c r="V55" s="481">
+        <f>U55*0.96777</f>
+        <v>19.819929600000002</v>
+      </c>
+      <c r="W55" s="481">
+        <f>U55*0.914844</f>
+        <v>18.736005120000002</v>
+      </c>
+      <c r="X55" s="481">
+        <f>U55*0.8181</f>
+        <v>16.754688000000002</v>
+      </c>
+      <c r="Y55" s="481">
+        <v>0.25</v>
+      </c>
+      <c r="Z55" s="112"/>
+      <c r="AA55" s="87">
         <v>7.52</v>
       </c>
-      <c r="V55" s="109">
-        <f>((JRC_Data!BC9+JRC_Data!BC45)*0.8/1000)*($T$147/$T$147)</f>
-        <v>7.28</v>
-      </c>
-      <c r="W55" s="109">
-        <f>((JRC_Data!BD9+JRC_Data!BD45)*0.8/1000)*($T$147/$T$147)</f>
-        <v>6.88</v>
-      </c>
-      <c r="X55" s="109">
-        <f>((JRC_Data!BE9+JRC_Data!BE45)*0.8/1000)*($T$147/$T$147)</f>
-        <v>6.16</v>
-      </c>
-      <c r="Y55" s="105">
-        <f>(JRC_Data!BL11)/1000</f>
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="Z55" s="112"/>
-      <c r="AA55" s="89"/>
-      <c r="AB55" s="119"/>
+      <c r="AB55" s="119">
+        <f>6.25/AA55</f>
+        <v>0.83111702127659581</v>
+      </c>
       <c r="AC55" s="119"/>
       <c r="AD55" s="119"/>
       <c r="AE55" s="109">
@@ -29163,11 +29203,11 @@
       </c>
       <c r="AI55" s="153"/>
       <c r="AJ55" s="152" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>R-SH_Att_WOO_N1</v>
       </c>
       <c r="AK55" s="152" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>Residential Biomass Boiler - New 1 SH</v>
       </c>
       <c r="AL55" s="153" t="s">
@@ -29212,44 +29252,43 @@
       <c r="M56" s="79"/>
       <c r="N56" s="92"/>
       <c r="O56" s="69">
-        <f t="shared" ref="O56:R58" si="34">G56*0.7</f>
+        <f t="shared" ref="O56:R58" si="41">G56*0.7</f>
         <v>0.7</v>
       </c>
       <c r="P56" s="70">
-        <f t="shared" si="34"/>
+        <f t="shared" si="41"/>
         <v>0.7</v>
       </c>
       <c r="Q56" s="70">
-        <f t="shared" si="34"/>
+        <f t="shared" si="41"/>
         <v>0.7</v>
       </c>
       <c r="R56" s="104">
-        <f t="shared" si="34"/>
+        <f t="shared" si="41"/>
         <v>0.7</v>
       </c>
       <c r="S56" s="100">
         <v>20</v>
       </c>
       <c r="T56" s="72"/>
-      <c r="U56" s="110">
-        <f>((JRC_Data!BB9+JRC_Data!BB45)*0.8/1000)*($T$148/$T$147)</f>
-        <v>7.6132231404958679</v>
-      </c>
-      <c r="V56" s="110">
-        <f>((JRC_Data!BC9+JRC_Data!BC45)*0.8/1000)*($T$148/$T$147)</f>
-        <v>7.3702479338842979</v>
-      </c>
-      <c r="W56" s="110">
-        <f>((JRC_Data!BD9+JRC_Data!BD45)*0.8/1000)*($T$148/$T$147)</f>
-        <v>6.9652892561983473</v>
-      </c>
-      <c r="X56" s="110">
-        <f>((JRC_Data!BE9+JRC_Data!BE45)*0.8/1000)*($T$148/$T$147)</f>
-        <v>6.2363636363636372</v>
-      </c>
-      <c r="Y56" s="105">
-        <f>(JRC_Data!BL11)/1000</f>
-        <v>2.5999999999999999E-2</v>
+      <c r="U56" s="482">
+        <f>U55*($T$148/$T$147)</f>
+        <v>20.733884297520664</v>
+      </c>
+      <c r="V56" s="482">
+        <f t="shared" ref="V56:X56" si="42">V55*($T$148/$T$147)</f>
+        <v>20.065631206611574</v>
+      </c>
+      <c r="W56" s="482">
+        <f t="shared" si="42"/>
+        <v>18.968269646280994</v>
+      </c>
+      <c r="X56" s="482">
+        <f t="shared" si="42"/>
+        <v>16.962390743801656</v>
+      </c>
+      <c r="Y56" s="482">
+        <v>0.25</v>
       </c>
       <c r="Z56" s="113"/>
       <c r="AA56" s="91"/>
@@ -29265,11 +29304,11 @@
       </c>
       <c r="AI56" s="156"/>
       <c r="AJ56" s="155" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>R-SW_Att_WOO_N1</v>
       </c>
       <c r="AK56" s="155" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>Residential Biomass Boiler - New 2 SH + WH</v>
       </c>
       <c r="AL56" s="156" t="s">
@@ -29313,19 +29352,19 @@
       <c r="M57" s="78"/>
       <c r="N57" s="90"/>
       <c r="O57" s="87">
-        <f t="shared" si="34"/>
+        <f t="shared" si="41"/>
         <v>0.7</v>
       </c>
       <c r="P57" s="76">
-        <f t="shared" si="34"/>
+        <f t="shared" si="41"/>
         <v>0.7</v>
       </c>
       <c r="Q57" s="76">
-        <f t="shared" si="34"/>
+        <f t="shared" si="41"/>
         <v>0.7</v>
       </c>
       <c r="R57" s="105">
-        <f t="shared" si="34"/>
+        <f t="shared" si="41"/>
         <v>0.7</v>
       </c>
       <c r="S57" s="101">
@@ -29366,11 +29405,11 @@
       </c>
       <c r="AI57" s="156"/>
       <c r="AJ57" s="155" t="str">
-        <f t="shared" ref="AJ57:AJ58" si="35">C57</f>
+        <f t="shared" ref="AJ57:AJ58" si="43">C57</f>
         <v>*R-H_Apt_HVO_N1</v>
       </c>
       <c r="AK57" s="155" t="str">
-        <f t="shared" ref="AK57:AK58" si="36">D57</f>
+        <f t="shared" ref="AK57:AK58" si="44">D57</f>
         <v>Residential  Hydrotreated vegetable oil - New 1 SH</v>
       </c>
       <c r="AL57" s="156" t="s">
@@ -29414,19 +29453,19 @@
       <c r="M58" s="97"/>
       <c r="N58" s="98"/>
       <c r="O58" s="346">
-        <f t="shared" si="34"/>
+        <f t="shared" si="41"/>
         <v>0.7</v>
       </c>
       <c r="P58" s="73">
-        <f t="shared" si="34"/>
+        <f t="shared" si="41"/>
         <v>0.7</v>
       </c>
       <c r="Q58" s="73">
-        <f t="shared" si="34"/>
+        <f t="shared" si="41"/>
         <v>0.7</v>
       </c>
       <c r="R58" s="106">
-        <f t="shared" si="34"/>
+        <f t="shared" si="41"/>
         <v>0.7</v>
       </c>
       <c r="S58" s="102">
@@ -29467,11 +29506,11 @@
       </c>
       <c r="AI58" s="156"/>
       <c r="AJ58" s="155" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="43"/>
         <v>*R-H_Apt_HVO_N2</v>
       </c>
       <c r="AK58" s="155" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="44"/>
         <v>Residential  Hydrotreated vegetable oil - New 1 SH + WH</v>
       </c>
       <c r="AL58" s="156" t="s">
@@ -29611,11 +29650,11 @@
       </c>
       <c r="AI60" s="151"/>
       <c r="AJ60" s="150" t="str">
-        <f t="shared" ref="AJ60:AK66" si="37">C62</f>
+        <f t="shared" ref="AJ60:AK66" si="45">C62</f>
         <v>R-SH_Att_ELC_HPN1</v>
       </c>
       <c r="AK60" s="150" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="45"/>
         <v>Residential Electric Heat Pump - Air to Air - SH</v>
       </c>
       <c r="AL60" s="151" t="s">
@@ -29665,11 +29704,11 @@
       <c r="AG61" s="81"/>
       <c r="AI61" s="153"/>
       <c r="AJ61" s="152" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="45"/>
         <v>R-HC_Att_ELC_HPN1</v>
       </c>
       <c r="AK61" s="152" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="45"/>
         <v>Residential Electric Heat Pump - Air to Air - SH + SC</v>
       </c>
       <c r="AL61" s="153" t="s">
@@ -29758,11 +29797,11 @@
       </c>
       <c r="AI62" s="153"/>
       <c r="AJ62" s="152" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="45"/>
         <v>R-SH_Att_ELC_HPN2</v>
       </c>
       <c r="AK62" s="152" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="45"/>
         <v>Residential Electric Heat Pump - Air to Water - SH</v>
       </c>
       <c r="AL62" s="153" t="s">
@@ -29862,11 +29901,11 @@
       </c>
       <c r="AI63" s="153"/>
       <c r="AJ63" s="152" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="45"/>
         <v>R-SW_Att_ELC_HPN1</v>
       </c>
       <c r="AK63" s="152" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="45"/>
         <v>Residential Electric Heat Pump - Air to Water - SH + WH</v>
       </c>
       <c r="AL63" s="153" t="s">
@@ -29921,25 +29960,23 @@
         <v>20</v>
       </c>
       <c r="T64" s="90"/>
-      <c r="U64" s="87">
-        <f>(JRC_Data!BB18/1000)*($T$147/$T$148)</f>
-        <v>10.865306122448981</v>
-      </c>
-      <c r="V64" s="87">
-        <f>(JRC_Data!BC18/1000)*($T$147/$T$148)</f>
-        <v>9.8775510204081645</v>
-      </c>
-      <c r="W64" s="87">
-        <f>(JRC_Data!BD18/1000)*($T$147/$T$148)</f>
-        <v>9.8775510204081645</v>
-      </c>
-      <c r="X64" s="109">
-        <f>(JRC_Data!BE18/1000)*($T$147/$T$148)</f>
-        <v>8.8897959183673478</v>
-      </c>
-      <c r="Y64" s="109">
-        <f>JRC_Data!BL18/1000</f>
-        <v>0.15</v>
+      <c r="U64" s="481">
+        <v>8.5299999999999994</v>
+      </c>
+      <c r="V64" s="481">
+        <f>U64*0.91</f>
+        <v>7.7622999999999998</v>
+      </c>
+      <c r="W64" s="481">
+        <f>V64*0.91</f>
+        <v>7.0636929999999998</v>
+      </c>
+      <c r="X64" s="481">
+        <f>U64*0.82</f>
+        <v>6.9945999999999993</v>
+      </c>
+      <c r="Y64" s="481">
+        <v>0.1</v>
       </c>
       <c r="Z64" s="109"/>
       <c r="AA64" s="109"/>
@@ -29955,11 +29992,11 @@
       </c>
       <c r="AI64" s="303"/>
       <c r="AJ64" s="152" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="45"/>
         <v>R-SW_Att_SOL_HPN2</v>
       </c>
       <c r="AK64" s="152" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="45"/>
         <v>Residential Electric Heat Pump - Air to Water - SH + WH + Solar</v>
       </c>
       <c r="AL64" s="153" t="s">
@@ -30011,40 +30048,39 @@
         <v>0.7</v>
       </c>
       <c r="P65" s="70">
-        <f t="shared" ref="P65:P66" si="38">H65*0.7</f>
+        <f t="shared" ref="P65:P66" si="46">H65*0.7</f>
         <v>0.76999999999999991</v>
       </c>
       <c r="Q65" s="70">
-        <f t="shared" ref="Q65:Q66" si="39">I65*0.7</f>
+        <f t="shared" ref="Q65:Q66" si="47">I65*0.7</f>
         <v>0.86333333333333329</v>
       </c>
       <c r="R65" s="104">
-        <f t="shared" ref="R65:R66" si="40">J65*0.7</f>
+        <f t="shared" ref="R65:R66" si="48">J65*0.7</f>
         <v>0.93333333333333324</v>
       </c>
       <c r="S65" s="100">
         <v>20</v>
       </c>
       <c r="T65" s="92"/>
-      <c r="U65" s="69">
-        <f>(JRC_Data!BB18/1000)*($T$148/$T$148)</f>
-        <v>11</v>
-      </c>
-      <c r="V65" s="69">
-        <f>(JRC_Data!BC18/1000)*($T$148/$T$148)</f>
-        <v>10</v>
-      </c>
-      <c r="W65" s="69">
-        <f>(JRC_Data!BD18/1000)*($T$148/$T$148)</f>
-        <v>10</v>
-      </c>
-      <c r="X65" s="110">
-        <f>(JRC_Data!BE18/1000)*($T$148/$T$148)</f>
-        <v>9</v>
-      </c>
-      <c r="Y65" s="110">
-        <f>JRC_Data!BL18/1000</f>
-        <v>0.15</v>
+      <c r="U65" s="482">
+        <f>U64*($T$146/$T$145)</f>
+        <v>8.6019831223628689</v>
+      </c>
+      <c r="V65" s="482">
+        <f t="shared" ref="V65" si="49">V64*($T$146/$T$145)</f>
+        <v>7.8278046413502116</v>
+      </c>
+      <c r="W65" s="482">
+        <f t="shared" ref="W65" si="50">W64*($T$146/$T$145)</f>
+        <v>7.1233022236286923</v>
+      </c>
+      <c r="X65" s="482">
+        <f t="shared" ref="X65" si="51">X64*($T$146/$T$145)</f>
+        <v>7.0536261603375525</v>
+      </c>
+      <c r="Y65" s="482">
+        <v>0.1</v>
       </c>
       <c r="Z65" s="110"/>
       <c r="AA65" s="110"/>
@@ -30060,11 +30096,11 @@
       </c>
       <c r="AI65" s="303"/>
       <c r="AJ65" s="152" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="45"/>
         <v>R-SH_Att_ELC_HPN3</v>
       </c>
       <c r="AK65" s="152" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="45"/>
         <v>Residential Electric Heat Pump - Ground to Water - SH</v>
       </c>
       <c r="AL65" s="153" t="s">
@@ -30113,15 +30149,15 @@
         <v>0.7</v>
       </c>
       <c r="P66" s="76">
-        <f t="shared" si="38"/>
+        <f t="shared" si="46"/>
         <v>0.77700000000000002</v>
       </c>
       <c r="Q66" s="76">
-        <f t="shared" si="39"/>
+        <f t="shared" si="47"/>
         <v>0.83299999999999996</v>
       </c>
       <c r="R66" s="105">
-        <f t="shared" si="40"/>
+        <f t="shared" si="48"/>
         <v>0.83299999999999996</v>
       </c>
       <c r="S66" s="101">
@@ -30166,11 +30202,11 @@
       </c>
       <c r="AI66" s="159"/>
       <c r="AJ66" s="155" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="45"/>
         <v>R-HC_Att_ELC_HPN2</v>
       </c>
       <c r="AK66" s="155" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="45"/>
         <v>Residential Electric Heat Pump - Ground to Water - SH + SC</v>
       </c>
       <c r="AL66" s="156" t="s">
@@ -30476,15 +30512,15 @@
         <v>0.7</v>
       </c>
       <c r="P70" s="341">
-        <f t="shared" ref="P70:P71" si="41">H70*0.7</f>
+        <f t="shared" ref="P70:P71" si="52">H70*0.7</f>
         <v>0.75185185185185177</v>
       </c>
       <c r="Q70" s="341">
-        <f t="shared" ref="Q70:Q71" si="42">I70*0.7</f>
+        <f t="shared" ref="Q70:Q71" si="53">I70*0.7</f>
         <v>0.88148148148148131</v>
       </c>
       <c r="R70" s="342">
-        <f t="shared" ref="R70:R71" si="43">J70*0.7</f>
+        <f t="shared" ref="R70:R71" si="54">J70*0.7</f>
         <v>0.88148148148148131</v>
       </c>
       <c r="S70" s="136">
@@ -30582,15 +30618,15 @@
         <v>0.77777777777777757</v>
       </c>
       <c r="P71" s="348">
-        <f t="shared" si="41"/>
+        <f t="shared" si="52"/>
         <v>0.8037037037037037</v>
       </c>
       <c r="Q71" s="348">
-        <f t="shared" si="42"/>
+        <f t="shared" si="53"/>
         <v>0.8037037037037037</v>
       </c>
       <c r="R71" s="349">
-        <f t="shared" si="43"/>
+        <f t="shared" si="54"/>
         <v>0.82962962962962949</v>
       </c>
       <c r="S71" s="74">
@@ -30685,11 +30721,11 @@
       <c r="AG72" s="81"/>
       <c r="AI72" s="306"/>
       <c r="AJ72" s="150" t="str">
-        <f t="shared" ref="AJ72:AK73" si="44">C78</f>
+        <f t="shared" ref="AJ72:AK73" si="55">C78</f>
         <v>R-WH_Att_ELC_N1</v>
       </c>
       <c r="AK72" s="150" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="55"/>
         <v xml:space="preserve">Residential Electric Water Heater </v>
       </c>
       <c r="AL72" s="151" t="s">
@@ -30738,15 +30774,15 @@
         <v>0.7</v>
       </c>
       <c r="P73" s="348">
-        <f t="shared" ref="P73" si="45">H73*0.7</f>
+        <f t="shared" ref="P73" si="56">H73*0.7</f>
         <v>0.73360000000000003</v>
       </c>
       <c r="Q73" s="348">
-        <f t="shared" ref="Q73" si="46">I73*0.7</f>
+        <f t="shared" ref="Q73" si="57">I73*0.7</f>
         <v>0.76789999999999992</v>
       </c>
       <c r="R73" s="349">
-        <f t="shared" ref="R73" si="47">J73*0.7</f>
+        <f t="shared" ref="R73" si="58">J73*0.7</f>
         <v>0.81269999999999998</v>
       </c>
       <c r="S73" s="5">
@@ -30790,11 +30826,11 @@
       </c>
       <c r="AI73" s="4"/>
       <c r="AJ73" s="152" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="55"/>
         <v>R-WH_Att_SOL_N1</v>
       </c>
       <c r="AK73" s="152" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="55"/>
         <v xml:space="preserve">Residential Solar Water Heater </v>
       </c>
       <c r="AL73" s="153" t="s">
@@ -31309,7 +31345,6 @@
       </c>
     </row>
     <row r="85" spans="3:41" x14ac:dyDescent="0.2">
-      <c r="AJ85" s="57"/>
       <c r="AK85" s="57"/>
       <c r="AL85" s="57"/>
       <c r="AM85" s="57"/>
@@ -31429,28 +31464,28 @@
       <c r="F88" s="63" t="s">
         <v>334</v>
       </c>
-      <c r="G88" s="506" t="s">
+      <c r="G88" s="509" t="s">
         <v>335</v>
       </c>
-      <c r="H88" s="507"/>
-      <c r="I88" s="507"/>
-      <c r="J88" s="508"/>
-      <c r="K88" s="506" t="s">
+      <c r="H88" s="510"/>
+      <c r="I88" s="510"/>
+      <c r="J88" s="511"/>
+      <c r="K88" s="509" t="s">
         <v>336</v>
       </c>
-      <c r="L88" s="507"/>
-      <c r="M88" s="507"/>
-      <c r="N88" s="508"/>
-      <c r="O88" s="506" t="s">
+      <c r="L88" s="510"/>
+      <c r="M88" s="510"/>
+      <c r="N88" s="511"/>
+      <c r="O88" s="509" t="s">
         <v>337</v>
       </c>
-      <c r="P88" s="507"/>
-      <c r="Q88" s="507"/>
-      <c r="R88" s="508"/>
-      <c r="S88" s="506" t="s">
+      <c r="P88" s="510"/>
+      <c r="Q88" s="510"/>
+      <c r="R88" s="511"/>
+      <c r="S88" s="509" t="s">
         <v>338</v>
       </c>
-      <c r="T88" s="508"/>
+      <c r="T88" s="511"/>
       <c r="U88" s="500" t="s">
         <v>339</v>
       </c>
@@ -31569,16 +31604,16 @@
       <c r="P90" s="504"/>
       <c r="Q90" s="504"/>
       <c r="R90" s="505"/>
-      <c r="S90" s="509" t="s">
+      <c r="S90" s="506" t="s">
         <v>312</v>
       </c>
-      <c r="T90" s="510"/>
-      <c r="U90" s="509" t="s">
+      <c r="T90" s="507"/>
+      <c r="U90" s="506" t="s">
         <v>1007</v>
       </c>
-      <c r="V90" s="511"/>
-      <c r="W90" s="511"/>
-      <c r="X90" s="510"/>
+      <c r="V90" s="508"/>
+      <c r="W90" s="508"/>
+      <c r="X90" s="507"/>
       <c r="Y90" s="475" t="s">
         <v>1019</v>
       </c>
@@ -31664,25 +31699,24 @@
         <v>20</v>
       </c>
       <c r="T91" s="88"/>
-      <c r="U91" s="109">
-        <f>(JRC_Data!BB7/1000)*$T$149</f>
-        <v>6.6</v>
-      </c>
-      <c r="V91" s="109">
-        <f>(JRC_Data!BC7/1000)*$T$149</f>
-        <v>6.6</v>
-      </c>
-      <c r="W91" s="109">
-        <f>(JRC_Data!BD7/1000)*$T$149</f>
-        <v>6.6</v>
-      </c>
-      <c r="X91" s="109">
-        <f>(JRC_Data!BE7/1000)*$T$149</f>
-        <v>6.6</v>
-      </c>
-      <c r="Y91" s="105">
-        <f>JRC_Data!BL7/1000</f>
-        <v>0.27</v>
+      <c r="U91" s="481">
+        <f>U95*1.3</f>
+        <v>4.5825000000000005</v>
+      </c>
+      <c r="V91" s="481">
+        <f t="shared" ref="V91:X91" si="59">V95*1.3</f>
+        <v>4.5825000000000005</v>
+      </c>
+      <c r="W91" s="481">
+        <f t="shared" si="59"/>
+        <v>4.5825000000000005</v>
+      </c>
+      <c r="X91" s="481">
+        <f t="shared" si="59"/>
+        <v>4.5825000000000005</v>
+      </c>
+      <c r="Y91" s="481">
+        <v>0.12</v>
       </c>
       <c r="Z91" s="112"/>
       <c r="AA91" s="89"/>
@@ -31753,40 +31787,39 @@
         <v>0.7</v>
       </c>
       <c r="P92" s="70">
-        <f t="shared" ref="P92:P94" si="48">H92*0.7</f>
+        <f t="shared" ref="P92:P94" si="60">H92*0.7</f>
         <v>0.7</v>
       </c>
       <c r="Q92" s="70">
-        <f t="shared" ref="Q92:Q94" si="49">I92*0.7</f>
+        <f t="shared" ref="Q92:Q94" si="61">I92*0.7</f>
         <v>0.7</v>
       </c>
       <c r="R92" s="104">
-        <f t="shared" ref="R92:R94" si="50">J92*0.7</f>
+        <f t="shared" ref="R92:R94" si="62">J92*0.7</f>
         <v>0.7</v>
       </c>
       <c r="S92" s="100">
         <v>20</v>
       </c>
       <c r="T92" s="72"/>
-      <c r="U92" s="110">
-        <f>(JRC_Data!BB7/1000)*$T$150</f>
-        <v>7.1223938223938221</v>
-      </c>
-      <c r="V92" s="110">
-        <f>(JRC_Data!BC7/1000)*$T$150</f>
-        <v>7.1223938223938221</v>
-      </c>
-      <c r="W92" s="110">
-        <f>(JRC_Data!BD7/1000)*$T$150</f>
-        <v>7.1223938223938221</v>
-      </c>
-      <c r="X92" s="110">
-        <f>(JRC_Data!BE7/1000)*$T$150</f>
-        <v>7.1223938223938221</v>
-      </c>
-      <c r="Y92" s="104">
-        <f>JRC_Data!BL7/1000</f>
-        <v>0.27</v>
+      <c r="U92" s="482">
+        <f>U96*1.3</f>
+        <v>4.9452075289575284</v>
+      </c>
+      <c r="V92" s="482">
+        <f t="shared" ref="V92:X92" si="63">V96*1.3</f>
+        <v>4.9452075289575284</v>
+      </c>
+      <c r="W92" s="482">
+        <f t="shared" si="63"/>
+        <v>4.9452075289575284</v>
+      </c>
+      <c r="X92" s="482">
+        <f t="shared" si="63"/>
+        <v>4.9452075289575284</v>
+      </c>
+      <c r="Y92" s="482">
+        <v>0.12</v>
       </c>
       <c r="Z92" s="113"/>
       <c r="AA92" s="91"/>
@@ -31802,11 +31835,11 @@
       </c>
       <c r="AI92" s="153"/>
       <c r="AJ92" s="152" t="str">
-        <f t="shared" ref="AJ92:AJ104" si="51">C92</f>
+        <f t="shared" ref="AJ92:AJ104" si="64">C92</f>
         <v>R-SW_Det_KER_N1</v>
       </c>
       <c r="AK92" s="152" t="str">
-        <f t="shared" ref="AK92:AK104" si="52">D92</f>
+        <f t="shared" ref="AK92:AK104" si="65">D92</f>
         <v>Residential Kerosene Heating Oil - New 2 SH + WH</v>
       </c>
       <c r="AL92" s="153" t="s">
@@ -31855,15 +31888,15 @@
         <v>0.7</v>
       </c>
       <c r="P93" s="76">
-        <f t="shared" si="48"/>
+        <f t="shared" si="60"/>
         <v>0.7</v>
       </c>
       <c r="Q93" s="76">
-        <f t="shared" si="49"/>
+        <f t="shared" si="61"/>
         <v>0.7</v>
       </c>
       <c r="R93" s="105">
-        <f t="shared" si="50"/>
+        <f t="shared" si="62"/>
         <v>0.7</v>
       </c>
       <c r="S93" s="101">
@@ -31908,11 +31941,11 @@
       </c>
       <c r="AI93" s="153"/>
       <c r="AJ93" s="152" t="str">
-        <f t="shared" si="51"/>
+        <f t="shared" si="64"/>
         <v>R-SW_Det_KER_N2</v>
       </c>
       <c r="AK93" s="152" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="65"/>
         <v>Residential Kerosene Heating Oil - New 3 SH+WH + Solar</v>
       </c>
       <c r="AL93" s="153" t="s">
@@ -31961,15 +31994,15 @@
         <v>0.7</v>
       </c>
       <c r="P94" s="70">
-        <f t="shared" si="48"/>
+        <f t="shared" si="60"/>
         <v>0.71749999999999992</v>
       </c>
       <c r="Q94" s="70">
-        <f t="shared" si="49"/>
+        <f t="shared" si="61"/>
         <v>0.71749999999999992</v>
       </c>
       <c r="R94" s="104">
-        <f t="shared" si="50"/>
+        <f t="shared" si="62"/>
         <v>0.71749999999999992</v>
       </c>
       <c r="S94" s="100">
@@ -32014,11 +32047,11 @@
       </c>
       <c r="AI94" s="153"/>
       <c r="AJ94" s="152" t="str">
-        <f t="shared" si="51"/>
+        <f t="shared" si="64"/>
         <v>R-SW_Det_KER_N3</v>
       </c>
       <c r="AK94" s="152" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="65"/>
         <v>Residential Kerosene Heating Oil - New 3 SH+WH + Wood Stove</v>
       </c>
       <c r="AL94" s="154" t="s">
@@ -32068,25 +32101,24 @@
         <v>20</v>
       </c>
       <c r="T95" s="88"/>
-      <c r="U95" s="109">
-        <f>(JRC_Data!BB9/1000)*($T$149/$T$147)</f>
-        <v>4.2809917355371896</v>
-      </c>
-      <c r="V95" s="109">
-        <f>(JRC_Data!BC9/1000)*($T$149/$T$147)</f>
-        <v>4.2809917355371896</v>
-      </c>
-      <c r="W95" s="109">
-        <f>(JRC_Data!BD9/1000)*($T$149/$T$147)</f>
-        <v>4.2809917355371896</v>
-      </c>
-      <c r="X95" s="109">
-        <f>(JRC_Data!BE9/1000)*($T$149/$T$147)</f>
-        <v>4.2809917355371896</v>
-      </c>
-      <c r="Y95" s="105">
-        <f>JRC_Data!BL9/1000</f>
-        <v>0.23499999999999999</v>
+      <c r="U95" s="481">
+        <f>3.525</f>
+        <v>3.5249999999999999</v>
+      </c>
+      <c r="V95" s="481">
+        <f t="shared" ref="V95:X95" si="66">3.525</f>
+        <v>3.5249999999999999</v>
+      </c>
+      <c r="W95" s="481">
+        <f t="shared" si="66"/>
+        <v>3.5249999999999999</v>
+      </c>
+      <c r="X95" s="481">
+        <f t="shared" si="66"/>
+        <v>3.5249999999999999</v>
+      </c>
+      <c r="Y95" s="481">
+        <v>0.12</v>
       </c>
       <c r="Z95" s="112"/>
       <c r="AA95" s="89"/>
@@ -32102,11 +32134,11 @@
       </c>
       <c r="AI95" s="153"/>
       <c r="AJ95" s="152" t="str">
-        <f t="shared" si="51"/>
+        <f t="shared" si="64"/>
         <v>R-SH_Det_GAS_N1</v>
       </c>
       <c r="AK95" s="152" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="65"/>
         <v>Residential Natural Gas Heating - New 1 SH</v>
       </c>
       <c r="AL95" s="153" t="s">
@@ -32155,40 +32187,39 @@
         <v>0.7</v>
       </c>
       <c r="P96" s="70">
-        <f t="shared" ref="P96:P98" si="53">H96*0.7</f>
+        <f t="shared" ref="P96:P98" si="67">H96*0.7</f>
         <v>0.7</v>
       </c>
       <c r="Q96" s="70">
-        <f t="shared" ref="Q96:Q98" si="54">I96*0.7</f>
+        <f t="shared" ref="Q96:Q98" si="68">I96*0.7</f>
         <v>0.7</v>
       </c>
       <c r="R96" s="104">
-        <f t="shared" ref="R96:R98" si="55">J96*0.7</f>
+        <f t="shared" ref="R96:R98" si="69">J96*0.7</f>
         <v>0.7</v>
       </c>
       <c r="S96" s="100">
         <v>20</v>
       </c>
       <c r="T96" s="72"/>
-      <c r="U96" s="110">
-        <f>(JRC_Data!BB9/1000)*($T$150/$T$147)</f>
-        <v>4.6198347107438016</v>
-      </c>
-      <c r="V96" s="110">
-        <f>(JRC_Data!BC9/1000)*($T$150/$T$147)</f>
-        <v>4.6198347107438016</v>
-      </c>
-      <c r="W96" s="110">
-        <f>(JRC_Data!BD9/1000)*($T$150/$T$147)</f>
-        <v>4.6198347107438016</v>
-      </c>
-      <c r="X96" s="110">
-        <f>(JRC_Data!BE9/1000)*($T$150/$T$147)</f>
-        <v>4.6198347107438016</v>
-      </c>
-      <c r="Y96" s="104">
-        <f>JRC_Data!BL9/1000</f>
-        <v>0.23499999999999999</v>
+      <c r="U96" s="482">
+        <f>U95*($T$150/$T$149)</f>
+        <v>3.8040057915057912</v>
+      </c>
+      <c r="V96" s="482">
+        <f t="shared" ref="V96:X96" si="70">V95*($T$150/$T$149)</f>
+        <v>3.8040057915057912</v>
+      </c>
+      <c r="W96" s="482">
+        <f t="shared" si="70"/>
+        <v>3.8040057915057912</v>
+      </c>
+      <c r="X96" s="482">
+        <f t="shared" si="70"/>
+        <v>3.8040057915057912</v>
+      </c>
+      <c r="Y96" s="482">
+        <v>0.12</v>
       </c>
       <c r="Z96" s="113"/>
       <c r="AA96" s="91"/>
@@ -32204,11 +32235,11 @@
       </c>
       <c r="AI96" s="153"/>
       <c r="AJ96" s="152" t="str">
-        <f t="shared" si="51"/>
+        <f t="shared" si="64"/>
         <v>R-SW_Det_GAS_N1</v>
       </c>
       <c r="AK96" s="152" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="65"/>
         <v>Residential Natural Gas Heating - New 2 SH + WH</v>
       </c>
       <c r="AL96" s="153" t="s">
@@ -32257,15 +32288,15 @@
         <v>0.7</v>
       </c>
       <c r="P97" s="76">
-        <f t="shared" si="53"/>
+        <f t="shared" si="67"/>
         <v>0.7</v>
       </c>
       <c r="Q97" s="76">
-        <f t="shared" si="54"/>
+        <f t="shared" si="68"/>
         <v>0.7</v>
       </c>
       <c r="R97" s="105">
-        <f t="shared" si="55"/>
+        <f t="shared" si="69"/>
         <v>0.7</v>
       </c>
       <c r="S97" s="101">
@@ -32273,24 +32304,22 @@
       </c>
       <c r="T97" s="88"/>
       <c r="U97" s="109">
-        <f>((JRC_Data!BB9+JRC_Data!BB45)*0.8/1000)*($T$150/$T$147)</f>
-        <v>8.685289256198347</v>
-      </c>
-      <c r="V97" s="109">
-        <f>((JRC_Data!BC9+JRC_Data!BC45)*0.8/1000)*($T$150/$T$147)</f>
-        <v>8.4080991735537189</v>
-      </c>
-      <c r="W97" s="109">
-        <f>((JRC_Data!BD9+JRC_Data!BD45)*0.8/1000)*($T$150/$T$147)</f>
-        <v>7.9461157024793385</v>
-      </c>
-      <c r="X97" s="109">
-        <f>((JRC_Data!BE9+JRC_Data!BE45)*0.8/1000)*($T$150/$T$147)</f>
-        <v>7.1145454545454543</v>
+        <v>13.025</v>
+      </c>
+      <c r="V97" s="481">
+        <f>U97*0.9685</f>
+        <v>12.614712500000001</v>
+      </c>
+      <c r="W97" s="481">
+        <f>U97*0.916</f>
+        <v>11.930900000000001</v>
+      </c>
+      <c r="X97" s="481">
+        <f>U97*0.812</f>
+        <v>10.576300000000002</v>
       </c>
       <c r="Y97" s="105">
-        <f>((JRC_Data!BL9+JRC_Data!BL45)*0.8)/1000</f>
-        <v>0.23760000000000003</v>
+        <v>0.19</v>
       </c>
       <c r="Z97" s="112"/>
       <c r="AA97" s="89">
@@ -32310,11 +32339,11 @@
       </c>
       <c r="AI97" s="153"/>
       <c r="AJ97" s="152" t="str">
-        <f t="shared" si="51"/>
+        <f t="shared" si="64"/>
         <v>R-SW_Det_GAS_N2</v>
       </c>
       <c r="AK97" s="152" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="65"/>
         <v>Residential Natural Gas Heating - New 3 SH + WH + Solar</v>
       </c>
       <c r="AL97" s="153" t="s">
@@ -32363,15 +32392,15 @@
         <v>0.7</v>
       </c>
       <c r="P98" s="70">
-        <f t="shared" si="53"/>
+        <f t="shared" si="67"/>
         <v>0.71749999999999992</v>
       </c>
       <c r="Q98" s="70">
-        <f t="shared" si="54"/>
+        <f t="shared" si="68"/>
         <v>0.71749999999999992</v>
       </c>
       <c r="R98" s="104">
-        <f t="shared" si="55"/>
+        <f t="shared" si="69"/>
         <v>0.71749999999999992</v>
       </c>
       <c r="S98" s="100">
@@ -32416,11 +32445,11 @@
       </c>
       <c r="AI98" s="153"/>
       <c r="AJ98" s="152" t="str">
-        <f t="shared" si="51"/>
+        <f t="shared" si="64"/>
         <v>R-SW_Det_GAS_N3</v>
       </c>
       <c r="AK98" s="152" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="65"/>
         <v>Residential Natural Gas Heating - New 4 SH + WH + Wood Stove</v>
       </c>
       <c r="AL98" s="153" t="s">
@@ -32472,25 +32501,24 @@
         <v>20</v>
       </c>
       <c r="T99" s="88"/>
-      <c r="U99" s="109">
-        <f>(JRC_Data!BB9/1000)*($T$149/$T$147)</f>
-        <v>4.2809917355371896</v>
-      </c>
-      <c r="V99" s="109">
-        <f>(JRC_Data!BC9/1000)*($T$149/$T$147)</f>
-        <v>4.2809917355371896</v>
-      </c>
-      <c r="W99" s="109">
-        <f>(JRC_Data!BD9/1000)*($T$149/$T$147)</f>
-        <v>4.2809917355371896</v>
-      </c>
-      <c r="X99" s="109">
-        <f>(JRC_Data!BE9/1000)*($T$149/$T$147)</f>
-        <v>4.2809917355371896</v>
-      </c>
-      <c r="Y99" s="105">
-        <f>JRC_Data!BL9/1000</f>
-        <v>0.23499999999999999</v>
+      <c r="U99" s="481">
+        <f>U95</f>
+        <v>3.5249999999999999</v>
+      </c>
+      <c r="V99" s="481">
+        <f t="shared" ref="V99:X99" si="71">V95</f>
+        <v>3.5249999999999999</v>
+      </c>
+      <c r="W99" s="481">
+        <f t="shared" si="71"/>
+        <v>3.5249999999999999</v>
+      </c>
+      <c r="X99" s="481">
+        <f t="shared" si="71"/>
+        <v>3.5249999999999999</v>
+      </c>
+      <c r="Y99" s="481">
+        <v>0.12</v>
       </c>
       <c r="Z99" s="112"/>
       <c r="AA99" s="89"/>
@@ -32506,11 +32534,11 @@
       </c>
       <c r="AI99" s="153"/>
       <c r="AJ99" s="152" t="str">
-        <f t="shared" si="51"/>
+        <f t="shared" si="64"/>
         <v>R-SH_Det_LPG_N1</v>
       </c>
       <c r="AK99" s="152" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="65"/>
         <v>Residential Liquid Petroleum Gas- New 1 SH</v>
       </c>
       <c r="AL99" s="153" t="s">
@@ -32559,40 +32587,39 @@
         <v>0.7</v>
       </c>
       <c r="P100" s="70">
-        <f t="shared" ref="P100" si="56">H100*0.7</f>
+        <f t="shared" ref="P100" si="72">H100*0.7</f>
         <v>0.7</v>
       </c>
       <c r="Q100" s="70">
-        <f t="shared" ref="Q100" si="57">I100*0.7</f>
+        <f t="shared" ref="Q100" si="73">I100*0.7</f>
         <v>0.7</v>
       </c>
       <c r="R100" s="104">
-        <f t="shared" ref="R100" si="58">J100*0.7</f>
+        <f t="shared" ref="R100" si="74">J100*0.7</f>
         <v>0.7</v>
       </c>
       <c r="S100" s="100">
         <v>20</v>
       </c>
       <c r="T100" s="72"/>
-      <c r="U100" s="110">
-        <f>(JRC_Data!BB9/1000)*($T$150/$T$147)</f>
-        <v>4.6198347107438016</v>
-      </c>
-      <c r="V100" s="110">
-        <f>(JRC_Data!BC9/1000)*($T$150/$T$147)</f>
-        <v>4.6198347107438016</v>
-      </c>
-      <c r="W100" s="110">
-        <f>(JRC_Data!BD9/1000)*($T$150/$T$147)</f>
-        <v>4.6198347107438016</v>
-      </c>
-      <c r="X100" s="110">
-        <f>(JRC_Data!BE9/1000)*($T$150/$T$147)</f>
-        <v>4.6198347107438016</v>
-      </c>
-      <c r="Y100" s="104">
-        <f>JRC_Data!BL9/1000</f>
-        <v>0.23499999999999999</v>
+      <c r="U100" s="482">
+        <f>U96</f>
+        <v>3.8040057915057912</v>
+      </c>
+      <c r="V100" s="482">
+        <f t="shared" ref="V100:X100" si="75">V96</f>
+        <v>3.8040057915057912</v>
+      </c>
+      <c r="W100" s="482">
+        <f t="shared" si="75"/>
+        <v>3.8040057915057912</v>
+      </c>
+      <c r="X100" s="482">
+        <f t="shared" si="75"/>
+        <v>3.8040057915057912</v>
+      </c>
+      <c r="Y100" s="482">
+        <v>0.12</v>
       </c>
       <c r="Z100" s="113"/>
       <c r="AA100" s="91"/>
@@ -32608,11 +32635,11 @@
       </c>
       <c r="AI100" s="153"/>
       <c r="AJ100" s="152" t="str">
-        <f t="shared" si="51"/>
+        <f t="shared" si="64"/>
         <v>R-SW_Det_LPG_N1</v>
       </c>
       <c r="AK100" s="152" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="65"/>
         <v>Residential Liquid Petroleum Gas- New 2 SH + WH</v>
       </c>
       <c r="AL100" s="153" t="s">
@@ -32664,25 +32691,23 @@
         <v>20</v>
       </c>
       <c r="T101" s="88"/>
-      <c r="U101" s="109">
-        <f>((JRC_Data!BB9+JRC_Data!BB45)*0.8/1000)*($T$149/$T$147)</f>
-        <v>8.0482644628099163</v>
-      </c>
-      <c r="V101" s="109">
-        <f>((JRC_Data!BC9+JRC_Data!BC45)*0.8/1000)*($T$149/$T$147)</f>
-        <v>7.7914049586776857</v>
-      </c>
-      <c r="W101" s="109">
-        <f>((JRC_Data!BD9+JRC_Data!BD45)*0.8/1000)*($T$149/$T$147)</f>
-        <v>7.3633057851239663</v>
-      </c>
-      <c r="X101" s="109">
-        <f>((JRC_Data!BE9+JRC_Data!BE45)*0.8/1000)*($T$149/$T$147)</f>
-        <v>6.5927272727272719</v>
-      </c>
-      <c r="Y101" s="105">
-        <f>(JRC_Data!BL11)/1000</f>
-        <v>2.5999999999999999E-2</v>
+      <c r="U101" s="481">
+        <v>22.5</v>
+      </c>
+      <c r="V101" s="481">
+        <f>U101*0.96777</f>
+        <v>21.774825</v>
+      </c>
+      <c r="W101" s="481">
+        <f>U101*0.914844</f>
+        <v>20.58399</v>
+      </c>
+      <c r="X101" s="481">
+        <f>U101*0.8181</f>
+        <v>18.407250000000001</v>
+      </c>
+      <c r="Y101" s="481">
+        <v>0.25</v>
       </c>
       <c r="Z101" s="112"/>
       <c r="AA101" s="89"/>
@@ -32698,11 +32723,11 @@
       </c>
       <c r="AI101" s="153"/>
       <c r="AJ101" s="152" t="str">
-        <f t="shared" si="51"/>
+        <f t="shared" si="64"/>
         <v>R-SH_Det_WOO_N1</v>
       </c>
       <c r="AK101" s="152" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="65"/>
         <v>Residential Biomass Boiler - New 1 SH</v>
       </c>
       <c r="AL101" s="153" t="s">
@@ -32747,44 +32772,43 @@
       <c r="M102" s="79"/>
       <c r="N102" s="92"/>
       <c r="O102" s="69">
-        <f t="shared" ref="O102:R104" si="59">G102*0.7</f>
+        <f t="shared" ref="O102:R104" si="76">G102*0.7</f>
         <v>0.7</v>
       </c>
       <c r="P102" s="70">
-        <f t="shared" si="59"/>
+        <f t="shared" si="76"/>
         <v>0.7</v>
       </c>
       <c r="Q102" s="70">
-        <f t="shared" si="59"/>
+        <f t="shared" si="76"/>
         <v>0.7</v>
       </c>
       <c r="R102" s="104">
-        <f t="shared" si="59"/>
+        <f t="shared" si="76"/>
         <v>0.7</v>
       </c>
       <c r="S102" s="100">
         <v>20</v>
       </c>
       <c r="T102" s="72"/>
-      <c r="U102" s="110">
-        <f>((JRC_Data!BB9+JRC_Data!BB45)*0.8/1000)*($T$150/$T$147)</f>
-        <v>8.685289256198347</v>
-      </c>
-      <c r="V102" s="110">
-        <f>((JRC_Data!BC9+JRC_Data!BC45)*0.8/1000)*($T$150/$T$147)</f>
-        <v>8.4080991735537189</v>
-      </c>
-      <c r="W102" s="110">
-        <f>((JRC_Data!BD9+JRC_Data!BD45)*0.8/1000)*($T$150/$T$147)</f>
-        <v>7.9461157024793385</v>
-      </c>
-      <c r="X102" s="110">
-        <f>((JRC_Data!BE9+JRC_Data!BE45)*0.8/1000)*($T$150/$T$147)</f>
-        <v>7.1145454545454543</v>
-      </c>
-      <c r="Y102" s="105">
-        <f>(JRC_Data!BL11)/1000</f>
-        <v>2.5999999999999999E-2</v>
+      <c r="U102" s="482">
+        <f>U101*($T$148/$T$147)</f>
+        <v>22.778925619834713</v>
+      </c>
+      <c r="V102" s="482">
+        <f t="shared" ref="V102" si="77">V101*($T$148/$T$147)</f>
+        <v>22.04476084710744</v>
+      </c>
+      <c r="W102" s="482">
+        <f t="shared" ref="W102" si="78">W101*($T$148/$T$147)</f>
+        <v>20.839163429752066</v>
+      </c>
+      <c r="X102" s="482">
+        <f t="shared" ref="X102" si="79">X101*($T$148/$T$147)</f>
+        <v>18.635439049586779</v>
+      </c>
+      <c r="Y102" s="482">
+        <v>0.25</v>
       </c>
       <c r="Z102" s="113"/>
       <c r="AA102" s="91"/>
@@ -32800,11 +32824,11 @@
       </c>
       <c r="AI102" s="156"/>
       <c r="AJ102" s="155" t="str">
-        <f t="shared" si="51"/>
+        <f t="shared" si="64"/>
         <v>R-SW_Det_WOO_N1</v>
       </c>
       <c r="AK102" s="155" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="65"/>
         <v>Residential Biomass Boiler - New 2 SH + WH</v>
       </c>
       <c r="AL102" s="156" t="s">
@@ -32848,19 +32872,19 @@
       <c r="M103" s="78"/>
       <c r="N103" s="90"/>
       <c r="O103" s="87">
-        <f t="shared" si="59"/>
+        <f t="shared" si="76"/>
         <v>0.7</v>
       </c>
       <c r="P103" s="76">
-        <f t="shared" si="59"/>
+        <f t="shared" si="76"/>
         <v>0.7</v>
       </c>
       <c r="Q103" s="76">
-        <f t="shared" si="59"/>
+        <f t="shared" si="76"/>
         <v>0.7</v>
       </c>
       <c r="R103" s="105">
-        <f t="shared" si="59"/>
+        <f t="shared" si="76"/>
         <v>0.7</v>
       </c>
       <c r="S103" s="101">
@@ -32901,11 +32925,11 @@
       </c>
       <c r="AI103" s="156"/>
       <c r="AJ103" s="155" t="str">
-        <f t="shared" si="51"/>
+        <f t="shared" si="64"/>
         <v>*R-H_Apt_HVO_N1</v>
       </c>
       <c r="AK103" s="155" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="65"/>
         <v>Residential  Hydrotreated vegetable oil - New 1 SH</v>
       </c>
       <c r="AL103" s="156" t="s">
@@ -32949,19 +32973,19 @@
       <c r="M104" s="97"/>
       <c r="N104" s="98"/>
       <c r="O104" s="346">
-        <f t="shared" si="59"/>
+        <f t="shared" si="76"/>
         <v>0.7</v>
       </c>
       <c r="P104" s="73">
-        <f t="shared" si="59"/>
+        <f t="shared" si="76"/>
         <v>0.7</v>
       </c>
       <c r="Q104" s="73">
-        <f t="shared" si="59"/>
+        <f t="shared" si="76"/>
         <v>0.7</v>
       </c>
       <c r="R104" s="106">
-        <f t="shared" si="59"/>
+        <f t="shared" si="76"/>
         <v>0.7</v>
       </c>
       <c r="S104" s="102">
@@ -33002,11 +33026,11 @@
       </c>
       <c r="AI104" s="156"/>
       <c r="AJ104" s="155" t="str">
-        <f t="shared" si="51"/>
+        <f t="shared" si="64"/>
         <v>*R-H_Apt_HVO_N2</v>
       </c>
       <c r="AK104" s="155" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="65"/>
         <v>Residential  Hydrotreated vegetable oil - New 1 SH + WH</v>
       </c>
       <c r="AL104" s="156" t="s">
@@ -33146,11 +33170,11 @@
       </c>
       <c r="AI106" s="151"/>
       <c r="AJ106" s="150" t="str">
-        <f t="shared" ref="AJ106:AJ112" si="60">C108</f>
+        <f t="shared" ref="AJ106:AJ112" si="80">C108</f>
         <v>R-SH_Det_ELC_HPN1</v>
       </c>
       <c r="AK106" s="150" t="str">
-        <f t="shared" ref="AK106:AK112" si="61">D108</f>
+        <f t="shared" ref="AK106:AK112" si="81">D108</f>
         <v>Residential Electric Heat Pump - Air to Air - SH</v>
       </c>
       <c r="AL106" s="151" t="s">
@@ -33200,11 +33224,11 @@
       <c r="AG107" s="81"/>
       <c r="AI107" s="153"/>
       <c r="AJ107" s="152" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="80"/>
         <v>R-HC_Det_ELC_HPN1</v>
       </c>
       <c r="AK107" s="152" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="81"/>
         <v>Residential Electric Heat Pump - Air to Air - SH + SC</v>
       </c>
       <c r="AL107" s="153" t="s">
@@ -33290,11 +33314,11 @@
       </c>
       <c r="AI108" s="153"/>
       <c r="AJ108" s="152" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="80"/>
         <v>R-SH_Det_ELC_HPN2</v>
       </c>
       <c r="AK108" s="152" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="81"/>
         <v>Residential Electric Heat Pump - Air to Water - SH</v>
       </c>
       <c r="AL108" s="153" t="s">
@@ -33388,11 +33412,11 @@
       </c>
       <c r="AI109" s="153"/>
       <c r="AJ109" s="152" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="80"/>
         <v>R-SW_Det_ELC_HPN1</v>
       </c>
       <c r="AK109" s="152" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="81"/>
         <v>Residential Electric Heat Pump - Air to Water - SH + WH</v>
       </c>
       <c r="AL109" s="153" t="s">
@@ -33444,25 +33468,23 @@
         <v>20</v>
       </c>
       <c r="T110" s="90"/>
-      <c r="U110" s="87">
-        <f>(JRC_Data!BB18/1000)*($T$149/$T$148)</f>
-        <v>11.628571428571428</v>
-      </c>
-      <c r="V110" s="87">
-        <f>(JRC_Data!BC18/1000)*($T$149/$T$148)</f>
-        <v>10.571428571428571</v>
-      </c>
-      <c r="W110" s="87">
-        <f>(JRC_Data!BD18/1000)*($T$149/$T$148)</f>
-        <v>10.571428571428571</v>
-      </c>
-      <c r="X110" s="87">
-        <f>(JRC_Data!BE18/1000)*($T$149/$T$148)</f>
-        <v>9.5142857142857142</v>
-      </c>
-      <c r="Y110" s="109">
-        <f>JRC_Data!BL18/1000</f>
-        <v>0.15</v>
+      <c r="U110" s="481">
+        <v>9.8469999999999995</v>
+      </c>
+      <c r="V110" s="481">
+        <f>U110*0.91</f>
+        <v>8.9607700000000001</v>
+      </c>
+      <c r="W110" s="481">
+        <f>V110*0.91</f>
+        <v>8.1543007000000003</v>
+      </c>
+      <c r="X110" s="481">
+        <f>U110*0.82</f>
+        <v>8.0745399999999989</v>
+      </c>
+      <c r="Y110" s="481">
+        <v>0.1</v>
       </c>
       <c r="Z110" s="109"/>
       <c r="AA110" s="109"/>
@@ -33478,11 +33500,11 @@
       </c>
       <c r="AI110" s="303"/>
       <c r="AJ110" s="152" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="80"/>
         <v>R-SW_Det_SOL_HPN2</v>
       </c>
       <c r="AK110" s="152" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="81"/>
         <v>Residential Electric Heat Pump - Air to Water - SH + WH + Solar</v>
       </c>
       <c r="AL110" s="153" t="s">
@@ -33531,40 +33553,39 @@
         <v>0.7</v>
       </c>
       <c r="P111" s="70">
-        <f t="shared" ref="P111:P112" si="62">H111*0.7</f>
+        <f t="shared" ref="P111:P112" si="82">H111*0.7</f>
         <v>0.76999999999999991</v>
       </c>
       <c r="Q111" s="70">
-        <f t="shared" ref="Q111:Q112" si="63">I111*0.7</f>
+        <f t="shared" ref="Q111:Q112" si="83">I111*0.7</f>
         <v>0.86333333333333329</v>
       </c>
       <c r="R111" s="104">
-        <f t="shared" ref="R111:R112" si="64">J111*0.7</f>
+        <f t="shared" ref="R111:R112" si="84">J111*0.7</f>
         <v>0.93333333333333324</v>
       </c>
       <c r="S111" s="100">
         <v>20</v>
       </c>
       <c r="T111" s="92"/>
-      <c r="U111" s="69">
-        <f>(JRC_Data!BB18/1000)*($T$150/$T$148)</f>
-        <v>12.548979591836734</v>
-      </c>
-      <c r="V111" s="69">
-        <f>(JRC_Data!BC18/1000)*($T$150/$T$148)</f>
-        <v>11.408163265306122</v>
-      </c>
-      <c r="W111" s="69">
-        <f>(JRC_Data!BD18/1000)*($T$150/$T$148)</f>
-        <v>11.408163265306122</v>
-      </c>
-      <c r="X111" s="69">
-        <f>(JRC_Data!BE18/1000)*($T$150/$T$148)</f>
-        <v>10.267346938775509</v>
-      </c>
-      <c r="Y111" s="110">
-        <f>JRC_Data!BL18/1000</f>
-        <v>0.15</v>
+      <c r="U111" s="482">
+        <f>U110*($T$146/$T$145)</f>
+        <v>9.9300970464135023</v>
+      </c>
+      <c r="V111" s="482">
+        <f t="shared" ref="V111" si="85">V110*($T$146/$T$145)</f>
+        <v>9.0363883122362889</v>
+      </c>
+      <c r="W111" s="482">
+        <f t="shared" ref="W111" si="86">W110*($T$146/$T$145)</f>
+        <v>8.2231133641350223</v>
+      </c>
+      <c r="X111" s="482">
+        <f t="shared" ref="X111" si="87">X110*($T$146/$T$145)</f>
+        <v>8.1426795780590719</v>
+      </c>
+      <c r="Y111" s="482">
+        <v>0.1</v>
       </c>
       <c r="Z111" s="110"/>
       <c r="AA111" s="110"/>
@@ -33580,11 +33601,11 @@
       </c>
       <c r="AI111" s="303"/>
       <c r="AJ111" s="152" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="80"/>
         <v>R-SH_Det_ELC_HPN3</v>
       </c>
       <c r="AK111" s="152" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="81"/>
         <v>Residential Electric Heat Pump - Ground to Water - SH</v>
       </c>
       <c r="AL111" s="153" t="s">
@@ -33633,15 +33654,15 @@
         <v>0.7</v>
       </c>
       <c r="P112" s="76">
-        <f t="shared" si="62"/>
+        <f t="shared" si="82"/>
         <v>0.77700000000000002</v>
       </c>
       <c r="Q112" s="76">
-        <f t="shared" si="63"/>
+        <f t="shared" si="83"/>
         <v>0.83299999999999996</v>
       </c>
       <c r="R112" s="105">
-        <f t="shared" si="64"/>
+        <f t="shared" si="84"/>
         <v>0.83299999999999996</v>
       </c>
       <c r="S112" s="101">
@@ -33686,11 +33707,11 @@
       </c>
       <c r="AI112" s="159"/>
       <c r="AJ112" s="155" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="80"/>
         <v>R-HC_Det_ELC_HPN2</v>
       </c>
       <c r="AK112" s="155" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="81"/>
         <v>Residential Electric Heat Pump - Ground to Water - SH + SC</v>
       </c>
       <c r="AL112" s="156" t="s">
@@ -33981,15 +34002,15 @@
         <v>0.7</v>
       </c>
       <c r="P116" s="341">
-        <f t="shared" ref="P116:P117" si="65">H116*0.7</f>
+        <f t="shared" ref="P116:P117" si="88">H116*0.7</f>
         <v>0.75185185185185177</v>
       </c>
       <c r="Q116" s="341">
-        <f t="shared" ref="Q116:Q117" si="66">I116*0.7</f>
+        <f t="shared" ref="Q116:Q117" si="89">I116*0.7</f>
         <v>0.88148148148148131</v>
       </c>
       <c r="R116" s="342">
-        <f t="shared" ref="R116:R117" si="67">J116*0.7</f>
+        <f t="shared" ref="R116:R117" si="90">J116*0.7</f>
         <v>0.88148148148148131</v>
       </c>
       <c r="S116" s="136">
@@ -34083,15 +34104,15 @@
         <v>0.77777777777777757</v>
       </c>
       <c r="P117" s="348">
-        <f t="shared" si="65"/>
+        <f t="shared" si="88"/>
         <v>0.8037037037037037</v>
       </c>
       <c r="Q117" s="348">
-        <f t="shared" si="66"/>
+        <f t="shared" si="89"/>
         <v>0.8037037037037037</v>
       </c>
       <c r="R117" s="349">
-        <f t="shared" si="67"/>
+        <f t="shared" si="90"/>
         <v>0.82962962962962949</v>
       </c>
       <c r="S117" s="74">
@@ -34186,11 +34207,11 @@
       <c r="AG118" s="81"/>
       <c r="AI118" s="306"/>
       <c r="AJ118" s="150" t="str">
-        <f t="shared" ref="AJ118:AJ119" si="68">C124</f>
+        <f t="shared" ref="AJ118:AJ119" si="91">C124</f>
         <v>R-WH_Det_ELC_N1</v>
       </c>
       <c r="AK118" s="150" t="str">
-        <f t="shared" ref="AK118:AK119" si="69">D124</f>
+        <f t="shared" ref="AK118:AK119" si="92">D124</f>
         <v xml:space="preserve">Residential Electric Water Heater </v>
       </c>
       <c r="AL118" s="151" t="s">
@@ -34239,15 +34260,15 @@
         <v>0.7</v>
       </c>
       <c r="P119" s="348">
-        <f t="shared" ref="P119" si="70">H119*0.7</f>
+        <f t="shared" ref="P119" si="93">H119*0.7</f>
         <v>0.73360000000000003</v>
       </c>
       <c r="Q119" s="348">
-        <f t="shared" ref="Q119" si="71">I119*0.7</f>
+        <f t="shared" ref="Q119" si="94">I119*0.7</f>
         <v>0.76789999999999992</v>
       </c>
       <c r="R119" s="349">
-        <f t="shared" ref="R119" si="72">J119*0.7</f>
+        <f t="shared" ref="R119" si="95">J119*0.7</f>
         <v>0.81269999999999998</v>
       </c>
       <c r="S119" s="5">
@@ -34291,11 +34312,11 @@
       </c>
       <c r="AI119" s="4"/>
       <c r="AJ119" s="152" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="91"/>
         <v>R-WH_Det_SOL_N1</v>
       </c>
       <c r="AK119" s="152" t="str">
-        <f t="shared" si="69"/>
+        <f t="shared" si="92"/>
         <v xml:space="preserve">Residential Solar Water Heater </v>
       </c>
       <c r="AL119" s="153" t="s">
@@ -35012,7 +35033,7 @@
         <v>3</v>
       </c>
       <c r="T141" s="479">
-        <f t="shared" ref="T141:T150" si="73">U141/$U$149</f>
+        <f t="shared" ref="T141:T150" si="96">U141/$U$149</f>
         <v>0.72929037751472525</v>
       </c>
       <c r="U141" s="480">
@@ -35042,7 +35063,7 @@
         <v>5</v>
       </c>
       <c r="T142" s="479">
-        <f t="shared" si="73"/>
+        <f t="shared" si="96"/>
         <v>0.79101166159768732</v>
       </c>
       <c r="U142" s="480">
@@ -35056,7 +35077,7 @@
         <v>8</v>
       </c>
       <c r="T143" s="479">
-        <f t="shared" si="73"/>
+        <f t="shared" si="96"/>
         <v>0.85077698714062355</v>
       </c>
       <c r="U143" s="480">
@@ -35070,7 +35091,7 @@
         <v>10</v>
       </c>
       <c r="T144" s="479">
-        <f t="shared" si="73"/>
+        <f t="shared" si="96"/>
         <v>0.86872586872586877</v>
       </c>
       <c r="U144" s="478">
@@ -35091,7 +35112,7 @@
         <v>15</v>
       </c>
       <c r="T145" s="469">
-        <f t="shared" si="73"/>
+        <f t="shared" si="96"/>
         <v>0.91505791505791501</v>
       </c>
       <c r="U145" s="5">
@@ -35118,7 +35139,7 @@
         <v>18</v>
       </c>
       <c r="T146" s="469">
-        <f t="shared" si="73"/>
+        <f t="shared" si="96"/>
         <v>0.92277992277992282</v>
       </c>
       <c r="U146" s="5">
@@ -35147,7 +35168,7 @@
         <v>20</v>
       </c>
       <c r="T147" s="479">
-        <f t="shared" si="73"/>
+        <f t="shared" si="96"/>
         <v>0.93436293436293438</v>
       </c>
       <c r="U147" s="478">
@@ -35177,7 +35198,7 @@
         <v>24</v>
       </c>
       <c r="T148" s="469">
-        <f t="shared" si="73"/>
+        <f t="shared" si="96"/>
         <v>0.94594594594594594</v>
       </c>
       <c r="U148" s="5">
@@ -35206,7 +35227,7 @@
         <v>30</v>
       </c>
       <c r="T149" s="469">
-        <f t="shared" si="73"/>
+        <f t="shared" si="96"/>
         <v>1</v>
       </c>
       <c r="U149" s="5">
@@ -35235,7 +35256,7 @@
         <v>35</v>
       </c>
       <c r="T150" s="469">
-        <f t="shared" si="73"/>
+        <f t="shared" si="96"/>
         <v>1.0791505791505791</v>
       </c>
       <c r="U150" s="5">
@@ -35280,26 +35301,6 @@
     <row r="162" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="G90:J90"/>
-    <mergeCell ref="K90:N90"/>
-    <mergeCell ref="O90:R90"/>
-    <mergeCell ref="S90:T90"/>
-    <mergeCell ref="U90:X90"/>
-    <mergeCell ref="G88:J88"/>
-    <mergeCell ref="K88:N88"/>
-    <mergeCell ref="O88:R88"/>
-    <mergeCell ref="S88:T88"/>
-    <mergeCell ref="U88:X88"/>
-    <mergeCell ref="G44:J44"/>
-    <mergeCell ref="K44:N44"/>
-    <mergeCell ref="O44:R44"/>
-    <mergeCell ref="S44:T44"/>
-    <mergeCell ref="U44:X44"/>
-    <mergeCell ref="G42:J42"/>
-    <mergeCell ref="K42:N42"/>
-    <mergeCell ref="O42:R42"/>
-    <mergeCell ref="S42:T42"/>
-    <mergeCell ref="U42:X42"/>
     <mergeCell ref="U4:X4"/>
     <mergeCell ref="U6:X6"/>
     <mergeCell ref="G4:J4"/>
@@ -35310,6 +35311,26 @@
     <mergeCell ref="O6:R6"/>
     <mergeCell ref="K6:N6"/>
     <mergeCell ref="G6:J6"/>
+    <mergeCell ref="G42:J42"/>
+    <mergeCell ref="K42:N42"/>
+    <mergeCell ref="O42:R42"/>
+    <mergeCell ref="S42:T42"/>
+    <mergeCell ref="U42:X42"/>
+    <mergeCell ref="G44:J44"/>
+    <mergeCell ref="K44:N44"/>
+    <mergeCell ref="O44:R44"/>
+    <mergeCell ref="S44:T44"/>
+    <mergeCell ref="U44:X44"/>
+    <mergeCell ref="G88:J88"/>
+    <mergeCell ref="K88:N88"/>
+    <mergeCell ref="O88:R88"/>
+    <mergeCell ref="S88:T88"/>
+    <mergeCell ref="U88:X88"/>
+    <mergeCell ref="G90:J90"/>
+    <mergeCell ref="K90:N90"/>
+    <mergeCell ref="O90:R90"/>
+    <mergeCell ref="S90:T90"/>
+    <mergeCell ref="U90:X90"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
@@ -35488,12 +35509,12 @@
       <c r="I6" s="84"/>
       <c r="J6" s="84"/>
       <c r="K6" s="84"/>
-      <c r="L6" s="509" t="s">
+      <c r="L6" s="506" t="s">
         <v>1007</v>
       </c>
-      <c r="M6" s="511"/>
-      <c r="N6" s="511"/>
-      <c r="O6" s="510"/>
+      <c r="M6" s="508"/>
+      <c r="N6" s="508"/>
+      <c r="O6" s="507"/>
       <c r="P6" s="475" t="s">
         <v>1019</v>
       </c>
@@ -47783,103 +47804,103 @@
       <c r="C4" s="381" t="s">
         <v>805</v>
       </c>
-      <c r="D4" s="513" t="s">
+      <c r="D4" s="514" t="s">
         <v>806</v>
       </c>
-      <c r="E4" s="514"/>
-      <c r="F4" s="514"/>
-      <c r="G4" s="514"/>
+      <c r="E4" s="513"/>
+      <c r="F4" s="513"/>
+      <c r="G4" s="513"/>
       <c r="H4" s="515"/>
-      <c r="I4" s="514" t="s">
+      <c r="I4" s="513" t="s">
         <v>807</v>
       </c>
-      <c r="J4" s="514"/>
-      <c r="K4" s="514"/>
-      <c r="L4" s="514"/>
+      <c r="J4" s="513"/>
+      <c r="K4" s="513"/>
+      <c r="L4" s="513"/>
       <c r="M4" s="515"/>
-      <c r="N4" s="514" t="s">
+      <c r="N4" s="513" t="s">
         <v>808</v>
       </c>
-      <c r="O4" s="514"/>
-      <c r="P4" s="514"/>
-      <c r="Q4" s="514"/>
+      <c r="O4" s="513"/>
+      <c r="P4" s="513"/>
+      <c r="Q4" s="513"/>
       <c r="R4" s="515"/>
-      <c r="S4" s="514" t="s">
+      <c r="S4" s="513" t="s">
         <v>809</v>
       </c>
-      <c r="T4" s="514"/>
-      <c r="U4" s="514"/>
-      <c r="V4" s="514"/>
+      <c r="T4" s="513"/>
+      <c r="U4" s="513"/>
+      <c r="V4" s="513"/>
       <c r="W4" s="515"/>
-      <c r="X4" s="514" t="s">
+      <c r="X4" s="513" t="s">
         <v>810</v>
       </c>
-      <c r="Y4" s="514"/>
-      <c r="Z4" s="514"/>
-      <c r="AA4" s="514"/>
+      <c r="Y4" s="513"/>
+      <c r="Z4" s="513"/>
+      <c r="AA4" s="513"/>
       <c r="AB4" s="515"/>
-      <c r="AC4" s="514" t="s">
+      <c r="AC4" s="513" t="s">
         <v>811</v>
       </c>
-      <c r="AD4" s="514"/>
-      <c r="AE4" s="514"/>
-      <c r="AF4" s="514"/>
+      <c r="AD4" s="513"/>
+      <c r="AE4" s="513"/>
+      <c r="AF4" s="513"/>
       <c r="AG4" s="515"/>
-      <c r="AH4" s="514" t="s">
+      <c r="AH4" s="513" t="s">
         <v>812</v>
       </c>
-      <c r="AI4" s="514"/>
-      <c r="AJ4" s="514"/>
-      <c r="AK4" s="514"/>
+      <c r="AI4" s="513"/>
+      <c r="AJ4" s="513"/>
+      <c r="AK4" s="513"/>
       <c r="AL4" s="515"/>
-      <c r="AM4" s="514" t="s">
+      <c r="AM4" s="513" t="s">
         <v>813</v>
       </c>
-      <c r="AN4" s="514"/>
-      <c r="AO4" s="514"/>
-      <c r="AP4" s="514"/>
+      <c r="AN4" s="513"/>
+      <c r="AO4" s="513"/>
+      <c r="AP4" s="513"/>
       <c r="AQ4" s="515"/>
-      <c r="AR4" s="514" t="s">
+      <c r="AR4" s="513" t="s">
         <v>814</v>
       </c>
-      <c r="AS4" s="514"/>
-      <c r="AT4" s="514"/>
-      <c r="AU4" s="514"/>
+      <c r="AS4" s="513"/>
+      <c r="AT4" s="513"/>
+      <c r="AU4" s="513"/>
       <c r="AV4" s="515"/>
-      <c r="AW4" s="514" t="s">
+      <c r="AW4" s="513" t="s">
         <v>815</v>
       </c>
-      <c r="AX4" s="514"/>
-      <c r="AY4" s="514"/>
-      <c r="AZ4" s="514"/>
-      <c r="BA4" s="514"/>
-      <c r="BB4" s="513" t="s">
+      <c r="AX4" s="513"/>
+      <c r="AY4" s="513"/>
+      <c r="AZ4" s="513"/>
+      <c r="BA4" s="513"/>
+      <c r="BB4" s="514" t="s">
         <v>816</v>
       </c>
-      <c r="BC4" s="514"/>
-      <c r="BD4" s="514"/>
-      <c r="BE4" s="514"/>
+      <c r="BC4" s="513"/>
+      <c r="BD4" s="513"/>
+      <c r="BE4" s="513"/>
       <c r="BF4" s="515"/>
-      <c r="BG4" s="514" t="s">
+      <c r="BG4" s="513" t="s">
         <v>817</v>
       </c>
-      <c r="BH4" s="514"/>
-      <c r="BI4" s="514"/>
-      <c r="BJ4" s="514"/>
-      <c r="BK4" s="514"/>
-      <c r="BL4" s="513" t="s">
+      <c r="BH4" s="513"/>
+      <c r="BI4" s="513"/>
+      <c r="BJ4" s="513"/>
+      <c r="BK4" s="513"/>
+      <c r="BL4" s="514" t="s">
         <v>818</v>
       </c>
-      <c r="BM4" s="514"/>
-      <c r="BN4" s="514"/>
-      <c r="BO4" s="514"/>
-      <c r="BP4" s="514"/>
-      <c r="BQ4" s="513" t="s">
+      <c r="BM4" s="513"/>
+      <c r="BN4" s="513"/>
+      <c r="BO4" s="513"/>
+      <c r="BP4" s="513"/>
+      <c r="BQ4" s="514" t="s">
         <v>819</v>
       </c>
-      <c r="BR4" s="514"/>
-      <c r="BS4" s="514"/>
-      <c r="BT4" s="514"/>
+      <c r="BR4" s="513"/>
+      <c r="BS4" s="513"/>
+      <c r="BT4" s="513"/>
       <c r="BU4" s="515"/>
       <c r="BV4" s="382" t="s">
         <v>820</v>
@@ -61473,6 +61494,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="BL4:BP4"/>
+    <mergeCell ref="BQ4:BU4"/>
+    <mergeCell ref="BW4:CA4"/>
+    <mergeCell ref="CB4:CF4"/>
+    <mergeCell ref="CG4:CK4"/>
     <mergeCell ref="BG4:BK4"/>
     <mergeCell ref="D4:H4"/>
     <mergeCell ref="I4:M4"/>
@@ -61485,11 +61511,6 @@
     <mergeCell ref="AR4:AV4"/>
     <mergeCell ref="AW4:BA4"/>
     <mergeCell ref="BB4:BF4"/>
-    <mergeCell ref="BL4:BP4"/>
-    <mergeCell ref="BQ4:BU4"/>
-    <mergeCell ref="BW4:CA4"/>
-    <mergeCell ref="CB4:CF4"/>
-    <mergeCell ref="CG4:CK4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
Upper Solar % in Heat Pump from 50% to 22%
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_RSD.xlsx
+++ b/SubRES_TMPL/SubRes_RSD.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B1BCE6D-564D-48F1-8B0E-3CDF9EC662A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAE06A4F-7CDC-42A4-9E06-C08B418ACA8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{34F9D92C-266F-476D-89E0-63153305AC39}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{34F9D92C-266F-476D-89E0-63153305AC39}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="34" r:id="rId1"/>
@@ -14236,6 +14236,15 @@
     <xf numFmtId="0" fontId="16" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="23" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -14245,22 +14254,13 @@
     <xf numFmtId="0" fontId="16" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="60" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="60" fillId="31" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="60" fillId="31" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="60" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="60" fillId="31" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -24903,8 +24903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{104F8057-C735-4662-BAA6-EEDCF7B57273}">
   <dimension ref="A2:AO162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="AA101" sqref="AA101"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="AB57" sqref="AB57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -25059,28 +25059,28 @@
       <c r="F4" s="63" t="s">
         <v>334</v>
       </c>
-      <c r="G4" s="509" t="s">
+      <c r="G4" s="506" t="s">
         <v>758</v>
       </c>
-      <c r="H4" s="510"/>
-      <c r="I4" s="510"/>
-      <c r="J4" s="511"/>
-      <c r="K4" s="509" t="s">
+      <c r="H4" s="507"/>
+      <c r="I4" s="507"/>
+      <c r="J4" s="508"/>
+      <c r="K4" s="506" t="s">
         <v>336</v>
       </c>
-      <c r="L4" s="510"/>
-      <c r="M4" s="510"/>
-      <c r="N4" s="511"/>
-      <c r="O4" s="509" t="s">
+      <c r="L4" s="507"/>
+      <c r="M4" s="507"/>
+      <c r="N4" s="508"/>
+      <c r="O4" s="506" t="s">
         <v>337</v>
       </c>
-      <c r="P4" s="510"/>
-      <c r="Q4" s="510"/>
-      <c r="R4" s="511"/>
-      <c r="S4" s="509" t="s">
+      <c r="P4" s="507"/>
+      <c r="Q4" s="507"/>
+      <c r="R4" s="508"/>
+      <c r="S4" s="506" t="s">
         <v>338</v>
       </c>
-      <c r="T4" s="511"/>
+      <c r="T4" s="508"/>
       <c r="U4" s="500" t="s">
         <v>339</v>
       </c>
@@ -27939,28 +27939,28 @@
       <c r="F42" s="63" t="s">
         <v>334</v>
       </c>
-      <c r="G42" s="509" t="s">
+      <c r="G42" s="506" t="s">
         <v>335</v>
       </c>
-      <c r="H42" s="510"/>
-      <c r="I42" s="510"/>
-      <c r="J42" s="511"/>
-      <c r="K42" s="509" t="s">
+      <c r="H42" s="507"/>
+      <c r="I42" s="507"/>
+      <c r="J42" s="508"/>
+      <c r="K42" s="506" t="s">
         <v>336</v>
       </c>
-      <c r="L42" s="510"/>
-      <c r="M42" s="510"/>
-      <c r="N42" s="511"/>
-      <c r="O42" s="509" t="s">
+      <c r="L42" s="507"/>
+      <c r="M42" s="507"/>
+      <c r="N42" s="508"/>
+      <c r="O42" s="506" t="s">
         <v>337</v>
       </c>
-      <c r="P42" s="510"/>
-      <c r="Q42" s="510"/>
-      <c r="R42" s="511"/>
-      <c r="S42" s="509" t="s">
+      <c r="P42" s="507"/>
+      <c r="Q42" s="507"/>
+      <c r="R42" s="508"/>
+      <c r="S42" s="506" t="s">
         <v>338</v>
       </c>
-      <c r="T42" s="511"/>
+      <c r="T42" s="508"/>
       <c r="U42" s="500" t="s">
         <v>339</v>
       </c>
@@ -28079,16 +28079,16 @@
       <c r="P44" s="504"/>
       <c r="Q44" s="504"/>
       <c r="R44" s="505"/>
-      <c r="S44" s="506" t="s">
+      <c r="S44" s="509" t="s">
         <v>312</v>
       </c>
-      <c r="T44" s="507"/>
-      <c r="U44" s="506" t="s">
+      <c r="T44" s="510"/>
+      <c r="U44" s="509" t="s">
         <v>1007</v>
       </c>
-      <c r="V44" s="508"/>
-      <c r="W44" s="508"/>
-      <c r="X44" s="507"/>
+      <c r="V44" s="511"/>
+      <c r="W44" s="511"/>
+      <c r="X44" s="510"/>
       <c r="Y44" s="475" t="s">
         <v>1019</v>
       </c>
@@ -29185,13 +29185,8 @@
         <v>0.25</v>
       </c>
       <c r="Z55" s="112"/>
-      <c r="AA55" s="87">
-        <v>7.52</v>
-      </c>
-      <c r="AB55" s="119">
-        <f>6.25/AA55</f>
-        <v>0.83111702127659581</v>
-      </c>
+      <c r="AA55" s="87"/>
+      <c r="AB55" s="119"/>
       <c r="AC55" s="119"/>
       <c r="AD55" s="119"/>
       <c r="AE55" s="109">
@@ -30186,7 +30181,7 @@
       </c>
       <c r="Z66" s="109"/>
       <c r="AA66" s="119">
-        <v>0.5</v>
+        <v>0.22</v>
       </c>
       <c r="AB66" s="109"/>
       <c r="AC66" s="109"/>
@@ -31464,28 +31459,28 @@
       <c r="F88" s="63" t="s">
         <v>334</v>
       </c>
-      <c r="G88" s="509" t="s">
+      <c r="G88" s="506" t="s">
         <v>335</v>
       </c>
-      <c r="H88" s="510"/>
-      <c r="I88" s="510"/>
-      <c r="J88" s="511"/>
-      <c r="K88" s="509" t="s">
+      <c r="H88" s="507"/>
+      <c r="I88" s="507"/>
+      <c r="J88" s="508"/>
+      <c r="K88" s="506" t="s">
         <v>336</v>
       </c>
-      <c r="L88" s="510"/>
-      <c r="M88" s="510"/>
-      <c r="N88" s="511"/>
-      <c r="O88" s="509" t="s">
+      <c r="L88" s="507"/>
+      <c r="M88" s="507"/>
+      <c r="N88" s="508"/>
+      <c r="O88" s="506" t="s">
         <v>337</v>
       </c>
-      <c r="P88" s="510"/>
-      <c r="Q88" s="510"/>
-      <c r="R88" s="511"/>
-      <c r="S88" s="509" t="s">
+      <c r="P88" s="507"/>
+      <c r="Q88" s="507"/>
+      <c r="R88" s="508"/>
+      <c r="S88" s="506" t="s">
         <v>338</v>
       </c>
-      <c r="T88" s="511"/>
+      <c r="T88" s="508"/>
       <c r="U88" s="500" t="s">
         <v>339</v>
       </c>
@@ -31604,16 +31599,16 @@
       <c r="P90" s="504"/>
       <c r="Q90" s="504"/>
       <c r="R90" s="505"/>
-      <c r="S90" s="506" t="s">
+      <c r="S90" s="509" t="s">
         <v>312</v>
       </c>
-      <c r="T90" s="507"/>
-      <c r="U90" s="506" t="s">
+      <c r="T90" s="510"/>
+      <c r="U90" s="509" t="s">
         <v>1007</v>
       </c>
-      <c r="V90" s="508"/>
-      <c r="W90" s="508"/>
-      <c r="X90" s="507"/>
+      <c r="V90" s="511"/>
+      <c r="W90" s="511"/>
+      <c r="X90" s="510"/>
       <c r="Y90" s="475" t="s">
         <v>1019</v>
       </c>
@@ -33691,7 +33686,7 @@
       </c>
       <c r="Z112" s="109"/>
       <c r="AA112" s="119">
-        <v>0.5</v>
+        <v>0.22</v>
       </c>
       <c r="AB112" s="109"/>
       <c r="AC112" s="109"/>
@@ -35301,6 +35296,26 @@
     <row r="162" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="G90:J90"/>
+    <mergeCell ref="K90:N90"/>
+    <mergeCell ref="O90:R90"/>
+    <mergeCell ref="S90:T90"/>
+    <mergeCell ref="U90:X90"/>
+    <mergeCell ref="G88:J88"/>
+    <mergeCell ref="K88:N88"/>
+    <mergeCell ref="O88:R88"/>
+    <mergeCell ref="S88:T88"/>
+    <mergeCell ref="U88:X88"/>
+    <mergeCell ref="G44:J44"/>
+    <mergeCell ref="K44:N44"/>
+    <mergeCell ref="O44:R44"/>
+    <mergeCell ref="S44:T44"/>
+    <mergeCell ref="U44:X44"/>
+    <mergeCell ref="G42:J42"/>
+    <mergeCell ref="K42:N42"/>
+    <mergeCell ref="O42:R42"/>
+    <mergeCell ref="S42:T42"/>
+    <mergeCell ref="U42:X42"/>
     <mergeCell ref="U4:X4"/>
     <mergeCell ref="U6:X6"/>
     <mergeCell ref="G4:J4"/>
@@ -35311,26 +35326,6 @@
     <mergeCell ref="O6:R6"/>
     <mergeCell ref="K6:N6"/>
     <mergeCell ref="G6:J6"/>
-    <mergeCell ref="G42:J42"/>
-    <mergeCell ref="K42:N42"/>
-    <mergeCell ref="O42:R42"/>
-    <mergeCell ref="S42:T42"/>
-    <mergeCell ref="U42:X42"/>
-    <mergeCell ref="G44:J44"/>
-    <mergeCell ref="K44:N44"/>
-    <mergeCell ref="O44:R44"/>
-    <mergeCell ref="S44:T44"/>
-    <mergeCell ref="U44:X44"/>
-    <mergeCell ref="G88:J88"/>
-    <mergeCell ref="K88:N88"/>
-    <mergeCell ref="O88:R88"/>
-    <mergeCell ref="S88:T88"/>
-    <mergeCell ref="U88:X88"/>
-    <mergeCell ref="G90:J90"/>
-    <mergeCell ref="K90:N90"/>
-    <mergeCell ref="O90:R90"/>
-    <mergeCell ref="S90:T90"/>
-    <mergeCell ref="U90:X90"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
@@ -35509,12 +35504,12 @@
       <c r="I6" s="84"/>
       <c r="J6" s="84"/>
       <c r="K6" s="84"/>
-      <c r="L6" s="506" t="s">
+      <c r="L6" s="509" t="s">
         <v>1007</v>
       </c>
-      <c r="M6" s="508"/>
-      <c r="N6" s="508"/>
-      <c r="O6" s="507"/>
+      <c r="M6" s="511"/>
+      <c r="N6" s="511"/>
+      <c r="O6" s="510"/>
       <c r="P6" s="475" t="s">
         <v>1019</v>
       </c>
@@ -47804,103 +47799,103 @@
       <c r="C4" s="381" t="s">
         <v>805</v>
       </c>
-      <c r="D4" s="514" t="s">
+      <c r="D4" s="513" t="s">
         <v>806</v>
       </c>
-      <c r="E4" s="513"/>
-      <c r="F4" s="513"/>
-      <c r="G4" s="513"/>
+      <c r="E4" s="514"/>
+      <c r="F4" s="514"/>
+      <c r="G4" s="514"/>
       <c r="H4" s="515"/>
-      <c r="I4" s="513" t="s">
+      <c r="I4" s="514" t="s">
         <v>807</v>
       </c>
-      <c r="J4" s="513"/>
-      <c r="K4" s="513"/>
-      <c r="L4" s="513"/>
+      <c r="J4" s="514"/>
+      <c r="K4" s="514"/>
+      <c r="L4" s="514"/>
       <c r="M4" s="515"/>
-      <c r="N4" s="513" t="s">
+      <c r="N4" s="514" t="s">
         <v>808</v>
       </c>
-      <c r="O4" s="513"/>
-      <c r="P4" s="513"/>
-      <c r="Q4" s="513"/>
+      <c r="O4" s="514"/>
+      <c r="P4" s="514"/>
+      <c r="Q4" s="514"/>
       <c r="R4" s="515"/>
-      <c r="S4" s="513" t="s">
+      <c r="S4" s="514" t="s">
         <v>809</v>
       </c>
-      <c r="T4" s="513"/>
-      <c r="U4" s="513"/>
-      <c r="V4" s="513"/>
+      <c r="T4" s="514"/>
+      <c r="U4" s="514"/>
+      <c r="V4" s="514"/>
       <c r="W4" s="515"/>
-      <c r="X4" s="513" t="s">
+      <c r="X4" s="514" t="s">
         <v>810</v>
       </c>
-      <c r="Y4" s="513"/>
-      <c r="Z4" s="513"/>
-      <c r="AA4" s="513"/>
+      <c r="Y4" s="514"/>
+      <c r="Z4" s="514"/>
+      <c r="AA4" s="514"/>
       <c r="AB4" s="515"/>
-      <c r="AC4" s="513" t="s">
+      <c r="AC4" s="514" t="s">
         <v>811</v>
       </c>
-      <c r="AD4" s="513"/>
-      <c r="AE4" s="513"/>
-      <c r="AF4" s="513"/>
+      <c r="AD4" s="514"/>
+      <c r="AE4" s="514"/>
+      <c r="AF4" s="514"/>
       <c r="AG4" s="515"/>
-      <c r="AH4" s="513" t="s">
+      <c r="AH4" s="514" t="s">
         <v>812</v>
       </c>
-      <c r="AI4" s="513"/>
-      <c r="AJ4" s="513"/>
-      <c r="AK4" s="513"/>
+      <c r="AI4" s="514"/>
+      <c r="AJ4" s="514"/>
+      <c r="AK4" s="514"/>
       <c r="AL4" s="515"/>
-      <c r="AM4" s="513" t="s">
+      <c r="AM4" s="514" t="s">
         <v>813</v>
       </c>
-      <c r="AN4" s="513"/>
-      <c r="AO4" s="513"/>
-      <c r="AP4" s="513"/>
+      <c r="AN4" s="514"/>
+      <c r="AO4" s="514"/>
+      <c r="AP4" s="514"/>
       <c r="AQ4" s="515"/>
-      <c r="AR4" s="513" t="s">
+      <c r="AR4" s="514" t="s">
         <v>814</v>
       </c>
-      <c r="AS4" s="513"/>
-      <c r="AT4" s="513"/>
-      <c r="AU4" s="513"/>
+      <c r="AS4" s="514"/>
+      <c r="AT4" s="514"/>
+      <c r="AU4" s="514"/>
       <c r="AV4" s="515"/>
-      <c r="AW4" s="513" t="s">
+      <c r="AW4" s="514" t="s">
         <v>815</v>
       </c>
-      <c r="AX4" s="513"/>
-      <c r="AY4" s="513"/>
-      <c r="AZ4" s="513"/>
-      <c r="BA4" s="513"/>
-      <c r="BB4" s="514" t="s">
+      <c r="AX4" s="514"/>
+      <c r="AY4" s="514"/>
+      <c r="AZ4" s="514"/>
+      <c r="BA4" s="514"/>
+      <c r="BB4" s="513" t="s">
         <v>816</v>
       </c>
-      <c r="BC4" s="513"/>
-      <c r="BD4" s="513"/>
-      <c r="BE4" s="513"/>
+      <c r="BC4" s="514"/>
+      <c r="BD4" s="514"/>
+      <c r="BE4" s="514"/>
       <c r="BF4" s="515"/>
-      <c r="BG4" s="513" t="s">
+      <c r="BG4" s="514" t="s">
         <v>817</v>
       </c>
-      <c r="BH4" s="513"/>
-      <c r="BI4" s="513"/>
-      <c r="BJ4" s="513"/>
-      <c r="BK4" s="513"/>
-      <c r="BL4" s="514" t="s">
+      <c r="BH4" s="514"/>
+      <c r="BI4" s="514"/>
+      <c r="BJ4" s="514"/>
+      <c r="BK4" s="514"/>
+      <c r="BL4" s="513" t="s">
         <v>818</v>
       </c>
-      <c r="BM4" s="513"/>
-      <c r="BN4" s="513"/>
-      <c r="BO4" s="513"/>
-      <c r="BP4" s="513"/>
-      <c r="BQ4" s="514" t="s">
+      <c r="BM4" s="514"/>
+      <c r="BN4" s="514"/>
+      <c r="BO4" s="514"/>
+      <c r="BP4" s="514"/>
+      <c r="BQ4" s="513" t="s">
         <v>819</v>
       </c>
-      <c r="BR4" s="513"/>
-      <c r="BS4" s="513"/>
-      <c r="BT4" s="513"/>
+      <c r="BR4" s="514"/>
+      <c r="BS4" s="514"/>
+      <c r="BT4" s="514"/>
       <c r="BU4" s="515"/>
       <c r="BV4" s="382" t="s">
         <v>820</v>
@@ -61494,11 +61489,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="BL4:BP4"/>
-    <mergeCell ref="BQ4:BU4"/>
-    <mergeCell ref="BW4:CA4"/>
-    <mergeCell ref="CB4:CF4"/>
-    <mergeCell ref="CG4:CK4"/>
     <mergeCell ref="BG4:BK4"/>
     <mergeCell ref="D4:H4"/>
     <mergeCell ref="I4:M4"/>
@@ -61511,6 +61501,11 @@
     <mergeCell ref="AR4:AV4"/>
     <mergeCell ref="AW4:BA4"/>
     <mergeCell ref="BB4:BF4"/>
+    <mergeCell ref="BL4:BP4"/>
+    <mergeCell ref="BQ4:BU4"/>
+    <mergeCell ref="BW4:CA4"/>
+    <mergeCell ref="CB4:CF4"/>
+    <mergeCell ref="CG4:CK4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
Restrict Share of Gas Cookers - Hannah Request
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_RSD.xlsx
+++ b/SubRES_TMPL/SubRes_RSD.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E22E8DE8-0977-42E6-A3B7-FE2AB81EFDD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D529299E-C665-4A0F-8240-74DC8534CD11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{34F9D92C-266F-476D-89E0-63153305AC39}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{34F9D92C-266F-476D-89E0-63153305AC39}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="34" r:id="rId1"/>
@@ -880,7 +880,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="W8" authorId="0" shapeId="0" xr:uid="{F4C0E48F-FDE9-4CD4-ABE3-46D39A24ADEC}">
+    <comment ref="X8" authorId="0" shapeId="0" xr:uid="{F4C0E48F-FDE9-4CD4-ABE3-46D39A24ADEC}">
       <text>
         <r>
           <rPr>
@@ -929,7 +929,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R15" authorId="0" shapeId="0" xr:uid="{D4205CCA-7C8D-4F75-8CA5-D31091C09E06}">
+    <comment ref="S15" authorId="0" shapeId="0" xr:uid="{D4205CCA-7C8D-4F75-8CA5-D31091C09E06}">
       <text>
         <r>
           <rPr>
@@ -8710,7 +8710,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3471" uniqueCount="1063">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3472" uniqueCount="1064">
   <si>
     <t>Document type:</t>
   </si>
@@ -11920,6 +11920,9 @@
   </si>
   <si>
     <t>Ratio</t>
+  </si>
+  <si>
+    <t>Share-I~UP</t>
   </si>
 </sst>
 </file>
@@ -13534,7 +13537,7 @@
     <xf numFmtId="0" fontId="39" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="54" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="544">
+  <cellXfs count="546">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -14524,6 +14527,8 @@
     <xf numFmtId="0" fontId="10" fillId="23" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="16" fillId="37" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="16" fillId="37" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -14563,6 +14568,12 @@
     <xf numFmtId="164" fontId="46" fillId="10" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="53" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -14584,6 +14595,15 @@
     <xf numFmtId="0" fontId="16" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="23" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -14592,15 +14612,6 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -14617,16 +14628,10 @@
     <xf numFmtId="0" fontId="16" fillId="23" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="60" fillId="31" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="60" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="31" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="60" fillId="31" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -14641,8 +14646,8 @@
     <xf numFmtId="0" fontId="60" fillId="32" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="16" fillId="37" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="16" fillId="37" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="40" fillId="0" borderId="40" xfId="15" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="40" fillId="21" borderId="40" xfId="15" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="20% - Colore 2" xfId="11" xr:uid="{3E3DAF22-4D86-48A9-B6EE-8D230C1E993C}"/>
@@ -16064,14 +16069,14 @@
       <c r="F16" s="216"/>
     </row>
     <row r="17" spans="1:14" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="504" t="s">
+      <c r="A17" s="506" t="s">
         <v>467</v>
       </c>
-      <c r="B17" s="504"/>
-      <c r="C17" s="504"/>
-      <c r="D17" s="504"/>
-      <c r="E17" s="504"/>
-      <c r="F17" s="504"/>
+      <c r="B17" s="506"/>
+      <c r="C17" s="506"/>
+      <c r="D17" s="506"/>
+      <c r="E17" s="506"/>
+      <c r="F17" s="506"/>
       <c r="G17" s="218"/>
       <c r="H17" s="218"/>
       <c r="I17" s="219"/>
@@ -16109,13 +16114,13 @@
       <c r="A20" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="505" t="s">
+      <c r="B20" s="507" t="s">
         <v>469</v>
       </c>
-      <c r="C20" s="505"/>
-      <c r="D20" s="505"/>
-      <c r="E20" s="505"/>
-      <c r="F20" s="505"/>
+      <c r="C20" s="507"/>
+      <c r="D20" s="507"/>
+      <c r="E20" s="507"/>
+      <c r="F20" s="507"/>
       <c r="G20" s="223"/>
       <c r="H20" s="223"/>
       <c r="I20" s="224"/>
@@ -16129,13 +16134,13 @@
       <c r="A21" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="506" t="s">
+      <c r="B21" s="508" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="506"/>
-      <c r="D21" s="506"/>
-      <c r="E21" s="506"/>
-      <c r="F21" s="506"/>
+      <c r="C21" s="508"/>
+      <c r="D21" s="508"/>
+      <c r="E21" s="508"/>
+      <c r="F21" s="508"/>
       <c r="G21" s="223"/>
       <c r="H21" s="223"/>
       <c r="I21" s="224"/>
@@ -16149,13 +16154,13 @@
       <c r="A22" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="506" t="s">
+      <c r="B22" s="508" t="s">
         <v>58</v>
       </c>
-      <c r="C22" s="506"/>
-      <c r="D22" s="506"/>
-      <c r="E22" s="506"/>
-      <c r="F22" s="506"/>
+      <c r="C22" s="508"/>
+      <c r="D22" s="508"/>
+      <c r="E22" s="508"/>
+      <c r="F22" s="508"/>
     </row>
     <row r="23" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
@@ -16184,22 +16189,22 @@
       <c r="H24" s="3"/>
     </row>
     <row r="25" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="507"/>
-      <c r="B25" s="507"/>
-      <c r="C25" s="507"/>
-      <c r="D25" s="507"/>
-      <c r="E25" s="507"/>
-      <c r="F25" s="507"/>
+      <c r="A25" s="509"/>
+      <c r="B25" s="509"/>
+      <c r="C25" s="509"/>
+      <c r="D25" s="509"/>
+      <c r="E25" s="509"/>
+      <c r="F25" s="509"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
     </row>
     <row r="26" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="503"/>
-      <c r="B26" s="503"/>
-      <c r="C26" s="503"/>
-      <c r="D26" s="503"/>
-      <c r="E26" s="503"/>
-      <c r="F26" s="503"/>
+      <c r="A26" s="505"/>
+      <c r="B26" s="505"/>
+      <c r="C26" s="505"/>
+      <c r="D26" s="505"/>
+      <c r="E26" s="505"/>
+      <c r="F26" s="505"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="216"/>
@@ -16386,16 +16391,16 @@
   <sheetData>
     <row r="1" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:20" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="508" t="s">
+      <c r="B2" s="510" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="509"/>
-      <c r="D2" s="509"/>
-      <c r="E2" s="510"/>
-      <c r="G2" s="508" t="s">
+      <c r="C2" s="511"/>
+      <c r="D2" s="511"/>
+      <c r="E2" s="512"/>
+      <c r="G2" s="510" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="510"/>
+      <c r="H2" s="512"/>
       <c r="I2" s="227"/>
       <c r="J2" s="227"/>
       <c r="K2" s="228"/>
@@ -16737,16 +16742,16 @@
     </row>
     <row r="19" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="2:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="511" t="s">
+      <c r="B20" s="513" t="s">
         <v>80</v>
       </c>
-      <c r="C20" s="512"/>
-      <c r="D20" s="512"/>
-      <c r="E20" s="513"/>
-      <c r="G20" s="508" t="s">
+      <c r="C20" s="514"/>
+      <c r="D20" s="514"/>
+      <c r="E20" s="515"/>
+      <c r="G20" s="510" t="s">
         <v>14</v>
       </c>
-      <c r="H20" s="510"/>
+      <c r="H20" s="512"/>
     </row>
     <row r="21" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="255" t="s">
@@ -16990,16 +16995,16 @@
     </row>
     <row r="37" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="38" spans="2:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="508" t="s">
+      <c r="B38" s="510" t="s">
         <v>88</v>
       </c>
-      <c r="C38" s="509"/>
-      <c r="D38" s="509"/>
-      <c r="E38" s="510"/>
-      <c r="G38" s="514" t="s">
+      <c r="C38" s="511"/>
+      <c r="D38" s="511"/>
+      <c r="E38" s="512"/>
+      <c r="G38" s="516" t="s">
         <v>82</v>
       </c>
-      <c r="H38" s="515"/>
+      <c r="H38" s="517"/>
     </row>
     <row r="39" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B39" s="276" t="s">
@@ -17165,13 +17170,13 @@
       <c r="L3" s="5" t="s">
         <v>419</v>
       </c>
-      <c r="R3" s="516" t="s">
+      <c r="R3" s="520" t="s">
         <v>715</v>
       </c>
-      <c r="S3" s="516"/>
-      <c r="T3" s="516"/>
-      <c r="U3" s="516"/>
-      <c r="V3" s="516"/>
+      <c r="S3" s="520"/>
+      <c r="T3" s="520"/>
+      <c r="U3" s="520"/>
+      <c r="V3" s="520"/>
     </row>
     <row r="4" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C4" s="63" t="s">
@@ -17611,25 +17616,25 @@
       <c r="I18" s="192">
         <v>2020</v>
       </c>
-      <c r="Q18" s="534" t="s">
+      <c r="Q18" s="518" t="s">
         <v>1061</v>
       </c>
-      <c r="R18" s="535"/>
-      <c r="S18" s="535"/>
-      <c r="T18" s="535"/>
-      <c r="U18" s="535"/>
-      <c r="V18" s="535"/>
-      <c r="W18" s="535"/>
-      <c r="X18" s="535"/>
-      <c r="Y18" s="535"/>
-      <c r="Z18" s="535"/>
-      <c r="AA18" s="535"/>
-      <c r="AB18" s="535"/>
-      <c r="AC18" s="535"/>
-      <c r="AD18" s="535"/>
-      <c r="AE18" s="535"/>
-      <c r="AF18" s="535"/>
-      <c r="AG18" s="535"/>
+      <c r="R18" s="519"/>
+      <c r="S18" s="519"/>
+      <c r="T18" s="519"/>
+      <c r="U18" s="519"/>
+      <c r="V18" s="519"/>
+      <c r="W18" s="519"/>
+      <c r="X18" s="519"/>
+      <c r="Y18" s="519"/>
+      <c r="Z18" s="519"/>
+      <c r="AA18" s="519"/>
+      <c r="AB18" s="519"/>
+      <c r="AC18" s="519"/>
+      <c r="AD18" s="519"/>
+      <c r="AE18" s="519"/>
+      <c r="AF18" s="519"/>
+      <c r="AG18" s="519"/>
     </row>
     <row r="19" spans="2:33" x14ac:dyDescent="0.2">
       <c r="C19" s="110"/>
@@ -24843,8 +24848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{104F8057-C735-4662-BAA6-EEDCF7B57273}">
   <dimension ref="A2:AO162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D71" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="T110" sqref="T110"/>
+    <sheetView topLeftCell="D1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="AA3" sqref="AA3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -24999,34 +25004,34 @@
       <c r="F4" s="63" t="s">
         <v>334</v>
       </c>
-      <c r="G4" s="526" t="s">
+      <c r="G4" s="527" t="s">
         <v>756</v>
       </c>
-      <c r="H4" s="527"/>
-      <c r="I4" s="527"/>
-      <c r="J4" s="528"/>
-      <c r="K4" s="526" t="s">
+      <c r="H4" s="528"/>
+      <c r="I4" s="528"/>
+      <c r="J4" s="529"/>
+      <c r="K4" s="527" t="s">
         <v>336</v>
       </c>
-      <c r="L4" s="527"/>
-      <c r="M4" s="527"/>
-      <c r="N4" s="528"/>
-      <c r="O4" s="526" t="s">
+      <c r="L4" s="528"/>
+      <c r="M4" s="528"/>
+      <c r="N4" s="529"/>
+      <c r="O4" s="527" t="s">
         <v>337</v>
       </c>
-      <c r="P4" s="527"/>
-      <c r="Q4" s="527"/>
-      <c r="R4" s="528"/>
-      <c r="S4" s="526" t="s">
+      <c r="P4" s="528"/>
+      <c r="Q4" s="528"/>
+      <c r="R4" s="529"/>
+      <c r="S4" s="527" t="s">
         <v>338</v>
       </c>
-      <c r="T4" s="528"/>
-      <c r="U4" s="517" t="s">
+      <c r="T4" s="529"/>
+      <c r="U4" s="521" t="s">
         <v>339</v>
       </c>
-      <c r="V4" s="518"/>
-      <c r="W4" s="518"/>
-      <c r="X4" s="519"/>
+      <c r="V4" s="522"/>
+      <c r="W4" s="522"/>
+      <c r="X4" s="523"/>
       <c r="Y4" s="107"/>
       <c r="Z4" s="107"/>
       <c r="AA4" s="115" t="s">
@@ -25121,34 +25126,34 @@
       <c r="D6" s="85"/>
       <c r="E6" s="85"/>
       <c r="F6" s="86"/>
-      <c r="G6" s="520" t="s">
+      <c r="G6" s="524" t="s">
         <v>1062</v>
       </c>
-      <c r="H6" s="521"/>
-      <c r="I6" s="521"/>
-      <c r="J6" s="522"/>
-      <c r="K6" s="520" t="s">
+      <c r="H6" s="525"/>
+      <c r="I6" s="525"/>
+      <c r="J6" s="526"/>
+      <c r="K6" s="524" t="s">
         <v>1062</v>
       </c>
-      <c r="L6" s="521"/>
-      <c r="M6" s="521"/>
-      <c r="N6" s="522"/>
-      <c r="O6" s="520" t="s">
+      <c r="L6" s="525"/>
+      <c r="M6" s="525"/>
+      <c r="N6" s="526"/>
+      <c r="O6" s="524" t="s">
         <v>1062</v>
       </c>
-      <c r="P6" s="521"/>
-      <c r="Q6" s="521"/>
-      <c r="R6" s="522"/>
-      <c r="S6" s="520" t="s">
+      <c r="P6" s="525"/>
+      <c r="Q6" s="525"/>
+      <c r="R6" s="526"/>
+      <c r="S6" s="524" t="s">
         <v>312</v>
       </c>
-      <c r="T6" s="522"/>
-      <c r="U6" s="520" t="s">
+      <c r="T6" s="526"/>
+      <c r="U6" s="524" t="s">
         <v>1005</v>
       </c>
-      <c r="V6" s="521"/>
-      <c r="W6" s="521"/>
-      <c r="X6" s="522"/>
+      <c r="V6" s="525"/>
+      <c r="W6" s="525"/>
+      <c r="X6" s="526"/>
       <c r="Y6" s="108" t="s">
         <v>1017</v>
       </c>
@@ -27879,34 +27884,34 @@
       <c r="F42" s="63" t="s">
         <v>334</v>
       </c>
-      <c r="G42" s="526" t="s">
+      <c r="G42" s="527" t="s">
         <v>335</v>
       </c>
-      <c r="H42" s="527"/>
-      <c r="I42" s="527"/>
-      <c r="J42" s="528"/>
-      <c r="K42" s="526" t="s">
+      <c r="H42" s="528"/>
+      <c r="I42" s="528"/>
+      <c r="J42" s="529"/>
+      <c r="K42" s="527" t="s">
         <v>336</v>
       </c>
-      <c r="L42" s="527"/>
-      <c r="M42" s="527"/>
-      <c r="N42" s="528"/>
-      <c r="O42" s="526" t="s">
+      <c r="L42" s="528"/>
+      <c r="M42" s="528"/>
+      <c r="N42" s="529"/>
+      <c r="O42" s="527" t="s">
         <v>337</v>
       </c>
-      <c r="P42" s="527"/>
-      <c r="Q42" s="527"/>
-      <c r="R42" s="528"/>
-      <c r="S42" s="526" t="s">
+      <c r="P42" s="528"/>
+      <c r="Q42" s="528"/>
+      <c r="R42" s="529"/>
+      <c r="S42" s="527" t="s">
         <v>338</v>
       </c>
-      <c r="T42" s="528"/>
-      <c r="U42" s="517" t="s">
+      <c r="T42" s="529"/>
+      <c r="U42" s="521" t="s">
         <v>339</v>
       </c>
-      <c r="V42" s="518"/>
-      <c r="W42" s="518"/>
-      <c r="X42" s="519"/>
+      <c r="V42" s="522"/>
+      <c r="W42" s="522"/>
+      <c r="X42" s="523"/>
       <c r="Y42" s="107"/>
       <c r="Z42" s="107"/>
       <c r="AA42" s="115" t="s">
@@ -28001,34 +28006,34 @@
       <c r="D44" s="85"/>
       <c r="E44" s="85"/>
       <c r="F44" s="86"/>
-      <c r="G44" s="520" t="s">
+      <c r="G44" s="524" t="s">
         <v>55</v>
       </c>
-      <c r="H44" s="521"/>
-      <c r="I44" s="521"/>
-      <c r="J44" s="522"/>
-      <c r="K44" s="521" t="s">
+      <c r="H44" s="525"/>
+      <c r="I44" s="525"/>
+      <c r="J44" s="526"/>
+      <c r="K44" s="525" t="s">
         <v>55</v>
       </c>
-      <c r="L44" s="521"/>
-      <c r="M44" s="521"/>
-      <c r="N44" s="522"/>
-      <c r="O44" s="520" t="s">
+      <c r="L44" s="525"/>
+      <c r="M44" s="525"/>
+      <c r="N44" s="526"/>
+      <c r="O44" s="524" t="s">
         <v>55</v>
       </c>
-      <c r="P44" s="521"/>
-      <c r="Q44" s="521"/>
-      <c r="R44" s="522"/>
-      <c r="S44" s="523" t="s">
+      <c r="P44" s="525"/>
+      <c r="Q44" s="525"/>
+      <c r="R44" s="526"/>
+      <c r="S44" s="530" t="s">
         <v>312</v>
       </c>
-      <c r="T44" s="524"/>
-      <c r="U44" s="523" t="s">
+      <c r="T44" s="531"/>
+      <c r="U44" s="530" t="s">
         <v>1005</v>
       </c>
-      <c r="V44" s="525"/>
-      <c r="W44" s="525"/>
-      <c r="X44" s="524"/>
+      <c r="V44" s="532"/>
+      <c r="W44" s="532"/>
+      <c r="X44" s="531"/>
       <c r="Y44" s="463" t="s">
         <v>1017</v>
       </c>
@@ -28339,7 +28344,7 @@
         <v>0.2656</v>
       </c>
       <c r="Z47" s="112"/>
-      <c r="AA47" s="542">
+      <c r="AA47" s="503">
         <v>0.1</v>
       </c>
       <c r="AB47" s="119"/>
@@ -28737,7 +28742,7 @@
         <v>0.19</v>
       </c>
       <c r="Z51" s="112"/>
-      <c r="AA51" s="542">
+      <c r="AA51" s="503">
         <v>0.1</v>
       </c>
       <c r="AB51" s="119"/>
@@ -30120,7 +30125,7 @@
         <v>0.16960000000000003</v>
       </c>
       <c r="Z66" s="109"/>
-      <c r="AA66" s="543">
+      <c r="AA66" s="504">
         <v>0.1</v>
       </c>
       <c r="AB66" s="109"/>
@@ -31399,34 +31404,34 @@
       <c r="F88" s="63" t="s">
         <v>334</v>
       </c>
-      <c r="G88" s="526" t="s">
+      <c r="G88" s="527" t="s">
         <v>335</v>
       </c>
-      <c r="H88" s="527"/>
-      <c r="I88" s="527"/>
-      <c r="J88" s="528"/>
-      <c r="K88" s="526" t="s">
+      <c r="H88" s="528"/>
+      <c r="I88" s="528"/>
+      <c r="J88" s="529"/>
+      <c r="K88" s="527" t="s">
         <v>336</v>
       </c>
-      <c r="L88" s="527"/>
-      <c r="M88" s="527"/>
-      <c r="N88" s="528"/>
-      <c r="O88" s="526" t="s">
+      <c r="L88" s="528"/>
+      <c r="M88" s="528"/>
+      <c r="N88" s="529"/>
+      <c r="O88" s="527" t="s">
         <v>337</v>
       </c>
-      <c r="P88" s="527"/>
-      <c r="Q88" s="527"/>
-      <c r="R88" s="528"/>
-      <c r="S88" s="526" t="s">
+      <c r="P88" s="528"/>
+      <c r="Q88" s="528"/>
+      <c r="R88" s="529"/>
+      <c r="S88" s="527" t="s">
         <v>338</v>
       </c>
-      <c r="T88" s="528"/>
-      <c r="U88" s="517" t="s">
+      <c r="T88" s="529"/>
+      <c r="U88" s="521" t="s">
         <v>339</v>
       </c>
-      <c r="V88" s="518"/>
-      <c r="W88" s="518"/>
-      <c r="X88" s="519"/>
+      <c r="V88" s="522"/>
+      <c r="W88" s="522"/>
+      <c r="X88" s="523"/>
       <c r="Y88" s="107"/>
       <c r="Z88" s="107"/>
       <c r="AA88" s="115" t="s">
@@ -31521,34 +31526,34 @@
       <c r="D90" s="85"/>
       <c r="E90" s="85"/>
       <c r="F90" s="86"/>
-      <c r="G90" s="520" t="s">
+      <c r="G90" s="524" t="s">
         <v>55</v>
       </c>
-      <c r="H90" s="521"/>
-      <c r="I90" s="521"/>
-      <c r="J90" s="522"/>
-      <c r="K90" s="521" t="s">
+      <c r="H90" s="525"/>
+      <c r="I90" s="525"/>
+      <c r="J90" s="526"/>
+      <c r="K90" s="525" t="s">
         <v>55</v>
       </c>
-      <c r="L90" s="521"/>
-      <c r="M90" s="521"/>
-      <c r="N90" s="522"/>
-      <c r="O90" s="520" t="s">
+      <c r="L90" s="525"/>
+      <c r="M90" s="525"/>
+      <c r="N90" s="526"/>
+      <c r="O90" s="524" t="s">
         <v>55</v>
       </c>
-      <c r="P90" s="521"/>
-      <c r="Q90" s="521"/>
-      <c r="R90" s="522"/>
-      <c r="S90" s="523" t="s">
+      <c r="P90" s="525"/>
+      <c r="Q90" s="525"/>
+      <c r="R90" s="526"/>
+      <c r="S90" s="530" t="s">
         <v>312</v>
       </c>
-      <c r="T90" s="524"/>
-      <c r="U90" s="523" t="s">
+      <c r="T90" s="531"/>
+      <c r="U90" s="530" t="s">
         <v>1005</v>
       </c>
-      <c r="V90" s="525"/>
-      <c r="W90" s="525"/>
-      <c r="X90" s="524"/>
+      <c r="V90" s="532"/>
+      <c r="W90" s="532"/>
+      <c r="X90" s="531"/>
       <c r="Y90" s="463" t="s">
         <v>1017</v>
       </c>
@@ -31859,7 +31864,7 @@
         <v>0.2656</v>
       </c>
       <c r="Z93" s="112"/>
-      <c r="AA93" s="542">
+      <c r="AA93" s="503">
         <v>0.1</v>
       </c>
       <c r="AB93" s="119"/>
@@ -32257,7 +32262,7 @@
         <v>0.19</v>
       </c>
       <c r="Z97" s="112"/>
-      <c r="AA97" s="542">
+      <c r="AA97" s="503">
         <v>0.1</v>
       </c>
       <c r="AB97" s="119"/>
@@ -33625,7 +33630,7 @@
         <v>0.16960000000000003</v>
       </c>
       <c r="Z112" s="109"/>
-      <c r="AA112" s="543">
+      <c r="AA112" s="504">
         <v>0.1</v>
       </c>
       <c r="AB112" s="109"/>
@@ -35236,6 +35241,26 @@
     <row r="162" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="G90:J90"/>
+    <mergeCell ref="K90:N90"/>
+    <mergeCell ref="O90:R90"/>
+    <mergeCell ref="S90:T90"/>
+    <mergeCell ref="U90:X90"/>
+    <mergeCell ref="G88:J88"/>
+    <mergeCell ref="K88:N88"/>
+    <mergeCell ref="O88:R88"/>
+    <mergeCell ref="S88:T88"/>
+    <mergeCell ref="U88:X88"/>
+    <mergeCell ref="G44:J44"/>
+    <mergeCell ref="K44:N44"/>
+    <mergeCell ref="O44:R44"/>
+    <mergeCell ref="S44:T44"/>
+    <mergeCell ref="U44:X44"/>
+    <mergeCell ref="G42:J42"/>
+    <mergeCell ref="K42:N42"/>
+    <mergeCell ref="O42:R42"/>
+    <mergeCell ref="S42:T42"/>
+    <mergeCell ref="U42:X42"/>
     <mergeCell ref="U4:X4"/>
     <mergeCell ref="U6:X6"/>
     <mergeCell ref="G4:J4"/>
@@ -35246,26 +35271,6 @@
     <mergeCell ref="O6:R6"/>
     <mergeCell ref="K6:N6"/>
     <mergeCell ref="G6:J6"/>
-    <mergeCell ref="G42:J42"/>
-    <mergeCell ref="K42:N42"/>
-    <mergeCell ref="O42:R42"/>
-    <mergeCell ref="S42:T42"/>
-    <mergeCell ref="U42:X42"/>
-    <mergeCell ref="G44:J44"/>
-    <mergeCell ref="K44:N44"/>
-    <mergeCell ref="O44:R44"/>
-    <mergeCell ref="S44:T44"/>
-    <mergeCell ref="U44:X44"/>
-    <mergeCell ref="G88:J88"/>
-    <mergeCell ref="K88:N88"/>
-    <mergeCell ref="O88:R88"/>
-    <mergeCell ref="S88:T88"/>
-    <mergeCell ref="U88:X88"/>
-    <mergeCell ref="G90:J90"/>
-    <mergeCell ref="K90:N90"/>
-    <mergeCell ref="O90:R90"/>
-    <mergeCell ref="S90:T90"/>
-    <mergeCell ref="U90:X90"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
@@ -35280,10 +35285,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CED359C-4B42-41C8-A7E8-4F6FC9AE57D2}">
-  <dimension ref="C2:W43"/>
+  <dimension ref="C2:X43"/>
   <sheetViews>
-    <sheetView topLeftCell="F5" workbookViewId="0">
-      <selection activeCell="U25" sqref="U25"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="S28" sqref="S28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -35305,7 +35310,7 @@
     <col min="36" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C2" s="200"/>
       <c r="D2" s="200"/>
       <c r="E2" s="200"/>
@@ -35319,7 +35324,7 @@
       <c r="M2" s="200"/>
       <c r="N2" s="200"/>
     </row>
-    <row r="3" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C3" s="200"/>
       <c r="D3" s="200"/>
       <c r="E3" s="200"/>
@@ -35335,7 +35340,7 @@
       <c r="M3" s="200"/>
       <c r="N3" s="200"/>
     </row>
-    <row r="4" spans="3:23" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:24" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C4" s="61" t="s">
         <v>38</v>
       </c>
@@ -35379,16 +35384,19 @@
         <v>91</v>
       </c>
       <c r="Q4" s="64" t="s">
+        <v>1063</v>
+      </c>
+      <c r="R4" s="64" t="s">
         <v>769</v>
       </c>
-      <c r="R4" s="64" t="s">
+      <c r="S4" s="64" t="s">
         <v>330</v>
       </c>
-      <c r="S4" s="64" t="s">
+      <c r="T4" s="64" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="5" spans="3:23" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="3:24" ht="38.25" x14ac:dyDescent="0.2">
       <c r="C5" s="63" t="s">
         <v>332</v>
       </c>
@@ -35408,29 +35416,30 @@
       <c r="I5" s="177"/>
       <c r="J5" s="177"/>
       <c r="K5" s="177"/>
-      <c r="L5" s="517" t="s">
+      <c r="L5" s="521" t="s">
         <v>339</v>
       </c>
-      <c r="M5" s="518"/>
-      <c r="N5" s="518"/>
-      <c r="O5" s="519"/>
+      <c r="M5" s="522"/>
+      <c r="N5" s="522"/>
+      <c r="O5" s="523"/>
       <c r="P5" s="107"/>
-      <c r="Q5" s="107" t="s">
+      <c r="Q5" s="107"/>
+      <c r="R5" s="107" t="s">
         <v>340</v>
       </c>
-      <c r="R5" s="107" t="s">
+      <c r="S5" s="107" t="s">
         <v>126</v>
       </c>
-      <c r="S5" s="107"/>
-      <c r="U5" s="107" t="s">
+      <c r="T5" s="107"/>
+      <c r="V5" s="107" t="s">
         <v>658</v>
       </c>
-      <c r="V5" s="107"/>
-      <c r="W5" s="107" t="s">
+      <c r="W5" s="107"/>
+      <c r="X5" s="107" t="s">
         <v>661</v>
       </c>
     </row>
-    <row r="6" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="6" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C6" s="84" t="s">
         <v>404</v>
       </c>
@@ -35444,35 +35453,36 @@
       <c r="I6" s="84"/>
       <c r="J6" s="84"/>
       <c r="K6" s="84"/>
-      <c r="L6" s="523" t="s">
+      <c r="L6" s="530" t="s">
         <v>1005</v>
       </c>
-      <c r="M6" s="525"/>
-      <c r="N6" s="525"/>
-      <c r="O6" s="524"/>
+      <c r="M6" s="532"/>
+      <c r="N6" s="532"/>
+      <c r="O6" s="531"/>
       <c r="P6" s="463" t="s">
         <v>1017</v>
       </c>
-      <c r="Q6" s="108" t="s">
+      <c r="Q6" s="108"/>
+      <c r="R6" s="108" t="s">
         <v>55</v>
       </c>
-      <c r="R6" s="117" t="s">
+      <c r="S6" s="117" t="s">
         <v>793</v>
       </c>
-      <c r="S6" s="108" t="s">
+      <c r="T6" s="108" t="s">
         <v>348</v>
       </c>
-      <c r="U6" s="108" t="s">
+      <c r="V6" s="108" t="s">
         <v>659</v>
       </c>
-      <c r="V6" s="117" t="s">
+      <c r="W6" s="117" t="s">
         <v>662</v>
       </c>
-      <c r="W6" s="108" t="s">
+      <c r="X6" s="108" t="s">
         <v>660</v>
       </c>
     </row>
-    <row r="7" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C7" s="207" t="str">
         <f>D20</f>
         <v>R-RSDRF_N1</v>
@@ -35503,42 +35513,43 @@
         <v>0.85</v>
       </c>
       <c r="L7" s="346">
-        <f t="shared" ref="L7:O13" si="0">L35/$V7/1000</f>
+        <f>L35/$W7/1000</f>
         <v>0.432</v>
       </c>
       <c r="M7" s="346">
-        <f t="shared" si="0"/>
+        <f>M35/$W7/1000</f>
         <v>0.432</v>
       </c>
       <c r="N7" s="346">
-        <f t="shared" si="0"/>
+        <f>N35/$W7/1000</f>
         <v>0.432</v>
       </c>
       <c r="O7" s="346">
-        <f t="shared" si="0"/>
+        <f>O35/$W7/1000</f>
         <v>0.432</v>
       </c>
       <c r="P7" s="212"/>
       <c r="Q7" s="212"/>
-      <c r="R7" s="352">
+      <c r="R7" s="212"/>
+      <c r="S7" s="352">
         <v>1</v>
       </c>
-      <c r="S7" s="212">
+      <c r="T7" s="212">
         <v>2020</v>
       </c>
-      <c r="U7" s="287">
+      <c r="V7" s="287">
         <v>0.18</v>
       </c>
-      <c r="V7" s="287">
-        <f>1/U7</f>
+      <c r="W7" s="287">
+        <f>1/V7</f>
         <v>5.5555555555555554</v>
       </c>
-      <c r="W7" s="287">
-        <f t="shared" ref="W7:W13" si="1">L35/V7</f>
+      <c r="X7" s="287">
+        <f>L35/W7</f>
         <v>432</v>
       </c>
     </row>
-    <row r="8" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C8" s="205" t="str">
         <f>D21</f>
         <v>R-RSDCK_ELC_N1</v>
@@ -35569,48 +35580,49 @@
         <v>0.8</v>
       </c>
       <c r="L8" s="347">
-        <f>$W$8/1000</f>
+        <f>$X$8/1000</f>
         <v>0.86975000000000002</v>
       </c>
       <c r="M8" s="347">
-        <f t="shared" ref="M8:O8" si="2">$W$8/1000</f>
+        <f>$X$8/1000</f>
         <v>0.86975000000000002</v>
       </c>
       <c r="N8" s="347">
-        <f t="shared" si="2"/>
+        <f>$X$8/1000</f>
         <v>0.86975000000000002</v>
       </c>
       <c r="O8" s="347">
-        <f t="shared" si="2"/>
+        <f>$X$8/1000</f>
         <v>0.86975000000000002</v>
       </c>
       <c r="P8" s="213"/>
       <c r="Q8" s="213"/>
-      <c r="R8" s="353">
+      <c r="R8" s="213"/>
+      <c r="S8" s="353">
         <v>1</v>
       </c>
-      <c r="S8" s="213">
+      <c r="T8" s="213">
         <v>2020</v>
       </c>
-      <c r="U8" s="287">
+      <c r="V8" s="287">
         <v>3</v>
       </c>
-      <c r="V8" s="287">
-        <f>1/U8</f>
+      <c r="W8" s="287">
+        <f>1/V8</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="W8" s="287">
-        <f>W9*1.42</f>
+      <c r="X8" s="287">
+        <f>X9*1.42</f>
         <v>869.75</v>
       </c>
     </row>
-    <row r="9" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C9" s="205" t="str">
-        <f t="shared" ref="C9:C10" si="3">D22</f>
+        <f t="shared" ref="C9:C10" si="0">D22</f>
         <v>R-RSDCK_GAS_N1</v>
       </c>
       <c r="D9" s="196" t="str">
-        <f t="shared" ref="D9:D10" si="4">LEFT($E$21,20)&amp;"_"&amp;RIGHT(E9,3)&amp;" - New"</f>
+        <f t="shared" ref="D9:D10" si="1">LEFT($E$21,20)&amp;"_"&amp;RIGHT(E9,3)&amp;" - New"</f>
         <v>Residential Cooking _GAS - New</v>
       </c>
       <c r="E9" s="196" t="s">
@@ -35635,48 +35647,51 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="L9" s="348">
-        <f>L37/$V9/1000</f>
+        <f>L37/$W9/1000</f>
         <v>0.61250000000000004</v>
       </c>
       <c r="M9" s="348">
+        <f>M37/$W9/1000</f>
+        <v>0.61250000000000004</v>
+      </c>
+      <c r="N9" s="348">
+        <f>N37/$W9/1000</f>
+        <v>0.61250000000000004</v>
+      </c>
+      <c r="O9" s="348">
+        <f>O37/$W9/1000</f>
+        <v>0.61250000000000004</v>
+      </c>
+      <c r="P9" s="214"/>
+      <c r="Q9" s="544">
+        <v>0.4</v>
+      </c>
+      <c r="R9" s="214"/>
+      <c r="S9" s="354">
+        <v>1</v>
+      </c>
+      <c r="T9" s="214">
+        <v>2020</v>
+      </c>
+      <c r="V9" s="287">
+        <v>3.5</v>
+      </c>
+      <c r="W9" s="287">
+        <f t="shared" ref="W9:W13" si="2">1/V9</f>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="X9" s="287">
+        <f>L37/W9</f>
+        <v>612.5</v>
+      </c>
+    </row>
+    <row r="10" spans="3:24" x14ac:dyDescent="0.2">
+      <c r="C10" s="205" t="str">
         <f t="shared" si="0"/>
-        <v>0.61250000000000004</v>
-      </c>
-      <c r="N9" s="348">
-        <f t="shared" si="0"/>
-        <v>0.61250000000000004</v>
-      </c>
-      <c r="O9" s="348">
-        <f t="shared" si="0"/>
-        <v>0.61250000000000004</v>
-      </c>
-      <c r="P9" s="214"/>
-      <c r="Q9" s="214"/>
-      <c r="R9" s="354">
-        <v>1</v>
-      </c>
-      <c r="S9" s="214">
-        <v>2020</v>
-      </c>
-      <c r="U9" s="287">
-        <v>3.5</v>
-      </c>
-      <c r="V9" s="287">
-        <f t="shared" ref="V9:V13" si="5">1/U9</f>
-        <v>0.2857142857142857</v>
-      </c>
-      <c r="W9" s="287">
-        <f>L37/V9</f>
-        <v>612.5</v>
-      </c>
-    </row>
-    <row r="10" spans="3:23" x14ac:dyDescent="0.2">
-      <c r="C10" s="205" t="str">
-        <f t="shared" si="3"/>
         <v>R-RSDCK_LPG_N1</v>
       </c>
       <c r="D10" s="195" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>Residential Cooking _LPG - New</v>
       </c>
       <c r="E10" s="195" t="s">
@@ -35701,48 +35716,51 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="L10" s="347">
-        <f>L38/$V10/1000</f>
+        <f>L38/$W10/1000</f>
         <v>0.61250000000000004</v>
       </c>
       <c r="M10" s="347">
-        <f t="shared" si="0"/>
+        <f>M38/$W10/1000</f>
         <v>0.61250000000000004</v>
       </c>
       <c r="N10" s="347">
-        <f t="shared" si="0"/>
+        <f>N38/$W10/1000</f>
         <v>0.61250000000000004</v>
       </c>
       <c r="O10" s="347">
-        <f t="shared" si="0"/>
+        <f>O38/$W10/1000</f>
         <v>0.61250000000000004</v>
       </c>
       <c r="P10" s="213"/>
-      <c r="Q10" s="213"/>
-      <c r="R10" s="353">
+      <c r="Q10" s="545">
+        <v>0.1</v>
+      </c>
+      <c r="R10" s="213"/>
+      <c r="S10" s="353">
         <v>1</v>
       </c>
-      <c r="S10" s="213">
+      <c r="T10" s="213">
         <v>2020</v>
       </c>
-      <c r="U10" s="287">
+      <c r="V10" s="287">
         <v>3.5</v>
       </c>
-      <c r="V10" s="287">
-        <f t="shared" si="5"/>
+      <c r="W10" s="287">
+        <f t="shared" si="2"/>
         <v>0.2857142857142857</v>
       </c>
-      <c r="W10" s="287">
-        <f t="shared" si="1"/>
+      <c r="X10" s="287">
+        <f>L38/W10</f>
         <v>612.5</v>
       </c>
     </row>
-    <row r="11" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="11" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C11" s="207" t="str">
-        <f t="shared" ref="C11:D15" si="6">D24</f>
+        <f t="shared" ref="C11:D15" si="3">D24</f>
         <v>R-RSDCW_N1</v>
       </c>
       <c r="D11" s="196" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>Residential Cloth Washing demand - New</v>
       </c>
       <c r="E11" s="196" t="s">
@@ -35767,48 +35785,49 @@
         <v>0.7</v>
       </c>
       <c r="L11" s="348">
-        <f t="shared" si="0"/>
+        <f>L39/$W11/1000</f>
         <v>0.55220000000000002</v>
       </c>
       <c r="M11" s="348">
-        <f t="shared" si="0"/>
+        <f>M39/$W11/1000</f>
         <v>0.55220000000000002</v>
       </c>
       <c r="N11" s="348">
-        <f t="shared" si="0"/>
+        <f>N39/$W11/1000</f>
         <v>0.55220000000000002</v>
       </c>
       <c r="O11" s="348">
-        <f t="shared" si="0"/>
+        <f>O39/$W11/1000</f>
         <v>0.55220000000000002</v>
       </c>
       <c r="P11" s="214"/>
       <c r="Q11" s="214"/>
-      <c r="R11" s="354">
+      <c r="R11" s="214"/>
+      <c r="S11" s="354">
         <v>1</v>
       </c>
-      <c r="S11" s="214">
+      <c r="T11" s="214">
         <v>2020</v>
       </c>
-      <c r="U11" s="287">
+      <c r="V11" s="287">
         <v>2.2000000000000002</v>
       </c>
-      <c r="V11" s="287">
-        <f t="shared" si="5"/>
+      <c r="W11" s="287">
+        <f t="shared" si="2"/>
         <v>0.45454545454545453</v>
       </c>
-      <c r="W11" s="287">
-        <f t="shared" si="1"/>
+      <c r="X11" s="287">
+        <f>L39/W11</f>
         <v>552.20000000000005</v>
       </c>
     </row>
-    <row r="12" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="12" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C12" s="205" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>R-RSDCD_N1</v>
       </c>
       <c r="D12" s="195" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>Residential Cloth Drying demand - New</v>
       </c>
       <c r="E12" s="195" t="s">
@@ -35833,48 +35852,49 @@
         <v>0.6</v>
       </c>
       <c r="L12" s="347">
-        <f t="shared" si="0"/>
+        <f>L40/$W12/1000</f>
         <v>0.53500000000000003</v>
       </c>
       <c r="M12" s="347">
-        <f t="shared" si="0"/>
+        <f>M40/$W12/1000</f>
         <v>0.53500000000000003</v>
       </c>
       <c r="N12" s="347">
-        <f t="shared" si="0"/>
+        <f>N40/$W12/1000</f>
         <v>0.53500000000000003</v>
       </c>
       <c r="O12" s="347">
-        <f t="shared" si="0"/>
+        <f>O40/$W12/1000</f>
         <v>0.53500000000000003</v>
       </c>
       <c r="P12" s="213"/>
       <c r="Q12" s="213"/>
-      <c r="R12" s="353">
+      <c r="R12" s="213"/>
+      <c r="S12" s="353">
         <v>1</v>
       </c>
-      <c r="S12" s="213">
+      <c r="T12" s="213">
         <v>2020</v>
       </c>
-      <c r="U12" s="287">
+      <c r="V12" s="287">
         <v>2.5</v>
       </c>
-      <c r="V12" s="287">
-        <f t="shared" si="5"/>
+      <c r="W12" s="287">
+        <f t="shared" si="2"/>
         <v>0.4</v>
       </c>
-      <c r="W12" s="287">
-        <f t="shared" si="1"/>
+      <c r="X12" s="287">
+        <f>L40/W12</f>
         <v>535</v>
       </c>
     </row>
-    <row r="13" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="13" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C13" s="207" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>R-RSDDW_N1</v>
       </c>
       <c r="D13" s="196" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>Residential Dish Washing demand - New</v>
       </c>
       <c r="E13" s="196" t="s">
@@ -35899,48 +35919,49 @@
         <v>0.7</v>
       </c>
       <c r="L13" s="348">
-        <f t="shared" si="0"/>
+        <f>L41/$W13/1000</f>
         <v>0.42019999999999996</v>
       </c>
       <c r="M13" s="348">
-        <f t="shared" si="0"/>
+        <f>M41/$W13/1000</f>
         <v>0.42019999999999996</v>
       </c>
       <c r="N13" s="348">
-        <f t="shared" si="0"/>
+        <f>N41/$W13/1000</f>
         <v>0.42019999999999996</v>
       </c>
       <c r="O13" s="348">
-        <f t="shared" si="0"/>
+        <f>O41/$W13/1000</f>
         <v>0.42019999999999996</v>
       </c>
       <c r="P13" s="214"/>
       <c r="Q13" s="214"/>
-      <c r="R13" s="354">
+      <c r="R13" s="214"/>
+      <c r="S13" s="354">
         <v>1</v>
       </c>
-      <c r="S13" s="214">
+      <c r="T13" s="214">
         <v>2020</v>
       </c>
-      <c r="U13" s="287">
+      <c r="V13" s="287">
         <v>2.2000000000000002</v>
       </c>
-      <c r="V13" s="287">
-        <f t="shared" si="5"/>
+      <c r="W13" s="287">
+        <f t="shared" si="2"/>
         <v>0.45454545454545453</v>
       </c>
-      <c r="W13" s="287">
-        <f t="shared" si="1"/>
+      <c r="X13" s="287">
+        <f>L41/W13</f>
         <v>420.2</v>
       </c>
     </row>
-    <row r="14" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="14" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C14" s="205" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>R-RSDOE_N1</v>
       </c>
       <c r="D14" s="195" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>Residential ELC Appliances - New</v>
       </c>
       <c r="E14" s="195" t="s">
@@ -35965,37 +35986,38 @@
         <v>0.85</v>
       </c>
       <c r="L14" s="356">
-        <f>L42/$V7/1000</f>
+        <f>L42/$W7/1000</f>
         <v>0.9</v>
       </c>
       <c r="M14" s="356">
-        <f>M42/$V7/1000</f>
+        <f>M42/$W7/1000</f>
         <v>0.9</v>
       </c>
       <c r="N14" s="356">
-        <f>N42/$V7/1000</f>
+        <f>N42/$W7/1000</f>
         <v>0.9</v>
       </c>
       <c r="O14" s="356">
-        <f>O42/$V7/1000</f>
+        <f>O42/$W7/1000</f>
         <v>0.9</v>
       </c>
       <c r="P14" s="213"/>
       <c r="Q14" s="213"/>
-      <c r="R14" s="353">
+      <c r="R14" s="213"/>
+      <c r="S14" s="353">
         <v>1</v>
       </c>
-      <c r="S14" s="213">
+      <c r="T14" s="213">
         <v>2020</v>
       </c>
     </row>
-    <row r="15" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="15" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C15" s="207" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>R-RSDOA_N1</v>
       </c>
       <c r="D15" s="196" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>Residential Other Applications - New</v>
       </c>
       <c r="E15" s="196" t="s">
@@ -36020,37 +36042,38 @@
         <v>0.85</v>
       </c>
       <c r="L15" s="357">
-        <f>L43/$V7/1000</f>
+        <f>L43/$W7/1000</f>
         <v>0.9</v>
       </c>
       <c r="M15" s="357">
-        <f>M43/$V7/1000</f>
+        <f>M43/$W7/1000</f>
         <v>0.9</v>
       </c>
       <c r="N15" s="357">
-        <f>N43/$V7/1000</f>
+        <f>N43/$W7/1000</f>
         <v>0.9</v>
       </c>
       <c r="O15" s="357">
-        <f>O43/$V7/1000</f>
+        <f>O43/$W7/1000</f>
         <v>0.9</v>
       </c>
       <c r="P15" s="215"/>
       <c r="Q15" s="215"/>
-      <c r="R15" s="355">
+      <c r="R15" s="215"/>
+      <c r="S15" s="355">
         <v>1</v>
       </c>
-      <c r="S15" s="215">
+      <c r="T15" s="215">
         <v>2020</v>
       </c>
-      <c r="U15" s="193" t="s">
+      <c r="V15" s="193" t="s">
         <v>655</v>
       </c>
-      <c r="V15" s="286" t="s">
+      <c r="W15" s="286" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="16" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="16" spans="3:24" x14ac:dyDescent="0.2">
       <c r="U16" s="193" t="s">
         <v>656</v>
       </c>
@@ -36062,10 +36085,10 @@
       <c r="C18" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="R18" s="529" t="s">
+      <c r="R18" s="533" t="s">
         <v>697</v>
       </c>
-      <c r="S18" s="529"/>
+      <c r="S18" s="533"/>
       <c r="U18" s="5" t="s">
         <v>898</v>
       </c>
@@ -36098,8 +36121,8 @@
       <c r="J19" s="199" t="s">
         <v>311</v>
       </c>
-      <c r="R19" s="529"/>
-      <c r="S19" s="529"/>
+      <c r="R19" s="533"/>
+      <c r="S19" s="533"/>
       <c r="V19" s="5" t="s">
         <v>1059</v>
       </c>
@@ -36125,8 +36148,8 @@
       <c r="J20" s="174" t="s">
         <v>445</v>
       </c>
-      <c r="R20" s="529"/>
-      <c r="S20" s="529"/>
+      <c r="R20" s="533"/>
+      <c r="S20" s="533"/>
       <c r="V20" s="5" t="s">
         <v>1060</v>
       </c>
@@ -36153,15 +36176,15 @@
       <c r="J21" s="174" t="s">
         <v>445</v>
       </c>
-      <c r="R21" s="529"/>
-      <c r="S21" s="529"/>
+      <c r="R21" s="533"/>
+      <c r="S21" s="533"/>
     </row>
     <row r="22" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C22" s="172" t="s">
         <v>48</v>
       </c>
       <c r="D22" s="173" t="str">
-        <f t="shared" ref="D22:D23" si="7">_xlfn.TEXTJOIN("_",TRUE,"R-RSDCK",RIGHT(E9,3),"N1")</f>
+        <f t="shared" ref="D22:D23" si="4">_xlfn.TEXTJOIN("_",TRUE,"R-RSDCK",RIGHT(E9,3),"N1")</f>
         <v>R-RSDCK_GAS_N1</v>
       </c>
       <c r="E22" s="173" t="s">
@@ -36178,15 +36201,15 @@
       <c r="J22" s="174" t="s">
         <v>445</v>
       </c>
-      <c r="R22" s="529"/>
-      <c r="S22" s="529"/>
+      <c r="R22" s="533"/>
+      <c r="S22" s="533"/>
     </row>
     <row r="23" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C23" s="172" t="s">
         <v>48</v>
       </c>
       <c r="D23" s="173" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>R-RSDCK_LPG_N1</v>
       </c>
       <c r="E23" s="173" t="s">
@@ -36269,6 +36292,7 @@
       <c r="J26" s="174" t="s">
         <v>445</v>
       </c>
+      <c r="Q26" s="193"/>
     </row>
     <row r="27" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C27" s="172" t="s">
@@ -36353,23 +36377,23 @@
       <c r="K33" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="L33" s="517" t="s">
+      <c r="L33" s="521" t="s">
         <v>339</v>
       </c>
-      <c r="M33" s="518"/>
-      <c r="N33" s="518"/>
-      <c r="O33" s="519"/>
+      <c r="M33" s="522"/>
+      <c r="N33" s="522"/>
+      <c r="O33" s="523"/>
     </row>
     <row r="34" spans="8:15" x14ac:dyDescent="0.2">
       <c r="H34" s="5" t="s">
         <v>404</v>
       </c>
-      <c r="L34" s="520" t="s">
+      <c r="L34" s="524" t="s">
         <v>345</v>
       </c>
-      <c r="M34" s="521"/>
-      <c r="N34" s="521"/>
-      <c r="O34" s="522"/>
+      <c r="M34" s="525"/>
+      <c r="N34" s="525"/>
+      <c r="O34" s="526"/>
     </row>
     <row r="35" spans="8:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H35" s="5" t="s">
@@ -36602,7 +36626,7 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="V15" r:id="rId1" xr:uid="{8872A4E8-1ED1-45C9-9AE2-8045F13A0849}"/>
+    <hyperlink ref="W15" r:id="rId1" xr:uid="{8872A4E8-1ED1-45C9-9AE2-8045F13A0849}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -36711,16 +36735,16 @@
       <c r="G4" s="177" t="s">
         <v>338</v>
       </c>
-      <c r="H4" s="526" t="s">
+      <c r="H4" s="527" t="s">
         <v>120</v>
       </c>
-      <c r="I4" s="527"/>
-      <c r="J4" s="528"/>
-      <c r="K4" s="517" t="s">
+      <c r="I4" s="528"/>
+      <c r="J4" s="529"/>
+      <c r="K4" s="521" t="s">
         <v>339</v>
       </c>
-      <c r="L4" s="518"/>
-      <c r="M4" s="519"/>
+      <c r="L4" s="522"/>
+      <c r="M4" s="523"/>
       <c r="N4" s="107"/>
       <c r="O4" s="107" t="s">
         <v>340</v>
@@ -36743,16 +36767,16 @@
       <c r="G5" s="471" t="s">
         <v>312</v>
       </c>
-      <c r="H5" s="531" t="s">
+      <c r="H5" s="535" t="s">
         <v>55</v>
       </c>
-      <c r="I5" s="532"/>
-      <c r="J5" s="533"/>
-      <c r="K5" s="531" t="s">
+      <c r="I5" s="536"/>
+      <c r="J5" s="537"/>
+      <c r="K5" s="535" t="s">
         <v>794</v>
       </c>
-      <c r="L5" s="532"/>
-      <c r="M5" s="533"/>
+      <c r="L5" s="536"/>
+      <c r="M5" s="537"/>
       <c r="N5" s="501" t="s">
         <v>346</v>
       </c>
@@ -36766,23 +36790,23 @@
         <v>348</v>
       </c>
       <c r="AA5" s="286"/>
-      <c r="AB5" s="535" t="s">
+      <c r="AB5" s="519" t="s">
         <v>1047</v>
       </c>
-      <c r="AC5" s="535"/>
+      <c r="AC5" s="519"/>
       <c r="AD5" s="474"/>
-      <c r="AE5" s="534" t="s">
+      <c r="AE5" s="518" t="s">
         <v>120</v>
       </c>
-      <c r="AF5" s="534"/>
-      <c r="AG5" s="534" t="s">
+      <c r="AF5" s="518"/>
+      <c r="AG5" s="518" t="s">
         <v>1056</v>
       </c>
-      <c r="AH5" s="534"/>
-      <c r="AI5" s="530" t="s">
+      <c r="AH5" s="518"/>
+      <c r="AI5" s="534" t="s">
         <v>1057</v>
       </c>
-      <c r="AJ5" s="530"/>
+      <c r="AJ5" s="534"/>
     </row>
     <row r="6" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C6" s="202" t="str">
@@ -37493,12 +37517,12 @@
       <c r="K27" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="L27" s="517" t="s">
+      <c r="L27" s="521" t="s">
         <v>339</v>
       </c>
-      <c r="M27" s="518"/>
-      <c r="N27" s="518"/>
-      <c r="O27" s="519"/>
+      <c r="M27" s="522"/>
+      <c r="N27" s="522"/>
+      <c r="O27" s="523"/>
       <c r="T27" s="288"/>
       <c r="U27" s="288"/>
     </row>
@@ -37506,12 +37530,12 @@
       <c r="J28" s="5" t="s">
         <v>404</v>
       </c>
-      <c r="L28" s="520" t="s">
+      <c r="L28" s="524" t="s">
         <v>345</v>
       </c>
-      <c r="M28" s="521"/>
-      <c r="N28" s="521"/>
-      <c r="O28" s="522"/>
+      <c r="M28" s="525"/>
+      <c r="N28" s="525"/>
+      <c r="O28" s="526"/>
       <c r="T28" s="288"/>
       <c r="U28" s="288"/>
     </row>
@@ -38905,16 +38929,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="AI5:AJ5"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="H5:J5"/>
     <mergeCell ref="L27:O27"/>
     <mergeCell ref="L28:O28"/>
     <mergeCell ref="AG5:AH5"/>
     <mergeCell ref="AB5:AC5"/>
     <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="AI5:AJ5"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="H5:J5"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
@@ -47944,128 +47968,128 @@
       <c r="C4" s="369" t="s">
         <v>803</v>
       </c>
-      <c r="D4" s="537" t="s">
+      <c r="D4" s="538" t="s">
         <v>804</v>
       </c>
-      <c r="E4" s="536"/>
-      <c r="F4" s="536"/>
-      <c r="G4" s="536"/>
-      <c r="H4" s="538"/>
-      <c r="I4" s="536" t="s">
+      <c r="E4" s="539"/>
+      <c r="F4" s="539"/>
+      <c r="G4" s="539"/>
+      <c r="H4" s="540"/>
+      <c r="I4" s="539" t="s">
         <v>805</v>
       </c>
-      <c r="J4" s="536"/>
-      <c r="K4" s="536"/>
-      <c r="L4" s="536"/>
-      <c r="M4" s="538"/>
-      <c r="N4" s="536" t="s">
+      <c r="J4" s="539"/>
+      <c r="K4" s="539"/>
+      <c r="L4" s="539"/>
+      <c r="M4" s="540"/>
+      <c r="N4" s="539" t="s">
         <v>806</v>
       </c>
-      <c r="O4" s="536"/>
-      <c r="P4" s="536"/>
-      <c r="Q4" s="536"/>
-      <c r="R4" s="538"/>
-      <c r="S4" s="536" t="s">
+      <c r="O4" s="539"/>
+      <c r="P4" s="539"/>
+      <c r="Q4" s="539"/>
+      <c r="R4" s="540"/>
+      <c r="S4" s="539" t="s">
         <v>807</v>
       </c>
-      <c r="T4" s="536"/>
-      <c r="U4" s="536"/>
-      <c r="V4" s="536"/>
-      <c r="W4" s="538"/>
-      <c r="X4" s="536" t="s">
+      <c r="T4" s="539"/>
+      <c r="U4" s="539"/>
+      <c r="V4" s="539"/>
+      <c r="W4" s="540"/>
+      <c r="X4" s="539" t="s">
         <v>808</v>
       </c>
-      <c r="Y4" s="536"/>
-      <c r="Z4" s="536"/>
-      <c r="AA4" s="536"/>
-      <c r="AB4" s="538"/>
-      <c r="AC4" s="536" t="s">
+      <c r="Y4" s="539"/>
+      <c r="Z4" s="539"/>
+      <c r="AA4" s="539"/>
+      <c r="AB4" s="540"/>
+      <c r="AC4" s="539" t="s">
         <v>809</v>
       </c>
-      <c r="AD4" s="536"/>
-      <c r="AE4" s="536"/>
-      <c r="AF4" s="536"/>
-      <c r="AG4" s="538"/>
-      <c r="AH4" s="536" t="s">
+      <c r="AD4" s="539"/>
+      <c r="AE4" s="539"/>
+      <c r="AF4" s="539"/>
+      <c r="AG4" s="540"/>
+      <c r="AH4" s="539" t="s">
         <v>810</v>
       </c>
-      <c r="AI4" s="536"/>
-      <c r="AJ4" s="536"/>
-      <c r="AK4" s="536"/>
-      <c r="AL4" s="538"/>
-      <c r="AM4" s="536" t="s">
+      <c r="AI4" s="539"/>
+      <c r="AJ4" s="539"/>
+      <c r="AK4" s="539"/>
+      <c r="AL4" s="540"/>
+      <c r="AM4" s="539" t="s">
         <v>811</v>
       </c>
-      <c r="AN4" s="536"/>
-      <c r="AO4" s="536"/>
-      <c r="AP4" s="536"/>
-      <c r="AQ4" s="538"/>
-      <c r="AR4" s="536" t="s">
+      <c r="AN4" s="539"/>
+      <c r="AO4" s="539"/>
+      <c r="AP4" s="539"/>
+      <c r="AQ4" s="540"/>
+      <c r="AR4" s="539" t="s">
         <v>812</v>
       </c>
-      <c r="AS4" s="536"/>
-      <c r="AT4" s="536"/>
-      <c r="AU4" s="536"/>
-      <c r="AV4" s="538"/>
-      <c r="AW4" s="536" t="s">
+      <c r="AS4" s="539"/>
+      <c r="AT4" s="539"/>
+      <c r="AU4" s="539"/>
+      <c r="AV4" s="540"/>
+      <c r="AW4" s="539" t="s">
         <v>813</v>
       </c>
-      <c r="AX4" s="536"/>
-      <c r="AY4" s="536"/>
-      <c r="AZ4" s="536"/>
-      <c r="BA4" s="536"/>
-      <c r="BB4" s="537" t="s">
+      <c r="AX4" s="539"/>
+      <c r="AY4" s="539"/>
+      <c r="AZ4" s="539"/>
+      <c r="BA4" s="539"/>
+      <c r="BB4" s="538" t="s">
         <v>814</v>
       </c>
-      <c r="BC4" s="536"/>
-      <c r="BD4" s="536"/>
-      <c r="BE4" s="536"/>
-      <c r="BF4" s="538"/>
-      <c r="BG4" s="536" t="s">
+      <c r="BC4" s="539"/>
+      <c r="BD4" s="539"/>
+      <c r="BE4" s="539"/>
+      <c r="BF4" s="540"/>
+      <c r="BG4" s="539" t="s">
         <v>815</v>
       </c>
-      <c r="BH4" s="536"/>
-      <c r="BI4" s="536"/>
-      <c r="BJ4" s="536"/>
-      <c r="BK4" s="536"/>
-      <c r="BL4" s="537" t="s">
+      <c r="BH4" s="539"/>
+      <c r="BI4" s="539"/>
+      <c r="BJ4" s="539"/>
+      <c r="BK4" s="539"/>
+      <c r="BL4" s="538" t="s">
         <v>816</v>
       </c>
-      <c r="BM4" s="536"/>
-      <c r="BN4" s="536"/>
-      <c r="BO4" s="536"/>
-      <c r="BP4" s="536"/>
-      <c r="BQ4" s="537" t="s">
+      <c r="BM4" s="539"/>
+      <c r="BN4" s="539"/>
+      <c r="BO4" s="539"/>
+      <c r="BP4" s="539"/>
+      <c r="BQ4" s="538" t="s">
         <v>817</v>
       </c>
-      <c r="BR4" s="536"/>
-      <c r="BS4" s="536"/>
-      <c r="BT4" s="536"/>
-      <c r="BU4" s="538"/>
+      <c r="BR4" s="539"/>
+      <c r="BS4" s="539"/>
+      <c r="BT4" s="539"/>
+      <c r="BU4" s="540"/>
       <c r="BV4" s="370" t="s">
         <v>818</v>
       </c>
-      <c r="BW4" s="539" t="s">
+      <c r="BW4" s="541" t="s">
         <v>819</v>
       </c>
-      <c r="BX4" s="540"/>
-      <c r="BY4" s="540"/>
-      <c r="BZ4" s="540"/>
-      <c r="CA4" s="541"/>
-      <c r="CB4" s="539" t="s">
+      <c r="BX4" s="542"/>
+      <c r="BY4" s="542"/>
+      <c r="BZ4" s="542"/>
+      <c r="CA4" s="543"/>
+      <c r="CB4" s="541" t="s">
         <v>820</v>
       </c>
-      <c r="CC4" s="540"/>
-      <c r="CD4" s="540"/>
-      <c r="CE4" s="540"/>
-      <c r="CF4" s="541"/>
-      <c r="CG4" s="539" t="s">
+      <c r="CC4" s="542"/>
+      <c r="CD4" s="542"/>
+      <c r="CE4" s="542"/>
+      <c r="CF4" s="543"/>
+      <c r="CG4" s="541" t="s">
         <v>821</v>
       </c>
-      <c r="CH4" s="540"/>
-      <c r="CI4" s="540"/>
-      <c r="CJ4" s="540"/>
-      <c r="CK4" s="541"/>
+      <c r="CH4" s="542"/>
+      <c r="CI4" s="542"/>
+      <c r="CJ4" s="542"/>
+      <c r="CK4" s="543"/>
     </row>
     <row r="5" spans="1:89" x14ac:dyDescent="0.2">
       <c r="A5" s="372"/>
@@ -61634,11 +61658,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="BL4:BP4"/>
-    <mergeCell ref="BQ4:BU4"/>
-    <mergeCell ref="BW4:CA4"/>
-    <mergeCell ref="CB4:CF4"/>
-    <mergeCell ref="CG4:CK4"/>
     <mergeCell ref="BG4:BK4"/>
     <mergeCell ref="D4:H4"/>
     <mergeCell ref="I4:M4"/>
@@ -61651,6 +61670,11 @@
     <mergeCell ref="AR4:AV4"/>
     <mergeCell ref="AW4:BA4"/>
     <mergeCell ref="BB4:BF4"/>
+    <mergeCell ref="BL4:BP4"/>
+    <mergeCell ref="BQ4:BU4"/>
+    <mergeCell ref="BW4:CA4"/>
+    <mergeCell ref="CB4:CF4"/>
+    <mergeCell ref="CG4:CK4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
Remove FLO_SHAR from techs with single commodity IN and OUT
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_RSD.xlsx
+++ b/SubRES_TMPL/SubRes_RSD.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF779A2B-16A0-4A34-A452-61931095BDEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E06D0FB1-9FBC-4361-9D5D-9896CA13D760}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{34F9D92C-266F-476D-89E0-63153305AC39}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="5" xr2:uid="{34F9D92C-266F-476D-89E0-63153305AC39}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="34" r:id="rId1"/>
@@ -781,7 +781,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="Z8" authorId="0" shapeId="0" xr:uid="{4CC7BAE4-B77F-4446-B919-7188CC25F5B2}">
+    <comment ref="W8" authorId="0" shapeId="0" xr:uid="{4CC7BAE4-B77F-4446-B919-7188CC25F5B2}">
       <text>
         <r>
           <rPr>
@@ -830,7 +830,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U15" authorId="0" shapeId="0" xr:uid="{6AD7F003-C0BD-4A39-A684-1B5072D780D3}">
+    <comment ref="R15" authorId="0" shapeId="0" xr:uid="{6AD7F003-C0BD-4A39-A684-1B5072D780D3}">
       <text>
         <r>
           <rPr>
@@ -854,7 +854,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L35" authorId="0" shapeId="0" xr:uid="{B2CBE2A3-43A2-4EFE-8157-00F31233ABB8}">
+    <comment ref="L36" authorId="0" shapeId="0" xr:uid="{B2CBE2A3-43A2-4EFE-8157-00F31233ABB8}">
       <text>
         <r>
           <rPr>
@@ -8611,7 +8611,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3433" uniqueCount="1036">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3430" uniqueCount="1033">
   <si>
     <t>Document type:</t>
   </si>
@@ -11722,15 +11722,6 @@
   </si>
   <si>
     <t>Theoretical limit for a white LED</t>
-  </si>
-  <si>
-    <t>FLO_SHAR~UP~2018</t>
-  </si>
-  <si>
-    <t>FLO_SHAR~UP~2070</t>
-  </si>
-  <si>
-    <t>FLO_SHAR~UP~0</t>
   </si>
   <si>
     <t>https://www.ransomspares.co.uk/blog/news/gas-cooker-vs-electric-cooker.htm#:~:text=According%20to%20Which%2C%20it%20costs,it%20works%20out%20more%20expensive.</t>
@@ -13348,7 +13339,7 @@
     <xf numFmtId="0" fontId="39" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="54" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="542">
+  <cellXfs count="541">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -14292,12 +14283,44 @@
     <xf numFmtId="0" fontId="16" fillId="23" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="40" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="40" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="40" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="40" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="40" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="40" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="40" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="40" fillId="21" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="40" fillId="21" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="40" fillId="21" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="40" fillId="21" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="40" fillId="21" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="15" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="40" fillId="0" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="40" fillId="0" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="40" fillId="0" borderId="69" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="40" fillId="0" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="40" fillId="0" borderId="69" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="40" fillId="21" borderId="70" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="40" fillId="21" borderId="70" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="40" fillId="21" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="40" fillId="21" borderId="72" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="40" fillId="21" borderId="70" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="40" fillId="21" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="40" fillId="21" borderId="72" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="173" fontId="44" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -14340,15 +14363,6 @@
     <xf numFmtId="0" fontId="53" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="23" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -14356,6 +14370,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -14367,22 +14390,40 @@
     <xf numFmtId="0" fontId="16" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="60" fillId="31" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="69" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="60" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="31" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="60" fillId="31" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -14397,64 +14438,9 @@
     <xf numFmtId="0" fontId="60" fillId="32" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="69" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="40" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="40" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="40" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="40" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="40" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="40" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="40" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="40" fillId="21" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="40" fillId="21" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="40" fillId="21" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="40" fillId="21" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="40" fillId="21" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="15" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="40" fillId="0" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="40" fillId="0" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="40" fillId="0" borderId="69" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="40" fillId="0" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="40" fillId="0" borderId="69" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="40" fillId="21" borderId="70" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="40" fillId="21" borderId="70" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="40" fillId="21" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="40" fillId="21" borderId="72" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="40" fillId="21" borderId="70" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="40" fillId="21" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="40" fillId="21" borderId="72" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="44" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="40" fillId="21" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="40" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="20% - Colore 2" xfId="11" xr:uid="{3E3DAF22-4D86-48A9-B6EE-8D230C1E993C}"/>
@@ -14474,14 +14460,7 @@
     <cellStyle name="Normal 4 2" xfId="9" xr:uid="{87BDABB2-3FF4-448F-8C91-A21FFDA39A5E}"/>
     <cellStyle name="Percent" xfId="15" builtinId="5"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="44"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -14499,7 +14478,7 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="1" xr9:uid="{6466AE88-DD34-414A-9E08-915E3C7C4193}">
-      <tableStyleElement type="firstRowStripe" dxfId="2"/>
+      <tableStyleElement type="firstRowStripe" dxfId="1"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -16178,14 +16157,14 @@
       <c r="F16" s="211"/>
     </row>
     <row r="17" spans="1:14" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="470" t="s">
+      <c r="A17" s="500" t="s">
         <v>439</v>
       </c>
-      <c r="B17" s="470"/>
-      <c r="C17" s="470"/>
-      <c r="D17" s="470"/>
-      <c r="E17" s="470"/>
-      <c r="F17" s="470"/>
+      <c r="B17" s="500"/>
+      <c r="C17" s="500"/>
+      <c r="D17" s="500"/>
+      <c r="E17" s="500"/>
+      <c r="F17" s="500"/>
       <c r="G17" s="213"/>
       <c r="H17" s="213"/>
       <c r="I17" s="214"/>
@@ -16223,13 +16202,13 @@
       <c r="A20" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="471" t="s">
+      <c r="B20" s="501" t="s">
         <v>441</v>
       </c>
-      <c r="C20" s="471"/>
-      <c r="D20" s="471"/>
-      <c r="E20" s="471"/>
-      <c r="F20" s="471"/>
+      <c r="C20" s="501"/>
+      <c r="D20" s="501"/>
+      <c r="E20" s="501"/>
+      <c r="F20" s="501"/>
       <c r="G20" s="218"/>
       <c r="H20" s="218"/>
       <c r="I20" s="219"/>
@@ -16243,13 +16222,13 @@
       <c r="A21" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="472" t="s">
+      <c r="B21" s="502" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="472"/>
-      <c r="D21" s="472"/>
-      <c r="E21" s="472"/>
-      <c r="F21" s="472"/>
+      <c r="C21" s="502"/>
+      <c r="D21" s="502"/>
+      <c r="E21" s="502"/>
+      <c r="F21" s="502"/>
       <c r="G21" s="218"/>
       <c r="H21" s="218"/>
       <c r="I21" s="219"/>
@@ -16263,13 +16242,13 @@
       <c r="A22" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="472" t="s">
+      <c r="B22" s="502" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="472"/>
-      <c r="D22" s="472"/>
-      <c r="E22" s="472"/>
-      <c r="F22" s="472"/>
+      <c r="C22" s="502"/>
+      <c r="D22" s="502"/>
+      <c r="E22" s="502"/>
+      <c r="F22" s="502"/>
     </row>
     <row r="23" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
@@ -16298,22 +16277,22 @@
       <c r="H24" s="3"/>
     </row>
     <row r="25" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="473"/>
-      <c r="B25" s="473"/>
-      <c r="C25" s="473"/>
-      <c r="D25" s="473"/>
-      <c r="E25" s="473"/>
-      <c r="F25" s="473"/>
+      <c r="A25" s="503"/>
+      <c r="B25" s="503"/>
+      <c r="C25" s="503"/>
+      <c r="D25" s="503"/>
+      <c r="E25" s="503"/>
+      <c r="F25" s="503"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
     </row>
     <row r="26" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="469"/>
-      <c r="B26" s="469"/>
-      <c r="C26" s="469"/>
-      <c r="D26" s="469"/>
-      <c r="E26" s="469"/>
-      <c r="F26" s="469"/>
+      <c r="A26" s="499"/>
+      <c r="B26" s="499"/>
+      <c r="C26" s="499"/>
+      <c r="D26" s="499"/>
+      <c r="E26" s="499"/>
+      <c r="F26" s="499"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="211"/>
@@ -16500,16 +16479,16 @@
   <sheetData>
     <row r="1" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:20" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="474" t="s">
+      <c r="B2" s="504" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="475"/>
-      <c r="D2" s="475"/>
-      <c r="E2" s="476"/>
-      <c r="G2" s="474" t="s">
+      <c r="C2" s="505"/>
+      <c r="D2" s="505"/>
+      <c r="E2" s="506"/>
+      <c r="G2" s="504" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="476"/>
+      <c r="H2" s="506"/>
       <c r="I2" s="222"/>
       <c r="J2" s="222"/>
       <c r="K2" s="223"/>
@@ -16851,16 +16830,16 @@
     </row>
     <row r="19" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="2:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="477" t="s">
+      <c r="B20" s="507" t="s">
         <v>70</v>
       </c>
-      <c r="C20" s="478"/>
-      <c r="D20" s="478"/>
-      <c r="E20" s="479"/>
-      <c r="G20" s="474" t="s">
+      <c r="C20" s="508"/>
+      <c r="D20" s="508"/>
+      <c r="E20" s="509"/>
+      <c r="G20" s="504" t="s">
         <v>14</v>
       </c>
-      <c r="H20" s="476"/>
+      <c r="H20" s="506"/>
     </row>
     <row r="21" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="250" t="s">
@@ -17104,16 +17083,16 @@
     </row>
     <row r="37" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="38" spans="2:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="474" t="s">
+      <c r="B38" s="504" t="s">
         <v>78</v>
       </c>
-      <c r="C38" s="475"/>
-      <c r="D38" s="475"/>
-      <c r="E38" s="476"/>
-      <c r="G38" s="480" t="s">
+      <c r="C38" s="505"/>
+      <c r="D38" s="505"/>
+      <c r="E38" s="506"/>
+      <c r="G38" s="510" t="s">
         <v>72</v>
       </c>
-      <c r="H38" s="481"/>
+      <c r="H38" s="511"/>
     </row>
     <row r="39" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B39" s="271" t="s">
@@ -17218,7 +17197,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4660B878-9B9C-4131-8EFF-29EF25ED69C5}">
   <dimension ref="A2:AM103"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
@@ -17282,13 +17261,13 @@
       <c r="M3" s="5" t="s">
         <v>391</v>
       </c>
-      <c r="S3" s="482" t="s">
+      <c r="S3" s="512" t="s">
         <v>687</v>
       </c>
-      <c r="T3" s="482"/>
-      <c r="U3" s="482"/>
-      <c r="V3" s="482"/>
-      <c r="W3" s="482"/>
+      <c r="T3" s="512"/>
+      <c r="U3" s="512"/>
+      <c r="V3" s="512"/>
+      <c r="W3" s="512"/>
     </row>
     <row r="4" spans="3:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C4" s="62" t="s">
@@ -24966,8 +24945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{104F8057-C735-4662-BAA6-EEDCF7B57273}">
   <dimension ref="A2:AO162"/>
   <sheetViews>
-    <sheetView topLeftCell="Q91" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J143" sqref="J143"/>
+    <sheetView topLeftCell="B9" zoomScale="64" zoomScaleNormal="110" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <selection activeCell="V41" sqref="V41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -25122,34 +25101,34 @@
       <c r="F4" s="62" t="s">
         <v>317</v>
       </c>
-      <c r="G4" s="489" t="s">
+      <c r="G4" s="519" t="s">
         <v>727</v>
       </c>
-      <c r="H4" s="490"/>
-      <c r="I4" s="490"/>
-      <c r="J4" s="491"/>
-      <c r="K4" s="489" t="s">
+      <c r="H4" s="520"/>
+      <c r="I4" s="520"/>
+      <c r="J4" s="521"/>
+      <c r="K4" s="519" t="s">
         <v>319</v>
       </c>
-      <c r="L4" s="490"/>
-      <c r="M4" s="490"/>
-      <c r="N4" s="491"/>
-      <c r="O4" s="489" t="s">
+      <c r="L4" s="520"/>
+      <c r="M4" s="520"/>
+      <c r="N4" s="521"/>
+      <c r="O4" s="519" t="s">
         <v>320</v>
       </c>
-      <c r="P4" s="490"/>
-      <c r="Q4" s="490"/>
-      <c r="R4" s="491"/>
-      <c r="S4" s="489" t="s">
+      <c r="P4" s="520"/>
+      <c r="Q4" s="520"/>
+      <c r="R4" s="521"/>
+      <c r="S4" s="519" t="s">
         <v>321</v>
       </c>
-      <c r="T4" s="491"/>
-      <c r="U4" s="483" t="s">
+      <c r="T4" s="521"/>
+      <c r="U4" s="522" t="s">
         <v>322</v>
       </c>
-      <c r="V4" s="484"/>
-      <c r="W4" s="484"/>
-      <c r="X4" s="485"/>
+      <c r="V4" s="523"/>
+      <c r="W4" s="523"/>
+      <c r="X4" s="524"/>
       <c r="Y4" s="106"/>
       <c r="Z4" s="106"/>
       <c r="AA4" s="114" t="s">
@@ -25244,34 +25223,34 @@
       <c r="D6" s="84"/>
       <c r="E6" s="84"/>
       <c r="F6" s="85"/>
-      <c r="G6" s="486" t="s">
+      <c r="G6" s="513" t="s">
         <v>45</v>
       </c>
-      <c r="H6" s="487"/>
-      <c r="I6" s="487"/>
-      <c r="J6" s="488"/>
-      <c r="K6" s="487" t="s">
+      <c r="H6" s="514"/>
+      <c r="I6" s="514"/>
+      <c r="J6" s="515"/>
+      <c r="K6" s="514" t="s">
         <v>45</v>
       </c>
-      <c r="L6" s="487"/>
-      <c r="M6" s="487"/>
-      <c r="N6" s="488"/>
-      <c r="O6" s="486" t="s">
+      <c r="L6" s="514"/>
+      <c r="M6" s="514"/>
+      <c r="N6" s="515"/>
+      <c r="O6" s="513" t="s">
         <v>45</v>
       </c>
-      <c r="P6" s="487"/>
-      <c r="Q6" s="487"/>
-      <c r="R6" s="488"/>
-      <c r="S6" s="486" t="s">
+      <c r="P6" s="514"/>
+      <c r="Q6" s="514"/>
+      <c r="R6" s="515"/>
+      <c r="S6" s="513" t="s">
         <v>302</v>
       </c>
-      <c r="T6" s="488"/>
-      <c r="U6" s="486" t="s">
+      <c r="T6" s="515"/>
+      <c r="U6" s="513" t="s">
         <v>976</v>
       </c>
-      <c r="V6" s="487"/>
-      <c r="W6" s="487"/>
-      <c r="X6" s="488"/>
+      <c r="V6" s="514"/>
+      <c r="W6" s="514"/>
+      <c r="X6" s="515"/>
       <c r="Y6" s="107" t="s">
         <v>988</v>
       </c>
@@ -28002,34 +27981,34 @@
       <c r="F42" s="62" t="s">
         <v>317</v>
       </c>
-      <c r="G42" s="489" t="s">
+      <c r="G42" s="519" t="s">
         <v>318</v>
       </c>
-      <c r="H42" s="490"/>
-      <c r="I42" s="490"/>
-      <c r="J42" s="491"/>
-      <c r="K42" s="489" t="s">
+      <c r="H42" s="520"/>
+      <c r="I42" s="520"/>
+      <c r="J42" s="521"/>
+      <c r="K42" s="519" t="s">
         <v>319</v>
       </c>
-      <c r="L42" s="490"/>
-      <c r="M42" s="490"/>
-      <c r="N42" s="491"/>
-      <c r="O42" s="489" t="s">
+      <c r="L42" s="520"/>
+      <c r="M42" s="520"/>
+      <c r="N42" s="521"/>
+      <c r="O42" s="519" t="s">
         <v>320</v>
       </c>
-      <c r="P42" s="490"/>
-      <c r="Q42" s="490"/>
-      <c r="R42" s="491"/>
-      <c r="S42" s="489" t="s">
+      <c r="P42" s="520"/>
+      <c r="Q42" s="520"/>
+      <c r="R42" s="521"/>
+      <c r="S42" s="519" t="s">
         <v>321</v>
       </c>
-      <c r="T42" s="491"/>
-      <c r="U42" s="483" t="s">
+      <c r="T42" s="521"/>
+      <c r="U42" s="522" t="s">
         <v>322</v>
       </c>
-      <c r="V42" s="484"/>
-      <c r="W42" s="484"/>
-      <c r="X42" s="485"/>
+      <c r="V42" s="523"/>
+      <c r="W42" s="523"/>
+      <c r="X42" s="524"/>
       <c r="Y42" s="106"/>
       <c r="Z42" s="106"/>
       <c r="AA42" s="114" t="s">
@@ -28124,34 +28103,34 @@
       <c r="D44" s="84"/>
       <c r="E44" s="84"/>
       <c r="F44" s="85"/>
-      <c r="G44" s="486" t="s">
+      <c r="G44" s="513" t="s">
         <v>45</v>
       </c>
-      <c r="H44" s="487"/>
-      <c r="I44" s="487"/>
-      <c r="J44" s="488"/>
-      <c r="K44" s="487" t="s">
+      <c r="H44" s="514"/>
+      <c r="I44" s="514"/>
+      <c r="J44" s="515"/>
+      <c r="K44" s="514" t="s">
         <v>45</v>
       </c>
-      <c r="L44" s="487"/>
-      <c r="M44" s="487"/>
-      <c r="N44" s="488"/>
-      <c r="O44" s="486" t="s">
+      <c r="L44" s="514"/>
+      <c r="M44" s="514"/>
+      <c r="N44" s="515"/>
+      <c r="O44" s="513" t="s">
         <v>45</v>
       </c>
-      <c r="P44" s="487"/>
-      <c r="Q44" s="487"/>
-      <c r="R44" s="488"/>
-      <c r="S44" s="492" t="s">
+      <c r="P44" s="514"/>
+      <c r="Q44" s="514"/>
+      <c r="R44" s="515"/>
+      <c r="S44" s="516" t="s">
         <v>302</v>
       </c>
-      <c r="T44" s="493"/>
-      <c r="U44" s="492" t="s">
+      <c r="T44" s="517"/>
+      <c r="U44" s="516" t="s">
         <v>976</v>
       </c>
-      <c r="V44" s="494"/>
-      <c r="W44" s="494"/>
-      <c r="X44" s="493"/>
+      <c r="V44" s="518"/>
+      <c r="W44" s="518"/>
+      <c r="X44" s="517"/>
       <c r="Y44" s="458" t="s">
         <v>988</v>
       </c>
@@ -31522,34 +31501,34 @@
       <c r="F88" s="62" t="s">
         <v>317</v>
       </c>
-      <c r="G88" s="489" t="s">
+      <c r="G88" s="519" t="s">
         <v>318</v>
       </c>
-      <c r="H88" s="490"/>
-      <c r="I88" s="490"/>
-      <c r="J88" s="491"/>
-      <c r="K88" s="489" t="s">
+      <c r="H88" s="520"/>
+      <c r="I88" s="520"/>
+      <c r="J88" s="521"/>
+      <c r="K88" s="519" t="s">
         <v>319</v>
       </c>
-      <c r="L88" s="490"/>
-      <c r="M88" s="490"/>
-      <c r="N88" s="491"/>
-      <c r="O88" s="489" t="s">
+      <c r="L88" s="520"/>
+      <c r="M88" s="520"/>
+      <c r="N88" s="521"/>
+      <c r="O88" s="519" t="s">
         <v>320</v>
       </c>
-      <c r="P88" s="490"/>
-      <c r="Q88" s="490"/>
-      <c r="R88" s="491"/>
-      <c r="S88" s="489" t="s">
+      <c r="P88" s="520"/>
+      <c r="Q88" s="520"/>
+      <c r="R88" s="521"/>
+      <c r="S88" s="519" t="s">
         <v>321</v>
       </c>
-      <c r="T88" s="491"/>
-      <c r="U88" s="483" t="s">
+      <c r="T88" s="521"/>
+      <c r="U88" s="522" t="s">
         <v>322</v>
       </c>
-      <c r="V88" s="484"/>
-      <c r="W88" s="484"/>
-      <c r="X88" s="485"/>
+      <c r="V88" s="523"/>
+      <c r="W88" s="523"/>
+      <c r="X88" s="524"/>
       <c r="Y88" s="106"/>
       <c r="Z88" s="106"/>
       <c r="AA88" s="114" t="s">
@@ -31644,34 +31623,34 @@
       <c r="D90" s="84"/>
       <c r="E90" s="84"/>
       <c r="F90" s="85"/>
-      <c r="G90" s="486" t="s">
+      <c r="G90" s="513" t="s">
         <v>45</v>
       </c>
-      <c r="H90" s="487"/>
-      <c r="I90" s="487"/>
-      <c r="J90" s="488"/>
-      <c r="K90" s="487" t="s">
+      <c r="H90" s="514"/>
+      <c r="I90" s="514"/>
+      <c r="J90" s="515"/>
+      <c r="K90" s="514" t="s">
         <v>45</v>
       </c>
-      <c r="L90" s="487"/>
-      <c r="M90" s="487"/>
-      <c r="N90" s="488"/>
-      <c r="O90" s="486" t="s">
+      <c r="L90" s="514"/>
+      <c r="M90" s="514"/>
+      <c r="N90" s="515"/>
+      <c r="O90" s="513" t="s">
         <v>45</v>
       </c>
-      <c r="P90" s="487"/>
-      <c r="Q90" s="487"/>
-      <c r="R90" s="488"/>
-      <c r="S90" s="492" t="s">
+      <c r="P90" s="514"/>
+      <c r="Q90" s="514"/>
+      <c r="R90" s="515"/>
+      <c r="S90" s="516" t="s">
         <v>302</v>
       </c>
-      <c r="T90" s="493"/>
-      <c r="U90" s="492" t="s">
+      <c r="T90" s="517"/>
+      <c r="U90" s="516" t="s">
         <v>976</v>
       </c>
-      <c r="V90" s="494"/>
-      <c r="W90" s="494"/>
-      <c r="X90" s="493"/>
+      <c r="V90" s="518"/>
+      <c r="W90" s="518"/>
+      <c r="X90" s="517"/>
       <c r="Y90" s="458" t="s">
         <v>988</v>
       </c>
@@ -35202,26 +35181,6 @@
     <row r="162" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="G90:J90"/>
-    <mergeCell ref="K90:N90"/>
-    <mergeCell ref="O90:R90"/>
-    <mergeCell ref="S90:T90"/>
-    <mergeCell ref="U90:X90"/>
-    <mergeCell ref="G88:J88"/>
-    <mergeCell ref="K88:N88"/>
-    <mergeCell ref="O88:R88"/>
-    <mergeCell ref="S88:T88"/>
-    <mergeCell ref="U88:X88"/>
-    <mergeCell ref="G44:J44"/>
-    <mergeCell ref="K44:N44"/>
-    <mergeCell ref="O44:R44"/>
-    <mergeCell ref="S44:T44"/>
-    <mergeCell ref="U44:X44"/>
-    <mergeCell ref="G42:J42"/>
-    <mergeCell ref="K42:N42"/>
-    <mergeCell ref="O42:R42"/>
-    <mergeCell ref="S42:T42"/>
-    <mergeCell ref="U42:X42"/>
     <mergeCell ref="U4:X4"/>
     <mergeCell ref="U6:X6"/>
     <mergeCell ref="G4:J4"/>
@@ -35232,6 +35191,26 @@
     <mergeCell ref="O6:R6"/>
     <mergeCell ref="K6:N6"/>
     <mergeCell ref="G6:J6"/>
+    <mergeCell ref="G42:J42"/>
+    <mergeCell ref="K42:N42"/>
+    <mergeCell ref="O42:R42"/>
+    <mergeCell ref="S42:T42"/>
+    <mergeCell ref="U42:X42"/>
+    <mergeCell ref="G44:J44"/>
+    <mergeCell ref="K44:N44"/>
+    <mergeCell ref="O44:R44"/>
+    <mergeCell ref="S44:T44"/>
+    <mergeCell ref="U44:X44"/>
+    <mergeCell ref="G88:J88"/>
+    <mergeCell ref="K88:N88"/>
+    <mergeCell ref="O88:R88"/>
+    <mergeCell ref="S88:T88"/>
+    <mergeCell ref="U88:X88"/>
+    <mergeCell ref="G90:J90"/>
+    <mergeCell ref="K90:N90"/>
+    <mergeCell ref="O90:R90"/>
+    <mergeCell ref="S90:T90"/>
+    <mergeCell ref="U90:X90"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
@@ -35246,10 +35225,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CED359C-4B42-41C8-A7E8-4F6FC9AE57D2}">
-  <dimension ref="C2:Z43"/>
+  <dimension ref="C2:Y44"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="O25" sqref="O25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S25" sqref="S25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -35273,37 +35252,37 @@
     <col min="36" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:26" x14ac:dyDescent="0.2">
-      <c r="C2" s="511"/>
-      <c r="D2" s="511"/>
-      <c r="E2" s="511"/>
-      <c r="F2" s="511"/>
-      <c r="G2" s="511"/>
-      <c r="H2" s="511"/>
-      <c r="I2" s="511"/>
-      <c r="J2" s="511"/>
-      <c r="K2" s="511"/>
-      <c r="L2" s="511"/>
-      <c r="M2" s="511"/>
-      <c r="N2" s="511"/>
-    </row>
-    <row r="3" spans="3:26" x14ac:dyDescent="0.2">
-      <c r="C3" s="511"/>
-      <c r="D3" s="511"/>
-      <c r="E3" s="511"/>
+    <row r="2" spans="3:25" x14ac:dyDescent="0.2">
+      <c r="C2" s="470"/>
+      <c r="D2" s="470"/>
+      <c r="E2" s="470"/>
+      <c r="F2" s="470"/>
+      <c r="G2" s="470"/>
+      <c r="H2" s="470"/>
+      <c r="I2" s="470"/>
+      <c r="J2" s="470"/>
+      <c r="K2" s="470"/>
+      <c r="L2" s="470"/>
+      <c r="M2" s="470"/>
+      <c r="N2" s="470"/>
+    </row>
+    <row r="3" spans="3:25" x14ac:dyDescent="0.2">
+      <c r="C3" s="470"/>
+      <c r="D3" s="470"/>
+      <c r="E3" s="470"/>
       <c r="F3" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="511"/>
-      <c r="H3" s="511"/>
-      <c r="I3" s="511"/>
-      <c r="J3" s="511"/>
-      <c r="K3" s="511"/>
-      <c r="L3" s="511"/>
-      <c r="M3" s="511"/>
-      <c r="N3" s="511"/>
-    </row>
-    <row r="4" spans="3:26" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G3" s="470"/>
+      <c r="H3" s="470"/>
+      <c r="I3" s="470"/>
+      <c r="J3" s="470"/>
+      <c r="K3" s="470"/>
+      <c r="L3" s="470"/>
+      <c r="M3" s="470"/>
+      <c r="N3" s="470"/>
+    </row>
+    <row r="4" spans="3:25" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C4" s="60" t="s">
         <v>28</v>
       </c>
@@ -35344,28 +35323,19 @@
         <v>326</v>
       </c>
       <c r="P4" s="63" t="s">
-        <v>1030</v>
+        <v>81</v>
       </c>
       <c r="Q4" s="63" t="s">
-        <v>1031</v>
+        <v>740</v>
       </c>
       <c r="R4" s="63" t="s">
-        <v>1032</v>
+        <v>313</v>
       </c>
       <c r="S4" s="63" t="s">
-        <v>81</v>
-      </c>
-      <c r="T4" s="63" t="s">
-        <v>740</v>
-      </c>
-      <c r="U4" s="63" t="s">
-        <v>313</v>
-      </c>
-      <c r="V4" s="63" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="5" spans="3:26" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="3:25" ht="38.25" x14ac:dyDescent="0.2">
       <c r="C5" s="62" t="s">
         <v>315</v>
       </c>
@@ -35385,32 +35355,29 @@
       <c r="I5" s="173"/>
       <c r="J5" s="173"/>
       <c r="K5" s="173"/>
-      <c r="L5" s="483" t="s">
+      <c r="L5" s="522" t="s">
         <v>322</v>
       </c>
-      <c r="M5" s="484"/>
-      <c r="N5" s="484"/>
-      <c r="O5" s="485"/>
-      <c r="P5" s="468"/>
-      <c r="Q5" s="468"/>
-      <c r="R5" s="468"/>
+      <c r="M5" s="523"/>
+      <c r="N5" s="523"/>
+      <c r="O5" s="524"/>
+      <c r="P5" s="106"/>
+      <c r="Q5" s="106" t="s">
+        <v>323</v>
+      </c>
+      <c r="R5" s="106" t="s">
+        <v>116</v>
+      </c>
       <c r="S5" s="106"/>
-      <c r="T5" s="106" t="s">
-        <v>323</v>
-      </c>
       <c r="U5" s="106" t="s">
-        <v>116</v>
+        <v>630</v>
       </c>
       <c r="V5" s="106"/>
-      <c r="X5" s="106" t="s">
-        <v>630</v>
-      </c>
-      <c r="Y5" s="106"/>
-      <c r="Z5" s="106" t="s">
+      <c r="W5" s="106" t="s">
         <v>633</v>
       </c>
     </row>
-    <row r="6" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="6" spans="3:25" x14ac:dyDescent="0.2">
       <c r="C6" s="83" t="s">
         <v>376</v>
       </c>
@@ -35424,44 +35391,41 @@
       <c r="I6" s="83"/>
       <c r="J6" s="83"/>
       <c r="K6" s="83"/>
-      <c r="L6" s="492" t="s">
+      <c r="L6" s="516" t="s">
         <v>976</v>
       </c>
-      <c r="M6" s="494"/>
-      <c r="N6" s="494"/>
-      <c r="O6" s="493"/>
-      <c r="P6" s="467"/>
-      <c r="Q6" s="467"/>
-      <c r="R6" s="467"/>
-      <c r="S6" s="458" t="s">
+      <c r="M6" s="518"/>
+      <c r="N6" s="518"/>
+      <c r="O6" s="517"/>
+      <c r="P6" s="458" t="s">
         <v>988</v>
       </c>
-      <c r="T6" s="107" t="s">
+      <c r="Q6" s="107" t="s">
         <v>45</v>
       </c>
-      <c r="U6" s="116" t="s">
+      <c r="R6" s="116" t="s">
         <v>764</v>
       </c>
-      <c r="V6" s="107" t="s">
+      <c r="S6" s="107" t="s">
         <v>331</v>
       </c>
-      <c r="X6" s="107" t="s">
+      <c r="U6" s="107" t="s">
         <v>631</v>
       </c>
-      <c r="Y6" s="116" t="s">
+      <c r="V6" s="116" t="s">
         <v>634</v>
       </c>
-      <c r="Z6" s="107" t="s">
+      <c r="W6" s="107" t="s">
         <v>632</v>
       </c>
     </row>
-    <row r="7" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:25" x14ac:dyDescent="0.2">
       <c r="C7" s="202" t="str">
-        <f>D20</f>
+        <f>D21</f>
         <v>R-RSDRF_N1</v>
       </c>
       <c r="D7" s="192" t="str">
-        <f>E20</f>
+        <f>E21</f>
         <v>Residential Refrigeration - New</v>
       </c>
       <c r="E7" s="192" t="s">
@@ -35486,51 +35450,48 @@
         <v>0.85</v>
       </c>
       <c r="L7" s="341">
-        <f>L35/$Y7/1000</f>
+        <f>L36/$V7/1000</f>
         <v>0.432</v>
       </c>
       <c r="M7" s="341">
-        <f>M35/$Y7/1000</f>
+        <f>M36/$V7/1000</f>
         <v>0.432</v>
       </c>
       <c r="N7" s="341">
-        <f>N35/$Y7/1000</f>
+        <f>N36/$V7/1000</f>
         <v>0.432</v>
       </c>
       <c r="O7" s="341">
-        <f>O35/$Y7/1000</f>
+        <f>O36/$V7/1000</f>
         <v>0.432</v>
       </c>
-      <c r="P7" s="341"/>
-      <c r="Q7" s="341"/>
-      <c r="R7" s="341"/>
-      <c r="S7" s="207"/>
-      <c r="T7" s="207"/>
-      <c r="U7" s="347">
+      <c r="P7" s="207"/>
+      <c r="Q7" s="207"/>
+      <c r="R7" s="347">
         <v>1</v>
       </c>
-      <c r="V7" s="207">
+      <c r="S7" s="207">
         <v>2020</v>
       </c>
-      <c r="X7" s="282">
+      <c r="U7" s="282">
         <v>0.18</v>
       </c>
-      <c r="Y7" s="282">
-        <f>1/X7</f>
+      <c r="V7" s="282">
+        <f>1/U7</f>
         <v>5.5555555555555554</v>
       </c>
-      <c r="Z7" s="282">
-        <f>L35/Y7</f>
+      <c r="W7" s="282">
+        <f>L36/V7</f>
         <v>432</v>
       </c>
     </row>
-    <row r="8" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="8" spans="3:25" x14ac:dyDescent="0.2">
       <c r="C8" s="200" t="str">
-        <f>D21</f>
+        <f>D22</f>
         <v>R-RSDCK_ELC_N1</v>
       </c>
       <c r="D8" s="191" t="str">
-        <f>LEFT($E$21,20)&amp;"_"&amp;RIGHT(E8,3)&amp;" - New"</f>
+        <f>LEFT($E$22,20)&amp;"_"&amp;RIGHT(E8,3)&amp;" - New"</f>
         <v>Residential Cooking _ELC - New</v>
       </c>
       <c r="E8" s="191" t="s">
@@ -35555,55 +35516,48 @@
         <v>0.85</v>
       </c>
       <c r="L8" s="342">
-        <f>$Z$8/1000</f>
+        <f>$W$8/1000</f>
         <v>0.86975000000000002</v>
       </c>
       <c r="M8" s="342">
-        <f>$Z$8/1000</f>
+        <f>$W$8/1000</f>
         <v>0.86975000000000002</v>
       </c>
       <c r="N8" s="342">
-        <f>$Z$8/1000</f>
+        <f>$W$8/1000</f>
         <v>0.86975000000000002</v>
       </c>
       <c r="O8" s="342">
-        <f>$Z$8/1000</f>
+        <f>$W$8/1000</f>
         <v>0.86975000000000002</v>
       </c>
-      <c r="P8" s="342"/>
-      <c r="Q8" s="342">
+      <c r="P8" s="208"/>
+      <c r="Q8" s="208"/>
+      <c r="R8" s="348">
         <v>1</v>
       </c>
-      <c r="R8" s="540">
-        <v>5</v>
-      </c>
-      <c r="S8" s="208"/>
-      <c r="T8" s="208"/>
-      <c r="U8" s="348">
-        <v>1</v>
-      </c>
-      <c r="V8" s="208">
+      <c r="S8" s="208">
         <v>2020</v>
       </c>
-      <c r="X8" s="282">
+      <c r="U8" s="282">
         <v>3</v>
       </c>
-      <c r="Y8" s="282">
-        <f>1/X8</f>
+      <c r="V8" s="282">
+        <f>1/U8</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="Z8" s="282">
-        <f>Z9*1.42</f>
+      <c r="W8" s="282">
+        <f>W9*1.42</f>
         <v>869.75</v>
       </c>
     </row>
-    <row r="9" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="9" spans="3:25" x14ac:dyDescent="0.2">
       <c r="C9" s="200" t="str">
-        <f t="shared" ref="C9:D15" si="0">D22</f>
+        <f t="shared" ref="C9:D15" si="0">D23</f>
         <v>R-RSDCK_GAS_N1</v>
       </c>
       <c r="D9" s="192" t="str">
-        <f t="shared" ref="D9:D10" si="1">LEFT($E$21,20)&amp;"_"&amp;RIGHT(E9,3)&amp;" - New"</f>
+        <f>LEFT($E$22,20)&amp;"_"&amp;RIGHT(E9,3)&amp;" - New"</f>
         <v>Residential Cooking _GAS - New</v>
       </c>
       <c r="E9" s="192" t="s">
@@ -35628,57 +35582,48 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="L9" s="343">
-        <f t="shared" ref="L9:O13" si="2">L37/$Y9/1000</f>
+        <f>L38/$V9/1000</f>
         <v>0.61250000000000004</v>
       </c>
       <c r="M9" s="343">
-        <f t="shared" si="2"/>
+        <f>M38/$V9/1000</f>
         <v>0.61250000000000004</v>
       </c>
       <c r="N9" s="343">
-        <f t="shared" si="2"/>
+        <f>N38/$V9/1000</f>
         <v>0.61250000000000004</v>
       </c>
       <c r="O9" s="343">
-        <f t="shared" si="2"/>
+        <f>O38/$V9/1000</f>
         <v>0.61250000000000004</v>
       </c>
-      <c r="P9" s="343">
-        <v>0.23</v>
-      </c>
-      <c r="Q9" s="343">
-        <v>0.4</v>
-      </c>
-      <c r="R9" s="541">
-        <v>5</v>
-      </c>
-      <c r="S9" s="209"/>
-      <c r="T9" s="209"/>
-      <c r="U9" s="349">
+      <c r="P9" s="209"/>
+      <c r="Q9" s="209"/>
+      <c r="R9" s="349">
         <v>1</v>
       </c>
-      <c r="V9" s="209">
+      <c r="S9" s="209">
         <v>2020</v>
       </c>
-      <c r="X9" s="282">
+      <c r="U9" s="282">
         <v>3.5</v>
       </c>
-      <c r="Y9" s="282">
-        <f t="shared" ref="Y9:Y13" si="3">1/X9</f>
+      <c r="V9" s="282">
+        <f t="shared" ref="V9:V13" si="1">1/U9</f>
         <v>0.2857142857142857</v>
       </c>
-      <c r="Z9" s="282">
-        <f>L37/Y9</f>
+      <c r="W9" s="282">
+        <f>L38/V9</f>
         <v>612.5</v>
       </c>
     </row>
-    <row r="10" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="10" spans="3:25" x14ac:dyDescent="0.2">
       <c r="C10" s="200" t="str">
         <f t="shared" si="0"/>
         <v>R-RSDCK_LPG_N1</v>
       </c>
       <c r="D10" s="191" t="str">
-        <f t="shared" si="1"/>
+        <f>LEFT($E$22,20)&amp;"_"&amp;RIGHT(E10,3)&amp;" - New"</f>
         <v>Residential Cooking _LPG - New</v>
       </c>
       <c r="E10" s="191" t="s">
@@ -35703,51 +35648,42 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="L10" s="342">
-        <f t="shared" si="2"/>
+        <f>L39/$V10/1000</f>
         <v>0.61250000000000004</v>
       </c>
       <c r="M10" s="342">
-        <f t="shared" si="2"/>
+        <f>M39/$V10/1000</f>
         <v>0.61250000000000004</v>
       </c>
       <c r="N10" s="342">
-        <f t="shared" si="2"/>
+        <f>N39/$V10/1000</f>
         <v>0.61250000000000004</v>
       </c>
       <c r="O10" s="342">
-        <f t="shared" si="2"/>
+        <f>O39/$V10/1000</f>
         <v>0.61250000000000004</v>
       </c>
-      <c r="P10" s="342">
-        <v>1.4E-2</v>
-      </c>
-      <c r="Q10" s="342">
-        <v>0.4</v>
-      </c>
-      <c r="R10" s="540">
-        <v>5</v>
-      </c>
-      <c r="S10" s="208"/>
-      <c r="T10" s="208"/>
-      <c r="U10" s="348">
+      <c r="P10" s="208"/>
+      <c r="Q10" s="208"/>
+      <c r="R10" s="348">
         <v>1</v>
       </c>
-      <c r="V10" s="208">
+      <c r="S10" s="208">
         <v>2020</v>
       </c>
-      <c r="X10" s="282">
+      <c r="U10" s="282">
         <v>3.5</v>
       </c>
-      <c r="Y10" s="282">
-        <f t="shared" si="3"/>
+      <c r="V10" s="282">
+        <f t="shared" si="1"/>
         <v>0.2857142857142857</v>
       </c>
-      <c r="Z10" s="282">
-        <f>L38/Y10</f>
+      <c r="W10" s="282">
+        <f>L39/V10</f>
         <v>612.5</v>
       </c>
     </row>
-    <row r="11" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="11" spans="3:25" x14ac:dyDescent="0.2">
       <c r="C11" s="202" t="str">
         <f t="shared" si="0"/>
         <v>R-RSDCW_N1</v>
@@ -35778,45 +35714,42 @@
         <v>0.7</v>
       </c>
       <c r="L11" s="343">
-        <f t="shared" si="2"/>
+        <f>L40/$V11/1000</f>
         <v>0.55220000000000002</v>
       </c>
       <c r="M11" s="343">
-        <f t="shared" si="2"/>
+        <f>M40/$V11/1000</f>
         <v>0.55220000000000002</v>
       </c>
       <c r="N11" s="343">
-        <f t="shared" si="2"/>
+        <f>N40/$V11/1000</f>
         <v>0.55220000000000002</v>
       </c>
       <c r="O11" s="343">
-        <f t="shared" si="2"/>
+        <f>O40/$V11/1000</f>
         <v>0.55220000000000002</v>
       </c>
-      <c r="P11" s="343"/>
-      <c r="Q11" s="343"/>
-      <c r="R11" s="343"/>
-      <c r="S11" s="209"/>
-      <c r="T11" s="209"/>
-      <c r="U11" s="349">
+      <c r="P11" s="209"/>
+      <c r="Q11" s="209"/>
+      <c r="R11" s="349">
         <v>1</v>
       </c>
-      <c r="V11" s="209">
+      <c r="S11" s="209">
         <v>2020</v>
       </c>
-      <c r="X11" s="282">
+      <c r="U11" s="282">
         <v>2.2000000000000002</v>
       </c>
-      <c r="Y11" s="282">
-        <f t="shared" si="3"/>
+      <c r="V11" s="282">
+        <f t="shared" si="1"/>
         <v>0.45454545454545453</v>
       </c>
-      <c r="Z11" s="282">
-        <f>L39/Y11</f>
+      <c r="W11" s="282">
+        <f>L40/V11</f>
         <v>552.20000000000005</v>
       </c>
     </row>
-    <row r="12" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="12" spans="3:25" x14ac:dyDescent="0.2">
       <c r="C12" s="200" t="str">
         <f t="shared" si="0"/>
         <v>R-RSDCD_N1</v>
@@ -35847,45 +35780,42 @@
         <v>0.6</v>
       </c>
       <c r="L12" s="342">
-        <f t="shared" si="2"/>
+        <f>L41/$V12/1000</f>
         <v>0.53500000000000003</v>
       </c>
       <c r="M12" s="342">
-        <f t="shared" si="2"/>
+        <f>M41/$V12/1000</f>
         <v>0.53500000000000003</v>
       </c>
       <c r="N12" s="342">
-        <f t="shared" si="2"/>
+        <f>N41/$V12/1000</f>
         <v>0.53500000000000003</v>
       </c>
       <c r="O12" s="342">
-        <f t="shared" si="2"/>
+        <f>O41/$V12/1000</f>
         <v>0.53500000000000003</v>
       </c>
-      <c r="P12" s="342"/>
-      <c r="Q12" s="342"/>
-      <c r="R12" s="342"/>
-      <c r="S12" s="208"/>
-      <c r="T12" s="208"/>
-      <c r="U12" s="348">
+      <c r="P12" s="208"/>
+      <c r="Q12" s="208"/>
+      <c r="R12" s="348">
         <v>1</v>
       </c>
-      <c r="V12" s="208">
+      <c r="S12" s="208">
         <v>2020</v>
       </c>
-      <c r="X12" s="282">
+      <c r="U12" s="282">
         <v>2.5</v>
       </c>
-      <c r="Y12" s="282">
-        <f t="shared" si="3"/>
+      <c r="V12" s="282">
+        <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
-      <c r="Z12" s="282">
-        <f>L40/Y12</f>
+      <c r="W12" s="282">
+        <f>L41/V12</f>
         <v>535</v>
       </c>
     </row>
-    <row r="13" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="13" spans="3:25" x14ac:dyDescent="0.2">
       <c r="C13" s="202" t="str">
         <f t="shared" si="0"/>
         <v>R-RSDDW_N1</v>
@@ -35916,45 +35846,42 @@
         <v>0.7</v>
       </c>
       <c r="L13" s="343">
-        <f t="shared" si="2"/>
+        <f>L42/$V13/1000</f>
         <v>0.42019999999999996</v>
       </c>
       <c r="M13" s="343">
-        <f t="shared" si="2"/>
+        <f>M42/$V13/1000</f>
         <v>0.42019999999999996</v>
       </c>
       <c r="N13" s="343">
-        <f t="shared" si="2"/>
+        <f>N42/$V13/1000</f>
         <v>0.42019999999999996</v>
       </c>
       <c r="O13" s="343">
-        <f t="shared" si="2"/>
+        <f>O42/$V13/1000</f>
         <v>0.42019999999999996</v>
       </c>
-      <c r="P13" s="343"/>
-      <c r="Q13" s="343"/>
-      <c r="R13" s="343"/>
-      <c r="S13" s="209"/>
-      <c r="T13" s="209"/>
-      <c r="U13" s="349">
+      <c r="P13" s="209"/>
+      <c r="Q13" s="209"/>
+      <c r="R13" s="349">
         <v>1</v>
       </c>
-      <c r="V13" s="209">
+      <c r="S13" s="209">
         <v>2020</v>
       </c>
-      <c r="X13" s="282">
+      <c r="U13" s="282">
         <v>2.2000000000000002</v>
       </c>
-      <c r="Y13" s="282">
-        <f t="shared" si="3"/>
+      <c r="V13" s="282">
+        <f t="shared" si="1"/>
         <v>0.45454545454545453</v>
       </c>
-      <c r="Z13" s="282">
-        <f>L41/Y13</f>
+      <c r="W13" s="282">
+        <f>L42/V13</f>
         <v>420.2</v>
       </c>
     </row>
-    <row r="14" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="14" spans="3:25" x14ac:dyDescent="0.2">
       <c r="C14" s="200" t="str">
         <f t="shared" si="0"/>
         <v>R-RSDOE_N1</v>
@@ -35985,34 +35912,31 @@
         <v>0.85</v>
       </c>
       <c r="L14" s="351">
-        <f>L42/$Y7/1000</f>
+        <f>L43/$V7/1000</f>
         <v>0.9</v>
       </c>
       <c r="M14" s="351">
-        <f>M42/$Y7/1000</f>
+        <f>M43/$V7/1000</f>
         <v>0.9</v>
       </c>
       <c r="N14" s="351">
-        <f>N42/$Y7/1000</f>
+        <f>N43/$V7/1000</f>
         <v>0.9</v>
       </c>
       <c r="O14" s="351">
-        <f>O42/$Y7/1000</f>
+        <f>O43/$V7/1000</f>
         <v>0.9</v>
       </c>
-      <c r="P14" s="351"/>
-      <c r="Q14" s="351"/>
-      <c r="R14" s="351"/>
-      <c r="S14" s="208"/>
-      <c r="T14" s="208"/>
-      <c r="U14" s="348">
+      <c r="P14" s="208"/>
+      <c r="Q14" s="208"/>
+      <c r="R14" s="348">
         <v>1</v>
       </c>
-      <c r="V14" s="208">
+      <c r="S14" s="208">
         <v>2020</v>
       </c>
     </row>
-    <row r="15" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="15" spans="3:25" x14ac:dyDescent="0.2">
       <c r="C15" s="202" t="str">
         <f t="shared" si="0"/>
         <v>R-RSDOA_N1</v>
@@ -36043,130 +35967,123 @@
         <v>0.85</v>
       </c>
       <c r="L15" s="352">
-        <f>L43/$Y7/1000</f>
+        <f>L44/$V7/1000</f>
         <v>0.9</v>
       </c>
       <c r="M15" s="352">
-        <f>M43/$Y7/1000</f>
+        <f>M44/$V7/1000</f>
         <v>0.9</v>
       </c>
       <c r="N15" s="352">
-        <f>N43/$Y7/1000</f>
+        <f>N44/$V7/1000</f>
         <v>0.9</v>
       </c>
       <c r="O15" s="352">
-        <f>O43/$Y7/1000</f>
+        <f>O44/$V7/1000</f>
         <v>0.9</v>
       </c>
-      <c r="P15" s="352"/>
-      <c r="Q15" s="352"/>
-      <c r="R15" s="352"/>
-      <c r="S15" s="210"/>
-      <c r="T15" s="210"/>
-      <c r="U15" s="350">
+      <c r="P15" s="210"/>
+      <c r="Q15" s="210"/>
+      <c r="R15" s="350">
         <v>1</v>
       </c>
-      <c r="V15" s="210">
+      <c r="S15" s="210">
         <v>2020</v>
       </c>
-      <c r="X15" s="189" t="s">
+      <c r="U15" s="189" t="s">
         <v>627</v>
       </c>
-      <c r="Y15" s="281" t="s">
+      <c r="V15" s="281" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="16" spans="3:26" x14ac:dyDescent="0.2">
-      <c r="R16" s="189" t="s">
+    <row r="16" spans="3:25" x14ac:dyDescent="0.2">
+      <c r="C16" s="538"/>
+      <c r="D16" s="538"/>
+      <c r="E16" s="538"/>
+      <c r="F16" s="538"/>
+      <c r="G16" s="538"/>
+      <c r="H16" s="538"/>
+      <c r="I16" s="538"/>
+      <c r="J16" s="538"/>
+      <c r="K16" s="538"/>
+      <c r="L16" s="539"/>
+      <c r="M16" s="539"/>
+      <c r="N16" s="539"/>
+      <c r="O16" s="539"/>
+      <c r="P16" s="539"/>
+      <c r="Q16" s="539"/>
+      <c r="R16" s="539"/>
+      <c r="S16" s="538"/>
+      <c r="T16" s="538"/>
+      <c r="U16" s="540"/>
+      <c r="V16" s="538"/>
+      <c r="X16" s="189"/>
+      <c r="Y16" s="281"/>
+    </row>
+    <row r="17" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="R17" s="189" t="s">
         <v>628</v>
       </c>
-      <c r="S16" s="5" t="s">
+      <c r="S17" s="5" t="s">
         <v>629</v>
       </c>
     </row>
-    <row r="18" spans="3:22" x14ac:dyDescent="0.2">
-      <c r="C18" s="5" t="s">
+    <row r="19" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="C19" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="R18" s="495" t="s">
+      <c r="R19" s="525" t="s">
         <v>669</v>
       </c>
-      <c r="S18" s="495"/>
-      <c r="U18" s="5" t="s">
+      <c r="S19" s="525"/>
+      <c r="U19" s="5" t="s">
         <v>869</v>
       </c>
-      <c r="V18" s="5" t="s">
-        <v>1033</v>
-      </c>
-    </row>
-    <row r="19" spans="3:22" x14ac:dyDescent="0.2">
-      <c r="C19" s="193" t="s">
+      <c r="V19" s="5" t="s">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="20" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="C20" s="193" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="194" t="s">
+      <c r="D20" s="194" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="194" t="s">
+      <c r="E20" s="194" t="s">
         <v>29</v>
       </c>
-      <c r="F19" s="194" t="s">
+      <c r="F20" s="194" t="s">
         <v>35</v>
       </c>
-      <c r="G19" s="194" t="s">
+      <c r="G20" s="194" t="s">
         <v>36</v>
       </c>
-      <c r="H19" s="194" t="s">
+      <c r="H20" s="194" t="s">
         <v>379</v>
       </c>
-      <c r="I19" s="194" t="s">
+      <c r="I20" s="194" t="s">
         <v>37</v>
       </c>
-      <c r="J19" s="195" t="s">
+      <c r="J20" s="195" t="s">
         <v>301</v>
       </c>
-      <c r="R19" s="495"/>
-      <c r="S19" s="495"/>
-      <c r="V19" s="5" t="s">
-        <v>1034</v>
-      </c>
-    </row>
-    <row r="20" spans="3:22" x14ac:dyDescent="0.2">
-      <c r="C20" s="168" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="169" t="s">
-        <v>757</v>
-      </c>
-      <c r="E20" s="169" t="s">
-        <v>416</v>
-      </c>
-      <c r="F20" s="169" t="s">
-        <v>16</v>
-      </c>
-      <c r="G20" s="169" t="s">
-        <v>363</v>
-      </c>
-      <c r="H20" s="169"/>
-      <c r="I20" s="169"/>
-      <c r="J20" s="170" t="s">
-        <v>417</v>
-      </c>
-      <c r="R20" s="495"/>
-      <c r="S20" s="495"/>
+      <c r="R20" s="525"/>
+      <c r="S20" s="525"/>
       <c r="V20" s="5" t="s">
-        <v>1035</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="21" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C21" s="168" t="s">
         <v>38</v>
       </c>
-      <c r="D21" s="169" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"R-RSDCK",RIGHT(E8,3),"N1")</f>
-        <v>R-RSDCK_ELC_N1</v>
+      <c r="D21" s="169" t="s">
+        <v>757</v>
       </c>
       <c r="E21" s="169" t="s">
-        <v>1001</v>
+        <v>416</v>
       </c>
       <c r="F21" s="169" t="s">
         <v>16</v>
@@ -36179,19 +36096,22 @@
       <c r="J21" s="170" t="s">
         <v>417</v>
       </c>
-      <c r="R21" s="495"/>
-      <c r="S21" s="495"/>
+      <c r="R21" s="525"/>
+      <c r="S21" s="525"/>
+      <c r="V21" s="5" t="s">
+        <v>1032</v>
+      </c>
     </row>
     <row r="22" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C22" s="168" t="s">
         <v>38</v>
       </c>
       <c r="D22" s="169" t="str">
-        <f t="shared" ref="D22:D23" si="4">_xlfn.TEXTJOIN("_",TRUE,"R-RSDCK",RIGHT(E9,3),"N1")</f>
-        <v>R-RSDCK_GAS_N1</v>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"R-RSDCK",RIGHT(E8,3),"N1")</f>
+        <v>R-RSDCK_ELC_N1</v>
       </c>
       <c r="E22" s="169" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="F22" s="169" t="s">
         <v>16</v>
@@ -36204,19 +36124,19 @@
       <c r="J22" s="170" t="s">
         <v>417</v>
       </c>
-      <c r="R22" s="495"/>
-      <c r="S22" s="495"/>
+      <c r="R22" s="525"/>
+      <c r="S22" s="525"/>
     </row>
     <row r="23" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C23" s="168" t="s">
         <v>38</v>
       </c>
       <c r="D23" s="169" t="str">
-        <f t="shared" si="4"/>
-        <v>R-RSDCK_LPG_N1</v>
+        <f t="shared" ref="D23:D24" si="2">_xlfn.TEXTJOIN("_",TRUE,"R-RSDCK",RIGHT(E9,3),"N1")</f>
+        <v>R-RSDCK_GAS_N1</v>
       </c>
       <c r="E23" s="169" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="F23" s="169" t="s">
         <v>16</v>
@@ -36229,16 +36149,19 @@
       <c r="J23" s="170" t="s">
         <v>417</v>
       </c>
+      <c r="R23" s="525"/>
+      <c r="S23" s="525"/>
     </row>
     <row r="24" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C24" s="168" t="s">
         <v>38</v>
       </c>
-      <c r="D24" s="169" t="s">
-        <v>759</v>
+      <c r="D24" s="169" t="str">
+        <f t="shared" si="2"/>
+        <v>R-RSDCK_LPG_N1</v>
       </c>
       <c r="E24" s="169" t="s">
-        <v>419</v>
+        <v>1003</v>
       </c>
       <c r="F24" s="169" t="s">
         <v>16</v>
@@ -36257,10 +36180,10 @@
         <v>38</v>
       </c>
       <c r="D25" s="169" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="E25" s="169" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F25" s="169" t="s">
         <v>16</v>
@@ -36279,10 +36202,10 @@
         <v>38</v>
       </c>
       <c r="D26" s="169" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="E26" s="169" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F26" s="169" t="s">
         <v>16</v>
@@ -36295,17 +36218,16 @@
       <c r="J26" s="170" t="s">
         <v>417</v>
       </c>
-      <c r="Q26" s="189"/>
     </row>
     <row r="27" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C27" s="168" t="s">
         <v>38</v>
       </c>
       <c r="D27" s="169" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="E27" s="169" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F27" s="169" t="s">
         <v>16</v>
@@ -36318,318 +36240,341 @@
       <c r="J27" s="170" t="s">
         <v>417</v>
       </c>
+      <c r="Q27" s="189"/>
     </row>
     <row r="28" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C28" s="168" t="s">
         <v>38</v>
       </c>
-      <c r="D28" s="171" t="s">
-        <v>763</v>
-      </c>
-      <c r="E28" s="171" t="s">
-        <v>423</v>
-      </c>
-      <c r="F28" s="171" t="s">
+      <c r="D28" s="169" t="s">
+        <v>762</v>
+      </c>
+      <c r="E28" s="169" t="s">
+        <v>422</v>
+      </c>
+      <c r="F28" s="169" t="s">
         <v>16</v>
       </c>
       <c r="G28" s="169" t="s">
         <v>363</v>
       </c>
-      <c r="H28" s="171"/>
-      <c r="I28" s="171"/>
-      <c r="J28" s="172" t="s">
+      <c r="H28" s="169"/>
+      <c r="I28" s="169"/>
+      <c r="J28" s="170" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="32" spans="3:22" ht="30" x14ac:dyDescent="0.2">
-      <c r="H32" s="5" t="s">
+    <row r="29" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="C29" s="168" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" s="171" t="s">
+        <v>763</v>
+      </c>
+      <c r="E29" s="171" t="s">
+        <v>423</v>
+      </c>
+      <c r="F29" s="171" t="s">
+        <v>16</v>
+      </c>
+      <c r="G29" s="169" t="s">
+        <v>363</v>
+      </c>
+      <c r="H29" s="171"/>
+      <c r="I29" s="171"/>
+      <c r="J29" s="172" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="33" spans="8:15" ht="30" x14ac:dyDescent="0.2">
+      <c r="H33" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="I32" s="5" t="s">
+      <c r="I33" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="J32" s="5" t="s">
+      <c r="J33" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="K32" s="5" t="s">
+      <c r="K33" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="L32" s="63" t="s">
+      <c r="L33" s="63" t="s">
         <v>668</v>
       </c>
-      <c r="M32" s="63" t="s">
+      <c r="M33" s="63" t="s">
         <v>324</v>
       </c>
-      <c r="N32" s="63" t="s">
+      <c r="N33" s="63" t="s">
         <v>325</v>
       </c>
-      <c r="O32" s="63" t="s">
+      <c r="O33" s="63" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="33" spans="8:15" x14ac:dyDescent="0.2">
-      <c r="H33" s="5" t="s">
-        <v>315</v>
-      </c>
-      <c r="I33" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="J33" s="5" t="s">
-        <v>316</v>
-      </c>
-      <c r="K33" s="5" t="s">
-        <v>317</v>
-      </c>
-      <c r="L33" s="483" t="s">
-        <v>322</v>
-      </c>
-      <c r="M33" s="484"/>
-      <c r="N33" s="484"/>
-      <c r="O33" s="485"/>
     </row>
     <row r="34" spans="8:15" x14ac:dyDescent="0.2">
       <c r="H34" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="I34" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="J34" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="K34" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="L34" s="522" t="s">
+        <v>322</v>
+      </c>
+      <c r="M34" s="523"/>
+      <c r="N34" s="523"/>
+      <c r="O34" s="524"/>
+    </row>
+    <row r="35" spans="8:15" x14ac:dyDescent="0.2">
+      <c r="H35" s="5" t="s">
         <v>376</v>
       </c>
-      <c r="L34" s="492" t="s">
+      <c r="L35" s="516" t="s">
         <v>328</v>
       </c>
-      <c r="M34" s="494"/>
-      <c r="N34" s="494"/>
-      <c r="O34" s="493"/>
-    </row>
-    <row r="35" spans="8:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H35" s="5" t="s">
+      <c r="M35" s="518"/>
+      <c r="N35" s="518"/>
+      <c r="O35" s="517"/>
+    </row>
+    <row r="36" spans="8:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H36" s="5" t="s">
         <v>757</v>
       </c>
-      <c r="I35" s="5" t="s">
+      <c r="I36" s="5" t="s">
         <v>416</v>
-      </c>
-      <c r="J35" s="5" t="s">
-        <v>408</v>
-      </c>
-      <c r="K35" s="5" t="s">
-        <v>409</v>
-      </c>
-      <c r="L35" s="197">
-        <v>2400</v>
-      </c>
-      <c r="M35" s="197">
-        <v>2400</v>
-      </c>
-      <c r="N35" s="197">
-        <v>2400</v>
-      </c>
-      <c r="O35" s="197">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="36" spans="8:15" x14ac:dyDescent="0.2">
-      <c r="H36" s="5" t="s">
-        <v>758</v>
-      </c>
-      <c r="I36" s="5" t="s">
-        <v>418</v>
       </c>
       <c r="J36" s="5" t="s">
         <v>408</v>
       </c>
       <c r="K36" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="L36" s="197">
+        <v>2400</v>
+      </c>
+      <c r="M36" s="197">
+        <v>2400</v>
+      </c>
+      <c r="N36" s="197">
+        <v>2400</v>
+      </c>
+      <c r="O36" s="197">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="37" spans="8:15" x14ac:dyDescent="0.2">
+      <c r="H37" s="5" t="s">
+        <v>758</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>418</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>408</v>
+      </c>
+      <c r="K37" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="L36" s="200">
+      <c r="L37" s="200">
         <v>175</v>
       </c>
-      <c r="M36" s="200">
+      <c r="M37" s="200">
         <v>175</v>
       </c>
-      <c r="N36" s="200">
+      <c r="N37" s="200">
         <v>175</v>
       </c>
-      <c r="O36" s="200">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="37" spans="8:15" x14ac:dyDescent="0.2">
-      <c r="J37" s="5" t="s">
-        <v>733</v>
-      </c>
-      <c r="L37" s="202">
-        <v>175</v>
-      </c>
-      <c r="M37" s="202">
-        <v>175</v>
-      </c>
-      <c r="N37" s="202">
-        <v>175</v>
-      </c>
-      <c r="O37" s="202">
+      <c r="O37" s="200">
         <v>175</v>
       </c>
     </row>
     <row r="38" spans="8:15" x14ac:dyDescent="0.2">
       <c r="J38" s="5" t="s">
+        <v>733</v>
+      </c>
+      <c r="L38" s="202">
+        <v>175</v>
+      </c>
+      <c r="M38" s="202">
+        <v>175</v>
+      </c>
+      <c r="N38" s="202">
+        <v>175</v>
+      </c>
+      <c r="O38" s="202">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="39" spans="8:15" x14ac:dyDescent="0.2">
+      <c r="J39" s="5" t="s">
         <v>729</v>
       </c>
-      <c r="L38" s="200">
+      <c r="L39" s="200">
         <v>175</v>
       </c>
-      <c r="M38" s="200">
+      <c r="M39" s="200">
         <v>175</v>
       </c>
-      <c r="N38" s="200">
+      <c r="N39" s="200">
         <v>175</v>
       </c>
-      <c r="O38" s="200">
+      <c r="O39" s="200">
         <v>175</v>
-      </c>
-    </row>
-    <row r="39" spans="8:15" x14ac:dyDescent="0.2">
-      <c r="H39" s="5" t="s">
-        <v>759</v>
-      </c>
-      <c r="I39" s="5" t="s">
-        <v>419</v>
-      </c>
-      <c r="J39" s="5" t="s">
-        <v>408</v>
-      </c>
-      <c r="K39" s="5" t="s">
-        <v>411</v>
-      </c>
-      <c r="L39" s="202">
-        <v>251</v>
-      </c>
-      <c r="M39" s="202">
-        <v>251</v>
-      </c>
-      <c r="N39" s="202">
-        <v>251</v>
-      </c>
-      <c r="O39" s="202">
-        <v>251</v>
       </c>
     </row>
     <row r="40" spans="8:15" x14ac:dyDescent="0.2">
       <c r="H40" s="5" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="J40" s="5" t="s">
         <v>408</v>
       </c>
       <c r="K40" s="5" t="s">
-        <v>412</v>
-      </c>
-      <c r="L40" s="200">
-        <v>214</v>
-      </c>
-      <c r="M40" s="200">
-        <v>214</v>
-      </c>
-      <c r="N40" s="200">
-        <v>214</v>
-      </c>
-      <c r="O40" s="200">
-        <v>214</v>
+        <v>411</v>
+      </c>
+      <c r="L40" s="202">
+        <v>251</v>
+      </c>
+      <c r="M40" s="202">
+        <v>251</v>
+      </c>
+      <c r="N40" s="202">
+        <v>251</v>
+      </c>
+      <c r="O40" s="202">
+        <v>251</v>
       </c>
     </row>
     <row r="41" spans="8:15" x14ac:dyDescent="0.2">
       <c r="H41" s="5" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="I41" s="5" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="J41" s="5" t="s">
         <v>408</v>
       </c>
       <c r="K41" s="5" t="s">
-        <v>413</v>
-      </c>
-      <c r="L41" s="202">
-        <v>191</v>
-      </c>
-      <c r="M41" s="202">
-        <v>191</v>
-      </c>
-      <c r="N41" s="202">
-        <v>191</v>
-      </c>
-      <c r="O41" s="202">
-        <v>191</v>
+        <v>412</v>
+      </c>
+      <c r="L41" s="200">
+        <v>214</v>
+      </c>
+      <c r="M41" s="200">
+        <v>214</v>
+      </c>
+      <c r="N41" s="200">
+        <v>214</v>
+      </c>
+      <c r="O41" s="200">
+        <v>214</v>
       </c>
     </row>
     <row r="42" spans="8:15" x14ac:dyDescent="0.2">
       <c r="H42" s="5" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="I42" s="5" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="J42" s="5" t="s">
         <v>408</v>
       </c>
       <c r="K42" s="5" t="s">
-        <v>414</v>
-      </c>
-      <c r="L42" s="200">
-        <v>5000</v>
-      </c>
-      <c r="M42" s="200">
-        <v>5000</v>
-      </c>
-      <c r="N42" s="200">
-        <v>5000</v>
-      </c>
-      <c r="O42" s="200">
-        <v>5000</v>
+        <v>413</v>
+      </c>
+      <c r="L42" s="202">
+        <v>191</v>
+      </c>
+      <c r="M42" s="202">
+        <v>191</v>
+      </c>
+      <c r="N42" s="202">
+        <v>191</v>
+      </c>
+      <c r="O42" s="202">
+        <v>191</v>
       </c>
     </row>
     <row r="43" spans="8:15" x14ac:dyDescent="0.2">
       <c r="H43" s="5" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="I43" s="5" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="J43" s="5" t="s">
         <v>408</v>
       </c>
       <c r="K43" s="5" t="s">
+        <v>414</v>
+      </c>
+      <c r="L43" s="200">
+        <v>5000</v>
+      </c>
+      <c r="M43" s="200">
+        <v>5000</v>
+      </c>
+      <c r="N43" s="200">
+        <v>5000</v>
+      </c>
+      <c r="O43" s="200">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="44" spans="8:15" x14ac:dyDescent="0.2">
+      <c r="H44" s="5" t="s">
+        <v>763</v>
+      </c>
+      <c r="I44" s="5" t="s">
+        <v>423</v>
+      </c>
+      <c r="J44" s="5" t="s">
+        <v>408</v>
+      </c>
+      <c r="K44" s="5" t="s">
         <v>415</v>
       </c>
-      <c r="L43" s="204">
+      <c r="L44" s="204">
         <v>5000</v>
       </c>
-      <c r="M43" s="204">
+      <c r="M44" s="204">
         <v>5000</v>
       </c>
-      <c r="N43" s="204">
+      <c r="N44" s="204">
         <v>5000</v>
       </c>
-      <c r="O43" s="204">
+      <c r="O44" s="204">
         <v>5000</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
+    <mergeCell ref="L35:O35"/>
     <mergeCell ref="L34:O34"/>
-    <mergeCell ref="L33:O33"/>
-    <mergeCell ref="R18:S22"/>
+    <mergeCell ref="R19:S23"/>
     <mergeCell ref="L5:O5"/>
     <mergeCell ref="L6:O6"/>
   </mergeCells>
-  <conditionalFormatting sqref="I19:I28">
+  <conditionalFormatting sqref="I20:I29">
     <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="between">
       <formula>0.000000001</formula>
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="Y15" r:id="rId1" xr:uid="{6F790111-B362-4390-963B-D2AEAFDB26BD}"/>
+    <hyperlink ref="V15" r:id="rId1" xr:uid="{6F790111-B362-4390-963B-D2AEAFDB26BD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -36738,16 +36683,16 @@
       <c r="G4" s="173" t="s">
         <v>321</v>
       </c>
-      <c r="H4" s="489" t="s">
+      <c r="H4" s="519" t="s">
         <v>110</v>
       </c>
-      <c r="I4" s="490"/>
-      <c r="J4" s="491"/>
-      <c r="K4" s="483" t="s">
+      <c r="I4" s="520"/>
+      <c r="J4" s="521"/>
+      <c r="K4" s="522" t="s">
         <v>322</v>
       </c>
-      <c r="L4" s="484"/>
-      <c r="M4" s="485"/>
+      <c r="L4" s="523"/>
+      <c r="M4" s="524"/>
       <c r="N4" s="106"/>
       <c r="O4" s="106" t="s">
         <v>323</v>
@@ -36770,46 +36715,46 @@
       <c r="G5" s="466" t="s">
         <v>302</v>
       </c>
-      <c r="H5" s="502" t="s">
+      <c r="H5" s="529" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="503"/>
-      <c r="J5" s="504"/>
-      <c r="K5" s="502" t="s">
+      <c r="I5" s="530"/>
+      <c r="J5" s="531"/>
+      <c r="K5" s="529" t="s">
         <v>765</v>
       </c>
-      <c r="L5" s="503"/>
-      <c r="M5" s="504"/>
-      <c r="N5" s="505" t="s">
+      <c r="L5" s="530"/>
+      <c r="M5" s="531"/>
+      <c r="N5" s="467" t="s">
         <v>329</v>
       </c>
-      <c r="O5" s="505" t="s">
+      <c r="O5" s="467" t="s">
         <v>45</v>
       </c>
-      <c r="P5" s="506" t="s">
+      <c r="P5" s="468" t="s">
         <v>764</v>
       </c>
-      <c r="Q5" s="505" t="s">
+      <c r="Q5" s="467" t="s">
         <v>331</v>
       </c>
       <c r="AA5" s="281"/>
-      <c r="AB5" s="507" t="s">
+      <c r="AB5" s="526" t="s">
         <v>1021</v>
       </c>
-      <c r="AC5" s="507"/>
-      <c r="AD5" s="508"/>
-      <c r="AE5" s="509" t="s">
+      <c r="AC5" s="526"/>
+      <c r="AD5" s="469"/>
+      <c r="AE5" s="527" t="s">
         <v>110</v>
       </c>
-      <c r="AF5" s="509"/>
-      <c r="AG5" s="509" t="s">
+      <c r="AF5" s="527"/>
+      <c r="AG5" s="527" t="s">
         <v>1022</v>
       </c>
-      <c r="AH5" s="509"/>
-      <c r="AI5" s="510" t="s">
+      <c r="AH5" s="527"/>
+      <c r="AI5" s="528" t="s">
         <v>1023</v>
       </c>
-      <c r="AJ5" s="510"/>
+      <c r="AJ5" s="528"/>
     </row>
     <row r="6" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C6" s="197" t="str">
@@ -36820,35 +36765,35 @@
         <f t="shared" si="0"/>
         <v>Residential Lighting Apartment New</v>
       </c>
-      <c r="E6" s="511" t="s">
+      <c r="E6" s="470" t="s">
         <v>408</v>
       </c>
       <c r="F6" s="199" t="s">
         <v>373</v>
       </c>
-      <c r="G6" s="512">
+      <c r="G6" s="471">
         <v>10</v>
       </c>
-      <c r="H6" s="513">
+      <c r="H6" s="472">
         <v>0.4</v>
       </c>
-      <c r="I6" s="514">
+      <c r="I6" s="473">
         <f>H6*(AC9/AB9)</f>
         <v>0.54333333333333333</v>
       </c>
-      <c r="J6" s="515">
+      <c r="J6" s="474">
         <f>H6*(AD9/AC9)</f>
         <v>0.73128834355828232</v>
       </c>
-      <c r="K6" s="516">
+      <c r="K6" s="475">
         <f t="shared" ref="K6:L11" si="1">L29/1000*$X6/1000</f>
         <v>1.1375E-2</v>
       </c>
-      <c r="L6" s="517">
+      <c r="L6" s="476">
         <f t="shared" si="1"/>
         <v>1.1375E-2</v>
       </c>
-      <c r="M6" s="518">
+      <c r="M6" s="477">
         <f t="shared" ref="M6:M11" si="2">O29/1000*$X6/1000</f>
         <v>1.1375E-2</v>
       </c>
@@ -36912,19 +36857,19 @@
       <c r="F7" s="201" t="s">
         <v>374</v>
       </c>
-      <c r="G7" s="519">
+      <c r="G7" s="478">
         <v>15</v>
       </c>
-      <c r="H7" s="520">
+      <c r="H7" s="479">
         <v>0.6</v>
       </c>
       <c r="I7" s="342">
         <v>0.6</v>
       </c>
-      <c r="J7" s="521">
+      <c r="J7" s="480">
         <v>0.6</v>
       </c>
-      <c r="K7" s="522">
+      <c r="K7" s="481">
         <f t="shared" si="1"/>
         <v>0.15</v>
       </c>
@@ -36932,7 +36877,7 @@
         <f t="shared" si="1"/>
         <v>0.15</v>
       </c>
-      <c r="M7" s="523">
+      <c r="M7" s="482">
         <f t="shared" si="2"/>
         <v>0.15</v>
       </c>
@@ -36959,22 +36904,22 @@
       <c r="AC7" s="5">
         <v>17</v>
       </c>
-      <c r="AE7" s="524">
+      <c r="AE7" s="483">
         <f>AB7/683</f>
         <v>2.4890190336749635E-2</v>
       </c>
-      <c r="AF7" s="524">
+      <c r="AF7" s="483">
         <f>AC7/683</f>
         <v>2.4890190336749635E-2</v>
       </c>
-      <c r="AG7" s="525">
+      <c r="AG7" s="484">
         <v>0.03</v>
       </c>
-      <c r="AI7" s="526">
+      <c r="AI7" s="485">
         <f t="shared" ref="AI7:AJ10" si="3">AE7*AG7</f>
         <v>7.4670571010248903E-4</v>
       </c>
-      <c r="AJ7" s="526">
+      <c r="AJ7" s="485">
         <f>AF7*AH7</f>
         <v>0</v>
       </c>
@@ -36988,27 +36933,27 @@
         <f t="shared" si="0"/>
         <v>Residential Lighting Attached New</v>
       </c>
-      <c r="E8" s="511" t="s">
+      <c r="E8" s="470" t="s">
         <v>408</v>
       </c>
       <c r="F8" s="203" t="s">
         <v>397</v>
       </c>
-      <c r="G8" s="527">
+      <c r="G8" s="486">
         <v>10</v>
       </c>
-      <c r="H8" s="528">
+      <c r="H8" s="487">
         <v>0.4</v>
       </c>
       <c r="I8" s="341">
         <f>H8*(AC9/AB9)</f>
         <v>0.54333333333333333</v>
       </c>
-      <c r="J8" s="529">
+      <c r="J8" s="488">
         <f>H6*(AD9/AC9)</f>
         <v>0.73128834355828232</v>
       </c>
-      <c r="K8" s="530">
+      <c r="K8" s="489">
         <f t="shared" si="1"/>
         <v>1.1375E-2</v>
       </c>
@@ -37016,7 +36961,7 @@
         <f t="shared" si="1"/>
         <v>1.1375E-2</v>
       </c>
-      <c r="M8" s="531">
+      <c r="M8" s="490">
         <f t="shared" si="2"/>
         <v>1.1375E-2</v>
       </c>
@@ -37043,25 +36988,25 @@
       <c r="AC8" s="5">
         <v>24</v>
       </c>
-      <c r="AE8" s="524">
+      <c r="AE8" s="483">
         <f t="shared" ref="AE8:AF10" si="4">AB8/683</f>
         <v>3.5139092240117131E-2</v>
       </c>
-      <c r="AF8" s="524">
+      <c r="AF8" s="483">
         <f t="shared" si="4"/>
         <v>3.5139092240117131E-2</v>
       </c>
-      <c r="AG8" s="525">
+      <c r="AG8" s="484">
         <v>0.05</v>
       </c>
-      <c r="AH8" s="525">
+      <c r="AH8" s="484">
         <v>0.01</v>
       </c>
-      <c r="AI8" s="526">
+      <c r="AI8" s="485">
         <f t="shared" si="3"/>
         <v>1.7569546120058566E-3</v>
       </c>
-      <c r="AJ8" s="526">
+      <c r="AJ8" s="485">
         <f t="shared" si="3"/>
         <v>3.5139092240117132E-4</v>
       </c>
@@ -37081,19 +37026,19 @@
       <c r="F9" s="201" t="s">
         <v>398</v>
       </c>
-      <c r="G9" s="519">
+      <c r="G9" s="478">
         <v>15</v>
       </c>
-      <c r="H9" s="520">
+      <c r="H9" s="479">
         <v>0.6</v>
       </c>
       <c r="I9" s="342">
         <v>0.6</v>
       </c>
-      <c r="J9" s="521">
+      <c r="J9" s="480">
         <v>0.6</v>
       </c>
-      <c r="K9" s="522">
+      <c r="K9" s="481">
         <f t="shared" si="1"/>
         <v>0.15</v>
       </c>
@@ -37101,7 +37046,7 @@
         <f t="shared" si="1"/>
         <v>0.15</v>
       </c>
-      <c r="M9" s="523">
+      <c r="M9" s="482">
         <f t="shared" si="2"/>
         <v>0.15</v>
       </c>
@@ -37128,25 +37073,25 @@
       <c r="AD9" s="5">
         <v>298</v>
       </c>
-      <c r="AE9" s="524">
+      <c r="AE9" s="483">
         <f t="shared" si="4"/>
         <v>0.17569546120058566</v>
       </c>
-      <c r="AF9" s="524">
+      <c r="AF9" s="483">
         <f t="shared" si="4"/>
         <v>0.23865300146412885</v>
       </c>
-      <c r="AG9" s="525">
+      <c r="AG9" s="484">
         <v>0.46</v>
       </c>
-      <c r="AH9" s="525">
+      <c r="AH9" s="484">
         <v>0.87</v>
       </c>
-      <c r="AI9" s="526">
+      <c r="AI9" s="485">
         <f>AE9*AG9</f>
         <v>8.0819912152269399E-2</v>
       </c>
-      <c r="AJ9" s="526">
+      <c r="AJ9" s="485">
         <f t="shared" si="3"/>
         <v>0.2076281112737921</v>
       </c>
@@ -37160,27 +37105,27 @@
         <f t="shared" si="0"/>
         <v>Residential Lighting Detached New</v>
       </c>
-      <c r="E10" s="511" t="s">
+      <c r="E10" s="470" t="s">
         <v>408</v>
       </c>
       <c r="F10" s="203" t="s">
         <v>405</v>
       </c>
-      <c r="G10" s="527">
+      <c r="G10" s="486">
         <v>10</v>
       </c>
-      <c r="H10" s="528">
+      <c r="H10" s="487">
         <v>0.4</v>
       </c>
       <c r="I10" s="341">
         <f>H10*(AC9/AB9)</f>
         <v>0.54333333333333333</v>
       </c>
-      <c r="J10" s="529">
+      <c r="J10" s="488">
         <f>H10*(AD9/AC9)</f>
         <v>0.73128834355828232</v>
       </c>
-      <c r="K10" s="530">
+      <c r="K10" s="489">
         <f t="shared" si="1"/>
         <v>1.1375E-2</v>
       </c>
@@ -37188,7 +37133,7 @@
         <f t="shared" si="1"/>
         <v>1.1375E-2</v>
       </c>
-      <c r="M10" s="531">
+      <c r="M10" s="490">
         <f t="shared" si="2"/>
         <v>1.1375E-2</v>
       </c>
@@ -37212,25 +37157,25 @@
       <c r="AC10" s="5">
         <v>100</v>
       </c>
-      <c r="AE10" s="524">
+      <c r="AE10" s="483">
         <f t="shared" si="4"/>
         <v>0.14641288433382138</v>
       </c>
-      <c r="AF10" s="524">
+      <c r="AF10" s="483">
         <f t="shared" si="4"/>
         <v>0.14641288433382138</v>
       </c>
-      <c r="AG10" s="525">
+      <c r="AG10" s="484">
         <v>0.46</v>
       </c>
-      <c r="AH10" s="525">
+      <c r="AH10" s="484">
         <v>0.12</v>
       </c>
-      <c r="AI10" s="526">
+      <c r="AI10" s="485">
         <f>AE10*AG10</f>
         <v>6.7349926793557835E-2</v>
       </c>
-      <c r="AJ10" s="526">
+      <c r="AJ10" s="485">
         <f t="shared" si="3"/>
         <v>1.7569546120058566E-2</v>
       </c>
@@ -37250,27 +37195,27 @@
       <c r="F11" s="201" t="s">
         <v>406</v>
       </c>
-      <c r="G11" s="532">
+      <c r="G11" s="491">
         <v>15</v>
       </c>
-      <c r="H11" s="533">
+      <c r="H11" s="492">
         <v>0.6</v>
       </c>
-      <c r="I11" s="534">
+      <c r="I11" s="493">
         <v>0.6</v>
       </c>
-      <c r="J11" s="535">
+      <c r="J11" s="494">
         <v>0.6</v>
       </c>
-      <c r="K11" s="536">
+      <c r="K11" s="495">
         <f t="shared" si="1"/>
         <v>0.15</v>
       </c>
-      <c r="L11" s="537">
+      <c r="L11" s="496">
         <f t="shared" si="1"/>
         <v>0.15</v>
       </c>
-      <c r="M11" s="538">
+      <c r="M11" s="497">
         <f t="shared" si="2"/>
         <v>0.15</v>
       </c>
@@ -37291,11 +37236,11 @@
       <c r="AB11" s="5">
         <v>275</v>
       </c>
-      <c r="AE11" s="524">
+      <c r="AE11" s="483">
         <f>AB11/683</f>
         <v>0.40263543191800877</v>
       </c>
-      <c r="AI11" s="526"/>
+      <c r="AI11" s="485"/>
     </row>
     <row r="12" spans="3:37" x14ac:dyDescent="0.2">
       <c r="AA12" s="5" t="s">
@@ -37304,21 +37249,21 @@
       <c r="AB12" s="5">
         <v>280</v>
       </c>
-      <c r="AE12" s="524">
+      <c r="AE12" s="483">
         <f>AB12/683</f>
         <v>0.40995607613469986</v>
       </c>
-      <c r="AI12" s="526"/>
+      <c r="AI12" s="485"/>
     </row>
     <row r="13" spans="3:37" x14ac:dyDescent="0.2">
       <c r="AA13" s="5" t="s">
         <v>1023</v>
       </c>
-      <c r="AI13" s="539">
+      <c r="AI13" s="498">
         <f>SUM(AI7:AI10)</f>
         <v>0.15067349926793558</v>
       </c>
-      <c r="AJ13" s="539">
+      <c r="AJ13" s="498">
         <f>SUM(AJ7:AJ10)</f>
         <v>0.22554904831625183</v>
       </c>
@@ -37520,12 +37465,12 @@
       <c r="K27" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="L27" s="483" t="s">
+      <c r="L27" s="522" t="s">
         <v>322</v>
       </c>
-      <c r="M27" s="484"/>
-      <c r="N27" s="484"/>
-      <c r="O27" s="485"/>
+      <c r="M27" s="523"/>
+      <c r="N27" s="523"/>
+      <c r="O27" s="524"/>
       <c r="T27" s="283"/>
       <c r="U27" s="283"/>
     </row>
@@ -37533,12 +37478,12 @@
       <c r="J28" s="5" t="s">
         <v>376</v>
       </c>
-      <c r="L28" s="486" t="s">
+      <c r="L28" s="513" t="s">
         <v>328</v>
       </c>
-      <c r="M28" s="487"/>
-      <c r="N28" s="487"/>
-      <c r="O28" s="488"/>
+      <c r="M28" s="514"/>
+      <c r="N28" s="514"/>
+      <c r="O28" s="515"/>
       <c r="T28" s="283"/>
       <c r="U28" s="283"/>
     </row>
@@ -38928,16 +38873,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="L28:O28"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="K5:M5"/>
     <mergeCell ref="AB5:AC5"/>
     <mergeCell ref="AE5:AF5"/>
     <mergeCell ref="AG5:AH5"/>
     <mergeCell ref="AI5:AJ5"/>
     <mergeCell ref="L27:O27"/>
-    <mergeCell ref="L28:O28"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="K5:M5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="S7" r:id="rId1" xr:uid="{B1EDD63D-40A5-4174-9D28-8666BD314B83}"/>
@@ -47966,128 +47911,128 @@
       <c r="C4" s="364" t="s">
         <v>774</v>
       </c>
-      <c r="D4" s="496" t="s">
+      <c r="D4" s="533" t="s">
         <v>775</v>
       </c>
-      <c r="E4" s="497"/>
-      <c r="F4" s="497"/>
-      <c r="G4" s="497"/>
-      <c r="H4" s="498"/>
-      <c r="I4" s="497" t="s">
+      <c r="E4" s="532"/>
+      <c r="F4" s="532"/>
+      <c r="G4" s="532"/>
+      <c r="H4" s="534"/>
+      <c r="I4" s="532" t="s">
         <v>776</v>
       </c>
-      <c r="J4" s="497"/>
-      <c r="K4" s="497"/>
-      <c r="L4" s="497"/>
-      <c r="M4" s="498"/>
-      <c r="N4" s="497" t="s">
+      <c r="J4" s="532"/>
+      <c r="K4" s="532"/>
+      <c r="L4" s="532"/>
+      <c r="M4" s="534"/>
+      <c r="N4" s="532" t="s">
         <v>777</v>
       </c>
-      <c r="O4" s="497"/>
-      <c r="P4" s="497"/>
-      <c r="Q4" s="497"/>
-      <c r="R4" s="498"/>
-      <c r="S4" s="497" t="s">
+      <c r="O4" s="532"/>
+      <c r="P4" s="532"/>
+      <c r="Q4" s="532"/>
+      <c r="R4" s="534"/>
+      <c r="S4" s="532" t="s">
         <v>778</v>
       </c>
-      <c r="T4" s="497"/>
-      <c r="U4" s="497"/>
-      <c r="V4" s="497"/>
-      <c r="W4" s="498"/>
-      <c r="X4" s="497" t="s">
+      <c r="T4" s="532"/>
+      <c r="U4" s="532"/>
+      <c r="V4" s="532"/>
+      <c r="W4" s="534"/>
+      <c r="X4" s="532" t="s">
         <v>779</v>
       </c>
-      <c r="Y4" s="497"/>
-      <c r="Z4" s="497"/>
-      <c r="AA4" s="497"/>
-      <c r="AB4" s="498"/>
-      <c r="AC4" s="497" t="s">
+      <c r="Y4" s="532"/>
+      <c r="Z4" s="532"/>
+      <c r="AA4" s="532"/>
+      <c r="AB4" s="534"/>
+      <c r="AC4" s="532" t="s">
         <v>780</v>
       </c>
-      <c r="AD4" s="497"/>
-      <c r="AE4" s="497"/>
-      <c r="AF4" s="497"/>
-      <c r="AG4" s="498"/>
-      <c r="AH4" s="497" t="s">
+      <c r="AD4" s="532"/>
+      <c r="AE4" s="532"/>
+      <c r="AF4" s="532"/>
+      <c r="AG4" s="534"/>
+      <c r="AH4" s="532" t="s">
         <v>781</v>
       </c>
-      <c r="AI4" s="497"/>
-      <c r="AJ4" s="497"/>
-      <c r="AK4" s="497"/>
-      <c r="AL4" s="498"/>
-      <c r="AM4" s="497" t="s">
+      <c r="AI4" s="532"/>
+      <c r="AJ4" s="532"/>
+      <c r="AK4" s="532"/>
+      <c r="AL4" s="534"/>
+      <c r="AM4" s="532" t="s">
         <v>782</v>
       </c>
-      <c r="AN4" s="497"/>
-      <c r="AO4" s="497"/>
-      <c r="AP4" s="497"/>
-      <c r="AQ4" s="498"/>
-      <c r="AR4" s="497" t="s">
+      <c r="AN4" s="532"/>
+      <c r="AO4" s="532"/>
+      <c r="AP4" s="532"/>
+      <c r="AQ4" s="534"/>
+      <c r="AR4" s="532" t="s">
         <v>783</v>
       </c>
-      <c r="AS4" s="497"/>
-      <c r="AT4" s="497"/>
-      <c r="AU4" s="497"/>
-      <c r="AV4" s="498"/>
-      <c r="AW4" s="497" t="s">
+      <c r="AS4" s="532"/>
+      <c r="AT4" s="532"/>
+      <c r="AU4" s="532"/>
+      <c r="AV4" s="534"/>
+      <c r="AW4" s="532" t="s">
         <v>784</v>
       </c>
-      <c r="AX4" s="497"/>
-      <c r="AY4" s="497"/>
-      <c r="AZ4" s="497"/>
-      <c r="BA4" s="497"/>
-      <c r="BB4" s="496" t="s">
+      <c r="AX4" s="532"/>
+      <c r="AY4" s="532"/>
+      <c r="AZ4" s="532"/>
+      <c r="BA4" s="532"/>
+      <c r="BB4" s="533" t="s">
         <v>785</v>
       </c>
-      <c r="BC4" s="497"/>
-      <c r="BD4" s="497"/>
-      <c r="BE4" s="497"/>
-      <c r="BF4" s="498"/>
-      <c r="BG4" s="497" t="s">
+      <c r="BC4" s="532"/>
+      <c r="BD4" s="532"/>
+      <c r="BE4" s="532"/>
+      <c r="BF4" s="534"/>
+      <c r="BG4" s="532" t="s">
         <v>786</v>
       </c>
-      <c r="BH4" s="497"/>
-      <c r="BI4" s="497"/>
-      <c r="BJ4" s="497"/>
-      <c r="BK4" s="497"/>
-      <c r="BL4" s="496" t="s">
+      <c r="BH4" s="532"/>
+      <c r="BI4" s="532"/>
+      <c r="BJ4" s="532"/>
+      <c r="BK4" s="532"/>
+      <c r="BL4" s="533" t="s">
         <v>787</v>
       </c>
-      <c r="BM4" s="497"/>
-      <c r="BN4" s="497"/>
-      <c r="BO4" s="497"/>
-      <c r="BP4" s="497"/>
-      <c r="BQ4" s="496" t="s">
+      <c r="BM4" s="532"/>
+      <c r="BN4" s="532"/>
+      <c r="BO4" s="532"/>
+      <c r="BP4" s="532"/>
+      <c r="BQ4" s="533" t="s">
         <v>788</v>
       </c>
-      <c r="BR4" s="497"/>
-      <c r="BS4" s="497"/>
-      <c r="BT4" s="497"/>
-      <c r="BU4" s="498"/>
+      <c r="BR4" s="532"/>
+      <c r="BS4" s="532"/>
+      <c r="BT4" s="532"/>
+      <c r="BU4" s="534"/>
       <c r="BV4" s="365" t="s">
         <v>789</v>
       </c>
-      <c r="BW4" s="499" t="s">
+      <c r="BW4" s="535" t="s">
         <v>790</v>
       </c>
-      <c r="BX4" s="500"/>
-      <c r="BY4" s="500"/>
-      <c r="BZ4" s="500"/>
-      <c r="CA4" s="501"/>
-      <c r="CB4" s="499" t="s">
+      <c r="BX4" s="536"/>
+      <c r="BY4" s="536"/>
+      <c r="BZ4" s="536"/>
+      <c r="CA4" s="537"/>
+      <c r="CB4" s="535" t="s">
         <v>791</v>
       </c>
-      <c r="CC4" s="500"/>
-      <c r="CD4" s="500"/>
-      <c r="CE4" s="500"/>
-      <c r="CF4" s="501"/>
-      <c r="CG4" s="499" t="s">
+      <c r="CC4" s="536"/>
+      <c r="CD4" s="536"/>
+      <c r="CE4" s="536"/>
+      <c r="CF4" s="537"/>
+      <c r="CG4" s="535" t="s">
         <v>792</v>
       </c>
-      <c r="CH4" s="500"/>
-      <c r="CI4" s="500"/>
-      <c r="CJ4" s="500"/>
-      <c r="CK4" s="501"/>
+      <c r="CH4" s="536"/>
+      <c r="CI4" s="536"/>
+      <c r="CJ4" s="536"/>
+      <c r="CK4" s="537"/>
     </row>
     <row r="5" spans="1:89" x14ac:dyDescent="0.2">
       <c r="A5" s="367"/>
@@ -61656,6 +61601,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="BL4:BP4"/>
+    <mergeCell ref="BQ4:BU4"/>
+    <mergeCell ref="BW4:CA4"/>
+    <mergeCell ref="CB4:CF4"/>
+    <mergeCell ref="CG4:CK4"/>
     <mergeCell ref="BG4:BK4"/>
     <mergeCell ref="D4:H4"/>
     <mergeCell ref="I4:M4"/>
@@ -61668,11 +61618,6 @@
     <mergeCell ref="AR4:AV4"/>
     <mergeCell ref="AW4:BA4"/>
     <mergeCell ref="BB4:BF4"/>
-    <mergeCell ref="BL4:BP4"/>
-    <mergeCell ref="BQ4:BU4"/>
-    <mergeCell ref="BW4:CA4"/>
-    <mergeCell ref="CB4:CF4"/>
-    <mergeCell ref="CG4:CK4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
Electric Heater Lifetime - 20 years
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_RSD.xlsx
+++ b/SubRES_TMPL/SubRes_RSD.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E06D0FB1-9FBC-4361-9D5D-9896CA13D760}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42D3B03E-8820-40C9-94C6-5F60EC4801ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="5" xr2:uid="{34F9D92C-266F-476D-89E0-63153305AC39}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="4" xr2:uid="{34F9D92C-266F-476D-89E0-63153305AC39}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="34" r:id="rId1"/>
@@ -781,7 +781,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="W8" authorId="0" shapeId="0" xr:uid="{4CC7BAE4-B77F-4446-B919-7188CC25F5B2}">
+    <comment ref="Z8" authorId="0" shapeId="0" xr:uid="{4CC7BAE4-B77F-4446-B919-7188CC25F5B2}">
       <text>
         <r>
           <rPr>
@@ -830,7 +830,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R15" authorId="0" shapeId="0" xr:uid="{6AD7F003-C0BD-4A39-A684-1B5072D780D3}">
+    <comment ref="U15" authorId="0" shapeId="0" xr:uid="{6AD7F003-C0BD-4A39-A684-1B5072D780D3}">
       <text>
         <r>
           <rPr>
@@ -854,7 +854,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L36" authorId="0" shapeId="0" xr:uid="{B2CBE2A3-43A2-4EFE-8157-00F31233ABB8}">
+    <comment ref="L35" authorId="0" shapeId="0" xr:uid="{B2CBE2A3-43A2-4EFE-8157-00F31233ABB8}">
       <text>
         <r>
           <rPr>
@@ -8611,7 +8611,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3430" uniqueCount="1033">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3433" uniqueCount="1036">
   <si>
     <t>Document type:</t>
   </si>
@@ -11722,6 +11722,15 @@
   </si>
   <si>
     <t>Theoretical limit for a white LED</t>
+  </si>
+  <si>
+    <t>FLO_SHAR~UP~2018</t>
+  </si>
+  <si>
+    <t>FLO_SHAR~UP~2070</t>
+  </si>
+  <si>
+    <t>FLO_SHAR~UP~0</t>
   </si>
   <si>
     <t>https://www.ransomspares.co.uk/blog/news/gas-cooker-vs-electric-cooker.htm#:~:text=According%20to%20Which%2C%20it%20costs,it%20works%20out%20more%20expensive.</t>
@@ -13339,7 +13348,7 @@
     <xf numFmtId="0" fontId="39" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="54" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="541">
+  <cellXfs count="542">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -14283,6 +14292,12 @@
     <xf numFmtId="0" fontId="16" fillId="23" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="23" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -14321,6 +14336,8 @@
     <xf numFmtId="172" fontId="40" fillId="21" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="172" fontId="40" fillId="21" borderId="72" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="173" fontId="44" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="40" fillId="21" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="40" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -14438,9 +14455,6 @@
     <xf numFmtId="0" fontId="60" fillId="32" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="20% - Colore 2" xfId="11" xr:uid="{3E3DAF22-4D86-48A9-B6EE-8D230C1E993C}"/>
@@ -16157,14 +16171,14 @@
       <c r="F16" s="211"/>
     </row>
     <row r="17" spans="1:14" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="500" t="s">
+      <c r="A17" s="504" t="s">
         <v>439</v>
       </c>
-      <c r="B17" s="500"/>
-      <c r="C17" s="500"/>
-      <c r="D17" s="500"/>
-      <c r="E17" s="500"/>
-      <c r="F17" s="500"/>
+      <c r="B17" s="504"/>
+      <c r="C17" s="504"/>
+      <c r="D17" s="504"/>
+      <c r="E17" s="504"/>
+      <c r="F17" s="504"/>
       <c r="G17" s="213"/>
       <c r="H17" s="213"/>
       <c r="I17" s="214"/>
@@ -16202,13 +16216,13 @@
       <c r="A20" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="501" t="s">
+      <c r="B20" s="505" t="s">
         <v>441</v>
       </c>
-      <c r="C20" s="501"/>
-      <c r="D20" s="501"/>
-      <c r="E20" s="501"/>
-      <c r="F20" s="501"/>
+      <c r="C20" s="505"/>
+      <c r="D20" s="505"/>
+      <c r="E20" s="505"/>
+      <c r="F20" s="505"/>
       <c r="G20" s="218"/>
       <c r="H20" s="218"/>
       <c r="I20" s="219"/>
@@ -16222,13 +16236,13 @@
       <c r="A21" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="502" t="s">
+      <c r="B21" s="506" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="502"/>
-      <c r="D21" s="502"/>
-      <c r="E21" s="502"/>
-      <c r="F21" s="502"/>
+      <c r="C21" s="506"/>
+      <c r="D21" s="506"/>
+      <c r="E21" s="506"/>
+      <c r="F21" s="506"/>
       <c r="G21" s="218"/>
       <c r="H21" s="218"/>
       <c r="I21" s="219"/>
@@ -16242,13 +16256,13 @@
       <c r="A22" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="502" t="s">
+      <c r="B22" s="506" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="502"/>
-      <c r="D22" s="502"/>
-      <c r="E22" s="502"/>
-      <c r="F22" s="502"/>
+      <c r="C22" s="506"/>
+      <c r="D22" s="506"/>
+      <c r="E22" s="506"/>
+      <c r="F22" s="506"/>
     </row>
     <row r="23" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
@@ -16277,22 +16291,22 @@
       <c r="H24" s="3"/>
     </row>
     <row r="25" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="503"/>
-      <c r="B25" s="503"/>
-      <c r="C25" s="503"/>
-      <c r="D25" s="503"/>
-      <c r="E25" s="503"/>
-      <c r="F25" s="503"/>
+      <c r="A25" s="507"/>
+      <c r="B25" s="507"/>
+      <c r="C25" s="507"/>
+      <c r="D25" s="507"/>
+      <c r="E25" s="507"/>
+      <c r="F25" s="507"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
     </row>
     <row r="26" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="499"/>
-      <c r="B26" s="499"/>
-      <c r="C26" s="499"/>
-      <c r="D26" s="499"/>
-      <c r="E26" s="499"/>
-      <c r="F26" s="499"/>
+      <c r="A26" s="503"/>
+      <c r="B26" s="503"/>
+      <c r="C26" s="503"/>
+      <c r="D26" s="503"/>
+      <c r="E26" s="503"/>
+      <c r="F26" s="503"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="211"/>
@@ -16479,16 +16493,16 @@
   <sheetData>
     <row r="1" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:20" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="504" t="s">
+      <c r="B2" s="508" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="505"/>
-      <c r="D2" s="505"/>
-      <c r="E2" s="506"/>
-      <c r="G2" s="504" t="s">
+      <c r="C2" s="509"/>
+      <c r="D2" s="509"/>
+      <c r="E2" s="510"/>
+      <c r="G2" s="508" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="506"/>
+      <c r="H2" s="510"/>
       <c r="I2" s="222"/>
       <c r="J2" s="222"/>
       <c r="K2" s="223"/>
@@ -16830,16 +16844,16 @@
     </row>
     <row r="19" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="2:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="507" t="s">
+      <c r="B20" s="511" t="s">
         <v>70</v>
       </c>
-      <c r="C20" s="508"/>
-      <c r="D20" s="508"/>
-      <c r="E20" s="509"/>
-      <c r="G20" s="504" t="s">
+      <c r="C20" s="512"/>
+      <c r="D20" s="512"/>
+      <c r="E20" s="513"/>
+      <c r="G20" s="508" t="s">
         <v>14</v>
       </c>
-      <c r="H20" s="506"/>
+      <c r="H20" s="510"/>
     </row>
     <row r="21" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="250" t="s">
@@ -17083,16 +17097,16 @@
     </row>
     <row r="37" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="38" spans="2:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="504" t="s">
+      <c r="B38" s="508" t="s">
         <v>78</v>
       </c>
-      <c r="C38" s="505"/>
-      <c r="D38" s="505"/>
-      <c r="E38" s="506"/>
-      <c r="G38" s="510" t="s">
+      <c r="C38" s="509"/>
+      <c r="D38" s="509"/>
+      <c r="E38" s="510"/>
+      <c r="G38" s="514" t="s">
         <v>72</v>
       </c>
-      <c r="H38" s="511"/>
+      <c r="H38" s="515"/>
     </row>
     <row r="39" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B39" s="271" t="s">
@@ -17261,13 +17275,13 @@
       <c r="M3" s="5" t="s">
         <v>391</v>
       </c>
-      <c r="S3" s="512" t="s">
+      <c r="S3" s="516" t="s">
         <v>687</v>
       </c>
-      <c r="T3" s="512"/>
-      <c r="U3" s="512"/>
-      <c r="V3" s="512"/>
-      <c r="W3" s="512"/>
+      <c r="T3" s="516"/>
+      <c r="U3" s="516"/>
+      <c r="V3" s="516"/>
+      <c r="W3" s="516"/>
     </row>
     <row r="4" spans="3:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C4" s="62" t="s">
@@ -24945,8 +24959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{104F8057-C735-4662-BAA6-EEDCF7B57273}">
   <dimension ref="A2:AO162"/>
   <sheetViews>
-    <sheetView topLeftCell="B9" zoomScale="64" zoomScaleNormal="110" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="V41" sqref="V41"/>
+    <sheetView tabSelected="1" topLeftCell="E10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -25101,34 +25115,34 @@
       <c r="F4" s="62" t="s">
         <v>317</v>
       </c>
-      <c r="G4" s="519" t="s">
+      <c r="G4" s="523" t="s">
         <v>727</v>
       </c>
-      <c r="H4" s="520"/>
-      <c r="I4" s="520"/>
-      <c r="J4" s="521"/>
-      <c r="K4" s="519" t="s">
+      <c r="H4" s="524"/>
+      <c r="I4" s="524"/>
+      <c r="J4" s="525"/>
+      <c r="K4" s="523" t="s">
         <v>319</v>
       </c>
-      <c r="L4" s="520"/>
-      <c r="M4" s="520"/>
-      <c r="N4" s="521"/>
-      <c r="O4" s="519" t="s">
+      <c r="L4" s="524"/>
+      <c r="M4" s="524"/>
+      <c r="N4" s="525"/>
+      <c r="O4" s="523" t="s">
         <v>320</v>
       </c>
-      <c r="P4" s="520"/>
-      <c r="Q4" s="520"/>
-      <c r="R4" s="521"/>
-      <c r="S4" s="519" t="s">
+      <c r="P4" s="524"/>
+      <c r="Q4" s="524"/>
+      <c r="R4" s="525"/>
+      <c r="S4" s="523" t="s">
         <v>321</v>
       </c>
-      <c r="T4" s="521"/>
-      <c r="U4" s="522" t="s">
+      <c r="T4" s="525"/>
+      <c r="U4" s="526" t="s">
         <v>322</v>
       </c>
-      <c r="V4" s="523"/>
-      <c r="W4" s="523"/>
-      <c r="X4" s="524"/>
+      <c r="V4" s="527"/>
+      <c r="W4" s="527"/>
+      <c r="X4" s="528"/>
       <c r="Y4" s="106"/>
       <c r="Z4" s="106"/>
       <c r="AA4" s="114" t="s">
@@ -25223,34 +25237,34 @@
       <c r="D6" s="84"/>
       <c r="E6" s="84"/>
       <c r="F6" s="85"/>
-      <c r="G6" s="513" t="s">
+      <c r="G6" s="517" t="s">
         <v>45</v>
       </c>
-      <c r="H6" s="514"/>
-      <c r="I6" s="514"/>
-      <c r="J6" s="515"/>
-      <c r="K6" s="514" t="s">
+      <c r="H6" s="518"/>
+      <c r="I6" s="518"/>
+      <c r="J6" s="519"/>
+      <c r="K6" s="518" t="s">
         <v>45</v>
       </c>
-      <c r="L6" s="514"/>
-      <c r="M6" s="514"/>
-      <c r="N6" s="515"/>
-      <c r="O6" s="513" t="s">
+      <c r="L6" s="518"/>
+      <c r="M6" s="518"/>
+      <c r="N6" s="519"/>
+      <c r="O6" s="517" t="s">
         <v>45</v>
       </c>
-      <c r="P6" s="514"/>
-      <c r="Q6" s="514"/>
-      <c r="R6" s="515"/>
-      <c r="S6" s="513" t="s">
+      <c r="P6" s="518"/>
+      <c r="Q6" s="518"/>
+      <c r="R6" s="519"/>
+      <c r="S6" s="517" t="s">
         <v>302</v>
       </c>
-      <c r="T6" s="515"/>
-      <c r="U6" s="513" t="s">
+      <c r="T6" s="519"/>
+      <c r="U6" s="517" t="s">
         <v>976</v>
       </c>
-      <c r="V6" s="514"/>
-      <c r="W6" s="514"/>
-      <c r="X6" s="515"/>
+      <c r="V6" s="518"/>
+      <c r="W6" s="518"/>
+      <c r="X6" s="519"/>
       <c r="Y6" s="107" t="s">
         <v>988</v>
       </c>
@@ -26147,7 +26161,7 @@
       <c r="Q16" s="121"/>
       <c r="R16" s="122"/>
       <c r="S16" s="167">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="T16" s="124"/>
       <c r="U16" s="125">
@@ -27981,34 +27995,34 @@
       <c r="F42" s="62" t="s">
         <v>317</v>
       </c>
-      <c r="G42" s="519" t="s">
+      <c r="G42" s="523" t="s">
         <v>318</v>
       </c>
-      <c r="H42" s="520"/>
-      <c r="I42" s="520"/>
-      <c r="J42" s="521"/>
-      <c r="K42" s="519" t="s">
+      <c r="H42" s="524"/>
+      <c r="I42" s="524"/>
+      <c r="J42" s="525"/>
+      <c r="K42" s="523" t="s">
         <v>319</v>
       </c>
-      <c r="L42" s="520"/>
-      <c r="M42" s="520"/>
-      <c r="N42" s="521"/>
-      <c r="O42" s="519" t="s">
+      <c r="L42" s="524"/>
+      <c r="M42" s="524"/>
+      <c r="N42" s="525"/>
+      <c r="O42" s="523" t="s">
         <v>320</v>
       </c>
-      <c r="P42" s="520"/>
-      <c r="Q42" s="520"/>
-      <c r="R42" s="521"/>
-      <c r="S42" s="519" t="s">
+      <c r="P42" s="524"/>
+      <c r="Q42" s="524"/>
+      <c r="R42" s="525"/>
+      <c r="S42" s="523" t="s">
         <v>321</v>
       </c>
-      <c r="T42" s="521"/>
-      <c r="U42" s="522" t="s">
+      <c r="T42" s="525"/>
+      <c r="U42" s="526" t="s">
         <v>322</v>
       </c>
-      <c r="V42" s="523"/>
-      <c r="W42" s="523"/>
-      <c r="X42" s="524"/>
+      <c r="V42" s="527"/>
+      <c r="W42" s="527"/>
+      <c r="X42" s="528"/>
       <c r="Y42" s="106"/>
       <c r="Z42" s="106"/>
       <c r="AA42" s="114" t="s">
@@ -28103,34 +28117,34 @@
       <c r="D44" s="84"/>
       <c r="E44" s="84"/>
       <c r="F44" s="85"/>
-      <c r="G44" s="513" t="s">
+      <c r="G44" s="517" t="s">
         <v>45</v>
       </c>
-      <c r="H44" s="514"/>
-      <c r="I44" s="514"/>
-      <c r="J44" s="515"/>
-      <c r="K44" s="514" t="s">
+      <c r="H44" s="518"/>
+      <c r="I44" s="518"/>
+      <c r="J44" s="519"/>
+      <c r="K44" s="518" t="s">
         <v>45</v>
       </c>
-      <c r="L44" s="514"/>
-      <c r="M44" s="514"/>
-      <c r="N44" s="515"/>
-      <c r="O44" s="513" t="s">
+      <c r="L44" s="518"/>
+      <c r="M44" s="518"/>
+      <c r="N44" s="519"/>
+      <c r="O44" s="517" t="s">
         <v>45</v>
       </c>
-      <c r="P44" s="514"/>
-      <c r="Q44" s="514"/>
-      <c r="R44" s="515"/>
-      <c r="S44" s="516" t="s">
+      <c r="P44" s="518"/>
+      <c r="Q44" s="518"/>
+      <c r="R44" s="519"/>
+      <c r="S44" s="520" t="s">
         <v>302</v>
       </c>
-      <c r="T44" s="517"/>
-      <c r="U44" s="516" t="s">
+      <c r="T44" s="521"/>
+      <c r="U44" s="520" t="s">
         <v>976</v>
       </c>
-      <c r="V44" s="518"/>
-      <c r="W44" s="518"/>
-      <c r="X44" s="517"/>
+      <c r="V44" s="522"/>
+      <c r="W44" s="522"/>
+      <c r="X44" s="521"/>
       <c r="Y44" s="458" t="s">
         <v>988</v>
       </c>
@@ -29650,7 +29664,7 @@
       <c r="Q60" s="121"/>
       <c r="R60" s="122"/>
       <c r="S60" s="123">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="T60" s="124"/>
       <c r="U60" s="125">
@@ -31501,34 +31515,34 @@
       <c r="F88" s="62" t="s">
         <v>317</v>
       </c>
-      <c r="G88" s="519" t="s">
+      <c r="G88" s="523" t="s">
         <v>318</v>
       </c>
-      <c r="H88" s="520"/>
-      <c r="I88" s="520"/>
-      <c r="J88" s="521"/>
-      <c r="K88" s="519" t="s">
+      <c r="H88" s="524"/>
+      <c r="I88" s="524"/>
+      <c r="J88" s="525"/>
+      <c r="K88" s="523" t="s">
         <v>319</v>
       </c>
-      <c r="L88" s="520"/>
-      <c r="M88" s="520"/>
-      <c r="N88" s="521"/>
-      <c r="O88" s="519" t="s">
+      <c r="L88" s="524"/>
+      <c r="M88" s="524"/>
+      <c r="N88" s="525"/>
+      <c r="O88" s="523" t="s">
         <v>320</v>
       </c>
-      <c r="P88" s="520"/>
-      <c r="Q88" s="520"/>
-      <c r="R88" s="521"/>
-      <c r="S88" s="519" t="s">
+      <c r="P88" s="524"/>
+      <c r="Q88" s="524"/>
+      <c r="R88" s="525"/>
+      <c r="S88" s="523" t="s">
         <v>321</v>
       </c>
-      <c r="T88" s="521"/>
-      <c r="U88" s="522" t="s">
+      <c r="T88" s="525"/>
+      <c r="U88" s="526" t="s">
         <v>322</v>
       </c>
-      <c r="V88" s="523"/>
-      <c r="W88" s="523"/>
-      <c r="X88" s="524"/>
+      <c r="V88" s="527"/>
+      <c r="W88" s="527"/>
+      <c r="X88" s="528"/>
       <c r="Y88" s="106"/>
       <c r="Z88" s="106"/>
       <c r="AA88" s="114" t="s">
@@ -31623,34 +31637,34 @@
       <c r="D90" s="84"/>
       <c r="E90" s="84"/>
       <c r="F90" s="85"/>
-      <c r="G90" s="513" t="s">
+      <c r="G90" s="517" t="s">
         <v>45</v>
       </c>
-      <c r="H90" s="514"/>
-      <c r="I90" s="514"/>
-      <c r="J90" s="515"/>
-      <c r="K90" s="514" t="s">
+      <c r="H90" s="518"/>
+      <c r="I90" s="518"/>
+      <c r="J90" s="519"/>
+      <c r="K90" s="518" t="s">
         <v>45</v>
       </c>
-      <c r="L90" s="514"/>
-      <c r="M90" s="514"/>
-      <c r="N90" s="515"/>
-      <c r="O90" s="513" t="s">
+      <c r="L90" s="518"/>
+      <c r="M90" s="518"/>
+      <c r="N90" s="519"/>
+      <c r="O90" s="517" t="s">
         <v>45</v>
       </c>
-      <c r="P90" s="514"/>
-      <c r="Q90" s="514"/>
-      <c r="R90" s="515"/>
-      <c r="S90" s="516" t="s">
+      <c r="P90" s="518"/>
+      <c r="Q90" s="518"/>
+      <c r="R90" s="519"/>
+      <c r="S90" s="520" t="s">
         <v>302</v>
       </c>
-      <c r="T90" s="517"/>
-      <c r="U90" s="516" t="s">
+      <c r="T90" s="521"/>
+      <c r="U90" s="520" t="s">
         <v>976</v>
       </c>
-      <c r="V90" s="518"/>
-      <c r="W90" s="518"/>
-      <c r="X90" s="517"/>
+      <c r="V90" s="522"/>
+      <c r="W90" s="522"/>
+      <c r="X90" s="521"/>
       <c r="Y90" s="458" t="s">
         <v>988</v>
       </c>
@@ -33170,7 +33184,7 @@
       <c r="Q106" s="121"/>
       <c r="R106" s="122"/>
       <c r="S106" s="123">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="T106" s="124"/>
       <c r="U106" s="125">
@@ -35225,10 +35239,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CED359C-4B42-41C8-A7E8-4F6FC9AE57D2}">
-  <dimension ref="C2:Y44"/>
+  <dimension ref="C2:Z43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S25" sqref="S25"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -35252,37 +35266,37 @@
     <col min="36" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:25" x14ac:dyDescent="0.2">
-      <c r="C2" s="470"/>
-      <c r="D2" s="470"/>
-      <c r="E2" s="470"/>
-      <c r="F2" s="470"/>
-      <c r="G2" s="470"/>
-      <c r="H2" s="470"/>
-      <c r="I2" s="470"/>
-      <c r="J2" s="470"/>
-      <c r="K2" s="470"/>
-      <c r="L2" s="470"/>
-      <c r="M2" s="470"/>
-      <c r="N2" s="470"/>
-    </row>
-    <row r="3" spans="3:25" x14ac:dyDescent="0.2">
-      <c r="C3" s="470"/>
-      <c r="D3" s="470"/>
-      <c r="E3" s="470"/>
+    <row r="2" spans="3:26" x14ac:dyDescent="0.2">
+      <c r="C2" s="472"/>
+      <c r="D2" s="472"/>
+      <c r="E2" s="472"/>
+      <c r="F2" s="472"/>
+      <c r="G2" s="472"/>
+      <c r="H2" s="472"/>
+      <c r="I2" s="472"/>
+      <c r="J2" s="472"/>
+      <c r="K2" s="472"/>
+      <c r="L2" s="472"/>
+      <c r="M2" s="472"/>
+      <c r="N2" s="472"/>
+    </row>
+    <row r="3" spans="3:26" x14ac:dyDescent="0.2">
+      <c r="C3" s="472"/>
+      <c r="D3" s="472"/>
+      <c r="E3" s="472"/>
       <c r="F3" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="470"/>
-      <c r="H3" s="470"/>
-      <c r="I3" s="470"/>
-      <c r="J3" s="470"/>
-      <c r="K3" s="470"/>
-      <c r="L3" s="470"/>
-      <c r="M3" s="470"/>
-      <c r="N3" s="470"/>
-    </row>
-    <row r="4" spans="3:25" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G3" s="472"/>
+      <c r="H3" s="472"/>
+      <c r="I3" s="472"/>
+      <c r="J3" s="472"/>
+      <c r="K3" s="472"/>
+      <c r="L3" s="472"/>
+      <c r="M3" s="472"/>
+      <c r="N3" s="472"/>
+    </row>
+    <row r="4" spans="3:26" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C4" s="60" t="s">
         <v>28</v>
       </c>
@@ -35323,19 +35337,28 @@
         <v>326</v>
       </c>
       <c r="P4" s="63" t="s">
+        <v>1030</v>
+      </c>
+      <c r="Q4" s="63" t="s">
+        <v>1031</v>
+      </c>
+      <c r="R4" s="63" t="s">
+        <v>1032</v>
+      </c>
+      <c r="S4" s="63" t="s">
         <v>81</v>
       </c>
-      <c r="Q4" s="63" t="s">
+      <c r="T4" s="63" t="s">
         <v>740</v>
       </c>
-      <c r="R4" s="63" t="s">
+      <c r="U4" s="63" t="s">
         <v>313</v>
       </c>
-      <c r="S4" s="63" t="s">
+      <c r="V4" s="63" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="5" spans="3:25" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="3:26" ht="38.25" x14ac:dyDescent="0.2">
       <c r="C5" s="62" t="s">
         <v>315</v>
       </c>
@@ -35355,29 +35378,32 @@
       <c r="I5" s="173"/>
       <c r="J5" s="173"/>
       <c r="K5" s="173"/>
-      <c r="L5" s="522" t="s">
+      <c r="L5" s="526" t="s">
         <v>322</v>
       </c>
-      <c r="M5" s="523"/>
-      <c r="N5" s="523"/>
-      <c r="O5" s="524"/>
-      <c r="P5" s="106"/>
-      <c r="Q5" s="106" t="s">
+      <c r="M5" s="527"/>
+      <c r="N5" s="527"/>
+      <c r="O5" s="528"/>
+      <c r="P5" s="468"/>
+      <c r="Q5" s="468"/>
+      <c r="R5" s="468"/>
+      <c r="S5" s="106"/>
+      <c r="T5" s="106" t="s">
         <v>323</v>
       </c>
-      <c r="R5" s="106" t="s">
+      <c r="U5" s="106" t="s">
         <v>116</v>
       </c>
-      <c r="S5" s="106"/>
-      <c r="U5" s="106" t="s">
+      <c r="V5" s="106"/>
+      <c r="X5" s="106" t="s">
         <v>630</v>
       </c>
-      <c r="V5" s="106"/>
-      <c r="W5" s="106" t="s">
+      <c r="Y5" s="106"/>
+      <c r="Z5" s="106" t="s">
         <v>633</v>
       </c>
     </row>
-    <row r="6" spans="3:25" x14ac:dyDescent="0.2">
+    <row r="6" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C6" s="83" t="s">
         <v>376</v>
       </c>
@@ -35391,41 +35417,44 @@
       <c r="I6" s="83"/>
       <c r="J6" s="83"/>
       <c r="K6" s="83"/>
-      <c r="L6" s="516" t="s">
+      <c r="L6" s="520" t="s">
         <v>976</v>
       </c>
-      <c r="M6" s="518"/>
-      <c r="N6" s="518"/>
-      <c r="O6" s="517"/>
-      <c r="P6" s="458" t="s">
+      <c r="M6" s="522"/>
+      <c r="N6" s="522"/>
+      <c r="O6" s="521"/>
+      <c r="P6" s="467"/>
+      <c r="Q6" s="467"/>
+      <c r="R6" s="467"/>
+      <c r="S6" s="458" t="s">
         <v>988</v>
       </c>
-      <c r="Q6" s="107" t="s">
+      <c r="T6" s="107" t="s">
         <v>45</v>
       </c>
-      <c r="R6" s="116" t="s">
+      <c r="U6" s="116" t="s">
         <v>764</v>
       </c>
-      <c r="S6" s="107" t="s">
+      <c r="V6" s="107" t="s">
         <v>331</v>
       </c>
-      <c r="U6" s="107" t="s">
+      <c r="X6" s="107" t="s">
         <v>631</v>
       </c>
-      <c r="V6" s="116" t="s">
+      <c r="Y6" s="116" t="s">
         <v>634</v>
       </c>
-      <c r="W6" s="107" t="s">
+      <c r="Z6" s="107" t="s">
         <v>632</v>
       </c>
     </row>
-    <row r="7" spans="3:25" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C7" s="202" t="str">
-        <f>D21</f>
+        <f>D20</f>
         <v>R-RSDRF_N1</v>
       </c>
       <c r="D7" s="192" t="str">
-        <f>E21</f>
+        <f>E20</f>
         <v>Residential Refrigeration - New</v>
       </c>
       <c r="E7" s="192" t="s">
@@ -35450,48 +35479,51 @@
         <v>0.85</v>
       </c>
       <c r="L7" s="341">
-        <f>L36/$V7/1000</f>
+        <f>L35/$Y7/1000</f>
         <v>0.432</v>
       </c>
       <c r="M7" s="341">
-        <f>M36/$V7/1000</f>
+        <f>M35/$Y7/1000</f>
         <v>0.432</v>
       </c>
       <c r="N7" s="341">
-        <f>N36/$V7/1000</f>
+        <f>N35/$Y7/1000</f>
         <v>0.432</v>
       </c>
       <c r="O7" s="341">
-        <f>O36/$V7/1000</f>
+        <f>O35/$Y7/1000</f>
         <v>0.432</v>
       </c>
-      <c r="P7" s="207"/>
-      <c r="Q7" s="207"/>
-      <c r="R7" s="347">
+      <c r="P7" s="341"/>
+      <c r="Q7" s="341"/>
+      <c r="R7" s="341"/>
+      <c r="S7" s="207"/>
+      <c r="T7" s="207"/>
+      <c r="U7" s="347">
         <v>1</v>
       </c>
-      <c r="S7" s="207">
+      <c r="V7" s="207">
         <v>2020</v>
       </c>
-      <c r="U7" s="282">
+      <c r="X7" s="282">
         <v>0.18</v>
       </c>
-      <c r="V7" s="282">
-        <f>1/U7</f>
+      <c r="Y7" s="282">
+        <f>1/X7</f>
         <v>5.5555555555555554</v>
       </c>
-      <c r="W7" s="282">
-        <f>L36/V7</f>
+      <c r="Z7" s="282">
+        <f>L35/Y7</f>
         <v>432</v>
       </c>
     </row>
-    <row r="8" spans="3:25" x14ac:dyDescent="0.2">
+    <row r="8" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C8" s="200" t="str">
-        <f>D22</f>
+        <f>D21</f>
         <v>R-RSDCK_ELC_N1</v>
       </c>
       <c r="D8" s="191" t="str">
-        <f>LEFT($E$22,20)&amp;"_"&amp;RIGHT(E8,3)&amp;" - New"</f>
+        <f>LEFT($E$21,20)&amp;"_"&amp;RIGHT(E8,3)&amp;" - New"</f>
         <v>Residential Cooking _ELC - New</v>
       </c>
       <c r="E8" s="191" t="s">
@@ -35516,48 +35548,55 @@
         <v>0.85</v>
       </c>
       <c r="L8" s="342">
-        <f>$W$8/1000</f>
+        <f>$Z$8/1000</f>
         <v>0.86975000000000002</v>
       </c>
       <c r="M8" s="342">
-        <f>$W$8/1000</f>
+        <f>$Z$8/1000</f>
         <v>0.86975000000000002</v>
       </c>
       <c r="N8" s="342">
-        <f>$W$8/1000</f>
+        <f>$Z$8/1000</f>
         <v>0.86975000000000002</v>
       </c>
       <c r="O8" s="342">
-        <f>$W$8/1000</f>
+        <f>$Z$8/1000</f>
         <v>0.86975000000000002</v>
       </c>
-      <c r="P8" s="208"/>
-      <c r="Q8" s="208"/>
-      <c r="R8" s="348">
+      <c r="P8" s="342"/>
+      <c r="Q8" s="342">
         <v>1</v>
       </c>
-      <c r="S8" s="208">
+      <c r="R8" s="501">
+        <v>5</v>
+      </c>
+      <c r="S8" s="208"/>
+      <c r="T8" s="208"/>
+      <c r="U8" s="348">
+        <v>1</v>
+      </c>
+      <c r="V8" s="208">
         <v>2020</v>
       </c>
-      <c r="U8" s="282">
+      <c r="X8" s="282">
         <v>3</v>
       </c>
-      <c r="V8" s="282">
-        <f>1/U8</f>
+      <c r="Y8" s="282">
+        <f>1/X8</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="W8" s="282">
-        <f>W9*1.42</f>
+      <c r="Z8" s="282">
+        <f>Z9*1.42</f>
         <v>869.75</v>
       </c>
     </row>
-    <row r="9" spans="3:25" x14ac:dyDescent="0.2">
+    <row r="9" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C9" s="200" t="str">
-        <f t="shared" ref="C9:D15" si="0">D23</f>
+        <f t="shared" ref="C9:D15" si="0">D22</f>
         <v>R-RSDCK_GAS_N1</v>
       </c>
       <c r="D9" s="192" t="str">
-        <f>LEFT($E$22,20)&amp;"_"&amp;RIGHT(E9,3)&amp;" - New"</f>
+        <f t="shared" ref="D9:D10" si="1">LEFT($E$21,20)&amp;"_"&amp;RIGHT(E9,3)&amp;" - New"</f>
         <v>Residential Cooking _GAS - New</v>
       </c>
       <c r="E9" s="192" t="s">
@@ -35582,48 +35621,57 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="L9" s="343">
-        <f>L38/$V9/1000</f>
+        <f t="shared" ref="L9:O13" si="2">L37/$Y9/1000</f>
         <v>0.61250000000000004</v>
       </c>
       <c r="M9" s="343">
-        <f>M38/$V9/1000</f>
+        <f t="shared" si="2"/>
         <v>0.61250000000000004</v>
       </c>
       <c r="N9" s="343">
-        <f>N38/$V9/1000</f>
+        <f t="shared" si="2"/>
         <v>0.61250000000000004</v>
       </c>
       <c r="O9" s="343">
-        <f>O38/$V9/1000</f>
+        <f t="shared" si="2"/>
         <v>0.61250000000000004</v>
       </c>
-      <c r="P9" s="209"/>
-      <c r="Q9" s="209"/>
-      <c r="R9" s="349">
+      <c r="P9" s="343">
+        <v>0.23</v>
+      </c>
+      <c r="Q9" s="343">
+        <v>0.4</v>
+      </c>
+      <c r="R9" s="502">
+        <v>5</v>
+      </c>
+      <c r="S9" s="209"/>
+      <c r="T9" s="209"/>
+      <c r="U9" s="349">
         <v>1</v>
       </c>
-      <c r="S9" s="209">
+      <c r="V9" s="209">
         <v>2020</v>
       </c>
-      <c r="U9" s="282">
+      <c r="X9" s="282">
         <v>3.5</v>
       </c>
-      <c r="V9" s="282">
-        <f t="shared" ref="V9:V13" si="1">1/U9</f>
+      <c r="Y9" s="282">
+        <f t="shared" ref="Y9:Y13" si="3">1/X9</f>
         <v>0.2857142857142857</v>
       </c>
-      <c r="W9" s="282">
-        <f>L38/V9</f>
+      <c r="Z9" s="282">
+        <f>L37/Y9</f>
         <v>612.5</v>
       </c>
     </row>
-    <row r="10" spans="3:25" x14ac:dyDescent="0.2">
+    <row r="10" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C10" s="200" t="str">
         <f t="shared" si="0"/>
         <v>R-RSDCK_LPG_N1</v>
       </c>
       <c r="D10" s="191" t="str">
-        <f>LEFT($E$22,20)&amp;"_"&amp;RIGHT(E10,3)&amp;" - New"</f>
+        <f t="shared" si="1"/>
         <v>Residential Cooking _LPG - New</v>
       </c>
       <c r="E10" s="191" t="s">
@@ -35648,42 +35696,51 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="L10" s="342">
-        <f>L39/$V10/1000</f>
+        <f t="shared" si="2"/>
         <v>0.61250000000000004</v>
       </c>
       <c r="M10" s="342">
-        <f>M39/$V10/1000</f>
+        <f t="shared" si="2"/>
         <v>0.61250000000000004</v>
       </c>
       <c r="N10" s="342">
-        <f>N39/$V10/1000</f>
+        <f t="shared" si="2"/>
         <v>0.61250000000000004</v>
       </c>
       <c r="O10" s="342">
-        <f>O39/$V10/1000</f>
+        <f t="shared" si="2"/>
         <v>0.61250000000000004</v>
       </c>
-      <c r="P10" s="208"/>
-      <c r="Q10" s="208"/>
-      <c r="R10" s="348">
+      <c r="P10" s="342">
+        <v>1.4E-2</v>
+      </c>
+      <c r="Q10" s="342">
+        <v>0.4</v>
+      </c>
+      <c r="R10" s="501">
+        <v>5</v>
+      </c>
+      <c r="S10" s="208"/>
+      <c r="T10" s="208"/>
+      <c r="U10" s="348">
         <v>1</v>
       </c>
-      <c r="S10" s="208">
+      <c r="V10" s="208">
         <v>2020</v>
       </c>
-      <c r="U10" s="282">
+      <c r="X10" s="282">
         <v>3.5</v>
       </c>
-      <c r="V10" s="282">
-        <f t="shared" si="1"/>
+      <c r="Y10" s="282">
+        <f t="shared" si="3"/>
         <v>0.2857142857142857</v>
       </c>
-      <c r="W10" s="282">
-        <f>L39/V10</f>
+      <c r="Z10" s="282">
+        <f>L38/Y10</f>
         <v>612.5</v>
       </c>
     </row>
-    <row r="11" spans="3:25" x14ac:dyDescent="0.2">
+    <row r="11" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C11" s="202" t="str">
         <f t="shared" si="0"/>
         <v>R-RSDCW_N1</v>
@@ -35714,42 +35771,45 @@
         <v>0.7</v>
       </c>
       <c r="L11" s="343">
-        <f>L40/$V11/1000</f>
+        <f t="shared" si="2"/>
         <v>0.55220000000000002</v>
       </c>
       <c r="M11" s="343">
-        <f>M40/$V11/1000</f>
+        <f t="shared" si="2"/>
         <v>0.55220000000000002</v>
       </c>
       <c r="N11" s="343">
-        <f>N40/$V11/1000</f>
+        <f t="shared" si="2"/>
         <v>0.55220000000000002</v>
       </c>
       <c r="O11" s="343">
-        <f>O40/$V11/1000</f>
+        <f t="shared" si="2"/>
         <v>0.55220000000000002</v>
       </c>
-      <c r="P11" s="209"/>
-      <c r="Q11" s="209"/>
-      <c r="R11" s="349">
+      <c r="P11" s="343"/>
+      <c r="Q11" s="343"/>
+      <c r="R11" s="343"/>
+      <c r="S11" s="209"/>
+      <c r="T11" s="209"/>
+      <c r="U11" s="349">
         <v>1</v>
       </c>
-      <c r="S11" s="209">
+      <c r="V11" s="209">
         <v>2020</v>
       </c>
-      <c r="U11" s="282">
+      <c r="X11" s="282">
         <v>2.2000000000000002</v>
       </c>
-      <c r="V11" s="282">
-        <f t="shared" si="1"/>
+      <c r="Y11" s="282">
+        <f t="shared" si="3"/>
         <v>0.45454545454545453</v>
       </c>
-      <c r="W11" s="282">
-        <f>L40/V11</f>
+      <c r="Z11" s="282">
+        <f>L39/Y11</f>
         <v>552.20000000000005</v>
       </c>
     </row>
-    <row r="12" spans="3:25" x14ac:dyDescent="0.2">
+    <row r="12" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C12" s="200" t="str">
         <f t="shared" si="0"/>
         <v>R-RSDCD_N1</v>
@@ -35780,42 +35840,45 @@
         <v>0.6</v>
       </c>
       <c r="L12" s="342">
-        <f>L41/$V12/1000</f>
+        <f t="shared" si="2"/>
         <v>0.53500000000000003</v>
       </c>
       <c r="M12" s="342">
-        <f>M41/$V12/1000</f>
+        <f t="shared" si="2"/>
         <v>0.53500000000000003</v>
       </c>
       <c r="N12" s="342">
-        <f>N41/$V12/1000</f>
+        <f t="shared" si="2"/>
         <v>0.53500000000000003</v>
       </c>
       <c r="O12" s="342">
-        <f>O41/$V12/1000</f>
+        <f t="shared" si="2"/>
         <v>0.53500000000000003</v>
       </c>
-      <c r="P12" s="208"/>
-      <c r="Q12" s="208"/>
-      <c r="R12" s="348">
+      <c r="P12" s="342"/>
+      <c r="Q12" s="342"/>
+      <c r="R12" s="342"/>
+      <c r="S12" s="208"/>
+      <c r="T12" s="208"/>
+      <c r="U12" s="348">
         <v>1</v>
       </c>
-      <c r="S12" s="208">
+      <c r="V12" s="208">
         <v>2020</v>
       </c>
-      <c r="U12" s="282">
+      <c r="X12" s="282">
         <v>2.5</v>
       </c>
-      <c r="V12" s="282">
-        <f t="shared" si="1"/>
+      <c r="Y12" s="282">
+        <f t="shared" si="3"/>
         <v>0.4</v>
       </c>
-      <c r="W12" s="282">
-        <f>L41/V12</f>
+      <c r="Z12" s="282">
+        <f>L40/Y12</f>
         <v>535</v>
       </c>
     </row>
-    <row r="13" spans="3:25" x14ac:dyDescent="0.2">
+    <row r="13" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C13" s="202" t="str">
         <f t="shared" si="0"/>
         <v>R-RSDDW_N1</v>
@@ -35846,42 +35909,45 @@
         <v>0.7</v>
       </c>
       <c r="L13" s="343">
-        <f>L42/$V13/1000</f>
+        <f t="shared" si="2"/>
         <v>0.42019999999999996</v>
       </c>
       <c r="M13" s="343">
-        <f>M42/$V13/1000</f>
+        <f t="shared" si="2"/>
         <v>0.42019999999999996</v>
       </c>
       <c r="N13" s="343">
-        <f>N42/$V13/1000</f>
+        <f t="shared" si="2"/>
         <v>0.42019999999999996</v>
       </c>
       <c r="O13" s="343">
-        <f>O42/$V13/1000</f>
+        <f t="shared" si="2"/>
         <v>0.42019999999999996</v>
       </c>
-      <c r="P13" s="209"/>
-      <c r="Q13" s="209"/>
-      <c r="R13" s="349">
+      <c r="P13" s="343"/>
+      <c r="Q13" s="343"/>
+      <c r="R13" s="343"/>
+      <c r="S13" s="209"/>
+      <c r="T13" s="209"/>
+      <c r="U13" s="349">
         <v>1</v>
       </c>
-      <c r="S13" s="209">
+      <c r="V13" s="209">
         <v>2020</v>
       </c>
-      <c r="U13" s="282">
+      <c r="X13" s="282">
         <v>2.2000000000000002</v>
       </c>
-      <c r="V13" s="282">
-        <f t="shared" si="1"/>
+      <c r="Y13" s="282">
+        <f t="shared" si="3"/>
         <v>0.45454545454545453</v>
       </c>
-      <c r="W13" s="282">
-        <f>L42/V13</f>
+      <c r="Z13" s="282">
+        <f>L41/Y13</f>
         <v>420.2</v>
       </c>
     </row>
-    <row r="14" spans="3:25" x14ac:dyDescent="0.2">
+    <row r="14" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C14" s="200" t="str">
         <f t="shared" si="0"/>
         <v>R-RSDOE_N1</v>
@@ -35912,31 +35978,34 @@
         <v>0.85</v>
       </c>
       <c r="L14" s="351">
-        <f>L43/$V7/1000</f>
+        <f>L42/$Y7/1000</f>
         <v>0.9</v>
       </c>
       <c r="M14" s="351">
-        <f>M43/$V7/1000</f>
+        <f>M42/$Y7/1000</f>
         <v>0.9</v>
       </c>
       <c r="N14" s="351">
-        <f>N43/$V7/1000</f>
+        <f>N42/$Y7/1000</f>
         <v>0.9</v>
       </c>
       <c r="O14" s="351">
-        <f>O43/$V7/1000</f>
+        <f>O42/$Y7/1000</f>
         <v>0.9</v>
       </c>
-      <c r="P14" s="208"/>
-      <c r="Q14" s="208"/>
-      <c r="R14" s="348">
+      <c r="P14" s="351"/>
+      <c r="Q14" s="351"/>
+      <c r="R14" s="351"/>
+      <c r="S14" s="208"/>
+      <c r="T14" s="208"/>
+      <c r="U14" s="348">
         <v>1</v>
       </c>
-      <c r="S14" s="208">
+      <c r="V14" s="208">
         <v>2020</v>
       </c>
     </row>
-    <row r="15" spans="3:25" x14ac:dyDescent="0.2">
+    <row r="15" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C15" s="202" t="str">
         <f t="shared" si="0"/>
         <v>R-RSDOA_N1</v>
@@ -35967,123 +36036,130 @@
         <v>0.85</v>
       </c>
       <c r="L15" s="352">
-        <f>L44/$V7/1000</f>
+        <f>L43/$Y7/1000</f>
         <v>0.9</v>
       </c>
       <c r="M15" s="352">
-        <f>M44/$V7/1000</f>
+        <f>M43/$Y7/1000</f>
         <v>0.9</v>
       </c>
       <c r="N15" s="352">
-        <f>N44/$V7/1000</f>
+        <f>N43/$Y7/1000</f>
         <v>0.9</v>
       </c>
       <c r="O15" s="352">
-        <f>O44/$V7/1000</f>
+        <f>O43/$Y7/1000</f>
         <v>0.9</v>
       </c>
-      <c r="P15" s="210"/>
-      <c r="Q15" s="210"/>
-      <c r="R15" s="350">
+      <c r="P15" s="352"/>
+      <c r="Q15" s="352"/>
+      <c r="R15" s="352"/>
+      <c r="S15" s="210"/>
+      <c r="T15" s="210"/>
+      <c r="U15" s="350">
         <v>1</v>
       </c>
-      <c r="S15" s="210">
+      <c r="V15" s="210">
         <v>2020</v>
       </c>
-      <c r="U15" s="189" t="s">
+      <c r="X15" s="189" t="s">
         <v>627</v>
       </c>
-      <c r="V15" s="281" t="s">
+      <c r="Y15" s="281" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="16" spans="3:25" x14ac:dyDescent="0.2">
-      <c r="C16" s="538"/>
-      <c r="D16" s="538"/>
-      <c r="E16" s="538"/>
-      <c r="F16" s="538"/>
-      <c r="G16" s="538"/>
-      <c r="H16" s="538"/>
-      <c r="I16" s="538"/>
-      <c r="J16" s="538"/>
-      <c r="K16" s="538"/>
-      <c r="L16" s="539"/>
-      <c r="M16" s="539"/>
-      <c r="N16" s="539"/>
-      <c r="O16" s="539"/>
-      <c r="P16" s="539"/>
-      <c r="Q16" s="539"/>
-      <c r="R16" s="539"/>
-      <c r="S16" s="538"/>
-      <c r="T16" s="538"/>
-      <c r="U16" s="540"/>
-      <c r="V16" s="538"/>
-      <c r="X16" s="189"/>
-      <c r="Y16" s="281"/>
-    </row>
-    <row r="17" spans="3:22" x14ac:dyDescent="0.2">
-      <c r="R17" s="189" t="s">
+    <row r="16" spans="3:26" x14ac:dyDescent="0.2">
+      <c r="R16" s="189" t="s">
         <v>628</v>
       </c>
-      <c r="S17" s="5" t="s">
+      <c r="S16" s="5" t="s">
         <v>629</v>
       </c>
     </row>
+    <row r="18" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="C18" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="R18" s="529" t="s">
+        <v>669</v>
+      </c>
+      <c r="S18" s="529"/>
+      <c r="U18" s="5" t="s">
+        <v>869</v>
+      </c>
+      <c r="V18" s="5" t="s">
+        <v>1033</v>
+      </c>
+    </row>
     <row r="19" spans="3:22" x14ac:dyDescent="0.2">
-      <c r="C19" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="R19" s="525" t="s">
-        <v>669</v>
-      </c>
-      <c r="S19" s="525"/>
-      <c r="U19" s="5" t="s">
-        <v>869</v>
-      </c>
+      <c r="C19" s="193" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="194" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="194" t="s">
+        <v>29</v>
+      </c>
+      <c r="F19" s="194" t="s">
+        <v>35</v>
+      </c>
+      <c r="G19" s="194" t="s">
+        <v>36</v>
+      </c>
+      <c r="H19" s="194" t="s">
+        <v>379</v>
+      </c>
+      <c r="I19" s="194" t="s">
+        <v>37</v>
+      </c>
+      <c r="J19" s="195" t="s">
+        <v>301</v>
+      </c>
+      <c r="R19" s="529"/>
+      <c r="S19" s="529"/>
       <c r="V19" s="5" t="s">
-        <v>1030</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="20" spans="3:22" x14ac:dyDescent="0.2">
-      <c r="C20" s="193" t="s">
-        <v>34</v>
-      </c>
-      <c r="D20" s="194" t="s">
-        <v>28</v>
-      </c>
-      <c r="E20" s="194" t="s">
-        <v>29</v>
-      </c>
-      <c r="F20" s="194" t="s">
-        <v>35</v>
-      </c>
-      <c r="G20" s="194" t="s">
-        <v>36</v>
-      </c>
-      <c r="H20" s="194" t="s">
-        <v>379</v>
-      </c>
-      <c r="I20" s="194" t="s">
-        <v>37</v>
-      </c>
-      <c r="J20" s="195" t="s">
-        <v>301</v>
-      </c>
-      <c r="R20" s="525"/>
-      <c r="S20" s="525"/>
+      <c r="C20" s="168" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="169" t="s">
+        <v>757</v>
+      </c>
+      <c r="E20" s="169" t="s">
+        <v>416</v>
+      </c>
+      <c r="F20" s="169" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20" s="169" t="s">
+        <v>363</v>
+      </c>
+      <c r="H20" s="169"/>
+      <c r="I20" s="169"/>
+      <c r="J20" s="170" t="s">
+        <v>417</v>
+      </c>
+      <c r="R20" s="529"/>
+      <c r="S20" s="529"/>
       <c r="V20" s="5" t="s">
-        <v>1031</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="21" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C21" s="168" t="s">
         <v>38</v>
       </c>
-      <c r="D21" s="169" t="s">
-        <v>757</v>
+      <c r="D21" s="169" t="str">
+        <f>_xlfn.TEXTJOIN("_",TRUE,"R-RSDCK",RIGHT(E8,3),"N1")</f>
+        <v>R-RSDCK_ELC_N1</v>
       </c>
       <c r="E21" s="169" t="s">
-        <v>416</v>
+        <v>1001</v>
       </c>
       <c r="F21" s="169" t="s">
         <v>16</v>
@@ -36096,22 +36172,19 @@
       <c r="J21" s="170" t="s">
         <v>417</v>
       </c>
-      <c r="R21" s="525"/>
-      <c r="S21" s="525"/>
-      <c r="V21" s="5" t="s">
-        <v>1032</v>
-      </c>
+      <c r="R21" s="529"/>
+      <c r="S21" s="529"/>
     </row>
     <row r="22" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C22" s="168" t="s">
         <v>38</v>
       </c>
       <c r="D22" s="169" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"R-RSDCK",RIGHT(E8,3),"N1")</f>
-        <v>R-RSDCK_ELC_N1</v>
+        <f t="shared" ref="D22:D23" si="4">_xlfn.TEXTJOIN("_",TRUE,"R-RSDCK",RIGHT(E9,3),"N1")</f>
+        <v>R-RSDCK_GAS_N1</v>
       </c>
       <c r="E22" s="169" t="s">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="F22" s="169" t="s">
         <v>16</v>
@@ -36124,19 +36197,19 @@
       <c r="J22" s="170" t="s">
         <v>417</v>
       </c>
-      <c r="R22" s="525"/>
-      <c r="S22" s="525"/>
+      <c r="R22" s="529"/>
+      <c r="S22" s="529"/>
     </row>
     <row r="23" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C23" s="168" t="s">
         <v>38</v>
       </c>
       <c r="D23" s="169" t="str">
-        <f t="shared" ref="D23:D24" si="2">_xlfn.TEXTJOIN("_",TRUE,"R-RSDCK",RIGHT(E9,3),"N1")</f>
-        <v>R-RSDCK_GAS_N1</v>
+        <f t="shared" si="4"/>
+        <v>R-RSDCK_LPG_N1</v>
       </c>
       <c r="E23" s="169" t="s">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="F23" s="169" t="s">
         <v>16</v>
@@ -36149,19 +36222,16 @@
       <c r="J23" s="170" t="s">
         <v>417</v>
       </c>
-      <c r="R23" s="525"/>
-      <c r="S23" s="525"/>
     </row>
     <row r="24" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C24" s="168" t="s">
         <v>38</v>
       </c>
-      <c r="D24" s="169" t="str">
-        <f t="shared" si="2"/>
-        <v>R-RSDCK_LPG_N1</v>
+      <c r="D24" s="169" t="s">
+        <v>759</v>
       </c>
       <c r="E24" s="169" t="s">
-        <v>1003</v>
+        <v>419</v>
       </c>
       <c r="F24" s="169" t="s">
         <v>16</v>
@@ -36180,10 +36250,10 @@
         <v>38</v>
       </c>
       <c r="D25" s="169" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="E25" s="169" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="F25" s="169" t="s">
         <v>16</v>
@@ -36202,10 +36272,10 @@
         <v>38</v>
       </c>
       <c r="D26" s="169" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="E26" s="169" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="F26" s="169" t="s">
         <v>16</v>
@@ -36218,16 +36288,17 @@
       <c r="J26" s="170" t="s">
         <v>417</v>
       </c>
+      <c r="Q26" s="189"/>
     </row>
     <row r="27" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C27" s="168" t="s">
         <v>38</v>
       </c>
       <c r="D27" s="169" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="E27" s="169" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="F27" s="169" t="s">
         <v>16</v>
@@ -36240,341 +36311,318 @@
       <c r="J27" s="170" t="s">
         <v>417</v>
       </c>
-      <c r="Q27" s="189"/>
     </row>
     <row r="28" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C28" s="168" t="s">
         <v>38</v>
       </c>
-      <c r="D28" s="169" t="s">
-        <v>762</v>
-      </c>
-      <c r="E28" s="169" t="s">
-        <v>422</v>
-      </c>
-      <c r="F28" s="169" t="s">
+      <c r="D28" s="171" t="s">
+        <v>763</v>
+      </c>
+      <c r="E28" s="171" t="s">
+        <v>423</v>
+      </c>
+      <c r="F28" s="171" t="s">
         <v>16</v>
       </c>
       <c r="G28" s="169" t="s">
         <v>363</v>
       </c>
-      <c r="H28" s="169"/>
-      <c r="I28" s="169"/>
-      <c r="J28" s="170" t="s">
+      <c r="H28" s="171"/>
+      <c r="I28" s="171"/>
+      <c r="J28" s="172" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="29" spans="3:22" x14ac:dyDescent="0.2">
-      <c r="C29" s="168" t="s">
-        <v>38</v>
-      </c>
-      <c r="D29" s="171" t="s">
-        <v>763</v>
-      </c>
-      <c r="E29" s="171" t="s">
-        <v>423</v>
-      </c>
-      <c r="F29" s="171" t="s">
-        <v>16</v>
-      </c>
-      <c r="G29" s="169" t="s">
-        <v>363</v>
-      </c>
-      <c r="H29" s="171"/>
-      <c r="I29" s="171"/>
-      <c r="J29" s="172" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="33" spans="8:15" ht="30" x14ac:dyDescent="0.2">
+    <row r="32" spans="3:22" ht="30" x14ac:dyDescent="0.2">
+      <c r="H32" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="J32" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K32" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L32" s="63" t="s">
+        <v>668</v>
+      </c>
+      <c r="M32" s="63" t="s">
+        <v>324</v>
+      </c>
+      <c r="N32" s="63" t="s">
+        <v>325</v>
+      </c>
+      <c r="O32" s="63" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="33" spans="8:15" x14ac:dyDescent="0.2">
       <c r="H33" s="5" t="s">
-        <v>28</v>
+        <v>315</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>30</v>
+        <v>316</v>
       </c>
       <c r="K33" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="L33" s="63" t="s">
-        <v>668</v>
-      </c>
-      <c r="M33" s="63" t="s">
-        <v>324</v>
-      </c>
-      <c r="N33" s="63" t="s">
-        <v>325</v>
-      </c>
-      <c r="O33" s="63" t="s">
-        <v>326</v>
-      </c>
+        <v>317</v>
+      </c>
+      <c r="L33" s="526" t="s">
+        <v>322</v>
+      </c>
+      <c r="M33" s="527"/>
+      <c r="N33" s="527"/>
+      <c r="O33" s="528"/>
     </row>
     <row r="34" spans="8:15" x14ac:dyDescent="0.2">
       <c r="H34" s="5" t="s">
-        <v>315</v>
-      </c>
-      <c r="I34" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="J34" s="5" t="s">
-        <v>316</v>
-      </c>
-      <c r="K34" s="5" t="s">
-        <v>317</v>
-      </c>
-      <c r="L34" s="522" t="s">
-        <v>322</v>
-      </c>
-      <c r="M34" s="523"/>
-      <c r="N34" s="523"/>
-      <c r="O34" s="524"/>
-    </row>
-    <row r="35" spans="8:15" x14ac:dyDescent="0.2">
+        <v>376</v>
+      </c>
+      <c r="L34" s="520" t="s">
+        <v>328</v>
+      </c>
+      <c r="M34" s="522"/>
+      <c r="N34" s="522"/>
+      <c r="O34" s="521"/>
+    </row>
+    <row r="35" spans="8:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H35" s="5" t="s">
-        <v>376</v>
-      </c>
-      <c r="L35" s="516" t="s">
-        <v>328</v>
-      </c>
-      <c r="M35" s="518"/>
-      <c r="N35" s="518"/>
-      <c r="O35" s="517"/>
-    </row>
-    <row r="36" spans="8:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>757</v>
+      </c>
+      <c r="I35" s="5" t="s">
+        <v>416</v>
+      </c>
+      <c r="J35" s="5" t="s">
+        <v>408</v>
+      </c>
+      <c r="K35" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="L35" s="197">
+        <v>2400</v>
+      </c>
+      <c r="M35" s="197">
+        <v>2400</v>
+      </c>
+      <c r="N35" s="197">
+        <v>2400</v>
+      </c>
+      <c r="O35" s="197">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="36" spans="8:15" x14ac:dyDescent="0.2">
       <c r="H36" s="5" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="J36" s="5" t="s">
         <v>408</v>
       </c>
       <c r="K36" s="5" t="s">
-        <v>409</v>
-      </c>
-      <c r="L36" s="197">
-        <v>2400</v>
-      </c>
-      <c r="M36" s="197">
-        <v>2400</v>
-      </c>
-      <c r="N36" s="197">
-        <v>2400</v>
-      </c>
-      <c r="O36" s="197">
-        <v>2400</v>
+        <v>410</v>
+      </c>
+      <c r="L36" s="200">
+        <v>175</v>
+      </c>
+      <c r="M36" s="200">
+        <v>175</v>
+      </c>
+      <c r="N36" s="200">
+        <v>175</v>
+      </c>
+      <c r="O36" s="200">
+        <v>175</v>
       </c>
     </row>
     <row r="37" spans="8:15" x14ac:dyDescent="0.2">
-      <c r="H37" s="5" t="s">
-        <v>758</v>
-      </c>
-      <c r="I37" s="5" t="s">
-        <v>418</v>
-      </c>
       <c r="J37" s="5" t="s">
-        <v>408</v>
-      </c>
-      <c r="K37" s="5" t="s">
-        <v>410</v>
-      </c>
-      <c r="L37" s="200">
+        <v>733</v>
+      </c>
+      <c r="L37" s="202">
         <v>175</v>
       </c>
-      <c r="M37" s="200">
+      <c r="M37" s="202">
         <v>175</v>
       </c>
-      <c r="N37" s="200">
+      <c r="N37" s="202">
         <v>175</v>
       </c>
-      <c r="O37" s="200">
+      <c r="O37" s="202">
         <v>175</v>
       </c>
     </row>
     <row r="38" spans="8:15" x14ac:dyDescent="0.2">
       <c r="J38" s="5" t="s">
-        <v>733</v>
-      </c>
-      <c r="L38" s="202">
+        <v>729</v>
+      </c>
+      <c r="L38" s="200">
         <v>175</v>
       </c>
-      <c r="M38" s="202">
+      <c r="M38" s="200">
         <v>175</v>
       </c>
-      <c r="N38" s="202">
+      <c r="N38" s="200">
         <v>175</v>
       </c>
-      <c r="O38" s="202">
+      <c r="O38" s="200">
         <v>175</v>
       </c>
     </row>
     <row r="39" spans="8:15" x14ac:dyDescent="0.2">
+      <c r="H39" s="5" t="s">
+        <v>759</v>
+      </c>
+      <c r="I39" s="5" t="s">
+        <v>419</v>
+      </c>
       <c r="J39" s="5" t="s">
-        <v>729</v>
-      </c>
-      <c r="L39" s="200">
-        <v>175</v>
-      </c>
-      <c r="M39" s="200">
-        <v>175</v>
-      </c>
-      <c r="N39" s="200">
-        <v>175</v>
-      </c>
-      <c r="O39" s="200">
-        <v>175</v>
+        <v>408</v>
+      </c>
+      <c r="K39" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="L39" s="202">
+        <v>251</v>
+      </c>
+      <c r="M39" s="202">
+        <v>251</v>
+      </c>
+      <c r="N39" s="202">
+        <v>251</v>
+      </c>
+      <c r="O39" s="202">
+        <v>251</v>
       </c>
     </row>
     <row r="40" spans="8:15" x14ac:dyDescent="0.2">
       <c r="H40" s="5" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="J40" s="5" t="s">
         <v>408</v>
       </c>
       <c r="K40" s="5" t="s">
-        <v>411</v>
-      </c>
-      <c r="L40" s="202">
-        <v>251</v>
-      </c>
-      <c r="M40" s="202">
-        <v>251</v>
-      </c>
-      <c r="N40" s="202">
-        <v>251</v>
-      </c>
-      <c r="O40" s="202">
-        <v>251</v>
+        <v>412</v>
+      </c>
+      <c r="L40" s="200">
+        <v>214</v>
+      </c>
+      <c r="M40" s="200">
+        <v>214</v>
+      </c>
+      <c r="N40" s="200">
+        <v>214</v>
+      </c>
+      <c r="O40" s="200">
+        <v>214</v>
       </c>
     </row>
     <row r="41" spans="8:15" x14ac:dyDescent="0.2">
       <c r="H41" s="5" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="I41" s="5" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="J41" s="5" t="s">
         <v>408</v>
       </c>
       <c r="K41" s="5" t="s">
-        <v>412</v>
-      </c>
-      <c r="L41" s="200">
-        <v>214</v>
-      </c>
-      <c r="M41" s="200">
-        <v>214</v>
-      </c>
-      <c r="N41" s="200">
-        <v>214</v>
-      </c>
-      <c r="O41" s="200">
-        <v>214</v>
+        <v>413</v>
+      </c>
+      <c r="L41" s="202">
+        <v>191</v>
+      </c>
+      <c r="M41" s="202">
+        <v>191</v>
+      </c>
+      <c r="N41" s="202">
+        <v>191</v>
+      </c>
+      <c r="O41" s="202">
+        <v>191</v>
       </c>
     </row>
     <row r="42" spans="8:15" x14ac:dyDescent="0.2">
       <c r="H42" s="5" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="I42" s="5" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="J42" s="5" t="s">
         <v>408</v>
       </c>
       <c r="K42" s="5" t="s">
-        <v>413</v>
-      </c>
-      <c r="L42" s="202">
-        <v>191</v>
-      </c>
-      <c r="M42" s="202">
-        <v>191</v>
-      </c>
-      <c r="N42" s="202">
-        <v>191</v>
-      </c>
-      <c r="O42" s="202">
-        <v>191</v>
+        <v>414</v>
+      </c>
+      <c r="L42" s="200">
+        <v>5000</v>
+      </c>
+      <c r="M42" s="200">
+        <v>5000</v>
+      </c>
+      <c r="N42" s="200">
+        <v>5000</v>
+      </c>
+      <c r="O42" s="200">
+        <v>5000</v>
       </c>
     </row>
     <row r="43" spans="8:15" x14ac:dyDescent="0.2">
       <c r="H43" s="5" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="I43" s="5" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="J43" s="5" t="s">
         <v>408</v>
       </c>
       <c r="K43" s="5" t="s">
-        <v>414</v>
-      </c>
-      <c r="L43" s="200">
+        <v>415</v>
+      </c>
+      <c r="L43" s="204">
         <v>5000</v>
       </c>
-      <c r="M43" s="200">
+      <c r="M43" s="204">
         <v>5000</v>
       </c>
-      <c r="N43" s="200">
+      <c r="N43" s="204">
         <v>5000</v>
       </c>
-      <c r="O43" s="200">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="44" spans="8:15" x14ac:dyDescent="0.2">
-      <c r="H44" s="5" t="s">
-        <v>763</v>
-      </c>
-      <c r="I44" s="5" t="s">
-        <v>423</v>
-      </c>
-      <c r="J44" s="5" t="s">
-        <v>408</v>
-      </c>
-      <c r="K44" s="5" t="s">
-        <v>415</v>
-      </c>
-      <c r="L44" s="204">
-        <v>5000</v>
-      </c>
-      <c r="M44" s="204">
-        <v>5000</v>
-      </c>
-      <c r="N44" s="204">
-        <v>5000</v>
-      </c>
-      <c r="O44" s="204">
+      <c r="O43" s="204">
         <v>5000</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="L35:O35"/>
     <mergeCell ref="L34:O34"/>
-    <mergeCell ref="R19:S23"/>
+    <mergeCell ref="L33:O33"/>
+    <mergeCell ref="R18:S22"/>
     <mergeCell ref="L5:O5"/>
     <mergeCell ref="L6:O6"/>
   </mergeCells>
-  <conditionalFormatting sqref="I20:I29">
+  <conditionalFormatting sqref="I19:I28">
     <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="between">
       <formula>0.000000001</formula>
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="V15" r:id="rId1" xr:uid="{6F790111-B362-4390-963B-D2AEAFDB26BD}"/>
+    <hyperlink ref="Y15" r:id="rId1" xr:uid="{6F790111-B362-4390-963B-D2AEAFDB26BD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -36683,16 +36731,16 @@
       <c r="G4" s="173" t="s">
         <v>321</v>
       </c>
-      <c r="H4" s="519" t="s">
+      <c r="H4" s="523" t="s">
         <v>110</v>
       </c>
-      <c r="I4" s="520"/>
-      <c r="J4" s="521"/>
-      <c r="K4" s="522" t="s">
+      <c r="I4" s="524"/>
+      <c r="J4" s="525"/>
+      <c r="K4" s="526" t="s">
         <v>322</v>
       </c>
-      <c r="L4" s="523"/>
-      <c r="M4" s="524"/>
+      <c r="L4" s="527"/>
+      <c r="M4" s="528"/>
       <c r="N4" s="106"/>
       <c r="O4" s="106" t="s">
         <v>323</v>
@@ -36715,46 +36763,46 @@
       <c r="G5" s="466" t="s">
         <v>302</v>
       </c>
-      <c r="H5" s="529" t="s">
+      <c r="H5" s="533" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="530"/>
-      <c r="J5" s="531"/>
-      <c r="K5" s="529" t="s">
+      <c r="I5" s="534"/>
+      <c r="J5" s="535"/>
+      <c r="K5" s="533" t="s">
         <v>765</v>
       </c>
-      <c r="L5" s="530"/>
-      <c r="M5" s="531"/>
-      <c r="N5" s="467" t="s">
+      <c r="L5" s="534"/>
+      <c r="M5" s="535"/>
+      <c r="N5" s="469" t="s">
         <v>329</v>
       </c>
-      <c r="O5" s="467" t="s">
+      <c r="O5" s="469" t="s">
         <v>45</v>
       </c>
-      <c r="P5" s="468" t="s">
+      <c r="P5" s="470" t="s">
         <v>764</v>
       </c>
-      <c r="Q5" s="467" t="s">
+      <c r="Q5" s="469" t="s">
         <v>331</v>
       </c>
       <c r="AA5" s="281"/>
-      <c r="AB5" s="526" t="s">
+      <c r="AB5" s="530" t="s">
         <v>1021</v>
       </c>
-      <c r="AC5" s="526"/>
-      <c r="AD5" s="469"/>
-      <c r="AE5" s="527" t="s">
+      <c r="AC5" s="530"/>
+      <c r="AD5" s="471"/>
+      <c r="AE5" s="531" t="s">
         <v>110</v>
       </c>
-      <c r="AF5" s="527"/>
-      <c r="AG5" s="527" t="s">
+      <c r="AF5" s="531"/>
+      <c r="AG5" s="531" t="s">
         <v>1022</v>
       </c>
-      <c r="AH5" s="527"/>
-      <c r="AI5" s="528" t="s">
+      <c r="AH5" s="531"/>
+      <c r="AI5" s="532" t="s">
         <v>1023</v>
       </c>
-      <c r="AJ5" s="528"/>
+      <c r="AJ5" s="532"/>
     </row>
     <row r="6" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C6" s="197" t="str">
@@ -36765,35 +36813,35 @@
         <f t="shared" si="0"/>
         <v>Residential Lighting Apartment New</v>
       </c>
-      <c r="E6" s="470" t="s">
+      <c r="E6" s="472" t="s">
         <v>408</v>
       </c>
       <c r="F6" s="199" t="s">
         <v>373</v>
       </c>
-      <c r="G6" s="471">
+      <c r="G6" s="473">
         <v>10</v>
       </c>
-      <c r="H6" s="472">
+      <c r="H6" s="474">
         <v>0.4</v>
       </c>
-      <c r="I6" s="473">
+      <c r="I6" s="475">
         <f>H6*(AC9/AB9)</f>
         <v>0.54333333333333333</v>
       </c>
-      <c r="J6" s="474">
+      <c r="J6" s="476">
         <f>H6*(AD9/AC9)</f>
         <v>0.73128834355828232</v>
       </c>
-      <c r="K6" s="475">
+      <c r="K6" s="477">
         <f t="shared" ref="K6:L11" si="1">L29/1000*$X6/1000</f>
         <v>1.1375E-2</v>
       </c>
-      <c r="L6" s="476">
+      <c r="L6" s="478">
         <f t="shared" si="1"/>
         <v>1.1375E-2</v>
       </c>
-      <c r="M6" s="477">
+      <c r="M6" s="479">
         <f t="shared" ref="M6:M11" si="2">O29/1000*$X6/1000</f>
         <v>1.1375E-2</v>
       </c>
@@ -36857,19 +36905,19 @@
       <c r="F7" s="201" t="s">
         <v>374</v>
       </c>
-      <c r="G7" s="478">
+      <c r="G7" s="480">
         <v>15</v>
       </c>
-      <c r="H7" s="479">
+      <c r="H7" s="481">
         <v>0.6</v>
       </c>
       <c r="I7" s="342">
         <v>0.6</v>
       </c>
-      <c r="J7" s="480">
+      <c r="J7" s="482">
         <v>0.6</v>
       </c>
-      <c r="K7" s="481">
+      <c r="K7" s="483">
         <f t="shared" si="1"/>
         <v>0.15</v>
       </c>
@@ -36877,7 +36925,7 @@
         <f t="shared" si="1"/>
         <v>0.15</v>
       </c>
-      <c r="M7" s="482">
+      <c r="M7" s="484">
         <f t="shared" si="2"/>
         <v>0.15</v>
       </c>
@@ -36904,22 +36952,22 @@
       <c r="AC7" s="5">
         <v>17</v>
       </c>
-      <c r="AE7" s="483">
+      <c r="AE7" s="485">
         <f>AB7/683</f>
         <v>2.4890190336749635E-2</v>
       </c>
-      <c r="AF7" s="483">
+      <c r="AF7" s="485">
         <f>AC7/683</f>
         <v>2.4890190336749635E-2</v>
       </c>
-      <c r="AG7" s="484">
+      <c r="AG7" s="486">
         <v>0.03</v>
       </c>
-      <c r="AI7" s="485">
+      <c r="AI7" s="487">
         <f t="shared" ref="AI7:AJ10" si="3">AE7*AG7</f>
         <v>7.4670571010248903E-4</v>
       </c>
-      <c r="AJ7" s="485">
+      <c r="AJ7" s="487">
         <f>AF7*AH7</f>
         <v>0</v>
       </c>
@@ -36933,27 +36981,27 @@
         <f t="shared" si="0"/>
         <v>Residential Lighting Attached New</v>
       </c>
-      <c r="E8" s="470" t="s">
+      <c r="E8" s="472" t="s">
         <v>408</v>
       </c>
       <c r="F8" s="203" t="s">
         <v>397</v>
       </c>
-      <c r="G8" s="486">
+      <c r="G8" s="488">
         <v>10</v>
       </c>
-      <c r="H8" s="487">
+      <c r="H8" s="489">
         <v>0.4</v>
       </c>
       <c r="I8" s="341">
         <f>H8*(AC9/AB9)</f>
         <v>0.54333333333333333</v>
       </c>
-      <c r="J8" s="488">
+      <c r="J8" s="490">
         <f>H6*(AD9/AC9)</f>
         <v>0.73128834355828232</v>
       </c>
-      <c r="K8" s="489">
+      <c r="K8" s="491">
         <f t="shared" si="1"/>
         <v>1.1375E-2</v>
       </c>
@@ -36961,7 +37009,7 @@
         <f t="shared" si="1"/>
         <v>1.1375E-2</v>
       </c>
-      <c r="M8" s="490">
+      <c r="M8" s="492">
         <f t="shared" si="2"/>
         <v>1.1375E-2</v>
       </c>
@@ -36988,25 +37036,25 @@
       <c r="AC8" s="5">
         <v>24</v>
       </c>
-      <c r="AE8" s="483">
+      <c r="AE8" s="485">
         <f t="shared" ref="AE8:AF10" si="4">AB8/683</f>
         <v>3.5139092240117131E-2</v>
       </c>
-      <c r="AF8" s="483">
+      <c r="AF8" s="485">
         <f t="shared" si="4"/>
         <v>3.5139092240117131E-2</v>
       </c>
-      <c r="AG8" s="484">
+      <c r="AG8" s="486">
         <v>0.05</v>
       </c>
-      <c r="AH8" s="484">
+      <c r="AH8" s="486">
         <v>0.01</v>
       </c>
-      <c r="AI8" s="485">
+      <c r="AI8" s="487">
         <f t="shared" si="3"/>
         <v>1.7569546120058566E-3</v>
       </c>
-      <c r="AJ8" s="485">
+      <c r="AJ8" s="487">
         <f t="shared" si="3"/>
         <v>3.5139092240117132E-4</v>
       </c>
@@ -37026,19 +37074,19 @@
       <c r="F9" s="201" t="s">
         <v>398</v>
       </c>
-      <c r="G9" s="478">
+      <c r="G9" s="480">
         <v>15</v>
       </c>
-      <c r="H9" s="479">
+      <c r="H9" s="481">
         <v>0.6</v>
       </c>
       <c r="I9" s="342">
         <v>0.6</v>
       </c>
-      <c r="J9" s="480">
+      <c r="J9" s="482">
         <v>0.6</v>
       </c>
-      <c r="K9" s="481">
+      <c r="K9" s="483">
         <f t="shared" si="1"/>
         <v>0.15</v>
       </c>
@@ -37046,7 +37094,7 @@
         <f t="shared" si="1"/>
         <v>0.15</v>
       </c>
-      <c r="M9" s="482">
+      <c r="M9" s="484">
         <f t="shared" si="2"/>
         <v>0.15</v>
       </c>
@@ -37073,25 +37121,25 @@
       <c r="AD9" s="5">
         <v>298</v>
       </c>
-      <c r="AE9" s="483">
+      <c r="AE9" s="485">
         <f t="shared" si="4"/>
         <v>0.17569546120058566</v>
       </c>
-      <c r="AF9" s="483">
+      <c r="AF9" s="485">
         <f t="shared" si="4"/>
         <v>0.23865300146412885</v>
       </c>
-      <c r="AG9" s="484">
+      <c r="AG9" s="486">
         <v>0.46</v>
       </c>
-      <c r="AH9" s="484">
+      <c r="AH9" s="486">
         <v>0.87</v>
       </c>
-      <c r="AI9" s="485">
+      <c r="AI9" s="487">
         <f>AE9*AG9</f>
         <v>8.0819912152269399E-2</v>
       </c>
-      <c r="AJ9" s="485">
+      <c r="AJ9" s="487">
         <f t="shared" si="3"/>
         <v>0.2076281112737921</v>
       </c>
@@ -37105,27 +37153,27 @@
         <f t="shared" si="0"/>
         <v>Residential Lighting Detached New</v>
       </c>
-      <c r="E10" s="470" t="s">
+      <c r="E10" s="472" t="s">
         <v>408</v>
       </c>
       <c r="F10" s="203" t="s">
         <v>405</v>
       </c>
-      <c r="G10" s="486">
+      <c r="G10" s="488">
         <v>10</v>
       </c>
-      <c r="H10" s="487">
+      <c r="H10" s="489">
         <v>0.4</v>
       </c>
       <c r="I10" s="341">
         <f>H10*(AC9/AB9)</f>
         <v>0.54333333333333333</v>
       </c>
-      <c r="J10" s="488">
+      <c r="J10" s="490">
         <f>H10*(AD9/AC9)</f>
         <v>0.73128834355828232</v>
       </c>
-      <c r="K10" s="489">
+      <c r="K10" s="491">
         <f t="shared" si="1"/>
         <v>1.1375E-2</v>
       </c>
@@ -37133,7 +37181,7 @@
         <f t="shared" si="1"/>
         <v>1.1375E-2</v>
       </c>
-      <c r="M10" s="490">
+      <c r="M10" s="492">
         <f t="shared" si="2"/>
         <v>1.1375E-2</v>
       </c>
@@ -37157,25 +37205,25 @@
       <c r="AC10" s="5">
         <v>100</v>
       </c>
-      <c r="AE10" s="483">
+      <c r="AE10" s="485">
         <f t="shared" si="4"/>
         <v>0.14641288433382138</v>
       </c>
-      <c r="AF10" s="483">
+      <c r="AF10" s="485">
         <f t="shared" si="4"/>
         <v>0.14641288433382138</v>
       </c>
-      <c r="AG10" s="484">
+      <c r="AG10" s="486">
         <v>0.46</v>
       </c>
-      <c r="AH10" s="484">
+      <c r="AH10" s="486">
         <v>0.12</v>
       </c>
-      <c r="AI10" s="485">
+      <c r="AI10" s="487">
         <f>AE10*AG10</f>
         <v>6.7349926793557835E-2</v>
       </c>
-      <c r="AJ10" s="485">
+      <c r="AJ10" s="487">
         <f t="shared" si="3"/>
         <v>1.7569546120058566E-2</v>
       </c>
@@ -37195,27 +37243,27 @@
       <c r="F11" s="201" t="s">
         <v>406</v>
       </c>
-      <c r="G11" s="491">
+      <c r="G11" s="493">
         <v>15</v>
       </c>
-      <c r="H11" s="492">
+      <c r="H11" s="494">
         <v>0.6</v>
       </c>
-      <c r="I11" s="493">
+      <c r="I11" s="495">
         <v>0.6</v>
       </c>
-      <c r="J11" s="494">
+      <c r="J11" s="496">
         <v>0.6</v>
       </c>
-      <c r="K11" s="495">
+      <c r="K11" s="497">
         <f t="shared" si="1"/>
         <v>0.15</v>
       </c>
-      <c r="L11" s="496">
+      <c r="L11" s="498">
         <f t="shared" si="1"/>
         <v>0.15</v>
       </c>
-      <c r="M11" s="497">
+      <c r="M11" s="499">
         <f t="shared" si="2"/>
         <v>0.15</v>
       </c>
@@ -37236,11 +37284,11 @@
       <c r="AB11" s="5">
         <v>275</v>
       </c>
-      <c r="AE11" s="483">
+      <c r="AE11" s="485">
         <f>AB11/683</f>
         <v>0.40263543191800877</v>
       </c>
-      <c r="AI11" s="485"/>
+      <c r="AI11" s="487"/>
     </row>
     <row r="12" spans="3:37" x14ac:dyDescent="0.2">
       <c r="AA12" s="5" t="s">
@@ -37249,21 +37297,21 @@
       <c r="AB12" s="5">
         <v>280</v>
       </c>
-      <c r="AE12" s="483">
+      <c r="AE12" s="485">
         <f>AB12/683</f>
         <v>0.40995607613469986</v>
       </c>
-      <c r="AI12" s="485"/>
+      <c r="AI12" s="487"/>
     </row>
     <row r="13" spans="3:37" x14ac:dyDescent="0.2">
       <c r="AA13" s="5" t="s">
         <v>1023</v>
       </c>
-      <c r="AI13" s="498">
+      <c r="AI13" s="500">
         <f>SUM(AI7:AI10)</f>
         <v>0.15067349926793558</v>
       </c>
-      <c r="AJ13" s="498">
+      <c r="AJ13" s="500">
         <f>SUM(AJ7:AJ10)</f>
         <v>0.22554904831625183</v>
       </c>
@@ -37465,12 +37513,12 @@
       <c r="K27" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="L27" s="522" t="s">
+      <c r="L27" s="526" t="s">
         <v>322</v>
       </c>
-      <c r="M27" s="523"/>
-      <c r="N27" s="523"/>
-      <c r="O27" s="524"/>
+      <c r="M27" s="527"/>
+      <c r="N27" s="527"/>
+      <c r="O27" s="528"/>
       <c r="T27" s="283"/>
       <c r="U27" s="283"/>
     </row>
@@ -37478,12 +37526,12 @@
       <c r="J28" s="5" t="s">
         <v>376</v>
       </c>
-      <c r="L28" s="513" t="s">
+      <c r="L28" s="517" t="s">
         <v>328</v>
       </c>
-      <c r="M28" s="514"/>
-      <c r="N28" s="514"/>
-      <c r="O28" s="515"/>
+      <c r="M28" s="518"/>
+      <c r="N28" s="518"/>
+      <c r="O28" s="519"/>
       <c r="T28" s="283"/>
       <c r="U28" s="283"/>
     </row>
@@ -47911,128 +47959,128 @@
       <c r="C4" s="364" t="s">
         <v>774</v>
       </c>
-      <c r="D4" s="533" t="s">
+      <c r="D4" s="537" t="s">
         <v>775</v>
       </c>
-      <c r="E4" s="532"/>
-      <c r="F4" s="532"/>
-      <c r="G4" s="532"/>
-      <c r="H4" s="534"/>
-      <c r="I4" s="532" t="s">
+      <c r="E4" s="536"/>
+      <c r="F4" s="536"/>
+      <c r="G4" s="536"/>
+      <c r="H4" s="538"/>
+      <c r="I4" s="536" t="s">
         <v>776</v>
       </c>
-      <c r="J4" s="532"/>
-      <c r="K4" s="532"/>
-      <c r="L4" s="532"/>
-      <c r="M4" s="534"/>
-      <c r="N4" s="532" t="s">
+      <c r="J4" s="536"/>
+      <c r="K4" s="536"/>
+      <c r="L4" s="536"/>
+      <c r="M4" s="538"/>
+      <c r="N4" s="536" t="s">
         <v>777</v>
       </c>
-      <c r="O4" s="532"/>
-      <c r="P4" s="532"/>
-      <c r="Q4" s="532"/>
-      <c r="R4" s="534"/>
-      <c r="S4" s="532" t="s">
+      <c r="O4" s="536"/>
+      <c r="P4" s="536"/>
+      <c r="Q4" s="536"/>
+      <c r="R4" s="538"/>
+      <c r="S4" s="536" t="s">
         <v>778</v>
       </c>
-      <c r="T4" s="532"/>
-      <c r="U4" s="532"/>
-      <c r="V4" s="532"/>
-      <c r="W4" s="534"/>
-      <c r="X4" s="532" t="s">
+      <c r="T4" s="536"/>
+      <c r="U4" s="536"/>
+      <c r="V4" s="536"/>
+      <c r="W4" s="538"/>
+      <c r="X4" s="536" t="s">
         <v>779</v>
       </c>
-      <c r="Y4" s="532"/>
-      <c r="Z4" s="532"/>
-      <c r="AA4" s="532"/>
-      <c r="AB4" s="534"/>
-      <c r="AC4" s="532" t="s">
+      <c r="Y4" s="536"/>
+      <c r="Z4" s="536"/>
+      <c r="AA4" s="536"/>
+      <c r="AB4" s="538"/>
+      <c r="AC4" s="536" t="s">
         <v>780</v>
       </c>
-      <c r="AD4" s="532"/>
-      <c r="AE4" s="532"/>
-      <c r="AF4" s="532"/>
-      <c r="AG4" s="534"/>
-      <c r="AH4" s="532" t="s">
+      <c r="AD4" s="536"/>
+      <c r="AE4" s="536"/>
+      <c r="AF4" s="536"/>
+      <c r="AG4" s="538"/>
+      <c r="AH4" s="536" t="s">
         <v>781</v>
       </c>
-      <c r="AI4" s="532"/>
-      <c r="AJ4" s="532"/>
-      <c r="AK4" s="532"/>
-      <c r="AL4" s="534"/>
-      <c r="AM4" s="532" t="s">
+      <c r="AI4" s="536"/>
+      <c r="AJ4" s="536"/>
+      <c r="AK4" s="536"/>
+      <c r="AL4" s="538"/>
+      <c r="AM4" s="536" t="s">
         <v>782</v>
       </c>
-      <c r="AN4" s="532"/>
-      <c r="AO4" s="532"/>
-      <c r="AP4" s="532"/>
-      <c r="AQ4" s="534"/>
-      <c r="AR4" s="532" t="s">
+      <c r="AN4" s="536"/>
+      <c r="AO4" s="536"/>
+      <c r="AP4" s="536"/>
+      <c r="AQ4" s="538"/>
+      <c r="AR4" s="536" t="s">
         <v>783</v>
       </c>
-      <c r="AS4" s="532"/>
-      <c r="AT4" s="532"/>
-      <c r="AU4" s="532"/>
-      <c r="AV4" s="534"/>
-      <c r="AW4" s="532" t="s">
+      <c r="AS4" s="536"/>
+      <c r="AT4" s="536"/>
+      <c r="AU4" s="536"/>
+      <c r="AV4" s="538"/>
+      <c r="AW4" s="536" t="s">
         <v>784</v>
       </c>
-      <c r="AX4" s="532"/>
-      <c r="AY4" s="532"/>
-      <c r="AZ4" s="532"/>
-      <c r="BA4" s="532"/>
-      <c r="BB4" s="533" t="s">
+      <c r="AX4" s="536"/>
+      <c r="AY4" s="536"/>
+      <c r="AZ4" s="536"/>
+      <c r="BA4" s="536"/>
+      <c r="BB4" s="537" t="s">
         <v>785</v>
       </c>
-      <c r="BC4" s="532"/>
-      <c r="BD4" s="532"/>
-      <c r="BE4" s="532"/>
-      <c r="BF4" s="534"/>
-      <c r="BG4" s="532" t="s">
+      <c r="BC4" s="536"/>
+      <c r="BD4" s="536"/>
+      <c r="BE4" s="536"/>
+      <c r="BF4" s="538"/>
+      <c r="BG4" s="536" t="s">
         <v>786</v>
       </c>
-      <c r="BH4" s="532"/>
-      <c r="BI4" s="532"/>
-      <c r="BJ4" s="532"/>
-      <c r="BK4" s="532"/>
-      <c r="BL4" s="533" t="s">
+      <c r="BH4" s="536"/>
+      <c r="BI4" s="536"/>
+      <c r="BJ4" s="536"/>
+      <c r="BK4" s="536"/>
+      <c r="BL4" s="537" t="s">
         <v>787</v>
       </c>
-      <c r="BM4" s="532"/>
-      <c r="BN4" s="532"/>
-      <c r="BO4" s="532"/>
-      <c r="BP4" s="532"/>
-      <c r="BQ4" s="533" t="s">
+      <c r="BM4" s="536"/>
+      <c r="BN4" s="536"/>
+      <c r="BO4" s="536"/>
+      <c r="BP4" s="536"/>
+      <c r="BQ4" s="537" t="s">
         <v>788</v>
       </c>
-      <c r="BR4" s="532"/>
-      <c r="BS4" s="532"/>
-      <c r="BT4" s="532"/>
-      <c r="BU4" s="534"/>
+      <c r="BR4" s="536"/>
+      <c r="BS4" s="536"/>
+      <c r="BT4" s="536"/>
+      <c r="BU4" s="538"/>
       <c r="BV4" s="365" t="s">
         <v>789</v>
       </c>
-      <c r="BW4" s="535" t="s">
+      <c r="BW4" s="539" t="s">
         <v>790</v>
       </c>
-      <c r="BX4" s="536"/>
-      <c r="BY4" s="536"/>
-      <c r="BZ4" s="536"/>
-      <c r="CA4" s="537"/>
-      <c r="CB4" s="535" t="s">
+      <c r="BX4" s="540"/>
+      <c r="BY4" s="540"/>
+      <c r="BZ4" s="540"/>
+      <c r="CA4" s="541"/>
+      <c r="CB4" s="539" t="s">
         <v>791</v>
       </c>
-      <c r="CC4" s="536"/>
-      <c r="CD4" s="536"/>
-      <c r="CE4" s="536"/>
-      <c r="CF4" s="537"/>
-      <c r="CG4" s="535" t="s">
+      <c r="CC4" s="540"/>
+      <c r="CD4" s="540"/>
+      <c r="CE4" s="540"/>
+      <c r="CF4" s="541"/>
+      <c r="CG4" s="539" t="s">
         <v>792</v>
       </c>
-      <c r="CH4" s="536"/>
-      <c r="CI4" s="536"/>
-      <c r="CJ4" s="536"/>
-      <c r="CK4" s="537"/>
+      <c r="CH4" s="540"/>
+      <c r="CI4" s="540"/>
+      <c r="CJ4" s="540"/>
+      <c r="CK4" s="541"/>
     </row>
     <row r="5" spans="1:89" x14ac:dyDescent="0.2">
       <c r="A5" s="367"/>

</xml_diff>

<commit_message>
Update RSD SubRES and UC
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_RSD.xlsx
+++ b/SubRES_TMPL/SubRes_RSD.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42D3B03E-8820-40C9-94C6-5F60EC4801ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38497F65-E71A-43CE-A840-CE16703F0BA1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="4" xr2:uid="{34F9D92C-266F-476D-89E0-63153305AC39}"/>
   </bookViews>
@@ -8611,7 +8611,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3433" uniqueCount="1036">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3433" uniqueCount="1037">
   <si>
     <t>Document type:</t>
   </si>
@@ -10845,9 +10845,6 @@
     <t>RSDBDL</t>
   </si>
   <si>
-    <t>RSDELC,RSDSOL</t>
-  </si>
-  <si>
     <t>RSDELC,RSDGAS</t>
   </si>
   <si>
@@ -11740,6 +11737,12 @@
   </si>
   <si>
     <t>Induction is more expensive and about 84% eff</t>
+  </si>
+  <si>
+    <t>RSDSOL,RSDELC</t>
+  </si>
+  <si>
+    <t>\I: Detached</t>
   </si>
 </sst>
 </file>
@@ -14380,6 +14383,15 @@
     <xf numFmtId="0" fontId="53" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="23" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -14387,15 +14399,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -14407,17 +14410,26 @@
     <xf numFmtId="0" fontId="16" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -14428,19 +14440,10 @@
     <xf numFmtId="0" fontId="69" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="60" fillId="31" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="60" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="31" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="60" fillId="31" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -17142,10 +17145,10 @@
         <v>446</v>
       </c>
       <c r="G40" s="261" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H40" s="261" t="s">
         <v>1016</v>
-      </c>
-      <c r="H40" s="261" t="s">
-        <v>1017</v>
       </c>
     </row>
     <row r="41" spans="2:8" ht="15" x14ac:dyDescent="0.25">
@@ -17261,7 +17264,7 @@
         <v>31</v>
       </c>
       <c r="G3" s="457" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="H3" s="64" t="s">
         <v>33</v>
@@ -18263,7 +18266,7 @@
     </row>
     <row r="28" spans="2:39" ht="15" x14ac:dyDescent="0.2">
       <c r="B28" s="168" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="C28" s="169" t="s">
         <v>364</v>
@@ -18334,7 +18337,7 @@
     </row>
     <row r="29" spans="2:39" ht="15" x14ac:dyDescent="0.2">
       <c r="B29" s="168" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="C29" s="169" t="s">
         <v>365</v>
@@ -18405,7 +18408,7 @@
     </row>
     <row r="30" spans="2:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B30" s="168" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="C30" s="171" t="s">
         <v>366</v>
@@ -24959,8 +24962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{104F8057-C735-4662-BAA6-EEDCF7B57273}">
   <dimension ref="A2:AO162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="S17" sqref="S17"/>
+    <sheetView tabSelected="1" topLeftCell="H83" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AG113" sqref="AG113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -25081,13 +25084,13 @@
         <v>82</v>
       </c>
       <c r="AA3" s="63" t="s">
+        <v>752</v>
+      </c>
+      <c r="AB3" s="63" t="s">
         <v>753</v>
       </c>
-      <c r="AB3" s="63" t="s">
+      <c r="AC3" s="63" t="s">
         <v>754</v>
-      </c>
-      <c r="AC3" s="63" t="s">
-        <v>755</v>
       </c>
       <c r="AD3" s="63" t="s">
         <v>671</v>
@@ -25096,7 +25099,7 @@
         <v>313</v>
       </c>
       <c r="AF3" s="63" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="AG3" s="63" t="s">
         <v>314</v>
@@ -25104,7 +25107,7 @@
     </row>
     <row r="4" spans="3:41" ht="38.25" x14ac:dyDescent="0.2">
       <c r="C4" s="62" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="D4" s="62" t="s">
         <v>42</v>
@@ -25137,12 +25140,12 @@
         <v>321</v>
       </c>
       <c r="T4" s="525"/>
-      <c r="U4" s="526" t="s">
+      <c r="U4" s="517" t="s">
         <v>322</v>
       </c>
-      <c r="V4" s="527"/>
-      <c r="W4" s="527"/>
-      <c r="X4" s="528"/>
+      <c r="V4" s="518"/>
+      <c r="W4" s="518"/>
+      <c r="X4" s="519"/>
       <c r="Y4" s="106"/>
       <c r="Z4" s="106"/>
       <c r="AA4" s="114" t="s">
@@ -25176,7 +25179,7 @@
     </row>
     <row r="5" spans="3:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C5" s="60" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="D5" s="60"/>
       <c r="E5" s="60"/>
@@ -25232,41 +25235,41 @@
     </row>
     <row r="6" spans="3:41" ht="33.75" x14ac:dyDescent="0.2">
       <c r="C6" s="83" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="D6" s="84"/>
       <c r="E6" s="84"/>
       <c r="F6" s="85"/>
-      <c r="G6" s="517" t="s">
+      <c r="G6" s="520" t="s">
         <v>45</v>
       </c>
-      <c r="H6" s="518"/>
-      <c r="I6" s="518"/>
-      <c r="J6" s="519"/>
-      <c r="K6" s="518" t="s">
+      <c r="H6" s="521"/>
+      <c r="I6" s="521"/>
+      <c r="J6" s="522"/>
+      <c r="K6" s="521" t="s">
         <v>45</v>
       </c>
-      <c r="L6" s="518"/>
-      <c r="M6" s="518"/>
-      <c r="N6" s="519"/>
-      <c r="O6" s="517" t="s">
+      <c r="L6" s="521"/>
+      <c r="M6" s="521"/>
+      <c r="N6" s="522"/>
+      <c r="O6" s="520" t="s">
         <v>45</v>
       </c>
-      <c r="P6" s="518"/>
-      <c r="Q6" s="518"/>
-      <c r="R6" s="519"/>
-      <c r="S6" s="517" t="s">
+      <c r="P6" s="521"/>
+      <c r="Q6" s="521"/>
+      <c r="R6" s="522"/>
+      <c r="S6" s="520" t="s">
         <v>302</v>
       </c>
-      <c r="T6" s="519"/>
-      <c r="U6" s="517" t="s">
-        <v>976</v>
-      </c>
-      <c r="V6" s="518"/>
-      <c r="W6" s="518"/>
-      <c r="X6" s="519"/>
+      <c r="T6" s="522"/>
+      <c r="U6" s="520" t="s">
+        <v>975</v>
+      </c>
+      <c r="V6" s="521"/>
+      <c r="W6" s="521"/>
+      <c r="X6" s="522"/>
       <c r="Y6" s="107" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="Z6" s="107" t="s">
         <v>330</v>
@@ -25282,7 +25285,7 @@
       </c>
       <c r="AD6" s="107"/>
       <c r="AE6" s="116" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="AF6" s="107" t="s">
         <v>45</v>
@@ -26074,7 +26077,7 @@
     </row>
     <row r="15" spans="3:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="79" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="D15" s="79"/>
       <c r="E15" s="80"/>
@@ -26218,7 +26221,7 @@
     </row>
     <row r="17" spans="3:41" ht="15" x14ac:dyDescent="0.25">
       <c r="C17" s="79" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D17" s="79"/>
       <c r="E17" s="80"/>
@@ -26865,7 +26868,7 @@
     </row>
     <row r="24" spans="3:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C24" s="79" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="D24" s="79"/>
       <c r="E24" s="80"/>
@@ -27130,7 +27133,7 @@
     </row>
     <row r="27" spans="3:41" ht="15" x14ac:dyDescent="0.25">
       <c r="C27" s="79" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="D27" s="79"/>
       <c r="E27" s="80"/>
@@ -27191,7 +27194,7 @@
         <v>362</v>
       </c>
       <c r="E28" s="167" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="F28" s="144" t="s">
         <v>721</v>
@@ -27290,7 +27293,7 @@
     </row>
     <row r="29" spans="3:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C29" s="79" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="D29" s="79"/>
       <c r="E29" s="80"/>
@@ -27310,7 +27313,7 @@
       <c r="S29" s="80"/>
       <c r="T29" s="80"/>
       <c r="U29" s="79" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="V29" s="79"/>
       <c r="W29" s="79"/>
@@ -27522,7 +27525,7 @@
     </row>
     <row r="32" spans="3:41" x14ac:dyDescent="0.2">
       <c r="C32" s="79" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="D32" s="79"/>
       <c r="E32" s="80"/>
@@ -27635,7 +27638,7 @@
         <v>360</v>
       </c>
       <c r="E34" s="70" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="F34" s="69" t="s">
         <v>372</v>
@@ -27701,7 +27704,7 @@
     </row>
     <row r="35" spans="3:41" x14ac:dyDescent="0.2">
       <c r="C35" s="79" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="D35" s="79"/>
       <c r="E35" s="80"/>
@@ -27740,7 +27743,7 @@
         <v>R-SC_Apt_ELC_N1</v>
       </c>
       <c r="D36" s="66" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="E36" s="135" t="s">
         <v>408</v>
@@ -27814,7 +27817,7 @@
         <v>R-SC_Apt_ELC_N2</v>
       </c>
       <c r="D37" s="72" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="E37" s="73" t="s">
         <v>408</v>
@@ -27961,13 +27964,13 @@
         <v>82</v>
       </c>
       <c r="AA41" s="63" t="s">
+        <v>752</v>
+      </c>
+      <c r="AB41" s="63" t="s">
         <v>753</v>
       </c>
-      <c r="AB41" s="63" t="s">
+      <c r="AC41" s="63" t="s">
         <v>754</v>
-      </c>
-      <c r="AC41" s="63" t="s">
-        <v>755</v>
       </c>
       <c r="AD41" s="63" t="s">
         <v>671</v>
@@ -27976,7 +27979,7 @@
         <v>313</v>
       </c>
       <c r="AF41" s="63" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="AG41" s="63" t="s">
         <v>314</v>
@@ -28017,12 +28020,12 @@
         <v>321</v>
       </c>
       <c r="T42" s="525"/>
-      <c r="U42" s="526" t="s">
+      <c r="U42" s="517" t="s">
         <v>322</v>
       </c>
-      <c r="V42" s="527"/>
-      <c r="W42" s="527"/>
-      <c r="X42" s="528"/>
+      <c r="V42" s="518"/>
+      <c r="W42" s="518"/>
+      <c r="X42" s="519"/>
       <c r="Y42" s="106"/>
       <c r="Z42" s="106"/>
       <c r="AA42" s="114" t="s">
@@ -28056,7 +28059,7 @@
     </row>
     <row r="43" spans="3:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C43" s="60" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="D43" s="60"/>
       <c r="E43" s="60"/>
@@ -28112,41 +28115,41 @@
     </row>
     <row r="44" spans="3:41" ht="33.75" x14ac:dyDescent="0.2">
       <c r="C44" s="83" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="D44" s="84"/>
       <c r="E44" s="84"/>
       <c r="F44" s="85"/>
-      <c r="G44" s="517" t="s">
+      <c r="G44" s="520" t="s">
         <v>45</v>
       </c>
-      <c r="H44" s="518"/>
-      <c r="I44" s="518"/>
-      <c r="J44" s="519"/>
-      <c r="K44" s="518" t="s">
+      <c r="H44" s="521"/>
+      <c r="I44" s="521"/>
+      <c r="J44" s="522"/>
+      <c r="K44" s="521" t="s">
         <v>45</v>
       </c>
-      <c r="L44" s="518"/>
-      <c r="M44" s="518"/>
-      <c r="N44" s="519"/>
-      <c r="O44" s="517" t="s">
+      <c r="L44" s="521"/>
+      <c r="M44" s="521"/>
+      <c r="N44" s="522"/>
+      <c r="O44" s="520" t="s">
         <v>45</v>
       </c>
-      <c r="P44" s="518"/>
-      <c r="Q44" s="518"/>
-      <c r="R44" s="519"/>
-      <c r="S44" s="520" t="s">
+      <c r="P44" s="521"/>
+      <c r="Q44" s="521"/>
+      <c r="R44" s="522"/>
+      <c r="S44" s="526" t="s">
         <v>302</v>
       </c>
-      <c r="T44" s="521"/>
-      <c r="U44" s="520" t="s">
-        <v>976</v>
-      </c>
-      <c r="V44" s="522"/>
-      <c r="W44" s="522"/>
-      <c r="X44" s="521"/>
+      <c r="T44" s="527"/>
+      <c r="U44" s="526" t="s">
+        <v>975</v>
+      </c>
+      <c r="V44" s="528"/>
+      <c r="W44" s="528"/>
+      <c r="X44" s="527"/>
       <c r="Y44" s="458" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="Z44" s="458" t="s">
         <v>330</v>
@@ -28162,7 +28165,7 @@
       </c>
       <c r="AD44" s="458"/>
       <c r="AE44" s="460" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="AF44" s="458" t="s">
         <v>45</v>
@@ -29476,10 +29479,10 @@
     </row>
     <row r="58" spans="3:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C58" s="68" t="s">
+        <v>998</v>
+      </c>
+      <c r="D58" s="69" t="s">
         <v>999</v>
-      </c>
-      <c r="D58" s="69" t="s">
-        <v>1000</v>
       </c>
       <c r="E58" s="70" t="s">
         <v>736</v>
@@ -29577,7 +29580,7 @@
     </row>
     <row r="59" spans="3:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C59" s="79" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="D59" s="79"/>
       <c r="E59" s="80"/>
@@ -29721,7 +29724,7 @@
     </row>
     <row r="61" spans="3:41" ht="15" x14ac:dyDescent="0.25">
       <c r="C61" s="79" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D61" s="79"/>
       <c r="E61" s="80"/>
@@ -30044,7 +30047,7 @@
       <c r="AI64" s="286"/>
       <c r="AJ64" s="151" t="str">
         <f t="shared" si="45"/>
-        <v>R-SW_Att_SOL_HPN2</v>
+        <v>R-SW_Att_ELC_HPN2</v>
       </c>
       <c r="AK64" s="151" t="str">
         <f t="shared" si="45"/>
@@ -30168,13 +30171,13 @@
     <row r="66" spans="3:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C66" s="86" t="str">
         <f>"R-SW_Att"&amp;"_"&amp;RIGHT(E66,3)&amp;"_HPN2"</f>
-        <v>R-SW_Att_SOL_HPN2</v>
+        <v>R-SW_Att_ELC_HPN2</v>
       </c>
       <c r="D66" s="75" t="s">
         <v>350</v>
       </c>
       <c r="E66" s="76" t="s">
-        <v>737</v>
+        <v>1035</v>
       </c>
       <c r="F66" s="104" t="s">
         <v>723</v>
@@ -30473,7 +30476,7 @@
     </row>
     <row r="69" spans="3:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C69" s="79" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="D69" s="79"/>
       <c r="E69" s="80"/>
@@ -30799,7 +30802,7 @@
         <v>362</v>
       </c>
       <c r="E73" s="167" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="F73" s="144" t="s">
         <v>723</v>
@@ -31222,7 +31225,7 @@
         <v>360</v>
       </c>
       <c r="E79" s="73" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="F79" s="105" t="s">
         <v>396</v>
@@ -31288,7 +31291,7 @@
     </row>
     <row r="80" spans="3:41" x14ac:dyDescent="0.2">
       <c r="C80" s="79" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="D80" s="79"/>
       <c r="E80" s="80"/>
@@ -31421,40 +31424,40 @@
         <v>31</v>
       </c>
       <c r="G87" s="63" t="s">
+        <v>1003</v>
+      </c>
+      <c r="H87" s="63" t="s">
         <v>1004</v>
       </c>
-      <c r="H87" s="63" t="s">
+      <c r="I87" s="63" t="s">
         <v>1005</v>
       </c>
-      <c r="I87" s="63" t="s">
+      <c r="J87" s="63" t="s">
         <v>1006</v>
       </c>
-      <c r="J87" s="63" t="s">
+      <c r="K87" s="63" t="s">
         <v>1007</v>
       </c>
-      <c r="K87" s="63" t="s">
+      <c r="L87" s="63" t="s">
         <v>1008</v>
       </c>
-      <c r="L87" s="63" t="s">
+      <c r="M87" s="63" t="s">
         <v>1009</v>
       </c>
-      <c r="M87" s="63" t="s">
+      <c r="N87" s="63" t="s">
         <v>1010</v>
       </c>
-      <c r="N87" s="63" t="s">
+      <c r="O87" s="63" t="s">
         <v>1011</v>
       </c>
-      <c r="O87" s="63" t="s">
+      <c r="P87" s="63" t="s">
         <v>1012</v>
       </c>
-      <c r="P87" s="63" t="s">
+      <c r="Q87" s="63" t="s">
         <v>1013</v>
       </c>
-      <c r="Q87" s="63" t="s">
+      <c r="R87" s="63" t="s">
         <v>1014</v>
-      </c>
-      <c r="R87" s="63" t="s">
-        <v>1015</v>
       </c>
       <c r="S87" s="64" t="s">
         <v>33</v>
@@ -31481,13 +31484,13 @@
         <v>82</v>
       </c>
       <c r="AA87" s="63" t="s">
+        <v>752</v>
+      </c>
+      <c r="AB87" s="63" t="s">
         <v>753</v>
       </c>
-      <c r="AB87" s="63" t="s">
+      <c r="AC87" s="63" t="s">
         <v>754</v>
-      </c>
-      <c r="AC87" s="63" t="s">
-        <v>755</v>
       </c>
       <c r="AD87" s="63" t="s">
         <v>671</v>
@@ -31496,7 +31499,7 @@
         <v>313</v>
       </c>
       <c r="AF87" s="63" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="AG87" s="63" t="s">
         <v>314</v>
@@ -31537,12 +31540,12 @@
         <v>321</v>
       </c>
       <c r="T88" s="525"/>
-      <c r="U88" s="526" t="s">
+      <c r="U88" s="517" t="s">
         <v>322</v>
       </c>
-      <c r="V88" s="527"/>
-      <c r="W88" s="527"/>
-      <c r="X88" s="528"/>
+      <c r="V88" s="518"/>
+      <c r="W88" s="518"/>
+      <c r="X88" s="519"/>
       <c r="Y88" s="106"/>
       <c r="Z88" s="106"/>
       <c r="AA88" s="114" t="s">
@@ -31576,7 +31579,7 @@
     </row>
     <row r="89" spans="3:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C89" s="60" t="s">
-        <v>752</v>
+        <v>1036</v>
       </c>
       <c r="D89" s="60"/>
       <c r="E89" s="60"/>
@@ -31632,41 +31635,41 @@
     </row>
     <row r="90" spans="3:41" ht="33.75" x14ac:dyDescent="0.2">
       <c r="C90" s="83" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="D90" s="84"/>
       <c r="E90" s="84"/>
       <c r="F90" s="85"/>
-      <c r="G90" s="517" t="s">
+      <c r="G90" s="520" t="s">
         <v>45</v>
       </c>
-      <c r="H90" s="518"/>
-      <c r="I90" s="518"/>
-      <c r="J90" s="519"/>
-      <c r="K90" s="518" t="s">
+      <c r="H90" s="521"/>
+      <c r="I90" s="521"/>
+      <c r="J90" s="522"/>
+      <c r="K90" s="521" t="s">
         <v>45</v>
       </c>
-      <c r="L90" s="518"/>
-      <c r="M90" s="518"/>
-      <c r="N90" s="519"/>
-      <c r="O90" s="517" t="s">
+      <c r="L90" s="521"/>
+      <c r="M90" s="521"/>
+      <c r="N90" s="522"/>
+      <c r="O90" s="520" t="s">
         <v>45</v>
       </c>
-      <c r="P90" s="518"/>
-      <c r="Q90" s="518"/>
-      <c r="R90" s="519"/>
-      <c r="S90" s="520" t="s">
+      <c r="P90" s="521"/>
+      <c r="Q90" s="521"/>
+      <c r="R90" s="522"/>
+      <c r="S90" s="526" t="s">
         <v>302</v>
       </c>
-      <c r="T90" s="521"/>
-      <c r="U90" s="520" t="s">
-        <v>976</v>
-      </c>
-      <c r="V90" s="522"/>
-      <c r="W90" s="522"/>
-      <c r="X90" s="521"/>
+      <c r="T90" s="527"/>
+      <c r="U90" s="526" t="s">
+        <v>975</v>
+      </c>
+      <c r="V90" s="528"/>
+      <c r="W90" s="528"/>
+      <c r="X90" s="527"/>
       <c r="Y90" s="458" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="Z90" s="458" t="s">
         <v>330</v>
@@ -31682,7 +31685,7 @@
       </c>
       <c r="AD90" s="458"/>
       <c r="AE90" s="460" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="AF90" s="458" t="s">
         <v>45</v>
@@ -32996,10 +32999,10 @@
     </row>
     <row r="104" spans="3:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C104" s="68" t="s">
+        <v>998</v>
+      </c>
+      <c r="D104" s="69" t="s">
         <v>999</v>
-      </c>
-      <c r="D104" s="69" t="s">
-        <v>1000</v>
       </c>
       <c r="E104" s="70" t="s">
         <v>736</v>
@@ -33097,7 +33100,7 @@
     </row>
     <row r="105" spans="3:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C105" s="79" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="D105" s="79"/>
       <c r="E105" s="80"/>
@@ -33241,7 +33244,7 @@
     </row>
     <row r="107" spans="3:41" ht="15" x14ac:dyDescent="0.25">
       <c r="C107" s="79" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D107" s="79"/>
       <c r="E107" s="80"/>
@@ -33552,7 +33555,7 @@
       <c r="AI110" s="286"/>
       <c r="AJ110" s="151" t="str">
         <f t="shared" si="80"/>
-        <v>R-SW_Det_SOL_HPN2</v>
+        <v>R-SW_Det_ELC_HPN2</v>
       </c>
       <c r="AK110" s="151" t="str">
         <f t="shared" si="81"/>
@@ -33673,13 +33676,13 @@
     <row r="112" spans="3:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C112" s="86" t="str">
         <f>"R-SW_Det"&amp;"_"&amp;RIGHT(E112,3)&amp;"_HPN2"</f>
-        <v>R-SW_Det_SOL_HPN2</v>
+        <v>R-SW_Det_ELC_HPN2</v>
       </c>
       <c r="D112" s="75" t="s">
         <v>350</v>
       </c>
       <c r="E112" s="76" t="s">
-        <v>737</v>
+        <v>1035</v>
       </c>
       <c r="F112" s="104" t="s">
         <v>725</v>
@@ -33966,7 +33969,7 @@
     </row>
     <row r="115" spans="3:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C115" s="79" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="D115" s="79"/>
       <c r="E115" s="80"/>
@@ -34285,7 +34288,7 @@
         <v>362</v>
       </c>
       <c r="E119" s="167" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="F119" s="144" t="s">
         <v>725</v>
@@ -34704,7 +34707,7 @@
         <v>360</v>
       </c>
       <c r="E125" s="73" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="F125" s="105" t="s">
         <v>404</v>
@@ -34770,7 +34773,7 @@
     </row>
     <row r="126" spans="3:41" x14ac:dyDescent="0.2">
       <c r="C126" s="79" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="D126" s="79"/>
       <c r="E126" s="80"/>
@@ -34923,7 +34926,7 @@
     <row r="139" spans="1:25" x14ac:dyDescent="0.2">
       <c r="I139" s="57"/>
       <c r="S139" s="5" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="140" spans="1:25" x14ac:dyDescent="0.2">
@@ -34932,10 +34935,10 @@
         <v>631</v>
       </c>
       <c r="T140" s="5" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="U140" s="5" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="141" spans="1:25" x14ac:dyDescent="0.2">
@@ -34996,7 +34999,7 @@
     <row r="145" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A145" s="4"/>
       <c r="L145" s="80" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="M145" s="80"/>
       <c r="N145" s="80"/>
@@ -35015,19 +35018,19 @@
     </row>
     <row r="146" spans="1:21" x14ac:dyDescent="0.2">
       <c r="L146" s="5" t="s">
+        <v>984</v>
+      </c>
+      <c r="M146" s="5" t="s">
         <v>985</v>
       </c>
-      <c r="M146" s="5" t="s">
+      <c r="N146" s="8" t="s">
+        <v>982</v>
+      </c>
+      <c r="O146" s="451" t="s">
         <v>986</v>
       </c>
-      <c r="N146" s="8" t="s">
-        <v>983</v>
-      </c>
-      <c r="O146" s="451" t="s">
-        <v>987</v>
-      </c>
       <c r="P146" s="8" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="S146" s="5">
         <v>18</v>
@@ -35075,7 +35078,7 @@
         <v>70</v>
       </c>
       <c r="M148" s="8" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="N148" s="8">
         <v>15</v>
@@ -35104,7 +35107,7 @@
         <v>99</v>
       </c>
       <c r="M149" s="8" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="N149" s="8">
         <v>20</v>
@@ -35133,7 +35136,7 @@
         <v>150</v>
       </c>
       <c r="M150" s="8" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="N150" s="8">
         <v>30</v>
@@ -35166,7 +35169,7 @@
     </row>
     <row r="152" spans="1:21" x14ac:dyDescent="0.2">
       <c r="L152" s="8" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="M152" s="8"/>
       <c r="N152" s="8"/>
@@ -35175,7 +35178,7 @@
     </row>
     <row r="153" spans="1:21" x14ac:dyDescent="0.2">
       <c r="L153" s="8" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="M153" s="8"/>
       <c r="N153" s="8"/>
@@ -35184,17 +35187,37 @@
     </row>
     <row r="154" spans="1:21" x14ac:dyDescent="0.2">
       <c r="L154" s="281" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="155" spans="1:21" x14ac:dyDescent="0.2">
       <c r="L155" s="5" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="162" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="G90:J90"/>
+    <mergeCell ref="K90:N90"/>
+    <mergeCell ref="O90:R90"/>
+    <mergeCell ref="S90:T90"/>
+    <mergeCell ref="U90:X90"/>
+    <mergeCell ref="G88:J88"/>
+    <mergeCell ref="K88:N88"/>
+    <mergeCell ref="O88:R88"/>
+    <mergeCell ref="S88:T88"/>
+    <mergeCell ref="U88:X88"/>
+    <mergeCell ref="G44:J44"/>
+    <mergeCell ref="K44:N44"/>
+    <mergeCell ref="O44:R44"/>
+    <mergeCell ref="S44:T44"/>
+    <mergeCell ref="U44:X44"/>
+    <mergeCell ref="G42:J42"/>
+    <mergeCell ref="K42:N42"/>
+    <mergeCell ref="O42:R42"/>
+    <mergeCell ref="S42:T42"/>
+    <mergeCell ref="U42:X42"/>
     <mergeCell ref="U4:X4"/>
     <mergeCell ref="U6:X6"/>
     <mergeCell ref="G4:J4"/>
@@ -35205,26 +35228,6 @@
     <mergeCell ref="O6:R6"/>
     <mergeCell ref="K6:N6"/>
     <mergeCell ref="G6:J6"/>
-    <mergeCell ref="G42:J42"/>
-    <mergeCell ref="K42:N42"/>
-    <mergeCell ref="O42:R42"/>
-    <mergeCell ref="S42:T42"/>
-    <mergeCell ref="U42:X42"/>
-    <mergeCell ref="G44:J44"/>
-    <mergeCell ref="K44:N44"/>
-    <mergeCell ref="O44:R44"/>
-    <mergeCell ref="S44:T44"/>
-    <mergeCell ref="U44:X44"/>
-    <mergeCell ref="G88:J88"/>
-    <mergeCell ref="K88:N88"/>
-    <mergeCell ref="O88:R88"/>
-    <mergeCell ref="S88:T88"/>
-    <mergeCell ref="U88:X88"/>
-    <mergeCell ref="G90:J90"/>
-    <mergeCell ref="K90:N90"/>
-    <mergeCell ref="O90:R90"/>
-    <mergeCell ref="S90:T90"/>
-    <mergeCell ref="U90:X90"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
@@ -35337,19 +35340,19 @@
         <v>326</v>
       </c>
       <c r="P4" s="63" t="s">
+        <v>1029</v>
+      </c>
+      <c r="Q4" s="63" t="s">
         <v>1030</v>
       </c>
-      <c r="Q4" s="63" t="s">
+      <c r="R4" s="63" t="s">
         <v>1031</v>
-      </c>
-      <c r="R4" s="63" t="s">
-        <v>1032</v>
       </c>
       <c r="S4" s="63" t="s">
         <v>81</v>
       </c>
       <c r="T4" s="63" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="U4" s="63" t="s">
         <v>313</v>
@@ -35378,12 +35381,12 @@
       <c r="I5" s="173"/>
       <c r="J5" s="173"/>
       <c r="K5" s="173"/>
-      <c r="L5" s="526" t="s">
+      <c r="L5" s="517" t="s">
         <v>322</v>
       </c>
-      <c r="M5" s="527"/>
-      <c r="N5" s="527"/>
-      <c r="O5" s="528"/>
+      <c r="M5" s="518"/>
+      <c r="N5" s="518"/>
+      <c r="O5" s="519"/>
       <c r="P5" s="468"/>
       <c r="Q5" s="468"/>
       <c r="R5" s="468"/>
@@ -35417,23 +35420,23 @@
       <c r="I6" s="83"/>
       <c r="J6" s="83"/>
       <c r="K6" s="83"/>
-      <c r="L6" s="520" t="s">
-        <v>976</v>
-      </c>
-      <c r="M6" s="522"/>
-      <c r="N6" s="522"/>
-      <c r="O6" s="521"/>
+      <c r="L6" s="526" t="s">
+        <v>975</v>
+      </c>
+      <c r="M6" s="528"/>
+      <c r="N6" s="528"/>
+      <c r="O6" s="527"/>
       <c r="P6" s="467"/>
       <c r="Q6" s="467"/>
       <c r="R6" s="467"/>
       <c r="S6" s="458" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="T6" s="107" t="s">
         <v>45</v>
       </c>
       <c r="U6" s="116" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="V6" s="107" t="s">
         <v>331</v>
@@ -36086,10 +36089,10 @@
       </c>
       <c r="S18" s="529"/>
       <c r="U18" s="5" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="V18" s="5" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="19" spans="3:22" x14ac:dyDescent="0.2">
@@ -36120,7 +36123,7 @@
       <c r="R19" s="529"/>
       <c r="S19" s="529"/>
       <c r="V19" s="5" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="20" spans="3:22" x14ac:dyDescent="0.2">
@@ -36128,7 +36131,7 @@
         <v>38</v>
       </c>
       <c r="D20" s="169" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="E20" s="169" t="s">
         <v>416</v>
@@ -36147,7 +36150,7 @@
       <c r="R20" s="529"/>
       <c r="S20" s="529"/>
       <c r="V20" s="5" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="21" spans="3:22" x14ac:dyDescent="0.2">
@@ -36159,7 +36162,7 @@
         <v>R-RSDCK_ELC_N1</v>
       </c>
       <c r="E21" s="169" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="F21" s="169" t="s">
         <v>16</v>
@@ -36184,7 +36187,7 @@
         <v>R-RSDCK_GAS_N1</v>
       </c>
       <c r="E22" s="169" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="F22" s="169" t="s">
         <v>16</v>
@@ -36209,7 +36212,7 @@
         <v>R-RSDCK_LPG_N1</v>
       </c>
       <c r="E23" s="169" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="F23" s="169" t="s">
         <v>16</v>
@@ -36228,7 +36231,7 @@
         <v>38</v>
       </c>
       <c r="D24" s="169" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="E24" s="169" t="s">
         <v>419</v>
@@ -36250,7 +36253,7 @@
         <v>38</v>
       </c>
       <c r="D25" s="169" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="E25" s="169" t="s">
         <v>420</v>
@@ -36272,7 +36275,7 @@
         <v>38</v>
       </c>
       <c r="D26" s="169" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="E26" s="169" t="s">
         <v>421</v>
@@ -36295,7 +36298,7 @@
         <v>38</v>
       </c>
       <c r="D27" s="169" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="E27" s="169" t="s">
         <v>422</v>
@@ -36317,7 +36320,7 @@
         <v>38</v>
       </c>
       <c r="D28" s="171" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="E28" s="171" t="s">
         <v>423</v>
@@ -36373,27 +36376,27 @@
       <c r="K33" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="L33" s="526" t="s">
+      <c r="L33" s="517" t="s">
         <v>322</v>
       </c>
-      <c r="M33" s="527"/>
-      <c r="N33" s="527"/>
-      <c r="O33" s="528"/>
+      <c r="M33" s="518"/>
+      <c r="N33" s="518"/>
+      <c r="O33" s="519"/>
     </row>
     <row r="34" spans="8:15" x14ac:dyDescent="0.2">
       <c r="H34" s="5" t="s">
         <v>376</v>
       </c>
-      <c r="L34" s="520" t="s">
+      <c r="L34" s="526" t="s">
         <v>328</v>
       </c>
-      <c r="M34" s="522"/>
-      <c r="N34" s="522"/>
-      <c r="O34" s="521"/>
+      <c r="M34" s="528"/>
+      <c r="N34" s="528"/>
+      <c r="O34" s="527"/>
     </row>
     <row r="35" spans="8:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H35" s="5" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="I35" s="5" t="s">
         <v>416</v>
@@ -36419,7 +36422,7 @@
     </row>
     <row r="36" spans="8:15" x14ac:dyDescent="0.2">
       <c r="H36" s="5" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="I36" s="5" t="s">
         <v>418</v>
@@ -36479,7 +36482,7 @@
     </row>
     <row r="39" spans="8:15" x14ac:dyDescent="0.2">
       <c r="H39" s="5" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="I39" s="5" t="s">
         <v>419</v>
@@ -36505,7 +36508,7 @@
     </row>
     <row r="40" spans="8:15" x14ac:dyDescent="0.2">
       <c r="H40" s="5" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="I40" s="5" t="s">
         <v>420</v>
@@ -36531,7 +36534,7 @@
     </row>
     <row r="41" spans="8:15" x14ac:dyDescent="0.2">
       <c r="H41" s="5" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="I41" s="5" t="s">
         <v>421</v>
@@ -36557,7 +36560,7 @@
     </row>
     <row r="42" spans="8:15" x14ac:dyDescent="0.2">
       <c r="H42" s="5" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="I42" s="5" t="s">
         <v>422</v>
@@ -36583,7 +36586,7 @@
     </row>
     <row r="43" spans="8:15" x14ac:dyDescent="0.2">
       <c r="H43" s="5" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="I43" s="5" t="s">
         <v>423</v>
@@ -36703,7 +36706,7 @@
         <v>81</v>
       </c>
       <c r="O3" s="63" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="P3" s="63" t="s">
         <v>313</v>
@@ -36712,7 +36715,7 @@
         <v>314</v>
       </c>
       <c r="AA3" s="281" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="4" spans="3:37" ht="38.25" x14ac:dyDescent="0.2">
@@ -36736,11 +36739,11 @@
       </c>
       <c r="I4" s="524"/>
       <c r="J4" s="525"/>
-      <c r="K4" s="526" t="s">
+      <c r="K4" s="517" t="s">
         <v>322</v>
       </c>
-      <c r="L4" s="527"/>
-      <c r="M4" s="528"/>
+      <c r="L4" s="518"/>
+      <c r="M4" s="519"/>
       <c r="N4" s="106"/>
       <c r="O4" s="106" t="s">
         <v>323</v>
@@ -36750,7 +36753,7 @@
       </c>
       <c r="Q4" s="106"/>
       <c r="AA4" s="281" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="5" spans="3:37" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -36763,16 +36766,16 @@
       <c r="G5" s="466" t="s">
         <v>302</v>
       </c>
-      <c r="H5" s="533" t="s">
+      <c r="H5" s="530" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="534"/>
-      <c r="J5" s="535"/>
-      <c r="K5" s="533" t="s">
-        <v>765</v>
-      </c>
-      <c r="L5" s="534"/>
-      <c r="M5" s="535"/>
+      <c r="I5" s="531"/>
+      <c r="J5" s="532"/>
+      <c r="K5" s="530" t="s">
+        <v>764</v>
+      </c>
+      <c r="L5" s="531"/>
+      <c r="M5" s="532"/>
       <c r="N5" s="469" t="s">
         <v>329</v>
       </c>
@@ -36780,29 +36783,29 @@
         <v>45</v>
       </c>
       <c r="P5" s="470" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="Q5" s="469" t="s">
         <v>331</v>
       </c>
       <c r="AA5" s="281"/>
-      <c r="AB5" s="530" t="s">
+      <c r="AB5" s="533" t="s">
+        <v>1020</v>
+      </c>
+      <c r="AC5" s="533"/>
+      <c r="AD5" s="471"/>
+      <c r="AE5" s="534" t="s">
+        <v>110</v>
+      </c>
+      <c r="AF5" s="534"/>
+      <c r="AG5" s="534" t="s">
         <v>1021</v>
       </c>
-      <c r="AC5" s="530"/>
-      <c r="AD5" s="471"/>
-      <c r="AE5" s="531" t="s">
-        <v>110</v>
-      </c>
-      <c r="AF5" s="531"/>
-      <c r="AG5" s="531" t="s">
+      <c r="AH5" s="534"/>
+      <c r="AI5" s="535" t="s">
         <v>1022</v>
       </c>
-      <c r="AH5" s="531"/>
-      <c r="AI5" s="532" t="s">
-        <v>1023</v>
-      </c>
-      <c r="AJ5" s="532"/>
+      <c r="AJ5" s="535"/>
     </row>
     <row r="6" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C6" s="197" t="str">
@@ -36944,7 +36947,7 @@
         <v>50</v>
       </c>
       <c r="AA7" s="5" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="AB7" s="5">
         <v>17</v>
@@ -37028,7 +37031,7 @@
         <v>6.5</v>
       </c>
       <c r="AA8" s="5" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="AB8" s="5">
         <v>24</v>
@@ -37110,7 +37113,7 @@
         <v>50</v>
       </c>
       <c r="AA9" s="5" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="AB9" s="5">
         <v>120</v>
@@ -37197,7 +37200,7 @@
         <v>6.5</v>
       </c>
       <c r="AA10" s="5" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="AB10" s="5">
         <v>100</v>
@@ -37279,7 +37282,7 @@
         <v>50</v>
       </c>
       <c r="AA11" s="5" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="AB11" s="5">
         <v>275</v>
@@ -37292,7 +37295,7 @@
     </row>
     <row r="12" spans="3:37" x14ac:dyDescent="0.2">
       <c r="AA12" s="5" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="AB12" s="5">
         <v>280</v>
@@ -37305,7 +37308,7 @@
     </row>
     <row r="13" spans="3:37" x14ac:dyDescent="0.2">
       <c r="AA13" s="5" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="AI13" s="500">
         <f>SUM(AI7:AI10)</f>
@@ -37513,12 +37516,12 @@
       <c r="K27" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="L27" s="526" t="s">
+      <c r="L27" s="517" t="s">
         <v>322</v>
       </c>
-      <c r="M27" s="527"/>
-      <c r="N27" s="527"/>
-      <c r="O27" s="528"/>
+      <c r="M27" s="518"/>
+      <c r="N27" s="518"/>
+      <c r="O27" s="519"/>
       <c r="T27" s="283"/>
       <c r="U27" s="283"/>
     </row>
@@ -37526,12 +37529,12 @@
       <c r="J28" s="5" t="s">
         <v>376</v>
       </c>
-      <c r="L28" s="517" t="s">
+      <c r="L28" s="520" t="s">
         <v>328</v>
       </c>
-      <c r="M28" s="518"/>
-      <c r="N28" s="518"/>
-      <c r="O28" s="519"/>
+      <c r="M28" s="521"/>
+      <c r="N28" s="521"/>
+      <c r="O28" s="522"/>
       <c r="T28" s="283"/>
       <c r="U28" s="283"/>
     </row>
@@ -38921,16 +38924,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="AB5:AC5"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AG5:AH5"/>
+    <mergeCell ref="AI5:AJ5"/>
+    <mergeCell ref="L27:O27"/>
     <mergeCell ref="L28:O28"/>
     <mergeCell ref="H4:J4"/>
     <mergeCell ref="K4:M4"/>
     <mergeCell ref="H5:J5"/>
     <mergeCell ref="K5:M5"/>
-    <mergeCell ref="AB5:AC5"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="AG5:AH5"/>
-    <mergeCell ref="AI5:AJ5"/>
-    <mergeCell ref="L27:O27"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="S7" r:id="rId1" xr:uid="{B1EDD63D-40A5-4174-9D28-8666BD314B83}"/>
@@ -47561,23 +47564,23 @@
   <sheetData>
     <row r="1" spans="1:89" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A1" s="353" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="AC1" s="355">
         <v>100</v>
       </c>
       <c r="BB1" s="356" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="BC1" s="357"/>
       <c r="BD1" s="357" t="s">
+        <v>767</v>
+      </c>
+      <c r="BE1" s="357" t="s">
         <v>768</v>
       </c>
-      <c r="BE1" s="357" t="s">
+      <c r="BF1" s="357" t="s">
         <v>769</v>
-      </c>
-      <c r="BF1" s="357" t="s">
-        <v>770</v>
       </c>
     </row>
     <row r="2" spans="1:89" x14ac:dyDescent="0.2">
@@ -47638,7 +47641,7 @@
       <c r="AZ2" s="359"/>
       <c r="BA2" s="359"/>
       <c r="BB2" s="360" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="BD2" s="361">
         <v>0.37830319888734398</v>
@@ -47667,7 +47670,7 @@
     </row>
     <row r="3" spans="1:89" x14ac:dyDescent="0.2">
       <c r="A3" s="354" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="B3" s="358" t="s">
         <v>676</v>
@@ -47951,131 +47954,131 @@
     </row>
     <row r="4" spans="1:89" s="366" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="362" t="s">
+        <v>771</v>
+      </c>
+      <c r="B4" s="363" t="s">
         <v>772</v>
       </c>
-      <c r="B4" s="363" t="s">
+      <c r="C4" s="364" t="s">
         <v>773</v>
       </c>
-      <c r="C4" s="364" t="s">
+      <c r="D4" s="536" t="s">
         <v>774</v>
       </c>
-      <c r="D4" s="537" t="s">
+      <c r="E4" s="537"/>
+      <c r="F4" s="537"/>
+      <c r="G4" s="537"/>
+      <c r="H4" s="538"/>
+      <c r="I4" s="537" t="s">
         <v>775</v>
       </c>
-      <c r="E4" s="536"/>
-      <c r="F4" s="536"/>
-      <c r="G4" s="536"/>
-      <c r="H4" s="538"/>
-      <c r="I4" s="536" t="s">
+      <c r="J4" s="537"/>
+      <c r="K4" s="537"/>
+      <c r="L4" s="537"/>
+      <c r="M4" s="538"/>
+      <c r="N4" s="537" t="s">
         <v>776</v>
       </c>
-      <c r="J4" s="536"/>
-      <c r="K4" s="536"/>
-      <c r="L4" s="536"/>
-      <c r="M4" s="538"/>
-      <c r="N4" s="536" t="s">
+      <c r="O4" s="537"/>
+      <c r="P4" s="537"/>
+      <c r="Q4" s="537"/>
+      <c r="R4" s="538"/>
+      <c r="S4" s="537" t="s">
         <v>777</v>
       </c>
-      <c r="O4" s="536"/>
-      <c r="P4" s="536"/>
-      <c r="Q4" s="536"/>
-      <c r="R4" s="538"/>
-      <c r="S4" s="536" t="s">
+      <c r="T4" s="537"/>
+      <c r="U4" s="537"/>
+      <c r="V4" s="537"/>
+      <c r="W4" s="538"/>
+      <c r="X4" s="537" t="s">
         <v>778</v>
       </c>
-      <c r="T4" s="536"/>
-      <c r="U4" s="536"/>
-      <c r="V4" s="536"/>
-      <c r="W4" s="538"/>
-      <c r="X4" s="536" t="s">
+      <c r="Y4" s="537"/>
+      <c r="Z4" s="537"/>
+      <c r="AA4" s="537"/>
+      <c r="AB4" s="538"/>
+      <c r="AC4" s="537" t="s">
         <v>779</v>
       </c>
-      <c r="Y4" s="536"/>
-      <c r="Z4" s="536"/>
-      <c r="AA4" s="536"/>
-      <c r="AB4" s="538"/>
-      <c r="AC4" s="536" t="s">
+      <c r="AD4" s="537"/>
+      <c r="AE4" s="537"/>
+      <c r="AF4" s="537"/>
+      <c r="AG4" s="538"/>
+      <c r="AH4" s="537" t="s">
         <v>780</v>
       </c>
-      <c r="AD4" s="536"/>
-      <c r="AE4" s="536"/>
-      <c r="AF4" s="536"/>
-      <c r="AG4" s="538"/>
-      <c r="AH4" s="536" t="s">
+      <c r="AI4" s="537"/>
+      <c r="AJ4" s="537"/>
+      <c r="AK4" s="537"/>
+      <c r="AL4" s="538"/>
+      <c r="AM4" s="537" t="s">
         <v>781</v>
       </c>
-      <c r="AI4" s="536"/>
-      <c r="AJ4" s="536"/>
-      <c r="AK4" s="536"/>
-      <c r="AL4" s="538"/>
-      <c r="AM4" s="536" t="s">
+      <c r="AN4" s="537"/>
+      <c r="AO4" s="537"/>
+      <c r="AP4" s="537"/>
+      <c r="AQ4" s="538"/>
+      <c r="AR4" s="537" t="s">
         <v>782</v>
       </c>
-      <c r="AN4" s="536"/>
-      <c r="AO4" s="536"/>
-      <c r="AP4" s="536"/>
-      <c r="AQ4" s="538"/>
-      <c r="AR4" s="536" t="s">
+      <c r="AS4" s="537"/>
+      <c r="AT4" s="537"/>
+      <c r="AU4" s="537"/>
+      <c r="AV4" s="538"/>
+      <c r="AW4" s="537" t="s">
         <v>783</v>
       </c>
-      <c r="AS4" s="536"/>
-      <c r="AT4" s="536"/>
-      <c r="AU4" s="536"/>
-      <c r="AV4" s="538"/>
-      <c r="AW4" s="536" t="s">
+      <c r="AX4" s="537"/>
+      <c r="AY4" s="537"/>
+      <c r="AZ4" s="537"/>
+      <c r="BA4" s="537"/>
+      <c r="BB4" s="536" t="s">
         <v>784</v>
       </c>
-      <c r="AX4" s="536"/>
-      <c r="AY4" s="536"/>
-      <c r="AZ4" s="536"/>
-      <c r="BA4" s="536"/>
-      <c r="BB4" s="537" t="s">
+      <c r="BC4" s="537"/>
+      <c r="BD4" s="537"/>
+      <c r="BE4" s="537"/>
+      <c r="BF4" s="538"/>
+      <c r="BG4" s="537" t="s">
         <v>785</v>
       </c>
-      <c r="BC4" s="536"/>
-      <c r="BD4" s="536"/>
-      <c r="BE4" s="536"/>
-      <c r="BF4" s="538"/>
-      <c r="BG4" s="536" t="s">
+      <c r="BH4" s="537"/>
+      <c r="BI4" s="537"/>
+      <c r="BJ4" s="537"/>
+      <c r="BK4" s="537"/>
+      <c r="BL4" s="536" t="s">
         <v>786</v>
       </c>
-      <c r="BH4" s="536"/>
-      <c r="BI4" s="536"/>
-      <c r="BJ4" s="536"/>
-      <c r="BK4" s="536"/>
-      <c r="BL4" s="537" t="s">
+      <c r="BM4" s="537"/>
+      <c r="BN4" s="537"/>
+      <c r="BO4" s="537"/>
+      <c r="BP4" s="537"/>
+      <c r="BQ4" s="536" t="s">
         <v>787</v>
       </c>
-      <c r="BM4" s="536"/>
-      <c r="BN4" s="536"/>
-      <c r="BO4" s="536"/>
-      <c r="BP4" s="536"/>
-      <c r="BQ4" s="537" t="s">
-        <v>788</v>
-      </c>
-      <c r="BR4" s="536"/>
-      <c r="BS4" s="536"/>
-      <c r="BT4" s="536"/>
+      <c r="BR4" s="537"/>
+      <c r="BS4" s="537"/>
+      <c r="BT4" s="537"/>
       <c r="BU4" s="538"/>
       <c r="BV4" s="365" t="s">
+        <v>788</v>
+      </c>
+      <c r="BW4" s="539" t="s">
         <v>789</v>
-      </c>
-      <c r="BW4" s="539" t="s">
-        <v>790</v>
       </c>
       <c r="BX4" s="540"/>
       <c r="BY4" s="540"/>
       <c r="BZ4" s="540"/>
       <c r="CA4" s="541"/>
       <c r="CB4" s="539" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="CC4" s="540"/>
       <c r="CD4" s="540"/>
       <c r="CE4" s="540"/>
       <c r="CF4" s="541"/>
       <c r="CG4" s="539" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="CH4" s="540"/>
       <c r="CI4" s="540"/>
@@ -48345,7 +48348,7 @@
     </row>
     <row r="6" spans="1:89" s="384" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="377" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="B6" s="378"/>
       <c r="C6" s="379"/>
@@ -48468,28 +48471,28 @@
     </row>
     <row r="7" spans="1:89" s="384" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="385" t="s">
+        <v>793</v>
+      </c>
+      <c r="B7" s="386" t="s">
+        <v>895</v>
+      </c>
+      <c r="C7" s="387" t="s">
         <v>794</v>
       </c>
-      <c r="B7" s="386" t="s">
+      <c r="D7" s="388" t="s">
         <v>896</v>
       </c>
-      <c r="C7" s="387" t="s">
-        <v>795</v>
-      </c>
-      <c r="D7" s="388" t="s">
-        <v>897</v>
-      </c>
       <c r="E7" s="389" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="F7" s="389" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="G7" s="389" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="H7" s="390" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="I7" s="389"/>
       <c r="J7" s="389"/>
@@ -48705,13 +48708,13 @@
     </row>
     <row r="8" spans="1:89" s="384" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="385" t="s">
+        <v>795</v>
+      </c>
+      <c r="B8" s="386" t="s">
+        <v>794</v>
+      </c>
+      <c r="C8" s="387" t="s">
         <v>796</v>
-      </c>
-      <c r="B8" s="386" t="s">
-        <v>795</v>
-      </c>
-      <c r="C8" s="387" t="s">
-        <v>797</v>
       </c>
       <c r="D8" s="388">
         <v>400</v>
@@ -48942,28 +48945,28 @@
     </row>
     <row r="9" spans="1:89" s="384" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="385" t="s">
+        <v>797</v>
+      </c>
+      <c r="B9" s="386" t="s">
         <v>798</v>
       </c>
-      <c r="B9" s="386" t="s">
-        <v>799</v>
-      </c>
       <c r="C9" s="387" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="D9" s="388" t="s">
+        <v>897</v>
+      </c>
+      <c r="E9" s="389" t="s">
         <v>898</v>
       </c>
-      <c r="E9" s="389" t="s">
+      <c r="F9" s="389" t="s">
         <v>899</v>
       </c>
-      <c r="F9" s="389" t="s">
+      <c r="G9" s="389" t="s">
+        <v>899</v>
+      </c>
+      <c r="H9" s="390" t="s">
         <v>900</v>
-      </c>
-      <c r="G9" s="389" t="s">
-        <v>900</v>
-      </c>
-      <c r="H9" s="390" t="s">
-        <v>901</v>
       </c>
       <c r="I9" s="389"/>
       <c r="J9" s="389"/>
@@ -49051,19 +49054,19 @@
         <v>0</v>
       </c>
       <c r="AR9" s="389" t="s">
+        <v>901</v>
+      </c>
+      <c r="AS9" s="389" t="s">
         <v>902</v>
       </c>
-      <c r="AS9" s="389" t="s">
+      <c r="AT9" s="389" t="s">
         <v>903</v>
       </c>
-      <c r="AT9" s="389" t="s">
+      <c r="AU9" s="389" t="s">
         <v>904</v>
       </c>
-      <c r="AU9" s="389" t="s">
-        <v>905</v>
-      </c>
       <c r="AV9" s="390" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="AW9" s="389">
         <v>22</v>
@@ -49131,7 +49134,7 @@
       <c r="BT9" s="389"/>
       <c r="BU9" s="390"/>
       <c r="BV9" s="396" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="BW9" s="397">
         <v>320</v>
@@ -49181,28 +49184,28 @@
     </row>
     <row r="10" spans="1:89" s="384" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="385" t="s">
+        <v>800</v>
+      </c>
+      <c r="B10" s="386" t="s">
+        <v>905</v>
+      </c>
+      <c r="C10" s="387" t="s">
         <v>801</v>
       </c>
-      <c r="B10" s="386" t="s">
+      <c r="D10" s="388" t="s">
         <v>906</v>
       </c>
-      <c r="C10" s="387" t="s">
-        <v>802</v>
-      </c>
-      <c r="D10" s="388" t="s">
-        <v>907</v>
-      </c>
       <c r="E10" s="389" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="F10" s="389" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="G10" s="389" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="H10" s="390" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="I10" s="389"/>
       <c r="J10" s="389"/>
@@ -49380,7 +49383,7 @@
         <v>2</v>
       </c>
       <c r="BV10" s="396" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="BW10" s="397">
         <v>58.441558441558442</v>
@@ -49430,28 +49433,28 @@
     </row>
     <row r="11" spans="1:89" s="384" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="385" t="s">
+        <v>802</v>
+      </c>
+      <c r="B11" s="386" t="s">
+        <v>907</v>
+      </c>
+      <c r="C11" s="387" t="s">
         <v>803</v>
       </c>
-      <c r="B11" s="386" t="s">
+      <c r="D11" s="388" t="s">
         <v>908</v>
       </c>
-      <c r="C11" s="387" t="s">
-        <v>804</v>
-      </c>
-      <c r="D11" s="388" t="s">
+      <c r="E11" s="389" t="s">
+        <v>897</v>
+      </c>
+      <c r="F11" s="389" t="s">
         <v>909</v>
       </c>
-      <c r="E11" s="389" t="s">
-        <v>898</v>
-      </c>
-      <c r="F11" s="389" t="s">
-        <v>910</v>
-      </c>
       <c r="G11" s="389" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="H11" s="390" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="I11" s="389"/>
       <c r="J11" s="389"/>
@@ -49619,7 +49622,7 @@
         <v>0</v>
       </c>
       <c r="BV11" s="396" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="BW11" s="397">
         <v>519.23076923076928</v>
@@ -49669,28 +49672,28 @@
     </row>
     <row r="12" spans="1:89" s="384" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="385" t="s">
+        <v>805</v>
+      </c>
+      <c r="B12" s="386" t="s">
+        <v>910</v>
+      </c>
+      <c r="C12" s="387" t="s">
         <v>806</v>
       </c>
-      <c r="B12" s="386" t="s">
+      <c r="D12" s="388" t="s">
         <v>911</v>
       </c>
-      <c r="C12" s="387" t="s">
-        <v>807</v>
-      </c>
-      <c r="D12" s="388" t="s">
-        <v>912</v>
-      </c>
       <c r="E12" s="389" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="F12" s="389" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="G12" s="389" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="H12" s="390" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="I12" s="389"/>
       <c r="J12" s="389"/>
@@ -49858,7 +49861,7 @@
         <v>0</v>
       </c>
       <c r="BV12" s="396" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="BW12" s="402">
         <v>170</v>
@@ -49908,28 +49911,28 @@
     </row>
     <row r="13" spans="1:89" s="384" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="385" t="s">
+        <v>808</v>
+      </c>
+      <c r="B13" s="386" t="s">
+        <v>912</v>
+      </c>
+      <c r="C13" s="387" t="s">
         <v>809</v>
       </c>
-      <c r="B13" s="386" t="s">
+      <c r="D13" s="388" t="s">
         <v>913</v>
       </c>
-      <c r="C13" s="387" t="s">
-        <v>810</v>
-      </c>
-      <c r="D13" s="388" t="s">
+      <c r="E13" s="389" t="s">
         <v>914</v>
       </c>
-      <c r="E13" s="389" t="s">
+      <c r="F13" s="389" t="s">
         <v>915</v>
       </c>
-      <c r="F13" s="389" t="s">
+      <c r="G13" s="389" t="s">
         <v>916</v>
       </c>
-      <c r="G13" s="389" t="s">
-        <v>917</v>
-      </c>
       <c r="H13" s="390" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="I13" s="389"/>
       <c r="J13" s="389"/>
@@ -50097,7 +50100,7 @@
         <v>0</v>
       </c>
       <c r="BV13" s="396" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="BW13" s="397">
         <v>346.66666666666669</v>
@@ -50149,7 +50152,7 @@
       <c r="A14" s="385"/>
       <c r="B14" s="386"/>
       <c r="C14" s="387" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="D14" s="388"/>
       <c r="E14" s="389"/>
@@ -50290,7 +50293,7 @@
     </row>
     <row r="15" spans="1:89" s="384" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="377" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="B15" s="378"/>
       <c r="C15" s="379"/>
@@ -50433,28 +50436,28 @@
     </row>
     <row r="16" spans="1:89" s="384" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="385" t="s">
+        <v>813</v>
+      </c>
+      <c r="B16" s="386" t="s">
+        <v>917</v>
+      </c>
+      <c r="C16" s="387" t="s">
         <v>814</v>
       </c>
-      <c r="B16" s="386" t="s">
+      <c r="D16" s="388" t="s">
         <v>918</v>
       </c>
-      <c r="C16" s="387" t="s">
-        <v>815</v>
-      </c>
-      <c r="D16" s="388" t="s">
-        <v>919</v>
-      </c>
       <c r="E16" s="389" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="F16" s="389" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="G16" s="389" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="H16" s="390" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="I16" s="389"/>
       <c r="J16" s="389"/>
@@ -50672,7 +50675,7 @@
       <c r="A17" s="385"/>
       <c r="B17" s="386"/>
       <c r="C17" s="387" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="D17" s="408">
         <v>63.7</v>
@@ -50855,13 +50858,13 @@
     </row>
     <row r="18" spans="1:89" s="384" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="385" t="s">
+        <v>816</v>
+      </c>
+      <c r="B18" s="386" t="s">
+        <v>919</v>
+      </c>
+      <c r="C18" s="387" t="s">
         <v>817</v>
-      </c>
-      <c r="B18" s="386" t="s">
-        <v>920</v>
-      </c>
-      <c r="C18" s="387" t="s">
-        <v>818</v>
       </c>
       <c r="D18" s="388">
         <v>10</v>
@@ -51044,7 +51047,7 @@
         <v>0</v>
       </c>
       <c r="BV18" s="396" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="BW18" s="393">
         <v>1100</v>
@@ -51094,28 +51097,28 @@
     </row>
     <row r="19" spans="1:89" s="384" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="385" t="s">
+        <v>819</v>
+      </c>
+      <c r="B19" s="386" t="s">
+        <v>920</v>
+      </c>
+      <c r="C19" s="387" t="s">
         <v>820</v>
       </c>
-      <c r="B19" s="386" t="s">
+      <c r="D19" s="388" t="s">
         <v>921</v>
       </c>
-      <c r="C19" s="387" t="s">
-        <v>821</v>
-      </c>
-      <c r="D19" s="388" t="s">
-        <v>922</v>
-      </c>
       <c r="E19" s="389" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="F19" s="389" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="G19" s="389" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="H19" s="390" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="I19" s="389"/>
       <c r="J19" s="389"/>
@@ -51299,19 +51302,19 @@
         <v>700</v>
       </c>
       <c r="CB19" s="393" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CC19" s="393" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CD19" s="393" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CE19" s="393" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CF19" s="394" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CG19" s="399">
         <v>1.125</v>
@@ -51331,13 +51334,13 @@
     </row>
     <row r="20" spans="1:89" s="384" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="385" t="s">
+        <v>821</v>
+      </c>
+      <c r="B20" s="386" t="s">
+        <v>923</v>
+      </c>
+      <c r="C20" s="387" t="s">
         <v>822</v>
-      </c>
-      <c r="B20" s="386" t="s">
-        <v>924</v>
-      </c>
-      <c r="C20" s="387" t="s">
-        <v>823</v>
       </c>
       <c r="D20" s="388">
         <v>10</v>
@@ -51520,7 +51523,7 @@
         <v>0</v>
       </c>
       <c r="BV20" s="396" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="BW20" s="393">
         <v>1400</v>
@@ -51570,28 +51573,28 @@
     </row>
     <row r="21" spans="1:89" s="384" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="385" t="s">
+        <v>824</v>
+      </c>
+      <c r="B21" s="386" t="s">
+        <v>924</v>
+      </c>
+      <c r="C21" s="387" t="s">
         <v>825</v>
       </c>
-      <c r="B21" s="386" t="s">
-        <v>925</v>
-      </c>
-      <c r="C21" s="387" t="s">
-        <v>826</v>
-      </c>
       <c r="D21" s="388" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="E21" s="389" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="F21" s="389" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="G21" s="389" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="H21" s="390" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="I21" s="389"/>
       <c r="J21" s="389"/>
@@ -51759,7 +51762,7 @@
         <v>0</v>
       </c>
       <c r="BV21" s="396" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="BW21" s="402">
         <v>900</v>
@@ -51809,13 +51812,13 @@
     </row>
     <row r="22" spans="1:89" s="384" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="385" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="B22" s="386" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="C22" s="387" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="D22" s="408">
         <v>15</v>
@@ -51998,7 +52001,7 @@
         <v>0</v>
       </c>
       <c r="BV22" s="396" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="BW22" s="393">
         <v>1090</v>
@@ -52050,7 +52053,7 @@
       <c r="A23" s="385"/>
       <c r="B23" s="386"/>
       <c r="C23" s="387" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="D23" s="408">
         <v>290</v>
@@ -52241,13 +52244,13 @@
     </row>
     <row r="24" spans="1:89" s="384" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="385" t="s">
+        <v>829</v>
+      </c>
+      <c r="B24" s="386" t="s">
+        <v>926</v>
+      </c>
+      <c r="C24" s="387" t="s">
         <v>830</v>
-      </c>
-      <c r="B24" s="386" t="s">
-        <v>927</v>
-      </c>
-      <c r="C24" s="387" t="s">
-        <v>831</v>
       </c>
       <c r="D24" s="388">
         <v>2</v>
@@ -52478,28 +52481,28 @@
     </row>
     <row r="25" spans="1:89" s="384" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="385" t="s">
+        <v>831</v>
+      </c>
+      <c r="B25" s="386" t="s">
+        <v>927</v>
+      </c>
+      <c r="C25" s="387" t="s">
         <v>832</v>
       </c>
-      <c r="B25" s="386" t="s">
+      <c r="D25" s="388" t="s">
         <v>928</v>
       </c>
-      <c r="C25" s="387" t="s">
-        <v>833</v>
-      </c>
-      <c r="D25" s="388" t="s">
-        <v>929</v>
-      </c>
       <c r="E25" s="389" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="F25" s="389" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="G25" s="389" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="H25" s="390" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="I25" s="389"/>
       <c r="J25" s="389"/>
@@ -52683,19 +52686,19 @@
         <v>700</v>
       </c>
       <c r="CB25" s="393" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CC25" s="393" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CD25" s="393" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CE25" s="393" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CF25" s="394" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CG25" s="399">
         <v>4.2056074766355138</v>
@@ -52715,13 +52718,13 @@
     </row>
     <row r="26" spans="1:89" s="384" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="386" t="s">
+        <v>996</v>
+      </c>
+      <c r="B26" s="386" t="s">
         <v>997</v>
       </c>
-      <c r="B26" s="386" t="s">
-        <v>998</v>
-      </c>
       <c r="C26" s="386" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="D26" s="388">
         <v>3.6</v>
@@ -52972,7 +52975,7 @@
     </row>
     <row r="27" spans="1:89" s="384" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="377" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="B27" s="378"/>
       <c r="C27" s="379"/>
@@ -53115,13 +53118,13 @@
     </row>
     <row r="28" spans="1:89" s="384" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="385" t="s">
+        <v>834</v>
+      </c>
+      <c r="B28" s="386" t="s">
+        <v>929</v>
+      </c>
+      <c r="C28" s="387" t="s">
         <v>835</v>
-      </c>
-      <c r="B28" s="386" t="s">
-        <v>930</v>
-      </c>
-      <c r="C28" s="387" t="s">
-        <v>836</v>
       </c>
       <c r="D28" s="388">
         <v>18</v>
@@ -53294,7 +53297,7 @@
       <c r="BT28" s="389"/>
       <c r="BU28" s="390"/>
       <c r="BV28" s="396" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="BW28" s="393">
         <v>866.66666666666663</v>
@@ -53344,13 +53347,13 @@
     </row>
     <row r="29" spans="1:89" s="384" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="385" t="s">
+        <v>837</v>
+      </c>
+      <c r="B29" s="386" t="s">
+        <v>930</v>
+      </c>
+      <c r="C29" s="387" t="s">
         <v>838</v>
-      </c>
-      <c r="B29" s="386" t="s">
-        <v>931</v>
-      </c>
-      <c r="C29" s="387" t="s">
-        <v>839</v>
       </c>
       <c r="D29" s="388">
         <v>44</v>
@@ -53523,7 +53526,7 @@
       <c r="BT29" s="389"/>
       <c r="BU29" s="390"/>
       <c r="BV29" s="396" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="BW29" s="393">
         <v>750</v>
@@ -53573,28 +53576,28 @@
     </row>
     <row r="30" spans="1:89" s="384" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="385" t="s">
+        <v>839</v>
+      </c>
+      <c r="B30" s="386" t="s">
+        <v>931</v>
+      </c>
+      <c r="C30" s="387" t="s">
         <v>840</v>
       </c>
-      <c r="B30" s="386" t="s">
-        <v>932</v>
-      </c>
-      <c r="C30" s="387" t="s">
-        <v>841</v>
-      </c>
       <c r="D30" s="388" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="E30" s="389" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="F30" s="389" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="G30" s="389" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="H30" s="390" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="I30" s="389"/>
       <c r="J30" s="389"/>
@@ -53687,19 +53690,19 @@
       <c r="AU30" s="389"/>
       <c r="AV30" s="390"/>
       <c r="AW30" s="389" t="s">
+        <v>932</v>
+      </c>
+      <c r="AX30" s="389" t="s">
         <v>933</v>
       </c>
-      <c r="AX30" s="389" t="s">
-        <v>934</v>
-      </c>
       <c r="AY30" s="389" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="AZ30" s="389" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="BA30" s="390" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="BB30" s="393">
         <v>47500</v>
@@ -53752,7 +53755,7 @@
       <c r="BT30" s="389"/>
       <c r="BU30" s="390"/>
       <c r="BV30" s="396" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="BW30" s="402">
         <v>950</v>
@@ -53802,28 +53805,28 @@
     </row>
     <row r="31" spans="1:89" s="384" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="385" t="s">
+        <v>842</v>
+      </c>
+      <c r="B31" s="386" t="s">
+        <v>934</v>
+      </c>
+      <c r="C31" s="413" t="s">
         <v>843</v>
       </c>
-      <c r="B31" s="386" t="s">
+      <c r="D31" s="388" t="s">
         <v>935</v>
       </c>
-      <c r="C31" s="413" t="s">
-        <v>844</v>
-      </c>
-      <c r="D31" s="388" t="s">
-        <v>936</v>
-      </c>
       <c r="E31" s="389" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="F31" s="389" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="G31" s="389" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="H31" s="390" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="I31" s="389"/>
       <c r="J31" s="389"/>
@@ -53981,7 +53984,7 @@
       <c r="BT31" s="389"/>
       <c r="BU31" s="390"/>
       <c r="BV31" s="396" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="BW31" s="397">
         <v>1696.969696969697</v>
@@ -54031,13 +54034,13 @@
     </row>
     <row r="32" spans="1:89" s="384" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="385" t="s">
+        <v>845</v>
+      </c>
+      <c r="B32" s="386" t="s">
+        <v>925</v>
+      </c>
+      <c r="C32" s="387" t="s">
         <v>846</v>
-      </c>
-      <c r="B32" s="386" t="s">
-        <v>926</v>
-      </c>
-      <c r="C32" s="387" t="s">
-        <v>847</v>
       </c>
       <c r="D32" s="388">
         <v>0</v>
@@ -54221,54 +54224,54 @@
       </c>
       <c r="BV32" s="396"/>
       <c r="BW32" s="393" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="BX32" s="393" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="BY32" s="393" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="BZ32" s="393" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CA32" s="394" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CB32" s="393" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CC32" s="393" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CD32" s="393" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CE32" s="393" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CF32" s="394" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CG32" s="395" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CH32" s="393" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CI32" s="393" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CJ32" s="393" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CK32" s="394" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="33" spans="1:89" s="384" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="377" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="B33" s="378"/>
       <c r="C33" s="379"/>
@@ -54401,13 +54404,13 @@
     </row>
     <row r="34" spans="1:89" s="384" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="385" t="s">
+        <v>848</v>
+      </c>
+      <c r="B34" s="386" t="s">
+        <v>925</v>
+      </c>
+      <c r="C34" s="387" t="s">
         <v>849</v>
-      </c>
-      <c r="B34" s="386" t="s">
-        <v>926</v>
-      </c>
-      <c r="C34" s="387" t="s">
-        <v>850</v>
       </c>
       <c r="D34" s="408">
         <v>30</v>
@@ -54590,7 +54593,7 @@
         <v>0</v>
       </c>
       <c r="BV34" s="396" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="BW34" s="393">
         <v>3466</v>
@@ -54642,7 +54645,7 @@
       <c r="A35" s="385"/>
       <c r="B35" s="386"/>
       <c r="C35" s="387" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="D35" s="408">
         <v>200</v>
@@ -54807,13 +54810,13 @@
     </row>
     <row r="36" spans="1:89" s="384" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="385" t="s">
+        <v>851</v>
+      </c>
+      <c r="B36" s="386" t="s">
+        <v>936</v>
+      </c>
+      <c r="C36" s="387" t="s">
         <v>852</v>
-      </c>
-      <c r="B36" s="386" t="s">
-        <v>937</v>
-      </c>
-      <c r="C36" s="387" t="s">
-        <v>853</v>
       </c>
       <c r="D36" s="388">
         <v>3.2</v>
@@ -54846,13 +54849,13 @@
         <v>0</v>
       </c>
       <c r="N36" s="389" t="s">
+        <v>937</v>
+      </c>
+      <c r="O36" s="389" t="s">
         <v>938</v>
       </c>
-      <c r="O36" s="389" t="s">
-        <v>939</v>
-      </c>
       <c r="P36" s="389" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="Q36" s="389">
         <v>0</v>
@@ -54866,13 +54869,13 @@
       <c r="V36" s="389"/>
       <c r="W36" s="390"/>
       <c r="X36" s="389" t="s">
+        <v>939</v>
+      </c>
+      <c r="Y36" s="389" t="s">
+        <v>939</v>
+      </c>
+      <c r="Z36" s="389" t="s">
         <v>940</v>
-      </c>
-      <c r="Y36" s="389" t="s">
-        <v>940</v>
-      </c>
-      <c r="Z36" s="389" t="s">
-        <v>941</v>
       </c>
       <c r="AA36" s="389">
         <v>0</v>
@@ -54934,10 +54937,10 @@
         <v>10</v>
       </c>
       <c r="AX36" s="389" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="AY36" s="389" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="AZ36" s="389">
         <v>0</v>
@@ -55006,7 +55009,7 @@
         <v>0</v>
       </c>
       <c r="BV36" s="396" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="BW36" s="393">
         <v>4687.5</v>
@@ -55033,10 +55036,10 @@
         <v>781.25</v>
       </c>
       <c r="CE36" s="421" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CF36" s="421" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CG36" s="395">
         <v>0</v>
@@ -55056,52 +55059,52 @@
     </row>
     <row r="37" spans="1:89" s="384" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="385" t="s">
+        <v>854</v>
+      </c>
+      <c r="B37" s="386" t="s">
+        <v>942</v>
+      </c>
+      <c r="C37" s="387" t="s">
         <v>855</v>
       </c>
-      <c r="B37" s="386" t="s">
+      <c r="D37" s="388" t="s">
         <v>943</v>
       </c>
-      <c r="C37" s="387" t="s">
-        <v>856</v>
-      </c>
-      <c r="D37" s="388" t="s">
+      <c r="E37" s="389" t="s">
+        <v>943</v>
+      </c>
+      <c r="F37" s="389" t="s">
+        <v>943</v>
+      </c>
+      <c r="G37" s="389">
+        <v>0</v>
+      </c>
+      <c r="H37" s="390">
+        <v>0</v>
+      </c>
+      <c r="I37" s="389" t="s">
         <v>944</v>
       </c>
-      <c r="E37" s="389" t="s">
-        <v>944</v>
-      </c>
-      <c r="F37" s="389" t="s">
-        <v>944</v>
-      </c>
-      <c r="G37" s="389">
-        <v>0</v>
-      </c>
-      <c r="H37" s="390">
-        <v>0</v>
-      </c>
-      <c r="I37" s="389" t="s">
+      <c r="J37" s="389" t="s">
         <v>945</v>
       </c>
-      <c r="J37" s="389" t="s">
+      <c r="K37" s="389" t="s">
         <v>946</v>
       </c>
-      <c r="K37" s="389" t="s">
+      <c r="L37" s="389">
+        <v>0</v>
+      </c>
+      <c r="M37" s="390">
+        <v>0</v>
+      </c>
+      <c r="N37" s="389" t="s">
         <v>947</v>
       </c>
-      <c r="L37" s="389">
-        <v>0</v>
-      </c>
-      <c r="M37" s="390">
-        <v>0</v>
-      </c>
-      <c r="N37" s="389" t="s">
-        <v>948</v>
-      </c>
       <c r="O37" s="389" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="P37" s="389" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="Q37" s="389">
         <v>0</v>
@@ -55115,13 +55118,13 @@
       <c r="V37" s="389"/>
       <c r="W37" s="390"/>
       <c r="X37" s="389" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="Y37" s="389" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="Z37" s="389" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="AA37" s="389">
         <v>0</v>
@@ -55180,13 +55183,13 @@
       <c r="AU37" s="389"/>
       <c r="AV37" s="390"/>
       <c r="AW37" s="389" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="AX37" s="389" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="AY37" s="389" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="AZ37" s="389">
         <v>0</v>
@@ -55255,7 +55258,7 @@
         <v>0</v>
       </c>
       <c r="BV37" s="396" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="BW37" s="397">
         <v>446.15384615384613</v>
@@ -55267,10 +55270,10 @@
         <v>446.15384615384613</v>
       </c>
       <c r="BZ37" s="397" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CA37" s="398" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CB37" s="411">
         <v>1.2307692307692308</v>
@@ -55282,10 +55285,10 @@
         <v>1.2307692307692308</v>
       </c>
       <c r="CE37" s="422" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CF37" s="423" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CG37" s="395">
         <v>0</v>
@@ -55297,24 +55300,24 @@
         <v>0</v>
       </c>
       <c r="CJ37" s="393" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CK37" s="394" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="38" spans="1:89" s="384" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="385" t="s">
+        <v>856</v>
+      </c>
+      <c r="B38" s="386" t="s">
+        <v>925</v>
+      </c>
+      <c r="C38" s="387" t="s">
         <v>857</v>
       </c>
-      <c r="B38" s="386" t="s">
-        <v>926</v>
-      </c>
-      <c r="C38" s="387" t="s">
+      <c r="D38" s="408" t="s">
         <v>858</v>
-      </c>
-      <c r="D38" s="408" t="s">
-        <v>859</v>
       </c>
       <c r="E38" s="404">
         <v>10</v>
@@ -55494,7 +55497,7 @@
         <v>0</v>
       </c>
       <c r="BV38" s="396" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="BW38" s="393">
         <v>2145</v>
@@ -55544,22 +55547,22 @@
     </row>
     <row r="39" spans="1:89" s="384" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="385" t="s">
+        <v>859</v>
+      </c>
+      <c r="B39" s="386" t="s">
+        <v>949</v>
+      </c>
+      <c r="C39" s="387" t="s">
         <v>860</v>
       </c>
-      <c r="B39" s="386" t="s">
+      <c r="D39" s="388" t="s">
         <v>950</v>
       </c>
-      <c r="C39" s="387" t="s">
-        <v>861</v>
-      </c>
-      <c r="D39" s="388" t="s">
+      <c r="E39" s="389" t="s">
         <v>951</v>
       </c>
-      <c r="E39" s="389" t="s">
+      <c r="F39" s="389" t="s">
         <v>952</v>
-      </c>
-      <c r="F39" s="389" t="s">
-        <v>953</v>
       </c>
       <c r="G39" s="389">
         <v>0</v>
@@ -55583,13 +55586,13 @@
         <v>0</v>
       </c>
       <c r="N39" s="389" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="O39" s="389" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="P39" s="389" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="Q39" s="389">
         <v>0</v>
@@ -55603,13 +55606,13 @@
       <c r="V39" s="389"/>
       <c r="W39" s="390"/>
       <c r="X39" s="389" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="Y39" s="389" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="Z39" s="389" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="AA39" s="389">
         <v>0</v>
@@ -55671,10 +55674,10 @@
         <v>10</v>
       </c>
       <c r="AX39" s="389" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="AY39" s="389" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="AZ39" s="389">
         <v>0</v>
@@ -55743,7 +55746,7 @@
         <v>0</v>
       </c>
       <c r="BV39" s="396" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="BW39" s="397">
         <v>1263.1578947368421</v>
@@ -55755,10 +55758,10 @@
         <v>909.09090909090912</v>
       </c>
       <c r="BZ39" s="397" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CA39" s="398" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CB39" s="397">
         <v>263.15789473684208</v>
@@ -55770,10 +55773,10 @@
         <v>454.54545454545456</v>
       </c>
       <c r="CE39" s="397" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CF39" s="398" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CG39" s="395">
         <v>0</v>
@@ -55793,13 +55796,13 @@
     </row>
     <row r="40" spans="1:89" s="384" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="385" t="s">
+        <v>862</v>
+      </c>
+      <c r="B40" s="386" t="s">
+        <v>954</v>
+      </c>
+      <c r="C40" s="387" t="s">
         <v>863</v>
-      </c>
-      <c r="B40" s="386" t="s">
-        <v>955</v>
-      </c>
-      <c r="C40" s="387" t="s">
-        <v>864</v>
       </c>
       <c r="D40" s="388">
         <v>15</v>
@@ -55832,13 +55835,13 @@
         <v>0</v>
       </c>
       <c r="N40" s="389" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="O40" s="389" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="P40" s="389" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="Q40" s="389">
         <v>0</v>
@@ -55852,13 +55855,13 @@
       <c r="V40" s="389"/>
       <c r="W40" s="390"/>
       <c r="X40" s="389" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="Y40" s="389" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="Z40" s="389" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="AA40" s="389">
         <v>0</v>
@@ -55920,10 +55923,10 @@
         <v>10</v>
       </c>
       <c r="AX40" s="389" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="AY40" s="389" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="AZ40" s="389">
         <v>0</v>
@@ -55992,7 +55995,7 @@
         <v>0</v>
       </c>
       <c r="BV40" s="396" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="BW40" s="393">
         <v>1333.3333333333333</v>
@@ -56042,52 +56045,52 @@
     </row>
     <row r="41" spans="1:89" s="384" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="385" t="s">
+        <v>864</v>
+      </c>
+      <c r="B41" s="386" t="s">
+        <v>956</v>
+      </c>
+      <c r="C41" s="387" t="s">
         <v>865</v>
       </c>
-      <c r="B41" s="386" t="s">
+      <c r="D41" s="388" t="s">
         <v>957</v>
       </c>
-      <c r="C41" s="387" t="s">
-        <v>866</v>
-      </c>
-      <c r="D41" s="388" t="s">
+      <c r="E41" s="389" t="s">
+        <v>957</v>
+      </c>
+      <c r="F41" s="389" t="s">
+        <v>957</v>
+      </c>
+      <c r="G41" s="389" t="s">
+        <v>922</v>
+      </c>
+      <c r="H41" s="390" t="s">
+        <v>922</v>
+      </c>
+      <c r="I41" s="389" t="s">
         <v>958</v>
       </c>
-      <c r="E41" s="389" t="s">
+      <c r="J41" s="389" t="s">
         <v>958</v>
       </c>
-      <c r="F41" s="389" t="s">
+      <c r="K41" s="389" t="s">
         <v>958</v>
       </c>
-      <c r="G41" s="389" t="s">
-        <v>923</v>
-      </c>
-      <c r="H41" s="390" t="s">
-        <v>923</v>
-      </c>
-      <c r="I41" s="389" t="s">
+      <c r="L41" s="389">
+        <v>0</v>
+      </c>
+      <c r="M41" s="390">
+        <v>0</v>
+      </c>
+      <c r="N41" s="389" t="s">
         <v>959</v>
       </c>
-      <c r="J41" s="389" t="s">
+      <c r="O41" s="389" t="s">
         <v>959</v>
       </c>
-      <c r="K41" s="389" t="s">
+      <c r="P41" s="389" t="s">
         <v>959</v>
-      </c>
-      <c r="L41" s="389">
-        <v>0</v>
-      </c>
-      <c r="M41" s="390">
-        <v>0</v>
-      </c>
-      <c r="N41" s="389" t="s">
-        <v>960</v>
-      </c>
-      <c r="O41" s="389" t="s">
-        <v>960</v>
-      </c>
-      <c r="P41" s="389" t="s">
-        <v>960</v>
       </c>
       <c r="Q41" s="389">
         <v>0</v>
@@ -56101,13 +56104,13 @@
       <c r="V41" s="389"/>
       <c r="W41" s="390"/>
       <c r="X41" s="389" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="Y41" s="389" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="Z41" s="389" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="AA41" s="389">
         <v>0</v>
@@ -56166,13 +56169,13 @@
       <c r="AU41" s="389"/>
       <c r="AV41" s="390"/>
       <c r="AW41" s="389" t="s">
+        <v>961</v>
+      </c>
+      <c r="AX41" s="389" t="s">
         <v>962</v>
       </c>
-      <c r="AX41" s="389" t="s">
-        <v>963</v>
-      </c>
       <c r="AY41" s="389" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="AZ41" s="389">
         <v>0</v>
@@ -56241,7 +56244,7 @@
         <v>0</v>
       </c>
       <c r="BV41" s="396" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="BW41" s="393">
         <v>14000</v>
@@ -56291,13 +56294,13 @@
     </row>
     <row r="42" spans="1:89" s="384" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="385" t="s">
+        <v>866</v>
+      </c>
+      <c r="B42" s="386" t="s">
+        <v>963</v>
+      </c>
+      <c r="C42" s="387" t="s">
         <v>867</v>
-      </c>
-      <c r="B42" s="386" t="s">
-        <v>964</v>
-      </c>
-      <c r="C42" s="387" t="s">
-        <v>868</v>
       </c>
       <c r="D42" s="388">
         <v>1.6</v>
@@ -56330,13 +56333,13 @@
         <v>0</v>
       </c>
       <c r="N42" s="389" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="O42" s="389" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="P42" s="389" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="Q42" s="389">
         <v>0</v>
@@ -56350,13 +56353,13 @@
       <c r="V42" s="389"/>
       <c r="W42" s="390"/>
       <c r="X42" s="389" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="Y42" s="389" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="Z42" s="389" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="AA42" s="389">
         <v>0</v>
@@ -56418,10 +56421,10 @@
         <v>7</v>
       </c>
       <c r="AX42" s="389" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="AY42" s="389" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="AZ42" s="389">
         <v>0</v>
@@ -56490,7 +56493,7 @@
         <v>0</v>
       </c>
       <c r="BV42" s="396" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="BW42" s="393">
         <v>6562.5</v>
@@ -56540,7 +56543,7 @@
     </row>
     <row r="43" spans="1:89" s="384" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="377" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="B43" s="378"/>
       <c r="C43" s="379"/>
@@ -56665,7 +56668,7 @@
       <c r="A44" s="385"/>
       <c r="B44" s="386"/>
       <c r="C44" s="387" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="D44" s="388"/>
       <c r="E44" s="389"/>
@@ -56796,13 +56799,13 @@
     </row>
     <row r="45" spans="1:89" s="384" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="385" t="s">
+        <v>870</v>
+      </c>
+      <c r="B45" s="386" t="s">
+        <v>964</v>
+      </c>
+      <c r="C45" s="387" t="s">
         <v>871</v>
-      </c>
-      <c r="B45" s="386" t="s">
-        <v>965</v>
-      </c>
-      <c r="C45" s="387" t="s">
-        <v>872</v>
       </c>
       <c r="D45" s="388">
         <v>4.2</v>
@@ -57023,13 +57026,13 @@
     </row>
     <row r="46" spans="1:89" s="384" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="385" t="s">
+        <v>872</v>
+      </c>
+      <c r="B46" s="386" t="s">
+        <v>965</v>
+      </c>
+      <c r="C46" s="387" t="s">
         <v>873</v>
-      </c>
-      <c r="B46" s="386" t="s">
-        <v>966</v>
-      </c>
-      <c r="C46" s="387" t="s">
-        <v>874</v>
       </c>
       <c r="D46" s="388">
         <v>140</v>
@@ -57252,7 +57255,7 @@
       <c r="A47" s="385"/>
       <c r="B47" s="386"/>
       <c r="C47" s="387" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="D47" s="388"/>
       <c r="E47" s="389"/>
@@ -57383,13 +57386,13 @@
     </row>
     <row r="48" spans="1:89" s="384" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="385" t="s">
+        <v>875</v>
+      </c>
+      <c r="B48" s="386" t="s">
+        <v>966</v>
+      </c>
+      <c r="C48" s="387" t="s">
         <v>876</v>
-      </c>
-      <c r="B48" s="386" t="s">
-        <v>967</v>
-      </c>
-      <c r="C48" s="387" t="s">
-        <v>877</v>
       </c>
       <c r="D48" s="388">
         <v>5</v>
@@ -57572,7 +57575,7 @@
         <v>0</v>
       </c>
       <c r="BV48" s="396" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="BW48" s="393">
         <v>800</v>
@@ -57622,13 +57625,13 @@
     </row>
     <row r="49" spans="1:89" s="384" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="385" t="s">
+        <v>878</v>
+      </c>
+      <c r="B49" s="386" t="s">
+        <v>967</v>
+      </c>
+      <c r="C49" s="387" t="s">
         <v>879</v>
-      </c>
-      <c r="B49" s="386" t="s">
-        <v>968</v>
-      </c>
-      <c r="C49" s="387" t="s">
-        <v>880</v>
       </c>
       <c r="D49" s="388">
         <v>400</v>
@@ -57811,7 +57814,7 @@
         <v>0</v>
       </c>
       <c r="BV49" s="396" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="BW49" s="393">
         <v>665</v>
@@ -57861,13 +57864,13 @@
     </row>
     <row r="50" spans="1:89" s="384" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="385" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="B50" s="386" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="C50" s="387" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="D50" s="388">
         <v>0</v>
@@ -58050,59 +58053,59 @@
         <v>0</v>
       </c>
       <c r="BV50" s="396" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="BW50" s="393" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="BX50" s="393" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="BY50" s="393" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="BZ50" s="393" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CA50" s="394" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CB50" s="393" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CC50" s="393" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CD50" s="393" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CE50" s="393" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CF50" s="394" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CG50" s="395" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CH50" s="393" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CI50" s="393" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CJ50" s="393" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CK50" s="394" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="51" spans="1:89" s="384" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="385"/>
       <c r="B51" s="386"/>
       <c r="C51" s="387" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="D51" s="388"/>
       <c r="E51" s="389"/>
@@ -58233,10 +58236,10 @@
     </row>
     <row r="52" spans="1:89" s="384" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="427" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="B52" s="428" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="C52" s="429"/>
       <c r="D52" s="430">
@@ -58420,60 +58423,60 @@
         <v>0</v>
       </c>
       <c r="BV52" s="438" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="BW52" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="BX52" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="BY52" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="BZ52" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CA52" s="437" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CB52" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CC52" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CD52" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CE52" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CF52" s="437" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CG52" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CH52" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CI52" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CJ52" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CK52" s="437" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="53" spans="1:89" s="384" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="427" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="B53" s="428" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="C53" s="429"/>
       <c r="D53" s="430">
@@ -58657,60 +58660,60 @@
         <v>0</v>
       </c>
       <c r="BV53" s="438" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="BW53" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="BX53" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="BY53" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="BZ53" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CA53" s="437" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CB53" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CC53" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CD53" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CE53" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CF53" s="437" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CG53" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CH53" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CI53" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CJ53" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CK53" s="437" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="54" spans="1:89" s="384" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="427" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="B54" s="428" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="C54" s="429"/>
       <c r="D54" s="430">
@@ -58894,60 +58897,60 @@
         <v>0</v>
       </c>
       <c r="BV54" s="438" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="BW54" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="BX54" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="BY54" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="BZ54" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CA54" s="437" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CB54" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CC54" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CD54" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CE54" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CF54" s="437" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CG54" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CH54" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CI54" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CJ54" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CK54" s="437" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="55" spans="1:89" s="384" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="427" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="B55" s="428" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="C55" s="429"/>
       <c r="D55" s="430">
@@ -59131,60 +59134,60 @@
         <v>0</v>
       </c>
       <c r="BV55" s="438" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="BW55" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="BX55" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="BY55" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="BZ55" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CA55" s="437" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CB55" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CC55" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CD55" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CE55" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CF55" s="437" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CG55" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CH55" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CI55" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CJ55" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CK55" s="437" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="56" spans="1:89" s="384" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="427" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="B56" s="428" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="C56" s="429"/>
       <c r="D56" s="430">
@@ -59368,60 +59371,60 @@
         <v>0</v>
       </c>
       <c r="BV56" s="438" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="BW56" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="BX56" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="BY56" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="BZ56" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CA56" s="437" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CB56" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CC56" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CD56" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CE56" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CF56" s="437" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CG56" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CH56" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CI56" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CJ56" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CK56" s="437" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="57" spans="1:89" s="384" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="427" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="B57" s="428" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="C57" s="429"/>
       <c r="D57" s="430">
@@ -59605,60 +59608,60 @@
         <v>0</v>
       </c>
       <c r="BV57" s="438" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="BW57" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="BX57" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="BY57" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="BZ57" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CA57" s="437" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CB57" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CC57" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CD57" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CE57" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CF57" s="437" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CG57" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CH57" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CI57" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CJ57" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CK57" s="437" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="58" spans="1:89" s="384" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="427" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="B58" s="428" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="C58" s="429"/>
       <c r="D58" s="430">
@@ -59842,60 +59845,60 @@
         <v>0</v>
       </c>
       <c r="BV58" s="438" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="BW58" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="BX58" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="BY58" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="BZ58" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CA58" s="437" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CB58" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CC58" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CD58" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CE58" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CF58" s="437" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CG58" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CH58" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CI58" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CJ58" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CK58" s="437" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="59" spans="1:89" s="384" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="427" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="B59" s="428" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="C59" s="429"/>
       <c r="D59" s="430">
@@ -60079,60 +60082,60 @@
         <v>0</v>
       </c>
       <c r="BV59" s="438" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="BW59" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="BX59" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="BY59" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="BZ59" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CA59" s="437" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CB59" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CC59" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CD59" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CE59" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CF59" s="437" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CG59" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CH59" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CI59" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CJ59" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CK59" s="437" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="60" spans="1:89" s="384" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="427" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="B60" s="428" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="C60" s="429"/>
       <c r="D60" s="430"/>
@@ -60211,34 +60214,34 @@
       <c r="AU60" s="431"/>
       <c r="AV60" s="432"/>
       <c r="AW60" s="431" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="AX60" s="431" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="AY60" s="431" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="AZ60" s="431" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="BA60" s="432" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="BB60" s="430" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="BC60" s="431" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="BD60" s="431" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="BE60" s="431" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="BF60" s="432" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="BG60" s="431">
         <v>0</v>
@@ -60287,57 +60290,57 @@
       </c>
       <c r="BV60" s="438"/>
       <c r="BW60" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="BX60" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="BY60" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="BZ60" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CA60" s="437" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CB60" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CC60" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CD60" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CE60" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CF60" s="437" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CG60" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CH60" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CI60" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CJ60" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CK60" s="437" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="61" spans="1:89" s="384" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="427" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="B61" s="428" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="C61" s="429"/>
       <c r="D61" s="430"/>
@@ -60416,64 +60419,64 @@
       <c r="AU61" s="431"/>
       <c r="AV61" s="432"/>
       <c r="AW61" s="431" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="AX61" s="431" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="AY61" s="431" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="AZ61" s="431" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="BA61" s="432" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="BB61" s="430" t="s">
+        <v>971</v>
+      </c>
+      <c r="BC61" s="431" t="s">
+        <v>971</v>
+      </c>
+      <c r="BD61" s="431" t="s">
+        <v>971</v>
+      </c>
+      <c r="BE61" s="431" t="s">
+        <v>971</v>
+      </c>
+      <c r="BF61" s="432" t="s">
+        <v>971</v>
+      </c>
+      <c r="BG61" s="431">
+        <v>0</v>
+      </c>
+      <c r="BH61" s="431">
+        <v>0</v>
+      </c>
+      <c r="BI61" s="431">
+        <v>0</v>
+      </c>
+      <c r="BJ61" s="431">
+        <v>0</v>
+      </c>
+      <c r="BK61" s="432">
+        <v>0</v>
+      </c>
+      <c r="BL61" s="431" t="s">
         <v>972</v>
       </c>
-      <c r="BC61" s="431" t="s">
+      <c r="BM61" s="431" t="s">
         <v>972</v>
       </c>
-      <c r="BD61" s="431" t="s">
+      <c r="BN61" s="431" t="s">
         <v>972</v>
       </c>
-      <c r="BE61" s="431" t="s">
+      <c r="BO61" s="431" t="s">
         <v>972</v>
       </c>
-      <c r="BF61" s="432" t="s">
+      <c r="BP61" s="432" t="s">
         <v>972</v>
-      </c>
-      <c r="BG61" s="431">
-        <v>0</v>
-      </c>
-      <c r="BH61" s="431">
-        <v>0</v>
-      </c>
-      <c r="BI61" s="431">
-        <v>0</v>
-      </c>
-      <c r="BJ61" s="431">
-        <v>0</v>
-      </c>
-      <c r="BK61" s="432">
-        <v>0</v>
-      </c>
-      <c r="BL61" s="431" t="s">
-        <v>973</v>
-      </c>
-      <c r="BM61" s="431" t="s">
-        <v>973</v>
-      </c>
-      <c r="BN61" s="431" t="s">
-        <v>973</v>
-      </c>
-      <c r="BO61" s="431" t="s">
-        <v>973</v>
-      </c>
-      <c r="BP61" s="432" t="s">
-        <v>973</v>
       </c>
       <c r="BQ61" s="430">
         <v>0</v>
@@ -60492,60 +60495,60 @@
       </c>
       <c r="BV61" s="438"/>
       <c r="BW61" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="BX61" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="BY61" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="BZ61" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CA61" s="437" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CB61" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CC61" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CD61" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CE61" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CF61" s="437" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CG61" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CH61" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CI61" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CJ61" s="436" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CK61" s="437" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="62" spans="1:89" s="384" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="385" t="s">
+        <v>892</v>
+      </c>
+      <c r="B62" s="386" t="s">
+        <v>973</v>
+      </c>
+      <c r="C62" s="387" t="s">
         <v>893</v>
-      </c>
-      <c r="B62" s="386" t="s">
-        <v>974</v>
-      </c>
-      <c r="C62" s="387" t="s">
-        <v>894</v>
       </c>
       <c r="D62" s="388">
         <v>10</v>
@@ -60776,10 +60779,10 @@
     </row>
     <row r="63" spans="1:89" s="384" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="439" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="B63" s="440" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="C63" s="441"/>
       <c r="D63" s="442">
@@ -60963,52 +60966,52 @@
         <v>0</v>
       </c>
       <c r="BV63" s="447" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="BW63" s="448" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="BX63" s="448" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="BY63" s="448" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="BZ63" s="448" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CA63" s="449" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CB63" s="448" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CC63" s="448" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CD63" s="448" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CE63" s="448" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CF63" s="449" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CG63" s="448" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CH63" s="448" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CI63" s="448" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CJ63" s="448" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="CK63" s="449" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="66" spans="1:74" x14ac:dyDescent="0.2">
@@ -61649,11 +61652,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="BL4:BP4"/>
-    <mergeCell ref="BQ4:BU4"/>
-    <mergeCell ref="BW4:CA4"/>
-    <mergeCell ref="CB4:CF4"/>
-    <mergeCell ref="CG4:CK4"/>
     <mergeCell ref="BG4:BK4"/>
     <mergeCell ref="D4:H4"/>
     <mergeCell ref="I4:M4"/>
@@ -61666,6 +61664,11 @@
     <mergeCell ref="AR4:AV4"/>
     <mergeCell ref="AW4:BA4"/>
     <mergeCell ref="BB4:BF4"/>
+    <mergeCell ref="BL4:BP4"/>
+    <mergeCell ref="BQ4:BU4"/>
+    <mergeCell ref="BW4:CA4"/>
+    <mergeCell ref="CB4:CF4"/>
+    <mergeCell ref="CG4:CK4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
Update Gas Heat Pump Efficiency
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_RSD.xlsx
+++ b/SubRES_TMPL/SubRes_RSD.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{800AAF9D-2689-4DF1-8B4F-F692A9896226}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C48677-BB15-4247-8B30-1398809A68C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{34F9D92C-266F-476D-89E0-63153305AC39}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="4" xr2:uid="{34F9D92C-266F-476D-89E0-63153305AC39}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="34" r:id="rId1"/>
@@ -18,9 +18,6 @@
     <sheet name="EPA" sheetId="49" r:id="rId8"/>
     <sheet name="JRC_Data" sheetId="60" r:id="rId9"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId10"/>
-  </externalReferences>
   <definedNames>
     <definedName name="aa" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
@@ -285,6 +282,31 @@
         </r>
       </text>
     </comment>
+    <comment ref="H28" authorId="0" shapeId="0" xr:uid="{A541497A-1730-4CA2-BDFD-1962906C5F35}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Hybrid  Heat Pump has  higher COP than standard heat pump
+https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/700572/Hybrid_heat_pumps_Final_report-.pdf</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="L28" authorId="0" shapeId="0" xr:uid="{D79935FD-51B8-420E-972C-340116DBF3B1}">
       <text>
         <r>
@@ -492,6 +514,31 @@
         </r>
       </text>
     </comment>
+    <comment ref="H73" authorId="0" shapeId="0" xr:uid="{6EA783DF-6A0C-424B-BE73-3D92CDA8F24D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Hybrid  Heat Pump has  higher COP than standard heat pump
+https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/700572/Hybrid_heat_pumps_Final_report-.pdf</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="L73" authorId="0" shapeId="0" xr:uid="{E26997F1-021A-4ED9-9557-6378828469C6}">
       <text>
         <r>
@@ -696,6 +743,31 @@
           </rPr>
           <t xml:space="preserve">
 from TIMES-Starter</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H119" authorId="0" shapeId="0" xr:uid="{F41CD4DC-47C2-4C12-9935-8DB4FBB0189E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Hybrid  Heat Pump has  higher COP than standard heat pump
+https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/700572/Hybrid_heat_pumps_Final_report-.pdf</t>
         </r>
       </text>
     </comment>
@@ -8539,7 +8611,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3480" uniqueCount="1036">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3481" uniqueCount="1037">
   <si>
     <t>Document type:</t>
   </si>
@@ -11668,6 +11740,9 @@
   </si>
   <si>
     <t>RSDAHT</t>
+  </si>
+  <si>
+    <t>Regions: Northern Europe, NE</t>
   </si>
 </sst>
 </file>
@@ -14437,6 +14512,15 @@
     <xf numFmtId="0" fontId="53" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="23" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -14444,15 +14528,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -14464,17 +14539,26 @@
     <xf numFmtId="0" fontId="16" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -14485,19 +14569,10 @@
     <xf numFmtId="0" fontId="69" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="60" fillId="31" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="60" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="31" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="60" fillId="31" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -15628,121 +15703,8 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="RSDTechsNE"/>
-      <sheetName val="COMTechsNE"/>
-      <sheetName val="Summary"/>
-      <sheetName val="Overview"/>
-      <sheetName val="Template"/>
-      <sheetName val="HOB-oil_DK"/>
-      <sheetName val="HOB-oil_DK_large"/>
-      <sheetName val="HOB-gas_DK"/>
-      <sheetName val="HOB-gas_DK_large"/>
-      <sheetName val="HOB-biomass_DK"/>
-      <sheetName val="HOB-biomass_DK_large"/>
-      <sheetName val="HOB-wood_DK"/>
-      <sheetName val="HP-e-air-to-air_DK"/>
-      <sheetName val="HP-e-air-to-water_DK"/>
-      <sheetName val="HP-e-air-to-water_DK_large"/>
-      <sheetName val="HP-e-ground_DK"/>
-      <sheetName val="HP-e-ground_DK_large"/>
-      <sheetName val="HP-e-groundwater"/>
-      <sheetName val="HP-e-ventilation_DK"/>
-      <sheetName val="HP-e-ventilation_DK_large"/>
-      <sheetName val="GHP-a-airbrine-water_DK"/>
-      <sheetName val="GHP-a-airbrine-water_DK_large"/>
-      <sheetName val="GHP-eng-airbrine-water_DK"/>
-      <sheetName val="GHP-ad-brine-water_DK"/>
-      <sheetName val="GHP-eng-groundwater"/>
-      <sheetName val="CHP-eng-micro-turbine"/>
-      <sheetName val="CHP-eng-gas_DK"/>
-      <sheetName val="CHP-eng-gas_DK_large"/>
-      <sheetName val="CHP-eng-diesel"/>
-      <sheetName val="CHP-eng-stirling_DK"/>
-      <sheetName val="CHP-eng-stirling_DK_large"/>
-      <sheetName val="CHP-fc-gas_DK"/>
-      <sheetName val="CHP-fc-hydrogen_DK"/>
-      <sheetName val="Solar_DK"/>
-      <sheetName val="Solar_DK_large"/>
-      <sheetName val="Electri_DK"/>
-      <sheetName val="Electri_DK_large"/>
-      <sheetName val="Storage"/>
-      <sheetName val="Comb-HP-PV"/>
-      <sheetName val="Comb-HP-wood pellet boiler"/>
-      <sheetName val="Comb-Solar-wood pellet boiler"/>
-      <sheetName val="Comb-HP-storage"/>
-      <sheetName val="Comb-HP-air-water and ground so"/>
-      <sheetName val="Comb-HP-gas boiler"/>
-      <sheetName val="Comb-HP-elec.boiler"/>
-      <sheetName val="Comb-HP-solar"/>
-      <sheetName val="Pipe network_DK_conv."/>
-      <sheetName val="Pipe network_DK_low temp."/>
-      <sheetName val="House installations_DK"/>
-      <sheetName val="Energy savings"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5">
-        <row r="4">
-          <cell r="C4" t="str">
-            <v>Northern Europe, NE</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
-      <sheetData sheetId="27"/>
-      <sheetData sheetId="28"/>
-      <sheetData sheetId="29"/>
-      <sheetData sheetId="30"/>
-      <sheetData sheetId="31"/>
-      <sheetData sheetId="32"/>
-      <sheetData sheetId="33"/>
-      <sheetData sheetId="34"/>
-      <sheetData sheetId="35"/>
-      <sheetData sheetId="36"/>
-      <sheetData sheetId="37"/>
-      <sheetData sheetId="38"/>
-      <sheetData sheetId="39"/>
-      <sheetData sheetId="40"/>
-      <sheetData sheetId="41"/>
-      <sheetData sheetId="42"/>
-      <sheetData sheetId="43"/>
-      <sheetData sheetId="44"/>
-      <sheetData sheetId="45"/>
-      <sheetData sheetId="46"/>
-      <sheetData sheetId="47"/>
-      <sheetData sheetId="48"/>
-      <sheetData sheetId="49"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -25018,8 +24980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{104F8057-C735-4662-BAA6-EEDCF7B57273}">
   <dimension ref="A2:AQ162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D119" sqref="D119"/>
+    <sheetView tabSelected="1" topLeftCell="C15" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M47" sqref="M47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -25205,12 +25167,12 @@
         <v>321</v>
       </c>
       <c r="U4" s="541"/>
-      <c r="V4" s="542" t="s">
+      <c r="V4" s="533" t="s">
         <v>322</v>
       </c>
-      <c r="W4" s="543"/>
-      <c r="X4" s="543"/>
-      <c r="Y4" s="544"/>
+      <c r="W4" s="534"/>
+      <c r="X4" s="534"/>
+      <c r="Y4" s="535"/>
       <c r="Z4" s="106"/>
       <c r="AA4" s="106"/>
       <c r="AB4" s="114" t="s">
@@ -25309,34 +25271,34 @@
       <c r="E6" s="84"/>
       <c r="F6" s="84"/>
       <c r="G6" s="85"/>
-      <c r="H6" s="533" t="s">
+      <c r="H6" s="536" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="534"/>
-      <c r="J6" s="534"/>
-      <c r="K6" s="535"/>
-      <c r="L6" s="534" t="s">
+      <c r="I6" s="537"/>
+      <c r="J6" s="537"/>
+      <c r="K6" s="538"/>
+      <c r="L6" s="537" t="s">
         <v>45</v>
       </c>
-      <c r="M6" s="534"/>
-      <c r="N6" s="534"/>
-      <c r="O6" s="535"/>
-      <c r="P6" s="533" t="s">
+      <c r="M6" s="537"/>
+      <c r="N6" s="537"/>
+      <c r="O6" s="538"/>
+      <c r="P6" s="536" t="s">
         <v>45</v>
       </c>
-      <c r="Q6" s="534"/>
-      <c r="R6" s="534"/>
-      <c r="S6" s="535"/>
-      <c r="T6" s="533" t="s">
+      <c r="Q6" s="537"/>
+      <c r="R6" s="537"/>
+      <c r="S6" s="538"/>
+      <c r="T6" s="536" t="s">
         <v>302</v>
       </c>
-      <c r="U6" s="535"/>
-      <c r="V6" s="533" t="s">
+      <c r="U6" s="538"/>
+      <c r="V6" s="536" t="s">
         <v>968</v>
       </c>
-      <c r="W6" s="534"/>
-      <c r="X6" s="534"/>
-      <c r="Y6" s="535"/>
+      <c r="W6" s="537"/>
+      <c r="X6" s="537"/>
+      <c r="Y6" s="538"/>
       <c r="Z6" s="107" t="s">
         <v>980</v>
       </c>
@@ -27111,20 +27073,21 @@
       <c r="G25" s="135" t="s">
         <v>714</v>
       </c>
-      <c r="H25" s="65">
-        <v>1</v>
-      </c>
-      <c r="I25" s="66">
-        <f>JRC_Data!AD28/JRC_Data!$AC$28</f>
-        <v>1.074074074074074</v>
-      </c>
-      <c r="J25" s="66">
-        <f>JRC_Data!AE28/JRC_Data!$AC$28</f>
-        <v>1.2592592592592591</v>
-      </c>
-      <c r="K25" s="66">
-        <f>JRC_Data!AF28/JRC_Data!$AC$28</f>
-        <v>1.2592592592592591</v>
+      <c r="H25" s="456">
+        <f>JRC_Data!AC28/0.81</f>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="I25" s="456">
+        <f>JRC_Data!AD28/0.81</f>
+        <v>1.7901234567901232</v>
+      </c>
+      <c r="J25" s="456">
+        <f>JRC_Data!AE28/0.81</f>
+        <v>2.0987654320987654</v>
+      </c>
+      <c r="K25" s="456">
+        <f>JRC_Data!AF28/0.81</f>
+        <v>2.0987654320987654</v>
       </c>
       <c r="L25" s="92"/>
       <c r="M25" s="93"/>
@@ -27132,19 +27095,19 @@
       <c r="O25" s="94"/>
       <c r="P25" s="65">
         <f>H25*0.7</f>
-        <v>0.7</v>
+        <v>1.1666666666666667</v>
       </c>
       <c r="Q25" s="66">
         <f t="shared" ref="Q25:S25" si="19">I25*0.7</f>
-        <v>0.75185185185185177</v>
+        <v>1.2530864197530862</v>
       </c>
       <c r="R25" s="66">
         <f t="shared" si="19"/>
-        <v>0.88148148148148131</v>
+        <v>1.4691358024691357</v>
       </c>
       <c r="S25" s="102">
         <f t="shared" si="19"/>
-        <v>0.88148148148148131</v>
+        <v>1.4691358024691357</v>
       </c>
       <c r="T25" s="135">
         <v>22</v>
@@ -27223,21 +27186,21 @@
       <c r="G26" s="73" t="s">
         <v>714</v>
       </c>
-      <c r="H26" s="68">
-        <f>JRC_Data!AC30/JRC_Data!$AC$28</f>
-        <v>1.1111111111111109</v>
-      </c>
-      <c r="I26" s="68">
-        <f>JRC_Data!AD30/JRC_Data!$AC$28</f>
-        <v>1.1481481481481481</v>
-      </c>
-      <c r="J26" s="68">
-        <f>JRC_Data!AE30/JRC_Data!$AC$28</f>
-        <v>1.1481481481481481</v>
-      </c>
-      <c r="K26" s="68">
-        <f>JRC_Data!AF30/JRC_Data!$AC$28</f>
-        <v>1.1851851851851851</v>
+      <c r="H26" s="457">
+        <f>JRC_Data!AC30/0.9</f>
+        <v>1.6666666666666665</v>
+      </c>
+      <c r="I26" s="457">
+        <f>JRC_Data!AD30/0.9</f>
+        <v>1.7222222222222223</v>
+      </c>
+      <c r="J26" s="457">
+        <f>JRC_Data!AE30/0.9</f>
+        <v>1.7222222222222223</v>
+      </c>
+      <c r="K26" s="457">
+        <f>JRC_Data!AF30/0.9</f>
+        <v>1.7777777777777779</v>
       </c>
       <c r="L26" s="95"/>
       <c r="M26" s="96"/>
@@ -27245,19 +27208,19 @@
       <c r="O26" s="97"/>
       <c r="P26" s="329">
         <f>H26*0.7</f>
-        <v>0.77777777777777757</v>
+        <v>1.1666666666666665</v>
       </c>
       <c r="Q26" s="72">
         <f t="shared" ref="Q26" si="21">I26*0.7</f>
-        <v>0.8037037037037037</v>
+        <v>1.2055555555555555</v>
       </c>
       <c r="R26" s="72">
         <f t="shared" ref="R26" si="22">J26*0.7</f>
-        <v>0.8037037037037037</v>
+        <v>1.2055555555555555</v>
       </c>
       <c r="S26" s="105">
         <f t="shared" ref="S26" si="23">K26*0.7</f>
-        <v>0.82962962962962949</v>
+        <v>1.2444444444444445</v>
       </c>
       <c r="T26" s="73">
         <v>15</v>
@@ -27327,11 +27290,11 @@
       <c r="E27" s="80"/>
       <c r="F27" s="80"/>
       <c r="G27" s="80"/>
-      <c r="H27" s="81"/>
-      <c r="I27" s="81"/>
-      <c r="J27" s="81"/>
-      <c r="K27" s="81"/>
-      <c r="L27" s="81"/>
+      <c r="H27" s="80"/>
+      <c r="I27" s="80"/>
+      <c r="J27" s="80"/>
+      <c r="K27" s="80"/>
+      <c r="L27" s="80"/>
       <c r="M27" s="81"/>
       <c r="N27" s="81"/>
       <c r="O27" s="81"/>
@@ -27392,37 +27355,41 @@
       <c r="G28" s="144" t="s">
         <v>714</v>
       </c>
-      <c r="H28" s="330">
-        <v>1</v>
-      </c>
-      <c r="I28" s="331">
-        <v>1.048</v>
-      </c>
-      <c r="J28" s="331">
-        <v>1.097</v>
-      </c>
-      <c r="K28" s="331">
-        <v>1.161</v>
+      <c r="H28" s="456">
+        <f>1.33*$AD$28+JRC_Data!AD18*(1.33-$AD$28)</f>
+        <v>3.798</v>
+      </c>
+      <c r="I28" s="456">
+        <f>1.33*$AD$28+JRC_Data!AE18*(1.33-$AD$28)</f>
+        <v>4.2100000000000009</v>
+      </c>
+      <c r="J28" s="456">
+        <f>1.33*$AD$28+JRC_Data!AF18*(1.33-$AD$28)</f>
+        <v>4.5190000000000001</v>
+      </c>
+      <c r="K28" s="456">
+        <f>1.33*$AD$28+JRC_Data!AG18*(1.33-$AD$28)</f>
+        <v>4.5190000000000001</v>
       </c>
       <c r="L28" s="95"/>
       <c r="M28" s="96"/>
       <c r="N28" s="96"/>
       <c r="O28" s="97"/>
-      <c r="P28" s="330">
+      <c r="P28" s="329">
         <f>H28*0.7</f>
-        <v>0.7</v>
-      </c>
-      <c r="Q28" s="331">
-        <f t="shared" ref="Q28:S28" si="24">I28*0.7</f>
-        <v>0.73360000000000003</v>
-      </c>
-      <c r="R28" s="331">
+        <v>2.6585999999999999</v>
+      </c>
+      <c r="Q28" s="72">
+        <f>I28*0.7</f>
+        <v>2.9470000000000005</v>
+      </c>
+      <c r="R28" s="72">
+        <f t="shared" ref="Q28:S28" si="24">J28*0.7</f>
+        <v>3.1633</v>
+      </c>
+      <c r="S28" s="105">
         <f t="shared" si="24"/>
-        <v>0.76789999999999992</v>
-      </c>
-      <c r="S28" s="332">
-        <f t="shared" si="24"/>
-        <v>0.81269999999999998</v>
+        <v>3.1633</v>
       </c>
       <c r="T28" s="333">
         <v>20</v>
@@ -28262,12 +28229,12 @@
         <v>321</v>
       </c>
       <c r="U42" s="541"/>
-      <c r="V42" s="542" t="s">
+      <c r="V42" s="533" t="s">
         <v>322</v>
       </c>
-      <c r="W42" s="543"/>
-      <c r="X42" s="543"/>
-      <c r="Y42" s="544"/>
+      <c r="W42" s="534"/>
+      <c r="X42" s="534"/>
+      <c r="Y42" s="535"/>
       <c r="Z42" s="106"/>
       <c r="AA42" s="106"/>
       <c r="AB42" s="114" t="s">
@@ -28366,34 +28333,34 @@
       <c r="E44" s="84"/>
       <c r="F44" s="84"/>
       <c r="G44" s="85"/>
-      <c r="H44" s="533" t="s">
+      <c r="H44" s="536" t="s">
         <v>45</v>
       </c>
-      <c r="I44" s="534"/>
-      <c r="J44" s="534"/>
-      <c r="K44" s="535"/>
-      <c r="L44" s="534" t="s">
+      <c r="I44" s="537"/>
+      <c r="J44" s="537"/>
+      <c r="K44" s="538"/>
+      <c r="L44" s="537" t="s">
         <v>45</v>
       </c>
-      <c r="M44" s="534"/>
-      <c r="N44" s="534"/>
-      <c r="O44" s="535"/>
-      <c r="P44" s="533" t="s">
+      <c r="M44" s="537"/>
+      <c r="N44" s="537"/>
+      <c r="O44" s="538"/>
+      <c r="P44" s="536" t="s">
         <v>45</v>
       </c>
-      <c r="Q44" s="534"/>
-      <c r="R44" s="534"/>
-      <c r="S44" s="535"/>
-      <c r="T44" s="536" t="s">
+      <c r="Q44" s="537"/>
+      <c r="R44" s="537"/>
+      <c r="S44" s="538"/>
+      <c r="T44" s="542" t="s">
         <v>302</v>
       </c>
-      <c r="U44" s="537"/>
-      <c r="V44" s="536" t="s">
+      <c r="U44" s="543"/>
+      <c r="V44" s="542" t="s">
         <v>968</v>
       </c>
-      <c r="W44" s="538"/>
-      <c r="X44" s="538"/>
-      <c r="Y44" s="537"/>
+      <c r="W44" s="544"/>
+      <c r="X44" s="544"/>
+      <c r="Y44" s="543"/>
       <c r="Z44" s="450" t="s">
         <v>980</v>
       </c>
@@ -30924,40 +30891,41 @@
       <c r="G70" s="135" t="s">
         <v>716</v>
       </c>
-      <c r="H70" s="65">
-        <v>1</v>
-      </c>
-      <c r="I70" s="66">
-        <f>JRC_Data!AD28/JRC_Data!$AC$28</f>
-        <v>1.074074074074074</v>
-      </c>
-      <c r="J70" s="66">
-        <f>JRC_Data!AE28/JRC_Data!$AC$28</f>
-        <v>1.2592592592592591</v>
-      </c>
-      <c r="K70" s="102">
-        <f>JRC_Data!AF28/JRC_Data!$AC$28</f>
-        <v>1.2592592592592591</v>
+      <c r="H70" s="456">
+        <f>JRC_Data!AC28/0.81</f>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="I70" s="456">
+        <f>JRC_Data!AD28/0.81</f>
+        <v>1.7901234567901232</v>
+      </c>
+      <c r="J70" s="456">
+        <f>JRC_Data!AE28/0.81</f>
+        <v>2.0987654320987654</v>
+      </c>
+      <c r="K70" s="456">
+        <f>JRC_Data!AF28/0.81</f>
+        <v>2.0987654320987654</v>
       </c>
       <c r="L70" s="92"/>
       <c r="M70" s="93"/>
       <c r="N70" s="93"/>
       <c r="O70" s="94"/>
-      <c r="P70" s="323">
+      <c r="P70" s="65">
         <f>H70*0.7</f>
-        <v>0.7</v>
-      </c>
-      <c r="Q70" s="324">
+        <v>1.1666666666666667</v>
+      </c>
+      <c r="Q70" s="66">
         <f t="shared" ref="Q70:Q71" si="55">I70*0.7</f>
-        <v>0.75185185185185177</v>
-      </c>
-      <c r="R70" s="324">
+        <v>1.2530864197530862</v>
+      </c>
+      <c r="R70" s="66">
         <f t="shared" ref="R70:R71" si="56">J70*0.7</f>
-        <v>0.88148148148148131</v>
-      </c>
-      <c r="S70" s="325">
+        <v>1.4691358024691357</v>
+      </c>
+      <c r="S70" s="102">
         <f t="shared" ref="S70:S71" si="57">K70*0.7</f>
-        <v>0.88148148148148131</v>
+        <v>1.4691358024691357</v>
       </c>
       <c r="T70" s="135">
         <v>22</v>
@@ -31036,41 +31004,41 @@
       <c r="G71" s="73" t="s">
         <v>716</v>
       </c>
-      <c r="H71" s="329">
-        <f>JRC_Data!AC30/JRC_Data!$AC$28</f>
-        <v>1.1111111111111109</v>
-      </c>
-      <c r="I71" s="72">
-        <f>JRC_Data!AD30/JRC_Data!$AC$28</f>
-        <v>1.1481481481481481</v>
-      </c>
-      <c r="J71" s="72">
-        <f>JRC_Data!AE30/JRC_Data!$AC$28</f>
-        <v>1.1481481481481481</v>
-      </c>
-      <c r="K71" s="105">
-        <f>JRC_Data!AF30/JRC_Data!$AC$28</f>
-        <v>1.1851851851851851</v>
+      <c r="H71" s="457">
+        <f>JRC_Data!AC30/0.9</f>
+        <v>1.6666666666666665</v>
+      </c>
+      <c r="I71" s="457">
+        <f>JRC_Data!AD30/0.9</f>
+        <v>1.7222222222222223</v>
+      </c>
+      <c r="J71" s="457">
+        <f>JRC_Data!AE30/0.9</f>
+        <v>1.7222222222222223</v>
+      </c>
+      <c r="K71" s="457">
+        <f>JRC_Data!AF30/0.9</f>
+        <v>1.7777777777777779</v>
       </c>
       <c r="L71" s="95"/>
       <c r="M71" s="96"/>
       <c r="N71" s="96"/>
       <c r="O71" s="97"/>
-      <c r="P71" s="330">
+      <c r="P71" s="329">
         <f>H71*0.7</f>
-        <v>0.77777777777777757</v>
-      </c>
-      <c r="Q71" s="331">
+        <v>1.1666666666666665</v>
+      </c>
+      <c r="Q71" s="72">
         <f t="shared" si="55"/>
-        <v>0.8037037037037037</v>
-      </c>
-      <c r="R71" s="331">
+        <v>1.2055555555555555</v>
+      </c>
+      <c r="R71" s="72">
         <f t="shared" si="56"/>
-        <v>0.8037037037037037</v>
-      </c>
-      <c r="S71" s="332">
+        <v>1.2055555555555555</v>
+      </c>
+      <c r="S71" s="105">
         <f t="shared" si="57"/>
-        <v>0.82962962962962949</v>
+        <v>1.2444444444444445</v>
       </c>
       <c r="T71" s="73">
         <v>15</v>
@@ -31140,18 +31108,18 @@
       <c r="E72" s="80"/>
       <c r="F72" s="80"/>
       <c r="G72" s="80"/>
-      <c r="H72" s="81"/>
-      <c r="I72" s="81"/>
-      <c r="J72" s="81"/>
-      <c r="K72" s="81"/>
+      <c r="H72" s="80"/>
+      <c r="I72" s="80"/>
+      <c r="J72" s="80"/>
+      <c r="K72" s="80"/>
       <c r="L72" s="81"/>
       <c r="M72" s="81"/>
       <c r="N72" s="81"/>
       <c r="O72" s="81"/>
-      <c r="P72" s="81"/>
-      <c r="Q72" s="81"/>
-      <c r="R72" s="81"/>
-      <c r="S72" s="81"/>
+      <c r="P72" s="79"/>
+      <c r="Q72" s="79"/>
+      <c r="R72" s="79"/>
+      <c r="S72" s="79"/>
       <c r="T72" s="80"/>
       <c r="U72" s="80"/>
       <c r="V72" s="79"/>
@@ -31205,37 +31173,41 @@
       <c r="G73" s="144" t="s">
         <v>716</v>
       </c>
-      <c r="H73" s="330">
-        <v>1</v>
-      </c>
-      <c r="I73" s="331">
-        <v>1.048</v>
-      </c>
-      <c r="J73" s="331">
-        <v>1.097</v>
-      </c>
-      <c r="K73" s="331">
-        <v>1.161</v>
+      <c r="H73" s="456">
+        <f>1.33*$AD$28+JRC_Data!AD18*(1.33-$AD$28)</f>
+        <v>3.798</v>
+      </c>
+      <c r="I73" s="456">
+        <f>1.33*$AD$28+JRC_Data!AE18*(1.33-$AD$28)</f>
+        <v>4.2100000000000009</v>
+      </c>
+      <c r="J73" s="456">
+        <f>1.33*$AD$28+JRC_Data!AF18*(1.33-$AD$28)</f>
+        <v>4.5190000000000001</v>
+      </c>
+      <c r="K73" s="456">
+        <f>1.33*$AD$28+JRC_Data!AG18*(1.33-$AD$28)</f>
+        <v>4.5190000000000001</v>
       </c>
       <c r="L73" s="95"/>
       <c r="M73" s="96"/>
       <c r="N73" s="96"/>
       <c r="O73" s="97"/>
-      <c r="P73" s="330">
+      <c r="P73" s="329">
         <f>H73*0.7</f>
-        <v>0.7</v>
-      </c>
-      <c r="Q73" s="331">
+        <v>2.6585999999999999</v>
+      </c>
+      <c r="Q73" s="72">
         <f t="shared" ref="Q73" si="58">I73*0.7</f>
-        <v>0.73360000000000003</v>
-      </c>
-      <c r="R73" s="331">
+        <v>2.9470000000000005</v>
+      </c>
+      <c r="R73" s="72">
         <f t="shared" ref="R73" si="59">J73*0.7</f>
-        <v>0.76789999999999992</v>
-      </c>
-      <c r="S73" s="332">
+        <v>3.1633</v>
+      </c>
+      <c r="S73" s="105">
         <f t="shared" ref="S73" si="60">K73*0.7</f>
-        <v>0.81269999999999998</v>
+        <v>3.1633</v>
       </c>
       <c r="T73" s="5">
         <v>20</v>
@@ -31982,12 +31954,12 @@
         <v>321</v>
       </c>
       <c r="U88" s="541"/>
-      <c r="V88" s="542" t="s">
+      <c r="V88" s="533" t="s">
         <v>322</v>
       </c>
-      <c r="W88" s="543"/>
-      <c r="X88" s="543"/>
-      <c r="Y88" s="544"/>
+      <c r="W88" s="534"/>
+      <c r="X88" s="534"/>
+      <c r="Y88" s="535"/>
       <c r="Z88" s="106"/>
       <c r="AA88" s="106"/>
       <c r="AB88" s="114" t="s">
@@ -32086,34 +32058,34 @@
       <c r="E90" s="84"/>
       <c r="F90" s="84"/>
       <c r="G90" s="85"/>
-      <c r="H90" s="533" t="s">
+      <c r="H90" s="536" t="s">
         <v>45</v>
       </c>
-      <c r="I90" s="534"/>
-      <c r="J90" s="534"/>
-      <c r="K90" s="535"/>
-      <c r="L90" s="534" t="s">
+      <c r="I90" s="537"/>
+      <c r="J90" s="537"/>
+      <c r="K90" s="538"/>
+      <c r="L90" s="537" t="s">
         <v>45</v>
       </c>
-      <c r="M90" s="534"/>
-      <c r="N90" s="534"/>
-      <c r="O90" s="535"/>
-      <c r="P90" s="533" t="s">
+      <c r="M90" s="537"/>
+      <c r="N90" s="537"/>
+      <c r="O90" s="538"/>
+      <c r="P90" s="536" t="s">
         <v>45</v>
       </c>
-      <c r="Q90" s="534"/>
-      <c r="R90" s="534"/>
-      <c r="S90" s="535"/>
-      <c r="T90" s="536" t="s">
+      <c r="Q90" s="537"/>
+      <c r="R90" s="537"/>
+      <c r="S90" s="538"/>
+      <c r="T90" s="542" t="s">
         <v>302</v>
       </c>
-      <c r="U90" s="537"/>
-      <c r="V90" s="536" t="s">
+      <c r="U90" s="543"/>
+      <c r="V90" s="542" t="s">
         <v>968</v>
       </c>
-      <c r="W90" s="538"/>
-      <c r="X90" s="538"/>
-      <c r="Y90" s="537"/>
+      <c r="W90" s="544"/>
+      <c r="X90" s="544"/>
+      <c r="Y90" s="543"/>
       <c r="Z90" s="450" t="s">
         <v>980</v>
       </c>
@@ -34617,37 +34589,41 @@
       <c r="G116" s="135" t="s">
         <v>718</v>
       </c>
-      <c r="H116" s="65">
-        <v>1</v>
-      </c>
-      <c r="I116" s="66">
-        <v>1.074074074074074</v>
-      </c>
-      <c r="J116" s="66">
-        <v>1.2592592592592591</v>
-      </c>
-      <c r="K116" s="102">
-        <v>1.2592592592592591</v>
+      <c r="H116" s="456">
+        <f>JRC_Data!AC28/0.81</f>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="I116" s="456">
+        <f>JRC_Data!AD28/0.81</f>
+        <v>1.7901234567901232</v>
+      </c>
+      <c r="J116" s="456">
+        <f>JRC_Data!AE28/0.81</f>
+        <v>2.0987654320987654</v>
+      </c>
+      <c r="K116" s="456">
+        <f>JRC_Data!AF28/0.81</f>
+        <v>2.0987654320987654</v>
       </c>
       <c r="L116" s="92"/>
       <c r="M116" s="93"/>
       <c r="N116" s="93"/>
       <c r="O116" s="94"/>
-      <c r="P116" s="323">
+      <c r="P116" s="65">
         <f>H116*0.7</f>
-        <v>0.7</v>
-      </c>
-      <c r="Q116" s="324">
+        <v>1.1666666666666667</v>
+      </c>
+      <c r="Q116" s="66">
         <f t="shared" ref="Q116:Q117" si="91">I116*0.7</f>
-        <v>0.75185185185185177</v>
-      </c>
-      <c r="R116" s="324">
+        <v>1.2530864197530862</v>
+      </c>
+      <c r="R116" s="66">
         <f t="shared" ref="R116:R117" si="92">J116*0.7</f>
-        <v>0.88148148148148131</v>
-      </c>
-      <c r="S116" s="325">
+        <v>1.4691358024691357</v>
+      </c>
+      <c r="S116" s="102">
         <f t="shared" ref="S116:S117" si="93">K116*0.7</f>
-        <v>0.88148148148148131</v>
+        <v>1.4691358024691357</v>
       </c>
       <c r="T116" s="135">
         <v>22</v>
@@ -34726,37 +34702,41 @@
       <c r="G117" s="73" t="s">
         <v>718</v>
       </c>
-      <c r="H117" s="329">
-        <v>1.1111111111111109</v>
-      </c>
-      <c r="I117" s="72">
-        <v>1.1481481481481481</v>
-      </c>
-      <c r="J117" s="72">
-        <v>1.1481481481481481</v>
-      </c>
-      <c r="K117" s="105">
-        <v>1.1851851851851851</v>
+      <c r="H117" s="457">
+        <f>JRC_Data!AC30/0.9</f>
+        <v>1.6666666666666665</v>
+      </c>
+      <c r="I117" s="457">
+        <f>JRC_Data!AD30/0.9</f>
+        <v>1.7222222222222223</v>
+      </c>
+      <c r="J117" s="457">
+        <f>JRC_Data!AE30/0.9</f>
+        <v>1.7222222222222223</v>
+      </c>
+      <c r="K117" s="457">
+        <f>JRC_Data!AF30/0.9</f>
+        <v>1.7777777777777779</v>
       </c>
       <c r="L117" s="95"/>
       <c r="M117" s="96"/>
       <c r="N117" s="96"/>
       <c r="O117" s="97"/>
-      <c r="P117" s="330">
+      <c r="P117" s="329">
         <f>H117*0.7</f>
-        <v>0.77777777777777757</v>
-      </c>
-      <c r="Q117" s="331">
+        <v>1.1666666666666665</v>
+      </c>
+      <c r="Q117" s="72">
         <f t="shared" si="91"/>
-        <v>0.8037037037037037</v>
-      </c>
-      <c r="R117" s="331">
+        <v>1.2055555555555555</v>
+      </c>
+      <c r="R117" s="72">
         <f t="shared" si="92"/>
-        <v>0.8037037037037037</v>
-      </c>
-      <c r="S117" s="332">
+        <v>1.2055555555555555</v>
+      </c>
+      <c r="S117" s="105">
         <f t="shared" si="93"/>
-        <v>0.82962962962962949</v>
+        <v>1.2444444444444445</v>
       </c>
       <c r="T117" s="73">
         <v>15</v>
@@ -34826,18 +34806,18 @@
       <c r="E118" s="80"/>
       <c r="F118" s="80"/>
       <c r="G118" s="80"/>
-      <c r="H118" s="81"/>
-      <c r="I118" s="81"/>
-      <c r="J118" s="81"/>
-      <c r="K118" s="81"/>
+      <c r="H118" s="80"/>
+      <c r="I118" s="80"/>
+      <c r="J118" s="80"/>
+      <c r="K118" s="80"/>
       <c r="L118" s="81"/>
       <c r="M118" s="81"/>
       <c r="N118" s="81"/>
       <c r="O118" s="81"/>
-      <c r="P118" s="81"/>
-      <c r="Q118" s="81"/>
-      <c r="R118" s="81"/>
-      <c r="S118" s="81"/>
+      <c r="P118" s="79"/>
+      <c r="Q118" s="79"/>
+      <c r="R118" s="79"/>
+      <c r="S118" s="79"/>
       <c r="T118" s="80"/>
       <c r="U118" s="80"/>
       <c r="V118" s="79"/>
@@ -34891,37 +34871,41 @@
       <c r="G119" s="144" t="s">
         <v>718</v>
       </c>
-      <c r="H119" s="330">
-        <v>1</v>
-      </c>
-      <c r="I119" s="331">
-        <v>1.048</v>
-      </c>
-      <c r="J119" s="331">
-        <v>1.097</v>
-      </c>
-      <c r="K119" s="331">
-        <v>1.161</v>
+      <c r="H119" s="456">
+        <f>1.33*$AD$28+JRC_Data!AD18*(1.33-$AD$28)</f>
+        <v>3.798</v>
+      </c>
+      <c r="I119" s="456">
+        <f>1.33*$AD$28+JRC_Data!AE18*(1.33-$AD$28)</f>
+        <v>4.2100000000000009</v>
+      </c>
+      <c r="J119" s="456">
+        <f>1.33*$AD$28+JRC_Data!AF18*(1.33-$AD$28)</f>
+        <v>4.5190000000000001</v>
+      </c>
+      <c r="K119" s="456">
+        <f>1.33*$AD$28+JRC_Data!AG18*(1.33-$AD$28)</f>
+        <v>4.5190000000000001</v>
       </c>
       <c r="L119" s="95"/>
       <c r="M119" s="96"/>
       <c r="N119" s="96"/>
       <c r="O119" s="97"/>
-      <c r="P119" s="330">
+      <c r="P119" s="329">
         <f>H119*0.7</f>
-        <v>0.7</v>
-      </c>
-      <c r="Q119" s="331">
+        <v>2.6585999999999999</v>
+      </c>
+      <c r="Q119" s="72">
         <f t="shared" ref="Q119" si="96">I119*0.7</f>
-        <v>0.73360000000000003</v>
-      </c>
-      <c r="R119" s="331">
+        <v>2.9470000000000005</v>
+      </c>
+      <c r="R119" s="72">
         <f t="shared" ref="R119" si="97">J119*0.7</f>
-        <v>0.76789999999999992</v>
-      </c>
-      <c r="S119" s="332">
+        <v>3.1633</v>
+      </c>
+      <c r="S119" s="105">
         <f t="shared" ref="S119" si="98">K119*0.7</f>
-        <v>0.81269999999999998</v>
+        <v>3.1633</v>
       </c>
       <c r="T119" s="5">
         <v>20</v>
@@ -35831,6 +35815,26 @@
     <row r="162" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="H90:K90"/>
+    <mergeCell ref="L90:O90"/>
+    <mergeCell ref="P90:S90"/>
+    <mergeCell ref="T90:U90"/>
+    <mergeCell ref="V90:Y90"/>
+    <mergeCell ref="H88:K88"/>
+    <mergeCell ref="L88:O88"/>
+    <mergeCell ref="P88:S88"/>
+    <mergeCell ref="T88:U88"/>
+    <mergeCell ref="V88:Y88"/>
+    <mergeCell ref="H44:K44"/>
+    <mergeCell ref="L44:O44"/>
+    <mergeCell ref="P44:S44"/>
+    <mergeCell ref="T44:U44"/>
+    <mergeCell ref="V44:Y44"/>
+    <mergeCell ref="H42:K42"/>
+    <mergeCell ref="L42:O42"/>
+    <mergeCell ref="P42:S42"/>
+    <mergeCell ref="T42:U42"/>
+    <mergeCell ref="V42:Y42"/>
     <mergeCell ref="V4:Y4"/>
     <mergeCell ref="V6:Y6"/>
     <mergeCell ref="H4:K4"/>
@@ -35841,26 +35845,6 @@
     <mergeCell ref="P6:S6"/>
     <mergeCell ref="L6:O6"/>
     <mergeCell ref="H6:K6"/>
-    <mergeCell ref="H42:K42"/>
-    <mergeCell ref="L42:O42"/>
-    <mergeCell ref="P42:S42"/>
-    <mergeCell ref="T42:U42"/>
-    <mergeCell ref="V42:Y42"/>
-    <mergeCell ref="H44:K44"/>
-    <mergeCell ref="L44:O44"/>
-    <mergeCell ref="P44:S44"/>
-    <mergeCell ref="T44:U44"/>
-    <mergeCell ref="V44:Y44"/>
-    <mergeCell ref="H88:K88"/>
-    <mergeCell ref="L88:O88"/>
-    <mergeCell ref="P88:S88"/>
-    <mergeCell ref="T88:U88"/>
-    <mergeCell ref="V88:Y88"/>
-    <mergeCell ref="H90:K90"/>
-    <mergeCell ref="L90:O90"/>
-    <mergeCell ref="P90:S90"/>
-    <mergeCell ref="T90:U90"/>
-    <mergeCell ref="V90:Y90"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
@@ -36005,12 +35989,12 @@
       <c r="I5" s="173"/>
       <c r="J5" s="173"/>
       <c r="K5" s="173"/>
-      <c r="L5" s="542" t="s">
+      <c r="L5" s="533" t="s">
         <v>322</v>
       </c>
-      <c r="M5" s="543"/>
-      <c r="N5" s="543"/>
-      <c r="O5" s="544"/>
+      <c r="M5" s="534"/>
+      <c r="N5" s="534"/>
+      <c r="O5" s="535"/>
       <c r="P5" s="106"/>
       <c r="Q5" s="106" t="s">
         <v>323</v>
@@ -36041,12 +36025,12 @@
       <c r="I6" s="83"/>
       <c r="J6" s="83"/>
       <c r="K6" s="83"/>
-      <c r="L6" s="536" t="s">
+      <c r="L6" s="542" t="s">
         <v>968</v>
       </c>
-      <c r="M6" s="538"/>
-      <c r="N6" s="538"/>
-      <c r="O6" s="537"/>
+      <c r="M6" s="544"/>
+      <c r="N6" s="544"/>
+      <c r="O6" s="543"/>
       <c r="P6" s="450" t="s">
         <v>980</v>
       </c>
@@ -36964,23 +36948,23 @@
       <c r="K33" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="L33" s="542" t="s">
+      <c r="L33" s="533" t="s">
         <v>322</v>
       </c>
-      <c r="M33" s="543"/>
-      <c r="N33" s="543"/>
-      <c r="O33" s="544"/>
+      <c r="M33" s="534"/>
+      <c r="N33" s="534"/>
+      <c r="O33" s="535"/>
     </row>
     <row r="34" spans="8:15" x14ac:dyDescent="0.2">
       <c r="H34" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="L34" s="536" t="s">
+      <c r="L34" s="542" t="s">
         <v>327</v>
       </c>
-      <c r="M34" s="538"/>
-      <c r="N34" s="538"/>
-      <c r="O34" s="537"/>
+      <c r="M34" s="544"/>
+      <c r="N34" s="544"/>
+      <c r="O34" s="543"/>
     </row>
     <row r="35" spans="8:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H35" s="5" t="s">
@@ -37327,11 +37311,11 @@
       </c>
       <c r="I4" s="540"/>
       <c r="J4" s="541"/>
-      <c r="K4" s="542" t="s">
+      <c r="K4" s="533" t="s">
         <v>322</v>
       </c>
-      <c r="L4" s="543"/>
-      <c r="M4" s="544"/>
+      <c r="L4" s="534"/>
+      <c r="M4" s="535"/>
       <c r="N4" s="106"/>
       <c r="O4" s="106" t="s">
         <v>323</v>
@@ -37357,16 +37341,16 @@
       <c r="G5" s="458" t="s">
         <v>302</v>
       </c>
-      <c r="H5" s="549" t="s">
+      <c r="H5" s="546" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="550"/>
-      <c r="J5" s="551"/>
-      <c r="K5" s="549" t="s">
+      <c r="I5" s="547"/>
+      <c r="J5" s="548"/>
+      <c r="K5" s="546" t="s">
         <v>757</v>
       </c>
-      <c r="L5" s="550"/>
-      <c r="M5" s="551"/>
+      <c r="L5" s="547"/>
+      <c r="M5" s="548"/>
       <c r="N5" s="459" t="s">
         <v>328</v>
       </c>
@@ -37383,23 +37367,23 @@
         <v>626</v>
       </c>
       <c r="AA5" s="281"/>
-      <c r="AB5" s="546" t="s">
+      <c r="AB5" s="549" t="s">
         <v>1013</v>
       </c>
-      <c r="AC5" s="546"/>
+      <c r="AC5" s="549"/>
       <c r="AD5" s="461"/>
-      <c r="AE5" s="547" t="s">
+      <c r="AE5" s="550" t="s">
         <v>110</v>
       </c>
-      <c r="AF5" s="547"/>
-      <c r="AG5" s="547" t="s">
+      <c r="AF5" s="550"/>
+      <c r="AG5" s="550" t="s">
         <v>1014</v>
       </c>
-      <c r="AH5" s="547"/>
-      <c r="AI5" s="548" t="s">
+      <c r="AH5" s="550"/>
+      <c r="AI5" s="551" t="s">
         <v>1015</v>
       </c>
-      <c r="AJ5" s="548"/>
+      <c r="AJ5" s="551"/>
     </row>
     <row r="6" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C6" s="505" t="str">
@@ -38137,12 +38121,12 @@
       <c r="K27" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="L27" s="542" t="s">
+      <c r="L27" s="533" t="s">
         <v>322</v>
       </c>
-      <c r="M27" s="543"/>
-      <c r="N27" s="543"/>
-      <c r="O27" s="544"/>
+      <c r="M27" s="534"/>
+      <c r="N27" s="534"/>
+      <c r="O27" s="535"/>
       <c r="T27" s="283"/>
       <c r="U27" s="283"/>
     </row>
@@ -38150,12 +38134,12 @@
       <c r="J28" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="L28" s="533" t="s">
+      <c r="L28" s="536" t="s">
         <v>327</v>
       </c>
-      <c r="M28" s="534"/>
-      <c r="N28" s="534"/>
-      <c r="O28" s="535"/>
+      <c r="M28" s="537"/>
+      <c r="N28" s="537"/>
+      <c r="O28" s="538"/>
       <c r="T28" s="283"/>
       <c r="U28" s="283"/>
     </row>
@@ -39545,16 +39529,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="AB5:AC5"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AG5:AH5"/>
+    <mergeCell ref="AI5:AJ5"/>
+    <mergeCell ref="L27:O27"/>
     <mergeCell ref="L28:O28"/>
     <mergeCell ref="H4:J4"/>
     <mergeCell ref="K4:M4"/>
     <mergeCell ref="H5:J5"/>
     <mergeCell ref="K5:M5"/>
-    <mergeCell ref="AB5:AC5"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="AG5:AH5"/>
-    <mergeCell ref="AI5:AJ5"/>
-    <mergeCell ref="L27:O27"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="S7" r:id="rId1" xr:uid="{B1EDD63D-40A5-4174-9D28-8666BD314B83}"/>
@@ -48170,7 +48154,7 @@
   <dimension ref="A1:CK183"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A30" sqref="A30:XFD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -48205,9 +48189,8 @@
       </c>
     </row>
     <row r="2" spans="1:89" x14ac:dyDescent="0.2">
-      <c r="A2" s="346" t="str">
-        <f>"Regions: "&amp;'[1]HOB-oil_DK'!$C$4</f>
-        <v>Regions: Northern Europe, NE</v>
+      <c r="A2" s="346" t="s">
+        <v>1036</v>
       </c>
       <c r="B2" s="350"/>
       <c r="C2" s="350"/>
@@ -48583,103 +48566,103 @@
       <c r="C4" s="356" t="s">
         <v>766</v>
       </c>
-      <c r="D4" s="553" t="s">
+      <c r="D4" s="552" t="s">
         <v>767</v>
       </c>
-      <c r="E4" s="552"/>
-      <c r="F4" s="552"/>
-      <c r="G4" s="552"/>
+      <c r="E4" s="553"/>
+      <c r="F4" s="553"/>
+      <c r="G4" s="553"/>
       <c r="H4" s="554"/>
-      <c r="I4" s="552" t="s">
+      <c r="I4" s="553" t="s">
         <v>768</v>
       </c>
-      <c r="J4" s="552"/>
-      <c r="K4" s="552"/>
-      <c r="L4" s="552"/>
+      <c r="J4" s="553"/>
+      <c r="K4" s="553"/>
+      <c r="L4" s="553"/>
       <c r="M4" s="554"/>
-      <c r="N4" s="552" t="s">
+      <c r="N4" s="553" t="s">
         <v>769</v>
       </c>
-      <c r="O4" s="552"/>
-      <c r="P4" s="552"/>
-      <c r="Q4" s="552"/>
+      <c r="O4" s="553"/>
+      <c r="P4" s="553"/>
+      <c r="Q4" s="553"/>
       <c r="R4" s="554"/>
-      <c r="S4" s="552" t="s">
+      <c r="S4" s="553" t="s">
         <v>770</v>
       </c>
-      <c r="T4" s="552"/>
-      <c r="U4" s="552"/>
-      <c r="V4" s="552"/>
+      <c r="T4" s="553"/>
+      <c r="U4" s="553"/>
+      <c r="V4" s="553"/>
       <c r="W4" s="554"/>
-      <c r="X4" s="552" t="s">
+      <c r="X4" s="553" t="s">
         <v>771</v>
       </c>
-      <c r="Y4" s="552"/>
-      <c r="Z4" s="552"/>
-      <c r="AA4" s="552"/>
+      <c r="Y4" s="553"/>
+      <c r="Z4" s="553"/>
+      <c r="AA4" s="553"/>
       <c r="AB4" s="554"/>
-      <c r="AC4" s="552" t="s">
+      <c r="AC4" s="553" t="s">
         <v>772</v>
       </c>
-      <c r="AD4" s="552"/>
-      <c r="AE4" s="552"/>
-      <c r="AF4" s="552"/>
+      <c r="AD4" s="553"/>
+      <c r="AE4" s="553"/>
+      <c r="AF4" s="553"/>
       <c r="AG4" s="554"/>
-      <c r="AH4" s="552" t="s">
+      <c r="AH4" s="553" t="s">
         <v>773</v>
       </c>
-      <c r="AI4" s="552"/>
-      <c r="AJ4" s="552"/>
-      <c r="AK4" s="552"/>
+      <c r="AI4" s="553"/>
+      <c r="AJ4" s="553"/>
+      <c r="AK4" s="553"/>
       <c r="AL4" s="554"/>
-      <c r="AM4" s="552" t="s">
+      <c r="AM4" s="553" t="s">
         <v>774</v>
       </c>
-      <c r="AN4" s="552"/>
-      <c r="AO4" s="552"/>
-      <c r="AP4" s="552"/>
+      <c r="AN4" s="553"/>
+      <c r="AO4" s="553"/>
+      <c r="AP4" s="553"/>
       <c r="AQ4" s="554"/>
-      <c r="AR4" s="552" t="s">
+      <c r="AR4" s="553" t="s">
         <v>775</v>
       </c>
-      <c r="AS4" s="552"/>
-      <c r="AT4" s="552"/>
-      <c r="AU4" s="552"/>
+      <c r="AS4" s="553"/>
+      <c r="AT4" s="553"/>
+      <c r="AU4" s="553"/>
       <c r="AV4" s="554"/>
-      <c r="AW4" s="552" t="s">
+      <c r="AW4" s="553" t="s">
         <v>776</v>
       </c>
-      <c r="AX4" s="552"/>
-      <c r="AY4" s="552"/>
-      <c r="AZ4" s="552"/>
-      <c r="BA4" s="552"/>
-      <c r="BB4" s="553" t="s">
+      <c r="AX4" s="553"/>
+      <c r="AY4" s="553"/>
+      <c r="AZ4" s="553"/>
+      <c r="BA4" s="553"/>
+      <c r="BB4" s="552" t="s">
         <v>777</v>
       </c>
-      <c r="BC4" s="552"/>
-      <c r="BD4" s="552"/>
-      <c r="BE4" s="552"/>
+      <c r="BC4" s="553"/>
+      <c r="BD4" s="553"/>
+      <c r="BE4" s="553"/>
       <c r="BF4" s="554"/>
-      <c r="BG4" s="552" t="s">
+      <c r="BG4" s="553" t="s">
         <v>778</v>
       </c>
-      <c r="BH4" s="552"/>
-      <c r="BI4" s="552"/>
-      <c r="BJ4" s="552"/>
-      <c r="BK4" s="552"/>
-      <c r="BL4" s="553" t="s">
+      <c r="BH4" s="553"/>
+      <c r="BI4" s="553"/>
+      <c r="BJ4" s="553"/>
+      <c r="BK4" s="553"/>
+      <c r="BL4" s="552" t="s">
         <v>779</v>
       </c>
-      <c r="BM4" s="552"/>
-      <c r="BN4" s="552"/>
-      <c r="BO4" s="552"/>
-      <c r="BP4" s="552"/>
-      <c r="BQ4" s="553" t="s">
+      <c r="BM4" s="553"/>
+      <c r="BN4" s="553"/>
+      <c r="BO4" s="553"/>
+      <c r="BP4" s="553"/>
+      <c r="BQ4" s="552" t="s">
         <v>780</v>
       </c>
-      <c r="BR4" s="552"/>
-      <c r="BS4" s="552"/>
-      <c r="BT4" s="552"/>
+      <c r="BR4" s="553"/>
+      <c r="BS4" s="553"/>
+      <c r="BT4" s="553"/>
       <c r="BU4" s="554"/>
       <c r="BV4" s="357" t="s">
         <v>781</v>
@@ -62273,11 +62256,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="BL4:BP4"/>
-    <mergeCell ref="BQ4:BU4"/>
-    <mergeCell ref="BW4:CA4"/>
-    <mergeCell ref="CB4:CF4"/>
-    <mergeCell ref="CG4:CK4"/>
     <mergeCell ref="BG4:BK4"/>
     <mergeCell ref="D4:H4"/>
     <mergeCell ref="I4:M4"/>
@@ -62290,6 +62268,11 @@
     <mergeCell ref="AR4:AV4"/>
     <mergeCell ref="AW4:BA4"/>
     <mergeCell ref="BB4:BF4"/>
+    <mergeCell ref="BL4:BP4"/>
+    <mergeCell ref="BQ4:BU4"/>
+    <mergeCell ref="BW4:CA4"/>
+    <mergeCell ref="CB4:CF4"/>
+    <mergeCell ref="CG4:CK4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
Update Heating Sizes and Heat Pump Assumptions
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_RSD.xlsx
+++ b/SubRES_TMPL/SubRes_RSD.xlsx
@@ -3,10 +3,10 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCDCB22B-F78A-424F-B946-0527B4B28434}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EBDAEA6-17D6-476C-A557-480ECE119734}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="4" xr2:uid="{34F9D92C-266F-476D-89E0-63153305AC39}"/>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="4" xr2:uid="{7D8B849B-5E55-4ACE-8CF4-3734B2491195}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="4" xr2:uid="{7D8B849B-5E55-4ACE-8CF4-3734B2491195}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="34" r:id="rId1"/>
@@ -14492,6 +14492,7 @@
     <xf numFmtId="0" fontId="40" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="40" fillId="21" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="40" fillId="21" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="16" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -14534,6 +14535,15 @@
     <xf numFmtId="0" fontId="53" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="23" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -14541,15 +14551,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -14561,17 +14562,26 @@
     <xf numFmtId="0" fontId="16" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -14582,19 +14592,10 @@
     <xf numFmtId="0" fontId="69" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="60" fillId="31" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="60" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="31" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="60" fillId="31" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -14609,7 +14610,6 @@
     <xf numFmtId="0" fontId="60" fillId="32" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="16" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="20% - Colore 2" xfId="11" xr:uid="{3E3DAF22-4D86-48A9-B6EE-8D230C1E993C}"/>
@@ -16210,14 +16210,14 @@
       <c r="F16" s="211"/>
     </row>
     <row r="17" spans="1:14" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="520" t="s">
+      <c r="A17" s="521" t="s">
         <v>434</v>
       </c>
-      <c r="B17" s="520"/>
-      <c r="C17" s="520"/>
-      <c r="D17" s="520"/>
-      <c r="E17" s="520"/>
-      <c r="F17" s="520"/>
+      <c r="B17" s="521"/>
+      <c r="C17" s="521"/>
+      <c r="D17" s="521"/>
+      <c r="E17" s="521"/>
+      <c r="F17" s="521"/>
       <c r="G17" s="213"/>
       <c r="H17" s="213"/>
       <c r="I17" s="214"/>
@@ -16255,13 +16255,13 @@
       <c r="A20" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="521" t="s">
+      <c r="B20" s="522" t="s">
         <v>436</v>
       </c>
-      <c r="C20" s="521"/>
-      <c r="D20" s="521"/>
-      <c r="E20" s="521"/>
-      <c r="F20" s="521"/>
+      <c r="C20" s="522"/>
+      <c r="D20" s="522"/>
+      <c r="E20" s="522"/>
+      <c r="F20" s="522"/>
       <c r="G20" s="218"/>
       <c r="H20" s="218"/>
       <c r="I20" s="219"/>
@@ -16275,13 +16275,13 @@
       <c r="A21" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="522" t="s">
+      <c r="B21" s="523" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="522"/>
-      <c r="D21" s="522"/>
-      <c r="E21" s="522"/>
-      <c r="F21" s="522"/>
+      <c r="C21" s="523"/>
+      <c r="D21" s="523"/>
+      <c r="E21" s="523"/>
+      <c r="F21" s="523"/>
       <c r="G21" s="218"/>
       <c r="H21" s="218"/>
       <c r="I21" s="219"/>
@@ -16295,13 +16295,13 @@
       <c r="A22" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="522" t="s">
+      <c r="B22" s="523" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="522"/>
-      <c r="D22" s="522"/>
-      <c r="E22" s="522"/>
-      <c r="F22" s="522"/>
+      <c r="C22" s="523"/>
+      <c r="D22" s="523"/>
+      <c r="E22" s="523"/>
+      <c r="F22" s="523"/>
     </row>
     <row r="23" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
@@ -16330,22 +16330,22 @@
       <c r="H24" s="3"/>
     </row>
     <row r="25" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="523"/>
-      <c r="B25" s="523"/>
-      <c r="C25" s="523"/>
-      <c r="D25" s="523"/>
-      <c r="E25" s="523"/>
-      <c r="F25" s="523"/>
+      <c r="A25" s="524"/>
+      <c r="B25" s="524"/>
+      <c r="C25" s="524"/>
+      <c r="D25" s="524"/>
+      <c r="E25" s="524"/>
+      <c r="F25" s="524"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
     </row>
     <row r="26" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="519"/>
-      <c r="B26" s="519"/>
-      <c r="C26" s="519"/>
-      <c r="D26" s="519"/>
-      <c r="E26" s="519"/>
-      <c r="F26" s="519"/>
+      <c r="A26" s="520"/>
+      <c r="B26" s="520"/>
+      <c r="C26" s="520"/>
+      <c r="D26" s="520"/>
+      <c r="E26" s="520"/>
+      <c r="F26" s="520"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="211"/>
@@ -16533,16 +16533,16 @@
   <sheetData>
     <row r="1" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:20" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="524" t="s">
+      <c r="B2" s="525" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="525"/>
-      <c r="D2" s="525"/>
-      <c r="E2" s="526"/>
-      <c r="G2" s="524" t="s">
+      <c r="C2" s="526"/>
+      <c r="D2" s="526"/>
+      <c r="E2" s="527"/>
+      <c r="G2" s="525" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="526"/>
+      <c r="H2" s="527"/>
       <c r="I2" s="222"/>
       <c r="J2" s="222"/>
       <c r="K2" s="223"/>
@@ -16884,16 +16884,16 @@
     </row>
     <row r="19" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="2:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="527" t="s">
+      <c r="B20" s="528" t="s">
         <v>70</v>
       </c>
-      <c r="C20" s="528"/>
-      <c r="D20" s="528"/>
-      <c r="E20" s="529"/>
-      <c r="G20" s="524" t="s">
+      <c r="C20" s="529"/>
+      <c r="D20" s="529"/>
+      <c r="E20" s="530"/>
+      <c r="G20" s="525" t="s">
         <v>14</v>
       </c>
-      <c r="H20" s="526"/>
+      <c r="H20" s="527"/>
     </row>
     <row r="21" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="250" t="s">
@@ -17137,16 +17137,16 @@
     </row>
     <row r="37" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="38" spans="2:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="524" t="s">
+      <c r="B38" s="525" t="s">
         <v>78</v>
       </c>
-      <c r="C38" s="525"/>
-      <c r="D38" s="525"/>
-      <c r="E38" s="526"/>
-      <c r="G38" s="530" t="s">
+      <c r="C38" s="526"/>
+      <c r="D38" s="526"/>
+      <c r="E38" s="527"/>
+      <c r="G38" s="531" t="s">
         <v>72</v>
       </c>
-      <c r="H38" s="531"/>
+      <c r="H38" s="532"/>
     </row>
     <row r="39" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B39" s="271" t="s">
@@ -17316,13 +17316,13 @@
       <c r="M3" s="5" t="s">
         <v>390</v>
       </c>
-      <c r="S3" s="532" t="s">
+      <c r="S3" s="533" t="s">
         <v>680</v>
       </c>
-      <c r="T3" s="532"/>
-      <c r="U3" s="532"/>
-      <c r="V3" s="532"/>
-      <c r="W3" s="532"/>
+      <c r="T3" s="533"/>
+      <c r="U3" s="533"/>
+      <c r="V3" s="533"/>
+      <c r="W3" s="533"/>
     </row>
     <row r="4" spans="3:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C4" s="62" t="s">
@@ -25003,11 +25003,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{104F8057-C735-4662-BAA6-EEDCF7B57273}">
   <dimension ref="A2:AQ166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H132" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="O153" sqref="O153"/>
     </sheetView>
-    <sheetView tabSelected="1" topLeftCell="F23" zoomScale="70" zoomScaleNormal="70" workbookViewId="1">
-      <selection activeCell="AI127" sqref="AI127"/>
+    <sheetView tabSelected="1" topLeftCell="F72" zoomScale="70" zoomScaleNormal="70" workbookViewId="1">
+      <selection activeCell="AI71" sqref="AI71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -25171,34 +25171,34 @@
       <c r="G4" s="62" t="s">
         <v>317</v>
       </c>
-      <c r="H4" s="539" t="s">
+      <c r="H4" s="540" t="s">
         <v>720</v>
       </c>
-      <c r="I4" s="540"/>
-      <c r="J4" s="540"/>
-      <c r="K4" s="541"/>
-      <c r="L4" s="539" t="s">
+      <c r="I4" s="541"/>
+      <c r="J4" s="541"/>
+      <c r="K4" s="542"/>
+      <c r="L4" s="540" t="s">
         <v>319</v>
       </c>
-      <c r="M4" s="540"/>
-      <c r="N4" s="540"/>
-      <c r="O4" s="541"/>
-      <c r="P4" s="539" t="s">
+      <c r="M4" s="541"/>
+      <c r="N4" s="541"/>
+      <c r="O4" s="542"/>
+      <c r="P4" s="540" t="s">
         <v>320</v>
       </c>
-      <c r="Q4" s="540"/>
-      <c r="R4" s="540"/>
-      <c r="S4" s="541"/>
-      <c r="T4" s="539" t="s">
+      <c r="Q4" s="541"/>
+      <c r="R4" s="541"/>
+      <c r="S4" s="542"/>
+      <c r="T4" s="540" t="s">
         <v>321</v>
       </c>
-      <c r="U4" s="541"/>
-      <c r="V4" s="542" t="s">
+      <c r="U4" s="542"/>
+      <c r="V4" s="534" t="s">
         <v>322</v>
       </c>
-      <c r="W4" s="543"/>
-      <c r="X4" s="543"/>
-      <c r="Y4" s="544"/>
+      <c r="W4" s="535"/>
+      <c r="X4" s="535"/>
+      <c r="Y4" s="536"/>
       <c r="Z4" s="106"/>
       <c r="AA4" s="106"/>
       <c r="AB4" s="114" t="s">
@@ -25297,34 +25297,34 @@
       <c r="E6" s="84"/>
       <c r="F6" s="84"/>
       <c r="G6" s="85"/>
-      <c r="H6" s="533" t="s">
+      <c r="H6" s="537" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="534"/>
-      <c r="J6" s="534"/>
-      <c r="K6" s="535"/>
-      <c r="L6" s="534" t="s">
+      <c r="I6" s="538"/>
+      <c r="J6" s="538"/>
+      <c r="K6" s="539"/>
+      <c r="L6" s="538" t="s">
         <v>45</v>
       </c>
-      <c r="M6" s="534"/>
-      <c r="N6" s="534"/>
-      <c r="O6" s="535"/>
-      <c r="P6" s="533" t="s">
+      <c r="M6" s="538"/>
+      <c r="N6" s="538"/>
+      <c r="O6" s="539"/>
+      <c r="P6" s="537" t="s">
         <v>45</v>
       </c>
-      <c r="Q6" s="534"/>
-      <c r="R6" s="534"/>
-      <c r="S6" s="535"/>
-      <c r="T6" s="533" t="s">
+      <c r="Q6" s="538"/>
+      <c r="R6" s="538"/>
+      <c r="S6" s="539"/>
+      <c r="T6" s="537" t="s">
         <v>302</v>
       </c>
-      <c r="U6" s="535"/>
-      <c r="V6" s="533" t="s">
+      <c r="U6" s="539"/>
+      <c r="V6" s="537" t="s">
         <v>968</v>
       </c>
-      <c r="W6" s="534"/>
-      <c r="X6" s="534"/>
-      <c r="Y6" s="535"/>
+      <c r="W6" s="538"/>
+      <c r="X6" s="538"/>
+      <c r="Y6" s="539"/>
       <c r="Z6" s="107" t="s">
         <v>980</v>
       </c>
@@ -28234,34 +28234,34 @@
       <c r="G42" s="62" t="s">
         <v>317</v>
       </c>
-      <c r="H42" s="539" t="s">
+      <c r="H42" s="540" t="s">
         <v>318</v>
       </c>
-      <c r="I42" s="540"/>
-      <c r="J42" s="540"/>
-      <c r="K42" s="541"/>
-      <c r="L42" s="539" t="s">
+      <c r="I42" s="541"/>
+      <c r="J42" s="541"/>
+      <c r="K42" s="542"/>
+      <c r="L42" s="540" t="s">
         <v>319</v>
       </c>
-      <c r="M42" s="540"/>
-      <c r="N42" s="540"/>
-      <c r="O42" s="541"/>
-      <c r="P42" s="539" t="s">
+      <c r="M42" s="541"/>
+      <c r="N42" s="541"/>
+      <c r="O42" s="542"/>
+      <c r="P42" s="540" t="s">
         <v>320</v>
       </c>
-      <c r="Q42" s="540"/>
-      <c r="R42" s="540"/>
-      <c r="S42" s="541"/>
-      <c r="T42" s="539" t="s">
+      <c r="Q42" s="541"/>
+      <c r="R42" s="541"/>
+      <c r="S42" s="542"/>
+      <c r="T42" s="540" t="s">
         <v>321</v>
       </c>
-      <c r="U42" s="541"/>
-      <c r="V42" s="542" t="s">
+      <c r="U42" s="542"/>
+      <c r="V42" s="534" t="s">
         <v>322</v>
       </c>
-      <c r="W42" s="543"/>
-      <c r="X42" s="543"/>
-      <c r="Y42" s="544"/>
+      <c r="W42" s="535"/>
+      <c r="X42" s="535"/>
+      <c r="Y42" s="536"/>
       <c r="Z42" s="106"/>
       <c r="AA42" s="106"/>
       <c r="AB42" s="114" t="s">
@@ -28360,34 +28360,34 @@
       <c r="E44" s="84"/>
       <c r="F44" s="84"/>
       <c r="G44" s="85"/>
-      <c r="H44" s="533" t="s">
+      <c r="H44" s="537" t="s">
         <v>45</v>
       </c>
-      <c r="I44" s="534"/>
-      <c r="J44" s="534"/>
-      <c r="K44" s="535"/>
-      <c r="L44" s="534" t="s">
+      <c r="I44" s="538"/>
+      <c r="J44" s="538"/>
+      <c r="K44" s="539"/>
+      <c r="L44" s="538" t="s">
         <v>45</v>
       </c>
-      <c r="M44" s="534"/>
-      <c r="N44" s="534"/>
-      <c r="O44" s="535"/>
-      <c r="P44" s="533" t="s">
+      <c r="M44" s="538"/>
+      <c r="N44" s="538"/>
+      <c r="O44" s="539"/>
+      <c r="P44" s="537" t="s">
         <v>45</v>
       </c>
-      <c r="Q44" s="534"/>
-      <c r="R44" s="534"/>
-      <c r="S44" s="535"/>
-      <c r="T44" s="536" t="s">
+      <c r="Q44" s="538"/>
+      <c r="R44" s="538"/>
+      <c r="S44" s="539"/>
+      <c r="T44" s="543" t="s">
         <v>302</v>
       </c>
-      <c r="U44" s="537"/>
-      <c r="V44" s="536" t="s">
+      <c r="U44" s="544"/>
+      <c r="V44" s="543" t="s">
         <v>968</v>
       </c>
-      <c r="W44" s="538"/>
-      <c r="X44" s="538"/>
-      <c r="Y44" s="537"/>
+      <c r="W44" s="545"/>
+      <c r="X44" s="545"/>
+      <c r="Y44" s="544"/>
       <c r="Z44" s="450" t="s">
         <v>980</v>
       </c>
@@ -29712,7 +29712,7 @@
       <c r="W57" s="457"/>
       <c r="X57" s="457"/>
       <c r="Y57" s="457"/>
-      <c r="Z57" s="558"/>
+      <c r="Z57" s="519"/>
       <c r="AA57" s="112"/>
       <c r="AB57" s="90"/>
       <c r="AC57" s="119"/>
@@ -29779,7 +29779,7 @@
       <c r="W58" s="457"/>
       <c r="X58" s="457"/>
       <c r="Y58" s="457"/>
-      <c r="Z58" s="558"/>
+      <c r="Z58" s="519"/>
       <c r="AA58" s="112"/>
       <c r="AB58" s="90"/>
       <c r="AC58" s="119"/>
@@ -30414,14 +30414,14 @@
       <c r="AE65" s="109"/>
       <c r="AF65" s="109">
         <f t="shared" si="26"/>
-        <v>0.25228800000000001</v>
+        <v>0.26805600000000002</v>
       </c>
       <c r="AG65" s="112"/>
       <c r="AH65" s="112">
         <v>2100</v>
       </c>
       <c r="AI65" s="112">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="AK65" s="152"/>
       <c r="AL65" s="151" t="str">
@@ -30623,14 +30623,14 @@
       <c r="AE67" s="109"/>
       <c r="AF67" s="109">
         <f t="shared" si="26"/>
-        <v>0.25228800000000001</v>
+        <v>0.26805600000000002</v>
       </c>
       <c r="AG67" s="112"/>
       <c r="AH67" s="112">
         <v>2019</v>
       </c>
       <c r="AI67" s="112">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="AK67" s="286"/>
       <c r="AL67" s="151" t="str">
@@ -30736,14 +30736,14 @@
       </c>
       <c r="AF68" s="108">
         <f t="shared" si="26"/>
-        <v>0.25228800000000001</v>
+        <v>0.26805600000000002</v>
       </c>
       <c r="AG68" s="111"/>
       <c r="AH68" s="111">
         <v>2019</v>
       </c>
       <c r="AI68" s="111">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="AK68" s="158"/>
       <c r="AL68" s="154" t="str">
@@ -30950,14 +30950,14 @@
       <c r="AE70" s="132"/>
       <c r="AF70" s="132">
         <f t="shared" si="26"/>
-        <v>0.25228800000000001</v>
+        <v>0.26805600000000002</v>
       </c>
       <c r="AG70" s="137"/>
       <c r="AH70" s="137">
         <v>2019</v>
       </c>
       <c r="AI70" s="137">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="AK70" s="287"/>
       <c r="AL70" s="154" t="str">
@@ -31404,7 +31404,7 @@
       </c>
       <c r="AF75" s="128">
         <f t="shared" si="26"/>
-        <v>0.41312159999999998</v>
+        <v>0.42415920000000001</v>
       </c>
       <c r="AG75" s="129"/>
       <c r="AH75" s="129">
@@ -31412,7 +31412,7 @@
       </c>
       <c r="AI75" s="129">
         <f>AI50*AD75+AI68*(1-AD75)</f>
-        <v>13.1</v>
+        <v>13.45</v>
       </c>
       <c r="AK75" s="4"/>
       <c r="AL75" s="151" t="str">
@@ -32094,34 +32094,34 @@
       <c r="G90" s="62" t="s">
         <v>317</v>
       </c>
-      <c r="H90" s="539" t="s">
+      <c r="H90" s="540" t="s">
         <v>318</v>
       </c>
-      <c r="I90" s="540"/>
-      <c r="J90" s="540"/>
-      <c r="K90" s="541"/>
-      <c r="L90" s="539" t="s">
+      <c r="I90" s="541"/>
+      <c r="J90" s="541"/>
+      <c r="K90" s="542"/>
+      <c r="L90" s="540" t="s">
         <v>319</v>
       </c>
-      <c r="M90" s="540"/>
-      <c r="N90" s="540"/>
-      <c r="O90" s="541"/>
-      <c r="P90" s="539" t="s">
+      <c r="M90" s="541"/>
+      <c r="N90" s="541"/>
+      <c r="O90" s="542"/>
+      <c r="P90" s="540" t="s">
         <v>320</v>
       </c>
-      <c r="Q90" s="540"/>
-      <c r="R90" s="540"/>
-      <c r="S90" s="541"/>
-      <c r="T90" s="539" t="s">
+      <c r="Q90" s="541"/>
+      <c r="R90" s="541"/>
+      <c r="S90" s="542"/>
+      <c r="T90" s="540" t="s">
         <v>321</v>
       </c>
-      <c r="U90" s="541"/>
-      <c r="V90" s="542" t="s">
+      <c r="U90" s="542"/>
+      <c r="V90" s="534" t="s">
         <v>322</v>
       </c>
-      <c r="W90" s="543"/>
-      <c r="X90" s="543"/>
-      <c r="Y90" s="544"/>
+      <c r="W90" s="535"/>
+      <c r="X90" s="535"/>
+      <c r="Y90" s="536"/>
       <c r="Z90" s="106"/>
       <c r="AA90" s="106"/>
       <c r="AB90" s="114" t="s">
@@ -32220,34 +32220,34 @@
       <c r="E92" s="84"/>
       <c r="F92" s="84"/>
       <c r="G92" s="85"/>
-      <c r="H92" s="533" t="s">
+      <c r="H92" s="537" t="s">
         <v>45</v>
       </c>
-      <c r="I92" s="534"/>
-      <c r="J92" s="534"/>
-      <c r="K92" s="535"/>
-      <c r="L92" s="534" t="s">
+      <c r="I92" s="538"/>
+      <c r="J92" s="538"/>
+      <c r="K92" s="539"/>
+      <c r="L92" s="538" t="s">
         <v>45</v>
       </c>
-      <c r="M92" s="534"/>
-      <c r="N92" s="534"/>
-      <c r="O92" s="535"/>
-      <c r="P92" s="533" t="s">
+      <c r="M92" s="538"/>
+      <c r="N92" s="538"/>
+      <c r="O92" s="539"/>
+      <c r="P92" s="537" t="s">
         <v>45</v>
       </c>
-      <c r="Q92" s="534"/>
-      <c r="R92" s="534"/>
-      <c r="S92" s="535"/>
-      <c r="T92" s="536" t="s">
+      <c r="Q92" s="538"/>
+      <c r="R92" s="538"/>
+      <c r="S92" s="539"/>
+      <c r="T92" s="543" t="s">
         <v>302</v>
       </c>
-      <c r="U92" s="537"/>
-      <c r="V92" s="536" t="s">
+      <c r="U92" s="544"/>
+      <c r="V92" s="543" t="s">
         <v>968</v>
       </c>
-      <c r="W92" s="538"/>
-      <c r="X92" s="538"/>
-      <c r="Y92" s="537"/>
+      <c r="W92" s="545"/>
+      <c r="X92" s="545"/>
+      <c r="Y92" s="544"/>
       <c r="Z92" s="450" t="s">
         <v>980</v>
       </c>
@@ -33572,7 +33572,7 @@
       <c r="W105" s="457"/>
       <c r="X105" s="457"/>
       <c r="Y105" s="457"/>
-      <c r="Z105" s="558"/>
+      <c r="Z105" s="519"/>
       <c r="AA105" s="112"/>
       <c r="AB105" s="90"/>
       <c r="AC105" s="119"/>
@@ -33639,7 +33639,7 @@
       <c r="W106" s="457"/>
       <c r="X106" s="457"/>
       <c r="Y106" s="457"/>
-      <c r="Z106" s="558"/>
+      <c r="Z106" s="519"/>
       <c r="AA106" s="112"/>
       <c r="AB106" s="90"/>
       <c r="AC106" s="119"/>
@@ -36112,6 +36112,26 @@
     <row r="166" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="H92:K92"/>
+    <mergeCell ref="L92:O92"/>
+    <mergeCell ref="P92:S92"/>
+    <mergeCell ref="T92:U92"/>
+    <mergeCell ref="V92:Y92"/>
+    <mergeCell ref="H90:K90"/>
+    <mergeCell ref="L90:O90"/>
+    <mergeCell ref="P90:S90"/>
+    <mergeCell ref="T90:U90"/>
+    <mergeCell ref="V90:Y90"/>
+    <mergeCell ref="H44:K44"/>
+    <mergeCell ref="L44:O44"/>
+    <mergeCell ref="P44:S44"/>
+    <mergeCell ref="T44:U44"/>
+    <mergeCell ref="V44:Y44"/>
+    <mergeCell ref="H42:K42"/>
+    <mergeCell ref="L42:O42"/>
+    <mergeCell ref="P42:S42"/>
+    <mergeCell ref="T42:U42"/>
+    <mergeCell ref="V42:Y42"/>
     <mergeCell ref="V4:Y4"/>
     <mergeCell ref="V6:Y6"/>
     <mergeCell ref="H4:K4"/>
@@ -36122,26 +36142,6 @@
     <mergeCell ref="P6:S6"/>
     <mergeCell ref="L6:O6"/>
     <mergeCell ref="H6:K6"/>
-    <mergeCell ref="H42:K42"/>
-    <mergeCell ref="L42:O42"/>
-    <mergeCell ref="P42:S42"/>
-    <mergeCell ref="T42:U42"/>
-    <mergeCell ref="V42:Y42"/>
-    <mergeCell ref="H44:K44"/>
-    <mergeCell ref="L44:O44"/>
-    <mergeCell ref="P44:S44"/>
-    <mergeCell ref="T44:U44"/>
-    <mergeCell ref="V44:Y44"/>
-    <mergeCell ref="H90:K90"/>
-    <mergeCell ref="L90:O90"/>
-    <mergeCell ref="P90:S90"/>
-    <mergeCell ref="T90:U90"/>
-    <mergeCell ref="V90:Y90"/>
-    <mergeCell ref="H92:K92"/>
-    <mergeCell ref="L92:O92"/>
-    <mergeCell ref="P92:S92"/>
-    <mergeCell ref="T92:U92"/>
-    <mergeCell ref="V92:Y92"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
@@ -36287,12 +36287,12 @@
       <c r="I5" s="173"/>
       <c r="J5" s="173"/>
       <c r="K5" s="173"/>
-      <c r="L5" s="542" t="s">
+      <c r="L5" s="534" t="s">
         <v>322</v>
       </c>
-      <c r="M5" s="543"/>
-      <c r="N5" s="543"/>
-      <c r="O5" s="544"/>
+      <c r="M5" s="535"/>
+      <c r="N5" s="535"/>
+      <c r="O5" s="536"/>
       <c r="P5" s="106"/>
       <c r="Q5" s="106" t="s">
         <v>323</v>
@@ -36323,12 +36323,12 @@
       <c r="I6" s="83"/>
       <c r="J6" s="83"/>
       <c r="K6" s="83"/>
-      <c r="L6" s="536" t="s">
+      <c r="L6" s="543" t="s">
         <v>968</v>
       </c>
-      <c r="M6" s="538"/>
-      <c r="N6" s="538"/>
-      <c r="O6" s="537"/>
+      <c r="M6" s="545"/>
+      <c r="N6" s="545"/>
+      <c r="O6" s="544"/>
       <c r="P6" s="450" t="s">
         <v>980</v>
       </c>
@@ -36954,10 +36954,10 @@
       <c r="C18" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="R18" s="545" t="s">
+      <c r="R18" s="546" t="s">
         <v>662</v>
       </c>
-      <c r="S18" s="545"/>
+      <c r="S18" s="546"/>
       <c r="U18" s="5" t="s">
         <v>861</v>
       </c>
@@ -36990,8 +36990,8 @@
       <c r="J19" s="195" t="s">
         <v>301</v>
       </c>
-      <c r="R19" s="545"/>
-      <c r="S19" s="545"/>
+      <c r="R19" s="546"/>
+      <c r="S19" s="546"/>
       <c r="V19" s="5" t="s">
         <v>1023</v>
       </c>
@@ -37017,8 +37017,8 @@
       <c r="J20" s="170" t="s">
         <v>1028</v>
       </c>
-      <c r="R20" s="545"/>
-      <c r="S20" s="545"/>
+      <c r="R20" s="546"/>
+      <c r="S20" s="546"/>
       <c r="V20" s="5" t="s">
         <v>1024</v>
       </c>
@@ -37045,8 +37045,8 @@
       <c r="J21" s="170" t="s">
         <v>1028</v>
       </c>
-      <c r="R21" s="545"/>
-      <c r="S21" s="545"/>
+      <c r="R21" s="546"/>
+      <c r="S21" s="546"/>
     </row>
     <row r="22" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C22" s="168" t="s">
@@ -37070,8 +37070,8 @@
       <c r="J22" s="170" t="s">
         <v>1028</v>
       </c>
-      <c r="R22" s="545"/>
-      <c r="S22" s="545"/>
+      <c r="R22" s="546"/>
+      <c r="S22" s="546"/>
     </row>
     <row r="23" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C23" s="168" t="s">
@@ -37246,23 +37246,23 @@
       <c r="K33" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="L33" s="542" t="s">
+      <c r="L33" s="534" t="s">
         <v>322</v>
       </c>
-      <c r="M33" s="543"/>
-      <c r="N33" s="543"/>
-      <c r="O33" s="544"/>
+      <c r="M33" s="535"/>
+      <c r="N33" s="535"/>
+      <c r="O33" s="536"/>
     </row>
     <row r="34" spans="8:15" x14ac:dyDescent="0.2">
       <c r="H34" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="L34" s="536" t="s">
+      <c r="L34" s="543" t="s">
         <v>327</v>
       </c>
-      <c r="M34" s="538"/>
-      <c r="N34" s="538"/>
-      <c r="O34" s="537"/>
+      <c r="M34" s="545"/>
+      <c r="N34" s="545"/>
+      <c r="O34" s="544"/>
     </row>
     <row r="35" spans="8:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H35" s="5" t="s">
@@ -37605,16 +37605,16 @@
       <c r="G4" s="173" t="s">
         <v>321</v>
       </c>
-      <c r="H4" s="539" t="s">
+      <c r="H4" s="540" t="s">
         <v>110</v>
       </c>
-      <c r="I4" s="540"/>
-      <c r="J4" s="541"/>
-      <c r="K4" s="542" t="s">
+      <c r="I4" s="541"/>
+      <c r="J4" s="542"/>
+      <c r="K4" s="534" t="s">
         <v>322</v>
       </c>
-      <c r="L4" s="543"/>
-      <c r="M4" s="544"/>
+      <c r="L4" s="535"/>
+      <c r="M4" s="536"/>
       <c r="N4" s="106"/>
       <c r="O4" s="106" t="s">
         <v>323</v>
@@ -37640,16 +37640,16 @@
       <c r="G5" s="458" t="s">
         <v>302</v>
       </c>
-      <c r="H5" s="549" t="s">
+      <c r="H5" s="547" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="550"/>
-      <c r="J5" s="551"/>
-      <c r="K5" s="549" t="s">
+      <c r="I5" s="548"/>
+      <c r="J5" s="549"/>
+      <c r="K5" s="547" t="s">
         <v>757</v>
       </c>
-      <c r="L5" s="550"/>
-      <c r="M5" s="551"/>
+      <c r="L5" s="548"/>
+      <c r="M5" s="549"/>
       <c r="N5" s="459" t="s">
         <v>328</v>
       </c>
@@ -37666,23 +37666,23 @@
         <v>626</v>
       </c>
       <c r="AA5" s="281"/>
-      <c r="AB5" s="546" t="s">
+      <c r="AB5" s="550" t="s">
         <v>1013</v>
       </c>
-      <c r="AC5" s="546"/>
+      <c r="AC5" s="550"/>
       <c r="AD5" s="461"/>
-      <c r="AE5" s="547" t="s">
+      <c r="AE5" s="551" t="s">
         <v>110</v>
       </c>
-      <c r="AF5" s="547"/>
-      <c r="AG5" s="547" t="s">
+      <c r="AF5" s="551"/>
+      <c r="AG5" s="551" t="s">
         <v>1014</v>
       </c>
-      <c r="AH5" s="547"/>
-      <c r="AI5" s="548" t="s">
+      <c r="AH5" s="551"/>
+      <c r="AI5" s="552" t="s">
         <v>1015</v>
       </c>
-      <c r="AJ5" s="548"/>
+      <c r="AJ5" s="552"/>
     </row>
     <row r="6" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C6" s="505" t="str">
@@ -38420,12 +38420,12 @@
       <c r="K27" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="L27" s="542" t="s">
+      <c r="L27" s="534" t="s">
         <v>322</v>
       </c>
-      <c r="M27" s="543"/>
-      <c r="N27" s="543"/>
-      <c r="O27" s="544"/>
+      <c r="M27" s="535"/>
+      <c r="N27" s="535"/>
+      <c r="O27" s="536"/>
       <c r="T27" s="283"/>
       <c r="U27" s="283"/>
     </row>
@@ -38433,12 +38433,12 @@
       <c r="J28" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="L28" s="533" t="s">
+      <c r="L28" s="537" t="s">
         <v>327</v>
       </c>
-      <c r="M28" s="534"/>
-      <c r="N28" s="534"/>
-      <c r="O28" s="535"/>
+      <c r="M28" s="538"/>
+      <c r="N28" s="538"/>
+      <c r="O28" s="539"/>
       <c r="T28" s="283"/>
       <c r="U28" s="283"/>
     </row>
@@ -39828,16 +39828,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="AB5:AC5"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AG5:AH5"/>
+    <mergeCell ref="AI5:AJ5"/>
+    <mergeCell ref="L27:O27"/>
     <mergeCell ref="L28:O28"/>
     <mergeCell ref="H4:J4"/>
     <mergeCell ref="K4:M4"/>
     <mergeCell ref="H5:J5"/>
     <mergeCell ref="K5:M5"/>
-    <mergeCell ref="AB5:AC5"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="AG5:AH5"/>
-    <mergeCell ref="AI5:AJ5"/>
-    <mergeCell ref="L27:O27"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="S7" r:id="rId1" xr:uid="{B1EDD63D-40A5-4174-9D28-8666BD314B83}"/>
@@ -48872,125 +48872,125 @@
       <c r="D4" s="553" t="s">
         <v>767</v>
       </c>
-      <c r="E4" s="552"/>
-      <c r="F4" s="552"/>
-      <c r="G4" s="552"/>
-      <c r="H4" s="554"/>
-      <c r="I4" s="552" t="s">
+      <c r="E4" s="554"/>
+      <c r="F4" s="554"/>
+      <c r="G4" s="554"/>
+      <c r="H4" s="555"/>
+      <c r="I4" s="554" t="s">
         <v>768</v>
       </c>
-      <c r="J4" s="552"/>
-      <c r="K4" s="552"/>
-      <c r="L4" s="552"/>
-      <c r="M4" s="554"/>
-      <c r="N4" s="552" t="s">
+      <c r="J4" s="554"/>
+      <c r="K4" s="554"/>
+      <c r="L4" s="554"/>
+      <c r="M4" s="555"/>
+      <c r="N4" s="554" t="s">
         <v>769</v>
       </c>
-      <c r="O4" s="552"/>
-      <c r="P4" s="552"/>
-      <c r="Q4" s="552"/>
-      <c r="R4" s="554"/>
-      <c r="S4" s="552" t="s">
+      <c r="O4" s="554"/>
+      <c r="P4" s="554"/>
+      <c r="Q4" s="554"/>
+      <c r="R4" s="555"/>
+      <c r="S4" s="554" t="s">
         <v>770</v>
       </c>
-      <c r="T4" s="552"/>
-      <c r="U4" s="552"/>
-      <c r="V4" s="552"/>
-      <c r="W4" s="554"/>
-      <c r="X4" s="552" t="s">
+      <c r="T4" s="554"/>
+      <c r="U4" s="554"/>
+      <c r="V4" s="554"/>
+      <c r="W4" s="555"/>
+      <c r="X4" s="554" t="s">
         <v>771</v>
       </c>
-      <c r="Y4" s="552"/>
-      <c r="Z4" s="552"/>
-      <c r="AA4" s="552"/>
-      <c r="AB4" s="554"/>
-      <c r="AC4" s="552" t="s">
+      <c r="Y4" s="554"/>
+      <c r="Z4" s="554"/>
+      <c r="AA4" s="554"/>
+      <c r="AB4" s="555"/>
+      <c r="AC4" s="554" t="s">
         <v>772</v>
       </c>
-      <c r="AD4" s="552"/>
-      <c r="AE4" s="552"/>
-      <c r="AF4" s="552"/>
-      <c r="AG4" s="554"/>
-      <c r="AH4" s="552" t="s">
+      <c r="AD4" s="554"/>
+      <c r="AE4" s="554"/>
+      <c r="AF4" s="554"/>
+      <c r="AG4" s="555"/>
+      <c r="AH4" s="554" t="s">
         <v>773</v>
       </c>
-      <c r="AI4" s="552"/>
-      <c r="AJ4" s="552"/>
-      <c r="AK4" s="552"/>
-      <c r="AL4" s="554"/>
-      <c r="AM4" s="552" t="s">
+      <c r="AI4" s="554"/>
+      <c r="AJ4" s="554"/>
+      <c r="AK4" s="554"/>
+      <c r="AL4" s="555"/>
+      <c r="AM4" s="554" t="s">
         <v>774</v>
       </c>
-      <c r="AN4" s="552"/>
-      <c r="AO4" s="552"/>
-      <c r="AP4" s="552"/>
-      <c r="AQ4" s="554"/>
-      <c r="AR4" s="552" t="s">
+      <c r="AN4" s="554"/>
+      <c r="AO4" s="554"/>
+      <c r="AP4" s="554"/>
+      <c r="AQ4" s="555"/>
+      <c r="AR4" s="554" t="s">
         <v>775</v>
       </c>
-      <c r="AS4" s="552"/>
-      <c r="AT4" s="552"/>
-      <c r="AU4" s="552"/>
-      <c r="AV4" s="554"/>
-      <c r="AW4" s="552" t="s">
+      <c r="AS4" s="554"/>
+      <c r="AT4" s="554"/>
+      <c r="AU4" s="554"/>
+      <c r="AV4" s="555"/>
+      <c r="AW4" s="554" t="s">
         <v>776</v>
       </c>
-      <c r="AX4" s="552"/>
-      <c r="AY4" s="552"/>
-      <c r="AZ4" s="552"/>
-      <c r="BA4" s="552"/>
+      <c r="AX4" s="554"/>
+      <c r="AY4" s="554"/>
+      <c r="AZ4" s="554"/>
+      <c r="BA4" s="554"/>
       <c r="BB4" s="553" t="s">
         <v>777</v>
       </c>
-      <c r="BC4" s="552"/>
-      <c r="BD4" s="552"/>
-      <c r="BE4" s="552"/>
-      <c r="BF4" s="554"/>
-      <c r="BG4" s="552" t="s">
+      <c r="BC4" s="554"/>
+      <c r="BD4" s="554"/>
+      <c r="BE4" s="554"/>
+      <c r="BF4" s="555"/>
+      <c r="BG4" s="554" t="s">
         <v>778</v>
       </c>
-      <c r="BH4" s="552"/>
-      <c r="BI4" s="552"/>
-      <c r="BJ4" s="552"/>
-      <c r="BK4" s="552"/>
+      <c r="BH4" s="554"/>
+      <c r="BI4" s="554"/>
+      <c r="BJ4" s="554"/>
+      <c r="BK4" s="554"/>
       <c r="BL4" s="553" t="s">
         <v>779</v>
       </c>
-      <c r="BM4" s="552"/>
-      <c r="BN4" s="552"/>
-      <c r="BO4" s="552"/>
-      <c r="BP4" s="552"/>
+      <c r="BM4" s="554"/>
+      <c r="BN4" s="554"/>
+      <c r="BO4" s="554"/>
+      <c r="BP4" s="554"/>
       <c r="BQ4" s="553" t="s">
         <v>780</v>
       </c>
-      <c r="BR4" s="552"/>
-      <c r="BS4" s="552"/>
-      <c r="BT4" s="552"/>
-      <c r="BU4" s="554"/>
+      <c r="BR4" s="554"/>
+      <c r="BS4" s="554"/>
+      <c r="BT4" s="554"/>
+      <c r="BU4" s="555"/>
       <c r="BV4" s="357" t="s">
         <v>781</v>
       </c>
-      <c r="BW4" s="555" t="s">
+      <c r="BW4" s="556" t="s">
         <v>782</v>
       </c>
-      <c r="BX4" s="556"/>
-      <c r="BY4" s="556"/>
-      <c r="BZ4" s="556"/>
-      <c r="CA4" s="557"/>
-      <c r="CB4" s="555" t="s">
+      <c r="BX4" s="557"/>
+      <c r="BY4" s="557"/>
+      <c r="BZ4" s="557"/>
+      <c r="CA4" s="558"/>
+      <c r="CB4" s="556" t="s">
         <v>783</v>
       </c>
-      <c r="CC4" s="556"/>
-      <c r="CD4" s="556"/>
-      <c r="CE4" s="556"/>
-      <c r="CF4" s="557"/>
-      <c r="CG4" s="555" t="s">
+      <c r="CC4" s="557"/>
+      <c r="CD4" s="557"/>
+      <c r="CE4" s="557"/>
+      <c r="CF4" s="558"/>
+      <c r="CG4" s="556" t="s">
         <v>784</v>
       </c>
-      <c r="CH4" s="556"/>
-      <c r="CI4" s="556"/>
-      <c r="CJ4" s="556"/>
-      <c r="CK4" s="557"/>
+      <c r="CH4" s="557"/>
+      <c r="CI4" s="557"/>
+      <c r="CJ4" s="557"/>
+      <c r="CK4" s="558"/>
     </row>
     <row r="5" spans="1:89" x14ac:dyDescent="0.2">
       <c r="A5" s="359"/>
@@ -62559,11 +62559,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="BL4:BP4"/>
-    <mergeCell ref="BQ4:BU4"/>
-    <mergeCell ref="BW4:CA4"/>
-    <mergeCell ref="CB4:CF4"/>
-    <mergeCell ref="CG4:CK4"/>
     <mergeCell ref="BG4:BK4"/>
     <mergeCell ref="D4:H4"/>
     <mergeCell ref="I4:M4"/>
@@ -62576,6 +62571,11 @@
     <mergeCell ref="AR4:AV4"/>
     <mergeCell ref="AW4:BA4"/>
     <mergeCell ref="BB4:BF4"/>
+    <mergeCell ref="BL4:BP4"/>
+    <mergeCell ref="BQ4:BU4"/>
+    <mergeCell ref="BW4:CA4"/>
+    <mergeCell ref="CB4:CF4"/>
+    <mergeCell ref="CG4:CK4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
Dummys - Update of New PJ/000 dwelllings
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_RSD.xlsx
+++ b/SubRES_TMPL/SubRes_RSD.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96EA81A1-9719-4C97-9A90-A66FDE4CC55E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7FD2507-CF56-44ED-9C2A-BB2CAE4A9C53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{34F9D92C-266F-476D-89E0-63153305AC39}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{34F9D92C-266F-476D-89E0-63153305AC39}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="34" r:id="rId1"/>
@@ -8611,7 +8611,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3505" uniqueCount="1044">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3509" uniqueCount="1046">
   <si>
     <t>Document type:</t>
   </si>
@@ -11764,6 +11764,12 @@
   </si>
   <si>
     <t>*R-SW_Det_FPL_N1</t>
+  </si>
+  <si>
+    <t>Lights</t>
+  </si>
+  <si>
+    <t>P&amp;F</t>
   </si>
 </sst>
 </file>
@@ -13489,7 +13495,7 @@
     <xf numFmtId="0" fontId="39" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="54" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="559">
+  <cellXfs count="560">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -14534,6 +14540,15 @@
     <xf numFmtId="0" fontId="53" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="23" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -14541,15 +14556,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -14561,17 +14567,26 @@
     <xf numFmtId="0" fontId="16" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -14582,19 +14597,10 @@
     <xf numFmtId="0" fontId="69" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="60" fillId="31" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="60" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="31" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="60" fillId="31" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -14608,6 +14614,9 @@
     </xf>
     <xf numFmtId="0" fontId="60" fillId="32" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="16">
@@ -17246,10 +17255,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4660B878-9B9C-4131-8EFF-29EF25ED69C5}">
-  <dimension ref="A2:AM103"/>
+  <dimension ref="A2:AL103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -17448,8 +17457,8 @@
       <c r="G7" s="71"/>
       <c r="H7" s="109"/>
       <c r="I7" s="314">
-        <f>AL22/2</f>
-        <v>5.3083202991120108E-4</v>
+        <f>(AK23*N11)/2</f>
+        <v>2.1494423184792772E-4</v>
       </c>
       <c r="J7" s="103"/>
       <c r="S7" s="300" t="s">
@@ -17478,8 +17487,8 @@
       <c r="G8" s="87"/>
       <c r="H8" s="108"/>
       <c r="I8" s="315">
-        <f>AJ22</f>
-        <v>3.2672173235706492E-3</v>
+        <f>AI23</f>
+        <v>7.9109298846992832E-3</v>
       </c>
       <c r="J8" s="104"/>
       <c r="S8" s="297" t="s">
@@ -17498,7 +17507,7 @@
         <v>123159.54010496697</v>
       </c>
     </row>
-    <row r="9" spans="3:23" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="3:23" ht="21.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C9" s="109"/>
       <c r="D9" s="109"/>
       <c r="E9" s="70" t="s">
@@ -17508,10 +17517,16 @@
       <c r="G9" s="71"/>
       <c r="H9" s="109"/>
       <c r="I9" s="314">
-        <f>AK22</f>
-        <v>1.4074238978033962E-3</v>
+        <f>AJ22*N10</f>
+        <v>5.6296955912135845E-4</v>
       </c>
       <c r="J9" s="103"/>
+      <c r="M9" s="559" t="s">
+        <v>110</v>
+      </c>
+      <c r="N9" s="559" t="s">
+        <v>110</v>
+      </c>
       <c r="S9" s="300" t="s">
         <v>669</v>
       </c>
@@ -17528,7 +17543,7 @@
         <v>592375.26452582516</v>
       </c>
     </row>
-    <row r="10" spans="3:23" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="3:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C10" s="132"/>
       <c r="D10" s="132"/>
       <c r="E10" s="165" t="s">
@@ -17538,10 +17553,16 @@
       <c r="G10" s="166"/>
       <c r="H10" s="132"/>
       <c r="I10" s="316">
-        <f>AL22/2</f>
-        <v>5.3083202991120108E-4</v>
+        <f>(AK23*N11)/2</f>
+        <v>2.1494423184792772E-4</v>
       </c>
       <c r="J10" s="141"/>
+      <c r="M10" s="291" t="s">
+        <v>1044</v>
+      </c>
+      <c r="N10" s="292">
+        <v>0.4</v>
+      </c>
       <c r="S10" s="297" t="s">
         <v>670</v>
       </c>
@@ -17573,6 +17594,12 @@
       <c r="J11" s="107" t="s">
         <v>330</v>
       </c>
+      <c r="M11" s="294" t="s">
+        <v>1045</v>
+      </c>
+      <c r="N11" s="295">
+        <v>0.6</v>
+      </c>
       <c r="S11" s="300" t="s">
         <v>671</v>
       </c>
@@ -17611,8 +17638,8 @@
         <v>100</v>
       </c>
       <c r="I12" s="313">
-        <f>AH37</f>
-        <v>9.510263559994104E-4</v>
+        <f>AH38</f>
+        <v>1.0242117509517548E-2</v>
       </c>
       <c r="J12" s="188">
         <v>2020</v>
@@ -17643,8 +17670,8 @@
       <c r="G13" s="71"/>
       <c r="H13" s="109"/>
       <c r="I13" s="314">
-        <f>AK37/2</f>
-        <v>6.2401308018242394E-4</v>
+        <f>(AK37*N11)/2</f>
+        <v>3.7440784810945435E-4</v>
       </c>
       <c r="J13" s="103"/>
       <c r="S13" s="303" t="s">
@@ -17673,8 +17700,8 @@
       <c r="G14" s="87"/>
       <c r="H14" s="108"/>
       <c r="I14" s="315">
-        <f>AI37</f>
-        <v>9.0638384319306538E-3</v>
+        <f>AI38</f>
+        <v>8.461889951638905E-3</v>
       </c>
       <c r="J14" s="104"/>
       <c r="S14" s="305" t="s">
@@ -17703,8 +17730,8 @@
       <c r="G15" s="71"/>
       <c r="H15" s="109"/>
       <c r="I15" s="314">
-        <f>AJ37</f>
-        <v>2.0645399747711616E-3</v>
+        <f>AJ37*N10</f>
+        <v>8.258159899084647E-4</v>
       </c>
       <c r="J15" s="103"/>
       <c r="S15" s="309" t="s">
@@ -17730,12 +17757,12 @@
       <c r="G16" s="166"/>
       <c r="H16" s="132"/>
       <c r="I16" s="316">
-        <f>AK37/2</f>
-        <v>6.2401308018242394E-4</v>
+        <f>(AK37*N11)/2</f>
+        <v>3.7440784810945435E-4</v>
       </c>
       <c r="J16" s="141"/>
     </row>
-    <row r="17" spans="2:39" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:38" x14ac:dyDescent="0.2">
       <c r="C17" s="83" t="s">
         <v>398</v>
       </c>
@@ -17751,7 +17778,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="18" spans="2:39" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:38" x14ac:dyDescent="0.2">
       <c r="C18" s="131" t="str">
         <f>C30</f>
         <v>R-BLD_Det-N1</v>
@@ -17773,14 +17800,14 @@
         <v>100</v>
       </c>
       <c r="I18" s="313">
-        <f>AH51</f>
-        <v>4.4121765529699531E-3</v>
+        <f>AH52</f>
+        <v>2.4280865417312326E-2</v>
       </c>
       <c r="J18" s="188">
         <v>2020</v>
       </c>
     </row>
-    <row r="19" spans="2:39" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:38" x14ac:dyDescent="0.2">
       <c r="C19" s="109"/>
       <c r="D19" s="109"/>
       <c r="E19" s="70" t="s">
@@ -17790,12 +17817,12 @@
       <c r="G19" s="71"/>
       <c r="H19" s="109"/>
       <c r="I19" s="314">
-        <f>AK51/2</f>
-        <v>9.2012709050415069E-4</v>
+        <f>(AK52*N11)/2</f>
+        <v>3.9601185380309516E-4</v>
       </c>
       <c r="J19" s="103"/>
     </row>
-    <row r="20" spans="2:39" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C20" s="108"/>
       <c r="D20" s="108"/>
       <c r="E20" s="76" t="s">
@@ -17839,23 +17866,23 @@
       <c r="AG20" s="5" t="s">
         <v>675</v>
       </c>
-      <c r="AI20" s="311" t="s">
+      <c r="AH20" s="311" t="s">
         <v>688</v>
       </c>
+      <c r="AI20" s="312" t="s">
+        <v>695</v>
+      </c>
       <c r="AJ20" s="312" t="s">
-        <v>695</v>
-      </c>
-      <c r="AK20" s="312" t="s">
         <v>696</v>
       </c>
-      <c r="AL20" s="5" t="s">
+      <c r="AK20" s="5" t="s">
         <v>691</v>
       </c>
-      <c r="AM20" s="310" t="s">
+      <c r="AL20" s="310" t="s">
         <v>697</v>
       </c>
     </row>
-    <row r="21" spans="2:39" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C21" s="109"/>
       <c r="D21" s="109"/>
       <c r="E21" s="70" t="s">
@@ -17865,8 +17892,8 @@
       <c r="G21" s="71"/>
       <c r="H21" s="109"/>
       <c r="I21" s="314">
-        <f>AJ51</f>
-        <v>3.5262400890868602E-3</v>
+        <f>AJ51*N10</f>
+        <v>1.4104960356347441E-3</v>
       </c>
       <c r="J21" s="103"/>
       <c r="W21" s="5" t="s">
@@ -17902,11 +17929,11 @@
       <c r="AG21" s="5" t="s">
         <v>686</v>
       </c>
-      <c r="AI21" s="310" t="s">
+      <c r="AH21" s="310" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="22" spans="2:39" ht="15" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:38" ht="15" x14ac:dyDescent="0.2">
       <c r="C22" s="132"/>
       <c r="D22" s="132"/>
       <c r="E22" s="165" t="s">
@@ -17916,67 +17943,67 @@
       <c r="G22" s="166"/>
       <c r="H22" s="132"/>
       <c r="I22" s="316">
-        <f>AK51/2</f>
-        <v>9.2012709050415069E-4</v>
+        <f>(AK52*N11)/2</f>
+        <v>3.9601185380309516E-4</v>
       </c>
       <c r="J22" s="141"/>
-      <c r="W22" s="5" t="s">
+      <c r="V22" s="5" t="s">
         <v>665</v>
       </c>
+      <c r="W22" s="180">
+        <v>6419</v>
+      </c>
       <c r="X22" s="180">
-        <v>6419</v>
-      </c>
-      <c r="Y22" s="180">
         <v>535137</v>
       </c>
-      <c r="Z22" s="5">
+      <c r="Y22" s="5">
         <v>52</v>
       </c>
+      <c r="Z22" s="180">
+        <v>-505747</v>
+      </c>
       <c r="AA22" s="180">
-        <v>-505747</v>
+        <v>11249</v>
       </c>
       <c r="AB22" s="180">
-        <v>11249</v>
+        <v>2509515</v>
       </c>
       <c r="AC22" s="180">
-        <v>2509515</v>
+        <v>1893006</v>
       </c>
       <c r="AD22" s="180">
-        <v>1893006</v>
+        <v>5793778</v>
       </c>
       <c r="AE22" s="180">
-        <v>5793778</v>
+        <v>31852</v>
       </c>
       <c r="AF22" s="180">
-        <v>31852</v>
-      </c>
-      <c r="AG22" s="180">
         <v>9733652</v>
       </c>
-      <c r="AH22" s="295">
+      <c r="AG22" s="295">
         <v>9418.8988568067343</v>
       </c>
+      <c r="AH22" s="5">
+        <v>0</v>
+      </c>
       <c r="AI22" s="5">
-        <v>0</v>
+        <f>((AG22/W22)*(AD22+AE22)*0.0000000036)/(AG22/1000)</f>
+        <v>3.2672173235706492E-3</v>
       </c>
       <c r="AJ22" s="5">
-        <f>((AH22/X22)*(AE22+AF22)*0.0000000036)/(AH22/1000)</f>
-        <v>3.2672173235706492E-3</v>
+        <f>((AG22/W22)*(AB22)*0.0000000036)/(AG22/1000)</f>
+        <v>1.4074238978033962E-3</v>
       </c>
       <c r="AK22" s="5">
-        <f>((AH22/X22)*(AC22)*0.0000000036)/(AH22/1000)</f>
-        <v>1.4074238978033962E-3</v>
+        <f>((AG22/W22)*(AC22)*0.0000000036)/(AG22/1000)</f>
+        <v>1.0616640598224022E-3</v>
       </c>
       <c r="AL22" s="5">
-        <f>((AH22/X22)*(AD22)*0.0000000036)/(AH22/1000)</f>
-        <v>1.0616640598224022E-3</v>
-      </c>
-      <c r="AM22" s="5">
-        <f>ABS(((AH22/X22)*$T$15*(AA22+AB22)*0.0000000036)/1000)</f>
+        <f>ABS(((AG22/W22)*$T$15*(Z22+AA22)*0.0000000036)/1000)</f>
         <v>1.9404747391189423E-6</v>
       </c>
     </row>
-    <row r="23" spans="2:39" ht="15" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:38" ht="15" x14ac:dyDescent="0.2">
       <c r="V23" s="5" t="s">
         <v>666</v>
       </c>
@@ -18030,7 +18057,7 @@
         <v>7.1648077282642571E-4</v>
       </c>
     </row>
-    <row r="24" spans="2:39" ht="15" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:38" ht="15" x14ac:dyDescent="0.2">
       <c r="V24" s="5" t="s">
         <v>667</v>
       </c>
@@ -18068,7 +18095,7 @@
         <v>14041.847426430093</v>
       </c>
       <c r="AH24" s="5">
-        <f t="shared" ref="AH24:AH30" si="3">((AG24/W24)*$T$15*(Z24+AA24)*0.0000000036)/(AG24/1000)</f>
+        <f>((AG24/W24)*$T$15*(Z24+AA24)*0.0000000036)/(AG24/1000)</f>
         <v>7.8845831836233844E-3</v>
       </c>
       <c r="AI24" s="5">
@@ -18084,7 +18111,7 @@
         <v>6.6022462781304097E-4</v>
       </c>
     </row>
-    <row r="25" spans="2:39" ht="15" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:38" ht="15" x14ac:dyDescent="0.2">
       <c r="B25" s="56" t="s">
         <v>27</v>
       </c>
@@ -18132,7 +18159,7 @@
         <v>19924.480375055824</v>
       </c>
       <c r="AH25" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="AH25:AH30" si="3">((AG25/W25)*$T$15*(Z25+AA25)*0.0000000036)/(AG25/1000)</f>
         <v>1.0639650151914025E-2</v>
       </c>
       <c r="AI25" s="5">
@@ -18148,7 +18175,7 @@
         <v>6.1162726602800291E-4</v>
       </c>
     </row>
-    <row r="26" spans="2:39" ht="15" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:38" ht="15" x14ac:dyDescent="0.2">
       <c r="B26" s="58" t="s">
         <v>34</v>
       </c>
@@ -18223,7 +18250,7 @@
         <v>4.097136724750911E-4</v>
       </c>
     </row>
-    <row r="27" spans="2:39" ht="23.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:38" ht="23.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B27" s="59" t="s">
         <v>476</v>
       </c>
@@ -18298,7 +18325,7 @@
         <v>1.7825362987830464E-4</v>
       </c>
     </row>
-    <row r="28" spans="2:39" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:38" ht="15" x14ac:dyDescent="0.2">
       <c r="B28" s="168" t="s">
         <v>733</v>
       </c>
@@ -18369,7 +18396,7 @@
         <v>1.3277848028214173E-4</v>
       </c>
     </row>
-    <row r="29" spans="2:39" ht="15" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:38" ht="15" x14ac:dyDescent="0.2">
       <c r="B29" s="168" t="s">
         <v>733</v>
       </c>
@@ -18440,7 +18467,7 @@
         <v>1.6302223078404931E-4</v>
       </c>
     </row>
-    <row r="30" spans="2:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B30" s="168" t="s">
         <v>733</v>
       </c>
@@ -18511,32 +18538,32 @@
         <v>1.3719450294485098E-4</v>
       </c>
     </row>
-    <row r="31" spans="2:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="AG31" s="306">
         <v>206798.88499999998</v>
       </c>
-      <c r="AH31" s="5">
+      <c r="AH31" s="180">
         <f>AVERAGE(AH22:AH30)</f>
-        <v>1046.5578079142385</v>
+        <v>1.3490491268107897E-2</v>
       </c>
       <c r="AI31" s="5">
         <f t="shared" ref="AI31:AL31" si="4">AVERAGE(AI22:AI30)</f>
-        <v>8.4541530766784768E-3</v>
+        <v>8.8171772237418834E-3</v>
       </c>
       <c r="AJ31" s="5">
         <f>AVERAGE(AJ22:AJ30)</f>
-        <v>1.9731438707527318E-3</v>
+        <v>1.7665001567785923E-3</v>
       </c>
       <c r="AK31" s="5">
         <f t="shared" si="4"/>
-        <v>4.9074656453725594E-4</v>
+        <v>4.5232880476158994E-4</v>
       </c>
       <c r="AL31" s="5">
         <f t="shared" si="4"/>
-        <v>1.0616640598224022E-3</v>
-      </c>
-    </row>
-    <row r="32" spans="2:39" x14ac:dyDescent="0.2">
+        <v>1.9404747391189423E-6</v>
+      </c>
+    </row>
+    <row r="32" spans="2:38" x14ac:dyDescent="0.2">
       <c r="AI32" s="311"/>
     </row>
     <row r="34" spans="1:38" x14ac:dyDescent="0.2">
@@ -20130,8 +20157,9 @@
     </row>
     <row r="103" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="S3:W3"/>
+    <mergeCell ref="M9:N9"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -25185,12 +25213,12 @@
         <v>321</v>
       </c>
       <c r="U4" s="542"/>
-      <c r="V4" s="543" t="s">
+      <c r="V4" s="534" t="s">
         <v>322</v>
       </c>
-      <c r="W4" s="544"/>
-      <c r="X4" s="544"/>
-      <c r="Y4" s="545"/>
+      <c r="W4" s="535"/>
+      <c r="X4" s="535"/>
+      <c r="Y4" s="536"/>
       <c r="Z4" s="106"/>
       <c r="AA4" s="106"/>
       <c r="AB4" s="114" t="s">
@@ -25289,34 +25317,34 @@
       <c r="E6" s="84"/>
       <c r="F6" s="84"/>
       <c r="G6" s="85"/>
-      <c r="H6" s="534" t="s">
+      <c r="H6" s="537" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="535"/>
-      <c r="J6" s="535"/>
-      <c r="K6" s="536"/>
-      <c r="L6" s="535" t="s">
+      <c r="I6" s="538"/>
+      <c r="J6" s="538"/>
+      <c r="K6" s="539"/>
+      <c r="L6" s="538" t="s">
         <v>45</v>
       </c>
-      <c r="M6" s="535"/>
-      <c r="N6" s="535"/>
-      <c r="O6" s="536"/>
-      <c r="P6" s="534" t="s">
+      <c r="M6" s="538"/>
+      <c r="N6" s="538"/>
+      <c r="O6" s="539"/>
+      <c r="P6" s="537" t="s">
         <v>45</v>
       </c>
-      <c r="Q6" s="535"/>
-      <c r="R6" s="535"/>
-      <c r="S6" s="536"/>
-      <c r="T6" s="534" t="s">
+      <c r="Q6" s="538"/>
+      <c r="R6" s="538"/>
+      <c r="S6" s="539"/>
+      <c r="T6" s="537" t="s">
         <v>302</v>
       </c>
-      <c r="U6" s="536"/>
-      <c r="V6" s="534" t="s">
+      <c r="U6" s="539"/>
+      <c r="V6" s="537" t="s">
         <v>968</v>
       </c>
-      <c r="W6" s="535"/>
-      <c r="X6" s="535"/>
-      <c r="Y6" s="536"/>
+      <c r="W6" s="538"/>
+      <c r="X6" s="538"/>
+      <c r="Y6" s="539"/>
       <c r="Z6" s="107" t="s">
         <v>980</v>
       </c>
@@ -28248,12 +28276,12 @@
         <v>321</v>
       </c>
       <c r="U42" s="542"/>
-      <c r="V42" s="543" t="s">
+      <c r="V42" s="534" t="s">
         <v>322</v>
       </c>
-      <c r="W42" s="544"/>
-      <c r="X42" s="544"/>
-      <c r="Y42" s="545"/>
+      <c r="W42" s="535"/>
+      <c r="X42" s="535"/>
+      <c r="Y42" s="536"/>
       <c r="Z42" s="106"/>
       <c r="AA42" s="106"/>
       <c r="AB42" s="114" t="s">
@@ -28352,34 +28380,34 @@
       <c r="E44" s="84"/>
       <c r="F44" s="84"/>
       <c r="G44" s="85"/>
-      <c r="H44" s="534" t="s">
+      <c r="H44" s="537" t="s">
         <v>45</v>
       </c>
-      <c r="I44" s="535"/>
-      <c r="J44" s="535"/>
-      <c r="K44" s="536"/>
-      <c r="L44" s="535" t="s">
+      <c r="I44" s="538"/>
+      <c r="J44" s="538"/>
+      <c r="K44" s="539"/>
+      <c r="L44" s="538" t="s">
         <v>45</v>
       </c>
-      <c r="M44" s="535"/>
-      <c r="N44" s="535"/>
-      <c r="O44" s="536"/>
-      <c r="P44" s="534" t="s">
+      <c r="M44" s="538"/>
+      <c r="N44" s="538"/>
+      <c r="O44" s="539"/>
+      <c r="P44" s="537" t="s">
         <v>45</v>
       </c>
-      <c r="Q44" s="535"/>
-      <c r="R44" s="535"/>
-      <c r="S44" s="536"/>
-      <c r="T44" s="537" t="s">
+      <c r="Q44" s="538"/>
+      <c r="R44" s="538"/>
+      <c r="S44" s="539"/>
+      <c r="T44" s="543" t="s">
         <v>302</v>
       </c>
-      <c r="U44" s="538"/>
-      <c r="V44" s="537" t="s">
+      <c r="U44" s="544"/>
+      <c r="V44" s="543" t="s">
         <v>968</v>
       </c>
-      <c r="W44" s="539"/>
-      <c r="X44" s="539"/>
-      <c r="Y44" s="538"/>
+      <c r="W44" s="545"/>
+      <c r="X44" s="545"/>
+      <c r="Y44" s="544"/>
       <c r="Z44" s="450" t="s">
         <v>980</v>
       </c>
@@ -32108,12 +32136,12 @@
         <v>321</v>
       </c>
       <c r="U90" s="542"/>
-      <c r="V90" s="543" t="s">
+      <c r="V90" s="534" t="s">
         <v>322</v>
       </c>
-      <c r="W90" s="544"/>
-      <c r="X90" s="544"/>
-      <c r="Y90" s="545"/>
+      <c r="W90" s="535"/>
+      <c r="X90" s="535"/>
+      <c r="Y90" s="536"/>
       <c r="Z90" s="106"/>
       <c r="AA90" s="106"/>
       <c r="AB90" s="114" t="s">
@@ -32212,34 +32240,34 @@
       <c r="E92" s="84"/>
       <c r="F92" s="84"/>
       <c r="G92" s="85"/>
-      <c r="H92" s="534" t="s">
+      <c r="H92" s="537" t="s">
         <v>45</v>
       </c>
-      <c r="I92" s="535"/>
-      <c r="J92" s="535"/>
-      <c r="K92" s="536"/>
-      <c r="L92" s="535" t="s">
+      <c r="I92" s="538"/>
+      <c r="J92" s="538"/>
+      <c r="K92" s="539"/>
+      <c r="L92" s="538" t="s">
         <v>45</v>
       </c>
-      <c r="M92" s="535"/>
-      <c r="N92" s="535"/>
-      <c r="O92" s="536"/>
-      <c r="P92" s="534" t="s">
+      <c r="M92" s="538"/>
+      <c r="N92" s="538"/>
+      <c r="O92" s="539"/>
+      <c r="P92" s="537" t="s">
         <v>45</v>
       </c>
-      <c r="Q92" s="535"/>
-      <c r="R92" s="535"/>
-      <c r="S92" s="536"/>
-      <c r="T92" s="537" t="s">
+      <c r="Q92" s="538"/>
+      <c r="R92" s="538"/>
+      <c r="S92" s="539"/>
+      <c r="T92" s="543" t="s">
         <v>302</v>
       </c>
-      <c r="U92" s="538"/>
-      <c r="V92" s="537" t="s">
+      <c r="U92" s="544"/>
+      <c r="V92" s="543" t="s">
         <v>968</v>
       </c>
-      <c r="W92" s="539"/>
-      <c r="X92" s="539"/>
-      <c r="Y92" s="538"/>
+      <c r="W92" s="545"/>
+      <c r="X92" s="545"/>
+      <c r="Y92" s="544"/>
       <c r="Z92" s="450" t="s">
         <v>980</v>
       </c>
@@ -36104,6 +36132,26 @@
     <row r="166" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="H92:K92"/>
+    <mergeCell ref="L92:O92"/>
+    <mergeCell ref="P92:S92"/>
+    <mergeCell ref="T92:U92"/>
+    <mergeCell ref="V92:Y92"/>
+    <mergeCell ref="H90:K90"/>
+    <mergeCell ref="L90:O90"/>
+    <mergeCell ref="P90:S90"/>
+    <mergeCell ref="T90:U90"/>
+    <mergeCell ref="V90:Y90"/>
+    <mergeCell ref="H44:K44"/>
+    <mergeCell ref="L44:O44"/>
+    <mergeCell ref="P44:S44"/>
+    <mergeCell ref="T44:U44"/>
+    <mergeCell ref="V44:Y44"/>
+    <mergeCell ref="H42:K42"/>
+    <mergeCell ref="L42:O42"/>
+    <mergeCell ref="P42:S42"/>
+    <mergeCell ref="T42:U42"/>
+    <mergeCell ref="V42:Y42"/>
     <mergeCell ref="V4:Y4"/>
     <mergeCell ref="V6:Y6"/>
     <mergeCell ref="H4:K4"/>
@@ -36114,26 +36162,6 @@
     <mergeCell ref="P6:S6"/>
     <mergeCell ref="L6:O6"/>
     <mergeCell ref="H6:K6"/>
-    <mergeCell ref="H42:K42"/>
-    <mergeCell ref="L42:O42"/>
-    <mergeCell ref="P42:S42"/>
-    <mergeCell ref="T42:U42"/>
-    <mergeCell ref="V42:Y42"/>
-    <mergeCell ref="H44:K44"/>
-    <mergeCell ref="L44:O44"/>
-    <mergeCell ref="P44:S44"/>
-    <mergeCell ref="T44:U44"/>
-    <mergeCell ref="V44:Y44"/>
-    <mergeCell ref="H90:K90"/>
-    <mergeCell ref="L90:O90"/>
-    <mergeCell ref="P90:S90"/>
-    <mergeCell ref="T90:U90"/>
-    <mergeCell ref="V90:Y90"/>
-    <mergeCell ref="H92:K92"/>
-    <mergeCell ref="L92:O92"/>
-    <mergeCell ref="P92:S92"/>
-    <mergeCell ref="T92:U92"/>
-    <mergeCell ref="V92:Y92"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
@@ -36278,12 +36306,12 @@
       <c r="I5" s="173"/>
       <c r="J5" s="173"/>
       <c r="K5" s="173"/>
-      <c r="L5" s="543" t="s">
+      <c r="L5" s="534" t="s">
         <v>322</v>
       </c>
-      <c r="M5" s="544"/>
-      <c r="N5" s="544"/>
-      <c r="O5" s="545"/>
+      <c r="M5" s="535"/>
+      <c r="N5" s="535"/>
+      <c r="O5" s="536"/>
       <c r="P5" s="106"/>
       <c r="Q5" s="106" t="s">
         <v>323</v>
@@ -36314,12 +36342,12 @@
       <c r="I6" s="83"/>
       <c r="J6" s="83"/>
       <c r="K6" s="83"/>
-      <c r="L6" s="537" t="s">
+      <c r="L6" s="543" t="s">
         <v>968</v>
       </c>
-      <c r="M6" s="539"/>
-      <c r="N6" s="539"/>
-      <c r="O6" s="538"/>
+      <c r="M6" s="545"/>
+      <c r="N6" s="545"/>
+      <c r="O6" s="544"/>
       <c r="P6" s="450" t="s">
         <v>980</v>
       </c>
@@ -37237,23 +37265,23 @@
       <c r="K33" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="L33" s="543" t="s">
+      <c r="L33" s="534" t="s">
         <v>322</v>
       </c>
-      <c r="M33" s="544"/>
-      <c r="N33" s="544"/>
-      <c r="O33" s="545"/>
+      <c r="M33" s="535"/>
+      <c r="N33" s="535"/>
+      <c r="O33" s="536"/>
     </row>
     <row r="34" spans="8:15" x14ac:dyDescent="0.2">
       <c r="H34" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="L34" s="537" t="s">
+      <c r="L34" s="543" t="s">
         <v>327</v>
       </c>
-      <c r="M34" s="539"/>
-      <c r="N34" s="539"/>
-      <c r="O34" s="538"/>
+      <c r="M34" s="545"/>
+      <c r="N34" s="545"/>
+      <c r="O34" s="544"/>
     </row>
     <row r="35" spans="8:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H35" s="5" t="s">
@@ -37600,11 +37628,11 @@
       </c>
       <c r="I4" s="541"/>
       <c r="J4" s="542"/>
-      <c r="K4" s="543" t="s">
+      <c r="K4" s="534" t="s">
         <v>322</v>
       </c>
-      <c r="L4" s="544"/>
-      <c r="M4" s="545"/>
+      <c r="L4" s="535"/>
+      <c r="M4" s="536"/>
       <c r="N4" s="106"/>
       <c r="O4" s="106" t="s">
         <v>323</v>
@@ -37630,16 +37658,16 @@
       <c r="G5" s="458" t="s">
         <v>302</v>
       </c>
-      <c r="H5" s="550" t="s">
+      <c r="H5" s="547" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="551"/>
-      <c r="J5" s="552"/>
-      <c r="K5" s="550" t="s">
+      <c r="I5" s="548"/>
+      <c r="J5" s="549"/>
+      <c r="K5" s="547" t="s">
         <v>757</v>
       </c>
-      <c r="L5" s="551"/>
-      <c r="M5" s="552"/>
+      <c r="L5" s="548"/>
+      <c r="M5" s="549"/>
       <c r="N5" s="459" t="s">
         <v>328</v>
       </c>
@@ -37656,23 +37684,23 @@
         <v>626</v>
       </c>
       <c r="AA5" s="281"/>
-      <c r="AB5" s="547" t="s">
+      <c r="AB5" s="550" t="s">
         <v>1013</v>
       </c>
-      <c r="AC5" s="547"/>
+      <c r="AC5" s="550"/>
       <c r="AD5" s="461"/>
-      <c r="AE5" s="548" t="s">
+      <c r="AE5" s="551" t="s">
         <v>110</v>
       </c>
-      <c r="AF5" s="548"/>
-      <c r="AG5" s="548" t="s">
+      <c r="AF5" s="551"/>
+      <c r="AG5" s="551" t="s">
         <v>1014</v>
       </c>
-      <c r="AH5" s="548"/>
-      <c r="AI5" s="549" t="s">
+      <c r="AH5" s="551"/>
+      <c r="AI5" s="552" t="s">
         <v>1015</v>
       </c>
-      <c r="AJ5" s="549"/>
+      <c r="AJ5" s="552"/>
     </row>
     <row r="6" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C6" s="505" t="str">
@@ -38410,12 +38438,12 @@
       <c r="K27" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="L27" s="543" t="s">
+      <c r="L27" s="534" t="s">
         <v>322</v>
       </c>
-      <c r="M27" s="544"/>
-      <c r="N27" s="544"/>
-      <c r="O27" s="545"/>
+      <c r="M27" s="535"/>
+      <c r="N27" s="535"/>
+      <c r="O27" s="536"/>
       <c r="T27" s="283"/>
       <c r="U27" s="283"/>
     </row>
@@ -38423,12 +38451,12 @@
       <c r="J28" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="L28" s="534" t="s">
+      <c r="L28" s="537" t="s">
         <v>327</v>
       </c>
-      <c r="M28" s="535"/>
-      <c r="N28" s="535"/>
-      <c r="O28" s="536"/>
+      <c r="M28" s="538"/>
+      <c r="N28" s="538"/>
+      <c r="O28" s="539"/>
       <c r="T28" s="283"/>
       <c r="U28" s="283"/>
     </row>
@@ -39818,16 +39846,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="AB5:AC5"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AG5:AH5"/>
+    <mergeCell ref="AI5:AJ5"/>
+    <mergeCell ref="L27:O27"/>
     <mergeCell ref="L28:O28"/>
     <mergeCell ref="H4:J4"/>
     <mergeCell ref="K4:M4"/>
     <mergeCell ref="H5:J5"/>
     <mergeCell ref="K5:M5"/>
-    <mergeCell ref="AB5:AC5"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="AG5:AH5"/>
-    <mergeCell ref="AI5:AJ5"/>
-    <mergeCell ref="L27:O27"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="S7" r:id="rId1" xr:uid="{B1EDD63D-40A5-4174-9D28-8666BD314B83}"/>
@@ -48855,103 +48883,103 @@
       <c r="C4" s="356" t="s">
         <v>766</v>
       </c>
-      <c r="D4" s="554" t="s">
+      <c r="D4" s="553" t="s">
         <v>767</v>
       </c>
-      <c r="E4" s="553"/>
-      <c r="F4" s="553"/>
-      <c r="G4" s="553"/>
+      <c r="E4" s="554"/>
+      <c r="F4" s="554"/>
+      <c r="G4" s="554"/>
       <c r="H4" s="555"/>
-      <c r="I4" s="553" t="s">
+      <c r="I4" s="554" t="s">
         <v>768</v>
       </c>
-      <c r="J4" s="553"/>
-      <c r="K4" s="553"/>
-      <c r="L4" s="553"/>
+      <c r="J4" s="554"/>
+      <c r="K4" s="554"/>
+      <c r="L4" s="554"/>
       <c r="M4" s="555"/>
-      <c r="N4" s="553" t="s">
+      <c r="N4" s="554" t="s">
         <v>769</v>
       </c>
-      <c r="O4" s="553"/>
-      <c r="P4" s="553"/>
-      <c r="Q4" s="553"/>
+      <c r="O4" s="554"/>
+      <c r="P4" s="554"/>
+      <c r="Q4" s="554"/>
       <c r="R4" s="555"/>
-      <c r="S4" s="553" t="s">
+      <c r="S4" s="554" t="s">
         <v>770</v>
       </c>
-      <c r="T4" s="553"/>
-      <c r="U4" s="553"/>
-      <c r="V4" s="553"/>
+      <c r="T4" s="554"/>
+      <c r="U4" s="554"/>
+      <c r="V4" s="554"/>
       <c r="W4" s="555"/>
-      <c r="X4" s="553" t="s">
+      <c r="X4" s="554" t="s">
         <v>771</v>
       </c>
-      <c r="Y4" s="553"/>
-      <c r="Z4" s="553"/>
-      <c r="AA4" s="553"/>
+      <c r="Y4" s="554"/>
+      <c r="Z4" s="554"/>
+      <c r="AA4" s="554"/>
       <c r="AB4" s="555"/>
-      <c r="AC4" s="553" t="s">
+      <c r="AC4" s="554" t="s">
         <v>772</v>
       </c>
-      <c r="AD4" s="553"/>
-      <c r="AE4" s="553"/>
-      <c r="AF4" s="553"/>
+      <c r="AD4" s="554"/>
+      <c r="AE4" s="554"/>
+      <c r="AF4" s="554"/>
       <c r="AG4" s="555"/>
-      <c r="AH4" s="553" t="s">
+      <c r="AH4" s="554" t="s">
         <v>773</v>
       </c>
-      <c r="AI4" s="553"/>
-      <c r="AJ4" s="553"/>
-      <c r="AK4" s="553"/>
+      <c r="AI4" s="554"/>
+      <c r="AJ4" s="554"/>
+      <c r="AK4" s="554"/>
       <c r="AL4" s="555"/>
-      <c r="AM4" s="553" t="s">
+      <c r="AM4" s="554" t="s">
         <v>774</v>
       </c>
-      <c r="AN4" s="553"/>
-      <c r="AO4" s="553"/>
-      <c r="AP4" s="553"/>
+      <c r="AN4" s="554"/>
+      <c r="AO4" s="554"/>
+      <c r="AP4" s="554"/>
       <c r="AQ4" s="555"/>
-      <c r="AR4" s="553" t="s">
+      <c r="AR4" s="554" t="s">
         <v>775</v>
       </c>
-      <c r="AS4" s="553"/>
-      <c r="AT4" s="553"/>
-      <c r="AU4" s="553"/>
+      <c r="AS4" s="554"/>
+      <c r="AT4" s="554"/>
+      <c r="AU4" s="554"/>
       <c r="AV4" s="555"/>
-      <c r="AW4" s="553" t="s">
+      <c r="AW4" s="554" t="s">
         <v>776</v>
       </c>
-      <c r="AX4" s="553"/>
-      <c r="AY4" s="553"/>
-      <c r="AZ4" s="553"/>
-      <c r="BA4" s="553"/>
-      <c r="BB4" s="554" t="s">
+      <c r="AX4" s="554"/>
+      <c r="AY4" s="554"/>
+      <c r="AZ4" s="554"/>
+      <c r="BA4" s="554"/>
+      <c r="BB4" s="553" t="s">
         <v>777</v>
       </c>
-      <c r="BC4" s="553"/>
-      <c r="BD4" s="553"/>
-      <c r="BE4" s="553"/>
+      <c r="BC4" s="554"/>
+      <c r="BD4" s="554"/>
+      <c r="BE4" s="554"/>
       <c r="BF4" s="555"/>
-      <c r="BG4" s="553" t="s">
+      <c r="BG4" s="554" t="s">
         <v>778</v>
       </c>
-      <c r="BH4" s="553"/>
-      <c r="BI4" s="553"/>
-      <c r="BJ4" s="553"/>
-      <c r="BK4" s="553"/>
-      <c r="BL4" s="554" t="s">
+      <c r="BH4" s="554"/>
+      <c r="BI4" s="554"/>
+      <c r="BJ4" s="554"/>
+      <c r="BK4" s="554"/>
+      <c r="BL4" s="553" t="s">
         <v>779</v>
       </c>
-      <c r="BM4" s="553"/>
-      <c r="BN4" s="553"/>
-      <c r="BO4" s="553"/>
-      <c r="BP4" s="553"/>
-      <c r="BQ4" s="554" t="s">
+      <c r="BM4" s="554"/>
+      <c r="BN4" s="554"/>
+      <c r="BO4" s="554"/>
+      <c r="BP4" s="554"/>
+      <c r="BQ4" s="553" t="s">
         <v>780</v>
       </c>
-      <c r="BR4" s="553"/>
-      <c r="BS4" s="553"/>
-      <c r="BT4" s="553"/>
+      <c r="BR4" s="554"/>
+      <c r="BS4" s="554"/>
+      <c r="BT4" s="554"/>
       <c r="BU4" s="555"/>
       <c r="BV4" s="357" t="s">
         <v>781</v>
@@ -62545,11 +62573,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="BL4:BP4"/>
-    <mergeCell ref="BQ4:BU4"/>
-    <mergeCell ref="BW4:CA4"/>
-    <mergeCell ref="CB4:CF4"/>
-    <mergeCell ref="CG4:CK4"/>
     <mergeCell ref="BG4:BK4"/>
     <mergeCell ref="D4:H4"/>
     <mergeCell ref="I4:M4"/>
@@ -62562,6 +62585,11 @@
     <mergeCell ref="AR4:AV4"/>
     <mergeCell ref="AW4:BA4"/>
     <mergeCell ref="BB4:BF4"/>
+    <mergeCell ref="BL4:BP4"/>
+    <mergeCell ref="BQ4:BU4"/>
+    <mergeCell ref="BW4:CA4"/>
+    <mergeCell ref="CB4:CF4"/>
+    <mergeCell ref="CG4:CK4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
LPG extra cost for install and tank rental
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_RSD.xlsx
+++ b/SubRES_TMPL/SubRes_RSD.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFEDF3C7-4654-4AAD-859E-15409B92DAA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E96BE67-93A6-4C79-8AA9-95F478771D71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{34F9D92C-266F-476D-89E0-63153305AC39}"/>
   </bookViews>
@@ -206,7 +206,32 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Data from AECOM report - https://www.gov.ie/en/publication/8b915-cost-optimal-residential-report-ireland-2018/</t>
+Data from AECOM report - https://www.gov.ie/en/publication/8b915-cost-optimal-residential-report-ireland-2018/
+Cost of install LPG tank 250euro</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Z11" authorId="0" shapeId="0" xr:uid="{9BBCE69B-267B-4D2A-99E0-0810B5648789}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+LPG tank rental is €150/yr https://selectra.ie/lpg/guides/lpg-tanks</t>
         </r>
       </text>
     </comment>
@@ -14510,6 +14535,8 @@
     <xf numFmtId="0" fontId="40" fillId="21" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="40" fillId="21" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="16" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="37" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="38" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -14555,6 +14582,15 @@
     <xf numFmtId="0" fontId="53" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="23" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -14562,15 +14598,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -14582,17 +14609,26 @@
     <xf numFmtId="0" fontId="16" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -14603,19 +14639,10 @@
     <xf numFmtId="0" fontId="69" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="60" fillId="31" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="60" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="31" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="60" fillId="31" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -14630,8 +14657,6 @@
     <xf numFmtId="0" fontId="60" fillId="32" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="37" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="38" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="20% - Colore 2" xfId="11" xr:uid="{3E3DAF22-4D86-48A9-B6EE-8D230C1E993C}"/>
@@ -15748,6 +15773,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -16231,14 +16260,14 @@
       <c r="F16" s="211"/>
     </row>
     <row r="17" spans="1:14" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="521" t="s">
+      <c r="A17" s="523" t="s">
         <v>434</v>
       </c>
-      <c r="B17" s="521"/>
-      <c r="C17" s="521"/>
-      <c r="D17" s="521"/>
-      <c r="E17" s="521"/>
-      <c r="F17" s="521"/>
+      <c r="B17" s="523"/>
+      <c r="C17" s="523"/>
+      <c r="D17" s="523"/>
+      <c r="E17" s="523"/>
+      <c r="F17" s="523"/>
       <c r="G17" s="213"/>
       <c r="H17" s="213"/>
       <c r="I17" s="214"/>
@@ -16276,13 +16305,13 @@
       <c r="A20" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="522" t="s">
+      <c r="B20" s="524" t="s">
         <v>436</v>
       </c>
-      <c r="C20" s="522"/>
-      <c r="D20" s="522"/>
-      <c r="E20" s="522"/>
-      <c r="F20" s="522"/>
+      <c r="C20" s="524"/>
+      <c r="D20" s="524"/>
+      <c r="E20" s="524"/>
+      <c r="F20" s="524"/>
       <c r="G20" s="218"/>
       <c r="H20" s="218"/>
       <c r="I20" s="219"/>
@@ -16296,13 +16325,13 @@
       <c r="A21" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="523" t="s">
+      <c r="B21" s="525" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="523"/>
-      <c r="D21" s="523"/>
-      <c r="E21" s="523"/>
-      <c r="F21" s="523"/>
+      <c r="C21" s="525"/>
+      <c r="D21" s="525"/>
+      <c r="E21" s="525"/>
+      <c r="F21" s="525"/>
       <c r="G21" s="218"/>
       <c r="H21" s="218"/>
       <c r="I21" s="219"/>
@@ -16316,13 +16345,13 @@
       <c r="A22" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="523" t="s">
+      <c r="B22" s="525" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="523"/>
-      <c r="D22" s="523"/>
-      <c r="E22" s="523"/>
-      <c r="F22" s="523"/>
+      <c r="C22" s="525"/>
+      <c r="D22" s="525"/>
+      <c r="E22" s="525"/>
+      <c r="F22" s="525"/>
     </row>
     <row r="23" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
@@ -16351,22 +16380,22 @@
       <c r="H24" s="3"/>
     </row>
     <row r="25" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="524"/>
-      <c r="B25" s="524"/>
-      <c r="C25" s="524"/>
-      <c r="D25" s="524"/>
-      <c r="E25" s="524"/>
-      <c r="F25" s="524"/>
+      <c r="A25" s="526"/>
+      <c r="B25" s="526"/>
+      <c r="C25" s="526"/>
+      <c r="D25" s="526"/>
+      <c r="E25" s="526"/>
+      <c r="F25" s="526"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
     </row>
     <row r="26" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="520"/>
-      <c r="B26" s="520"/>
-      <c r="C26" s="520"/>
-      <c r="D26" s="520"/>
-      <c r="E26" s="520"/>
-      <c r="F26" s="520"/>
+      <c r="A26" s="522"/>
+      <c r="B26" s="522"/>
+      <c r="C26" s="522"/>
+      <c r="D26" s="522"/>
+      <c r="E26" s="522"/>
+      <c r="F26" s="522"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="211"/>
@@ -16553,16 +16582,16 @@
   <sheetData>
     <row r="1" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:20" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="525" t="s">
+      <c r="B2" s="527" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="526"/>
-      <c r="D2" s="526"/>
-      <c r="E2" s="527"/>
-      <c r="G2" s="525" t="s">
+      <c r="C2" s="528"/>
+      <c r="D2" s="528"/>
+      <c r="E2" s="529"/>
+      <c r="G2" s="527" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="527"/>
+      <c r="H2" s="529"/>
       <c r="I2" s="222"/>
       <c r="J2" s="222"/>
       <c r="K2" s="223"/>
@@ -16904,16 +16933,16 @@
     </row>
     <row r="19" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="2:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="528" t="s">
+      <c r="B20" s="530" t="s">
         <v>70</v>
       </c>
-      <c r="C20" s="529"/>
-      <c r="D20" s="529"/>
-      <c r="E20" s="530"/>
-      <c r="G20" s="525" t="s">
+      <c r="C20" s="531"/>
+      <c r="D20" s="531"/>
+      <c r="E20" s="532"/>
+      <c r="G20" s="527" t="s">
         <v>14</v>
       </c>
-      <c r="H20" s="527"/>
+      <c r="H20" s="529"/>
     </row>
     <row r="21" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="250" t="s">
@@ -17157,16 +17186,16 @@
     </row>
     <row r="37" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="38" spans="2:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="525" t="s">
+      <c r="B38" s="527" t="s">
         <v>78</v>
       </c>
-      <c r="C38" s="526"/>
-      <c r="D38" s="526"/>
-      <c r="E38" s="527"/>
-      <c r="G38" s="531" t="s">
+      <c r="C38" s="528"/>
+      <c r="D38" s="528"/>
+      <c r="E38" s="529"/>
+      <c r="G38" s="533" t="s">
         <v>72</v>
       </c>
-      <c r="H38" s="532"/>
+      <c r="H38" s="534"/>
     </row>
     <row r="39" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B39" s="271" t="s">
@@ -17335,13 +17364,13 @@
       <c r="M3" s="5" t="s">
         <v>390</v>
       </c>
-      <c r="S3" s="533" t="s">
+      <c r="S3" s="535" t="s">
         <v>680</v>
       </c>
-      <c r="T3" s="533"/>
-      <c r="U3" s="533"/>
-      <c r="V3" s="533"/>
-      <c r="W3" s="533"/>
+      <c r="T3" s="535"/>
+      <c r="U3" s="535"/>
+      <c r="V3" s="535"/>
+      <c r="W3" s="535"/>
     </row>
     <row r="4" spans="3:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C4" s="62" t="s">
@@ -17535,10 +17564,10 @@
         <v>5.6296955912135845E-4</v>
       </c>
       <c r="J9" s="103"/>
-      <c r="M9" s="534" t="s">
+      <c r="M9" s="536" t="s">
         <v>110</v>
       </c>
-      <c r="N9" s="534" t="s">
+      <c r="N9" s="536" t="s">
         <v>110</v>
       </c>
       <c r="S9" s="300" t="s">
@@ -25040,8 +25069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{104F8057-C735-4662-BAA6-EEDCF7B57273}">
   <dimension ref="A2:AQ166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H94" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M105" sqref="M105"/>
+    <sheetView tabSelected="1" topLeftCell="H10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AD13" sqref="AD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -25205,34 +25234,34 @@
       <c r="G4" s="62" t="s">
         <v>317</v>
       </c>
-      <c r="H4" s="541" t="s">
+      <c r="H4" s="543" t="s">
         <v>720</v>
       </c>
-      <c r="I4" s="542"/>
-      <c r="J4" s="542"/>
-      <c r="K4" s="543"/>
-      <c r="L4" s="541" t="s">
+      <c r="I4" s="544"/>
+      <c r="J4" s="544"/>
+      <c r="K4" s="545"/>
+      <c r="L4" s="543" t="s">
         <v>319</v>
       </c>
-      <c r="M4" s="542"/>
-      <c r="N4" s="542"/>
-      <c r="O4" s="543"/>
-      <c r="P4" s="541" t="s">
+      <c r="M4" s="544"/>
+      <c r="N4" s="544"/>
+      <c r="O4" s="545"/>
+      <c r="P4" s="543" t="s">
         <v>320</v>
       </c>
-      <c r="Q4" s="542"/>
-      <c r="R4" s="542"/>
-      <c r="S4" s="543"/>
-      <c r="T4" s="541" t="s">
+      <c r="Q4" s="544"/>
+      <c r="R4" s="544"/>
+      <c r="S4" s="545"/>
+      <c r="T4" s="543" t="s">
         <v>321</v>
       </c>
-      <c r="U4" s="543"/>
-      <c r="V4" s="544" t="s">
+      <c r="U4" s="545"/>
+      <c r="V4" s="537" t="s">
         <v>322</v>
       </c>
-      <c r="W4" s="545"/>
-      <c r="X4" s="545"/>
-      <c r="Y4" s="546"/>
+      <c r="W4" s="538"/>
+      <c r="X4" s="538"/>
+      <c r="Y4" s="539"/>
       <c r="Z4" s="106"/>
       <c r="AA4" s="106"/>
       <c r="AB4" s="114" t="s">
@@ -25331,34 +25360,34 @@
       <c r="E6" s="84"/>
       <c r="F6" s="84"/>
       <c r="G6" s="85"/>
-      <c r="H6" s="535" t="s">
+      <c r="H6" s="540" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="536"/>
-      <c r="J6" s="536"/>
-      <c r="K6" s="537"/>
-      <c r="L6" s="536" t="s">
+      <c r="I6" s="541"/>
+      <c r="J6" s="541"/>
+      <c r="K6" s="542"/>
+      <c r="L6" s="541" t="s">
         <v>45</v>
       </c>
-      <c r="M6" s="536"/>
-      <c r="N6" s="536"/>
-      <c r="O6" s="537"/>
-      <c r="P6" s="535" t="s">
+      <c r="M6" s="541"/>
+      <c r="N6" s="541"/>
+      <c r="O6" s="542"/>
+      <c r="P6" s="540" t="s">
         <v>45</v>
       </c>
-      <c r="Q6" s="536"/>
-      <c r="R6" s="536"/>
-      <c r="S6" s="537"/>
-      <c r="T6" s="535" t="s">
+      <c r="Q6" s="541"/>
+      <c r="R6" s="541"/>
+      <c r="S6" s="542"/>
+      <c r="T6" s="540" t="s">
         <v>302</v>
       </c>
-      <c r="U6" s="537"/>
-      <c r="V6" s="535" t="s">
+      <c r="U6" s="542"/>
+      <c r="V6" s="540" t="s">
         <v>968</v>
       </c>
-      <c r="W6" s="536"/>
-      <c r="X6" s="536"/>
-      <c r="Y6" s="537"/>
+      <c r="W6" s="541"/>
+      <c r="X6" s="541"/>
+      <c r="Y6" s="542"/>
       <c r="Z6" s="107" t="s">
         <v>980</v>
       </c>
@@ -25851,23 +25880,24 @@
       </c>
       <c r="U11" s="76"/>
       <c r="V11" s="456">
-        <f>2.79</f>
-        <v>2.79</v>
+        <f>SUM(2.79+0.25)</f>
+        <v>3.04</v>
       </c>
       <c r="W11" s="456">
-        <f t="shared" si="7"/>
-        <v>2.79</v>
+        <f t="shared" ref="W11:Y11" si="11">SUM(2.79+0.25)</f>
+        <v>3.04</v>
       </c>
       <c r="X11" s="456">
-        <f t="shared" si="7"/>
-        <v>2.79</v>
+        <f t="shared" si="11"/>
+        <v>3.04</v>
       </c>
       <c r="Y11" s="456">
-        <f t="shared" si="7"/>
-        <v>2.79</v>
+        <f t="shared" si="11"/>
+        <v>3.04</v>
       </c>
       <c r="Z11" s="456">
-        <v>0.12</v>
+        <f>0.12+0.15</f>
+        <v>0.27</v>
       </c>
       <c r="AA11" s="111"/>
       <c r="AB11" s="118"/>
@@ -25941,15 +25971,15 @@
         <v>0.7</v>
       </c>
       <c r="Q12" s="321">
-        <f t="shared" ref="Q12:S12" si="11">I12*0.7</f>
+        <f t="shared" ref="Q12:S12" si="12">I12*0.7</f>
         <v>0.7</v>
       </c>
       <c r="R12" s="321">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.7</v>
       </c>
       <c r="S12" s="322">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.7</v>
       </c>
       <c r="T12" s="99">
@@ -25958,22 +25988,23 @@
       <c r="U12" s="70"/>
       <c r="V12" s="457">
         <f>V11*($U$150/$U$149)</f>
-        <v>2.8135443037974688</v>
+        <v>3.0656540084388189</v>
       </c>
       <c r="W12" s="457">
         <f>W11*($U$150/$U$149)</f>
-        <v>2.8135443037974688</v>
+        <v>3.0656540084388189</v>
       </c>
       <c r="X12" s="457">
         <f>X11*($U$150/$U$149)</f>
-        <v>2.8135443037974688</v>
+        <v>3.0656540084388189</v>
       </c>
       <c r="Y12" s="457">
         <f>Y11*($U$150/$U$149)</f>
-        <v>2.8135443037974688</v>
+        <v>3.0656540084388189</v>
       </c>
       <c r="Z12" s="457">
-        <v>0.12</v>
+        <f>0.12+0.15</f>
+        <v>0.27</v>
       </c>
       <c r="AA12" s="112"/>
       <c r="AB12" s="119"/>
@@ -26135,19 +26166,19 @@
       <c r="N14" s="78"/>
       <c r="O14" s="91"/>
       <c r="P14" s="320">
-        <f t="shared" ref="P14:S14" si="12">H14*0.7</f>
+        <f t="shared" ref="P14:S14" si="13">H14*0.7</f>
         <v>0.7</v>
       </c>
       <c r="Q14" s="321">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.7</v>
       </c>
       <c r="R14" s="321">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.7</v>
       </c>
       <c r="S14" s="322">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.7</v>
       </c>
       <c r="T14" s="99">
@@ -26342,11 +26373,11 @@
       </c>
       <c r="AK16" s="150"/>
       <c r="AL16" s="149" t="str">
-        <f t="shared" ref="AL16:AM21" si="13">C18</f>
+        <f t="shared" ref="AL16:AM21" si="14">C18</f>
         <v>R-SH_Apt_ELC_HPN1</v>
       </c>
       <c r="AM16" s="149" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Residential Electric Heat Pump - Air to Air - SH</v>
       </c>
       <c r="AN16" s="150" t="s">
@@ -26407,11 +26438,11 @@
       <c r="AI17" s="80"/>
       <c r="AK17" s="152"/>
       <c r="AL17" s="151" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>R-HC_Apt_ELC_HPN1</v>
       </c>
       <c r="AM17" s="151" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Residential Electric Heat Pump - Air to Air - SH + SC</v>
       </c>
       <c r="AN17" s="152" t="s">
@@ -26495,7 +26526,7 @@
       <c r="AD18" s="337"/>
       <c r="AE18" s="337"/>
       <c r="AF18" s="131">
-        <f t="shared" ref="AF18:AF23" si="14">31.536*(AI18/1000)</f>
+        <f t="shared" ref="AF18:AF23" si="15">31.536*(AI18/1000)</f>
         <v>0.15768000000000001</v>
       </c>
       <c r="AG18" s="134"/>
@@ -26507,11 +26538,11 @@
       </c>
       <c r="AK18" s="152"/>
       <c r="AL18" s="151" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>R-SH_Apt_ELC_HPN2</v>
       </c>
       <c r="AM18" s="151" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Residential Electric Heat Pump - Air to Water - SH</v>
       </c>
       <c r="AN18" s="152" t="s">
@@ -26606,7 +26637,7 @@
       <c r="AD19" s="119"/>
       <c r="AE19" s="119"/>
       <c r="AF19" s="109">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.15768000000000001</v>
       </c>
       <c r="AG19" s="112"/>
@@ -26618,11 +26649,11 @@
       </c>
       <c r="AK19" s="152"/>
       <c r="AL19" s="151" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>R-SW_Apt_ELC_HPN1</v>
       </c>
       <c r="AM19" s="151" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Residential Electric Heat Pump - Air to Water - SH + WH</v>
       </c>
       <c r="AN19" s="152" t="s">
@@ -26705,7 +26736,7 @@
       <c r="AD20" s="118"/>
       <c r="AE20" s="118"/>
       <c r="AF20" s="108">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.15768000000000001</v>
       </c>
       <c r="AG20" s="111"/>
@@ -26717,11 +26748,11 @@
       </c>
       <c r="AK20" s="286"/>
       <c r="AL20" s="151" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>R-SH_Apt_ELC_HPN3</v>
       </c>
       <c r="AM20" s="151" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Residential Electric Heat Pump - Ground to Water - SH</v>
       </c>
       <c r="AN20" s="152" t="s">
@@ -26777,15 +26808,15 @@
         <v>0.7</v>
       </c>
       <c r="Q21" s="69">
-        <f t="shared" ref="Q21:S21" si="15">I21*0.7</f>
+        <f t="shared" ref="Q21:S21" si="16">I21*0.7</f>
         <v>0.76999999999999991</v>
       </c>
       <c r="R21" s="69">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.86333333333333329</v>
       </c>
       <c r="S21" s="103">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.93333333333333324</v>
       </c>
       <c r="T21" s="99">
@@ -26817,7 +26848,7 @@
       <c r="AD21" s="119"/>
       <c r="AE21" s="119"/>
       <c r="AF21" s="109">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.18921600000000002</v>
       </c>
       <c r="AG21" s="112"/>
@@ -26829,11 +26860,11 @@
       </c>
       <c r="AK21" s="158"/>
       <c r="AL21" s="154" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>R-HC_Apt_ELC_HPN2</v>
       </c>
       <c r="AM21" s="154" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Residential Electric Heat Pump - Ground to Water - SH + SC</v>
       </c>
       <c r="AN21" s="155" t="s">
@@ -26918,7 +26949,7 @@
       <c r="AD22" s="118"/>
       <c r="AE22" s="118"/>
       <c r="AF22" s="108">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.15768000000000001</v>
       </c>
       <c r="AG22" s="111"/>
@@ -27030,7 +27061,7 @@
       <c r="AD23" s="119"/>
       <c r="AE23" s="119"/>
       <c r="AF23" s="109">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.15768000000000001</v>
       </c>
       <c r="AG23" s="112"/>
@@ -27158,15 +27189,15 @@
         <v>1.1666666666666667</v>
       </c>
       <c r="Q25" s="66">
-        <f t="shared" ref="Q25:S25" si="16">I25*0.7</f>
+        <f t="shared" ref="Q25:S25" si="17">I25*0.7</f>
         <v>1.2530864197530862</v>
       </c>
       <c r="R25" s="66">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1.4691358024691357</v>
       </c>
       <c r="S25" s="102">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1.4691358024691357</v>
       </c>
       <c r="T25" s="135">
@@ -27199,7 +27230,7 @@
       <c r="AD25" s="131"/>
       <c r="AE25" s="131"/>
       <c r="AF25" s="131">
-        <f t="shared" ref="AF25:AF26" si="17">31.536*(AI25/1000)</f>
+        <f t="shared" ref="AF25:AF26" si="18">31.536*(AI25/1000)</f>
         <v>0.56764799999999993</v>
       </c>
       <c r="AG25" s="134"/>
@@ -27271,15 +27302,15 @@
         <v>1.1666666666666665</v>
       </c>
       <c r="Q26" s="72">
-        <f t="shared" ref="Q26" si="18">I26*0.7</f>
+        <f t="shared" ref="Q26" si="19">I26*0.7</f>
         <v>1.2055555555555555</v>
       </c>
       <c r="R26" s="72">
-        <f t="shared" ref="R26" si="19">J26*0.7</f>
+        <f t="shared" ref="R26" si="20">J26*0.7</f>
         <v>1.2055555555555555</v>
       </c>
       <c r="S26" s="105">
-        <f t="shared" ref="S26" si="20">K26*0.7</f>
+        <f t="shared" ref="S26" si="21">K26*0.7</f>
         <v>1.2444444444444445</v>
       </c>
       <c r="T26" s="73">
@@ -27312,7 +27343,7 @@
       <c r="AD26" s="110"/>
       <c r="AE26" s="110"/>
       <c r="AF26" s="110">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.56764799999999993</v>
       </c>
       <c r="AG26" s="113"/>
@@ -27444,11 +27475,11 @@
         <v>2.5409999999999995</v>
       </c>
       <c r="R28" s="72">
-        <f t="shared" ref="R28:S28" si="21">J28*0.7</f>
+        <f t="shared" ref="R28:S28" si="22">J28*0.7</f>
         <v>2.7299999999999995</v>
       </c>
       <c r="S28" s="105">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>2.7299999999999995</v>
       </c>
       <c r="T28" s="333">
@@ -27647,7 +27678,7 @@
       <c r="AD30" s="131"/>
       <c r="AE30" s="131"/>
       <c r="AF30" s="131">
-        <f t="shared" ref="AF30:AF31" si="22">31.536*(AI30/1000)</f>
+        <f t="shared" ref="AF30:AF31" si="23">31.536*(AI30/1000)</f>
         <v>0.56764799999999993</v>
       </c>
       <c r="AG30" s="134"/>
@@ -27749,7 +27780,7 @@
       <c r="AD31" s="109"/>
       <c r="AE31" s="109"/>
       <c r="AF31" s="110">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.56764799999999993</v>
       </c>
       <c r="AG31" s="113"/>
@@ -27862,7 +27893,7 @@
       <c r="AD33" s="131"/>
       <c r="AE33" s="131"/>
       <c r="AF33" s="131">
-        <f t="shared" ref="AF33:AF34" si="23">31.536*(AI33/1000)</f>
+        <f t="shared" ref="AF33:AF34" si="24">31.536*(AI33/1000)</f>
         <v>0.15768000000000001</v>
       </c>
       <c r="AG33" s="134"/>
@@ -27940,7 +27971,7 @@
       <c r="AD34" s="109"/>
       <c r="AE34" s="109"/>
       <c r="AF34" s="109">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0.15768000000000001</v>
       </c>
       <c r="AG34" s="112"/>
@@ -28056,7 +28087,7 @@
       <c r="AD36" s="131"/>
       <c r="AE36" s="131"/>
       <c r="AF36" s="131">
-        <f t="shared" ref="AF36:AF37" si="24">31.536*(AI36/1000)</f>
+        <f t="shared" ref="AF36:AF37" si="25">31.536*(AI36/1000)</f>
         <v>0.15768000000000001</v>
       </c>
       <c r="AG36" s="134"/>
@@ -28135,7 +28166,7 @@
       <c r="AD37" s="109"/>
       <c r="AE37" s="109"/>
       <c r="AF37" s="110">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0.15768000000000001</v>
       </c>
       <c r="AG37" s="113"/>
@@ -28268,34 +28299,34 @@
       <c r="G42" s="62" t="s">
         <v>317</v>
       </c>
-      <c r="H42" s="541" t="s">
+      <c r="H42" s="543" t="s">
         <v>318</v>
       </c>
-      <c r="I42" s="542"/>
-      <c r="J42" s="542"/>
-      <c r="K42" s="543"/>
-      <c r="L42" s="541" t="s">
+      <c r="I42" s="544"/>
+      <c r="J42" s="544"/>
+      <c r="K42" s="545"/>
+      <c r="L42" s="543" t="s">
         <v>319</v>
       </c>
-      <c r="M42" s="542"/>
-      <c r="N42" s="542"/>
-      <c r="O42" s="543"/>
-      <c r="P42" s="541" t="s">
+      <c r="M42" s="544"/>
+      <c r="N42" s="544"/>
+      <c r="O42" s="545"/>
+      <c r="P42" s="543" t="s">
         <v>320</v>
       </c>
-      <c r="Q42" s="542"/>
-      <c r="R42" s="542"/>
-      <c r="S42" s="543"/>
-      <c r="T42" s="541" t="s">
+      <c r="Q42" s="544"/>
+      <c r="R42" s="544"/>
+      <c r="S42" s="545"/>
+      <c r="T42" s="543" t="s">
         <v>321</v>
       </c>
-      <c r="U42" s="543"/>
-      <c r="V42" s="544" t="s">
+      <c r="U42" s="545"/>
+      <c r="V42" s="537" t="s">
         <v>322</v>
       </c>
-      <c r="W42" s="545"/>
-      <c r="X42" s="545"/>
-      <c r="Y42" s="546"/>
+      <c r="W42" s="538"/>
+      <c r="X42" s="538"/>
+      <c r="Y42" s="539"/>
       <c r="Z42" s="106"/>
       <c r="AA42" s="106"/>
       <c r="AB42" s="114" t="s">
@@ -28394,34 +28425,34 @@
       <c r="E44" s="84"/>
       <c r="F44" s="84"/>
       <c r="G44" s="85"/>
-      <c r="H44" s="535" t="s">
+      <c r="H44" s="540" t="s">
         <v>45</v>
       </c>
-      <c r="I44" s="536"/>
-      <c r="J44" s="536"/>
-      <c r="K44" s="537"/>
-      <c r="L44" s="536" t="s">
+      <c r="I44" s="541"/>
+      <c r="J44" s="541"/>
+      <c r="K44" s="542"/>
+      <c r="L44" s="541" t="s">
         <v>45</v>
       </c>
-      <c r="M44" s="536"/>
-      <c r="N44" s="536"/>
-      <c r="O44" s="537"/>
-      <c r="P44" s="535" t="s">
+      <c r="M44" s="541"/>
+      <c r="N44" s="541"/>
+      <c r="O44" s="542"/>
+      <c r="P44" s="540" t="s">
         <v>45</v>
       </c>
-      <c r="Q44" s="536"/>
-      <c r="R44" s="536"/>
-      <c r="S44" s="537"/>
-      <c r="T44" s="538" t="s">
+      <c r="Q44" s="541"/>
+      <c r="R44" s="541"/>
+      <c r="S44" s="542"/>
+      <c r="T44" s="546" t="s">
         <v>302</v>
       </c>
-      <c r="U44" s="539"/>
-      <c r="V44" s="538" t="s">
+      <c r="U44" s="547"/>
+      <c r="V44" s="546" t="s">
         <v>968</v>
       </c>
-      <c r="W44" s="540"/>
-      <c r="X44" s="540"/>
-      <c r="Y44" s="539"/>
+      <c r="W44" s="548"/>
+      <c r="X44" s="548"/>
+      <c r="Y44" s="547"/>
       <c r="Z44" s="450" t="s">
         <v>980</v>
       </c>
@@ -28516,15 +28547,15 @@
         <v>4.2250000000000005</v>
       </c>
       <c r="W45" s="456">
-        <f t="shared" ref="W45:Y45" si="25">W49*1.3</f>
+        <f t="shared" ref="W45:Y45" si="26">W49*1.3</f>
         <v>4.2250000000000005</v>
       </c>
       <c r="X45" s="456">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>4.2250000000000005</v>
       </c>
       <c r="Y45" s="456">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>4.2250000000000005</v>
       </c>
       <c r="Z45" s="456">
@@ -28536,7 +28567,7 @@
       <c r="AD45" s="118"/>
       <c r="AE45" s="118"/>
       <c r="AF45" s="108">
-        <f t="shared" ref="AF45:AF83" si="26">31.536*(AI45/1000)</f>
+        <f t="shared" ref="AF45:AF83" si="27">31.536*(AI45/1000)</f>
         <v>0.63072000000000006</v>
       </c>
       <c r="AG45" s="111"/>
@@ -28550,11 +28581,11 @@
         <v>38</v>
       </c>
       <c r="AL45" s="151" t="str">
-        <f t="shared" ref="AL45:AL60" si="27">C45</f>
+        <f t="shared" ref="AL45:AL60" si="28">C45</f>
         <v>R-SH_Att_KER_N1</v>
       </c>
       <c r="AM45" s="151" t="str">
-        <f t="shared" ref="AM45:AM60" si="28">D45</f>
+        <f t="shared" ref="AM45:AM60" si="29">D45</f>
         <v>Residential Kerosene Heating Oil - New 1 SH</v>
       </c>
       <c r="AN45" s="152" t="s">
@@ -28604,15 +28635,15 @@
         <v>0.7</v>
       </c>
       <c r="Q46" s="69">
-        <f t="shared" ref="Q46:Q48" si="29">I46*0.7</f>
+        <f t="shared" ref="Q46:Q48" si="30">I46*0.7</f>
         <v>0.7</v>
       </c>
       <c r="R46" s="69">
-        <f t="shared" ref="R46:R48" si="30">J46*0.7</f>
+        <f t="shared" ref="R46:R48" si="31">J46*0.7</f>
         <v>0.7</v>
       </c>
       <c r="S46" s="103">
-        <f t="shared" ref="S46:S48" si="31">K46*0.7</f>
+        <f t="shared" ref="S46:S48" si="32">K46*0.7</f>
         <v>0.7</v>
       </c>
       <c r="T46" s="99">
@@ -28624,15 +28655,15 @@
         <v>4.2773760330578519</v>
       </c>
       <c r="W46" s="457">
-        <f t="shared" ref="W46:Y46" si="32">W50*1.3</f>
+        <f t="shared" ref="W46:Y46" si="33">W50*1.3</f>
         <v>4.2773760330578519</v>
       </c>
       <c r="X46" s="457">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>4.2773760330578519</v>
       </c>
       <c r="Y46" s="457">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>4.2773760330578519</v>
       </c>
       <c r="Z46" s="457">
@@ -28644,7 +28675,7 @@
       <c r="AD46" s="119"/>
       <c r="AE46" s="119"/>
       <c r="AF46" s="109">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.7884000000000001</v>
       </c>
       <c r="AG46" s="112"/>
@@ -28656,11 +28687,11 @@
       </c>
       <c r="AK46" s="152"/>
       <c r="AL46" s="151" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>R-SW_Att_KER_N1</v>
       </c>
       <c r="AM46" s="151" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>Residential Kerosene Heating Oil - New 2 SH + WH</v>
       </c>
       <c r="AN46" s="152" t="s">
@@ -28710,15 +28741,15 @@
         <v>0.7</v>
       </c>
       <c r="Q47" s="75">
-        <f t="shared" si="29"/>
-        <v>0.7</v>
-      </c>
-      <c r="R47" s="75">
         <f t="shared" si="30"/>
         <v>0.7</v>
       </c>
+      <c r="R47" s="75">
+        <f t="shared" si="31"/>
+        <v>0.7</v>
+      </c>
       <c r="S47" s="104">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.7</v>
       </c>
       <c r="T47" s="100">
@@ -28755,7 +28786,7 @@
         <v>5</v>
       </c>
       <c r="AF47" s="108">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.7884000000000001</v>
       </c>
       <c r="AG47" s="111"/>
@@ -28767,11 +28798,11 @@
       </c>
       <c r="AK47" s="152"/>
       <c r="AL47" s="151" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>R-SW_Att_KER_N2</v>
       </c>
       <c r="AM47" s="151" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>Residential Kerosene Heating Oil - New 3 SH+WH + Solar</v>
       </c>
       <c r="AN47" s="152" t="s">
@@ -28821,15 +28852,15 @@
         <v>0.7</v>
       </c>
       <c r="Q48" s="69">
-        <f t="shared" si="29"/>
-        <v>0.71749999999999992</v>
-      </c>
-      <c r="R48" s="69">
         <f t="shared" si="30"/>
         <v>0.71749999999999992</v>
       </c>
+      <c r="R48" s="69">
+        <f t="shared" si="31"/>
+        <v>0.71749999999999992</v>
+      </c>
       <c r="S48" s="103">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.71749999999999992</v>
       </c>
       <c r="T48" s="99">
@@ -28878,11 +28909,11 @@
       </c>
       <c r="AK48" s="152"/>
       <c r="AL48" s="151" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>R-SW_Att_KER_N3</v>
       </c>
       <c r="AM48" s="151" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>Residential Kerosene Heating Oil - New 3 SH+WH + Wood Stove</v>
       </c>
       <c r="AN48" s="153" t="s">
@@ -28938,15 +28969,15 @@
         <v>3.25</v>
       </c>
       <c r="W49" s="456">
-        <f t="shared" ref="W49:Y49" si="33">3.25</f>
+        <f t="shared" ref="W49:Y49" si="34">3.25</f>
         <v>3.25</v>
       </c>
       <c r="X49" s="456">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>3.25</v>
       </c>
       <c r="Y49" s="456">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>3.25</v>
       </c>
       <c r="Z49" s="456">
@@ -28958,7 +28989,7 @@
       <c r="AD49" s="118"/>
       <c r="AE49" s="118"/>
       <c r="AF49" s="108">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.63072000000000006</v>
       </c>
       <c r="AG49" s="111"/>
@@ -28970,11 +29001,11 @@
       </c>
       <c r="AK49" s="152"/>
       <c r="AL49" s="151" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>R-SH_Att_GAS_N1</v>
       </c>
       <c r="AM49" s="151" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>Residential Natural Gas Heating - New 1 SH</v>
       </c>
       <c r="AN49" s="152" t="s">
@@ -29024,15 +29055,15 @@
         <v>0.7</v>
       </c>
       <c r="Q50" s="69">
-        <f t="shared" ref="Q50:Q52" si="34">I50*0.7</f>
+        <f t="shared" ref="Q50:Q52" si="35">I50*0.7</f>
         <v>0.7</v>
       </c>
       <c r="R50" s="69">
-        <f t="shared" ref="R50:R52" si="35">J50*0.7</f>
+        <f t="shared" ref="R50:R52" si="36">J50*0.7</f>
         <v>0.7</v>
       </c>
       <c r="S50" s="103">
-        <f t="shared" ref="S50:S52" si="36">K50*0.7</f>
+        <f t="shared" ref="S50:S52" si="37">K50*0.7</f>
         <v>0.7</v>
       </c>
       <c r="T50" s="99">
@@ -29064,7 +29095,7 @@
       <c r="AD50" s="119"/>
       <c r="AE50" s="119"/>
       <c r="AF50" s="109">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.7884000000000001</v>
       </c>
       <c r="AG50" s="112"/>
@@ -29076,11 +29107,11 @@
       </c>
       <c r="AK50" s="152"/>
       <c r="AL50" s="151" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>R-SW_Att_GAS_N1</v>
       </c>
       <c r="AM50" s="151" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>Residential Natural Gas Heating - New 2 SH + WH</v>
       </c>
       <c r="AN50" s="152" t="s">
@@ -29130,15 +29161,15 @@
         <v>0.7</v>
       </c>
       <c r="Q51" s="75">
-        <f t="shared" si="34"/>
-        <v>0.7</v>
-      </c>
-      <c r="R51" s="75">
         <f t="shared" si="35"/>
         <v>0.7</v>
       </c>
+      <c r="R51" s="75">
+        <f t="shared" si="36"/>
+        <v>0.7</v>
+      </c>
       <c r="S51" s="104">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>0.7</v>
       </c>
       <c r="T51" s="100">
@@ -29173,7 +29204,7 @@
         <v>5</v>
       </c>
       <c r="AF51" s="108">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.7884000000000001</v>
       </c>
       <c r="AG51" s="111"/>
@@ -29185,11 +29216,11 @@
       </c>
       <c r="AK51" s="152"/>
       <c r="AL51" s="151" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>R-SW_Att_GAS_N2</v>
       </c>
       <c r="AM51" s="151" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>Residential Natural Gas Heating - New 3 SH + WH + Solar</v>
       </c>
       <c r="AN51" s="152" t="s">
@@ -29239,15 +29270,15 @@
         <v>0.7</v>
       </c>
       <c r="Q52" s="69">
-        <f t="shared" si="34"/>
-        <v>0.71749999999999992</v>
-      </c>
-      <c r="R52" s="69">
         <f t="shared" si="35"/>
         <v>0.71749999999999992</v>
       </c>
+      <c r="R52" s="69">
+        <f t="shared" si="36"/>
+        <v>0.71749999999999992</v>
+      </c>
       <c r="S52" s="103">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>0.71749999999999992</v>
       </c>
       <c r="T52" s="99">
@@ -29284,7 +29315,7 @@
         <v>5</v>
       </c>
       <c r="AF52" s="109">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.7884000000000001</v>
       </c>
       <c r="AG52" s="112"/>
@@ -29296,11 +29327,11 @@
       </c>
       <c r="AK52" s="152"/>
       <c r="AL52" s="151" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>R-SW_Att_GAS_N3</v>
       </c>
       <c r="AM52" s="151" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>Residential Natural Gas Heating - New 4 SH + WH + Wood Stove</v>
       </c>
       <c r="AN52" s="152" t="s">
@@ -29354,23 +29385,24 @@
       </c>
       <c r="U53" s="87"/>
       <c r="V53" s="456">
-        <f>V49</f>
-        <v>3.25</v>
+        <f>SUM(V49+0.25)</f>
+        <v>3.5</v>
       </c>
       <c r="W53" s="456">
-        <f t="shared" ref="W53:Y53" si="37">W49</f>
-        <v>3.25</v>
+        <f t="shared" ref="W53:Y53" si="38">SUM(W49+0.25)</f>
+        <v>3.5</v>
       </c>
       <c r="X53" s="456">
-        <f t="shared" si="37"/>
-        <v>3.25</v>
+        <f t="shared" si="38"/>
+        <v>3.5</v>
       </c>
       <c r="Y53" s="456">
-        <f t="shared" si="37"/>
-        <v>3.25</v>
+        <f t="shared" si="38"/>
+        <v>3.5</v>
       </c>
       <c r="Z53" s="456">
-        <v>0.12</v>
+        <f>SUM(0.12+0.15)</f>
+        <v>0.27</v>
       </c>
       <c r="AA53" s="111"/>
       <c r="AB53" s="88"/>
@@ -29378,7 +29410,7 @@
       <c r="AD53" s="118"/>
       <c r="AE53" s="118"/>
       <c r="AF53" s="108">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.63072000000000006</v>
       </c>
       <c r="AG53" s="111"/>
@@ -29390,11 +29422,11 @@
       </c>
       <c r="AK53" s="152"/>
       <c r="AL53" s="151" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>R-SH_Att_LPG_N1</v>
       </c>
       <c r="AM53" s="151" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>Residential Liquid Petroleum Gas- New 1 SH</v>
       </c>
       <c r="AN53" s="152" t="s">
@@ -29444,15 +29476,15 @@
         <v>0.7</v>
       </c>
       <c r="Q54" s="69">
-        <f t="shared" ref="Q54" si="38">I54*0.7</f>
+        <f t="shared" ref="Q54" si="39">I54*0.7</f>
         <v>0.7</v>
       </c>
       <c r="R54" s="69">
-        <f t="shared" ref="R54" si="39">J54*0.7</f>
+        <f t="shared" ref="R54" si="40">J54*0.7</f>
         <v>0.7</v>
       </c>
       <c r="S54" s="103">
-        <f t="shared" ref="S54" si="40">K54*0.7</f>
+        <f t="shared" ref="S54" si="41">K54*0.7</f>
         <v>0.7</v>
       </c>
       <c r="T54" s="99">
@@ -29460,23 +29492,24 @@
       </c>
       <c r="U54" s="71"/>
       <c r="V54" s="457">
-        <f>V50</f>
-        <v>3.2902892561983474</v>
+        <f>V49*($U$152/$U$151)+0.25</f>
+        <v>3.5402892561983474</v>
       </c>
       <c r="W54" s="457">
-        <f t="shared" ref="W54:Y54" si="41">W50</f>
-        <v>3.2902892561983474</v>
+        <f t="shared" ref="W54:Y54" si="42">W49*($U$152/$U$151)+0.25</f>
+        <v>3.5402892561983474</v>
       </c>
       <c r="X54" s="457">
-        <f t="shared" si="41"/>
-        <v>3.2902892561983474</v>
+        <f t="shared" si="42"/>
+        <v>3.5402892561983474</v>
       </c>
       <c r="Y54" s="457">
-        <f t="shared" si="41"/>
-        <v>3.2902892561983474</v>
-      </c>
-      <c r="Z54" s="457">
-        <v>0.12</v>
+        <f t="shared" si="42"/>
+        <v>3.5402892561983474</v>
+      </c>
+      <c r="Z54" s="456">
+        <f>SUM(0.12+0.15)</f>
+        <v>0.27</v>
       </c>
       <c r="AA54" s="112"/>
       <c r="AB54" s="90"/>
@@ -29484,7 +29517,7 @@
       <c r="AD54" s="119"/>
       <c r="AE54" s="119"/>
       <c r="AF54" s="109">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.7884000000000001</v>
       </c>
       <c r="AG54" s="112"/>
@@ -29496,11 +29529,11 @@
       </c>
       <c r="AK54" s="152"/>
       <c r="AL54" s="151" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>R-SW_Att_LPG_N1</v>
       </c>
       <c r="AM54" s="151" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>Residential Liquid Petroleum Gas- New 2 SH + WH</v>
       </c>
       <c r="AN54" s="152" t="s">
@@ -29577,7 +29610,7 @@
       <c r="AD55" s="118"/>
       <c r="AE55" s="118"/>
       <c r="AF55" s="108">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.63072000000000006</v>
       </c>
       <c r="AG55" s="111"/>
@@ -29589,11 +29622,11 @@
       </c>
       <c r="AK55" s="152"/>
       <c r="AL55" s="151" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>R-SH_Att_WOO_N1</v>
       </c>
       <c r="AM55" s="151" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>Residential Biomass Boiler - New 1 SH</v>
       </c>
       <c r="AN55" s="152" t="s">
@@ -29639,19 +29672,19 @@
       <c r="N56" s="78"/>
       <c r="O56" s="91"/>
       <c r="P56" s="68">
-        <f t="shared" ref="P56:S60" si="42">H56*0.7</f>
+        <f t="shared" ref="P56:S60" si="43">H56*0.7</f>
         <v>0.7</v>
       </c>
       <c r="Q56" s="69">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>0.7</v>
       </c>
       <c r="R56" s="69">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>0.7</v>
       </c>
       <c r="S56" s="103">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>0.7</v>
       </c>
       <c r="T56" s="99">
@@ -29683,7 +29716,7 @@
       <c r="AD56" s="119"/>
       <c r="AE56" s="119"/>
       <c r="AF56" s="109">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.7884000000000001</v>
       </c>
       <c r="AG56" s="112"/>
@@ -29695,11 +29728,11 @@
       </c>
       <c r="AK56" s="155"/>
       <c r="AL56" s="154" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>R-SW_Att_WOO_N1</v>
       </c>
       <c r="AM56" s="154" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>Residential Biomass Boiler - New 2 SH + WH</v>
       </c>
       <c r="AN56" s="155" t="s">
@@ -29753,7 +29786,7 @@
       <c r="AD57" s="119"/>
       <c r="AE57" s="119"/>
       <c r="AF57" s="109">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.63072000000000006</v>
       </c>
       <c r="AG57" s="112"/>
@@ -29768,7 +29801,7 @@
         <v>1038</v>
       </c>
       <c r="AM57" s="154" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>Residential  Fireplace New 1 - SH</v>
       </c>
       <c r="AN57" s="152" t="s">
@@ -29820,7 +29853,7 @@
       <c r="AD58" s="119"/>
       <c r="AE58" s="119"/>
       <c r="AF58" s="109">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.7884000000000001</v>
       </c>
       <c r="AG58" s="112"/>
@@ -29835,7 +29868,7 @@
         <v>1040</v>
       </c>
       <c r="AM58" s="154" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>Residential  Fireplace with back boiler New 1 - SH +WH</v>
       </c>
       <c r="AN58" s="155" t="s">
@@ -29878,19 +29911,19 @@
       <c r="N59" s="77"/>
       <c r="O59" s="89"/>
       <c r="P59" s="86">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>0.7</v>
       </c>
       <c r="Q59" s="75">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>0.7</v>
       </c>
       <c r="R59" s="75">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>0.7</v>
       </c>
       <c r="S59" s="104">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>0.7</v>
       </c>
       <c r="T59" s="100">
@@ -29923,7 +29956,7 @@
       <c r="AD59" s="118"/>
       <c r="AE59" s="118"/>
       <c r="AF59" s="108">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.63072000000000006</v>
       </c>
       <c r="AG59" s="111"/>
@@ -29935,11 +29968,11 @@
       </c>
       <c r="AK59" s="155"/>
       <c r="AL59" s="154" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>*R-H_Apt_HVO_N1</v>
       </c>
       <c r="AM59" s="154" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>Residential  Hydrotreated vegetable oil - New 1 SH</v>
       </c>
       <c r="AN59" s="155" t="s">
@@ -29984,19 +30017,19 @@
       <c r="N60" s="96"/>
       <c r="O60" s="97"/>
       <c r="P60" s="329">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>0.7</v>
       </c>
       <c r="Q60" s="72">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>0.7</v>
       </c>
       <c r="R60" s="72">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>0.7</v>
       </c>
       <c r="S60" s="105">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>0.7</v>
       </c>
       <c r="T60" s="101">
@@ -30029,7 +30062,7 @@
       <c r="AD60" s="119"/>
       <c r="AE60" s="119"/>
       <c r="AF60" s="109">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.7884000000000001</v>
       </c>
       <c r="AG60" s="113"/>
@@ -30041,11 +30074,11 @@
       </c>
       <c r="AK60" s="155"/>
       <c r="AL60" s="154" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>*R-H_Apt_HVO_N2</v>
       </c>
       <c r="AM60" s="154" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>Residential  Hydrotreated vegetable oil - New 1 SH + WH</v>
       </c>
       <c r="AN60" s="155" t="s">
@@ -30180,7 +30213,7 @@
       <c r="AD62" s="130"/>
       <c r="AE62" s="130"/>
       <c r="AF62" s="128">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.63072000000000006</v>
       </c>
       <c r="AG62" s="129"/>
@@ -30192,11 +30225,11 @@
       </c>
       <c r="AK62" s="150"/>
       <c r="AL62" s="149" t="str">
-        <f t="shared" ref="AL62:AM68" si="43">C64</f>
+        <f t="shared" ref="AL62:AM68" si="44">C64</f>
         <v>R-SH_Att_ELC_HPN1</v>
       </c>
       <c r="AM62" s="149" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>Residential Electric Heat Pump - Air to Air - SH</v>
       </c>
       <c r="AN62" s="150" t="s">
@@ -30248,11 +30281,11 @@
       <c r="AI63" s="80"/>
       <c r="AK63" s="152"/>
       <c r="AL63" s="151" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>R-HC_Att_ELC_HPN1</v>
       </c>
       <c r="AM63" s="151" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>Residential Electric Heat Pump - Air to Air - SH + SC</v>
       </c>
       <c r="AN63" s="152" t="s">
@@ -30336,7 +30369,7 @@
       <c r="AD64" s="131"/>
       <c r="AE64" s="131"/>
       <c r="AF64" s="131">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.220752</v>
       </c>
       <c r="AG64" s="134"/>
@@ -30348,11 +30381,11 @@
       </c>
       <c r="AK64" s="152"/>
       <c r="AL64" s="151" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>R-SH_Att_ELC_HPN2</v>
       </c>
       <c r="AM64" s="151" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>Residential Electric Heat Pump - Air to Water - SH</v>
       </c>
       <c r="AN64" s="152" t="s">
@@ -30447,7 +30480,7 @@
       <c r="AD65" s="109"/>
       <c r="AE65" s="109"/>
       <c r="AF65" s="109">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.26805600000000002</v>
       </c>
       <c r="AG65" s="112"/>
@@ -30459,11 +30492,11 @@
       </c>
       <c r="AK65" s="152"/>
       <c r="AL65" s="151" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>R-SW_Att_ELC_HPN1</v>
       </c>
       <c r="AM65" s="151" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>Residential Electric Heat Pump - Air to Water - SH + WH</v>
       </c>
       <c r="AN65" s="152" t="s">
@@ -30545,7 +30578,7 @@
       <c r="AD66" s="108"/>
       <c r="AE66" s="108"/>
       <c r="AF66" s="108">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.220752</v>
       </c>
       <c r="AG66" s="111"/>
@@ -30557,11 +30590,11 @@
       </c>
       <c r="AK66" s="286"/>
       <c r="AL66" s="151" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>R-SW_Att_ELC_HPN2</v>
       </c>
       <c r="AM66" s="151" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>Residential Electric Heat Pump - Air to Water - SH + WH + Solar</v>
       </c>
       <c r="AN66" s="152" t="s">
@@ -30616,15 +30649,15 @@
         <v>0.7</v>
       </c>
       <c r="Q67" s="69">
-        <f t="shared" ref="Q67:Q68" si="44">I67*0.7</f>
+        <f t="shared" ref="Q67:Q68" si="45">I67*0.7</f>
         <v>0.76999999999999991</v>
       </c>
       <c r="R67" s="69">
-        <f t="shared" ref="R67:R68" si="45">J67*0.7</f>
+        <f t="shared" ref="R67:R68" si="46">J67*0.7</f>
         <v>0.86333333333333329</v>
       </c>
       <c r="S67" s="103">
-        <f t="shared" ref="S67:S68" si="46">K67*0.7</f>
+        <f t="shared" ref="S67:S68" si="47">K67*0.7</f>
         <v>0.93333333333333324</v>
       </c>
       <c r="T67" s="99">
@@ -30656,7 +30689,7 @@
       <c r="AD67" s="109"/>
       <c r="AE67" s="109"/>
       <c r="AF67" s="109">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.26805600000000002</v>
       </c>
       <c r="AG67" s="112"/>
@@ -30668,11 +30701,11 @@
       </c>
       <c r="AK67" s="286"/>
       <c r="AL67" s="151" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>R-SH_Att_ELC_HPN3</v>
       </c>
       <c r="AM67" s="151" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>Residential Electric Heat Pump - Ground to Water - SH</v>
       </c>
       <c r="AN67" s="152" t="s">
@@ -30724,15 +30757,15 @@
         <v>0.7</v>
       </c>
       <c r="Q68" s="75">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>0.77700000000000002</v>
       </c>
       <c r="R68" s="75">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>0.83299999999999996</v>
       </c>
       <c r="S68" s="104">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>0.83299999999999996</v>
       </c>
       <c r="T68" s="100">
@@ -30769,7 +30802,7 @@
         <v>5</v>
       </c>
       <c r="AF68" s="108">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.26805600000000002</v>
       </c>
       <c r="AG68" s="111"/>
@@ -30781,11 +30814,11 @@
       </c>
       <c r="AK68" s="158"/>
       <c r="AL68" s="154" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>R-HC_Att_ELC_HPN2</v>
       </c>
       <c r="AM68" s="154" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>Residential Electric Heat Pump - Ground to Water - SH + SC</v>
       </c>
       <c r="AN68" s="155" t="s">
@@ -30870,7 +30903,7 @@
       <c r="AD69" s="109"/>
       <c r="AE69" s="109"/>
       <c r="AF69" s="109">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.220752</v>
       </c>
       <c r="AG69" s="112"/>
@@ -30983,7 +31016,7 @@
       <c r="AD70" s="132"/>
       <c r="AE70" s="132"/>
       <c r="AF70" s="132">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.26805600000000002</v>
       </c>
       <c r="AG70" s="137"/>
@@ -31111,15 +31144,15 @@
         <v>1.1666666666666667</v>
       </c>
       <c r="Q72" s="66">
-        <f t="shared" ref="Q72:Q73" si="47">I72*0.7</f>
+        <f t="shared" ref="Q72:Q73" si="48">I72*0.7</f>
         <v>1.2530864197530862</v>
       </c>
       <c r="R72" s="66">
-        <f t="shared" ref="R72:R73" si="48">J72*0.7</f>
+        <f t="shared" ref="R72:R73" si="49">J72*0.7</f>
         <v>1.4691358024691357</v>
       </c>
       <c r="S72" s="102">
-        <f t="shared" ref="S72:S73" si="49">K72*0.7</f>
+        <f t="shared" ref="S72:S73" si="50">K72*0.7</f>
         <v>1.4691358024691357</v>
       </c>
       <c r="T72" s="135">
@@ -31152,7 +31185,7 @@
       <c r="AD72" s="131"/>
       <c r="AE72" s="131"/>
       <c r="AF72" s="131">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.7884000000000001</v>
       </c>
       <c r="AG72" s="134"/>
@@ -31224,15 +31257,15 @@
         <v>1.1666666666666665</v>
       </c>
       <c r="Q73" s="72">
-        <f t="shared" si="47"/>
-        <v>1.2055555555555555</v>
-      </c>
-      <c r="R73" s="72">
         <f t="shared" si="48"/>
         <v>1.2055555555555555</v>
       </c>
+      <c r="R73" s="72">
+        <f t="shared" si="49"/>
+        <v>1.2055555555555555</v>
+      </c>
       <c r="S73" s="105">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>1.2444444444444445</v>
       </c>
       <c r="T73" s="73">
@@ -31393,15 +31426,15 @@
         <v>2.2889999999999997</v>
       </c>
       <c r="Q75" s="72">
-        <f t="shared" ref="Q75" si="50">I75*0.7</f>
+        <f t="shared" ref="Q75" si="51">I75*0.7</f>
         <v>2.5409999999999995</v>
       </c>
       <c r="R75" s="72">
-        <f t="shared" ref="R75" si="51">J75*0.7</f>
+        <f t="shared" ref="R75" si="52">J75*0.7</f>
         <v>2.7299999999999995</v>
       </c>
       <c r="S75" s="105">
-        <f t="shared" ref="S75" si="52">K75*0.7</f>
+        <f t="shared" ref="S75" si="53">K75*0.7</f>
         <v>2.7299999999999995</v>
       </c>
       <c r="T75" s="5">
@@ -31437,7 +31470,7 @@
         <v>5</v>
       </c>
       <c r="AF75" s="128">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.42415920000000001</v>
       </c>
       <c r="AG75" s="129"/>
@@ -31597,7 +31630,7 @@
       <c r="AD77" s="131"/>
       <c r="AE77" s="131"/>
       <c r="AF77" s="131">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.7884000000000001</v>
       </c>
       <c r="AG77" s="134"/>
@@ -31681,7 +31714,7 @@
       <c r="AD78" s="110"/>
       <c r="AE78" s="110"/>
       <c r="AF78" s="110">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.7884000000000001</v>
       </c>
       <c r="AG78" s="113"/>
@@ -31794,7 +31827,7 @@
       <c r="AD80" s="131"/>
       <c r="AE80" s="131"/>
       <c r="AF80" s="131">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.18921600000000002</v>
       </c>
       <c r="AG80" s="134"/>
@@ -31872,7 +31905,7 @@
       <c r="AD81" s="109"/>
       <c r="AE81" s="109"/>
       <c r="AF81" s="109">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.18921600000000002</v>
       </c>
       <c r="AG81" s="113"/>
@@ -31988,7 +32021,7 @@
       <c r="AD83" s="139"/>
       <c r="AE83" s="139"/>
       <c r="AF83" s="139">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.18921600000000002</v>
       </c>
       <c r="AG83" s="138"/>
@@ -32128,34 +32161,34 @@
       <c r="G90" s="62" t="s">
         <v>317</v>
       </c>
-      <c r="H90" s="541" t="s">
+      <c r="H90" s="543" t="s">
         <v>318</v>
       </c>
-      <c r="I90" s="542"/>
-      <c r="J90" s="542"/>
-      <c r="K90" s="543"/>
-      <c r="L90" s="541" t="s">
+      <c r="I90" s="544"/>
+      <c r="J90" s="544"/>
+      <c r="K90" s="545"/>
+      <c r="L90" s="543" t="s">
         <v>319</v>
       </c>
-      <c r="M90" s="542"/>
-      <c r="N90" s="542"/>
-      <c r="O90" s="543"/>
-      <c r="P90" s="541" t="s">
+      <c r="M90" s="544"/>
+      <c r="N90" s="544"/>
+      <c r="O90" s="545"/>
+      <c r="P90" s="543" t="s">
         <v>320</v>
       </c>
-      <c r="Q90" s="542"/>
-      <c r="R90" s="542"/>
-      <c r="S90" s="543"/>
-      <c r="T90" s="541" t="s">
+      <c r="Q90" s="544"/>
+      <c r="R90" s="544"/>
+      <c r="S90" s="545"/>
+      <c r="T90" s="543" t="s">
         <v>321</v>
       </c>
-      <c r="U90" s="543"/>
-      <c r="V90" s="544" t="s">
+      <c r="U90" s="545"/>
+      <c r="V90" s="537" t="s">
         <v>322</v>
       </c>
-      <c r="W90" s="545"/>
-      <c r="X90" s="545"/>
-      <c r="Y90" s="546"/>
+      <c r="W90" s="538"/>
+      <c r="X90" s="538"/>
+      <c r="Y90" s="539"/>
       <c r="Z90" s="106"/>
       <c r="AA90" s="106"/>
       <c r="AB90" s="114" t="s">
@@ -32254,34 +32287,34 @@
       <c r="E92" s="84"/>
       <c r="F92" s="84"/>
       <c r="G92" s="85"/>
-      <c r="H92" s="535" t="s">
+      <c r="H92" s="540" t="s">
         <v>45</v>
       </c>
-      <c r="I92" s="536"/>
-      <c r="J92" s="536"/>
-      <c r="K92" s="537"/>
-      <c r="L92" s="536" t="s">
+      <c r="I92" s="541"/>
+      <c r="J92" s="541"/>
+      <c r="K92" s="542"/>
+      <c r="L92" s="541" t="s">
         <v>45</v>
       </c>
-      <c r="M92" s="536"/>
-      <c r="N92" s="536"/>
-      <c r="O92" s="537"/>
-      <c r="P92" s="535" t="s">
+      <c r="M92" s="541"/>
+      <c r="N92" s="541"/>
+      <c r="O92" s="542"/>
+      <c r="P92" s="540" t="s">
         <v>45</v>
       </c>
-      <c r="Q92" s="536"/>
-      <c r="R92" s="536"/>
-      <c r="S92" s="537"/>
-      <c r="T92" s="538" t="s">
+      <c r="Q92" s="541"/>
+      <c r="R92" s="541"/>
+      <c r="S92" s="542"/>
+      <c r="T92" s="546" t="s">
         <v>302</v>
       </c>
-      <c r="U92" s="539"/>
-      <c r="V92" s="538" t="s">
+      <c r="U92" s="547"/>
+      <c r="V92" s="546" t="s">
         <v>968</v>
       </c>
-      <c r="W92" s="540"/>
-      <c r="X92" s="540"/>
-      <c r="Y92" s="539"/>
+      <c r="W92" s="548"/>
+      <c r="X92" s="548"/>
+      <c r="Y92" s="547"/>
       <c r="Z92" s="450" t="s">
         <v>980</v>
       </c>
@@ -32376,15 +32409,15 @@
         <v>4.5825000000000005</v>
       </c>
       <c r="W93" s="456">
-        <f t="shared" ref="W93:Y93" si="53">W97*1.3</f>
+        <f t="shared" ref="W93:Y93" si="54">W97*1.3</f>
         <v>4.5825000000000005</v>
       </c>
       <c r="X93" s="456">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>4.5825000000000005</v>
       </c>
       <c r="Y93" s="456">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>4.5825000000000005</v>
       </c>
       <c r="Z93" s="456">
@@ -32396,7 +32429,7 @@
       <c r="AD93" s="118"/>
       <c r="AE93" s="118"/>
       <c r="AF93" s="108">
-        <f t="shared" ref="AF93:AF131" si="54">31.536*(AI93/1000)</f>
+        <f t="shared" ref="AF93:AF131" si="55">31.536*(AI93/1000)</f>
         <v>0.94608000000000003</v>
       </c>
       <c r="AG93" s="111"/>
@@ -32464,15 +32497,15 @@
         <v>0.7</v>
       </c>
       <c r="Q94" s="69">
-        <f t="shared" ref="Q94:Q96" si="55">I94*0.7</f>
+        <f t="shared" ref="Q94:Q96" si="56">I94*0.7</f>
         <v>0.7</v>
       </c>
       <c r="R94" s="69">
-        <f t="shared" ref="R94:R96" si="56">J94*0.7</f>
+        <f t="shared" ref="R94:R96" si="57">J94*0.7</f>
         <v>0.7</v>
       </c>
       <c r="S94" s="103">
-        <f t="shared" ref="S94:S96" si="57">K94*0.7</f>
+        <f t="shared" ref="S94:S96" si="58">K94*0.7</f>
         <v>0.7</v>
       </c>
       <c r="T94" s="99">
@@ -32484,15 +32517,15 @@
         <v>4.9452075289575284</v>
       </c>
       <c r="W94" s="457">
-        <f t="shared" ref="W94:Y94" si="58">W98*1.3</f>
+        <f t="shared" ref="W94:Y94" si="59">W98*1.3</f>
         <v>4.9452075289575284</v>
       </c>
       <c r="X94" s="457">
-        <f t="shared" si="58"/>
+        <f t="shared" si="59"/>
         <v>4.9452075289575284</v>
       </c>
       <c r="Y94" s="457">
-        <f t="shared" si="58"/>
+        <f t="shared" si="59"/>
         <v>4.9452075289575284</v>
       </c>
       <c r="Z94" s="457">
@@ -32504,7 +32537,7 @@
       <c r="AD94" s="119"/>
       <c r="AE94" s="119"/>
       <c r="AF94" s="109">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AG94" s="112"/>
@@ -32516,11 +32549,11 @@
       </c>
       <c r="AK94" s="152"/>
       <c r="AL94" s="151" t="str">
-        <f t="shared" ref="AL94:AL108" si="59">C94</f>
+        <f t="shared" ref="AL94:AL108" si="60">C94</f>
         <v>R-SW_Det_KER_N1</v>
       </c>
       <c r="AM94" s="151" t="str">
-        <f t="shared" ref="AM94:AM108" si="60">D94</f>
+        <f t="shared" ref="AM94:AM108" si="61">D94</f>
         <v>Residential Kerosene Heating Oil - New 2 SH + WH</v>
       </c>
       <c r="AN94" s="152" t="s">
@@ -32570,15 +32603,15 @@
         <v>0.7</v>
       </c>
       <c r="Q95" s="75">
-        <f t="shared" si="55"/>
-        <v>0.7</v>
-      </c>
-      <c r="R95" s="75">
         <f t="shared" si="56"/>
         <v>0.7</v>
       </c>
+      <c r="R95" s="75">
+        <f t="shared" si="57"/>
+        <v>0.7</v>
+      </c>
       <c r="S95" s="104">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>0.7</v>
       </c>
       <c r="T95" s="100">
@@ -32615,7 +32648,7 @@
         <v>5</v>
       </c>
       <c r="AF95" s="108">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AG95" s="111"/>
@@ -32627,11 +32660,11 @@
       </c>
       <c r="AK95" s="152"/>
       <c r="AL95" s="151" t="str">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>R-SW_Det_KER_N2</v>
       </c>
       <c r="AM95" s="151" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="61"/>
         <v>Residential Kerosene Heating Oil - New 3 SH+WH + Solar</v>
       </c>
       <c r="AN95" s="152" t="s">
@@ -32681,15 +32714,15 @@
         <v>0.7</v>
       </c>
       <c r="Q96" s="69">
-        <f t="shared" si="55"/>
-        <v>0.71749999999999992</v>
-      </c>
-      <c r="R96" s="69">
         <f t="shared" si="56"/>
         <v>0.71749999999999992</v>
       </c>
+      <c r="R96" s="69">
+        <f t="shared" si="57"/>
+        <v>0.71749999999999992</v>
+      </c>
       <c r="S96" s="103">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>0.71749999999999992</v>
       </c>
       <c r="T96" s="99">
@@ -32726,7 +32759,7 @@
         <v>5</v>
       </c>
       <c r="AF96" s="109">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AG96" s="112"/>
@@ -32738,11 +32771,11 @@
       </c>
       <c r="AK96" s="152"/>
       <c r="AL96" s="151" t="str">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>R-SW_Det_KER_N3</v>
       </c>
       <c r="AM96" s="151" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="61"/>
         <v>Residential Kerosene Heating Oil - New 3 SH+WH + Wood Stove</v>
       </c>
       <c r="AN96" s="153" t="s">
@@ -32798,15 +32831,15 @@
         <v>3.5249999999999999</v>
       </c>
       <c r="W97" s="456">
-        <f t="shared" ref="W97:Y97" si="61">3.525</f>
+        <f t="shared" ref="W97:Y97" si="62">3.525</f>
         <v>3.5249999999999999</v>
       </c>
       <c r="X97" s="456">
-        <f t="shared" si="61"/>
+        <f t="shared" si="62"/>
         <v>3.5249999999999999</v>
       </c>
       <c r="Y97" s="456">
-        <f t="shared" si="61"/>
+        <f t="shared" si="62"/>
         <v>3.5249999999999999</v>
       </c>
       <c r="Z97" s="456">
@@ -32818,7 +32851,7 @@
       <c r="AD97" s="118"/>
       <c r="AE97" s="118"/>
       <c r="AF97" s="108">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>0.94608000000000003</v>
       </c>
       <c r="AG97" s="111"/>
@@ -32830,11 +32863,11 @@
       </c>
       <c r="AK97" s="152"/>
       <c r="AL97" s="151" t="str">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>R-SH_Det_GAS_N1</v>
       </c>
       <c r="AM97" s="151" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="61"/>
         <v>Residential Natural Gas Heating - New 1 SH</v>
       </c>
       <c r="AN97" s="152" t="s">
@@ -32884,15 +32917,15 @@
         <v>0.7</v>
       </c>
       <c r="Q98" s="69">
-        <f t="shared" ref="Q98:Q100" si="62">I98*0.7</f>
+        <f t="shared" ref="Q98:Q100" si="63">I98*0.7</f>
         <v>0.7</v>
       </c>
       <c r="R98" s="69">
-        <f t="shared" ref="R98:R100" si="63">J98*0.7</f>
+        <f t="shared" ref="R98:R100" si="64">J98*0.7</f>
         <v>0.7</v>
       </c>
       <c r="S98" s="103">
-        <f t="shared" ref="S98:S100" si="64">K98*0.7</f>
+        <f t="shared" ref="S98:S100" si="65">K98*0.7</f>
         <v>0.7</v>
       </c>
       <c r="T98" s="99">
@@ -32924,7 +32957,7 @@
       <c r="AD98" s="119"/>
       <c r="AE98" s="119"/>
       <c r="AF98" s="109">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AG98" s="112"/>
@@ -32936,11 +32969,11 @@
       </c>
       <c r="AK98" s="152"/>
       <c r="AL98" s="151" t="str">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>R-SW_Det_GAS_N1</v>
       </c>
       <c r="AM98" s="151" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="61"/>
         <v>Residential Natural Gas Heating - New 2 SH + WH</v>
       </c>
       <c r="AN98" s="152" t="s">
@@ -32990,15 +33023,15 @@
         <v>0.7</v>
       </c>
       <c r="Q99" s="75">
-        <f t="shared" si="62"/>
-        <v>0.7</v>
-      </c>
-      <c r="R99" s="75">
         <f t="shared" si="63"/>
         <v>0.7</v>
       </c>
+      <c r="R99" s="75">
+        <f t="shared" si="64"/>
+        <v>0.7</v>
+      </c>
       <c r="S99" s="104">
-        <f t="shared" si="64"/>
+        <f t="shared" si="65"/>
         <v>0.7</v>
       </c>
       <c r="T99" s="100">
@@ -33033,7 +33066,7 @@
         <v>5</v>
       </c>
       <c r="AF99" s="108">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AG99" s="111"/>
@@ -33045,11 +33078,11 @@
       </c>
       <c r="AK99" s="152"/>
       <c r="AL99" s="151" t="str">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>R-SW_Det_GAS_N2</v>
       </c>
       <c r="AM99" s="151" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="61"/>
         <v>Residential Natural Gas Heating - New 3 SH + WH + Solar</v>
       </c>
       <c r="AN99" s="152" t="s">
@@ -33099,15 +33132,15 @@
         <v>0.7</v>
       </c>
       <c r="Q100" s="69">
-        <f t="shared" si="62"/>
-        <v>0.71749999999999992</v>
-      </c>
-      <c r="R100" s="69">
         <f t="shared" si="63"/>
         <v>0.71749999999999992</v>
       </c>
+      <c r="R100" s="69">
+        <f t="shared" si="64"/>
+        <v>0.71749999999999992</v>
+      </c>
       <c r="S100" s="103">
-        <f t="shared" si="64"/>
+        <f t="shared" si="65"/>
         <v>0.71749999999999992</v>
       </c>
       <c r="T100" s="99">
@@ -33144,7 +33177,7 @@
         <v>5</v>
       </c>
       <c r="AF100" s="109">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AG100" s="112"/>
@@ -33156,11 +33189,11 @@
       </c>
       <c r="AK100" s="152"/>
       <c r="AL100" s="151" t="str">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>R-SW_Det_GAS_N3</v>
       </c>
       <c r="AM100" s="151" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="61"/>
         <v>Residential Natural Gas Heating - New 4 SH + WH + Wood Stove</v>
       </c>
       <c r="AN100" s="152" t="s">
@@ -33214,23 +33247,24 @@
       </c>
       <c r="U101" s="87"/>
       <c r="V101" s="456">
-        <f>V97</f>
-        <v>3.5249999999999999</v>
+        <f>V97+0.25</f>
+        <v>3.7749999999999999</v>
       </c>
       <c r="W101" s="456">
-        <f t="shared" ref="W101:Y101" si="65">W97</f>
-        <v>3.5249999999999999</v>
+        <f t="shared" ref="W101:Y101" si="66">W97+0.25</f>
+        <v>3.7749999999999999</v>
       </c>
       <c r="X101" s="456">
-        <f t="shared" si="65"/>
-        <v>3.5249999999999999</v>
+        <f t="shared" si="66"/>
+        <v>3.7749999999999999</v>
       </c>
       <c r="Y101" s="456">
-        <f t="shared" si="65"/>
-        <v>3.5249999999999999</v>
+        <f t="shared" si="66"/>
+        <v>3.7749999999999999</v>
       </c>
       <c r="Z101" s="456">
-        <v>0.12</v>
+        <f>SUM(0.12+0.15)</f>
+        <v>0.27</v>
       </c>
       <c r="AA101" s="111"/>
       <c r="AB101" s="88"/>
@@ -33238,7 +33272,7 @@
       <c r="AD101" s="118"/>
       <c r="AE101" s="118"/>
       <c r="AF101" s="108">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>0.94608000000000003</v>
       </c>
       <c r="AG101" s="111"/>
@@ -33250,11 +33284,11 @@
       </c>
       <c r="AK101" s="152"/>
       <c r="AL101" s="151" t="str">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>R-SH_Det_LPG_N1</v>
       </c>
       <c r="AM101" s="151" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="61"/>
         <v>Residential Liquid Petroleum Gas- New 1 SH</v>
       </c>
       <c r="AN101" s="152" t="s">
@@ -33304,15 +33338,15 @@
         <v>0.7</v>
       </c>
       <c r="Q102" s="69">
-        <f t="shared" ref="Q102" si="66">I102*0.7</f>
+        <f t="shared" ref="Q102" si="67">I102*0.7</f>
         <v>0.7</v>
       </c>
       <c r="R102" s="69">
-        <f t="shared" ref="R102" si="67">J102*0.7</f>
+        <f t="shared" ref="R102" si="68">J102*0.7</f>
         <v>0.7</v>
       </c>
       <c r="S102" s="103">
-        <f t="shared" ref="S102" si="68">K102*0.7</f>
+        <f t="shared" ref="S102" si="69">K102*0.7</f>
         <v>0.7</v>
       </c>
       <c r="T102" s="99">
@@ -33324,19 +33358,20 @@
         <v>3.8040057915057912</v>
       </c>
       <c r="W102" s="457">
-        <f t="shared" ref="W102:Y102" si="69">W98</f>
+        <f t="shared" ref="W102:Y102" si="70">W98</f>
         <v>3.8040057915057912</v>
       </c>
       <c r="X102" s="457">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>3.8040057915057912</v>
       </c>
       <c r="Y102" s="457">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>3.8040057915057912</v>
       </c>
-      <c r="Z102" s="457">
-        <v>0.12</v>
+      <c r="Z102" s="456">
+        <f>SUM(0.12+0.15)</f>
+        <v>0.27</v>
       </c>
       <c r="AA102" s="112"/>
       <c r="AB102" s="90"/>
@@ -33344,7 +33379,7 @@
       <c r="AD102" s="119"/>
       <c r="AE102" s="119"/>
       <c r="AF102" s="109">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AG102" s="112"/>
@@ -33356,11 +33391,11 @@
       </c>
       <c r="AK102" s="152"/>
       <c r="AL102" s="151" t="str">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>R-SW_Det_LPG_N1</v>
       </c>
       <c r="AM102" s="151" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="61"/>
         <v>Residential Liquid Petroleum Gas- New 2 SH + WH</v>
       </c>
       <c r="AN102" s="152" t="s">
@@ -33437,7 +33472,7 @@
       <c r="AD103" s="118"/>
       <c r="AE103" s="118"/>
       <c r="AF103" s="108">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>0.94608000000000003</v>
       </c>
       <c r="AG103" s="111"/>
@@ -33449,11 +33484,11 @@
       </c>
       <c r="AK103" s="152"/>
       <c r="AL103" s="151" t="str">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>R-SH_Det_WOO_N1</v>
       </c>
       <c r="AM103" s="151" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="61"/>
         <v>Residential Biomass Boiler - New 1 SH</v>
       </c>
       <c r="AN103" s="152" t="s">
@@ -33499,19 +33534,19 @@
       <c r="N104" s="78"/>
       <c r="O104" s="91"/>
       <c r="P104" s="68">
-        <f t="shared" ref="P104:S108" si="70">H104*0.7</f>
+        <f t="shared" ref="P104:S108" si="71">H104*0.7</f>
         <v>0.7</v>
       </c>
       <c r="Q104" s="69">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>0.7</v>
       </c>
       <c r="R104" s="69">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>0.7</v>
       </c>
       <c r="S104" s="103">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>0.7</v>
       </c>
       <c r="T104" s="99">
@@ -33523,15 +33558,15 @@
         <v>22.778925619834713</v>
       </c>
       <c r="W104" s="457">
-        <f t="shared" ref="W104" si="71">W103*($U$152/$U$151)</f>
+        <f t="shared" ref="W104" si="72">W103*($U$152/$U$151)</f>
         <v>22.04476084710744</v>
       </c>
       <c r="X104" s="457">
-        <f t="shared" ref="X104" si="72">X103*($U$152/$U$151)</f>
+        <f t="shared" ref="X104" si="73">X103*($U$152/$U$151)</f>
         <v>20.839163429752066</v>
       </c>
       <c r="Y104" s="457">
-        <f t="shared" ref="Y104" si="73">Y103*($U$152/$U$151)</f>
+        <f t="shared" ref="Y104" si="74">Y103*($U$152/$U$151)</f>
         <v>18.635439049586779</v>
       </c>
       <c r="Z104" s="457">
@@ -33543,7 +33578,7 @@
       <c r="AD104" s="119"/>
       <c r="AE104" s="119"/>
       <c r="AF104" s="109">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AG104" s="112"/>
@@ -33555,11 +33590,11 @@
       </c>
       <c r="AK104" s="155"/>
       <c r="AL104" s="154" t="str">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>R-SW_Det_WOO_N1</v>
       </c>
       <c r="AM104" s="154" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="61"/>
         <v>Residential Biomass Boiler - New 2 SH + WH</v>
       </c>
       <c r="AN104" s="155" t="s">
@@ -33613,7 +33648,7 @@
       <c r="AD105" s="119"/>
       <c r="AE105" s="119"/>
       <c r="AF105" s="109">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>0.94608000000000003</v>
       </c>
       <c r="AG105" s="112"/>
@@ -33628,7 +33663,7 @@
         <v>1042</v>
       </c>
       <c r="AM105" s="154" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="61"/>
         <v>Residential  Fireplace New 1 - SH</v>
       </c>
       <c r="AN105" s="152" t="s">
@@ -33680,7 +33715,7 @@
       <c r="AD106" s="119"/>
       <c r="AE106" s="119"/>
       <c r="AF106" s="109">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AG106" s="112"/>
@@ -33695,7 +33730,7 @@
         <v>1043</v>
       </c>
       <c r="AM106" s="154" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="61"/>
         <v>Residential  Fireplace with back boiler New 1 - SH +WH</v>
       </c>
       <c r="AN106" s="155" t="s">
@@ -33738,19 +33773,19 @@
       <c r="N107" s="77"/>
       <c r="O107" s="89"/>
       <c r="P107" s="86">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>0.7</v>
       </c>
       <c r="Q107" s="75">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>0.7</v>
       </c>
       <c r="R107" s="75">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>0.7</v>
       </c>
       <c r="S107" s="104">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>0.7</v>
       </c>
       <c r="T107" s="100">
@@ -33783,7 +33818,7 @@
       <c r="AD107" s="118"/>
       <c r="AE107" s="118"/>
       <c r="AF107" s="108">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>0.94608000000000003</v>
       </c>
       <c r="AG107" s="111"/>
@@ -33795,11 +33830,11 @@
       </c>
       <c r="AK107" s="155"/>
       <c r="AL107" s="154" t="str">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>*R-H_Apt_HVO_N1</v>
       </c>
       <c r="AM107" s="154" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="61"/>
         <v>Residential  Hydrotreated vegetable oil - New 1 SH</v>
       </c>
       <c r="AN107" s="155" t="s">
@@ -33844,19 +33879,19 @@
       <c r="N108" s="96"/>
       <c r="O108" s="97"/>
       <c r="P108" s="329">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>0.7</v>
       </c>
       <c r="Q108" s="72">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>0.7</v>
       </c>
       <c r="R108" s="72">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>0.7</v>
       </c>
       <c r="S108" s="105">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>0.7</v>
       </c>
       <c r="T108" s="101">
@@ -33889,7 +33924,7 @@
       <c r="AD108" s="119"/>
       <c r="AE108" s="119"/>
       <c r="AF108" s="109">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AG108" s="113"/>
@@ -33901,11 +33936,11 @@
       </c>
       <c r="AK108" s="155"/>
       <c r="AL108" s="154" t="str">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>*R-H_Apt_HVO_N2</v>
       </c>
       <c r="AM108" s="154" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="61"/>
         <v>Residential  Hydrotreated vegetable oil - New 1 SH + WH</v>
       </c>
       <c r="AN108" s="155" t="s">
@@ -34040,7 +34075,7 @@
       <c r="AD110" s="130"/>
       <c r="AE110" s="130"/>
       <c r="AF110" s="128">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>0.94608000000000003</v>
       </c>
       <c r="AG110" s="129"/>
@@ -34052,11 +34087,11 @@
       </c>
       <c r="AK110" s="150"/>
       <c r="AL110" s="149" t="str">
-        <f t="shared" ref="AL110:AL116" si="74">C112</f>
+        <f t="shared" ref="AL110:AL116" si="75">C112</f>
         <v>R-SH_Det_ELC_HPN1</v>
       </c>
       <c r="AM110" s="149" t="str">
-        <f t="shared" ref="AM110:AM116" si="75">D112</f>
+        <f t="shared" ref="AM110:AM116" si="76">D112</f>
         <v>Residential Electric Heat Pump - Air to Air - SH</v>
       </c>
       <c r="AN110" s="150" t="s">
@@ -34108,11 +34143,11 @@
       <c r="AI111" s="80"/>
       <c r="AK111" s="152"/>
       <c r="AL111" s="151" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v>R-HC_Det_ELC_HPN1</v>
       </c>
       <c r="AM111" s="151" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v>Residential Electric Heat Pump - Air to Air - SH + SC</v>
       </c>
       <c r="AN111" s="152" t="s">
@@ -34193,7 +34228,7 @@
       <c r="AD112" s="131"/>
       <c r="AE112" s="131"/>
       <c r="AF112" s="131">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>0.31536000000000003</v>
       </c>
       <c r="AG112" s="134"/>
@@ -34205,11 +34240,11 @@
       </c>
       <c r="AK112" s="152"/>
       <c r="AL112" s="151" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v>R-SH_Det_ELC_HPN2</v>
       </c>
       <c r="AM112" s="151" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v>Residential Electric Heat Pump - Air to Water - SH</v>
       </c>
       <c r="AN112" s="152" t="s">
@@ -34298,7 +34333,7 @@
       <c r="AD113" s="109"/>
       <c r="AE113" s="109"/>
       <c r="AF113" s="109">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>0.37843200000000005</v>
       </c>
       <c r="AG113" s="112"/>
@@ -34310,11 +34345,11 @@
       </c>
       <c r="AK113" s="152"/>
       <c r="AL113" s="151" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v>R-SW_Det_ELC_HPN1</v>
       </c>
       <c r="AM113" s="151" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v>Residential Electric Heat Pump - Air to Water - SH + WH</v>
       </c>
       <c r="AN113" s="152" t="s">
@@ -34393,7 +34428,7 @@
       <c r="AD114" s="108"/>
       <c r="AE114" s="108"/>
       <c r="AF114" s="108">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>0.31536000000000003</v>
       </c>
       <c r="AG114" s="111"/>
@@ -34405,11 +34440,11 @@
       </c>
       <c r="AK114" s="286"/>
       <c r="AL114" s="151" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v>R-SW_Det_ELC_HPN2</v>
       </c>
       <c r="AM114" s="151" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v>Residential Electric Heat Pump - Air to Water - SH + WH + Solar</v>
       </c>
       <c r="AN114" s="152" t="s">
@@ -34461,15 +34496,15 @@
         <v>0.7</v>
       </c>
       <c r="Q115" s="69">
-        <f t="shared" ref="Q115:Q116" si="76">I115*0.7</f>
+        <f t="shared" ref="Q115:Q116" si="77">I115*0.7</f>
         <v>0.76999999999999991</v>
       </c>
       <c r="R115" s="69">
-        <f t="shared" ref="R115:R116" si="77">J115*0.7</f>
+        <f t="shared" ref="R115:R116" si="78">J115*0.7</f>
         <v>0.86333333333333329</v>
       </c>
       <c r="S115" s="103">
-        <f t="shared" ref="S115:S116" si="78">K115*0.7</f>
+        <f t="shared" ref="S115:S116" si="79">K115*0.7</f>
         <v>0.93333333333333324</v>
       </c>
       <c r="T115" s="99">
@@ -34481,15 +34516,15 @@
         <v>9.9300970464135023</v>
       </c>
       <c r="W115" s="457">
-        <f t="shared" ref="W115" si="79">W114*($U$150/$U$149)</f>
+        <f t="shared" ref="W115" si="80">W114*($U$150/$U$149)</f>
         <v>9.0363883122362889</v>
       </c>
       <c r="X115" s="457">
-        <f t="shared" ref="X115" si="80">X114*($U$150/$U$149)</f>
+        <f t="shared" ref="X115" si="81">X114*($U$150/$U$149)</f>
         <v>8.2231133641350223</v>
       </c>
       <c r="Y115" s="457">
-        <f t="shared" ref="Y115" si="81">Y114*($U$150/$U$149)</f>
+        <f t="shared" ref="Y115" si="82">Y114*($U$150/$U$149)</f>
         <v>8.1426795780590719</v>
       </c>
       <c r="Z115" s="457">
@@ -34501,7 +34536,7 @@
       <c r="AD115" s="109"/>
       <c r="AE115" s="109"/>
       <c r="AF115" s="109">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>0.37843200000000005</v>
       </c>
       <c r="AG115" s="112"/>
@@ -34513,11 +34548,11 @@
       </c>
       <c r="AK115" s="286"/>
       <c r="AL115" s="151" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v>R-SH_Det_ELC_HPN3</v>
       </c>
       <c r="AM115" s="151" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v>Residential Electric Heat Pump - Ground to Water - SH</v>
       </c>
       <c r="AN115" s="152" t="s">
@@ -34569,15 +34604,15 @@
         <v>0.7</v>
       </c>
       <c r="Q116" s="75">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>0.77700000000000002</v>
       </c>
       <c r="R116" s="75">
-        <f t="shared" si="77"/>
+        <f t="shared" si="78"/>
         <v>0.83299999999999996</v>
       </c>
       <c r="S116" s="104">
-        <f t="shared" si="78"/>
+        <f t="shared" si="79"/>
         <v>0.83299999999999996</v>
       </c>
       <c r="T116" s="100">
@@ -34614,7 +34649,7 @@
         <v>5</v>
       </c>
       <c r="AF116" s="108">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>0.37843200000000005</v>
       </c>
       <c r="AG116" s="111"/>
@@ -34626,11 +34661,11 @@
       </c>
       <c r="AK116" s="158"/>
       <c r="AL116" s="154" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v>R-HC_Det_ELC_HPN2</v>
       </c>
       <c r="AM116" s="154" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v>Residential Electric Heat Pump - Ground to Water - SH + SC</v>
       </c>
       <c r="AN116" s="155" t="s">
@@ -34711,7 +34746,7 @@
       <c r="AD117" s="109"/>
       <c r="AE117" s="109"/>
       <c r="AF117" s="109">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>0.31536000000000003</v>
       </c>
       <c r="AG117" s="112"/>
@@ -34816,7 +34851,7 @@
       <c r="AD118" s="132"/>
       <c r="AE118" s="132"/>
       <c r="AF118" s="132">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>0.37843200000000005</v>
       </c>
       <c r="AG118" s="137"/>
@@ -34944,15 +34979,15 @@
         <v>1.1666666666666667</v>
       </c>
       <c r="Q120" s="66">
-        <f t="shared" ref="Q120:Q121" si="82">I120*0.7</f>
+        <f t="shared" ref="Q120:Q121" si="83">I120*0.7</f>
         <v>1.2530864197530862</v>
       </c>
       <c r="R120" s="66">
-        <f t="shared" ref="R120:R121" si="83">J120*0.7</f>
+        <f t="shared" ref="R120:R121" si="84">J120*0.7</f>
         <v>1.4691358024691357</v>
       </c>
       <c r="S120" s="102">
-        <f t="shared" ref="S120:S121" si="84">K120*0.7</f>
+        <f t="shared" ref="S120:S121" si="85">K120*0.7</f>
         <v>1.4691358024691357</v>
       </c>
       <c r="T120" s="135">
@@ -34985,11 +35020,11 @@
       <c r="AD120" s="131"/>
       <c r="AE120" s="131"/>
       <c r="AF120" s="131">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AG120" s="134"/>
-      <c r="AH120" s="560">
+      <c r="AH120" s="520">
         <v>2100</v>
       </c>
       <c r="AI120" s="134">
@@ -35057,15 +35092,15 @@
         <v>1.1666666666666665</v>
       </c>
       <c r="Q121" s="72">
-        <f t="shared" si="82"/>
-        <v>1.2055555555555555</v>
-      </c>
-      <c r="R121" s="72">
         <f t="shared" si="83"/>
         <v>1.2055555555555555</v>
       </c>
+      <c r="R121" s="72">
+        <f t="shared" si="84"/>
+        <v>1.2055555555555555</v>
+      </c>
       <c r="S121" s="105">
-        <f t="shared" si="84"/>
+        <f t="shared" si="85"/>
         <v>1.2444444444444445</v>
       </c>
       <c r="T121" s="73">
@@ -35098,11 +35133,11 @@
       <c r="AD121" s="110"/>
       <c r="AE121" s="110"/>
       <c r="AF121" s="110">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AG121" s="113"/>
-      <c r="AH121" s="561">
+      <c r="AH121" s="521">
         <v>2100</v>
       </c>
       <c r="AI121" s="113">
@@ -35166,11 +35201,11 @@
       <c r="AI122" s="80"/>
       <c r="AK122" s="289"/>
       <c r="AL122" s="149" t="str">
-        <f t="shared" ref="AL122:AL123" si="85">C128</f>
+        <f t="shared" ref="AL122:AL123" si="86">C128</f>
         <v>R-WH_Det_ELC_N1</v>
       </c>
       <c r="AM122" s="149" t="str">
-        <f t="shared" ref="AM122:AM123" si="86">D128</f>
+        <f t="shared" ref="AM122:AM123" si="87">D128</f>
         <v xml:space="preserve">Residential Electric Water Heater </v>
       </c>
       <c r="AN122" s="150" t="s">
@@ -35226,15 +35261,15 @@
         <v>2.2889999999999997</v>
       </c>
       <c r="Q123" s="72">
-        <f t="shared" ref="Q123" si="87">I123*0.7</f>
+        <f t="shared" ref="Q123" si="88">I123*0.7</f>
         <v>2.5409999999999995</v>
       </c>
       <c r="R123" s="72">
-        <f t="shared" ref="R123" si="88">J123*0.7</f>
+        <f t="shared" ref="R123" si="89">J123*0.7</f>
         <v>2.7299999999999995</v>
       </c>
       <c r="S123" s="105">
-        <f t="shared" ref="S123" si="89">K123*0.7</f>
+        <f t="shared" ref="S123" si="90">K123*0.7</f>
         <v>2.7299999999999995</v>
       </c>
       <c r="T123" s="5">
@@ -35270,7 +35305,7 @@
         <v>5</v>
       </c>
       <c r="AF123" s="128">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>0.62441279999999999</v>
       </c>
       <c r="AG123" s="129"/>
@@ -35283,11 +35318,11 @@
       </c>
       <c r="AK123" s="4"/>
       <c r="AL123" s="151" t="str">
-        <f t="shared" si="85"/>
+        <f t="shared" si="86"/>
         <v>R-WH_Det_SOL_N1</v>
       </c>
       <c r="AM123" s="151" t="str">
-        <f t="shared" si="86"/>
+        <f t="shared" si="87"/>
         <v xml:space="preserve">Residential Solar Water Heater </v>
       </c>
       <c r="AN123" s="152" t="s">
@@ -35430,7 +35465,7 @@
       <c r="AD125" s="131"/>
       <c r="AE125" s="131"/>
       <c r="AF125" s="131">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AG125" s="134"/>
@@ -35510,7 +35545,7 @@
       <c r="AD126" s="110"/>
       <c r="AE126" s="110"/>
       <c r="AF126" s="110">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AG126" s="113"/>
@@ -35623,7 +35658,7 @@
       <c r="AD128" s="131"/>
       <c r="AE128" s="131"/>
       <c r="AF128" s="131">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>0.25228800000000001</v>
       </c>
       <c r="AG128" s="134"/>
@@ -35701,7 +35736,7 @@
       <c r="AD129" s="109"/>
       <c r="AE129" s="109"/>
       <c r="AF129" s="109">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>0.25228800000000001</v>
       </c>
       <c r="AG129" s="113"/>
@@ -35814,7 +35849,7 @@
       <c r="AD131" s="139"/>
       <c r="AE131" s="139"/>
       <c r="AF131" s="139">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>0.25228800000000001</v>
       </c>
       <c r="AG131" s="138"/>
@@ -35895,7 +35930,7 @@
         <v>3</v>
       </c>
       <c r="U145" s="454">
-        <f t="shared" ref="U145:U154" si="90">V145/$V$153</f>
+        <f t="shared" ref="U145:U154" si="91">V145/$V$153</f>
         <v>0.72929037751472525</v>
       </c>
       <c r="V145" s="455">
@@ -35909,7 +35944,7 @@
         <v>5</v>
       </c>
       <c r="U146" s="454">
-        <f t="shared" si="90"/>
+        <f t="shared" si="91"/>
         <v>0.79101166159768732</v>
       </c>
       <c r="V146" s="455">
@@ -35922,7 +35957,7 @@
         <v>8</v>
       </c>
       <c r="U147" s="454">
-        <f t="shared" si="90"/>
+        <f t="shared" si="91"/>
         <v>0.85077698714062355</v>
       </c>
       <c r="V147" s="455">
@@ -35936,7 +35971,7 @@
         <v>10</v>
       </c>
       <c r="U148" s="454">
-        <f t="shared" si="90"/>
+        <f t="shared" si="91"/>
         <v>0.86872586872586877</v>
       </c>
       <c r="V148" s="453">
@@ -35957,7 +35992,7 @@
         <v>15</v>
       </c>
       <c r="U149" s="444">
-        <f t="shared" si="90"/>
+        <f t="shared" si="91"/>
         <v>0.91505791505791501</v>
       </c>
       <c r="V149" s="5">
@@ -35984,7 +36019,7 @@
         <v>18</v>
       </c>
       <c r="U150" s="444">
-        <f t="shared" si="90"/>
+        <f t="shared" si="91"/>
         <v>0.92277992277992282</v>
       </c>
       <c r="V150" s="5">
@@ -36013,7 +36048,7 @@
         <v>20</v>
       </c>
       <c r="U151" s="454">
-        <f t="shared" si="90"/>
+        <f t="shared" si="91"/>
         <v>0.93436293436293438</v>
       </c>
       <c r="V151" s="453">
@@ -36043,7 +36078,7 @@
         <v>24</v>
       </c>
       <c r="U152" s="444">
-        <f t="shared" si="90"/>
+        <f t="shared" si="91"/>
         <v>0.94594594594594594</v>
       </c>
       <c r="V152" s="5">
@@ -36072,7 +36107,7 @@
         <v>30</v>
       </c>
       <c r="U153" s="444">
-        <f t="shared" si="90"/>
+        <f t="shared" si="91"/>
         <v>1</v>
       </c>
       <c r="V153" s="5">
@@ -36101,7 +36136,7 @@
         <v>35</v>
       </c>
       <c r="U154" s="444">
-        <f t="shared" si="90"/>
+        <f t="shared" si="91"/>
         <v>1.0791505791505791</v>
       </c>
       <c r="V154" s="5">
@@ -36146,6 +36181,26 @@
     <row r="166" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="H92:K92"/>
+    <mergeCell ref="L92:O92"/>
+    <mergeCell ref="P92:S92"/>
+    <mergeCell ref="T92:U92"/>
+    <mergeCell ref="V92:Y92"/>
+    <mergeCell ref="H90:K90"/>
+    <mergeCell ref="L90:O90"/>
+    <mergeCell ref="P90:S90"/>
+    <mergeCell ref="T90:U90"/>
+    <mergeCell ref="V90:Y90"/>
+    <mergeCell ref="H44:K44"/>
+    <mergeCell ref="L44:O44"/>
+    <mergeCell ref="P44:S44"/>
+    <mergeCell ref="T44:U44"/>
+    <mergeCell ref="V44:Y44"/>
+    <mergeCell ref="H42:K42"/>
+    <mergeCell ref="L42:O42"/>
+    <mergeCell ref="P42:S42"/>
+    <mergeCell ref="T42:U42"/>
+    <mergeCell ref="V42:Y42"/>
     <mergeCell ref="V4:Y4"/>
     <mergeCell ref="V6:Y6"/>
     <mergeCell ref="H4:K4"/>
@@ -36156,26 +36211,6 @@
     <mergeCell ref="P6:S6"/>
     <mergeCell ref="L6:O6"/>
     <mergeCell ref="H6:K6"/>
-    <mergeCell ref="H42:K42"/>
-    <mergeCell ref="L42:O42"/>
-    <mergeCell ref="P42:S42"/>
-    <mergeCell ref="T42:U42"/>
-    <mergeCell ref="V42:Y42"/>
-    <mergeCell ref="H44:K44"/>
-    <mergeCell ref="L44:O44"/>
-    <mergeCell ref="P44:S44"/>
-    <mergeCell ref="T44:U44"/>
-    <mergeCell ref="V44:Y44"/>
-    <mergeCell ref="H90:K90"/>
-    <mergeCell ref="L90:O90"/>
-    <mergeCell ref="P90:S90"/>
-    <mergeCell ref="T90:U90"/>
-    <mergeCell ref="V90:Y90"/>
-    <mergeCell ref="H92:K92"/>
-    <mergeCell ref="L92:O92"/>
-    <mergeCell ref="P92:S92"/>
-    <mergeCell ref="T92:U92"/>
-    <mergeCell ref="V92:Y92"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
@@ -36320,12 +36355,12 @@
       <c r="I5" s="173"/>
       <c r="J5" s="173"/>
       <c r="K5" s="173"/>
-      <c r="L5" s="544" t="s">
+      <c r="L5" s="537" t="s">
         <v>322</v>
       </c>
-      <c r="M5" s="545"/>
-      <c r="N5" s="545"/>
-      <c r="O5" s="546"/>
+      <c r="M5" s="538"/>
+      <c r="N5" s="538"/>
+      <c r="O5" s="539"/>
       <c r="P5" s="106"/>
       <c r="Q5" s="106" t="s">
         <v>323</v>
@@ -36356,12 +36391,12 @@
       <c r="I6" s="83"/>
       <c r="J6" s="83"/>
       <c r="K6" s="83"/>
-      <c r="L6" s="538" t="s">
+      <c r="L6" s="546" t="s">
         <v>968</v>
       </c>
-      <c r="M6" s="540"/>
-      <c r="N6" s="540"/>
-      <c r="O6" s="539"/>
+      <c r="M6" s="548"/>
+      <c r="N6" s="548"/>
+      <c r="O6" s="547"/>
       <c r="P6" s="450" t="s">
         <v>980</v>
       </c>
@@ -36987,10 +37022,10 @@
       <c r="C18" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="R18" s="547" t="s">
+      <c r="R18" s="549" t="s">
         <v>662</v>
       </c>
-      <c r="S18" s="547"/>
+      <c r="S18" s="549"/>
       <c r="U18" s="5" t="s">
         <v>861</v>
       </c>
@@ -37023,8 +37058,8 @@
       <c r="J19" s="195" t="s">
         <v>301</v>
       </c>
-      <c r="R19" s="547"/>
-      <c r="S19" s="547"/>
+      <c r="R19" s="549"/>
+      <c r="S19" s="549"/>
       <c r="V19" s="5" t="s">
         <v>1023</v>
       </c>
@@ -37050,8 +37085,8 @@
       <c r="J20" s="170" t="s">
         <v>1028</v>
       </c>
-      <c r="R20" s="547"/>
-      <c r="S20" s="547"/>
+      <c r="R20" s="549"/>
+      <c r="S20" s="549"/>
       <c r="V20" s="5" t="s">
         <v>1024</v>
       </c>
@@ -37078,8 +37113,8 @@
       <c r="J21" s="170" t="s">
         <v>1028</v>
       </c>
-      <c r="R21" s="547"/>
-      <c r="S21" s="547"/>
+      <c r="R21" s="549"/>
+      <c r="S21" s="549"/>
     </row>
     <row r="22" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C22" s="168" t="s">
@@ -37103,8 +37138,8 @@
       <c r="J22" s="170" t="s">
         <v>1028</v>
       </c>
-      <c r="R22" s="547"/>
-      <c r="S22" s="547"/>
+      <c r="R22" s="549"/>
+      <c r="S22" s="549"/>
     </row>
     <row r="23" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C23" s="168" t="s">
@@ -37279,23 +37314,23 @@
       <c r="K33" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="L33" s="544" t="s">
+      <c r="L33" s="537" t="s">
         <v>322</v>
       </c>
-      <c r="M33" s="545"/>
-      <c r="N33" s="545"/>
-      <c r="O33" s="546"/>
+      <c r="M33" s="538"/>
+      <c r="N33" s="538"/>
+      <c r="O33" s="539"/>
     </row>
     <row r="34" spans="8:15" x14ac:dyDescent="0.2">
       <c r="H34" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="L34" s="538" t="s">
+      <c r="L34" s="546" t="s">
         <v>327</v>
       </c>
-      <c r="M34" s="540"/>
-      <c r="N34" s="540"/>
-      <c r="O34" s="539"/>
+      <c r="M34" s="548"/>
+      <c r="N34" s="548"/>
+      <c r="O34" s="547"/>
     </row>
     <row r="35" spans="8:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H35" s="5" t="s">
@@ -37637,16 +37672,16 @@
       <c r="G4" s="173" t="s">
         <v>321</v>
       </c>
-      <c r="H4" s="541" t="s">
+      <c r="H4" s="543" t="s">
         <v>110</v>
       </c>
-      <c r="I4" s="542"/>
-      <c r="J4" s="543"/>
-      <c r="K4" s="544" t="s">
+      <c r="I4" s="544"/>
+      <c r="J4" s="545"/>
+      <c r="K4" s="537" t="s">
         <v>322</v>
       </c>
-      <c r="L4" s="545"/>
-      <c r="M4" s="546"/>
+      <c r="L4" s="538"/>
+      <c r="M4" s="539"/>
       <c r="N4" s="106"/>
       <c r="O4" s="106" t="s">
         <v>323</v>
@@ -37672,16 +37707,16 @@
       <c r="G5" s="458" t="s">
         <v>302</v>
       </c>
-      <c r="H5" s="551" t="s">
+      <c r="H5" s="550" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="552"/>
-      <c r="J5" s="553"/>
-      <c r="K5" s="551" t="s">
+      <c r="I5" s="551"/>
+      <c r="J5" s="552"/>
+      <c r="K5" s="550" t="s">
         <v>757</v>
       </c>
-      <c r="L5" s="552"/>
-      <c r="M5" s="553"/>
+      <c r="L5" s="551"/>
+      <c r="M5" s="552"/>
       <c r="N5" s="459" t="s">
         <v>328</v>
       </c>
@@ -37698,23 +37733,23 @@
         <v>626</v>
       </c>
       <c r="AA5" s="281"/>
-      <c r="AB5" s="548" t="s">
+      <c r="AB5" s="553" t="s">
         <v>1013</v>
       </c>
-      <c r="AC5" s="548"/>
+      <c r="AC5" s="553"/>
       <c r="AD5" s="461"/>
-      <c r="AE5" s="549" t="s">
+      <c r="AE5" s="554" t="s">
         <v>110</v>
       </c>
-      <c r="AF5" s="549"/>
-      <c r="AG5" s="549" t="s">
+      <c r="AF5" s="554"/>
+      <c r="AG5" s="554" t="s">
         <v>1014</v>
       </c>
-      <c r="AH5" s="549"/>
-      <c r="AI5" s="550" t="s">
+      <c r="AH5" s="554"/>
+      <c r="AI5" s="555" t="s">
         <v>1015</v>
       </c>
-      <c r="AJ5" s="550"/>
+      <c r="AJ5" s="555"/>
     </row>
     <row r="6" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C6" s="505" t="str">
@@ -38452,12 +38487,12 @@
       <c r="K27" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="L27" s="544" t="s">
+      <c r="L27" s="537" t="s">
         <v>322</v>
       </c>
-      <c r="M27" s="545"/>
-      <c r="N27" s="545"/>
-      <c r="O27" s="546"/>
+      <c r="M27" s="538"/>
+      <c r="N27" s="538"/>
+      <c r="O27" s="539"/>
       <c r="T27" s="283"/>
       <c r="U27" s="283"/>
     </row>
@@ -38465,12 +38500,12 @@
       <c r="J28" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="L28" s="535" t="s">
+      <c r="L28" s="540" t="s">
         <v>327</v>
       </c>
-      <c r="M28" s="536"/>
-      <c r="N28" s="536"/>
-      <c r="O28" s="537"/>
+      <c r="M28" s="541"/>
+      <c r="N28" s="541"/>
+      <c r="O28" s="542"/>
       <c r="T28" s="283"/>
       <c r="U28" s="283"/>
     </row>
@@ -39860,16 +39895,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="AB5:AC5"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AG5:AH5"/>
+    <mergeCell ref="AI5:AJ5"/>
+    <mergeCell ref="L27:O27"/>
     <mergeCell ref="L28:O28"/>
     <mergeCell ref="H4:J4"/>
     <mergeCell ref="K4:M4"/>
     <mergeCell ref="H5:J5"/>
     <mergeCell ref="K5:M5"/>
-    <mergeCell ref="AB5:AC5"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="AG5:AH5"/>
-    <mergeCell ref="AI5:AJ5"/>
-    <mergeCell ref="L27:O27"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="S7" r:id="rId1" xr:uid="{B1EDD63D-40A5-4174-9D28-8666BD314B83}"/>
@@ -48897,128 +48932,128 @@
       <c r="C4" s="356" t="s">
         <v>766</v>
       </c>
-      <c r="D4" s="555" t="s">
+      <c r="D4" s="556" t="s">
         <v>767</v>
       </c>
-      <c r="E4" s="554"/>
-      <c r="F4" s="554"/>
-      <c r="G4" s="554"/>
-      <c r="H4" s="556"/>
-      <c r="I4" s="554" t="s">
+      <c r="E4" s="557"/>
+      <c r="F4" s="557"/>
+      <c r="G4" s="557"/>
+      <c r="H4" s="558"/>
+      <c r="I4" s="557" t="s">
         <v>768</v>
       </c>
-      <c r="J4" s="554"/>
-      <c r="K4" s="554"/>
-      <c r="L4" s="554"/>
-      <c r="M4" s="556"/>
-      <c r="N4" s="554" t="s">
+      <c r="J4" s="557"/>
+      <c r="K4" s="557"/>
+      <c r="L4" s="557"/>
+      <c r="M4" s="558"/>
+      <c r="N4" s="557" t="s">
         <v>769</v>
       </c>
-      <c r="O4" s="554"/>
-      <c r="P4" s="554"/>
-      <c r="Q4" s="554"/>
-      <c r="R4" s="556"/>
-      <c r="S4" s="554" t="s">
+      <c r="O4" s="557"/>
+      <c r="P4" s="557"/>
+      <c r="Q4" s="557"/>
+      <c r="R4" s="558"/>
+      <c r="S4" s="557" t="s">
         <v>770</v>
       </c>
-      <c r="T4" s="554"/>
-      <c r="U4" s="554"/>
-      <c r="V4" s="554"/>
-      <c r="W4" s="556"/>
-      <c r="X4" s="554" t="s">
+      <c r="T4" s="557"/>
+      <c r="U4" s="557"/>
+      <c r="V4" s="557"/>
+      <c r="W4" s="558"/>
+      <c r="X4" s="557" t="s">
         <v>771</v>
       </c>
-      <c r="Y4" s="554"/>
-      <c r="Z4" s="554"/>
-      <c r="AA4" s="554"/>
-      <c r="AB4" s="556"/>
-      <c r="AC4" s="554" t="s">
+      <c r="Y4" s="557"/>
+      <c r="Z4" s="557"/>
+      <c r="AA4" s="557"/>
+      <c r="AB4" s="558"/>
+      <c r="AC4" s="557" t="s">
         <v>772</v>
       </c>
-      <c r="AD4" s="554"/>
-      <c r="AE4" s="554"/>
-      <c r="AF4" s="554"/>
-      <c r="AG4" s="556"/>
-      <c r="AH4" s="554" t="s">
+      <c r="AD4" s="557"/>
+      <c r="AE4" s="557"/>
+      <c r="AF4" s="557"/>
+      <c r="AG4" s="558"/>
+      <c r="AH4" s="557" t="s">
         <v>773</v>
       </c>
-      <c r="AI4" s="554"/>
-      <c r="AJ4" s="554"/>
-      <c r="AK4" s="554"/>
-      <c r="AL4" s="556"/>
-      <c r="AM4" s="554" t="s">
+      <c r="AI4" s="557"/>
+      <c r="AJ4" s="557"/>
+      <c r="AK4" s="557"/>
+      <c r="AL4" s="558"/>
+      <c r="AM4" s="557" t="s">
         <v>774</v>
       </c>
-      <c r="AN4" s="554"/>
-      <c r="AO4" s="554"/>
-      <c r="AP4" s="554"/>
-      <c r="AQ4" s="556"/>
-      <c r="AR4" s="554" t="s">
+      <c r="AN4" s="557"/>
+      <c r="AO4" s="557"/>
+      <c r="AP4" s="557"/>
+      <c r="AQ4" s="558"/>
+      <c r="AR4" s="557" t="s">
         <v>775</v>
       </c>
-      <c r="AS4" s="554"/>
-      <c r="AT4" s="554"/>
-      <c r="AU4" s="554"/>
-      <c r="AV4" s="556"/>
-      <c r="AW4" s="554" t="s">
+      <c r="AS4" s="557"/>
+      <c r="AT4" s="557"/>
+      <c r="AU4" s="557"/>
+      <c r="AV4" s="558"/>
+      <c r="AW4" s="557" t="s">
         <v>776</v>
       </c>
-      <c r="AX4" s="554"/>
-      <c r="AY4" s="554"/>
-      <c r="AZ4" s="554"/>
-      <c r="BA4" s="554"/>
-      <c r="BB4" s="555" t="s">
+      <c r="AX4" s="557"/>
+      <c r="AY4" s="557"/>
+      <c r="AZ4" s="557"/>
+      <c r="BA4" s="557"/>
+      <c r="BB4" s="556" t="s">
         <v>777</v>
       </c>
-      <c r="BC4" s="554"/>
-      <c r="BD4" s="554"/>
-      <c r="BE4" s="554"/>
-      <c r="BF4" s="556"/>
-      <c r="BG4" s="554" t="s">
+      <c r="BC4" s="557"/>
+      <c r="BD4" s="557"/>
+      <c r="BE4" s="557"/>
+      <c r="BF4" s="558"/>
+      <c r="BG4" s="557" t="s">
         <v>778</v>
       </c>
-      <c r="BH4" s="554"/>
-      <c r="BI4" s="554"/>
-      <c r="BJ4" s="554"/>
-      <c r="BK4" s="554"/>
-      <c r="BL4" s="555" t="s">
+      <c r="BH4" s="557"/>
+      <c r="BI4" s="557"/>
+      <c r="BJ4" s="557"/>
+      <c r="BK4" s="557"/>
+      <c r="BL4" s="556" t="s">
         <v>779</v>
       </c>
-      <c r="BM4" s="554"/>
-      <c r="BN4" s="554"/>
-      <c r="BO4" s="554"/>
-      <c r="BP4" s="554"/>
-      <c r="BQ4" s="555" t="s">
+      <c r="BM4" s="557"/>
+      <c r="BN4" s="557"/>
+      <c r="BO4" s="557"/>
+      <c r="BP4" s="557"/>
+      <c r="BQ4" s="556" t="s">
         <v>780</v>
       </c>
-      <c r="BR4" s="554"/>
-      <c r="BS4" s="554"/>
-      <c r="BT4" s="554"/>
-      <c r="BU4" s="556"/>
+      <c r="BR4" s="557"/>
+      <c r="BS4" s="557"/>
+      <c r="BT4" s="557"/>
+      <c r="BU4" s="558"/>
       <c r="BV4" s="357" t="s">
         <v>781</v>
       </c>
-      <c r="BW4" s="557" t="s">
+      <c r="BW4" s="559" t="s">
         <v>782</v>
       </c>
-      <c r="BX4" s="558"/>
-      <c r="BY4" s="558"/>
-      <c r="BZ4" s="558"/>
-      <c r="CA4" s="559"/>
-      <c r="CB4" s="557" t="s">
+      <c r="BX4" s="560"/>
+      <c r="BY4" s="560"/>
+      <c r="BZ4" s="560"/>
+      <c r="CA4" s="561"/>
+      <c r="CB4" s="559" t="s">
         <v>783</v>
       </c>
-      <c r="CC4" s="558"/>
-      <c r="CD4" s="558"/>
-      <c r="CE4" s="558"/>
-      <c r="CF4" s="559"/>
-      <c r="CG4" s="557" t="s">
+      <c r="CC4" s="560"/>
+      <c r="CD4" s="560"/>
+      <c r="CE4" s="560"/>
+      <c r="CF4" s="561"/>
+      <c r="CG4" s="559" t="s">
         <v>784</v>
       </c>
-      <c r="CH4" s="558"/>
-      <c r="CI4" s="558"/>
-      <c r="CJ4" s="558"/>
-      <c r="CK4" s="559"/>
+      <c r="CH4" s="560"/>
+      <c r="CI4" s="560"/>
+      <c r="CJ4" s="560"/>
+      <c r="CK4" s="561"/>
     </row>
     <row r="5" spans="1:89" x14ac:dyDescent="0.2">
       <c r="A5" s="359"/>
@@ -62587,11 +62622,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="BL4:BP4"/>
-    <mergeCell ref="BQ4:BU4"/>
-    <mergeCell ref="BW4:CA4"/>
-    <mergeCell ref="CB4:CF4"/>
-    <mergeCell ref="CG4:CK4"/>
     <mergeCell ref="BG4:BK4"/>
     <mergeCell ref="D4:H4"/>
     <mergeCell ref="I4:M4"/>
@@ -62604,6 +62634,11 @@
     <mergeCell ref="AR4:AV4"/>
     <mergeCell ref="AW4:BA4"/>
     <mergeCell ref="BB4:BF4"/>
+    <mergeCell ref="BL4:BP4"/>
+    <mergeCell ref="BQ4:BU4"/>
+    <mergeCell ref="BW4:CA4"/>
+    <mergeCell ref="CB4:CF4"/>
+    <mergeCell ref="CG4:CK4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
District Heat Cost raised 50% in Detached
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_RSD.xlsx
+++ b/SubRES_TMPL/SubRes_RSD.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E96BE67-93A6-4C79-8AA9-95F478771D71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F50CD5-30C8-4D63-B382-6BAACB8262D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{34F9D92C-266F-476D-89E0-63153305AC39}"/>
   </bookViews>
@@ -817,6 +817,30 @@
           </rPr>
           <t xml:space="preserve">
 Element Energy - Hybrid Heat Pump Study Final Report</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="V125" authorId="0" shapeId="0" xr:uid="{3114F588-A8D1-4057-B548-C533DB1E88B9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Add 50% Cost to Detached</t>
         </r>
       </text>
     </comment>
@@ -12270,7 +12294,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="39">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -12482,18 +12506,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor theme="6" tint="0.79998168889431442"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -13532,7 +13544,7 @@
     <xf numFmtId="0" fontId="39" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="54" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="562">
+  <cellXfs count="560">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -14535,8 +14547,6 @@
     <xf numFmtId="0" fontId="40" fillId="21" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="40" fillId="21" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="16" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="37" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="38" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -14582,15 +14592,6 @@
     <xf numFmtId="0" fontId="53" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="23" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -14598,6 +14599,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -14609,17 +14619,26 @@
     <xf numFmtId="0" fontId="16" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="69" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="23" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -14630,19 +14649,10 @@
     <xf numFmtId="0" fontId="16" fillId="23" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="69" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="60" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="60" fillId="31" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="60" fillId="31" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -15773,10 +15783,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -16260,14 +16266,14 @@
       <c r="F16" s="211"/>
     </row>
     <row r="17" spans="1:14" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="523" t="s">
+      <c r="A17" s="521" t="s">
         <v>434</v>
       </c>
-      <c r="B17" s="523"/>
-      <c r="C17" s="523"/>
-      <c r="D17" s="523"/>
-      <c r="E17" s="523"/>
-      <c r="F17" s="523"/>
+      <c r="B17" s="521"/>
+      <c r="C17" s="521"/>
+      <c r="D17" s="521"/>
+      <c r="E17" s="521"/>
+      <c r="F17" s="521"/>
       <c r="G17" s="213"/>
       <c r="H17" s="213"/>
       <c r="I17" s="214"/>
@@ -16305,13 +16311,13 @@
       <c r="A20" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="524" t="s">
+      <c r="B20" s="522" t="s">
         <v>436</v>
       </c>
-      <c r="C20" s="524"/>
-      <c r="D20" s="524"/>
-      <c r="E20" s="524"/>
-      <c r="F20" s="524"/>
+      <c r="C20" s="522"/>
+      <c r="D20" s="522"/>
+      <c r="E20" s="522"/>
+      <c r="F20" s="522"/>
       <c r="G20" s="218"/>
       <c r="H20" s="218"/>
       <c r="I20" s="219"/>
@@ -16325,13 +16331,13 @@
       <c r="A21" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="525" t="s">
+      <c r="B21" s="523" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="525"/>
-      <c r="D21" s="525"/>
-      <c r="E21" s="525"/>
-      <c r="F21" s="525"/>
+      <c r="C21" s="523"/>
+      <c r="D21" s="523"/>
+      <c r="E21" s="523"/>
+      <c r="F21" s="523"/>
       <c r="G21" s="218"/>
       <c r="H21" s="218"/>
       <c r="I21" s="219"/>
@@ -16345,13 +16351,13 @@
       <c r="A22" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="525" t="s">
+      <c r="B22" s="523" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="525"/>
-      <c r="D22" s="525"/>
-      <c r="E22" s="525"/>
-      <c r="F22" s="525"/>
+      <c r="C22" s="523"/>
+      <c r="D22" s="523"/>
+      <c r="E22" s="523"/>
+      <c r="F22" s="523"/>
     </row>
     <row r="23" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
@@ -16380,22 +16386,22 @@
       <c r="H24" s="3"/>
     </row>
     <row r="25" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="526"/>
-      <c r="B25" s="526"/>
-      <c r="C25" s="526"/>
-      <c r="D25" s="526"/>
-      <c r="E25" s="526"/>
-      <c r="F25" s="526"/>
+      <c r="A25" s="524"/>
+      <c r="B25" s="524"/>
+      <c r="C25" s="524"/>
+      <c r="D25" s="524"/>
+      <c r="E25" s="524"/>
+      <c r="F25" s="524"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
     </row>
     <row r="26" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="522"/>
-      <c r="B26" s="522"/>
-      <c r="C26" s="522"/>
-      <c r="D26" s="522"/>
-      <c r="E26" s="522"/>
-      <c r="F26" s="522"/>
+      <c r="A26" s="520"/>
+      <c r="B26" s="520"/>
+      <c r="C26" s="520"/>
+      <c r="D26" s="520"/>
+      <c r="E26" s="520"/>
+      <c r="F26" s="520"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="211"/>
@@ -16582,16 +16588,16 @@
   <sheetData>
     <row r="1" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:20" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="527" t="s">
+      <c r="B2" s="525" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="528"/>
-      <c r="D2" s="528"/>
-      <c r="E2" s="529"/>
-      <c r="G2" s="527" t="s">
+      <c r="C2" s="526"/>
+      <c r="D2" s="526"/>
+      <c r="E2" s="527"/>
+      <c r="G2" s="525" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="529"/>
+      <c r="H2" s="527"/>
       <c r="I2" s="222"/>
       <c r="J2" s="222"/>
       <c r="K2" s="223"/>
@@ -16933,16 +16939,16 @@
     </row>
     <row r="19" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="2:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="530" t="s">
+      <c r="B20" s="528" t="s">
         <v>70</v>
       </c>
-      <c r="C20" s="531"/>
-      <c r="D20" s="531"/>
-      <c r="E20" s="532"/>
-      <c r="G20" s="527" t="s">
+      <c r="C20" s="529"/>
+      <c r="D20" s="529"/>
+      <c r="E20" s="530"/>
+      <c r="G20" s="525" t="s">
         <v>14</v>
       </c>
-      <c r="H20" s="529"/>
+      <c r="H20" s="527"/>
     </row>
     <row r="21" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="250" t="s">
@@ -17186,16 +17192,16 @@
     </row>
     <row r="37" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="38" spans="2:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="527" t="s">
+      <c r="B38" s="525" t="s">
         <v>78</v>
       </c>
-      <c r="C38" s="528"/>
-      <c r="D38" s="528"/>
-      <c r="E38" s="529"/>
-      <c r="G38" s="533" t="s">
+      <c r="C38" s="526"/>
+      <c r="D38" s="526"/>
+      <c r="E38" s="527"/>
+      <c r="G38" s="531" t="s">
         <v>72</v>
       </c>
-      <c r="H38" s="534"/>
+      <c r="H38" s="532"/>
     </row>
     <row r="39" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B39" s="271" t="s">
@@ -17364,13 +17370,13 @@
       <c r="M3" s="5" t="s">
         <v>390</v>
       </c>
-      <c r="S3" s="535" t="s">
+      <c r="S3" s="533" t="s">
         <v>680</v>
       </c>
-      <c r="T3" s="535"/>
-      <c r="U3" s="535"/>
-      <c r="V3" s="535"/>
-      <c r="W3" s="535"/>
+      <c r="T3" s="533"/>
+      <c r="U3" s="533"/>
+      <c r="V3" s="533"/>
+      <c r="W3" s="533"/>
     </row>
     <row r="4" spans="3:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C4" s="62" t="s">
@@ -17564,10 +17570,10 @@
         <v>5.6296955912135845E-4</v>
       </c>
       <c r="J9" s="103"/>
-      <c r="M9" s="536" t="s">
+      <c r="M9" s="534" t="s">
         <v>110</v>
       </c>
-      <c r="N9" s="536" t="s">
+      <c r="N9" s="534" t="s">
         <v>110</v>
       </c>
       <c r="S9" s="300" t="s">
@@ -25069,8 +25075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{104F8057-C735-4662-BAA6-EEDCF7B57273}">
   <dimension ref="A2:AQ166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AD13" sqref="AD13"/>
+    <sheetView tabSelected="1" topLeftCell="H93" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="X122" sqref="X122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -25234,34 +25240,34 @@
       <c r="G4" s="62" t="s">
         <v>317</v>
       </c>
-      <c r="H4" s="543" t="s">
+      <c r="H4" s="541" t="s">
         <v>720</v>
       </c>
-      <c r="I4" s="544"/>
-      <c r="J4" s="544"/>
-      <c r="K4" s="545"/>
-      <c r="L4" s="543" t="s">
+      <c r="I4" s="542"/>
+      <c r="J4" s="542"/>
+      <c r="K4" s="543"/>
+      <c r="L4" s="541" t="s">
         <v>319</v>
       </c>
-      <c r="M4" s="544"/>
-      <c r="N4" s="544"/>
-      <c r="O4" s="545"/>
-      <c r="P4" s="543" t="s">
+      <c r="M4" s="542"/>
+      <c r="N4" s="542"/>
+      <c r="O4" s="543"/>
+      <c r="P4" s="541" t="s">
         <v>320</v>
       </c>
-      <c r="Q4" s="544"/>
-      <c r="R4" s="544"/>
-      <c r="S4" s="545"/>
-      <c r="T4" s="543" t="s">
+      <c r="Q4" s="542"/>
+      <c r="R4" s="542"/>
+      <c r="S4" s="543"/>
+      <c r="T4" s="541" t="s">
         <v>321</v>
       </c>
-      <c r="U4" s="545"/>
-      <c r="V4" s="537" t="s">
+      <c r="U4" s="543"/>
+      <c r="V4" s="544" t="s">
         <v>322</v>
       </c>
-      <c r="W4" s="538"/>
-      <c r="X4" s="538"/>
-      <c r="Y4" s="539"/>
+      <c r="W4" s="545"/>
+      <c r="X4" s="545"/>
+      <c r="Y4" s="546"/>
       <c r="Z4" s="106"/>
       <c r="AA4" s="106"/>
       <c r="AB4" s="114" t="s">
@@ -25360,34 +25366,34 @@
       <c r="E6" s="84"/>
       <c r="F6" s="84"/>
       <c r="G6" s="85"/>
-      <c r="H6" s="540" t="s">
+      <c r="H6" s="535" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="541"/>
-      <c r="J6" s="541"/>
-      <c r="K6" s="542"/>
-      <c r="L6" s="541" t="s">
+      <c r="I6" s="536"/>
+      <c r="J6" s="536"/>
+      <c r="K6" s="537"/>
+      <c r="L6" s="536" t="s">
         <v>45</v>
       </c>
-      <c r="M6" s="541"/>
-      <c r="N6" s="541"/>
-      <c r="O6" s="542"/>
-      <c r="P6" s="540" t="s">
+      <c r="M6" s="536"/>
+      <c r="N6" s="536"/>
+      <c r="O6" s="537"/>
+      <c r="P6" s="535" t="s">
         <v>45</v>
       </c>
-      <c r="Q6" s="541"/>
-      <c r="R6" s="541"/>
-      <c r="S6" s="542"/>
-      <c r="T6" s="540" t="s">
+      <c r="Q6" s="536"/>
+      <c r="R6" s="536"/>
+      <c r="S6" s="537"/>
+      <c r="T6" s="535" t="s">
         <v>302</v>
       </c>
-      <c r="U6" s="542"/>
-      <c r="V6" s="540" t="s">
+      <c r="U6" s="537"/>
+      <c r="V6" s="535" t="s">
         <v>968</v>
       </c>
-      <c r="W6" s="541"/>
-      <c r="X6" s="541"/>
-      <c r="Y6" s="542"/>
+      <c r="W6" s="536"/>
+      <c r="X6" s="536"/>
+      <c r="Y6" s="537"/>
       <c r="Z6" s="107" t="s">
         <v>980</v>
       </c>
@@ -25684,7 +25690,7 @@
         <v>2.79</v>
       </c>
       <c r="W9" s="456">
-        <f t="shared" ref="W9:Y11" si="7">2.79</f>
+        <f t="shared" ref="W9:Y9" si="7">2.79</f>
         <v>2.79</v>
       </c>
       <c r="X9" s="456">
@@ -28299,34 +28305,34 @@
       <c r="G42" s="62" t="s">
         <v>317</v>
       </c>
-      <c r="H42" s="543" t="s">
+      <c r="H42" s="541" t="s">
         <v>318</v>
       </c>
-      <c r="I42" s="544"/>
-      <c r="J42" s="544"/>
-      <c r="K42" s="545"/>
-      <c r="L42" s="543" t="s">
+      <c r="I42" s="542"/>
+      <c r="J42" s="542"/>
+      <c r="K42" s="543"/>
+      <c r="L42" s="541" t="s">
         <v>319</v>
       </c>
-      <c r="M42" s="544"/>
-      <c r="N42" s="544"/>
-      <c r="O42" s="545"/>
-      <c r="P42" s="543" t="s">
+      <c r="M42" s="542"/>
+      <c r="N42" s="542"/>
+      <c r="O42" s="543"/>
+      <c r="P42" s="541" t="s">
         <v>320</v>
       </c>
-      <c r="Q42" s="544"/>
-      <c r="R42" s="544"/>
-      <c r="S42" s="545"/>
-      <c r="T42" s="543" t="s">
+      <c r="Q42" s="542"/>
+      <c r="R42" s="542"/>
+      <c r="S42" s="543"/>
+      <c r="T42" s="541" t="s">
         <v>321</v>
       </c>
-      <c r="U42" s="545"/>
-      <c r="V42" s="537" t="s">
+      <c r="U42" s="543"/>
+      <c r="V42" s="544" t="s">
         <v>322</v>
       </c>
-      <c r="W42" s="538"/>
-      <c r="X42" s="538"/>
-      <c r="Y42" s="539"/>
+      <c r="W42" s="545"/>
+      <c r="X42" s="545"/>
+      <c r="Y42" s="546"/>
       <c r="Z42" s="106"/>
       <c r="AA42" s="106"/>
       <c r="AB42" s="114" t="s">
@@ -28425,34 +28431,34 @@
       <c r="E44" s="84"/>
       <c r="F44" s="84"/>
       <c r="G44" s="85"/>
-      <c r="H44" s="540" t="s">
+      <c r="H44" s="535" t="s">
         <v>45</v>
       </c>
-      <c r="I44" s="541"/>
-      <c r="J44" s="541"/>
-      <c r="K44" s="542"/>
-      <c r="L44" s="541" t="s">
+      <c r="I44" s="536"/>
+      <c r="J44" s="536"/>
+      <c r="K44" s="537"/>
+      <c r="L44" s="536" t="s">
         <v>45</v>
       </c>
-      <c r="M44" s="541"/>
-      <c r="N44" s="541"/>
-      <c r="O44" s="542"/>
-      <c r="P44" s="540" t="s">
+      <c r="M44" s="536"/>
+      <c r="N44" s="536"/>
+      <c r="O44" s="537"/>
+      <c r="P44" s="535" t="s">
         <v>45</v>
       </c>
-      <c r="Q44" s="541"/>
-      <c r="R44" s="541"/>
-      <c r="S44" s="542"/>
-      <c r="T44" s="546" t="s">
+      <c r="Q44" s="536"/>
+      <c r="R44" s="536"/>
+      <c r="S44" s="537"/>
+      <c r="T44" s="538" t="s">
         <v>302</v>
       </c>
-      <c r="U44" s="547"/>
-      <c r="V44" s="546" t="s">
+      <c r="U44" s="539"/>
+      <c r="V44" s="538" t="s">
         <v>968</v>
       </c>
-      <c r="W44" s="548"/>
-      <c r="X44" s="548"/>
-      <c r="Y44" s="547"/>
+      <c r="W44" s="540"/>
+      <c r="X44" s="540"/>
+      <c r="Y44" s="539"/>
       <c r="Z44" s="450" t="s">
         <v>980</v>
       </c>
@@ -32161,34 +32167,34 @@
       <c r="G90" s="62" t="s">
         <v>317</v>
       </c>
-      <c r="H90" s="543" t="s">
+      <c r="H90" s="541" t="s">
         <v>318</v>
       </c>
-      <c r="I90" s="544"/>
-      <c r="J90" s="544"/>
-      <c r="K90" s="545"/>
-      <c r="L90" s="543" t="s">
+      <c r="I90" s="542"/>
+      <c r="J90" s="542"/>
+      <c r="K90" s="543"/>
+      <c r="L90" s="541" t="s">
         <v>319</v>
       </c>
-      <c r="M90" s="544"/>
-      <c r="N90" s="544"/>
-      <c r="O90" s="545"/>
-      <c r="P90" s="543" t="s">
+      <c r="M90" s="542"/>
+      <c r="N90" s="542"/>
+      <c r="O90" s="543"/>
+      <c r="P90" s="541" t="s">
         <v>320</v>
       </c>
-      <c r="Q90" s="544"/>
-      <c r="R90" s="544"/>
-      <c r="S90" s="545"/>
-      <c r="T90" s="543" t="s">
+      <c r="Q90" s="542"/>
+      <c r="R90" s="542"/>
+      <c r="S90" s="543"/>
+      <c r="T90" s="541" t="s">
         <v>321</v>
       </c>
-      <c r="U90" s="545"/>
-      <c r="V90" s="537" t="s">
+      <c r="U90" s="543"/>
+      <c r="V90" s="544" t="s">
         <v>322</v>
       </c>
-      <c r="W90" s="538"/>
-      <c r="X90" s="538"/>
-      <c r="Y90" s="539"/>
+      <c r="W90" s="545"/>
+      <c r="X90" s="545"/>
+      <c r="Y90" s="546"/>
       <c r="Z90" s="106"/>
       <c r="AA90" s="106"/>
       <c r="AB90" s="114" t="s">
@@ -32287,34 +32293,34 @@
       <c r="E92" s="84"/>
       <c r="F92" s="84"/>
       <c r="G92" s="85"/>
-      <c r="H92" s="540" t="s">
+      <c r="H92" s="535" t="s">
         <v>45</v>
       </c>
-      <c r="I92" s="541"/>
-      <c r="J92" s="541"/>
-      <c r="K92" s="542"/>
-      <c r="L92" s="541" t="s">
+      <c r="I92" s="536"/>
+      <c r="J92" s="536"/>
+      <c r="K92" s="537"/>
+      <c r="L92" s="536" t="s">
         <v>45</v>
       </c>
-      <c r="M92" s="541"/>
-      <c r="N92" s="541"/>
-      <c r="O92" s="542"/>
-      <c r="P92" s="540" t="s">
+      <c r="M92" s="536"/>
+      <c r="N92" s="536"/>
+      <c r="O92" s="537"/>
+      <c r="P92" s="535" t="s">
         <v>45</v>
       </c>
-      <c r="Q92" s="541"/>
-      <c r="R92" s="541"/>
-      <c r="S92" s="542"/>
-      <c r="T92" s="546" t="s">
+      <c r="Q92" s="536"/>
+      <c r="R92" s="536"/>
+      <c r="S92" s="537"/>
+      <c r="T92" s="538" t="s">
         <v>302</v>
       </c>
-      <c r="U92" s="547"/>
-      <c r="V92" s="546" t="s">
+      <c r="U92" s="539"/>
+      <c r="V92" s="538" t="s">
         <v>968</v>
       </c>
-      <c r="W92" s="548"/>
-      <c r="X92" s="548"/>
-      <c r="Y92" s="547"/>
+      <c r="W92" s="540"/>
+      <c r="X92" s="540"/>
+      <c r="Y92" s="539"/>
       <c r="Z92" s="450" t="s">
         <v>980</v>
       </c>
@@ -35024,8 +35030,8 @@
         <v>1.1983680000000001</v>
       </c>
       <c r="AG120" s="134"/>
-      <c r="AH120" s="520">
-        <v>2100</v>
+      <c r="AH120" s="111">
+        <v>2019</v>
       </c>
       <c r="AI120" s="134">
         <v>38</v>
@@ -35137,8 +35143,8 @@
         <v>1.1983680000000001</v>
       </c>
       <c r="AG121" s="113"/>
-      <c r="AH121" s="521">
-        <v>2100</v>
+      <c r="AH121" s="112">
+        <v>2019</v>
       </c>
       <c r="AI121" s="113">
         <v>38</v>
@@ -35440,20 +35446,20 @@
       </c>
       <c r="U125" s="94"/>
       <c r="V125" s="65">
-        <f>(JRC_Data!BB62/1000)*($U$154/$U$148)</f>
-        <v>3.1055555555555552</v>
+        <f>(JRC_Data!BB62/1000)*($U$154/$U$148)*1.5</f>
+        <v>4.6583333333333332</v>
       </c>
       <c r="W125" s="65">
-        <f>(JRC_Data!BC62/1000)*($U$154/$U$148)</f>
-        <v>3.1055555555555552</v>
+        <f>(JRC_Data!BC62/1000)*($U$154/$U$148)*1.5</f>
+        <v>4.6583333333333332</v>
       </c>
       <c r="X125" s="65">
-        <f>(JRC_Data!BD62/1000)*($U$154/$U$148)</f>
-        <v>3.1055555555555552</v>
+        <f>(JRC_Data!BD62/1000)*($U$154/$U$148)*1.5</f>
+        <v>4.6583333333333332</v>
       </c>
       <c r="Y125" s="65">
-        <f>(JRC_Data!BE62/1000)*($U$154/$U$148)</f>
-        <v>3.1055555555555552</v>
+        <f>(JRC_Data!BE62/1000)*($U$154/$U$148)*1.5</f>
+        <v>4.6583333333333332</v>
       </c>
       <c r="Z125" s="131">
         <f>JRC_Data!BL62/1000</f>
@@ -35469,7 +35475,7 @@
         <v>1.1983680000000001</v>
       </c>
       <c r="AG125" s="134"/>
-      <c r="AH125" s="134">
+      <c r="AH125" s="111">
         <v>2019</v>
       </c>
       <c r="AI125" s="134">
@@ -35524,16 +35530,20 @@
       </c>
       <c r="U126" s="97"/>
       <c r="V126" s="329">
-        <v>2.7222222222222219</v>
+        <f>(JRC_Data!BB62/1000)*($U$154/$U$148)*1.5</f>
+        <v>4.6583333333333332</v>
       </c>
       <c r="W126" s="329">
-        <v>2.7222222222222219</v>
+        <f>(JRC_Data!BC62/1000)*($U$154/$U$148)*1.5</f>
+        <v>4.6583333333333332</v>
       </c>
       <c r="X126" s="329">
-        <v>2.7222222222222219</v>
+        <f>(JRC_Data!BD62/1000)*($U$154/$U$148)*1.5</f>
+        <v>4.6583333333333332</v>
       </c>
       <c r="Y126" s="329">
-        <v>2.7222222222222219</v>
+        <f>(JRC_Data!BE62/1000)*($U$154/$U$148)*1.5</f>
+        <v>4.6583333333333332</v>
       </c>
       <c r="Z126" s="110">
         <f>JRC_Data!BL62/1000</f>
@@ -35549,7 +35559,7 @@
         <v>1.1983680000000001</v>
       </c>
       <c r="AG126" s="113"/>
-      <c r="AH126" s="113">
+      <c r="AH126" s="112">
         <v>2019</v>
       </c>
       <c r="AI126" s="113">
@@ -36181,26 +36191,6 @@
     <row r="166" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="H92:K92"/>
-    <mergeCell ref="L92:O92"/>
-    <mergeCell ref="P92:S92"/>
-    <mergeCell ref="T92:U92"/>
-    <mergeCell ref="V92:Y92"/>
-    <mergeCell ref="H90:K90"/>
-    <mergeCell ref="L90:O90"/>
-    <mergeCell ref="P90:S90"/>
-    <mergeCell ref="T90:U90"/>
-    <mergeCell ref="V90:Y90"/>
-    <mergeCell ref="H44:K44"/>
-    <mergeCell ref="L44:O44"/>
-    <mergeCell ref="P44:S44"/>
-    <mergeCell ref="T44:U44"/>
-    <mergeCell ref="V44:Y44"/>
-    <mergeCell ref="H42:K42"/>
-    <mergeCell ref="L42:O42"/>
-    <mergeCell ref="P42:S42"/>
-    <mergeCell ref="T42:U42"/>
-    <mergeCell ref="V42:Y42"/>
     <mergeCell ref="V4:Y4"/>
     <mergeCell ref="V6:Y6"/>
     <mergeCell ref="H4:K4"/>
@@ -36211,6 +36201,26 @@
     <mergeCell ref="P6:S6"/>
     <mergeCell ref="L6:O6"/>
     <mergeCell ref="H6:K6"/>
+    <mergeCell ref="H42:K42"/>
+    <mergeCell ref="L42:O42"/>
+    <mergeCell ref="P42:S42"/>
+    <mergeCell ref="T42:U42"/>
+    <mergeCell ref="V42:Y42"/>
+    <mergeCell ref="H44:K44"/>
+    <mergeCell ref="L44:O44"/>
+    <mergeCell ref="P44:S44"/>
+    <mergeCell ref="T44:U44"/>
+    <mergeCell ref="V44:Y44"/>
+    <mergeCell ref="H90:K90"/>
+    <mergeCell ref="L90:O90"/>
+    <mergeCell ref="P90:S90"/>
+    <mergeCell ref="T90:U90"/>
+    <mergeCell ref="V90:Y90"/>
+    <mergeCell ref="H92:K92"/>
+    <mergeCell ref="L92:O92"/>
+    <mergeCell ref="P92:S92"/>
+    <mergeCell ref="T92:U92"/>
+    <mergeCell ref="V92:Y92"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
@@ -36355,12 +36365,12 @@
       <c r="I5" s="173"/>
       <c r="J5" s="173"/>
       <c r="K5" s="173"/>
-      <c r="L5" s="537" t="s">
+      <c r="L5" s="544" t="s">
         <v>322</v>
       </c>
-      <c r="M5" s="538"/>
-      <c r="N5" s="538"/>
-      <c r="O5" s="539"/>
+      <c r="M5" s="545"/>
+      <c r="N5" s="545"/>
+      <c r="O5" s="546"/>
       <c r="P5" s="106"/>
       <c r="Q5" s="106" t="s">
         <v>323</v>
@@ -36391,12 +36401,12 @@
       <c r="I6" s="83"/>
       <c r="J6" s="83"/>
       <c r="K6" s="83"/>
-      <c r="L6" s="546" t="s">
+      <c r="L6" s="538" t="s">
         <v>968</v>
       </c>
-      <c r="M6" s="548"/>
-      <c r="N6" s="548"/>
-      <c r="O6" s="547"/>
+      <c r="M6" s="540"/>
+      <c r="N6" s="540"/>
+      <c r="O6" s="539"/>
       <c r="P6" s="450" t="s">
         <v>980</v>
       </c>
@@ -37022,10 +37032,10 @@
       <c r="C18" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="R18" s="549" t="s">
+      <c r="R18" s="547" t="s">
         <v>662</v>
       </c>
-      <c r="S18" s="549"/>
+      <c r="S18" s="547"/>
       <c r="U18" s="5" t="s">
         <v>861</v>
       </c>
@@ -37058,8 +37068,8 @@
       <c r="J19" s="195" t="s">
         <v>301</v>
       </c>
-      <c r="R19" s="549"/>
-      <c r="S19" s="549"/>
+      <c r="R19" s="547"/>
+      <c r="S19" s="547"/>
       <c r="V19" s="5" t="s">
         <v>1023</v>
       </c>
@@ -37085,8 +37095,8 @@
       <c r="J20" s="170" t="s">
         <v>1028</v>
       </c>
-      <c r="R20" s="549"/>
-      <c r="S20" s="549"/>
+      <c r="R20" s="547"/>
+      <c r="S20" s="547"/>
       <c r="V20" s="5" t="s">
         <v>1024</v>
       </c>
@@ -37113,8 +37123,8 @@
       <c r="J21" s="170" t="s">
         <v>1028</v>
       </c>
-      <c r="R21" s="549"/>
-      <c r="S21" s="549"/>
+      <c r="R21" s="547"/>
+      <c r="S21" s="547"/>
     </row>
     <row r="22" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C22" s="168" t="s">
@@ -37138,8 +37148,8 @@
       <c r="J22" s="170" t="s">
         <v>1028</v>
       </c>
-      <c r="R22" s="549"/>
-      <c r="S22" s="549"/>
+      <c r="R22" s="547"/>
+      <c r="S22" s="547"/>
     </row>
     <row r="23" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C23" s="168" t="s">
@@ -37314,23 +37324,23 @@
       <c r="K33" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="L33" s="537" t="s">
+      <c r="L33" s="544" t="s">
         <v>322</v>
       </c>
-      <c r="M33" s="538"/>
-      <c r="N33" s="538"/>
-      <c r="O33" s="539"/>
+      <c r="M33" s="545"/>
+      <c r="N33" s="545"/>
+      <c r="O33" s="546"/>
     </row>
     <row r="34" spans="8:15" x14ac:dyDescent="0.2">
       <c r="H34" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="L34" s="546" t="s">
+      <c r="L34" s="538" t="s">
         <v>327</v>
       </c>
-      <c r="M34" s="548"/>
-      <c r="N34" s="548"/>
-      <c r="O34" s="547"/>
+      <c r="M34" s="540"/>
+      <c r="N34" s="540"/>
+      <c r="O34" s="539"/>
     </row>
     <row r="35" spans="8:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H35" s="5" t="s">
@@ -37672,16 +37682,16 @@
       <c r="G4" s="173" t="s">
         <v>321</v>
       </c>
-      <c r="H4" s="543" t="s">
+      <c r="H4" s="541" t="s">
         <v>110</v>
       </c>
-      <c r="I4" s="544"/>
-      <c r="J4" s="545"/>
-      <c r="K4" s="537" t="s">
+      <c r="I4" s="542"/>
+      <c r="J4" s="543"/>
+      <c r="K4" s="544" t="s">
         <v>322</v>
       </c>
-      <c r="L4" s="538"/>
-      <c r="M4" s="539"/>
+      <c r="L4" s="545"/>
+      <c r="M4" s="546"/>
       <c r="N4" s="106"/>
       <c r="O4" s="106" t="s">
         <v>323</v>
@@ -37707,16 +37717,16 @@
       <c r="G5" s="458" t="s">
         <v>302</v>
       </c>
-      <c r="H5" s="550" t="s">
+      <c r="H5" s="551" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="551"/>
-      <c r="J5" s="552"/>
-      <c r="K5" s="550" t="s">
+      <c r="I5" s="552"/>
+      <c r="J5" s="553"/>
+      <c r="K5" s="551" t="s">
         <v>757</v>
       </c>
-      <c r="L5" s="551"/>
-      <c r="M5" s="552"/>
+      <c r="L5" s="552"/>
+      <c r="M5" s="553"/>
       <c r="N5" s="459" t="s">
         <v>328</v>
       </c>
@@ -37733,23 +37743,23 @@
         <v>626</v>
       </c>
       <c r="AA5" s="281"/>
-      <c r="AB5" s="553" t="s">
+      <c r="AB5" s="548" t="s">
         <v>1013</v>
       </c>
-      <c r="AC5" s="553"/>
+      <c r="AC5" s="548"/>
       <c r="AD5" s="461"/>
-      <c r="AE5" s="554" t="s">
+      <c r="AE5" s="549" t="s">
         <v>110</v>
       </c>
-      <c r="AF5" s="554"/>
-      <c r="AG5" s="554" t="s">
+      <c r="AF5" s="549"/>
+      <c r="AG5" s="549" t="s">
         <v>1014</v>
       </c>
-      <c r="AH5" s="554"/>
-      <c r="AI5" s="555" t="s">
+      <c r="AH5" s="549"/>
+      <c r="AI5" s="550" t="s">
         <v>1015</v>
       </c>
-      <c r="AJ5" s="555"/>
+      <c r="AJ5" s="550"/>
     </row>
     <row r="6" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C6" s="505" t="str">
@@ -38487,12 +38497,12 @@
       <c r="K27" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="L27" s="537" t="s">
+      <c r="L27" s="544" t="s">
         <v>322</v>
       </c>
-      <c r="M27" s="538"/>
-      <c r="N27" s="538"/>
-      <c r="O27" s="539"/>
+      <c r="M27" s="545"/>
+      <c r="N27" s="545"/>
+      <c r="O27" s="546"/>
       <c r="T27" s="283"/>
       <c r="U27" s="283"/>
     </row>
@@ -38500,12 +38510,12 @@
       <c r="J28" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="L28" s="540" t="s">
+      <c r="L28" s="535" t="s">
         <v>327</v>
       </c>
-      <c r="M28" s="541"/>
-      <c r="N28" s="541"/>
-      <c r="O28" s="542"/>
+      <c r="M28" s="536"/>
+      <c r="N28" s="536"/>
+      <c r="O28" s="537"/>
       <c r="T28" s="283"/>
       <c r="U28" s="283"/>
     </row>
@@ -39895,16 +39905,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="L28:O28"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="K5:M5"/>
     <mergeCell ref="AB5:AC5"/>
     <mergeCell ref="AE5:AF5"/>
     <mergeCell ref="AG5:AH5"/>
     <mergeCell ref="AI5:AJ5"/>
     <mergeCell ref="L27:O27"/>
-    <mergeCell ref="L28:O28"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="K5:M5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="S7" r:id="rId1" xr:uid="{B1EDD63D-40A5-4174-9D28-8666BD314B83}"/>
@@ -48932,128 +48942,128 @@
       <c r="C4" s="356" t="s">
         <v>766</v>
       </c>
-      <c r="D4" s="556" t="s">
+      <c r="D4" s="555" t="s">
         <v>767</v>
       </c>
-      <c r="E4" s="557"/>
-      <c r="F4" s="557"/>
-      <c r="G4" s="557"/>
-      <c r="H4" s="558"/>
-      <c r="I4" s="557" t="s">
+      <c r="E4" s="554"/>
+      <c r="F4" s="554"/>
+      <c r="G4" s="554"/>
+      <c r="H4" s="556"/>
+      <c r="I4" s="554" t="s">
         <v>768</v>
       </c>
-      <c r="J4" s="557"/>
-      <c r="K4" s="557"/>
-      <c r="L4" s="557"/>
-      <c r="M4" s="558"/>
-      <c r="N4" s="557" t="s">
+      <c r="J4" s="554"/>
+      <c r="K4" s="554"/>
+      <c r="L4" s="554"/>
+      <c r="M4" s="556"/>
+      <c r="N4" s="554" t="s">
         <v>769</v>
       </c>
-      <c r="O4" s="557"/>
-      <c r="P4" s="557"/>
-      <c r="Q4" s="557"/>
-      <c r="R4" s="558"/>
-      <c r="S4" s="557" t="s">
+      <c r="O4" s="554"/>
+      <c r="P4" s="554"/>
+      <c r="Q4" s="554"/>
+      <c r="R4" s="556"/>
+      <c r="S4" s="554" t="s">
         <v>770</v>
       </c>
-      <c r="T4" s="557"/>
-      <c r="U4" s="557"/>
-      <c r="V4" s="557"/>
-      <c r="W4" s="558"/>
-      <c r="X4" s="557" t="s">
+      <c r="T4" s="554"/>
+      <c r="U4" s="554"/>
+      <c r="V4" s="554"/>
+      <c r="W4" s="556"/>
+      <c r="X4" s="554" t="s">
         <v>771</v>
       </c>
-      <c r="Y4" s="557"/>
-      <c r="Z4" s="557"/>
-      <c r="AA4" s="557"/>
-      <c r="AB4" s="558"/>
-      <c r="AC4" s="557" t="s">
+      <c r="Y4" s="554"/>
+      <c r="Z4" s="554"/>
+      <c r="AA4" s="554"/>
+      <c r="AB4" s="556"/>
+      <c r="AC4" s="554" t="s">
         <v>772</v>
       </c>
-      <c r="AD4" s="557"/>
-      <c r="AE4" s="557"/>
-      <c r="AF4" s="557"/>
-      <c r="AG4" s="558"/>
-      <c r="AH4" s="557" t="s">
+      <c r="AD4" s="554"/>
+      <c r="AE4" s="554"/>
+      <c r="AF4" s="554"/>
+      <c r="AG4" s="556"/>
+      <c r="AH4" s="554" t="s">
         <v>773</v>
       </c>
-      <c r="AI4" s="557"/>
-      <c r="AJ4" s="557"/>
-      <c r="AK4" s="557"/>
-      <c r="AL4" s="558"/>
-      <c r="AM4" s="557" t="s">
+      <c r="AI4" s="554"/>
+      <c r="AJ4" s="554"/>
+      <c r="AK4" s="554"/>
+      <c r="AL4" s="556"/>
+      <c r="AM4" s="554" t="s">
         <v>774</v>
       </c>
-      <c r="AN4" s="557"/>
-      <c r="AO4" s="557"/>
-      <c r="AP4" s="557"/>
-      <c r="AQ4" s="558"/>
-      <c r="AR4" s="557" t="s">
+      <c r="AN4" s="554"/>
+      <c r="AO4" s="554"/>
+      <c r="AP4" s="554"/>
+      <c r="AQ4" s="556"/>
+      <c r="AR4" s="554" t="s">
         <v>775</v>
       </c>
-      <c r="AS4" s="557"/>
-      <c r="AT4" s="557"/>
-      <c r="AU4" s="557"/>
-      <c r="AV4" s="558"/>
-      <c r="AW4" s="557" t="s">
+      <c r="AS4" s="554"/>
+      <c r="AT4" s="554"/>
+      <c r="AU4" s="554"/>
+      <c r="AV4" s="556"/>
+      <c r="AW4" s="554" t="s">
         <v>776</v>
       </c>
-      <c r="AX4" s="557"/>
-      <c r="AY4" s="557"/>
-      <c r="AZ4" s="557"/>
-      <c r="BA4" s="557"/>
-      <c r="BB4" s="556" t="s">
+      <c r="AX4" s="554"/>
+      <c r="AY4" s="554"/>
+      <c r="AZ4" s="554"/>
+      <c r="BA4" s="554"/>
+      <c r="BB4" s="555" t="s">
         <v>777</v>
       </c>
-      <c r="BC4" s="557"/>
-      <c r="BD4" s="557"/>
-      <c r="BE4" s="557"/>
-      <c r="BF4" s="558"/>
-      <c r="BG4" s="557" t="s">
+      <c r="BC4" s="554"/>
+      <c r="BD4" s="554"/>
+      <c r="BE4" s="554"/>
+      <c r="BF4" s="556"/>
+      <c r="BG4" s="554" t="s">
         <v>778</v>
       </c>
-      <c r="BH4" s="557"/>
-      <c r="BI4" s="557"/>
-      <c r="BJ4" s="557"/>
-      <c r="BK4" s="557"/>
-      <c r="BL4" s="556" t="s">
+      <c r="BH4" s="554"/>
+      <c r="BI4" s="554"/>
+      <c r="BJ4" s="554"/>
+      <c r="BK4" s="554"/>
+      <c r="BL4" s="555" t="s">
         <v>779</v>
       </c>
-      <c r="BM4" s="557"/>
-      <c r="BN4" s="557"/>
-      <c r="BO4" s="557"/>
-      <c r="BP4" s="557"/>
-      <c r="BQ4" s="556" t="s">
+      <c r="BM4" s="554"/>
+      <c r="BN4" s="554"/>
+      <c r="BO4" s="554"/>
+      <c r="BP4" s="554"/>
+      <c r="BQ4" s="555" t="s">
         <v>780</v>
       </c>
-      <c r="BR4" s="557"/>
-      <c r="BS4" s="557"/>
-      <c r="BT4" s="557"/>
-      <c r="BU4" s="558"/>
+      <c r="BR4" s="554"/>
+      <c r="BS4" s="554"/>
+      <c r="BT4" s="554"/>
+      <c r="BU4" s="556"/>
       <c r="BV4" s="357" t="s">
         <v>781</v>
       </c>
-      <c r="BW4" s="559" t="s">
+      <c r="BW4" s="557" t="s">
         <v>782</v>
       </c>
-      <c r="BX4" s="560"/>
-      <c r="BY4" s="560"/>
-      <c r="BZ4" s="560"/>
-      <c r="CA4" s="561"/>
-      <c r="CB4" s="559" t="s">
+      <c r="BX4" s="558"/>
+      <c r="BY4" s="558"/>
+      <c r="BZ4" s="558"/>
+      <c r="CA4" s="559"/>
+      <c r="CB4" s="557" t="s">
         <v>783</v>
       </c>
-      <c r="CC4" s="560"/>
-      <c r="CD4" s="560"/>
-      <c r="CE4" s="560"/>
-      <c r="CF4" s="561"/>
-      <c r="CG4" s="559" t="s">
+      <c r="CC4" s="558"/>
+      <c r="CD4" s="558"/>
+      <c r="CE4" s="558"/>
+      <c r="CF4" s="559"/>
+      <c r="CG4" s="557" t="s">
         <v>784</v>
       </c>
-      <c r="CH4" s="560"/>
-      <c r="CI4" s="560"/>
-      <c r="CJ4" s="560"/>
-      <c r="CK4" s="561"/>
+      <c r="CH4" s="558"/>
+      <c r="CI4" s="558"/>
+      <c r="CJ4" s="558"/>
+      <c r="CK4" s="559"/>
     </row>
     <row r="5" spans="1:89" x14ac:dyDescent="0.2">
       <c r="A5" s="359"/>
@@ -62622,6 +62632,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="BL4:BP4"/>
+    <mergeCell ref="BQ4:BU4"/>
+    <mergeCell ref="BW4:CA4"/>
+    <mergeCell ref="CB4:CF4"/>
+    <mergeCell ref="CG4:CK4"/>
     <mergeCell ref="BG4:BK4"/>
     <mergeCell ref="D4:H4"/>
     <mergeCell ref="I4:M4"/>
@@ -62634,11 +62649,6 @@
     <mergeCell ref="AR4:AV4"/>
     <mergeCell ref="AW4:BA4"/>
     <mergeCell ref="BB4:BF4"/>
-    <mergeCell ref="BL4:BP4"/>
-    <mergeCell ref="BQ4:BU4"/>
-    <mergeCell ref="BW4:CA4"/>
-    <mergeCell ref="CB4:CF4"/>
-    <mergeCell ref="CG4:CK4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
DH cost in detached doubled
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_RSD.xlsx
+++ b/SubRES_TMPL/SubRes_RSD.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F50CD5-30C8-4D63-B382-6BAACB8262D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5408B471-41AF-4A71-8D79-70B6346F3FC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{34F9D92C-266F-476D-89E0-63153305AC39}"/>
   </bookViews>
@@ -14592,6 +14592,15 @@
     <xf numFmtId="0" fontId="53" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="23" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -14599,15 +14608,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -14619,17 +14619,26 @@
     <xf numFmtId="0" fontId="16" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -14640,19 +14649,10 @@
     <xf numFmtId="0" fontId="69" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="60" fillId="31" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="60" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="31" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="60" fillId="31" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -25075,8 +25075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{104F8057-C735-4662-BAA6-EEDCF7B57273}">
   <dimension ref="A2:AQ166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H93" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="X122" sqref="X122"/>
+    <sheetView tabSelected="1" topLeftCell="H91" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="V125" sqref="V125:Y126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -25262,12 +25262,12 @@
         <v>321</v>
       </c>
       <c r="U4" s="543"/>
-      <c r="V4" s="544" t="s">
+      <c r="V4" s="535" t="s">
         <v>322</v>
       </c>
-      <c r="W4" s="545"/>
-      <c r="X4" s="545"/>
-      <c r="Y4" s="546"/>
+      <c r="W4" s="536"/>
+      <c r="X4" s="536"/>
+      <c r="Y4" s="537"/>
       <c r="Z4" s="106"/>
       <c r="AA4" s="106"/>
       <c r="AB4" s="114" t="s">
@@ -25366,34 +25366,34 @@
       <c r="E6" s="84"/>
       <c r="F6" s="84"/>
       <c r="G6" s="85"/>
-      <c r="H6" s="535" t="s">
+      <c r="H6" s="538" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="536"/>
-      <c r="J6" s="536"/>
-      <c r="K6" s="537"/>
-      <c r="L6" s="536" t="s">
+      <c r="I6" s="539"/>
+      <c r="J6" s="539"/>
+      <c r="K6" s="540"/>
+      <c r="L6" s="539" t="s">
         <v>45</v>
       </c>
-      <c r="M6" s="536"/>
-      <c r="N6" s="536"/>
-      <c r="O6" s="537"/>
-      <c r="P6" s="535" t="s">
+      <c r="M6" s="539"/>
+      <c r="N6" s="539"/>
+      <c r="O6" s="540"/>
+      <c r="P6" s="538" t="s">
         <v>45</v>
       </c>
-      <c r="Q6" s="536"/>
-      <c r="R6" s="536"/>
-      <c r="S6" s="537"/>
-      <c r="T6" s="535" t="s">
+      <c r="Q6" s="539"/>
+      <c r="R6" s="539"/>
+      <c r="S6" s="540"/>
+      <c r="T6" s="538" t="s">
         <v>302</v>
       </c>
-      <c r="U6" s="537"/>
-      <c r="V6" s="535" t="s">
+      <c r="U6" s="540"/>
+      <c r="V6" s="538" t="s">
         <v>968</v>
       </c>
-      <c r="W6" s="536"/>
-      <c r="X6" s="536"/>
-      <c r="Y6" s="537"/>
+      <c r="W6" s="539"/>
+      <c r="X6" s="539"/>
+      <c r="Y6" s="540"/>
       <c r="Z6" s="107" t="s">
         <v>980</v>
       </c>
@@ -28327,12 +28327,12 @@
         <v>321</v>
       </c>
       <c r="U42" s="543"/>
-      <c r="V42" s="544" t="s">
+      <c r="V42" s="535" t="s">
         <v>322</v>
       </c>
-      <c r="W42" s="545"/>
-      <c r="X42" s="545"/>
-      <c r="Y42" s="546"/>
+      <c r="W42" s="536"/>
+      <c r="X42" s="536"/>
+      <c r="Y42" s="537"/>
       <c r="Z42" s="106"/>
       <c r="AA42" s="106"/>
       <c r="AB42" s="114" t="s">
@@ -28431,34 +28431,34 @@
       <c r="E44" s="84"/>
       <c r="F44" s="84"/>
       <c r="G44" s="85"/>
-      <c r="H44" s="535" t="s">
+      <c r="H44" s="538" t="s">
         <v>45</v>
       </c>
-      <c r="I44" s="536"/>
-      <c r="J44" s="536"/>
-      <c r="K44" s="537"/>
-      <c r="L44" s="536" t="s">
+      <c r="I44" s="539"/>
+      <c r="J44" s="539"/>
+      <c r="K44" s="540"/>
+      <c r="L44" s="539" t="s">
         <v>45</v>
       </c>
-      <c r="M44" s="536"/>
-      <c r="N44" s="536"/>
-      <c r="O44" s="537"/>
-      <c r="P44" s="535" t="s">
+      <c r="M44" s="539"/>
+      <c r="N44" s="539"/>
+      <c r="O44" s="540"/>
+      <c r="P44" s="538" t="s">
         <v>45</v>
       </c>
-      <c r="Q44" s="536"/>
-      <c r="R44" s="536"/>
-      <c r="S44" s="537"/>
-      <c r="T44" s="538" t="s">
+      <c r="Q44" s="539"/>
+      <c r="R44" s="539"/>
+      <c r="S44" s="540"/>
+      <c r="T44" s="544" t="s">
         <v>302</v>
       </c>
-      <c r="U44" s="539"/>
-      <c r="V44" s="538" t="s">
+      <c r="U44" s="545"/>
+      <c r="V44" s="544" t="s">
         <v>968</v>
       </c>
-      <c r="W44" s="540"/>
-      <c r="X44" s="540"/>
-      <c r="Y44" s="539"/>
+      <c r="W44" s="546"/>
+      <c r="X44" s="546"/>
+      <c r="Y44" s="545"/>
       <c r="Z44" s="450" t="s">
         <v>980</v>
       </c>
@@ -32189,12 +32189,12 @@
         <v>321</v>
       </c>
       <c r="U90" s="543"/>
-      <c r="V90" s="544" t="s">
+      <c r="V90" s="535" t="s">
         <v>322</v>
       </c>
-      <c r="W90" s="545"/>
-      <c r="X90" s="545"/>
-      <c r="Y90" s="546"/>
+      <c r="W90" s="536"/>
+      <c r="X90" s="536"/>
+      <c r="Y90" s="537"/>
       <c r="Z90" s="106"/>
       <c r="AA90" s="106"/>
       <c r="AB90" s="114" t="s">
@@ -32293,34 +32293,34 @@
       <c r="E92" s="84"/>
       <c r="F92" s="84"/>
       <c r="G92" s="85"/>
-      <c r="H92" s="535" t="s">
+      <c r="H92" s="538" t="s">
         <v>45</v>
       </c>
-      <c r="I92" s="536"/>
-      <c r="J92" s="536"/>
-      <c r="K92" s="537"/>
-      <c r="L92" s="536" t="s">
+      <c r="I92" s="539"/>
+      <c r="J92" s="539"/>
+      <c r="K92" s="540"/>
+      <c r="L92" s="539" t="s">
         <v>45</v>
       </c>
-      <c r="M92" s="536"/>
-      <c r="N92" s="536"/>
-      <c r="O92" s="537"/>
-      <c r="P92" s="535" t="s">
+      <c r="M92" s="539"/>
+      <c r="N92" s="539"/>
+      <c r="O92" s="540"/>
+      <c r="P92" s="538" t="s">
         <v>45</v>
       </c>
-      <c r="Q92" s="536"/>
-      <c r="R92" s="536"/>
-      <c r="S92" s="537"/>
-      <c r="T92" s="538" t="s">
+      <c r="Q92" s="539"/>
+      <c r="R92" s="539"/>
+      <c r="S92" s="540"/>
+      <c r="T92" s="544" t="s">
         <v>302</v>
       </c>
-      <c r="U92" s="539"/>
-      <c r="V92" s="538" t="s">
+      <c r="U92" s="545"/>
+      <c r="V92" s="544" t="s">
         <v>968</v>
       </c>
-      <c r="W92" s="540"/>
-      <c r="X92" s="540"/>
-      <c r="Y92" s="539"/>
+      <c r="W92" s="546"/>
+      <c r="X92" s="546"/>
+      <c r="Y92" s="545"/>
       <c r="Z92" s="450" t="s">
         <v>980</v>
       </c>
@@ -35446,20 +35446,20 @@
       </c>
       <c r="U125" s="94"/>
       <c r="V125" s="65">
-        <f>(JRC_Data!BB62/1000)*($U$154/$U$148)*1.5</f>
-        <v>4.6583333333333332</v>
+        <f>(JRC_Data!BB62/1000)*($U$154/$U$148)*2</f>
+        <v>6.2111111111111104</v>
       </c>
       <c r="W125" s="65">
-        <f>(JRC_Data!BC62/1000)*($U$154/$U$148)*1.5</f>
-        <v>4.6583333333333332</v>
+        <f>(JRC_Data!BC62/1000)*($U$154/$U$148)*2</f>
+        <v>6.2111111111111104</v>
       </c>
       <c r="X125" s="65">
-        <f>(JRC_Data!BD62/1000)*($U$154/$U$148)*1.5</f>
-        <v>4.6583333333333332</v>
+        <f>(JRC_Data!BD62/1000)*($U$154/$U$148)*2</f>
+        <v>6.2111111111111104</v>
       </c>
       <c r="Y125" s="65">
-        <f>(JRC_Data!BE62/1000)*($U$154/$U$148)*1.5</f>
-        <v>4.6583333333333332</v>
+        <f>(JRC_Data!BE62/1000)*($U$154/$U$148)*2</f>
+        <v>6.2111111111111104</v>
       </c>
       <c r="Z125" s="131">
         <f>JRC_Data!BL62/1000</f>
@@ -35530,20 +35530,20 @@
       </c>
       <c r="U126" s="97"/>
       <c r="V126" s="329">
-        <f>(JRC_Data!BB62/1000)*($U$154/$U$148)*1.5</f>
-        <v>4.6583333333333332</v>
+        <f>(JRC_Data!BB62/1000)*($U$154/$U$148)*2</f>
+        <v>6.2111111111111104</v>
       </c>
       <c r="W126" s="329">
-        <f>(JRC_Data!BC62/1000)*($U$154/$U$148)*1.5</f>
-        <v>4.6583333333333332</v>
+        <f>(JRC_Data!BC62/1000)*($U$154/$U$148)*2</f>
+        <v>6.2111111111111104</v>
       </c>
       <c r="X126" s="329">
-        <f>(JRC_Data!BD62/1000)*($U$154/$U$148)*1.5</f>
-        <v>4.6583333333333332</v>
+        <f>(JRC_Data!BD62/1000)*($U$154/$U$148)*2</f>
+        <v>6.2111111111111104</v>
       </c>
       <c r="Y126" s="329">
-        <f>(JRC_Data!BE62/1000)*($U$154/$U$148)*1.5</f>
-        <v>4.6583333333333332</v>
+        <f>(JRC_Data!BE62/1000)*($U$154/$U$148)*2</f>
+        <v>6.2111111111111104</v>
       </c>
       <c r="Z126" s="110">
         <f>JRC_Data!BL62/1000</f>
@@ -36191,6 +36191,26 @@
     <row r="166" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="H92:K92"/>
+    <mergeCell ref="L92:O92"/>
+    <mergeCell ref="P92:S92"/>
+    <mergeCell ref="T92:U92"/>
+    <mergeCell ref="V92:Y92"/>
+    <mergeCell ref="H90:K90"/>
+    <mergeCell ref="L90:O90"/>
+    <mergeCell ref="P90:S90"/>
+    <mergeCell ref="T90:U90"/>
+    <mergeCell ref="V90:Y90"/>
+    <mergeCell ref="H44:K44"/>
+    <mergeCell ref="L44:O44"/>
+    <mergeCell ref="P44:S44"/>
+    <mergeCell ref="T44:U44"/>
+    <mergeCell ref="V44:Y44"/>
+    <mergeCell ref="H42:K42"/>
+    <mergeCell ref="L42:O42"/>
+    <mergeCell ref="P42:S42"/>
+    <mergeCell ref="T42:U42"/>
+    <mergeCell ref="V42:Y42"/>
     <mergeCell ref="V4:Y4"/>
     <mergeCell ref="V6:Y6"/>
     <mergeCell ref="H4:K4"/>
@@ -36201,26 +36221,6 @@
     <mergeCell ref="P6:S6"/>
     <mergeCell ref="L6:O6"/>
     <mergeCell ref="H6:K6"/>
-    <mergeCell ref="H42:K42"/>
-    <mergeCell ref="L42:O42"/>
-    <mergeCell ref="P42:S42"/>
-    <mergeCell ref="T42:U42"/>
-    <mergeCell ref="V42:Y42"/>
-    <mergeCell ref="H44:K44"/>
-    <mergeCell ref="L44:O44"/>
-    <mergeCell ref="P44:S44"/>
-    <mergeCell ref="T44:U44"/>
-    <mergeCell ref="V44:Y44"/>
-    <mergeCell ref="H90:K90"/>
-    <mergeCell ref="L90:O90"/>
-    <mergeCell ref="P90:S90"/>
-    <mergeCell ref="T90:U90"/>
-    <mergeCell ref="V90:Y90"/>
-    <mergeCell ref="H92:K92"/>
-    <mergeCell ref="L92:O92"/>
-    <mergeCell ref="P92:S92"/>
-    <mergeCell ref="T92:U92"/>
-    <mergeCell ref="V92:Y92"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
@@ -36365,12 +36365,12 @@
       <c r="I5" s="173"/>
       <c r="J5" s="173"/>
       <c r="K5" s="173"/>
-      <c r="L5" s="544" t="s">
+      <c r="L5" s="535" t="s">
         <v>322</v>
       </c>
-      <c r="M5" s="545"/>
-      <c r="N5" s="545"/>
-      <c r="O5" s="546"/>
+      <c r="M5" s="536"/>
+      <c r="N5" s="536"/>
+      <c r="O5" s="537"/>
       <c r="P5" s="106"/>
       <c r="Q5" s="106" t="s">
         <v>323</v>
@@ -36401,12 +36401,12 @@
       <c r="I6" s="83"/>
       <c r="J6" s="83"/>
       <c r="K6" s="83"/>
-      <c r="L6" s="538" t="s">
+      <c r="L6" s="544" t="s">
         <v>968</v>
       </c>
-      <c r="M6" s="540"/>
-      <c r="N6" s="540"/>
-      <c r="O6" s="539"/>
+      <c r="M6" s="546"/>
+      <c r="N6" s="546"/>
+      <c r="O6" s="545"/>
       <c r="P6" s="450" t="s">
         <v>980</v>
       </c>
@@ -37324,23 +37324,23 @@
       <c r="K33" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="L33" s="544" t="s">
+      <c r="L33" s="535" t="s">
         <v>322</v>
       </c>
-      <c r="M33" s="545"/>
-      <c r="N33" s="545"/>
-      <c r="O33" s="546"/>
+      <c r="M33" s="536"/>
+      <c r="N33" s="536"/>
+      <c r="O33" s="537"/>
     </row>
     <row r="34" spans="8:15" x14ac:dyDescent="0.2">
       <c r="H34" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="L34" s="538" t="s">
+      <c r="L34" s="544" t="s">
         <v>327</v>
       </c>
-      <c r="M34" s="540"/>
-      <c r="N34" s="540"/>
-      <c r="O34" s="539"/>
+      <c r="M34" s="546"/>
+      <c r="N34" s="546"/>
+      <c r="O34" s="545"/>
     </row>
     <row r="35" spans="8:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H35" s="5" t="s">
@@ -37687,11 +37687,11 @@
       </c>
       <c r="I4" s="542"/>
       <c r="J4" s="543"/>
-      <c r="K4" s="544" t="s">
+      <c r="K4" s="535" t="s">
         <v>322</v>
       </c>
-      <c r="L4" s="545"/>
-      <c r="M4" s="546"/>
+      <c r="L4" s="536"/>
+      <c r="M4" s="537"/>
       <c r="N4" s="106"/>
       <c r="O4" s="106" t="s">
         <v>323</v>
@@ -37717,16 +37717,16 @@
       <c r="G5" s="458" t="s">
         <v>302</v>
       </c>
-      <c r="H5" s="551" t="s">
+      <c r="H5" s="548" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="552"/>
-      <c r="J5" s="553"/>
-      <c r="K5" s="551" t="s">
+      <c r="I5" s="549"/>
+      <c r="J5" s="550"/>
+      <c r="K5" s="548" t="s">
         <v>757</v>
       </c>
-      <c r="L5" s="552"/>
-      <c r="M5" s="553"/>
+      <c r="L5" s="549"/>
+      <c r="M5" s="550"/>
       <c r="N5" s="459" t="s">
         <v>328</v>
       </c>
@@ -37743,23 +37743,23 @@
         <v>626</v>
       </c>
       <c r="AA5" s="281"/>
-      <c r="AB5" s="548" t="s">
+      <c r="AB5" s="551" t="s">
         <v>1013</v>
       </c>
-      <c r="AC5" s="548"/>
+      <c r="AC5" s="551"/>
       <c r="AD5" s="461"/>
-      <c r="AE5" s="549" t="s">
+      <c r="AE5" s="552" t="s">
         <v>110</v>
       </c>
-      <c r="AF5" s="549"/>
-      <c r="AG5" s="549" t="s">
+      <c r="AF5" s="552"/>
+      <c r="AG5" s="552" t="s">
         <v>1014</v>
       </c>
-      <c r="AH5" s="549"/>
-      <c r="AI5" s="550" t="s">
+      <c r="AH5" s="552"/>
+      <c r="AI5" s="553" t="s">
         <v>1015</v>
       </c>
-      <c r="AJ5" s="550"/>
+      <c r="AJ5" s="553"/>
     </row>
     <row r="6" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C6" s="505" t="str">
@@ -38497,12 +38497,12 @@
       <c r="K27" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="L27" s="544" t="s">
+      <c r="L27" s="535" t="s">
         <v>322</v>
       </c>
-      <c r="M27" s="545"/>
-      <c r="N27" s="545"/>
-      <c r="O27" s="546"/>
+      <c r="M27" s="536"/>
+      <c r="N27" s="536"/>
+      <c r="O27" s="537"/>
       <c r="T27" s="283"/>
       <c r="U27" s="283"/>
     </row>
@@ -38510,12 +38510,12 @@
       <c r="J28" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="L28" s="535" t="s">
+      <c r="L28" s="538" t="s">
         <v>327</v>
       </c>
-      <c r="M28" s="536"/>
-      <c r="N28" s="536"/>
-      <c r="O28" s="537"/>
+      <c r="M28" s="539"/>
+      <c r="N28" s="539"/>
+      <c r="O28" s="540"/>
       <c r="T28" s="283"/>
       <c r="U28" s="283"/>
     </row>
@@ -39905,16 +39905,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="AB5:AC5"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AG5:AH5"/>
+    <mergeCell ref="AI5:AJ5"/>
+    <mergeCell ref="L27:O27"/>
     <mergeCell ref="L28:O28"/>
     <mergeCell ref="H4:J4"/>
     <mergeCell ref="K4:M4"/>
     <mergeCell ref="H5:J5"/>
     <mergeCell ref="K5:M5"/>
-    <mergeCell ref="AB5:AC5"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="AG5:AH5"/>
-    <mergeCell ref="AI5:AJ5"/>
-    <mergeCell ref="L27:O27"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="S7" r:id="rId1" xr:uid="{B1EDD63D-40A5-4174-9D28-8666BD314B83}"/>
@@ -48942,103 +48942,103 @@
       <c r="C4" s="356" t="s">
         <v>766</v>
       </c>
-      <c r="D4" s="555" t="s">
+      <c r="D4" s="554" t="s">
         <v>767</v>
       </c>
-      <c r="E4" s="554"/>
-      <c r="F4" s="554"/>
-      <c r="G4" s="554"/>
+      <c r="E4" s="555"/>
+      <c r="F4" s="555"/>
+      <c r="G4" s="555"/>
       <c r="H4" s="556"/>
-      <c r="I4" s="554" t="s">
+      <c r="I4" s="555" t="s">
         <v>768</v>
       </c>
-      <c r="J4" s="554"/>
-      <c r="K4" s="554"/>
-      <c r="L4" s="554"/>
+      <c r="J4" s="555"/>
+      <c r="K4" s="555"/>
+      <c r="L4" s="555"/>
       <c r="M4" s="556"/>
-      <c r="N4" s="554" t="s">
+      <c r="N4" s="555" t="s">
         <v>769</v>
       </c>
-      <c r="O4" s="554"/>
-      <c r="P4" s="554"/>
-      <c r="Q4" s="554"/>
+      <c r="O4" s="555"/>
+      <c r="P4" s="555"/>
+      <c r="Q4" s="555"/>
       <c r="R4" s="556"/>
-      <c r="S4" s="554" t="s">
+      <c r="S4" s="555" t="s">
         <v>770</v>
       </c>
-      <c r="T4" s="554"/>
-      <c r="U4" s="554"/>
-      <c r="V4" s="554"/>
+      <c r="T4" s="555"/>
+      <c r="U4" s="555"/>
+      <c r="V4" s="555"/>
       <c r="W4" s="556"/>
-      <c r="X4" s="554" t="s">
+      <c r="X4" s="555" t="s">
         <v>771</v>
       </c>
-      <c r="Y4" s="554"/>
-      <c r="Z4" s="554"/>
-      <c r="AA4" s="554"/>
+      <c r="Y4" s="555"/>
+      <c r="Z4" s="555"/>
+      <c r="AA4" s="555"/>
       <c r="AB4" s="556"/>
-      <c r="AC4" s="554" t="s">
+      <c r="AC4" s="555" t="s">
         <v>772</v>
       </c>
-      <c r="AD4" s="554"/>
-      <c r="AE4" s="554"/>
-      <c r="AF4" s="554"/>
+      <c r="AD4" s="555"/>
+      <c r="AE4" s="555"/>
+      <c r="AF4" s="555"/>
       <c r="AG4" s="556"/>
-      <c r="AH4" s="554" t="s">
+      <c r="AH4" s="555" t="s">
         <v>773</v>
       </c>
-      <c r="AI4" s="554"/>
-      <c r="AJ4" s="554"/>
-      <c r="AK4" s="554"/>
+      <c r="AI4" s="555"/>
+      <c r="AJ4" s="555"/>
+      <c r="AK4" s="555"/>
       <c r="AL4" s="556"/>
-      <c r="AM4" s="554" t="s">
+      <c r="AM4" s="555" t="s">
         <v>774</v>
       </c>
-      <c r="AN4" s="554"/>
-      <c r="AO4" s="554"/>
-      <c r="AP4" s="554"/>
+      <c r="AN4" s="555"/>
+      <c r="AO4" s="555"/>
+      <c r="AP4" s="555"/>
       <c r="AQ4" s="556"/>
-      <c r="AR4" s="554" t="s">
+      <c r="AR4" s="555" t="s">
         <v>775</v>
       </c>
-      <c r="AS4" s="554"/>
-      <c r="AT4" s="554"/>
-      <c r="AU4" s="554"/>
+      <c r="AS4" s="555"/>
+      <c r="AT4" s="555"/>
+      <c r="AU4" s="555"/>
       <c r="AV4" s="556"/>
-      <c r="AW4" s="554" t="s">
+      <c r="AW4" s="555" t="s">
         <v>776</v>
       </c>
-      <c r="AX4" s="554"/>
-      <c r="AY4" s="554"/>
-      <c r="AZ4" s="554"/>
-      <c r="BA4" s="554"/>
-      <c r="BB4" s="555" t="s">
+      <c r="AX4" s="555"/>
+      <c r="AY4" s="555"/>
+      <c r="AZ4" s="555"/>
+      <c r="BA4" s="555"/>
+      <c r="BB4" s="554" t="s">
         <v>777</v>
       </c>
-      <c r="BC4" s="554"/>
-      <c r="BD4" s="554"/>
-      <c r="BE4" s="554"/>
+      <c r="BC4" s="555"/>
+      <c r="BD4" s="555"/>
+      <c r="BE4" s="555"/>
       <c r="BF4" s="556"/>
-      <c r="BG4" s="554" t="s">
+      <c r="BG4" s="555" t="s">
         <v>778</v>
       </c>
-      <c r="BH4" s="554"/>
-      <c r="BI4" s="554"/>
-      <c r="BJ4" s="554"/>
-      <c r="BK4" s="554"/>
-      <c r="BL4" s="555" t="s">
+      <c r="BH4" s="555"/>
+      <c r="BI4" s="555"/>
+      <c r="BJ4" s="555"/>
+      <c r="BK4" s="555"/>
+      <c r="BL4" s="554" t="s">
         <v>779</v>
       </c>
-      <c r="BM4" s="554"/>
-      <c r="BN4" s="554"/>
-      <c r="BO4" s="554"/>
-      <c r="BP4" s="554"/>
-      <c r="BQ4" s="555" t="s">
+      <c r="BM4" s="555"/>
+      <c r="BN4" s="555"/>
+      <c r="BO4" s="555"/>
+      <c r="BP4" s="555"/>
+      <c r="BQ4" s="554" t="s">
         <v>780</v>
       </c>
-      <c r="BR4" s="554"/>
-      <c r="BS4" s="554"/>
-      <c r="BT4" s="554"/>
+      <c r="BR4" s="555"/>
+      <c r="BS4" s="555"/>
+      <c r="BT4" s="555"/>
       <c r="BU4" s="556"/>
       <c r="BV4" s="357" t="s">
         <v>781</v>
@@ -62632,11 +62632,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="BL4:BP4"/>
-    <mergeCell ref="BQ4:BU4"/>
-    <mergeCell ref="BW4:CA4"/>
-    <mergeCell ref="CB4:CF4"/>
-    <mergeCell ref="CG4:CK4"/>
     <mergeCell ref="BG4:BK4"/>
     <mergeCell ref="D4:H4"/>
     <mergeCell ref="I4:M4"/>
@@ -62649,6 +62644,11 @@
     <mergeCell ref="AR4:AV4"/>
     <mergeCell ref="AW4:BA4"/>
     <mergeCell ref="BB4:BF4"/>
+    <mergeCell ref="BL4:BP4"/>
+    <mergeCell ref="BQ4:BU4"/>
+    <mergeCell ref="BW4:CA4"/>
+    <mergeCell ref="CB4:CF4"/>
+    <mergeCell ref="CG4:CK4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
DH cost in detached back to 50% higher and comes in 2035
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_RSD.xlsx
+++ b/SubRES_TMPL/SubRes_RSD.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5408B471-41AF-4A71-8D79-70B6346F3FC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{788EC548-EA10-426C-B690-81C132EEF447}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{34F9D92C-266F-476D-89E0-63153305AC39}"/>
   </bookViews>
@@ -14592,15 +14592,6 @@
     <xf numFmtId="0" fontId="53" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="23" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -14608,6 +14599,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -14619,17 +14619,26 @@
     <xf numFmtId="0" fontId="16" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="69" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="23" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -14640,19 +14649,10 @@
     <xf numFmtId="0" fontId="16" fillId="23" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="69" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="60" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="60" fillId="31" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="60" fillId="31" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -25076,7 +25076,7 @@
   <dimension ref="A2:AQ166"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H91" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="V125" sqref="V125:Y126"/>
+      <selection activeCell="AD113" sqref="AD113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -25262,12 +25262,12 @@
         <v>321</v>
       </c>
       <c r="U4" s="543"/>
-      <c r="V4" s="535" t="s">
+      <c r="V4" s="544" t="s">
         <v>322</v>
       </c>
-      <c r="W4" s="536"/>
-      <c r="X4" s="536"/>
-      <c r="Y4" s="537"/>
+      <c r="W4" s="545"/>
+      <c r="X4" s="545"/>
+      <c r="Y4" s="546"/>
       <c r="Z4" s="106"/>
       <c r="AA4" s="106"/>
       <c r="AB4" s="114" t="s">
@@ -25366,34 +25366,34 @@
       <c r="E6" s="84"/>
       <c r="F6" s="84"/>
       <c r="G6" s="85"/>
-      <c r="H6" s="538" t="s">
+      <c r="H6" s="535" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="539"/>
-      <c r="J6" s="539"/>
-      <c r="K6" s="540"/>
-      <c r="L6" s="539" t="s">
+      <c r="I6" s="536"/>
+      <c r="J6" s="536"/>
+      <c r="K6" s="537"/>
+      <c r="L6" s="536" t="s">
         <v>45</v>
       </c>
-      <c r="M6" s="539"/>
-      <c r="N6" s="539"/>
-      <c r="O6" s="540"/>
-      <c r="P6" s="538" t="s">
+      <c r="M6" s="536"/>
+      <c r="N6" s="536"/>
+      <c r="O6" s="537"/>
+      <c r="P6" s="535" t="s">
         <v>45</v>
       </c>
-      <c r="Q6" s="539"/>
-      <c r="R6" s="539"/>
-      <c r="S6" s="540"/>
-      <c r="T6" s="538" t="s">
+      <c r="Q6" s="536"/>
+      <c r="R6" s="536"/>
+      <c r="S6" s="537"/>
+      <c r="T6" s="535" t="s">
         <v>302</v>
       </c>
-      <c r="U6" s="540"/>
-      <c r="V6" s="538" t="s">
+      <c r="U6" s="537"/>
+      <c r="V6" s="535" t="s">
         <v>968</v>
       </c>
-      <c r="W6" s="539"/>
-      <c r="X6" s="539"/>
-      <c r="Y6" s="540"/>
+      <c r="W6" s="536"/>
+      <c r="X6" s="536"/>
+      <c r="Y6" s="537"/>
       <c r="Z6" s="107" t="s">
         <v>980</v>
       </c>
@@ -28327,12 +28327,12 @@
         <v>321</v>
       </c>
       <c r="U42" s="543"/>
-      <c r="V42" s="535" t="s">
+      <c r="V42" s="544" t="s">
         <v>322</v>
       </c>
-      <c r="W42" s="536"/>
-      <c r="X42" s="536"/>
-      <c r="Y42" s="537"/>
+      <c r="W42" s="545"/>
+      <c r="X42" s="545"/>
+      <c r="Y42" s="546"/>
       <c r="Z42" s="106"/>
       <c r="AA42" s="106"/>
       <c r="AB42" s="114" t="s">
@@ -28431,34 +28431,34 @@
       <c r="E44" s="84"/>
       <c r="F44" s="84"/>
       <c r="G44" s="85"/>
-      <c r="H44" s="538" t="s">
+      <c r="H44" s="535" t="s">
         <v>45</v>
       </c>
-      <c r="I44" s="539"/>
-      <c r="J44" s="539"/>
-      <c r="K44" s="540"/>
-      <c r="L44" s="539" t="s">
+      <c r="I44" s="536"/>
+      <c r="J44" s="536"/>
+      <c r="K44" s="537"/>
+      <c r="L44" s="536" t="s">
         <v>45</v>
       </c>
-      <c r="M44" s="539"/>
-      <c r="N44" s="539"/>
-      <c r="O44" s="540"/>
-      <c r="P44" s="538" t="s">
+      <c r="M44" s="536"/>
+      <c r="N44" s="536"/>
+      <c r="O44" s="537"/>
+      <c r="P44" s="535" t="s">
         <v>45</v>
       </c>
-      <c r="Q44" s="539"/>
-      <c r="R44" s="539"/>
-      <c r="S44" s="540"/>
-      <c r="T44" s="544" t="s">
+      <c r="Q44" s="536"/>
+      <c r="R44" s="536"/>
+      <c r="S44" s="537"/>
+      <c r="T44" s="538" t="s">
         <v>302</v>
       </c>
-      <c r="U44" s="545"/>
-      <c r="V44" s="544" t="s">
+      <c r="U44" s="539"/>
+      <c r="V44" s="538" t="s">
         <v>968</v>
       </c>
-      <c r="W44" s="546"/>
-      <c r="X44" s="546"/>
-      <c r="Y44" s="545"/>
+      <c r="W44" s="540"/>
+      <c r="X44" s="540"/>
+      <c r="Y44" s="539"/>
       <c r="Z44" s="450" t="s">
         <v>980</v>
       </c>
@@ -32189,12 +32189,12 @@
         <v>321</v>
       </c>
       <c r="U90" s="543"/>
-      <c r="V90" s="535" t="s">
+      <c r="V90" s="544" t="s">
         <v>322</v>
       </c>
-      <c r="W90" s="536"/>
-      <c r="X90" s="536"/>
-      <c r="Y90" s="537"/>
+      <c r="W90" s="545"/>
+      <c r="X90" s="545"/>
+      <c r="Y90" s="546"/>
       <c r="Z90" s="106"/>
       <c r="AA90" s="106"/>
       <c r="AB90" s="114" t="s">
@@ -32293,34 +32293,34 @@
       <c r="E92" s="84"/>
       <c r="F92" s="84"/>
       <c r="G92" s="85"/>
-      <c r="H92" s="538" t="s">
+      <c r="H92" s="535" t="s">
         <v>45</v>
       </c>
-      <c r="I92" s="539"/>
-      <c r="J92" s="539"/>
-      <c r="K92" s="540"/>
-      <c r="L92" s="539" t="s">
+      <c r="I92" s="536"/>
+      <c r="J92" s="536"/>
+      <c r="K92" s="537"/>
+      <c r="L92" s="536" t="s">
         <v>45</v>
       </c>
-      <c r="M92" s="539"/>
-      <c r="N92" s="539"/>
-      <c r="O92" s="540"/>
-      <c r="P92" s="538" t="s">
+      <c r="M92" s="536"/>
+      <c r="N92" s="536"/>
+      <c r="O92" s="537"/>
+      <c r="P92" s="535" t="s">
         <v>45</v>
       </c>
-      <c r="Q92" s="539"/>
-      <c r="R92" s="539"/>
-      <c r="S92" s="540"/>
-      <c r="T92" s="544" t="s">
+      <c r="Q92" s="536"/>
+      <c r="R92" s="536"/>
+      <c r="S92" s="537"/>
+      <c r="T92" s="538" t="s">
         <v>302</v>
       </c>
-      <c r="U92" s="545"/>
-      <c r="V92" s="544" t="s">
+      <c r="U92" s="539"/>
+      <c r="V92" s="538" t="s">
         <v>968</v>
       </c>
-      <c r="W92" s="546"/>
-      <c r="X92" s="546"/>
-      <c r="Y92" s="545"/>
+      <c r="W92" s="540"/>
+      <c r="X92" s="540"/>
+      <c r="Y92" s="539"/>
       <c r="Z92" s="450" t="s">
         <v>980</v>
       </c>
@@ -35446,20 +35446,20 @@
       </c>
       <c r="U125" s="94"/>
       <c r="V125" s="65">
-        <f>(JRC_Data!BB62/1000)*($U$154/$U$148)*2</f>
-        <v>6.2111111111111104</v>
+        <f>(JRC_Data!BB62/1000)*($U$154/$U$148)*1.5</f>
+        <v>4.6583333333333332</v>
       </c>
       <c r="W125" s="65">
-        <f>(JRC_Data!BC62/1000)*($U$154/$U$148)*2</f>
-        <v>6.2111111111111104</v>
+        <f>(JRC_Data!BC62/1000)*($U$154/$U$148)*1.5</f>
+        <v>4.6583333333333332</v>
       </c>
       <c r="X125" s="65">
-        <f>(JRC_Data!BD62/1000)*($U$154/$U$148)*2</f>
-        <v>6.2111111111111104</v>
+        <f>(JRC_Data!BD62/1000)*($U$154/$U$148)*1.5</f>
+        <v>4.6583333333333332</v>
       </c>
       <c r="Y125" s="65">
-        <f>(JRC_Data!BE62/1000)*($U$154/$U$148)*2</f>
-        <v>6.2111111111111104</v>
+        <f>(JRC_Data!BE62/1000)*($U$154/$U$148)*1.5</f>
+        <v>4.6583333333333332</v>
       </c>
       <c r="Z125" s="131">
         <f>JRC_Data!BL62/1000</f>
@@ -35476,7 +35476,7 @@
       </c>
       <c r="AG125" s="134"/>
       <c r="AH125" s="111">
-        <v>2019</v>
+        <v>2035</v>
       </c>
       <c r="AI125" s="134">
         <v>38</v>
@@ -35530,20 +35530,20 @@
       </c>
       <c r="U126" s="97"/>
       <c r="V126" s="329">
-        <f>(JRC_Data!BB62/1000)*($U$154/$U$148)*2</f>
-        <v>6.2111111111111104</v>
+        <f>(JRC_Data!BB62/1000)*($U$154/$U$148)*1.5</f>
+        <v>4.6583333333333332</v>
       </c>
       <c r="W126" s="329">
-        <f>(JRC_Data!BC62/1000)*($U$154/$U$148)*2</f>
-        <v>6.2111111111111104</v>
+        <f>(JRC_Data!BC62/1000)*($U$154/$U$148)*1.5</f>
+        <v>4.6583333333333332</v>
       </c>
       <c r="X126" s="329">
-        <f>(JRC_Data!BD62/1000)*($U$154/$U$148)*2</f>
-        <v>6.2111111111111104</v>
+        <f>(JRC_Data!BD62/1000)*($U$154/$U$148)*1.5</f>
+        <v>4.6583333333333332</v>
       </c>
       <c r="Y126" s="329">
-        <f>(JRC_Data!BE62/1000)*($U$154/$U$148)*2</f>
-        <v>6.2111111111111104</v>
+        <f>(JRC_Data!BE62/1000)*($U$154/$U$148)*1.5</f>
+        <v>4.6583333333333332</v>
       </c>
       <c r="Z126" s="110">
         <f>JRC_Data!BL62/1000</f>
@@ -35560,7 +35560,7 @@
       </c>
       <c r="AG126" s="113"/>
       <c r="AH126" s="112">
-        <v>2019</v>
+        <v>2035</v>
       </c>
       <c r="AI126" s="113">
         <v>38</v>
@@ -36191,26 +36191,6 @@
     <row r="166" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="H92:K92"/>
-    <mergeCell ref="L92:O92"/>
-    <mergeCell ref="P92:S92"/>
-    <mergeCell ref="T92:U92"/>
-    <mergeCell ref="V92:Y92"/>
-    <mergeCell ref="H90:K90"/>
-    <mergeCell ref="L90:O90"/>
-    <mergeCell ref="P90:S90"/>
-    <mergeCell ref="T90:U90"/>
-    <mergeCell ref="V90:Y90"/>
-    <mergeCell ref="H44:K44"/>
-    <mergeCell ref="L44:O44"/>
-    <mergeCell ref="P44:S44"/>
-    <mergeCell ref="T44:U44"/>
-    <mergeCell ref="V44:Y44"/>
-    <mergeCell ref="H42:K42"/>
-    <mergeCell ref="L42:O42"/>
-    <mergeCell ref="P42:S42"/>
-    <mergeCell ref="T42:U42"/>
-    <mergeCell ref="V42:Y42"/>
     <mergeCell ref="V4:Y4"/>
     <mergeCell ref="V6:Y6"/>
     <mergeCell ref="H4:K4"/>
@@ -36221,6 +36201,26 @@
     <mergeCell ref="P6:S6"/>
     <mergeCell ref="L6:O6"/>
     <mergeCell ref="H6:K6"/>
+    <mergeCell ref="H42:K42"/>
+    <mergeCell ref="L42:O42"/>
+    <mergeCell ref="P42:S42"/>
+    <mergeCell ref="T42:U42"/>
+    <mergeCell ref="V42:Y42"/>
+    <mergeCell ref="H44:K44"/>
+    <mergeCell ref="L44:O44"/>
+    <mergeCell ref="P44:S44"/>
+    <mergeCell ref="T44:U44"/>
+    <mergeCell ref="V44:Y44"/>
+    <mergeCell ref="H90:K90"/>
+    <mergeCell ref="L90:O90"/>
+    <mergeCell ref="P90:S90"/>
+    <mergeCell ref="T90:U90"/>
+    <mergeCell ref="V90:Y90"/>
+    <mergeCell ref="H92:K92"/>
+    <mergeCell ref="L92:O92"/>
+    <mergeCell ref="P92:S92"/>
+    <mergeCell ref="T92:U92"/>
+    <mergeCell ref="V92:Y92"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
@@ -36365,12 +36365,12 @@
       <c r="I5" s="173"/>
       <c r="J5" s="173"/>
       <c r="K5" s="173"/>
-      <c r="L5" s="535" t="s">
+      <c r="L5" s="544" t="s">
         <v>322</v>
       </c>
-      <c r="M5" s="536"/>
-      <c r="N5" s="536"/>
-      <c r="O5" s="537"/>
+      <c r="M5" s="545"/>
+      <c r="N5" s="545"/>
+      <c r="O5" s="546"/>
       <c r="P5" s="106"/>
       <c r="Q5" s="106" t="s">
         <v>323</v>
@@ -36401,12 +36401,12 @@
       <c r="I6" s="83"/>
       <c r="J6" s="83"/>
       <c r="K6" s="83"/>
-      <c r="L6" s="544" t="s">
+      <c r="L6" s="538" t="s">
         <v>968</v>
       </c>
-      <c r="M6" s="546"/>
-      <c r="N6" s="546"/>
-      <c r="O6" s="545"/>
+      <c r="M6" s="540"/>
+      <c r="N6" s="540"/>
+      <c r="O6" s="539"/>
       <c r="P6" s="450" t="s">
         <v>980</v>
       </c>
@@ -37324,23 +37324,23 @@
       <c r="K33" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="L33" s="535" t="s">
+      <c r="L33" s="544" t="s">
         <v>322</v>
       </c>
-      <c r="M33" s="536"/>
-      <c r="N33" s="536"/>
-      <c r="O33" s="537"/>
+      <c r="M33" s="545"/>
+      <c r="N33" s="545"/>
+      <c r="O33" s="546"/>
     </row>
     <row r="34" spans="8:15" x14ac:dyDescent="0.2">
       <c r="H34" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="L34" s="544" t="s">
+      <c r="L34" s="538" t="s">
         <v>327</v>
       </c>
-      <c r="M34" s="546"/>
-      <c r="N34" s="546"/>
-      <c r="O34" s="545"/>
+      <c r="M34" s="540"/>
+      <c r="N34" s="540"/>
+      <c r="O34" s="539"/>
     </row>
     <row r="35" spans="8:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H35" s="5" t="s">
@@ -37687,11 +37687,11 @@
       </c>
       <c r="I4" s="542"/>
       <c r="J4" s="543"/>
-      <c r="K4" s="535" t="s">
+      <c r="K4" s="544" t="s">
         <v>322</v>
       </c>
-      <c r="L4" s="536"/>
-      <c r="M4" s="537"/>
+      <c r="L4" s="545"/>
+      <c r="M4" s="546"/>
       <c r="N4" s="106"/>
       <c r="O4" s="106" t="s">
         <v>323</v>
@@ -37717,16 +37717,16 @@
       <c r="G5" s="458" t="s">
         <v>302</v>
       </c>
-      <c r="H5" s="548" t="s">
+      <c r="H5" s="551" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="549"/>
-      <c r="J5" s="550"/>
-      <c r="K5" s="548" t="s">
+      <c r="I5" s="552"/>
+      <c r="J5" s="553"/>
+      <c r="K5" s="551" t="s">
         <v>757</v>
       </c>
-      <c r="L5" s="549"/>
-      <c r="M5" s="550"/>
+      <c r="L5" s="552"/>
+      <c r="M5" s="553"/>
       <c r="N5" s="459" t="s">
         <v>328</v>
       </c>
@@ -37743,23 +37743,23 @@
         <v>626</v>
       </c>
       <c r="AA5" s="281"/>
-      <c r="AB5" s="551" t="s">
+      <c r="AB5" s="548" t="s">
         <v>1013</v>
       </c>
-      <c r="AC5" s="551"/>
+      <c r="AC5" s="548"/>
       <c r="AD5" s="461"/>
-      <c r="AE5" s="552" t="s">
+      <c r="AE5" s="549" t="s">
         <v>110</v>
       </c>
-      <c r="AF5" s="552"/>
-      <c r="AG5" s="552" t="s">
+      <c r="AF5" s="549"/>
+      <c r="AG5" s="549" t="s">
         <v>1014</v>
       </c>
-      <c r="AH5" s="552"/>
-      <c r="AI5" s="553" t="s">
+      <c r="AH5" s="549"/>
+      <c r="AI5" s="550" t="s">
         <v>1015</v>
       </c>
-      <c r="AJ5" s="553"/>
+      <c r="AJ5" s="550"/>
     </row>
     <row r="6" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C6" s="505" t="str">
@@ -38497,12 +38497,12 @@
       <c r="K27" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="L27" s="535" t="s">
+      <c r="L27" s="544" t="s">
         <v>322</v>
       </c>
-      <c r="M27" s="536"/>
-      <c r="N27" s="536"/>
-      <c r="O27" s="537"/>
+      <c r="M27" s="545"/>
+      <c r="N27" s="545"/>
+      <c r="O27" s="546"/>
       <c r="T27" s="283"/>
       <c r="U27" s="283"/>
     </row>
@@ -38510,12 +38510,12 @@
       <c r="J28" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="L28" s="538" t="s">
+      <c r="L28" s="535" t="s">
         <v>327</v>
       </c>
-      <c r="M28" s="539"/>
-      <c r="N28" s="539"/>
-      <c r="O28" s="540"/>
+      <c r="M28" s="536"/>
+      <c r="N28" s="536"/>
+      <c r="O28" s="537"/>
       <c r="T28" s="283"/>
       <c r="U28" s="283"/>
     </row>
@@ -39905,16 +39905,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="L28:O28"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="K5:M5"/>
     <mergeCell ref="AB5:AC5"/>
     <mergeCell ref="AE5:AF5"/>
     <mergeCell ref="AG5:AH5"/>
     <mergeCell ref="AI5:AJ5"/>
     <mergeCell ref="L27:O27"/>
-    <mergeCell ref="L28:O28"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="K5:M5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="S7" r:id="rId1" xr:uid="{B1EDD63D-40A5-4174-9D28-8666BD314B83}"/>
@@ -48942,103 +48942,103 @@
       <c r="C4" s="356" t="s">
         <v>766</v>
       </c>
-      <c r="D4" s="554" t="s">
+      <c r="D4" s="555" t="s">
         <v>767</v>
       </c>
-      <c r="E4" s="555"/>
-      <c r="F4" s="555"/>
-      <c r="G4" s="555"/>
+      <c r="E4" s="554"/>
+      <c r="F4" s="554"/>
+      <c r="G4" s="554"/>
       <c r="H4" s="556"/>
-      <c r="I4" s="555" t="s">
+      <c r="I4" s="554" t="s">
         <v>768</v>
       </c>
-      <c r="J4" s="555"/>
-      <c r="K4" s="555"/>
-      <c r="L4" s="555"/>
+      <c r="J4" s="554"/>
+      <c r="K4" s="554"/>
+      <c r="L4" s="554"/>
       <c r="M4" s="556"/>
-      <c r="N4" s="555" t="s">
+      <c r="N4" s="554" t="s">
         <v>769</v>
       </c>
-      <c r="O4" s="555"/>
-      <c r="P4" s="555"/>
-      <c r="Q4" s="555"/>
+      <c r="O4" s="554"/>
+      <c r="P4" s="554"/>
+      <c r="Q4" s="554"/>
       <c r="R4" s="556"/>
-      <c r="S4" s="555" t="s">
+      <c r="S4" s="554" t="s">
         <v>770</v>
       </c>
-      <c r="T4" s="555"/>
-      <c r="U4" s="555"/>
-      <c r="V4" s="555"/>
+      <c r="T4" s="554"/>
+      <c r="U4" s="554"/>
+      <c r="V4" s="554"/>
       <c r="W4" s="556"/>
-      <c r="X4" s="555" t="s">
+      <c r="X4" s="554" t="s">
         <v>771</v>
       </c>
-      <c r="Y4" s="555"/>
-      <c r="Z4" s="555"/>
-      <c r="AA4" s="555"/>
+      <c r="Y4" s="554"/>
+      <c r="Z4" s="554"/>
+      <c r="AA4" s="554"/>
       <c r="AB4" s="556"/>
-      <c r="AC4" s="555" t="s">
+      <c r="AC4" s="554" t="s">
         <v>772</v>
       </c>
-      <c r="AD4" s="555"/>
-      <c r="AE4" s="555"/>
-      <c r="AF4" s="555"/>
+      <c r="AD4" s="554"/>
+      <c r="AE4" s="554"/>
+      <c r="AF4" s="554"/>
       <c r="AG4" s="556"/>
-      <c r="AH4" s="555" t="s">
+      <c r="AH4" s="554" t="s">
         <v>773</v>
       </c>
-      <c r="AI4" s="555"/>
-      <c r="AJ4" s="555"/>
-      <c r="AK4" s="555"/>
+      <c r="AI4" s="554"/>
+      <c r="AJ4" s="554"/>
+      <c r="AK4" s="554"/>
       <c r="AL4" s="556"/>
-      <c r="AM4" s="555" t="s">
+      <c r="AM4" s="554" t="s">
         <v>774</v>
       </c>
-      <c r="AN4" s="555"/>
-      <c r="AO4" s="555"/>
-      <c r="AP4" s="555"/>
+      <c r="AN4" s="554"/>
+      <c r="AO4" s="554"/>
+      <c r="AP4" s="554"/>
       <c r="AQ4" s="556"/>
-      <c r="AR4" s="555" t="s">
+      <c r="AR4" s="554" t="s">
         <v>775</v>
       </c>
-      <c r="AS4" s="555"/>
-      <c r="AT4" s="555"/>
-      <c r="AU4" s="555"/>
+      <c r="AS4" s="554"/>
+      <c r="AT4" s="554"/>
+      <c r="AU4" s="554"/>
       <c r="AV4" s="556"/>
-      <c r="AW4" s="555" t="s">
+      <c r="AW4" s="554" t="s">
         <v>776</v>
       </c>
-      <c r="AX4" s="555"/>
-      <c r="AY4" s="555"/>
-      <c r="AZ4" s="555"/>
-      <c r="BA4" s="555"/>
-      <c r="BB4" s="554" t="s">
+      <c r="AX4" s="554"/>
+      <c r="AY4" s="554"/>
+      <c r="AZ4" s="554"/>
+      <c r="BA4" s="554"/>
+      <c r="BB4" s="555" t="s">
         <v>777</v>
       </c>
-      <c r="BC4" s="555"/>
-      <c r="BD4" s="555"/>
-      <c r="BE4" s="555"/>
+      <c r="BC4" s="554"/>
+      <c r="BD4" s="554"/>
+      <c r="BE4" s="554"/>
       <c r="BF4" s="556"/>
-      <c r="BG4" s="555" t="s">
+      <c r="BG4" s="554" t="s">
         <v>778</v>
       </c>
-      <c r="BH4" s="555"/>
-      <c r="BI4" s="555"/>
-      <c r="BJ4" s="555"/>
-      <c r="BK4" s="555"/>
-      <c r="BL4" s="554" t="s">
+      <c r="BH4" s="554"/>
+      <c r="BI4" s="554"/>
+      <c r="BJ4" s="554"/>
+      <c r="BK4" s="554"/>
+      <c r="BL4" s="555" t="s">
         <v>779</v>
       </c>
-      <c r="BM4" s="555"/>
-      <c r="BN4" s="555"/>
-      <c r="BO4" s="555"/>
-      <c r="BP4" s="555"/>
-      <c r="BQ4" s="554" t="s">
+      <c r="BM4" s="554"/>
+      <c r="BN4" s="554"/>
+      <c r="BO4" s="554"/>
+      <c r="BP4" s="554"/>
+      <c r="BQ4" s="555" t="s">
         <v>780</v>
       </c>
-      <c r="BR4" s="555"/>
-      <c r="BS4" s="555"/>
-      <c r="BT4" s="555"/>
+      <c r="BR4" s="554"/>
+      <c r="BS4" s="554"/>
+      <c r="BT4" s="554"/>
       <c r="BU4" s="556"/>
       <c r="BV4" s="357" t="s">
         <v>781</v>
@@ -62632,6 +62632,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="BL4:BP4"/>
+    <mergeCell ref="BQ4:BU4"/>
+    <mergeCell ref="BW4:CA4"/>
+    <mergeCell ref="CB4:CF4"/>
+    <mergeCell ref="CG4:CK4"/>
     <mergeCell ref="BG4:BK4"/>
     <mergeCell ref="D4:H4"/>
     <mergeCell ref="I4:M4"/>
@@ -62644,11 +62649,6 @@
     <mergeCell ref="AR4:AV4"/>
     <mergeCell ref="AW4:BA4"/>
     <mergeCell ref="BB4:BF4"/>
-    <mergeCell ref="BL4:BP4"/>
-    <mergeCell ref="BQ4:BU4"/>
-    <mergeCell ref="BW4:CA4"/>
-    <mergeCell ref="CB4:CF4"/>
-    <mergeCell ref="CG4:CK4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
Cookers to equal houses and Gas UP UC changed
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_RSD.xlsx
+++ b/SubRES_TMPL/SubRes_RSD.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{788EC548-EA10-426C-B690-81C132EEF447}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{599A8A1B-D114-4839-9AE9-A58F80079DF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{34F9D92C-266F-476D-89E0-63153305AC39}"/>
   </bookViews>
@@ -14592,6 +14592,15 @@
     <xf numFmtId="0" fontId="53" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="23" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -14599,15 +14608,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -14619,17 +14619,26 @@
     <xf numFmtId="0" fontId="16" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -14640,19 +14649,10 @@
     <xf numFmtId="0" fontId="69" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="60" fillId="31" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="60" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="31" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="60" fillId="31" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -25075,8 +25075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{104F8057-C735-4662-BAA6-EEDCF7B57273}">
   <dimension ref="A2:AQ166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H91" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AD113" sqref="AD113"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -25262,12 +25262,12 @@
         <v>321</v>
       </c>
       <c r="U4" s="543"/>
-      <c r="V4" s="544" t="s">
+      <c r="V4" s="535" t="s">
         <v>322</v>
       </c>
-      <c r="W4" s="545"/>
-      <c r="X4" s="545"/>
-      <c r="Y4" s="546"/>
+      <c r="W4" s="536"/>
+      <c r="X4" s="536"/>
+      <c r="Y4" s="537"/>
       <c r="Z4" s="106"/>
       <c r="AA4" s="106"/>
       <c r="AB4" s="114" t="s">
@@ -25366,34 +25366,34 @@
       <c r="E6" s="84"/>
       <c r="F6" s="84"/>
       <c r="G6" s="85"/>
-      <c r="H6" s="535" t="s">
+      <c r="H6" s="538" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="536"/>
-      <c r="J6" s="536"/>
-      <c r="K6" s="537"/>
-      <c r="L6" s="536" t="s">
+      <c r="I6" s="539"/>
+      <c r="J6" s="539"/>
+      <c r="K6" s="540"/>
+      <c r="L6" s="539" t="s">
         <v>45</v>
       </c>
-      <c r="M6" s="536"/>
-      <c r="N6" s="536"/>
-      <c r="O6" s="537"/>
-      <c r="P6" s="535" t="s">
+      <c r="M6" s="539"/>
+      <c r="N6" s="539"/>
+      <c r="O6" s="540"/>
+      <c r="P6" s="538" t="s">
         <v>45</v>
       </c>
-      <c r="Q6" s="536"/>
-      <c r="R6" s="536"/>
-      <c r="S6" s="537"/>
-      <c r="T6" s="535" t="s">
+      <c r="Q6" s="539"/>
+      <c r="R6" s="539"/>
+      <c r="S6" s="540"/>
+      <c r="T6" s="538" t="s">
         <v>302</v>
       </c>
-      <c r="U6" s="537"/>
-      <c r="V6" s="535" t="s">
+      <c r="U6" s="540"/>
+      <c r="V6" s="538" t="s">
         <v>968</v>
       </c>
-      <c r="W6" s="536"/>
-      <c r="X6" s="536"/>
-      <c r="Y6" s="537"/>
+      <c r="W6" s="539"/>
+      <c r="X6" s="539"/>
+      <c r="Y6" s="540"/>
       <c r="Z6" s="107" t="s">
         <v>980</v>
       </c>
@@ -28327,12 +28327,12 @@
         <v>321</v>
       </c>
       <c r="U42" s="543"/>
-      <c r="V42" s="544" t="s">
+      <c r="V42" s="535" t="s">
         <v>322</v>
       </c>
-      <c r="W42" s="545"/>
-      <c r="X42" s="545"/>
-      <c r="Y42" s="546"/>
+      <c r="W42" s="536"/>
+      <c r="X42" s="536"/>
+      <c r="Y42" s="537"/>
       <c r="Z42" s="106"/>
       <c r="AA42" s="106"/>
       <c r="AB42" s="114" t="s">
@@ -28431,34 +28431,34 @@
       <c r="E44" s="84"/>
       <c r="F44" s="84"/>
       <c r="G44" s="85"/>
-      <c r="H44" s="535" t="s">
+      <c r="H44" s="538" t="s">
         <v>45</v>
       </c>
-      <c r="I44" s="536"/>
-      <c r="J44" s="536"/>
-      <c r="K44" s="537"/>
-      <c r="L44" s="536" t="s">
+      <c r="I44" s="539"/>
+      <c r="J44" s="539"/>
+      <c r="K44" s="540"/>
+      <c r="L44" s="539" t="s">
         <v>45</v>
       </c>
-      <c r="M44" s="536"/>
-      <c r="N44" s="536"/>
-      <c r="O44" s="537"/>
-      <c r="P44" s="535" t="s">
+      <c r="M44" s="539"/>
+      <c r="N44" s="539"/>
+      <c r="O44" s="540"/>
+      <c r="P44" s="538" t="s">
         <v>45</v>
       </c>
-      <c r="Q44" s="536"/>
-      <c r="R44" s="536"/>
-      <c r="S44" s="537"/>
-      <c r="T44" s="538" t="s">
+      <c r="Q44" s="539"/>
+      <c r="R44" s="539"/>
+      <c r="S44" s="540"/>
+      <c r="T44" s="544" t="s">
         <v>302</v>
       </c>
-      <c r="U44" s="539"/>
-      <c r="V44" s="538" t="s">
+      <c r="U44" s="545"/>
+      <c r="V44" s="544" t="s">
         <v>968</v>
       </c>
-      <c r="W44" s="540"/>
-      <c r="X44" s="540"/>
-      <c r="Y44" s="539"/>
+      <c r="W44" s="546"/>
+      <c r="X44" s="546"/>
+      <c r="Y44" s="545"/>
       <c r="Z44" s="450" t="s">
         <v>980</v>
       </c>
@@ -32189,12 +32189,12 @@
         <v>321</v>
       </c>
       <c r="U90" s="543"/>
-      <c r="V90" s="544" t="s">
+      <c r="V90" s="535" t="s">
         <v>322</v>
       </c>
-      <c r="W90" s="545"/>
-      <c r="X90" s="545"/>
-      <c r="Y90" s="546"/>
+      <c r="W90" s="536"/>
+      <c r="X90" s="536"/>
+      <c r="Y90" s="537"/>
       <c r="Z90" s="106"/>
       <c r="AA90" s="106"/>
       <c r="AB90" s="114" t="s">
@@ -32293,34 +32293,34 @@
       <c r="E92" s="84"/>
       <c r="F92" s="84"/>
       <c r="G92" s="85"/>
-      <c r="H92" s="535" t="s">
+      <c r="H92" s="538" t="s">
         <v>45</v>
       </c>
-      <c r="I92" s="536"/>
-      <c r="J92" s="536"/>
-      <c r="K92" s="537"/>
-      <c r="L92" s="536" t="s">
+      <c r="I92" s="539"/>
+      <c r="J92" s="539"/>
+      <c r="K92" s="540"/>
+      <c r="L92" s="539" t="s">
         <v>45</v>
       </c>
-      <c r="M92" s="536"/>
-      <c r="N92" s="536"/>
-      <c r="O92" s="537"/>
-      <c r="P92" s="535" t="s">
+      <c r="M92" s="539"/>
+      <c r="N92" s="539"/>
+      <c r="O92" s="540"/>
+      <c r="P92" s="538" t="s">
         <v>45</v>
       </c>
-      <c r="Q92" s="536"/>
-      <c r="R92" s="536"/>
-      <c r="S92" s="537"/>
-      <c r="T92" s="538" t="s">
+      <c r="Q92" s="539"/>
+      <c r="R92" s="539"/>
+      <c r="S92" s="540"/>
+      <c r="T92" s="544" t="s">
         <v>302</v>
       </c>
-      <c r="U92" s="539"/>
-      <c r="V92" s="538" t="s">
+      <c r="U92" s="545"/>
+      <c r="V92" s="544" t="s">
         <v>968</v>
       </c>
-      <c r="W92" s="540"/>
-      <c r="X92" s="540"/>
-      <c r="Y92" s="539"/>
+      <c r="W92" s="546"/>
+      <c r="X92" s="546"/>
+      <c r="Y92" s="545"/>
       <c r="Z92" s="450" t="s">
         <v>980</v>
       </c>
@@ -36191,6 +36191,26 @@
     <row r="166" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="H92:K92"/>
+    <mergeCell ref="L92:O92"/>
+    <mergeCell ref="P92:S92"/>
+    <mergeCell ref="T92:U92"/>
+    <mergeCell ref="V92:Y92"/>
+    <mergeCell ref="H90:K90"/>
+    <mergeCell ref="L90:O90"/>
+    <mergeCell ref="P90:S90"/>
+    <mergeCell ref="T90:U90"/>
+    <mergeCell ref="V90:Y90"/>
+    <mergeCell ref="H44:K44"/>
+    <mergeCell ref="L44:O44"/>
+    <mergeCell ref="P44:S44"/>
+    <mergeCell ref="T44:U44"/>
+    <mergeCell ref="V44:Y44"/>
+    <mergeCell ref="H42:K42"/>
+    <mergeCell ref="L42:O42"/>
+    <mergeCell ref="P42:S42"/>
+    <mergeCell ref="T42:U42"/>
+    <mergeCell ref="V42:Y42"/>
     <mergeCell ref="V4:Y4"/>
     <mergeCell ref="V6:Y6"/>
     <mergeCell ref="H4:K4"/>
@@ -36201,26 +36221,6 @@
     <mergeCell ref="P6:S6"/>
     <mergeCell ref="L6:O6"/>
     <mergeCell ref="H6:K6"/>
-    <mergeCell ref="H42:K42"/>
-    <mergeCell ref="L42:O42"/>
-    <mergeCell ref="P42:S42"/>
-    <mergeCell ref="T42:U42"/>
-    <mergeCell ref="V42:Y42"/>
-    <mergeCell ref="H44:K44"/>
-    <mergeCell ref="L44:O44"/>
-    <mergeCell ref="P44:S44"/>
-    <mergeCell ref="T44:U44"/>
-    <mergeCell ref="V44:Y44"/>
-    <mergeCell ref="H90:K90"/>
-    <mergeCell ref="L90:O90"/>
-    <mergeCell ref="P90:S90"/>
-    <mergeCell ref="T90:U90"/>
-    <mergeCell ref="V90:Y90"/>
-    <mergeCell ref="H92:K92"/>
-    <mergeCell ref="L92:O92"/>
-    <mergeCell ref="P92:S92"/>
-    <mergeCell ref="T92:U92"/>
-    <mergeCell ref="V92:Y92"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
@@ -36365,12 +36365,12 @@
       <c r="I5" s="173"/>
       <c r="J5" s="173"/>
       <c r="K5" s="173"/>
-      <c r="L5" s="544" t="s">
+      <c r="L5" s="535" t="s">
         <v>322</v>
       </c>
-      <c r="M5" s="545"/>
-      <c r="N5" s="545"/>
-      <c r="O5" s="546"/>
+      <c r="M5" s="536"/>
+      <c r="N5" s="536"/>
+      <c r="O5" s="537"/>
       <c r="P5" s="106"/>
       <c r="Q5" s="106" t="s">
         <v>323</v>
@@ -36401,12 +36401,12 @@
       <c r="I6" s="83"/>
       <c r="J6" s="83"/>
       <c r="K6" s="83"/>
-      <c r="L6" s="538" t="s">
+      <c r="L6" s="544" t="s">
         <v>968</v>
       </c>
-      <c r="M6" s="540"/>
-      <c r="N6" s="540"/>
-      <c r="O6" s="539"/>
+      <c r="M6" s="546"/>
+      <c r="N6" s="546"/>
+      <c r="O6" s="545"/>
       <c r="P6" s="450" t="s">
         <v>980</v>
       </c>
@@ -37324,23 +37324,23 @@
       <c r="K33" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="L33" s="544" t="s">
+      <c r="L33" s="535" t="s">
         <v>322</v>
       </c>
-      <c r="M33" s="545"/>
-      <c r="N33" s="545"/>
-      <c r="O33" s="546"/>
+      <c r="M33" s="536"/>
+      <c r="N33" s="536"/>
+      <c r="O33" s="537"/>
     </row>
     <row r="34" spans="8:15" x14ac:dyDescent="0.2">
       <c r="H34" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="L34" s="538" t="s">
+      <c r="L34" s="544" t="s">
         <v>327</v>
       </c>
-      <c r="M34" s="540"/>
-      <c r="N34" s="540"/>
-      <c r="O34" s="539"/>
+      <c r="M34" s="546"/>
+      <c r="N34" s="546"/>
+      <c r="O34" s="545"/>
     </row>
     <row r="35" spans="8:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H35" s="5" t="s">
@@ -37687,11 +37687,11 @@
       </c>
       <c r="I4" s="542"/>
       <c r="J4" s="543"/>
-      <c r="K4" s="544" t="s">
+      <c r="K4" s="535" t="s">
         <v>322</v>
       </c>
-      <c r="L4" s="545"/>
-      <c r="M4" s="546"/>
+      <c r="L4" s="536"/>
+      <c r="M4" s="537"/>
       <c r="N4" s="106"/>
       <c r="O4" s="106" t="s">
         <v>323</v>
@@ -37717,16 +37717,16 @@
       <c r="G5" s="458" t="s">
         <v>302</v>
       </c>
-      <c r="H5" s="551" t="s">
+      <c r="H5" s="548" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="552"/>
-      <c r="J5" s="553"/>
-      <c r="K5" s="551" t="s">
+      <c r="I5" s="549"/>
+      <c r="J5" s="550"/>
+      <c r="K5" s="548" t="s">
         <v>757</v>
       </c>
-      <c r="L5" s="552"/>
-      <c r="M5" s="553"/>
+      <c r="L5" s="549"/>
+      <c r="M5" s="550"/>
       <c r="N5" s="459" t="s">
         <v>328</v>
       </c>
@@ -37743,23 +37743,23 @@
         <v>626</v>
       </c>
       <c r="AA5" s="281"/>
-      <c r="AB5" s="548" t="s">
+      <c r="AB5" s="551" t="s">
         <v>1013</v>
       </c>
-      <c r="AC5" s="548"/>
+      <c r="AC5" s="551"/>
       <c r="AD5" s="461"/>
-      <c r="AE5" s="549" t="s">
+      <c r="AE5" s="552" t="s">
         <v>110</v>
       </c>
-      <c r="AF5" s="549"/>
-      <c r="AG5" s="549" t="s">
+      <c r="AF5" s="552"/>
+      <c r="AG5" s="552" t="s">
         <v>1014</v>
       </c>
-      <c r="AH5" s="549"/>
-      <c r="AI5" s="550" t="s">
+      <c r="AH5" s="552"/>
+      <c r="AI5" s="553" t="s">
         <v>1015</v>
       </c>
-      <c r="AJ5" s="550"/>
+      <c r="AJ5" s="553"/>
     </row>
     <row r="6" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C6" s="505" t="str">
@@ -38497,12 +38497,12 @@
       <c r="K27" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="L27" s="544" t="s">
+      <c r="L27" s="535" t="s">
         <v>322</v>
       </c>
-      <c r="M27" s="545"/>
-      <c r="N27" s="545"/>
-      <c r="O27" s="546"/>
+      <c r="M27" s="536"/>
+      <c r="N27" s="536"/>
+      <c r="O27" s="537"/>
       <c r="T27" s="283"/>
       <c r="U27" s="283"/>
     </row>
@@ -38510,12 +38510,12 @@
       <c r="J28" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="L28" s="535" t="s">
+      <c r="L28" s="538" t="s">
         <v>327</v>
       </c>
-      <c r="M28" s="536"/>
-      <c r="N28" s="536"/>
-      <c r="O28" s="537"/>
+      <c r="M28" s="539"/>
+      <c r="N28" s="539"/>
+      <c r="O28" s="540"/>
       <c r="T28" s="283"/>
       <c r="U28" s="283"/>
     </row>
@@ -39905,16 +39905,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="AB5:AC5"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AG5:AH5"/>
+    <mergeCell ref="AI5:AJ5"/>
+    <mergeCell ref="L27:O27"/>
     <mergeCell ref="L28:O28"/>
     <mergeCell ref="H4:J4"/>
     <mergeCell ref="K4:M4"/>
     <mergeCell ref="H5:J5"/>
     <mergeCell ref="K5:M5"/>
-    <mergeCell ref="AB5:AC5"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="AG5:AH5"/>
-    <mergeCell ref="AI5:AJ5"/>
-    <mergeCell ref="L27:O27"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="S7" r:id="rId1" xr:uid="{B1EDD63D-40A5-4174-9D28-8666BD314B83}"/>
@@ -48942,103 +48942,103 @@
       <c r="C4" s="356" t="s">
         <v>766</v>
       </c>
-      <c r="D4" s="555" t="s">
+      <c r="D4" s="554" t="s">
         <v>767</v>
       </c>
-      <c r="E4" s="554"/>
-      <c r="F4" s="554"/>
-      <c r="G4" s="554"/>
+      <c r="E4" s="555"/>
+      <c r="F4" s="555"/>
+      <c r="G4" s="555"/>
       <c r="H4" s="556"/>
-      <c r="I4" s="554" t="s">
+      <c r="I4" s="555" t="s">
         <v>768</v>
       </c>
-      <c r="J4" s="554"/>
-      <c r="K4" s="554"/>
-      <c r="L4" s="554"/>
+      <c r="J4" s="555"/>
+      <c r="K4" s="555"/>
+      <c r="L4" s="555"/>
       <c r="M4" s="556"/>
-      <c r="N4" s="554" t="s">
+      <c r="N4" s="555" t="s">
         <v>769</v>
       </c>
-      <c r="O4" s="554"/>
-      <c r="P4" s="554"/>
-      <c r="Q4" s="554"/>
+      <c r="O4" s="555"/>
+      <c r="P4" s="555"/>
+      <c r="Q4" s="555"/>
       <c r="R4" s="556"/>
-      <c r="S4" s="554" t="s">
+      <c r="S4" s="555" t="s">
         <v>770</v>
       </c>
-      <c r="T4" s="554"/>
-      <c r="U4" s="554"/>
-      <c r="V4" s="554"/>
+      <c r="T4" s="555"/>
+      <c r="U4" s="555"/>
+      <c r="V4" s="555"/>
       <c r="W4" s="556"/>
-      <c r="X4" s="554" t="s">
+      <c r="X4" s="555" t="s">
         <v>771</v>
       </c>
-      <c r="Y4" s="554"/>
-      <c r="Z4" s="554"/>
-      <c r="AA4" s="554"/>
+      <c r="Y4" s="555"/>
+      <c r="Z4" s="555"/>
+      <c r="AA4" s="555"/>
       <c r="AB4" s="556"/>
-      <c r="AC4" s="554" t="s">
+      <c r="AC4" s="555" t="s">
         <v>772</v>
       </c>
-      <c r="AD4" s="554"/>
-      <c r="AE4" s="554"/>
-      <c r="AF4" s="554"/>
+      <c r="AD4" s="555"/>
+      <c r="AE4" s="555"/>
+      <c r="AF4" s="555"/>
       <c r="AG4" s="556"/>
-      <c r="AH4" s="554" t="s">
+      <c r="AH4" s="555" t="s">
         <v>773</v>
       </c>
-      <c r="AI4" s="554"/>
-      <c r="AJ4" s="554"/>
-      <c r="AK4" s="554"/>
+      <c r="AI4" s="555"/>
+      <c r="AJ4" s="555"/>
+      <c r="AK4" s="555"/>
       <c r="AL4" s="556"/>
-      <c r="AM4" s="554" t="s">
+      <c r="AM4" s="555" t="s">
         <v>774</v>
       </c>
-      <c r="AN4" s="554"/>
-      <c r="AO4" s="554"/>
-      <c r="AP4" s="554"/>
+      <c r="AN4" s="555"/>
+      <c r="AO4" s="555"/>
+      <c r="AP4" s="555"/>
       <c r="AQ4" s="556"/>
-      <c r="AR4" s="554" t="s">
+      <c r="AR4" s="555" t="s">
         <v>775</v>
       </c>
-      <c r="AS4" s="554"/>
-      <c r="AT4" s="554"/>
-      <c r="AU4" s="554"/>
+      <c r="AS4" s="555"/>
+      <c r="AT4" s="555"/>
+      <c r="AU4" s="555"/>
       <c r="AV4" s="556"/>
-      <c r="AW4" s="554" t="s">
+      <c r="AW4" s="555" t="s">
         <v>776</v>
       </c>
-      <c r="AX4" s="554"/>
-      <c r="AY4" s="554"/>
-      <c r="AZ4" s="554"/>
-      <c r="BA4" s="554"/>
-      <c r="BB4" s="555" t="s">
+      <c r="AX4" s="555"/>
+      <c r="AY4" s="555"/>
+      <c r="AZ4" s="555"/>
+      <c r="BA4" s="555"/>
+      <c r="BB4" s="554" t="s">
         <v>777</v>
       </c>
-      <c r="BC4" s="554"/>
-      <c r="BD4" s="554"/>
-      <c r="BE4" s="554"/>
+      <c r="BC4" s="555"/>
+      <c r="BD4" s="555"/>
+      <c r="BE4" s="555"/>
       <c r="BF4" s="556"/>
-      <c r="BG4" s="554" t="s">
+      <c r="BG4" s="555" t="s">
         <v>778</v>
       </c>
-      <c r="BH4" s="554"/>
-      <c r="BI4" s="554"/>
-      <c r="BJ4" s="554"/>
-      <c r="BK4" s="554"/>
-      <c r="BL4" s="555" t="s">
+      <c r="BH4" s="555"/>
+      <c r="BI4" s="555"/>
+      <c r="BJ4" s="555"/>
+      <c r="BK4" s="555"/>
+      <c r="BL4" s="554" t="s">
         <v>779</v>
       </c>
-      <c r="BM4" s="554"/>
-      <c r="BN4" s="554"/>
-      <c r="BO4" s="554"/>
-      <c r="BP4" s="554"/>
-      <c r="BQ4" s="555" t="s">
+      <c r="BM4" s="555"/>
+      <c r="BN4" s="555"/>
+      <c r="BO4" s="555"/>
+      <c r="BP4" s="555"/>
+      <c r="BQ4" s="554" t="s">
         <v>780</v>
       </c>
-      <c r="BR4" s="554"/>
-      <c r="BS4" s="554"/>
-      <c r="BT4" s="554"/>
+      <c r="BR4" s="555"/>
+      <c r="BS4" s="555"/>
+      <c r="BT4" s="555"/>
       <c r="BU4" s="556"/>
       <c r="BV4" s="357" t="s">
         <v>781</v>
@@ -62632,11 +62632,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="BL4:BP4"/>
-    <mergeCell ref="BQ4:BU4"/>
-    <mergeCell ref="BW4:CA4"/>
-    <mergeCell ref="CB4:CF4"/>
-    <mergeCell ref="CG4:CK4"/>
     <mergeCell ref="BG4:BK4"/>
     <mergeCell ref="D4:H4"/>
     <mergeCell ref="I4:M4"/>
@@ -62649,6 +62644,11 @@
     <mergeCell ref="AR4:AV4"/>
     <mergeCell ref="AW4:BA4"/>
     <mergeCell ref="BB4:BF4"/>
+    <mergeCell ref="BL4:BP4"/>
+    <mergeCell ref="BQ4:BU4"/>
+    <mergeCell ref="BW4:CA4"/>
+    <mergeCell ref="CB4:CF4"/>
+    <mergeCell ref="CG4:CK4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
Hybrid Heat Pumps Updated
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_RSD.xlsx
+++ b/SubRES_TMPL/SubRes_RSD.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{599A8A1B-D114-4839-9AE9-A58F80079DF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C1D4CC9-E37E-4515-871F-A1DB2738DAB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{34F9D92C-266F-476D-89E0-63153305AC39}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{34F9D92C-266F-476D-89E0-63153305AC39}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="34" r:id="rId1"/>
@@ -14592,15 +14592,6 @@
     <xf numFmtId="0" fontId="53" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="23" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -14608,6 +14599,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -14619,17 +14619,26 @@
     <xf numFmtId="0" fontId="16" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="69" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="23" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -14640,19 +14649,10 @@
     <xf numFmtId="0" fontId="16" fillId="23" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="69" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="60" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="60" fillId="31" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="60" fillId="31" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -25075,8 +25075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{104F8057-C735-4662-BAA6-EEDCF7B57273}">
   <dimension ref="A2:AQ166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E72" sqref="E72"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="AC111" sqref="AC111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -25262,12 +25262,12 @@
         <v>321</v>
       </c>
       <c r="U4" s="543"/>
-      <c r="V4" s="535" t="s">
+      <c r="V4" s="544" t="s">
         <v>322</v>
       </c>
-      <c r="W4" s="536"/>
-      <c r="X4" s="536"/>
-      <c r="Y4" s="537"/>
+      <c r="W4" s="545"/>
+      <c r="X4" s="545"/>
+      <c r="Y4" s="546"/>
       <c r="Z4" s="106"/>
       <c r="AA4" s="106"/>
       <c r="AB4" s="114" t="s">
@@ -25366,34 +25366,34 @@
       <c r="E6" s="84"/>
       <c r="F6" s="84"/>
       <c r="G6" s="85"/>
-      <c r="H6" s="538" t="s">
+      <c r="H6" s="535" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="539"/>
-      <c r="J6" s="539"/>
-      <c r="K6" s="540"/>
-      <c r="L6" s="539" t="s">
+      <c r="I6" s="536"/>
+      <c r="J6" s="536"/>
+      <c r="K6" s="537"/>
+      <c r="L6" s="536" t="s">
         <v>45</v>
       </c>
-      <c r="M6" s="539"/>
-      <c r="N6" s="539"/>
-      <c r="O6" s="540"/>
-      <c r="P6" s="538" t="s">
+      <c r="M6" s="536"/>
+      <c r="N6" s="536"/>
+      <c r="O6" s="537"/>
+      <c r="P6" s="535" t="s">
         <v>45</v>
       </c>
-      <c r="Q6" s="539"/>
-      <c r="R6" s="539"/>
-      <c r="S6" s="540"/>
-      <c r="T6" s="538" t="s">
+      <c r="Q6" s="536"/>
+      <c r="R6" s="536"/>
+      <c r="S6" s="537"/>
+      <c r="T6" s="535" t="s">
         <v>302</v>
       </c>
-      <c r="U6" s="540"/>
-      <c r="V6" s="538" t="s">
+      <c r="U6" s="537"/>
+      <c r="V6" s="535" t="s">
         <v>968</v>
       </c>
-      <c r="W6" s="539"/>
-      <c r="X6" s="539"/>
-      <c r="Y6" s="540"/>
+      <c r="W6" s="536"/>
+      <c r="X6" s="536"/>
+      <c r="Y6" s="537"/>
       <c r="Z6" s="107" t="s">
         <v>980</v>
       </c>
@@ -27493,20 +27493,20 @@
       </c>
       <c r="U28" s="334"/>
       <c r="V28" s="125">
-        <f>((JRC_Data!BB18+JRC_Data!BB9*0.8)/1000)*($U$149/$U$152)</f>
-        <v>13.736326530612244</v>
+        <f>(V21+V10)*0.8</f>
+        <v>8.3046953586497896</v>
       </c>
       <c r="W28" s="125">
-        <f>((JRC_Data!BC18+JRC_Data!BC9*0.8)/1000)*($U$149/$U$152)</f>
-        <v>12.768979591836732</v>
+        <f t="shared" ref="W28:Y28" si="23">(W21+W10)*0.8</f>
+        <v>7.7598479662447266</v>
       </c>
       <c r="X28" s="125">
-        <f>((JRC_Data!BD18+JRC_Data!BD9*0.8)/1000)*($U$149/$U$152)</f>
-        <v>12.768979591836732</v>
+        <f t="shared" si="23"/>
+        <v>7.2640368391561196</v>
       </c>
       <c r="Y28" s="125">
-        <f>((JRC_Data!BE18+JRC_Data!BE9*0.8)/1000)*($U$149/$U$152)</f>
-        <v>11.801632653061223</v>
+        <f t="shared" si="23"/>
+        <v>7.2150005738396636</v>
       </c>
       <c r="Z28" s="338">
         <f>(JRC_Data!BL9+JRC_Data!BL18)*0.8/1000</f>
@@ -27684,7 +27684,7 @@
       <c r="AD30" s="131"/>
       <c r="AE30" s="131"/>
       <c r="AF30" s="131">
-        <f t="shared" ref="AF30:AF31" si="23">31.536*(AI30/1000)</f>
+        <f t="shared" ref="AF30:AF31" si="24">31.536*(AI30/1000)</f>
         <v>0.56764799999999993</v>
       </c>
       <c r="AG30" s="134"/>
@@ -27786,7 +27786,7 @@
       <c r="AD31" s="109"/>
       <c r="AE31" s="109"/>
       <c r="AF31" s="110">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0.56764799999999993</v>
       </c>
       <c r="AG31" s="113"/>
@@ -27899,7 +27899,7 @@
       <c r="AD33" s="131"/>
       <c r="AE33" s="131"/>
       <c r="AF33" s="131">
-        <f t="shared" ref="AF33:AF34" si="24">31.536*(AI33/1000)</f>
+        <f t="shared" ref="AF33:AF34" si="25">31.536*(AI33/1000)</f>
         <v>0.15768000000000001</v>
       </c>
       <c r="AG33" s="134"/>
@@ -27977,7 +27977,7 @@
       <c r="AD34" s="109"/>
       <c r="AE34" s="109"/>
       <c r="AF34" s="109">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0.15768000000000001</v>
       </c>
       <c r="AG34" s="112"/>
@@ -28093,7 +28093,7 @@
       <c r="AD36" s="131"/>
       <c r="AE36" s="131"/>
       <c r="AF36" s="131">
-        <f t="shared" ref="AF36:AF37" si="25">31.536*(AI36/1000)</f>
+        <f t="shared" ref="AF36:AF37" si="26">31.536*(AI36/1000)</f>
         <v>0.15768000000000001</v>
       </c>
       <c r="AG36" s="134"/>
@@ -28172,7 +28172,7 @@
       <c r="AD37" s="109"/>
       <c r="AE37" s="109"/>
       <c r="AF37" s="110">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.15768000000000001</v>
       </c>
       <c r="AG37" s="113"/>
@@ -28327,12 +28327,12 @@
         <v>321</v>
       </c>
       <c r="U42" s="543"/>
-      <c r="V42" s="535" t="s">
+      <c r="V42" s="544" t="s">
         <v>322</v>
       </c>
-      <c r="W42" s="536"/>
-      <c r="X42" s="536"/>
-      <c r="Y42" s="537"/>
+      <c r="W42" s="545"/>
+      <c r="X42" s="545"/>
+      <c r="Y42" s="546"/>
       <c r="Z42" s="106"/>
       <c r="AA42" s="106"/>
       <c r="AB42" s="114" t="s">
@@ -28431,34 +28431,34 @@
       <c r="E44" s="84"/>
       <c r="F44" s="84"/>
       <c r="G44" s="85"/>
-      <c r="H44" s="538" t="s">
+      <c r="H44" s="535" t="s">
         <v>45</v>
       </c>
-      <c r="I44" s="539"/>
-      <c r="J44" s="539"/>
-      <c r="K44" s="540"/>
-      <c r="L44" s="539" t="s">
+      <c r="I44" s="536"/>
+      <c r="J44" s="536"/>
+      <c r="K44" s="537"/>
+      <c r="L44" s="536" t="s">
         <v>45</v>
       </c>
-      <c r="M44" s="539"/>
-      <c r="N44" s="539"/>
-      <c r="O44" s="540"/>
-      <c r="P44" s="538" t="s">
+      <c r="M44" s="536"/>
+      <c r="N44" s="536"/>
+      <c r="O44" s="537"/>
+      <c r="P44" s="535" t="s">
         <v>45</v>
       </c>
-      <c r="Q44" s="539"/>
-      <c r="R44" s="539"/>
-      <c r="S44" s="540"/>
-      <c r="T44" s="544" t="s">
+      <c r="Q44" s="536"/>
+      <c r="R44" s="536"/>
+      <c r="S44" s="537"/>
+      <c r="T44" s="538" t="s">
         <v>302</v>
       </c>
-      <c r="U44" s="545"/>
-      <c r="V44" s="544" t="s">
+      <c r="U44" s="539"/>
+      <c r="V44" s="538" t="s">
         <v>968</v>
       </c>
-      <c r="W44" s="546"/>
-      <c r="X44" s="546"/>
-      <c r="Y44" s="545"/>
+      <c r="W44" s="540"/>
+      <c r="X44" s="540"/>
+      <c r="Y44" s="539"/>
       <c r="Z44" s="450" t="s">
         <v>980</v>
       </c>
@@ -28553,15 +28553,15 @@
         <v>4.2250000000000005</v>
       </c>
       <c r="W45" s="456">
-        <f t="shared" ref="W45:Y45" si="26">W49*1.3</f>
+        <f t="shared" ref="W45:Y45" si="27">W49*1.3</f>
         <v>4.2250000000000005</v>
       </c>
       <c r="X45" s="456">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>4.2250000000000005</v>
       </c>
       <c r="Y45" s="456">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>4.2250000000000005</v>
       </c>
       <c r="Z45" s="456">
@@ -28573,7 +28573,7 @@
       <c r="AD45" s="118"/>
       <c r="AE45" s="118"/>
       <c r="AF45" s="108">
-        <f t="shared" ref="AF45:AF83" si="27">31.536*(AI45/1000)</f>
+        <f t="shared" ref="AF45:AF83" si="28">31.536*(AI45/1000)</f>
         <v>0.63072000000000006</v>
       </c>
       <c r="AG45" s="111"/>
@@ -28587,11 +28587,11 @@
         <v>38</v>
       </c>
       <c r="AL45" s="151" t="str">
-        <f t="shared" ref="AL45:AL60" si="28">C45</f>
+        <f t="shared" ref="AL45:AL60" si="29">C45</f>
         <v>R-SH_Att_KER_N1</v>
       </c>
       <c r="AM45" s="151" t="str">
-        <f t="shared" ref="AM45:AM60" si="29">D45</f>
+        <f t="shared" ref="AM45:AM60" si="30">D45</f>
         <v>Residential Kerosene Heating Oil - New 1 SH</v>
       </c>
       <c r="AN45" s="152" t="s">
@@ -28641,15 +28641,15 @@
         <v>0.7</v>
       </c>
       <c r="Q46" s="69">
-        <f t="shared" ref="Q46:Q48" si="30">I46*0.7</f>
+        <f t="shared" ref="Q46:Q48" si="31">I46*0.7</f>
         <v>0.7</v>
       </c>
       <c r="R46" s="69">
-        <f t="shared" ref="R46:R48" si="31">J46*0.7</f>
+        <f t="shared" ref="R46:R48" si="32">J46*0.7</f>
         <v>0.7</v>
       </c>
       <c r="S46" s="103">
-        <f t="shared" ref="S46:S48" si="32">K46*0.7</f>
+        <f t="shared" ref="S46:S48" si="33">K46*0.7</f>
         <v>0.7</v>
       </c>
       <c r="T46" s="99">
@@ -28661,15 +28661,15 @@
         <v>4.2773760330578519</v>
       </c>
       <c r="W46" s="457">
-        <f t="shared" ref="W46:Y46" si="33">W50*1.3</f>
+        <f t="shared" ref="W46:Y46" si="34">W50*1.3</f>
         <v>4.2773760330578519</v>
       </c>
       <c r="X46" s="457">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>4.2773760330578519</v>
       </c>
       <c r="Y46" s="457">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>4.2773760330578519</v>
       </c>
       <c r="Z46" s="457">
@@ -28681,7 +28681,7 @@
       <c r="AD46" s="119"/>
       <c r="AE46" s="119"/>
       <c r="AF46" s="109">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.7884000000000001</v>
       </c>
       <c r="AG46" s="112"/>
@@ -28693,11 +28693,11 @@
       </c>
       <c r="AK46" s="152"/>
       <c r="AL46" s="151" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>R-SW_Att_KER_N1</v>
       </c>
       <c r="AM46" s="151" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>Residential Kerosene Heating Oil - New 2 SH + WH</v>
       </c>
       <c r="AN46" s="152" t="s">
@@ -28747,15 +28747,15 @@
         <v>0.7</v>
       </c>
       <c r="Q47" s="75">
-        <f t="shared" si="30"/>
-        <v>0.7</v>
-      </c>
-      <c r="R47" s="75">
         <f t="shared" si="31"/>
         <v>0.7</v>
       </c>
+      <c r="R47" s="75">
+        <f t="shared" si="32"/>
+        <v>0.7</v>
+      </c>
       <c r="S47" s="104">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.7</v>
       </c>
       <c r="T47" s="100">
@@ -28792,7 +28792,7 @@
         <v>5</v>
       </c>
       <c r="AF47" s="108">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.7884000000000001</v>
       </c>
       <c r="AG47" s="111"/>
@@ -28804,11 +28804,11 @@
       </c>
       <c r="AK47" s="152"/>
       <c r="AL47" s="151" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>R-SW_Att_KER_N2</v>
       </c>
       <c r="AM47" s="151" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>Residential Kerosene Heating Oil - New 3 SH+WH + Solar</v>
       </c>
       <c r="AN47" s="152" t="s">
@@ -28858,15 +28858,15 @@
         <v>0.7</v>
       </c>
       <c r="Q48" s="69">
-        <f t="shared" si="30"/>
-        <v>0.71749999999999992</v>
-      </c>
-      <c r="R48" s="69">
         <f t="shared" si="31"/>
         <v>0.71749999999999992</v>
       </c>
+      <c r="R48" s="69">
+        <f t="shared" si="32"/>
+        <v>0.71749999999999992</v>
+      </c>
       <c r="S48" s="103">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.71749999999999992</v>
       </c>
       <c r="T48" s="99">
@@ -28915,11 +28915,11 @@
       </c>
       <c r="AK48" s="152"/>
       <c r="AL48" s="151" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>R-SW_Att_KER_N3</v>
       </c>
       <c r="AM48" s="151" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>Residential Kerosene Heating Oil - New 3 SH+WH + Wood Stove</v>
       </c>
       <c r="AN48" s="153" t="s">
@@ -28975,15 +28975,15 @@
         <v>3.25</v>
       </c>
       <c r="W49" s="456">
-        <f t="shared" ref="W49:Y49" si="34">3.25</f>
+        <f t="shared" ref="W49:Y49" si="35">3.25</f>
         <v>3.25</v>
       </c>
       <c r="X49" s="456">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>3.25</v>
       </c>
       <c r="Y49" s="456">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>3.25</v>
       </c>
       <c r="Z49" s="456">
@@ -28995,7 +28995,7 @@
       <c r="AD49" s="118"/>
       <c r="AE49" s="118"/>
       <c r="AF49" s="108">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.63072000000000006</v>
       </c>
       <c r="AG49" s="111"/>
@@ -29007,11 +29007,11 @@
       </c>
       <c r="AK49" s="152"/>
       <c r="AL49" s="151" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>R-SH_Att_GAS_N1</v>
       </c>
       <c r="AM49" s="151" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>Residential Natural Gas Heating - New 1 SH</v>
       </c>
       <c r="AN49" s="152" t="s">
@@ -29061,15 +29061,15 @@
         <v>0.7</v>
       </c>
       <c r="Q50" s="69">
-        <f t="shared" ref="Q50:Q52" si="35">I50*0.7</f>
+        <f t="shared" ref="Q50:Q52" si="36">I50*0.7</f>
         <v>0.7</v>
       </c>
       <c r="R50" s="69">
-        <f t="shared" ref="R50:R52" si="36">J50*0.7</f>
+        <f t="shared" ref="R50:R52" si="37">J50*0.7</f>
         <v>0.7</v>
       </c>
       <c r="S50" s="103">
-        <f t="shared" ref="S50:S52" si="37">K50*0.7</f>
+        <f t="shared" ref="S50:S52" si="38">K50*0.7</f>
         <v>0.7</v>
       </c>
       <c r="T50" s="99">
@@ -29101,7 +29101,7 @@
       <c r="AD50" s="119"/>
       <c r="AE50" s="119"/>
       <c r="AF50" s="109">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.7884000000000001</v>
       </c>
       <c r="AG50" s="112"/>
@@ -29113,11 +29113,11 @@
       </c>
       <c r="AK50" s="152"/>
       <c r="AL50" s="151" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>R-SW_Att_GAS_N1</v>
       </c>
       <c r="AM50" s="151" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>Residential Natural Gas Heating - New 2 SH + WH</v>
       </c>
       <c r="AN50" s="152" t="s">
@@ -29167,15 +29167,15 @@
         <v>0.7</v>
       </c>
       <c r="Q51" s="75">
-        <f t="shared" si="35"/>
-        <v>0.7</v>
-      </c>
-      <c r="R51" s="75">
         <f t="shared" si="36"/>
         <v>0.7</v>
       </c>
+      <c r="R51" s="75">
+        <f t="shared" si="37"/>
+        <v>0.7</v>
+      </c>
       <c r="S51" s="104">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>0.7</v>
       </c>
       <c r="T51" s="100">
@@ -29210,7 +29210,7 @@
         <v>5</v>
       </c>
       <c r="AF51" s="108">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.7884000000000001</v>
       </c>
       <c r="AG51" s="111"/>
@@ -29222,11 +29222,11 @@
       </c>
       <c r="AK51" s="152"/>
       <c r="AL51" s="151" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>R-SW_Att_GAS_N2</v>
       </c>
       <c r="AM51" s="151" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>Residential Natural Gas Heating - New 3 SH + WH + Solar</v>
       </c>
       <c r="AN51" s="152" t="s">
@@ -29276,15 +29276,15 @@
         <v>0.7</v>
       </c>
       <c r="Q52" s="69">
-        <f t="shared" si="35"/>
-        <v>0.71749999999999992</v>
-      </c>
-      <c r="R52" s="69">
         <f t="shared" si="36"/>
         <v>0.71749999999999992</v>
       </c>
+      <c r="R52" s="69">
+        <f t="shared" si="37"/>
+        <v>0.71749999999999992</v>
+      </c>
       <c r="S52" s="103">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>0.71749999999999992</v>
       </c>
       <c r="T52" s="99">
@@ -29321,7 +29321,7 @@
         <v>5</v>
       </c>
       <c r="AF52" s="109">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.7884000000000001</v>
       </c>
       <c r="AG52" s="112"/>
@@ -29333,11 +29333,11 @@
       </c>
       <c r="AK52" s="152"/>
       <c r="AL52" s="151" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>R-SW_Att_GAS_N3</v>
       </c>
       <c r="AM52" s="151" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>Residential Natural Gas Heating - New 4 SH + WH + Wood Stove</v>
       </c>
       <c r="AN52" s="152" t="s">
@@ -29395,15 +29395,15 @@
         <v>3.5</v>
       </c>
       <c r="W53" s="456">
-        <f t="shared" ref="W53:Y53" si="38">SUM(W49+0.25)</f>
+        <f t="shared" ref="W53:Y53" si="39">SUM(W49+0.25)</f>
         <v>3.5</v>
       </c>
       <c r="X53" s="456">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>3.5</v>
       </c>
       <c r="Y53" s="456">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>3.5</v>
       </c>
       <c r="Z53" s="456">
@@ -29416,7 +29416,7 @@
       <c r="AD53" s="118"/>
       <c r="AE53" s="118"/>
       <c r="AF53" s="108">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.63072000000000006</v>
       </c>
       <c r="AG53" s="111"/>
@@ -29428,11 +29428,11 @@
       </c>
       <c r="AK53" s="152"/>
       <c r="AL53" s="151" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>R-SH_Att_LPG_N1</v>
       </c>
       <c r="AM53" s="151" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>Residential Liquid Petroleum Gas- New 1 SH</v>
       </c>
       <c r="AN53" s="152" t="s">
@@ -29482,15 +29482,15 @@
         <v>0.7</v>
       </c>
       <c r="Q54" s="69">
-        <f t="shared" ref="Q54" si="39">I54*0.7</f>
+        <f t="shared" ref="Q54" si="40">I54*0.7</f>
         <v>0.7</v>
       </c>
       <c r="R54" s="69">
-        <f t="shared" ref="R54" si="40">J54*0.7</f>
+        <f t="shared" ref="R54" si="41">J54*0.7</f>
         <v>0.7</v>
       </c>
       <c r="S54" s="103">
-        <f t="shared" ref="S54" si="41">K54*0.7</f>
+        <f t="shared" ref="S54" si="42">K54*0.7</f>
         <v>0.7</v>
       </c>
       <c r="T54" s="99">
@@ -29502,15 +29502,15 @@
         <v>3.5402892561983474</v>
       </c>
       <c r="W54" s="457">
-        <f t="shared" ref="W54:Y54" si="42">W49*($U$152/$U$151)+0.25</f>
+        <f t="shared" ref="W54:Y54" si="43">W49*($U$152/$U$151)+0.25</f>
         <v>3.5402892561983474</v>
       </c>
       <c r="X54" s="457">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>3.5402892561983474</v>
       </c>
       <c r="Y54" s="457">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>3.5402892561983474</v>
       </c>
       <c r="Z54" s="456">
@@ -29523,7 +29523,7 @@
       <c r="AD54" s="119"/>
       <c r="AE54" s="119"/>
       <c r="AF54" s="109">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.7884000000000001</v>
       </c>
       <c r="AG54" s="112"/>
@@ -29535,11 +29535,11 @@
       </c>
       <c r="AK54" s="152"/>
       <c r="AL54" s="151" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>R-SW_Att_LPG_N1</v>
       </c>
       <c r="AM54" s="151" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>Residential Liquid Petroleum Gas- New 2 SH + WH</v>
       </c>
       <c r="AN54" s="152" t="s">
@@ -29616,7 +29616,7 @@
       <c r="AD55" s="118"/>
       <c r="AE55" s="118"/>
       <c r="AF55" s="108">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.63072000000000006</v>
       </c>
       <c r="AG55" s="111"/>
@@ -29628,11 +29628,11 @@
       </c>
       <c r="AK55" s="152"/>
       <c r="AL55" s="151" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>R-SH_Att_WOO_N1</v>
       </c>
       <c r="AM55" s="151" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>Residential Biomass Boiler - New 1 SH</v>
       </c>
       <c r="AN55" s="152" t="s">
@@ -29678,19 +29678,19 @@
       <c r="N56" s="78"/>
       <c r="O56" s="91"/>
       <c r="P56" s="68">
-        <f t="shared" ref="P56:S60" si="43">H56*0.7</f>
+        <f t="shared" ref="P56:S60" si="44">H56*0.7</f>
         <v>0.7</v>
       </c>
       <c r="Q56" s="69">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>0.7</v>
       </c>
       <c r="R56" s="69">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>0.7</v>
       </c>
       <c r="S56" s="103">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>0.7</v>
       </c>
       <c r="T56" s="99">
@@ -29722,7 +29722,7 @@
       <c r="AD56" s="119"/>
       <c r="AE56" s="119"/>
       <c r="AF56" s="109">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.7884000000000001</v>
       </c>
       <c r="AG56" s="112"/>
@@ -29734,11 +29734,11 @@
       </c>
       <c r="AK56" s="155"/>
       <c r="AL56" s="154" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>R-SW_Att_WOO_N1</v>
       </c>
       <c r="AM56" s="154" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>Residential Biomass Boiler - New 2 SH + WH</v>
       </c>
       <c r="AN56" s="155" t="s">
@@ -29792,7 +29792,7 @@
       <c r="AD57" s="119"/>
       <c r="AE57" s="119"/>
       <c r="AF57" s="109">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.63072000000000006</v>
       </c>
       <c r="AG57" s="112"/>
@@ -29807,7 +29807,7 @@
         <v>1038</v>
       </c>
       <c r="AM57" s="154" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>Residential  Fireplace New 1 - SH</v>
       </c>
       <c r="AN57" s="152" t="s">
@@ -29859,7 +29859,7 @@
       <c r="AD58" s="119"/>
       <c r="AE58" s="119"/>
       <c r="AF58" s="109">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.7884000000000001</v>
       </c>
       <c r="AG58" s="112"/>
@@ -29874,7 +29874,7 @@
         <v>1040</v>
       </c>
       <c r="AM58" s="154" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>Residential  Fireplace with back boiler New 1 - SH +WH</v>
       </c>
       <c r="AN58" s="155" t="s">
@@ -29917,19 +29917,19 @@
       <c r="N59" s="77"/>
       <c r="O59" s="89"/>
       <c r="P59" s="86">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>0.7</v>
       </c>
       <c r="Q59" s="75">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>0.7</v>
       </c>
       <c r="R59" s="75">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>0.7</v>
       </c>
       <c r="S59" s="104">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>0.7</v>
       </c>
       <c r="T59" s="100">
@@ -29962,7 +29962,7 @@
       <c r="AD59" s="118"/>
       <c r="AE59" s="118"/>
       <c r="AF59" s="108">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.63072000000000006</v>
       </c>
       <c r="AG59" s="111"/>
@@ -29974,11 +29974,11 @@
       </c>
       <c r="AK59" s="155"/>
       <c r="AL59" s="154" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>*R-H_Apt_HVO_N1</v>
       </c>
       <c r="AM59" s="154" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>Residential  Hydrotreated vegetable oil - New 1 SH</v>
       </c>
       <c r="AN59" s="155" t="s">
@@ -30023,19 +30023,19 @@
       <c r="N60" s="96"/>
       <c r="O60" s="97"/>
       <c r="P60" s="329">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>0.7</v>
       </c>
       <c r="Q60" s="72">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>0.7</v>
       </c>
       <c r="R60" s="72">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>0.7</v>
       </c>
       <c r="S60" s="105">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>0.7</v>
       </c>
       <c r="T60" s="101">
@@ -30068,7 +30068,7 @@
       <c r="AD60" s="119"/>
       <c r="AE60" s="119"/>
       <c r="AF60" s="109">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.7884000000000001</v>
       </c>
       <c r="AG60" s="113"/>
@@ -30080,11 +30080,11 @@
       </c>
       <c r="AK60" s="155"/>
       <c r="AL60" s="154" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>*R-H_Apt_HVO_N2</v>
       </c>
       <c r="AM60" s="154" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>Residential  Hydrotreated vegetable oil - New 1 SH + WH</v>
       </c>
       <c r="AN60" s="155" t="s">
@@ -30219,7 +30219,7 @@
       <c r="AD62" s="130"/>
       <c r="AE62" s="130"/>
       <c r="AF62" s="128">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.63072000000000006</v>
       </c>
       <c r="AG62" s="129"/>
@@ -30231,11 +30231,11 @@
       </c>
       <c r="AK62" s="150"/>
       <c r="AL62" s="149" t="str">
-        <f t="shared" ref="AL62:AM68" si="44">C64</f>
+        <f t="shared" ref="AL62:AM68" si="45">C64</f>
         <v>R-SH_Att_ELC_HPN1</v>
       </c>
       <c r="AM62" s="149" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>Residential Electric Heat Pump - Air to Air - SH</v>
       </c>
       <c r="AN62" s="150" t="s">
@@ -30287,11 +30287,11 @@
       <c r="AI63" s="80"/>
       <c r="AK63" s="152"/>
       <c r="AL63" s="151" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>R-HC_Att_ELC_HPN1</v>
       </c>
       <c r="AM63" s="151" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>Residential Electric Heat Pump - Air to Air - SH + SC</v>
       </c>
       <c r="AN63" s="152" t="s">
@@ -30375,7 +30375,7 @@
       <c r="AD64" s="131"/>
       <c r="AE64" s="131"/>
       <c r="AF64" s="131">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.220752</v>
       </c>
       <c r="AG64" s="134"/>
@@ -30387,11 +30387,11 @@
       </c>
       <c r="AK64" s="152"/>
       <c r="AL64" s="151" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>R-SH_Att_ELC_HPN2</v>
       </c>
       <c r="AM64" s="151" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>Residential Electric Heat Pump - Air to Water - SH</v>
       </c>
       <c r="AN64" s="152" t="s">
@@ -30486,7 +30486,7 @@
       <c r="AD65" s="109"/>
       <c r="AE65" s="109"/>
       <c r="AF65" s="109">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.26805600000000002</v>
       </c>
       <c r="AG65" s="112"/>
@@ -30498,11 +30498,11 @@
       </c>
       <c r="AK65" s="152"/>
       <c r="AL65" s="151" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>R-SW_Att_ELC_HPN1</v>
       </c>
       <c r="AM65" s="151" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>Residential Electric Heat Pump - Air to Water - SH + WH</v>
       </c>
       <c r="AN65" s="152" t="s">
@@ -30584,7 +30584,7 @@
       <c r="AD66" s="108"/>
       <c r="AE66" s="108"/>
       <c r="AF66" s="108">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.220752</v>
       </c>
       <c r="AG66" s="111"/>
@@ -30596,11 +30596,11 @@
       </c>
       <c r="AK66" s="286"/>
       <c r="AL66" s="151" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>R-SW_Att_ELC_HPN2</v>
       </c>
       <c r="AM66" s="151" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>Residential Electric Heat Pump - Air to Water - SH + WH + Solar</v>
       </c>
       <c r="AN66" s="152" t="s">
@@ -30655,15 +30655,15 @@
         <v>0.7</v>
       </c>
       <c r="Q67" s="69">
-        <f t="shared" ref="Q67:Q68" si="45">I67*0.7</f>
+        <f t="shared" ref="Q67:Q68" si="46">I67*0.7</f>
         <v>0.76999999999999991</v>
       </c>
       <c r="R67" s="69">
-        <f t="shared" ref="R67:R68" si="46">J67*0.7</f>
+        <f t="shared" ref="R67:R68" si="47">J67*0.7</f>
         <v>0.86333333333333329</v>
       </c>
       <c r="S67" s="103">
-        <f t="shared" ref="S67:S68" si="47">K67*0.7</f>
+        <f t="shared" ref="S67:S68" si="48">K67*0.7</f>
         <v>0.93333333333333324</v>
       </c>
       <c r="T67" s="99">
@@ -30695,7 +30695,7 @@
       <c r="AD67" s="109"/>
       <c r="AE67" s="109"/>
       <c r="AF67" s="109">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.26805600000000002</v>
       </c>
       <c r="AG67" s="112"/>
@@ -30707,11 +30707,11 @@
       </c>
       <c r="AK67" s="286"/>
       <c r="AL67" s="151" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>R-SH_Att_ELC_HPN3</v>
       </c>
       <c r="AM67" s="151" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>Residential Electric Heat Pump - Ground to Water - SH</v>
       </c>
       <c r="AN67" s="152" t="s">
@@ -30763,15 +30763,15 @@
         <v>0.7</v>
       </c>
       <c r="Q68" s="75">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>0.77700000000000002</v>
       </c>
       <c r="R68" s="75">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>0.83299999999999996</v>
       </c>
       <c r="S68" s="104">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>0.83299999999999996</v>
       </c>
       <c r="T68" s="100">
@@ -30808,7 +30808,7 @@
         <v>5</v>
       </c>
       <c r="AF68" s="108">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.26805600000000002</v>
       </c>
       <c r="AG68" s="111"/>
@@ -30820,11 +30820,11 @@
       </c>
       <c r="AK68" s="158"/>
       <c r="AL68" s="154" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>R-HC_Att_ELC_HPN2</v>
       </c>
       <c r="AM68" s="154" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>Residential Electric Heat Pump - Ground to Water - SH + SC</v>
       </c>
       <c r="AN68" s="155" t="s">
@@ -30909,7 +30909,7 @@
       <c r="AD69" s="109"/>
       <c r="AE69" s="109"/>
       <c r="AF69" s="109">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.220752</v>
       </c>
       <c r="AG69" s="112"/>
@@ -31022,7 +31022,7 @@
       <c r="AD70" s="132"/>
       <c r="AE70" s="132"/>
       <c r="AF70" s="132">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.26805600000000002</v>
       </c>
       <c r="AG70" s="137"/>
@@ -31150,15 +31150,15 @@
         <v>1.1666666666666667</v>
       </c>
       <c r="Q72" s="66">
-        <f t="shared" ref="Q72:Q73" si="48">I72*0.7</f>
+        <f t="shared" ref="Q72:Q73" si="49">I72*0.7</f>
         <v>1.2530864197530862</v>
       </c>
       <c r="R72" s="66">
-        <f t="shared" ref="R72:R73" si="49">J72*0.7</f>
+        <f t="shared" ref="R72:R73" si="50">J72*0.7</f>
         <v>1.4691358024691357</v>
       </c>
       <c r="S72" s="102">
-        <f t="shared" ref="S72:S73" si="50">K72*0.7</f>
+        <f t="shared" ref="S72:S73" si="51">K72*0.7</f>
         <v>1.4691358024691357</v>
       </c>
       <c r="T72" s="135">
@@ -31191,7 +31191,7 @@
       <c r="AD72" s="131"/>
       <c r="AE72" s="131"/>
       <c r="AF72" s="131">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.7884000000000001</v>
       </c>
       <c r="AG72" s="134"/>
@@ -31263,15 +31263,15 @@
         <v>1.1666666666666665</v>
       </c>
       <c r="Q73" s="72">
-        <f t="shared" si="48"/>
-        <v>1.2055555555555555</v>
-      </c>
-      <c r="R73" s="72">
         <f t="shared" si="49"/>
         <v>1.2055555555555555</v>
       </c>
+      <c r="R73" s="72">
+        <f t="shared" si="50"/>
+        <v>1.2055555555555555</v>
+      </c>
       <c r="S73" s="105">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>1.2444444444444445</v>
       </c>
       <c r="T73" s="73">
@@ -31432,35 +31432,35 @@
         <v>2.2889999999999997</v>
       </c>
       <c r="Q75" s="72">
-        <f t="shared" ref="Q75" si="51">I75*0.7</f>
+        <f t="shared" ref="Q75" si="52">I75*0.7</f>
         <v>2.5409999999999995</v>
       </c>
       <c r="R75" s="72">
-        <f t="shared" ref="R75" si="52">J75*0.7</f>
+        <f t="shared" ref="R75" si="53">J75*0.7</f>
         <v>2.7299999999999995</v>
       </c>
       <c r="S75" s="105">
-        <f t="shared" ref="S75" si="53">K75*0.7</f>
+        <f t="shared" ref="S75" si="54">K75*0.7</f>
         <v>2.7299999999999995</v>
       </c>
       <c r="T75" s="5">
         <v>20</v>
       </c>
       <c r="V75" s="125">
-        <f>((JRC_Data!BB18+JRC_Data!BB9*0.8)/1000)*($U$152/$U$152)</f>
-        <v>14.2</v>
+        <f>(V67+V50)*0.8</f>
+        <v>9.5138179028489738</v>
       </c>
       <c r="W75" s="125">
-        <f>((JRC_Data!BC18+JRC_Data!BC9*0.8)/1000)*($U$152/$U$152)</f>
-        <v>13.2</v>
+        <f t="shared" ref="W75:Y75" si="55">(W67+W50)*0.8</f>
+        <v>8.8944751180388462</v>
       </c>
       <c r="X75" s="125">
-        <f>((JRC_Data!BD18+JRC_Data!BD9*0.8)/1000)*($U$152/$U$152)</f>
-        <v>13.2</v>
+        <f t="shared" si="55"/>
+        <v>8.3308731838616321</v>
       </c>
       <c r="Y75" s="125">
-        <f>((JRC_Data!BE18+JRC_Data!BE9*0.8)/1000)*($U$152/$U$152)</f>
-        <v>12.2</v>
+        <f t="shared" si="55"/>
+        <v>8.2751323332287203</v>
       </c>
       <c r="Z75" s="448">
         <f>(JRC_Data!BL9+JRC_Data!BL18)*0.8/1000</f>
@@ -31476,7 +31476,7 @@
         <v>5</v>
       </c>
       <c r="AF75" s="128">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.42415920000000001</v>
       </c>
       <c r="AG75" s="129"/>
@@ -31636,7 +31636,7 @@
       <c r="AD77" s="131"/>
       <c r="AE77" s="131"/>
       <c r="AF77" s="131">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.7884000000000001</v>
       </c>
       <c r="AG77" s="134"/>
@@ -31720,7 +31720,7 @@
       <c r="AD78" s="110"/>
       <c r="AE78" s="110"/>
       <c r="AF78" s="110">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.7884000000000001</v>
       </c>
       <c r="AG78" s="113"/>
@@ -31833,7 +31833,7 @@
       <c r="AD80" s="131"/>
       <c r="AE80" s="131"/>
       <c r="AF80" s="131">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.18921600000000002</v>
       </c>
       <c r="AG80" s="134"/>
@@ -31911,7 +31911,7 @@
       <c r="AD81" s="109"/>
       <c r="AE81" s="109"/>
       <c r="AF81" s="109">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.18921600000000002</v>
       </c>
       <c r="AG81" s="113"/>
@@ -32027,7 +32027,7 @@
       <c r="AD83" s="139"/>
       <c r="AE83" s="139"/>
       <c r="AF83" s="139">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.18921600000000002</v>
       </c>
       <c r="AG83" s="138"/>
@@ -32189,12 +32189,12 @@
         <v>321</v>
       </c>
       <c r="U90" s="543"/>
-      <c r="V90" s="535" t="s">
+      <c r="V90" s="544" t="s">
         <v>322</v>
       </c>
-      <c r="W90" s="536"/>
-      <c r="X90" s="536"/>
-      <c r="Y90" s="537"/>
+      <c r="W90" s="545"/>
+      <c r="X90" s="545"/>
+      <c r="Y90" s="546"/>
       <c r="Z90" s="106"/>
       <c r="AA90" s="106"/>
       <c r="AB90" s="114" t="s">
@@ -32293,34 +32293,34 @@
       <c r="E92" s="84"/>
       <c r="F92" s="84"/>
       <c r="G92" s="85"/>
-      <c r="H92" s="538" t="s">
+      <c r="H92" s="535" t="s">
         <v>45</v>
       </c>
-      <c r="I92" s="539"/>
-      <c r="J92" s="539"/>
-      <c r="K92" s="540"/>
-      <c r="L92" s="539" t="s">
+      <c r="I92" s="536"/>
+      <c r="J92" s="536"/>
+      <c r="K92" s="537"/>
+      <c r="L92" s="536" t="s">
         <v>45</v>
       </c>
-      <c r="M92" s="539"/>
-      <c r="N92" s="539"/>
-      <c r="O92" s="540"/>
-      <c r="P92" s="538" t="s">
+      <c r="M92" s="536"/>
+      <c r="N92" s="536"/>
+      <c r="O92" s="537"/>
+      <c r="P92" s="535" t="s">
         <v>45</v>
       </c>
-      <c r="Q92" s="539"/>
-      <c r="R92" s="539"/>
-      <c r="S92" s="540"/>
-      <c r="T92" s="544" t="s">
+      <c r="Q92" s="536"/>
+      <c r="R92" s="536"/>
+      <c r="S92" s="537"/>
+      <c r="T92" s="538" t="s">
         <v>302</v>
       </c>
-      <c r="U92" s="545"/>
-      <c r="V92" s="544" t="s">
+      <c r="U92" s="539"/>
+      <c r="V92" s="538" t="s">
         <v>968</v>
       </c>
-      <c r="W92" s="546"/>
-      <c r="X92" s="546"/>
-      <c r="Y92" s="545"/>
+      <c r="W92" s="540"/>
+      <c r="X92" s="540"/>
+      <c r="Y92" s="539"/>
       <c r="Z92" s="450" t="s">
         <v>980</v>
       </c>
@@ -32415,15 +32415,15 @@
         <v>4.5825000000000005</v>
       </c>
       <c r="W93" s="456">
-        <f t="shared" ref="W93:Y93" si="54">W97*1.3</f>
+        <f t="shared" ref="W93:Y93" si="56">W97*1.3</f>
         <v>4.5825000000000005</v>
       </c>
       <c r="X93" s="456">
-        <f t="shared" si="54"/>
+        <f t="shared" si="56"/>
         <v>4.5825000000000005</v>
       </c>
       <c r="Y93" s="456">
-        <f t="shared" si="54"/>
+        <f t="shared" si="56"/>
         <v>4.5825000000000005</v>
       </c>
       <c r="Z93" s="456">
@@ -32435,7 +32435,7 @@
       <c r="AD93" s="118"/>
       <c r="AE93" s="118"/>
       <c r="AF93" s="108">
-        <f t="shared" ref="AF93:AF131" si="55">31.536*(AI93/1000)</f>
+        <f t="shared" ref="AF93:AF131" si="57">31.536*(AI93/1000)</f>
         <v>0.94608000000000003</v>
       </c>
       <c r="AG93" s="111"/>
@@ -32503,15 +32503,15 @@
         <v>0.7</v>
       </c>
       <c r="Q94" s="69">
-        <f t="shared" ref="Q94:Q96" si="56">I94*0.7</f>
+        <f t="shared" ref="Q94:Q96" si="58">I94*0.7</f>
         <v>0.7</v>
       </c>
       <c r="R94" s="69">
-        <f t="shared" ref="R94:R96" si="57">J94*0.7</f>
+        <f t="shared" ref="R94:R96" si="59">J94*0.7</f>
         <v>0.7</v>
       </c>
       <c r="S94" s="103">
-        <f t="shared" ref="S94:S96" si="58">K94*0.7</f>
+        <f t="shared" ref="S94:S96" si="60">K94*0.7</f>
         <v>0.7</v>
       </c>
       <c r="T94" s="99">
@@ -32523,15 +32523,15 @@
         <v>4.9452075289575284</v>
       </c>
       <c r="W94" s="457">
-        <f t="shared" ref="W94:Y94" si="59">W98*1.3</f>
+        <f t="shared" ref="W94:Y94" si="61">W98*1.3</f>
         <v>4.9452075289575284</v>
       </c>
       <c r="X94" s="457">
-        <f t="shared" si="59"/>
+        <f t="shared" si="61"/>
         <v>4.9452075289575284</v>
       </c>
       <c r="Y94" s="457">
-        <f t="shared" si="59"/>
+        <f t="shared" si="61"/>
         <v>4.9452075289575284</v>
       </c>
       <c r="Z94" s="457">
@@ -32543,7 +32543,7 @@
       <c r="AD94" s="119"/>
       <c r="AE94" s="119"/>
       <c r="AF94" s="109">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AG94" s="112"/>
@@ -32555,11 +32555,11 @@
       </c>
       <c r="AK94" s="152"/>
       <c r="AL94" s="151" t="str">
-        <f t="shared" ref="AL94:AL108" si="60">C94</f>
+        <f t="shared" ref="AL94:AL108" si="62">C94</f>
         <v>R-SW_Det_KER_N1</v>
       </c>
       <c r="AM94" s="151" t="str">
-        <f t="shared" ref="AM94:AM108" si="61">D94</f>
+        <f t="shared" ref="AM94:AM108" si="63">D94</f>
         <v>Residential Kerosene Heating Oil - New 2 SH + WH</v>
       </c>
       <c r="AN94" s="152" t="s">
@@ -32609,15 +32609,15 @@
         <v>0.7</v>
       </c>
       <c r="Q95" s="75">
-        <f t="shared" si="56"/>
+        <f t="shared" si="58"/>
         <v>0.7</v>
       </c>
       <c r="R95" s="75">
-        <f t="shared" si="57"/>
+        <f t="shared" si="59"/>
         <v>0.7</v>
       </c>
       <c r="S95" s="104">
-        <f t="shared" si="58"/>
+        <f t="shared" si="60"/>
         <v>0.7</v>
       </c>
       <c r="T95" s="100">
@@ -32654,7 +32654,7 @@
         <v>5</v>
       </c>
       <c r="AF95" s="108">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AG95" s="111"/>
@@ -32666,11 +32666,11 @@
       </c>
       <c r="AK95" s="152"/>
       <c r="AL95" s="151" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="62"/>
         <v>R-SW_Det_KER_N2</v>
       </c>
       <c r="AM95" s="151" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="63"/>
         <v>Residential Kerosene Heating Oil - New 3 SH+WH + Solar</v>
       </c>
       <c r="AN95" s="152" t="s">
@@ -32720,15 +32720,15 @@
         <v>0.7</v>
       </c>
       <c r="Q96" s="69">
-        <f t="shared" si="56"/>
+        <f t="shared" si="58"/>
         <v>0.71749999999999992</v>
       </c>
       <c r="R96" s="69">
-        <f t="shared" si="57"/>
+        <f t="shared" si="59"/>
         <v>0.71749999999999992</v>
       </c>
       <c r="S96" s="103">
-        <f t="shared" si="58"/>
+        <f t="shared" si="60"/>
         <v>0.71749999999999992</v>
       </c>
       <c r="T96" s="99">
@@ -32765,7 +32765,7 @@
         <v>5</v>
       </c>
       <c r="AF96" s="109">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AG96" s="112"/>
@@ -32777,11 +32777,11 @@
       </c>
       <c r="AK96" s="152"/>
       <c r="AL96" s="151" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="62"/>
         <v>R-SW_Det_KER_N3</v>
       </c>
       <c r="AM96" s="151" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="63"/>
         <v>Residential Kerosene Heating Oil - New 3 SH+WH + Wood Stove</v>
       </c>
       <c r="AN96" s="153" t="s">
@@ -32837,15 +32837,15 @@
         <v>3.5249999999999999</v>
       </c>
       <c r="W97" s="456">
-        <f t="shared" ref="W97:Y97" si="62">3.525</f>
+        <f t="shared" ref="W97:Y97" si="64">3.525</f>
         <v>3.5249999999999999</v>
       </c>
       <c r="X97" s="456">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>3.5249999999999999</v>
       </c>
       <c r="Y97" s="456">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>3.5249999999999999</v>
       </c>
       <c r="Z97" s="456">
@@ -32857,7 +32857,7 @@
       <c r="AD97" s="118"/>
       <c r="AE97" s="118"/>
       <c r="AF97" s="108">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>0.94608000000000003</v>
       </c>
       <c r="AG97" s="111"/>
@@ -32869,11 +32869,11 @@
       </c>
       <c r="AK97" s="152"/>
       <c r="AL97" s="151" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="62"/>
         <v>R-SH_Det_GAS_N1</v>
       </c>
       <c r="AM97" s="151" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="63"/>
         <v>Residential Natural Gas Heating - New 1 SH</v>
       </c>
       <c r="AN97" s="152" t="s">
@@ -32923,15 +32923,15 @@
         <v>0.7</v>
       </c>
       <c r="Q98" s="69">
-        <f t="shared" ref="Q98:Q100" si="63">I98*0.7</f>
+        <f t="shared" ref="Q98:Q100" si="65">I98*0.7</f>
         <v>0.7</v>
       </c>
       <c r="R98" s="69">
-        <f t="shared" ref="R98:R100" si="64">J98*0.7</f>
+        <f t="shared" ref="R98:R100" si="66">J98*0.7</f>
         <v>0.7</v>
       </c>
       <c r="S98" s="103">
-        <f t="shared" ref="S98:S100" si="65">K98*0.7</f>
+        <f t="shared" ref="S98:S100" si="67">K98*0.7</f>
         <v>0.7</v>
       </c>
       <c r="T98" s="99">
@@ -32963,7 +32963,7 @@
       <c r="AD98" s="119"/>
       <c r="AE98" s="119"/>
       <c r="AF98" s="109">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AG98" s="112"/>
@@ -32975,11 +32975,11 @@
       </c>
       <c r="AK98" s="152"/>
       <c r="AL98" s="151" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="62"/>
         <v>R-SW_Det_GAS_N1</v>
       </c>
       <c r="AM98" s="151" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="63"/>
         <v>Residential Natural Gas Heating - New 2 SH + WH</v>
       </c>
       <c r="AN98" s="152" t="s">
@@ -33029,15 +33029,15 @@
         <v>0.7</v>
       </c>
       <c r="Q99" s="75">
-        <f t="shared" si="63"/>
+        <f t="shared" si="65"/>
         <v>0.7</v>
       </c>
       <c r="R99" s="75">
-        <f t="shared" si="64"/>
+        <f t="shared" si="66"/>
         <v>0.7</v>
       </c>
       <c r="S99" s="104">
-        <f t="shared" si="65"/>
+        <f t="shared" si="67"/>
         <v>0.7</v>
       </c>
       <c r="T99" s="100">
@@ -33072,7 +33072,7 @@
         <v>5</v>
       </c>
       <c r="AF99" s="108">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AG99" s="111"/>
@@ -33084,11 +33084,11 @@
       </c>
       <c r="AK99" s="152"/>
       <c r="AL99" s="151" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="62"/>
         <v>R-SW_Det_GAS_N2</v>
       </c>
       <c r="AM99" s="151" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="63"/>
         <v>Residential Natural Gas Heating - New 3 SH + WH + Solar</v>
       </c>
       <c r="AN99" s="152" t="s">
@@ -33138,15 +33138,15 @@
         <v>0.7</v>
       </c>
       <c r="Q100" s="69">
-        <f t="shared" si="63"/>
+        <f t="shared" si="65"/>
         <v>0.71749999999999992</v>
       </c>
       <c r="R100" s="69">
-        <f t="shared" si="64"/>
+        <f t="shared" si="66"/>
         <v>0.71749999999999992</v>
       </c>
       <c r="S100" s="103">
-        <f t="shared" si="65"/>
+        <f t="shared" si="67"/>
         <v>0.71749999999999992</v>
       </c>
       <c r="T100" s="99">
@@ -33183,7 +33183,7 @@
         <v>5</v>
       </c>
       <c r="AF100" s="109">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AG100" s="112"/>
@@ -33195,11 +33195,11 @@
       </c>
       <c r="AK100" s="152"/>
       <c r="AL100" s="151" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="62"/>
         <v>R-SW_Det_GAS_N3</v>
       </c>
       <c r="AM100" s="151" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="63"/>
         <v>Residential Natural Gas Heating - New 4 SH + WH + Wood Stove</v>
       </c>
       <c r="AN100" s="152" t="s">
@@ -33257,15 +33257,15 @@
         <v>3.7749999999999999</v>
       </c>
       <c r="W101" s="456">
-        <f t="shared" ref="W101:Y101" si="66">W97+0.25</f>
+        <f t="shared" ref="W101:Y101" si="68">W97+0.25</f>
         <v>3.7749999999999999</v>
       </c>
       <c r="X101" s="456">
-        <f t="shared" si="66"/>
+        <f t="shared" si="68"/>
         <v>3.7749999999999999</v>
       </c>
       <c r="Y101" s="456">
-        <f t="shared" si="66"/>
+        <f t="shared" si="68"/>
         <v>3.7749999999999999</v>
       </c>
       <c r="Z101" s="456">
@@ -33278,7 +33278,7 @@
       <c r="AD101" s="118"/>
       <c r="AE101" s="118"/>
       <c r="AF101" s="108">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>0.94608000000000003</v>
       </c>
       <c r="AG101" s="111"/>
@@ -33290,11 +33290,11 @@
       </c>
       <c r="AK101" s="152"/>
       <c r="AL101" s="151" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="62"/>
         <v>R-SH_Det_LPG_N1</v>
       </c>
       <c r="AM101" s="151" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="63"/>
         <v>Residential Liquid Petroleum Gas- New 1 SH</v>
       </c>
       <c r="AN101" s="152" t="s">
@@ -33344,15 +33344,15 @@
         <v>0.7</v>
       </c>
       <c r="Q102" s="69">
-        <f t="shared" ref="Q102" si="67">I102*0.7</f>
+        <f t="shared" ref="Q102" si="69">I102*0.7</f>
         <v>0.7</v>
       </c>
       <c r="R102" s="69">
-        <f t="shared" ref="R102" si="68">J102*0.7</f>
+        <f t="shared" ref="R102" si="70">J102*0.7</f>
         <v>0.7</v>
       </c>
       <c r="S102" s="103">
-        <f t="shared" ref="S102" si="69">K102*0.7</f>
+        <f t="shared" ref="S102" si="71">K102*0.7</f>
         <v>0.7</v>
       </c>
       <c r="T102" s="99">
@@ -33364,15 +33364,15 @@
         <v>3.8040057915057912</v>
       </c>
       <c r="W102" s="457">
-        <f t="shared" ref="W102:Y102" si="70">W98</f>
+        <f t="shared" ref="W102:Y102" si="72">W98</f>
         <v>3.8040057915057912</v>
       </c>
       <c r="X102" s="457">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>3.8040057915057912</v>
       </c>
       <c r="Y102" s="457">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>3.8040057915057912</v>
       </c>
       <c r="Z102" s="456">
@@ -33385,7 +33385,7 @@
       <c r="AD102" s="119"/>
       <c r="AE102" s="119"/>
       <c r="AF102" s="109">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AG102" s="112"/>
@@ -33397,11 +33397,11 @@
       </c>
       <c r="AK102" s="152"/>
       <c r="AL102" s="151" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="62"/>
         <v>R-SW_Det_LPG_N1</v>
       </c>
       <c r="AM102" s="151" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="63"/>
         <v>Residential Liquid Petroleum Gas- New 2 SH + WH</v>
       </c>
       <c r="AN102" s="152" t="s">
@@ -33478,7 +33478,7 @@
       <c r="AD103" s="118"/>
       <c r="AE103" s="118"/>
       <c r="AF103" s="108">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>0.94608000000000003</v>
       </c>
       <c r="AG103" s="111"/>
@@ -33490,11 +33490,11 @@
       </c>
       <c r="AK103" s="152"/>
       <c r="AL103" s="151" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="62"/>
         <v>R-SH_Det_WOO_N1</v>
       </c>
       <c r="AM103" s="151" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="63"/>
         <v>Residential Biomass Boiler - New 1 SH</v>
       </c>
       <c r="AN103" s="152" t="s">
@@ -33540,19 +33540,19 @@
       <c r="N104" s="78"/>
       <c r="O104" s="91"/>
       <c r="P104" s="68">
-        <f t="shared" ref="P104:S108" si="71">H104*0.7</f>
+        <f t="shared" ref="P104:S108" si="73">H104*0.7</f>
         <v>0.7</v>
       </c>
       <c r="Q104" s="69">
-        <f t="shared" si="71"/>
+        <f t="shared" si="73"/>
         <v>0.7</v>
       </c>
       <c r="R104" s="69">
-        <f t="shared" si="71"/>
+        <f t="shared" si="73"/>
         <v>0.7</v>
       </c>
       <c r="S104" s="103">
-        <f t="shared" si="71"/>
+        <f t="shared" si="73"/>
         <v>0.7</v>
       </c>
       <c r="T104" s="99">
@@ -33564,15 +33564,15 @@
         <v>22.778925619834713</v>
       </c>
       <c r="W104" s="457">
-        <f t="shared" ref="W104" si="72">W103*($U$152/$U$151)</f>
+        <f t="shared" ref="W104" si="74">W103*($U$152/$U$151)</f>
         <v>22.04476084710744</v>
       </c>
       <c r="X104" s="457">
-        <f t="shared" ref="X104" si="73">X103*($U$152/$U$151)</f>
+        <f t="shared" ref="X104" si="75">X103*($U$152/$U$151)</f>
         <v>20.839163429752066</v>
       </c>
       <c r="Y104" s="457">
-        <f t="shared" ref="Y104" si="74">Y103*($U$152/$U$151)</f>
+        <f t="shared" ref="Y104" si="76">Y103*($U$152/$U$151)</f>
         <v>18.635439049586779</v>
       </c>
       <c r="Z104" s="457">
@@ -33584,7 +33584,7 @@
       <c r="AD104" s="119"/>
       <c r="AE104" s="119"/>
       <c r="AF104" s="109">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AG104" s="112"/>
@@ -33596,11 +33596,11 @@
       </c>
       <c r="AK104" s="155"/>
       <c r="AL104" s="154" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="62"/>
         <v>R-SW_Det_WOO_N1</v>
       </c>
       <c r="AM104" s="154" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="63"/>
         <v>Residential Biomass Boiler - New 2 SH + WH</v>
       </c>
       <c r="AN104" s="155" t="s">
@@ -33654,7 +33654,7 @@
       <c r="AD105" s="119"/>
       <c r="AE105" s="119"/>
       <c r="AF105" s="109">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>0.94608000000000003</v>
       </c>
       <c r="AG105" s="112"/>
@@ -33669,7 +33669,7 @@
         <v>1042</v>
       </c>
       <c r="AM105" s="154" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="63"/>
         <v>Residential  Fireplace New 1 - SH</v>
       </c>
       <c r="AN105" s="152" t="s">
@@ -33721,7 +33721,7 @@
       <c r="AD106" s="119"/>
       <c r="AE106" s="119"/>
       <c r="AF106" s="109">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AG106" s="112"/>
@@ -33736,7 +33736,7 @@
         <v>1043</v>
       </c>
       <c r="AM106" s="154" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="63"/>
         <v>Residential  Fireplace with back boiler New 1 - SH +WH</v>
       </c>
       <c r="AN106" s="155" t="s">
@@ -33779,19 +33779,19 @@
       <c r="N107" s="77"/>
       <c r="O107" s="89"/>
       <c r="P107" s="86">
-        <f t="shared" si="71"/>
+        <f t="shared" si="73"/>
         <v>0.7</v>
       </c>
       <c r="Q107" s="75">
-        <f t="shared" si="71"/>
+        <f t="shared" si="73"/>
         <v>0.7</v>
       </c>
       <c r="R107" s="75">
-        <f t="shared" si="71"/>
+        <f t="shared" si="73"/>
         <v>0.7</v>
       </c>
       <c r="S107" s="104">
-        <f t="shared" si="71"/>
+        <f t="shared" si="73"/>
         <v>0.7</v>
       </c>
       <c r="T107" s="100">
@@ -33824,7 +33824,7 @@
       <c r="AD107" s="118"/>
       <c r="AE107" s="118"/>
       <c r="AF107" s="108">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>0.94608000000000003</v>
       </c>
       <c r="AG107" s="111"/>
@@ -33836,11 +33836,11 @@
       </c>
       <c r="AK107" s="155"/>
       <c r="AL107" s="154" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="62"/>
         <v>*R-H_Apt_HVO_N1</v>
       </c>
       <c r="AM107" s="154" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="63"/>
         <v>Residential  Hydrotreated vegetable oil - New 1 SH</v>
       </c>
       <c r="AN107" s="155" t="s">
@@ -33885,19 +33885,19 @@
       <c r="N108" s="96"/>
       <c r="O108" s="97"/>
       <c r="P108" s="329">
-        <f t="shared" si="71"/>
+        <f t="shared" si="73"/>
         <v>0.7</v>
       </c>
       <c r="Q108" s="72">
-        <f t="shared" si="71"/>
+        <f t="shared" si="73"/>
         <v>0.7</v>
       </c>
       <c r="R108" s="72">
-        <f t="shared" si="71"/>
+        <f t="shared" si="73"/>
         <v>0.7</v>
       </c>
       <c r="S108" s="105">
-        <f t="shared" si="71"/>
+        <f t="shared" si="73"/>
         <v>0.7</v>
       </c>
       <c r="T108" s="101">
@@ -33930,7 +33930,7 @@
       <c r="AD108" s="119"/>
       <c r="AE108" s="119"/>
       <c r="AF108" s="109">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AG108" s="113"/>
@@ -33942,11 +33942,11 @@
       </c>
       <c r="AK108" s="155"/>
       <c r="AL108" s="154" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="62"/>
         <v>*R-H_Apt_HVO_N2</v>
       </c>
       <c r="AM108" s="154" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="63"/>
         <v>Residential  Hydrotreated vegetable oil - New 1 SH + WH</v>
       </c>
       <c r="AN108" s="155" t="s">
@@ -34081,7 +34081,7 @@
       <c r="AD110" s="130"/>
       <c r="AE110" s="130"/>
       <c r="AF110" s="128">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>0.94608000000000003</v>
       </c>
       <c r="AG110" s="129"/>
@@ -34093,11 +34093,11 @@
       </c>
       <c r="AK110" s="150"/>
       <c r="AL110" s="149" t="str">
-        <f t="shared" ref="AL110:AL116" si="75">C112</f>
+        <f t="shared" ref="AL110:AL116" si="77">C112</f>
         <v>R-SH_Det_ELC_HPN1</v>
       </c>
       <c r="AM110" s="149" t="str">
-        <f t="shared" ref="AM110:AM116" si="76">D112</f>
+        <f t="shared" ref="AM110:AM116" si="78">D112</f>
         <v>Residential Electric Heat Pump - Air to Air - SH</v>
       </c>
       <c r="AN110" s="150" t="s">
@@ -34149,11 +34149,11 @@
       <c r="AI111" s="80"/>
       <c r="AK111" s="152"/>
       <c r="AL111" s="151" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="77"/>
         <v>R-HC_Det_ELC_HPN1</v>
       </c>
       <c r="AM111" s="151" t="str">
-        <f t="shared" si="76"/>
+        <f t="shared" si="78"/>
         <v>Residential Electric Heat Pump - Air to Air - SH + SC</v>
       </c>
       <c r="AN111" s="152" t="s">
@@ -34234,7 +34234,7 @@
       <c r="AD112" s="131"/>
       <c r="AE112" s="131"/>
       <c r="AF112" s="131">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>0.31536000000000003</v>
       </c>
       <c r="AG112" s="134"/>
@@ -34246,11 +34246,11 @@
       </c>
       <c r="AK112" s="152"/>
       <c r="AL112" s="151" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="77"/>
         <v>R-SH_Det_ELC_HPN2</v>
       </c>
       <c r="AM112" s="151" t="str">
-        <f t="shared" si="76"/>
+        <f t="shared" si="78"/>
         <v>Residential Electric Heat Pump - Air to Water - SH</v>
       </c>
       <c r="AN112" s="152" t="s">
@@ -34339,7 +34339,7 @@
       <c r="AD113" s="109"/>
       <c r="AE113" s="109"/>
       <c r="AF113" s="109">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>0.37843200000000005</v>
       </c>
       <c r="AG113" s="112"/>
@@ -34351,11 +34351,11 @@
       </c>
       <c r="AK113" s="152"/>
       <c r="AL113" s="151" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="77"/>
         <v>R-SW_Det_ELC_HPN1</v>
       </c>
       <c r="AM113" s="151" t="str">
-        <f t="shared" si="76"/>
+        <f t="shared" si="78"/>
         <v>Residential Electric Heat Pump - Air to Water - SH + WH</v>
       </c>
       <c r="AN113" s="152" t="s">
@@ -34434,7 +34434,7 @@
       <c r="AD114" s="108"/>
       <c r="AE114" s="108"/>
       <c r="AF114" s="108">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>0.31536000000000003</v>
       </c>
       <c r="AG114" s="111"/>
@@ -34446,11 +34446,11 @@
       </c>
       <c r="AK114" s="286"/>
       <c r="AL114" s="151" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="77"/>
         <v>R-SW_Det_ELC_HPN2</v>
       </c>
       <c r="AM114" s="151" t="str">
-        <f t="shared" si="76"/>
+        <f t="shared" si="78"/>
         <v>Residential Electric Heat Pump - Air to Water - SH + WH + Solar</v>
       </c>
       <c r="AN114" s="152" t="s">
@@ -34502,15 +34502,15 @@
         <v>0.7</v>
       </c>
       <c r="Q115" s="69">
-        <f t="shared" ref="Q115:Q116" si="77">I115*0.7</f>
+        <f t="shared" ref="Q115:Q116" si="79">I115*0.7</f>
         <v>0.76999999999999991</v>
       </c>
       <c r="R115" s="69">
-        <f t="shared" ref="R115:R116" si="78">J115*0.7</f>
+        <f t="shared" ref="R115:R116" si="80">J115*0.7</f>
         <v>0.86333333333333329</v>
       </c>
       <c r="S115" s="103">
-        <f t="shared" ref="S115:S116" si="79">K115*0.7</f>
+        <f t="shared" ref="S115:S116" si="81">K115*0.7</f>
         <v>0.93333333333333324</v>
       </c>
       <c r="T115" s="99">
@@ -34522,15 +34522,15 @@
         <v>9.9300970464135023</v>
       </c>
       <c r="W115" s="457">
-        <f t="shared" ref="W115" si="80">W114*($U$150/$U$149)</f>
+        <f t="shared" ref="W115" si="82">W114*($U$150/$U$149)</f>
         <v>9.0363883122362889</v>
       </c>
       <c r="X115" s="457">
-        <f t="shared" ref="X115" si="81">X114*($U$150/$U$149)</f>
+        <f t="shared" ref="X115" si="83">X114*($U$150/$U$149)</f>
         <v>8.2231133641350223</v>
       </c>
       <c r="Y115" s="457">
-        <f t="shared" ref="Y115" si="82">Y114*($U$150/$U$149)</f>
+        <f t="shared" ref="Y115" si="84">Y114*($U$150/$U$149)</f>
         <v>8.1426795780590719</v>
       </c>
       <c r="Z115" s="457">
@@ -34542,7 +34542,7 @@
       <c r="AD115" s="109"/>
       <c r="AE115" s="109"/>
       <c r="AF115" s="109">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>0.37843200000000005</v>
       </c>
       <c r="AG115" s="112"/>
@@ -34554,11 +34554,11 @@
       </c>
       <c r="AK115" s="286"/>
       <c r="AL115" s="151" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="77"/>
         <v>R-SH_Det_ELC_HPN3</v>
       </c>
       <c r="AM115" s="151" t="str">
-        <f t="shared" si="76"/>
+        <f t="shared" si="78"/>
         <v>Residential Electric Heat Pump - Ground to Water - SH</v>
       </c>
       <c r="AN115" s="152" t="s">
@@ -34610,15 +34610,15 @@
         <v>0.7</v>
       </c>
       <c r="Q116" s="75">
-        <f t="shared" si="77"/>
+        <f t="shared" si="79"/>
         <v>0.77700000000000002</v>
       </c>
       <c r="R116" s="75">
-        <f t="shared" si="78"/>
+        <f t="shared" si="80"/>
         <v>0.83299999999999996</v>
       </c>
       <c r="S116" s="104">
-        <f t="shared" si="79"/>
+        <f t="shared" si="81"/>
         <v>0.83299999999999996</v>
       </c>
       <c r="T116" s="100">
@@ -34655,7 +34655,7 @@
         <v>5</v>
       </c>
       <c r="AF116" s="108">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>0.37843200000000005</v>
       </c>
       <c r="AG116" s="111"/>
@@ -34667,11 +34667,11 @@
       </c>
       <c r="AK116" s="158"/>
       <c r="AL116" s="154" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="77"/>
         <v>R-HC_Det_ELC_HPN2</v>
       </c>
       <c r="AM116" s="154" t="str">
-        <f t="shared" si="76"/>
+        <f t="shared" si="78"/>
         <v>Residential Electric Heat Pump - Ground to Water - SH + SC</v>
       </c>
       <c r="AN116" s="155" t="s">
@@ -34752,7 +34752,7 @@
       <c r="AD117" s="109"/>
       <c r="AE117" s="109"/>
       <c r="AF117" s="109">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>0.31536000000000003</v>
       </c>
       <c r="AG117" s="112"/>
@@ -34857,7 +34857,7 @@
       <c r="AD118" s="132"/>
       <c r="AE118" s="132"/>
       <c r="AF118" s="132">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>0.37843200000000005</v>
       </c>
       <c r="AG118" s="137"/>
@@ -34985,15 +34985,15 @@
         <v>1.1666666666666667</v>
       </c>
       <c r="Q120" s="66">
-        <f t="shared" ref="Q120:Q121" si="83">I120*0.7</f>
+        <f t="shared" ref="Q120:Q121" si="85">I120*0.7</f>
         <v>1.2530864197530862</v>
       </c>
       <c r="R120" s="66">
-        <f t="shared" ref="R120:R121" si="84">J120*0.7</f>
+        <f t="shared" ref="R120:R121" si="86">J120*0.7</f>
         <v>1.4691358024691357</v>
       </c>
       <c r="S120" s="102">
-        <f t="shared" ref="S120:S121" si="85">K120*0.7</f>
+        <f t="shared" ref="S120:S121" si="87">K120*0.7</f>
         <v>1.4691358024691357</v>
       </c>
       <c r="T120" s="135">
@@ -35026,7 +35026,7 @@
       <c r="AD120" s="131"/>
       <c r="AE120" s="131"/>
       <c r="AF120" s="131">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AG120" s="134"/>
@@ -35098,15 +35098,15 @@
         <v>1.1666666666666665</v>
       </c>
       <c r="Q121" s="72">
-        <f t="shared" si="83"/>
+        <f t="shared" si="85"/>
         <v>1.2055555555555555</v>
       </c>
       <c r="R121" s="72">
-        <f t="shared" si="84"/>
+        <f t="shared" si="86"/>
         <v>1.2055555555555555</v>
       </c>
       <c r="S121" s="105">
-        <f t="shared" si="85"/>
+        <f t="shared" si="87"/>
         <v>1.2444444444444445</v>
       </c>
       <c r="T121" s="73">
@@ -35139,7 +35139,7 @@
       <c r="AD121" s="110"/>
       <c r="AE121" s="110"/>
       <c r="AF121" s="110">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AG121" s="113"/>
@@ -35207,11 +35207,11 @@
       <c r="AI122" s="80"/>
       <c r="AK122" s="289"/>
       <c r="AL122" s="149" t="str">
-        <f t="shared" ref="AL122:AL123" si="86">C128</f>
+        <f t="shared" ref="AL122:AL123" si="88">C128</f>
         <v>R-WH_Det_ELC_N1</v>
       </c>
       <c r="AM122" s="149" t="str">
-        <f t="shared" ref="AM122:AM123" si="87">D128</f>
+        <f t="shared" ref="AM122:AM123" si="89">D128</f>
         <v xml:space="preserve">Residential Electric Water Heater </v>
       </c>
       <c r="AN122" s="150" t="s">
@@ -35267,35 +35267,35 @@
         <v>2.2889999999999997</v>
       </c>
       <c r="Q123" s="72">
-        <f t="shared" ref="Q123" si="88">I123*0.7</f>
+        <f t="shared" ref="Q123" si="90">I123*0.7</f>
         <v>2.5409999999999995</v>
       </c>
       <c r="R123" s="72">
-        <f t="shared" ref="R123" si="89">J123*0.7</f>
+        <f t="shared" ref="R123" si="91">J123*0.7</f>
         <v>2.7299999999999995</v>
       </c>
       <c r="S123" s="105">
-        <f t="shared" ref="S123" si="90">K123*0.7</f>
+        <f t="shared" ref="S123" si="92">K123*0.7</f>
         <v>2.7299999999999995</v>
       </c>
       <c r="T123" s="5">
         <v>20</v>
       </c>
       <c r="V123" s="125">
-        <f>((JRC_Data!BB18+JRC_Data!BB9*0.8)/1000)*($U$154/$U$152)</f>
-        <v>16.19959183673469</v>
+        <f>(V115+V98)*0.8</f>
+        <v>10.987282270335434</v>
       </c>
       <c r="W123" s="125">
-        <f>((JRC_Data!BC18+JRC_Data!BC9*0.8)/1000)*($U$154/$U$152)</f>
-        <v>15.058775510204079</v>
+        <f t="shared" ref="W123:Y123" si="93">(W115+W98)*0.8</f>
+        <v>10.272315282993665</v>
       </c>
       <c r="X123" s="125">
-        <f>((JRC_Data!BD18+JRC_Data!BD9*0.8)/1000)*($U$154/$U$152)</f>
-        <v>15.058775510204079</v>
+        <f t="shared" si="93"/>
+        <v>9.6216953245126504</v>
       </c>
       <c r="Y123" s="125">
-        <f>((JRC_Data!BE18+JRC_Data!BE9*0.8)/1000)*($U$154/$U$152)</f>
-        <v>13.917959183673467</v>
+        <f t="shared" si="93"/>
+        <v>9.5573482956518898</v>
       </c>
       <c r="Z123" s="448">
         <f>(JRC_Data!BL9+JRC_Data!BL18)*0.8/1000</f>
@@ -35311,7 +35311,7 @@
         <v>5</v>
       </c>
       <c r="AF123" s="128">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>0.62441279999999999</v>
       </c>
       <c r="AG123" s="129"/>
@@ -35324,11 +35324,11 @@
       </c>
       <c r="AK123" s="4"/>
       <c r="AL123" s="151" t="str">
-        <f t="shared" si="86"/>
+        <f t="shared" si="88"/>
         <v>R-WH_Det_SOL_N1</v>
       </c>
       <c r="AM123" s="151" t="str">
-        <f t="shared" si="87"/>
+        <f t="shared" si="89"/>
         <v xml:space="preserve">Residential Solar Water Heater </v>
       </c>
       <c r="AN123" s="152" t="s">
@@ -35471,7 +35471,7 @@
       <c r="AD125" s="131"/>
       <c r="AE125" s="131"/>
       <c r="AF125" s="131">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AG125" s="134"/>
@@ -35555,7 +35555,7 @@
       <c r="AD126" s="110"/>
       <c r="AE126" s="110"/>
       <c r="AF126" s="110">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AG126" s="113"/>
@@ -35668,7 +35668,7 @@
       <c r="AD128" s="131"/>
       <c r="AE128" s="131"/>
       <c r="AF128" s="131">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>0.25228800000000001</v>
       </c>
       <c r="AG128" s="134"/>
@@ -35746,7 +35746,7 @@
       <c r="AD129" s="109"/>
       <c r="AE129" s="109"/>
       <c r="AF129" s="109">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>0.25228800000000001</v>
       </c>
       <c r="AG129" s="113"/>
@@ -35859,7 +35859,7 @@
       <c r="AD131" s="139"/>
       <c r="AE131" s="139"/>
       <c r="AF131" s="139">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>0.25228800000000001</v>
       </c>
       <c r="AG131" s="138"/>
@@ -35940,7 +35940,7 @@
         <v>3</v>
       </c>
       <c r="U145" s="454">
-        <f t="shared" ref="U145:U154" si="91">V145/$V$153</f>
+        <f t="shared" ref="U145:U154" si="94">V145/$V$153</f>
         <v>0.72929037751472525</v>
       </c>
       <c r="V145" s="455">
@@ -35954,7 +35954,7 @@
         <v>5</v>
       </c>
       <c r="U146" s="454">
-        <f t="shared" si="91"/>
+        <f t="shared" si="94"/>
         <v>0.79101166159768732</v>
       </c>
       <c r="V146" s="455">
@@ -35967,7 +35967,7 @@
         <v>8</v>
       </c>
       <c r="U147" s="454">
-        <f t="shared" si="91"/>
+        <f t="shared" si="94"/>
         <v>0.85077698714062355</v>
       </c>
       <c r="V147" s="455">
@@ -35981,7 +35981,7 @@
         <v>10</v>
       </c>
       <c r="U148" s="454">
-        <f t="shared" si="91"/>
+        <f t="shared" si="94"/>
         <v>0.86872586872586877</v>
       </c>
       <c r="V148" s="453">
@@ -36002,7 +36002,7 @@
         <v>15</v>
       </c>
       <c r="U149" s="444">
-        <f t="shared" si="91"/>
+        <f t="shared" si="94"/>
         <v>0.91505791505791501</v>
       </c>
       <c r="V149" s="5">
@@ -36029,7 +36029,7 @@
         <v>18</v>
       </c>
       <c r="U150" s="444">
-        <f t="shared" si="91"/>
+        <f t="shared" si="94"/>
         <v>0.92277992277992282</v>
       </c>
       <c r="V150" s="5">
@@ -36058,7 +36058,7 @@
         <v>20</v>
       </c>
       <c r="U151" s="454">
-        <f t="shared" si="91"/>
+        <f t="shared" si="94"/>
         <v>0.93436293436293438</v>
       </c>
       <c r="V151" s="453">
@@ -36088,7 +36088,7 @@
         <v>24</v>
       </c>
       <c r="U152" s="444">
-        <f t="shared" si="91"/>
+        <f t="shared" si="94"/>
         <v>0.94594594594594594</v>
       </c>
       <c r="V152" s="5">
@@ -36117,7 +36117,7 @@
         <v>30</v>
       </c>
       <c r="U153" s="444">
-        <f t="shared" si="91"/>
+        <f t="shared" si="94"/>
         <v>1</v>
       </c>
       <c r="V153" s="5">
@@ -36146,7 +36146,7 @@
         <v>35</v>
       </c>
       <c r="U154" s="444">
-        <f t="shared" si="91"/>
+        <f t="shared" si="94"/>
         <v>1.0791505791505791</v>
       </c>
       <c r="V154" s="5">
@@ -36191,26 +36191,6 @@
     <row r="166" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="H92:K92"/>
-    <mergeCell ref="L92:O92"/>
-    <mergeCell ref="P92:S92"/>
-    <mergeCell ref="T92:U92"/>
-    <mergeCell ref="V92:Y92"/>
-    <mergeCell ref="H90:K90"/>
-    <mergeCell ref="L90:O90"/>
-    <mergeCell ref="P90:S90"/>
-    <mergeCell ref="T90:U90"/>
-    <mergeCell ref="V90:Y90"/>
-    <mergeCell ref="H44:K44"/>
-    <mergeCell ref="L44:O44"/>
-    <mergeCell ref="P44:S44"/>
-    <mergeCell ref="T44:U44"/>
-    <mergeCell ref="V44:Y44"/>
-    <mergeCell ref="H42:K42"/>
-    <mergeCell ref="L42:O42"/>
-    <mergeCell ref="P42:S42"/>
-    <mergeCell ref="T42:U42"/>
-    <mergeCell ref="V42:Y42"/>
     <mergeCell ref="V4:Y4"/>
     <mergeCell ref="V6:Y6"/>
     <mergeCell ref="H4:K4"/>
@@ -36221,6 +36201,26 @@
     <mergeCell ref="P6:S6"/>
     <mergeCell ref="L6:O6"/>
     <mergeCell ref="H6:K6"/>
+    <mergeCell ref="H42:K42"/>
+    <mergeCell ref="L42:O42"/>
+    <mergeCell ref="P42:S42"/>
+    <mergeCell ref="T42:U42"/>
+    <mergeCell ref="V42:Y42"/>
+    <mergeCell ref="H44:K44"/>
+    <mergeCell ref="L44:O44"/>
+    <mergeCell ref="P44:S44"/>
+    <mergeCell ref="T44:U44"/>
+    <mergeCell ref="V44:Y44"/>
+    <mergeCell ref="H90:K90"/>
+    <mergeCell ref="L90:O90"/>
+    <mergeCell ref="P90:S90"/>
+    <mergeCell ref="T90:U90"/>
+    <mergeCell ref="V90:Y90"/>
+    <mergeCell ref="H92:K92"/>
+    <mergeCell ref="L92:O92"/>
+    <mergeCell ref="P92:S92"/>
+    <mergeCell ref="T92:U92"/>
+    <mergeCell ref="V92:Y92"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
@@ -36365,12 +36365,12 @@
       <c r="I5" s="173"/>
       <c r="J5" s="173"/>
       <c r="K5" s="173"/>
-      <c r="L5" s="535" t="s">
+      <c r="L5" s="544" t="s">
         <v>322</v>
       </c>
-      <c r="M5" s="536"/>
-      <c r="N5" s="536"/>
-      <c r="O5" s="537"/>
+      <c r="M5" s="545"/>
+      <c r="N5" s="545"/>
+      <c r="O5" s="546"/>
       <c r="P5" s="106"/>
       <c r="Q5" s="106" t="s">
         <v>323</v>
@@ -36401,12 +36401,12 @@
       <c r="I6" s="83"/>
       <c r="J6" s="83"/>
       <c r="K6" s="83"/>
-      <c r="L6" s="544" t="s">
+      <c r="L6" s="538" t="s">
         <v>968</v>
       </c>
-      <c r="M6" s="546"/>
-      <c r="N6" s="546"/>
-      <c r="O6" s="545"/>
+      <c r="M6" s="540"/>
+      <c r="N6" s="540"/>
+      <c r="O6" s="539"/>
       <c r="P6" s="450" t="s">
         <v>980</v>
       </c>
@@ -37324,23 +37324,23 @@
       <c r="K33" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="L33" s="535" t="s">
+      <c r="L33" s="544" t="s">
         <v>322</v>
       </c>
-      <c r="M33" s="536"/>
-      <c r="N33" s="536"/>
-      <c r="O33" s="537"/>
+      <c r="M33" s="545"/>
+      <c r="N33" s="545"/>
+      <c r="O33" s="546"/>
     </row>
     <row r="34" spans="8:15" x14ac:dyDescent="0.2">
       <c r="H34" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="L34" s="544" t="s">
+      <c r="L34" s="538" t="s">
         <v>327</v>
       </c>
-      <c r="M34" s="546"/>
-      <c r="N34" s="546"/>
-      <c r="O34" s="545"/>
+      <c r="M34" s="540"/>
+      <c r="N34" s="540"/>
+      <c r="O34" s="539"/>
     </row>
     <row r="35" spans="8:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H35" s="5" t="s">
@@ -37687,11 +37687,11 @@
       </c>
       <c r="I4" s="542"/>
       <c r="J4" s="543"/>
-      <c r="K4" s="535" t="s">
+      <c r="K4" s="544" t="s">
         <v>322</v>
       </c>
-      <c r="L4" s="536"/>
-      <c r="M4" s="537"/>
+      <c r="L4" s="545"/>
+      <c r="M4" s="546"/>
       <c r="N4" s="106"/>
       <c r="O4" s="106" t="s">
         <v>323</v>
@@ -37717,16 +37717,16 @@
       <c r="G5" s="458" t="s">
         <v>302</v>
       </c>
-      <c r="H5" s="548" t="s">
+      <c r="H5" s="551" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="549"/>
-      <c r="J5" s="550"/>
-      <c r="K5" s="548" t="s">
+      <c r="I5" s="552"/>
+      <c r="J5" s="553"/>
+      <c r="K5" s="551" t="s">
         <v>757</v>
       </c>
-      <c r="L5" s="549"/>
-      <c r="M5" s="550"/>
+      <c r="L5" s="552"/>
+      <c r="M5" s="553"/>
       <c r="N5" s="459" t="s">
         <v>328</v>
       </c>
@@ -37743,23 +37743,23 @@
         <v>626</v>
       </c>
       <c r="AA5" s="281"/>
-      <c r="AB5" s="551" t="s">
+      <c r="AB5" s="548" t="s">
         <v>1013</v>
       </c>
-      <c r="AC5" s="551"/>
+      <c r="AC5" s="548"/>
       <c r="AD5" s="461"/>
-      <c r="AE5" s="552" t="s">
+      <c r="AE5" s="549" t="s">
         <v>110</v>
       </c>
-      <c r="AF5" s="552"/>
-      <c r="AG5" s="552" t="s">
+      <c r="AF5" s="549"/>
+      <c r="AG5" s="549" t="s">
         <v>1014</v>
       </c>
-      <c r="AH5" s="552"/>
-      <c r="AI5" s="553" t="s">
+      <c r="AH5" s="549"/>
+      <c r="AI5" s="550" t="s">
         <v>1015</v>
       </c>
-      <c r="AJ5" s="553"/>
+      <c r="AJ5" s="550"/>
     </row>
     <row r="6" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C6" s="505" t="str">
@@ -38497,12 +38497,12 @@
       <c r="K27" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="L27" s="535" t="s">
+      <c r="L27" s="544" t="s">
         <v>322</v>
       </c>
-      <c r="M27" s="536"/>
-      <c r="N27" s="536"/>
-      <c r="O27" s="537"/>
+      <c r="M27" s="545"/>
+      <c r="N27" s="545"/>
+      <c r="O27" s="546"/>
       <c r="T27" s="283"/>
       <c r="U27" s="283"/>
     </row>
@@ -38510,12 +38510,12 @@
       <c r="J28" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="L28" s="538" t="s">
+      <c r="L28" s="535" t="s">
         <v>327</v>
       </c>
-      <c r="M28" s="539"/>
-      <c r="N28" s="539"/>
-      <c r="O28" s="540"/>
+      <c r="M28" s="536"/>
+      <c r="N28" s="536"/>
+      <c r="O28" s="537"/>
       <c r="T28" s="283"/>
       <c r="U28" s="283"/>
     </row>
@@ -39905,16 +39905,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="L28:O28"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="K5:M5"/>
     <mergeCell ref="AB5:AC5"/>
     <mergeCell ref="AE5:AF5"/>
     <mergeCell ref="AG5:AH5"/>
     <mergeCell ref="AI5:AJ5"/>
     <mergeCell ref="L27:O27"/>
-    <mergeCell ref="L28:O28"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="K5:M5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="S7" r:id="rId1" xr:uid="{B1EDD63D-40A5-4174-9D28-8666BD314B83}"/>
@@ -48942,103 +48942,103 @@
       <c r="C4" s="356" t="s">
         <v>766</v>
       </c>
-      <c r="D4" s="554" t="s">
+      <c r="D4" s="555" t="s">
         <v>767</v>
       </c>
-      <c r="E4" s="555"/>
-      <c r="F4" s="555"/>
-      <c r="G4" s="555"/>
+      <c r="E4" s="554"/>
+      <c r="F4" s="554"/>
+      <c r="G4" s="554"/>
       <c r="H4" s="556"/>
-      <c r="I4" s="555" t="s">
+      <c r="I4" s="554" t="s">
         <v>768</v>
       </c>
-      <c r="J4" s="555"/>
-      <c r="K4" s="555"/>
-      <c r="L4" s="555"/>
+      <c r="J4" s="554"/>
+      <c r="K4" s="554"/>
+      <c r="L4" s="554"/>
       <c r="M4" s="556"/>
-      <c r="N4" s="555" t="s">
+      <c r="N4" s="554" t="s">
         <v>769</v>
       </c>
-      <c r="O4" s="555"/>
-      <c r="P4" s="555"/>
-      <c r="Q4" s="555"/>
+      <c r="O4" s="554"/>
+      <c r="P4" s="554"/>
+      <c r="Q4" s="554"/>
       <c r="R4" s="556"/>
-      <c r="S4" s="555" t="s">
+      <c r="S4" s="554" t="s">
         <v>770</v>
       </c>
-      <c r="T4" s="555"/>
-      <c r="U4" s="555"/>
-      <c r="V4" s="555"/>
+      <c r="T4" s="554"/>
+      <c r="U4" s="554"/>
+      <c r="V4" s="554"/>
       <c r="W4" s="556"/>
-      <c r="X4" s="555" t="s">
+      <c r="X4" s="554" t="s">
         <v>771</v>
       </c>
-      <c r="Y4" s="555"/>
-      <c r="Z4" s="555"/>
-      <c r="AA4" s="555"/>
+      <c r="Y4" s="554"/>
+      <c r="Z4" s="554"/>
+      <c r="AA4" s="554"/>
       <c r="AB4" s="556"/>
-      <c r="AC4" s="555" t="s">
+      <c r="AC4" s="554" t="s">
         <v>772</v>
       </c>
-      <c r="AD4" s="555"/>
-      <c r="AE4" s="555"/>
-      <c r="AF4" s="555"/>
+      <c r="AD4" s="554"/>
+      <c r="AE4" s="554"/>
+      <c r="AF4" s="554"/>
       <c r="AG4" s="556"/>
-      <c r="AH4" s="555" t="s">
+      <c r="AH4" s="554" t="s">
         <v>773</v>
       </c>
-      <c r="AI4" s="555"/>
-      <c r="AJ4" s="555"/>
-      <c r="AK4" s="555"/>
+      <c r="AI4" s="554"/>
+      <c r="AJ4" s="554"/>
+      <c r="AK4" s="554"/>
       <c r="AL4" s="556"/>
-      <c r="AM4" s="555" t="s">
+      <c r="AM4" s="554" t="s">
         <v>774</v>
       </c>
-      <c r="AN4" s="555"/>
-      <c r="AO4" s="555"/>
-      <c r="AP4" s="555"/>
+      <c r="AN4" s="554"/>
+      <c r="AO4" s="554"/>
+      <c r="AP4" s="554"/>
       <c r="AQ4" s="556"/>
-      <c r="AR4" s="555" t="s">
+      <c r="AR4" s="554" t="s">
         <v>775</v>
       </c>
-      <c r="AS4" s="555"/>
-      <c r="AT4" s="555"/>
-      <c r="AU4" s="555"/>
+      <c r="AS4" s="554"/>
+      <c r="AT4" s="554"/>
+      <c r="AU4" s="554"/>
       <c r="AV4" s="556"/>
-      <c r="AW4" s="555" t="s">
+      <c r="AW4" s="554" t="s">
         <v>776</v>
       </c>
-      <c r="AX4" s="555"/>
-      <c r="AY4" s="555"/>
-      <c r="AZ4" s="555"/>
-      <c r="BA4" s="555"/>
-      <c r="BB4" s="554" t="s">
+      <c r="AX4" s="554"/>
+      <c r="AY4" s="554"/>
+      <c r="AZ4" s="554"/>
+      <c r="BA4" s="554"/>
+      <c r="BB4" s="555" t="s">
         <v>777</v>
       </c>
-      <c r="BC4" s="555"/>
-      <c r="BD4" s="555"/>
-      <c r="BE4" s="555"/>
+      <c r="BC4" s="554"/>
+      <c r="BD4" s="554"/>
+      <c r="BE4" s="554"/>
       <c r="BF4" s="556"/>
-      <c r="BG4" s="555" t="s">
+      <c r="BG4" s="554" t="s">
         <v>778</v>
       </c>
-      <c r="BH4" s="555"/>
-      <c r="BI4" s="555"/>
-      <c r="BJ4" s="555"/>
-      <c r="BK4" s="555"/>
-      <c r="BL4" s="554" t="s">
+      <c r="BH4" s="554"/>
+      <c r="BI4" s="554"/>
+      <c r="BJ4" s="554"/>
+      <c r="BK4" s="554"/>
+      <c r="BL4" s="555" t="s">
         <v>779</v>
       </c>
-      <c r="BM4" s="555"/>
-      <c r="BN4" s="555"/>
-      <c r="BO4" s="555"/>
-      <c r="BP4" s="555"/>
-      <c r="BQ4" s="554" t="s">
+      <c r="BM4" s="554"/>
+      <c r="BN4" s="554"/>
+      <c r="BO4" s="554"/>
+      <c r="BP4" s="554"/>
+      <c r="BQ4" s="555" t="s">
         <v>780</v>
       </c>
-      <c r="BR4" s="555"/>
-      <c r="BS4" s="555"/>
-      <c r="BT4" s="555"/>
+      <c r="BR4" s="554"/>
+      <c r="BS4" s="554"/>
+      <c r="BT4" s="554"/>
       <c r="BU4" s="556"/>
       <c r="BV4" s="357" t="s">
         <v>781</v>
@@ -62632,6 +62632,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="BL4:BP4"/>
+    <mergeCell ref="BQ4:BU4"/>
+    <mergeCell ref="BW4:CA4"/>
+    <mergeCell ref="CB4:CF4"/>
+    <mergeCell ref="CG4:CK4"/>
     <mergeCell ref="BG4:BK4"/>
     <mergeCell ref="D4:H4"/>
     <mergeCell ref="I4:M4"/>
@@ -62644,11 +62649,6 @@
     <mergeCell ref="AR4:AV4"/>
     <mergeCell ref="AW4:BA4"/>
     <mergeCell ref="BB4:BF4"/>
-    <mergeCell ref="BL4:BP4"/>
-    <mergeCell ref="BQ4:BU4"/>
-    <mergeCell ref="BW4:CA4"/>
-    <mergeCell ref="CB4:CF4"/>
-    <mergeCell ref="CG4:CK4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
Max Non-HP Elec changed
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_RSD.xlsx
+++ b/SubRES_TMPL/SubRes_RSD.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C1D4CC9-E37E-4515-871F-A1DB2738DAB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8CDF414-CF6D-4549-8C2B-E8744EB008A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{34F9D92C-266F-476D-89E0-63153305AC39}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{34F9D92C-266F-476D-89E0-63153305AC39}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="34" r:id="rId1"/>
@@ -25075,8 +25075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{104F8057-C735-4662-BAA6-EEDCF7B57273}">
   <dimension ref="A2:AQ166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="AC111" sqref="AC111"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:XFD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -27207,7 +27207,7 @@
         <v>1.4691358024691357</v>
       </c>
       <c r="T25" s="135">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="U25" s="94"/>
       <c r="V25" s="65">
@@ -31162,7 +31162,7 @@
         <v>1.4691358024691357</v>
       </c>
       <c r="T72" s="135">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="U72" s="94"/>
       <c r="V72" s="65">
@@ -34997,7 +34997,7 @@
         <v>1.4691358024691357</v>
       </c>
       <c r="T120" s="135">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="U120" s="94"/>
       <c r="V120" s="65">

</xml_diff>

<commit_message>
Stove Efficiency update and Biodiesel growth contraint added
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_RSD.xlsx
+++ b/SubRES_TMPL/SubRes_RSD.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA12166B-9502-44A3-A81B-064EF53FB0C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B21491C8-F697-4397-B64A-3C01E4A5F9E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{34F9D92C-266F-476D-89E0-63153305AC39}"/>
   </bookViews>
@@ -11797,12 +11797,6 @@
     <t>R-SW_Att_FPL_N1</t>
   </si>
   <si>
-    <t>*R-SH_Det_FPL_N1</t>
-  </si>
-  <si>
-    <t>*R-SW_Det_FPL_N1</t>
-  </si>
-  <si>
     <t>Lights</t>
   </si>
   <si>
@@ -11825,6 +11819,12 @@
   </si>
   <si>
     <t>R-SW_Det_HVO_N1</t>
+  </si>
+  <si>
+    <t>R-SH_Det_FPL_N1</t>
+  </si>
+  <si>
+    <t>R-SW_Det_FPL_N1</t>
   </si>
 </sst>
 </file>
@@ -13550,7 +13550,7 @@
     <xf numFmtId="0" fontId="39" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="54" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="560">
+  <cellXfs count="561">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -14598,15 +14598,6 @@
     <xf numFmtId="0" fontId="53" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="23" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -14614,6 +14605,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -14625,17 +14625,26 @@
     <xf numFmtId="0" fontId="16" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="69" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="23" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -14646,19 +14655,10 @@
     <xf numFmtId="0" fontId="16" fillId="23" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="69" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="60" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="60" fillId="31" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="60" fillId="31" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -14673,6 +14673,7 @@
     <xf numFmtId="0" fontId="60" fillId="32" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="20% - Colore 2" xfId="11" xr:uid="{3E3DAF22-4D86-48A9-B6EE-8D230C1E993C}"/>
@@ -17613,7 +17614,7 @@
       </c>
       <c r="J10" s="141"/>
       <c r="M10" s="291" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
       <c r="N10" s="292">
         <v>0.4</v>
@@ -17650,7 +17651,7 @@
         <v>330</v>
       </c>
       <c r="M11" s="294" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
       <c r="N11" s="295">
         <v>0.6</v>
@@ -25081,8 +25082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{104F8057-C735-4662-BAA6-EEDCF7B57273}">
   <dimension ref="A2:AQ166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C69" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="V106" sqref="V106:Y106"/>
+    <sheetView tabSelected="1" topLeftCell="K67" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="AL105" sqref="AL105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -25268,12 +25269,12 @@
         <v>321</v>
       </c>
       <c r="U4" s="543"/>
-      <c r="V4" s="535" t="s">
+      <c r="V4" s="544" t="s">
         <v>322</v>
       </c>
-      <c r="W4" s="536"/>
-      <c r="X4" s="536"/>
-      <c r="Y4" s="537"/>
+      <c r="W4" s="545"/>
+      <c r="X4" s="545"/>
+      <c r="Y4" s="546"/>
       <c r="Z4" s="106"/>
       <c r="AA4" s="106"/>
       <c r="AB4" s="114" t="s">
@@ -25372,34 +25373,34 @@
       <c r="E6" s="84"/>
       <c r="F6" s="84"/>
       <c r="G6" s="85"/>
-      <c r="H6" s="538" t="s">
+      <c r="H6" s="535" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="539"/>
-      <c r="J6" s="539"/>
-      <c r="K6" s="540"/>
-      <c r="L6" s="539" t="s">
+      <c r="I6" s="536"/>
+      <c r="J6" s="536"/>
+      <c r="K6" s="537"/>
+      <c r="L6" s="536" t="s">
         <v>45</v>
       </c>
-      <c r="M6" s="539"/>
-      <c r="N6" s="539"/>
-      <c r="O6" s="540"/>
-      <c r="P6" s="538" t="s">
+      <c r="M6" s="536"/>
+      <c r="N6" s="536"/>
+      <c r="O6" s="537"/>
+      <c r="P6" s="535" t="s">
         <v>45</v>
       </c>
-      <c r="Q6" s="539"/>
-      <c r="R6" s="539"/>
-      <c r="S6" s="540"/>
-      <c r="T6" s="538" t="s">
+      <c r="Q6" s="536"/>
+      <c r="R6" s="536"/>
+      <c r="S6" s="537"/>
+      <c r="T6" s="535" t="s">
         <v>302</v>
       </c>
-      <c r="U6" s="540"/>
-      <c r="V6" s="538" t="s">
+      <c r="U6" s="537"/>
+      <c r="V6" s="535" t="s">
         <v>967</v>
       </c>
-      <c r="W6" s="539"/>
-      <c r="X6" s="539"/>
-      <c r="Y6" s="540"/>
+      <c r="W6" s="536"/>
+      <c r="X6" s="536"/>
+      <c r="Y6" s="537"/>
       <c r="Z6" s="107" t="s">
         <v>979</v>
       </c>
@@ -28333,12 +28334,12 @@
         <v>321</v>
       </c>
       <c r="U42" s="543"/>
-      <c r="V42" s="535" t="s">
+      <c r="V42" s="544" t="s">
         <v>322</v>
       </c>
-      <c r="W42" s="536"/>
-      <c r="X42" s="536"/>
-      <c r="Y42" s="537"/>
+      <c r="W42" s="545"/>
+      <c r="X42" s="545"/>
+      <c r="Y42" s="546"/>
       <c r="Z42" s="106"/>
       <c r="AA42" s="106"/>
       <c r="AB42" s="114" t="s">
@@ -28437,34 +28438,34 @@
       <c r="E44" s="84"/>
       <c r="F44" s="84"/>
       <c r="G44" s="85"/>
-      <c r="H44" s="538" t="s">
+      <c r="H44" s="535" t="s">
         <v>45</v>
       </c>
-      <c r="I44" s="539"/>
-      <c r="J44" s="539"/>
-      <c r="K44" s="540"/>
-      <c r="L44" s="539" t="s">
+      <c r="I44" s="536"/>
+      <c r="J44" s="536"/>
+      <c r="K44" s="537"/>
+      <c r="L44" s="536" t="s">
         <v>45</v>
       </c>
-      <c r="M44" s="539"/>
-      <c r="N44" s="539"/>
-      <c r="O44" s="540"/>
-      <c r="P44" s="538" t="s">
+      <c r="M44" s="536"/>
+      <c r="N44" s="536"/>
+      <c r="O44" s="537"/>
+      <c r="P44" s="535" t="s">
         <v>45</v>
       </c>
-      <c r="Q44" s="539"/>
-      <c r="R44" s="539"/>
-      <c r="S44" s="540"/>
-      <c r="T44" s="544" t="s">
+      <c r="Q44" s="536"/>
+      <c r="R44" s="536"/>
+      <c r="S44" s="537"/>
+      <c r="T44" s="538" t="s">
         <v>302</v>
       </c>
-      <c r="U44" s="545"/>
-      <c r="V44" s="544" t="s">
+      <c r="U44" s="539"/>
+      <c r="V44" s="538" t="s">
         <v>967</v>
       </c>
-      <c r="W44" s="546"/>
-      <c r="X44" s="546"/>
-      <c r="Y44" s="545"/>
+      <c r="W44" s="540"/>
+      <c r="X44" s="540"/>
+      <c r="Y44" s="539"/>
       <c r="Z44" s="450" t="s">
         <v>979</v>
       </c>
@@ -29764,7 +29765,7 @@
         <v>R-SH_Att_FPL_N1</v>
       </c>
       <c r="D57" s="75" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="E57" s="76" t="s">
         <v>1035</v>
@@ -29774,16 +29775,20 @@
         <v>392</v>
       </c>
       <c r="H57" s="86">
-        <v>1</v>
-      </c>
-      <c r="I57" s="75">
-        <v>1</v>
-      </c>
-      <c r="J57" s="75">
-        <v>1</v>
-      </c>
-      <c r="K57" s="104">
-        <v>1</v>
+        <f>JRC_Data!AD13</f>
+        <v>0.7</v>
+      </c>
+      <c r="I57" s="86">
+        <f>JRC_Data!AE13</f>
+        <v>0.75</v>
+      </c>
+      <c r="J57" s="86">
+        <f>JRC_Data!AF13</f>
+        <v>0.75</v>
+      </c>
+      <c r="K57" s="86">
+        <f>JRC_Data!AG13</f>
+        <v>0.75</v>
       </c>
       <c r="L57" s="90"/>
       <c r="M57" s="78"/>
@@ -29855,7 +29860,7 @@
         <v>R-SW_Att_FPL_N1</v>
       </c>
       <c r="D58" s="69" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
       <c r="E58" s="70" t="s">
         <v>1035</v>
@@ -29865,16 +29870,20 @@
         <v>715</v>
       </c>
       <c r="H58" s="68">
-        <v>1</v>
-      </c>
-      <c r="I58" s="69">
-        <v>1</v>
-      </c>
-      <c r="J58" s="69">
-        <v>1</v>
-      </c>
-      <c r="K58" s="103">
-        <v>1</v>
+        <f>JRC_Data!AD13</f>
+        <v>0.7</v>
+      </c>
+      <c r="I58" s="68">
+        <f>JRC_Data!AE13</f>
+        <v>0.75</v>
+      </c>
+      <c r="J58" s="68">
+        <f>JRC_Data!AF13</f>
+        <v>0.75</v>
+      </c>
+      <c r="K58" s="68">
+        <f>JRC_Data!AG13</f>
+        <v>0.75</v>
       </c>
       <c r="L58" s="90"/>
       <c r="M58" s="78"/>
@@ -29882,19 +29891,19 @@
       <c r="O58" s="91"/>
       <c r="P58" s="68">
         <f t="shared" ref="P58" si="45">H58*0.7</f>
-        <v>0.7</v>
+        <v>0.48999999999999994</v>
       </c>
       <c r="Q58" s="69">
         <f t="shared" ref="Q58" si="46">I58*0.7</f>
-        <v>0.7</v>
+        <v>0.52499999999999991</v>
       </c>
       <c r="R58" s="69">
         <f t="shared" ref="R58" si="47">J58*0.7</f>
-        <v>0.7</v>
+        <v>0.52499999999999991</v>
       </c>
       <c r="S58" s="103">
         <f t="shared" ref="S58" si="48">K58*0.7</f>
-        <v>0.7</v>
+        <v>0.52499999999999991</v>
       </c>
       <c r="T58" s="99">
         <v>20</v>
@@ -29954,7 +29963,7 @@
     </row>
     <row r="59" spans="3:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C59" s="86" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
       <c r="D59" s="75" t="s">
         <v>698</v>
@@ -30060,7 +30069,7 @@
     </row>
     <row r="60" spans="3:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C60" s="68" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
       <c r="D60" s="69" t="s">
         <v>990</v>
@@ -32255,12 +32264,12 @@
         <v>321</v>
       </c>
       <c r="U90" s="543"/>
-      <c r="V90" s="535" t="s">
+      <c r="V90" s="544" t="s">
         <v>322</v>
       </c>
-      <c r="W90" s="536"/>
-      <c r="X90" s="536"/>
-      <c r="Y90" s="537"/>
+      <c r="W90" s="545"/>
+      <c r="X90" s="545"/>
+      <c r="Y90" s="546"/>
       <c r="Z90" s="106"/>
       <c r="AA90" s="106"/>
       <c r="AB90" s="114" t="s">
@@ -32359,34 +32368,34 @@
       <c r="E92" s="84"/>
       <c r="F92" s="84"/>
       <c r="G92" s="85"/>
-      <c r="H92" s="538" t="s">
+      <c r="H92" s="535" t="s">
         <v>45</v>
       </c>
-      <c r="I92" s="539"/>
-      <c r="J92" s="539"/>
-      <c r="K92" s="540"/>
-      <c r="L92" s="539" t="s">
+      <c r="I92" s="536"/>
+      <c r="J92" s="536"/>
+      <c r="K92" s="537"/>
+      <c r="L92" s="536" t="s">
         <v>45</v>
       </c>
-      <c r="M92" s="539"/>
-      <c r="N92" s="539"/>
-      <c r="O92" s="540"/>
-      <c r="P92" s="538" t="s">
+      <c r="M92" s="536"/>
+      <c r="N92" s="536"/>
+      <c r="O92" s="537"/>
+      <c r="P92" s="535" t="s">
         <v>45</v>
       </c>
-      <c r="Q92" s="539"/>
-      <c r="R92" s="539"/>
-      <c r="S92" s="540"/>
-      <c r="T92" s="544" t="s">
+      <c r="Q92" s="536"/>
+      <c r="R92" s="536"/>
+      <c r="S92" s="537"/>
+      <c r="T92" s="538" t="s">
         <v>302</v>
       </c>
-      <c r="U92" s="545"/>
-      <c r="V92" s="544" t="s">
+      <c r="U92" s="539"/>
+      <c r="V92" s="538" t="s">
         <v>967</v>
       </c>
-      <c r="W92" s="546"/>
-      <c r="X92" s="546"/>
-      <c r="Y92" s="545"/>
+      <c r="W92" s="540"/>
+      <c r="X92" s="540"/>
+      <c r="Y92" s="539"/>
       <c r="Z92" s="450" t="s">
         <v>979</v>
       </c>
@@ -33606,7 +33615,7 @@
       <c r="N104" s="78"/>
       <c r="O104" s="91"/>
       <c r="P104" s="68">
-        <f t="shared" ref="P104:S108" si="79">H104*0.7</f>
+        <f t="shared" ref="P104:S104" si="79">H104*0.7</f>
         <v>0.7</v>
       </c>
       <c r="Q104" s="69">
@@ -33686,7 +33695,7 @@
         <v>R-SH_Det_FPL_N1</v>
       </c>
       <c r="D105" s="75" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="E105" s="76" t="s">
         <v>1035</v>
@@ -33696,16 +33705,20 @@
         <v>400</v>
       </c>
       <c r="H105" s="86">
-        <v>1</v>
-      </c>
-      <c r="I105" s="75">
-        <v>1</v>
-      </c>
-      <c r="J105" s="75">
-        <v>1</v>
-      </c>
-      <c r="K105" s="104">
-        <v>1</v>
+        <f>JRC_Data!AD13</f>
+        <v>0.7</v>
+      </c>
+      <c r="I105" s="86">
+        <f>JRC_Data!AE13</f>
+        <v>0.75</v>
+      </c>
+      <c r="J105" s="86">
+        <f>JRC_Data!AF13</f>
+        <v>0.75</v>
+      </c>
+      <c r="K105" s="86">
+        <f>JRC_Data!AG13</f>
+        <v>0.75</v>
       </c>
       <c r="L105" s="90"/>
       <c r="M105" s="78"/>
@@ -33755,8 +33768,8 @@
         <v>30</v>
       </c>
       <c r="AK105" s="155"/>
-      <c r="AL105" s="154" t="s">
-        <v>1038</v>
+      <c r="AL105" s="560" t="s">
+        <v>1046</v>
       </c>
       <c r="AM105" s="154" t="str">
         <f t="shared" si="69"/>
@@ -33777,7 +33790,7 @@
         <v>R-SW_Det_FPL_N1</v>
       </c>
       <c r="D106" s="69" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
       <c r="E106" s="70" t="s">
         <v>1035</v>
@@ -33787,16 +33800,20 @@
         <v>717</v>
       </c>
       <c r="H106" s="68">
-        <v>1</v>
-      </c>
-      <c r="I106" s="69">
-        <v>1</v>
-      </c>
-      <c r="J106" s="69">
-        <v>1</v>
-      </c>
-      <c r="K106" s="103">
-        <v>1</v>
+        <f>JRC_Data!AD13</f>
+        <v>0.7</v>
+      </c>
+      <c r="I106" s="68">
+        <f>JRC_Data!AE13</f>
+        <v>0.75</v>
+      </c>
+      <c r="J106" s="68">
+        <f>JRC_Data!AF13</f>
+        <v>0.75</v>
+      </c>
+      <c r="K106" s="68">
+        <f>JRC_Data!AG13</f>
+        <v>0.75</v>
       </c>
       <c r="L106" s="90"/>
       <c r="M106" s="78"/>
@@ -33804,19 +33821,19 @@
       <c r="O106" s="91"/>
       <c r="P106" s="68">
         <f t="shared" ref="P106:P108" si="83">H106*0.7</f>
-        <v>0.7</v>
+        <v>0.48999999999999994</v>
       </c>
       <c r="Q106" s="69">
         <f t="shared" ref="Q106:Q108" si="84">I106*0.7</f>
-        <v>0.7</v>
+        <v>0.52499999999999991</v>
       </c>
       <c r="R106" s="69">
         <f t="shared" ref="R106:R108" si="85">J106*0.7</f>
-        <v>0.7</v>
+        <v>0.52499999999999991</v>
       </c>
       <c r="S106" s="103">
         <f t="shared" ref="S106:S108" si="86">K106*0.7</f>
-        <v>0.7</v>
+        <v>0.52499999999999991</v>
       </c>
       <c r="T106" s="99">
         <v>20</v>
@@ -33858,8 +33875,8 @@
         <v>38</v>
       </c>
       <c r="AK106" s="155"/>
-      <c r="AL106" s="154" t="s">
-        <v>1039</v>
+      <c r="AL106" s="560" t="s">
+        <v>1047</v>
       </c>
       <c r="AM106" s="154" t="str">
         <f t="shared" si="69"/>
@@ -33876,7 +33893,7 @@
     </row>
     <row r="107" spans="3:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C107" s="86" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="D107" s="75" t="s">
         <v>698</v>
@@ -33982,7 +33999,7 @@
     </row>
     <row r="108" spans="3:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C108" s="68" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
       <c r="D108" s="69" t="s">
         <v>990</v>
@@ -36317,26 +36334,6 @@
     <row r="166" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="H92:K92"/>
-    <mergeCell ref="L92:O92"/>
-    <mergeCell ref="P92:S92"/>
-    <mergeCell ref="T92:U92"/>
-    <mergeCell ref="V92:Y92"/>
-    <mergeCell ref="H90:K90"/>
-    <mergeCell ref="L90:O90"/>
-    <mergeCell ref="P90:S90"/>
-    <mergeCell ref="T90:U90"/>
-    <mergeCell ref="V90:Y90"/>
-    <mergeCell ref="H44:K44"/>
-    <mergeCell ref="L44:O44"/>
-    <mergeCell ref="P44:S44"/>
-    <mergeCell ref="T44:U44"/>
-    <mergeCell ref="V44:Y44"/>
-    <mergeCell ref="H42:K42"/>
-    <mergeCell ref="L42:O42"/>
-    <mergeCell ref="P42:S42"/>
-    <mergeCell ref="T42:U42"/>
-    <mergeCell ref="V42:Y42"/>
     <mergeCell ref="V4:Y4"/>
     <mergeCell ref="V6:Y6"/>
     <mergeCell ref="H4:K4"/>
@@ -36347,6 +36344,26 @@
     <mergeCell ref="P6:S6"/>
     <mergeCell ref="L6:O6"/>
     <mergeCell ref="H6:K6"/>
+    <mergeCell ref="H42:K42"/>
+    <mergeCell ref="L42:O42"/>
+    <mergeCell ref="P42:S42"/>
+    <mergeCell ref="T42:U42"/>
+    <mergeCell ref="V42:Y42"/>
+    <mergeCell ref="H44:K44"/>
+    <mergeCell ref="L44:O44"/>
+    <mergeCell ref="P44:S44"/>
+    <mergeCell ref="T44:U44"/>
+    <mergeCell ref="V44:Y44"/>
+    <mergeCell ref="H90:K90"/>
+    <mergeCell ref="L90:O90"/>
+    <mergeCell ref="P90:S90"/>
+    <mergeCell ref="T90:U90"/>
+    <mergeCell ref="V90:Y90"/>
+    <mergeCell ref="H92:K92"/>
+    <mergeCell ref="L92:O92"/>
+    <mergeCell ref="P92:S92"/>
+    <mergeCell ref="T92:U92"/>
+    <mergeCell ref="V92:Y92"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
@@ -36491,12 +36508,12 @@
       <c r="I5" s="173"/>
       <c r="J5" s="173"/>
       <c r="K5" s="173"/>
-      <c r="L5" s="535" t="s">
+      <c r="L5" s="544" t="s">
         <v>322</v>
       </c>
-      <c r="M5" s="536"/>
-      <c r="N5" s="536"/>
-      <c r="O5" s="537"/>
+      <c r="M5" s="545"/>
+      <c r="N5" s="545"/>
+      <c r="O5" s="546"/>
       <c r="P5" s="106"/>
       <c r="Q5" s="106" t="s">
         <v>323</v>
@@ -36527,12 +36544,12 @@
       <c r="I6" s="83"/>
       <c r="J6" s="83"/>
       <c r="K6" s="83"/>
-      <c r="L6" s="544" t="s">
+      <c r="L6" s="538" t="s">
         <v>967</v>
       </c>
-      <c r="M6" s="546"/>
-      <c r="N6" s="546"/>
-      <c r="O6" s="545"/>
+      <c r="M6" s="540"/>
+      <c r="N6" s="540"/>
+      <c r="O6" s="539"/>
       <c r="P6" s="450" t="s">
         <v>979</v>
       </c>
@@ -37450,23 +37467,23 @@
       <c r="K33" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="L33" s="535" t="s">
+      <c r="L33" s="544" t="s">
         <v>322</v>
       </c>
-      <c r="M33" s="536"/>
-      <c r="N33" s="536"/>
-      <c r="O33" s="537"/>
+      <c r="M33" s="545"/>
+      <c r="N33" s="545"/>
+      <c r="O33" s="546"/>
     </row>
     <row r="34" spans="8:15" x14ac:dyDescent="0.2">
       <c r="H34" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="L34" s="544" t="s">
+      <c r="L34" s="538" t="s">
         <v>327</v>
       </c>
-      <c r="M34" s="546"/>
-      <c r="N34" s="546"/>
-      <c r="O34" s="545"/>
+      <c r="M34" s="540"/>
+      <c r="N34" s="540"/>
+      <c r="O34" s="539"/>
     </row>
     <row r="35" spans="8:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H35" s="5" t="s">
@@ -37813,11 +37830,11 @@
       </c>
       <c r="I4" s="542"/>
       <c r="J4" s="543"/>
-      <c r="K4" s="535" t="s">
+      <c r="K4" s="544" t="s">
         <v>322</v>
       </c>
-      <c r="L4" s="536"/>
-      <c r="M4" s="537"/>
+      <c r="L4" s="545"/>
+      <c r="M4" s="546"/>
       <c r="N4" s="106"/>
       <c r="O4" s="106" t="s">
         <v>323</v>
@@ -37843,16 +37860,16 @@
       <c r="G5" s="458" t="s">
         <v>302</v>
       </c>
-      <c r="H5" s="548" t="s">
+      <c r="H5" s="551" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="549"/>
-      <c r="J5" s="550"/>
-      <c r="K5" s="548" t="s">
+      <c r="I5" s="552"/>
+      <c r="J5" s="553"/>
+      <c r="K5" s="551" t="s">
         <v>756</v>
       </c>
-      <c r="L5" s="549"/>
-      <c r="M5" s="550"/>
+      <c r="L5" s="552"/>
+      <c r="M5" s="553"/>
       <c r="N5" s="459" t="s">
         <v>328</v>
       </c>
@@ -37869,23 +37886,23 @@
         <v>626</v>
       </c>
       <c r="AA5" s="281"/>
-      <c r="AB5" s="551" t="s">
+      <c r="AB5" s="548" t="s">
         <v>1011</v>
       </c>
-      <c r="AC5" s="551"/>
+      <c r="AC5" s="548"/>
       <c r="AD5" s="461"/>
-      <c r="AE5" s="552" t="s">
+      <c r="AE5" s="549" t="s">
         <v>110</v>
       </c>
-      <c r="AF5" s="552"/>
-      <c r="AG5" s="552" t="s">
+      <c r="AF5" s="549"/>
+      <c r="AG5" s="549" t="s">
         <v>1012</v>
       </c>
-      <c r="AH5" s="552"/>
-      <c r="AI5" s="553" t="s">
+      <c r="AH5" s="549"/>
+      <c r="AI5" s="550" t="s">
         <v>1013</v>
       </c>
-      <c r="AJ5" s="553"/>
+      <c r="AJ5" s="550"/>
     </row>
     <row r="6" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C6" s="505" t="str">
@@ -38623,12 +38640,12 @@
       <c r="K27" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="L27" s="535" t="s">
+      <c r="L27" s="544" t="s">
         <v>322</v>
       </c>
-      <c r="M27" s="536"/>
-      <c r="N27" s="536"/>
-      <c r="O27" s="537"/>
+      <c r="M27" s="545"/>
+      <c r="N27" s="545"/>
+      <c r="O27" s="546"/>
       <c r="T27" s="283"/>
       <c r="U27" s="283"/>
     </row>
@@ -38636,12 +38653,12 @@
       <c r="J28" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="L28" s="538" t="s">
+      <c r="L28" s="535" t="s">
         <v>327</v>
       </c>
-      <c r="M28" s="539"/>
-      <c r="N28" s="539"/>
-      <c r="O28" s="540"/>
+      <c r="M28" s="536"/>
+      <c r="N28" s="536"/>
+      <c r="O28" s="537"/>
       <c r="T28" s="283"/>
       <c r="U28" s="283"/>
     </row>
@@ -40031,16 +40048,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="L28:O28"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="K5:M5"/>
     <mergeCell ref="AB5:AC5"/>
     <mergeCell ref="AE5:AF5"/>
     <mergeCell ref="AG5:AH5"/>
     <mergeCell ref="AI5:AJ5"/>
     <mergeCell ref="L27:O27"/>
-    <mergeCell ref="L28:O28"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="K5:M5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="S7" r:id="rId1" xr:uid="{B1EDD63D-40A5-4174-9D28-8666BD314B83}"/>
@@ -48657,8 +48674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A061230A-839F-45A9-841C-C412BBE6D334}">
   <dimension ref="A1:CK183"/>
   <sheetViews>
-    <sheetView topLeftCell="Z1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+    <sheetView topLeftCell="L1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AD13" sqref="AD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -49070,103 +49087,103 @@
       <c r="C4" s="356" t="s">
         <v>765</v>
       </c>
-      <c r="D4" s="554" t="s">
+      <c r="D4" s="555" t="s">
         <v>766</v>
       </c>
-      <c r="E4" s="555"/>
-      <c r="F4" s="555"/>
-      <c r="G4" s="555"/>
+      <c r="E4" s="554"/>
+      <c r="F4" s="554"/>
+      <c r="G4" s="554"/>
       <c r="H4" s="556"/>
-      <c r="I4" s="555" t="s">
+      <c r="I4" s="554" t="s">
         <v>767</v>
       </c>
-      <c r="J4" s="555"/>
-      <c r="K4" s="555"/>
-      <c r="L4" s="555"/>
+      <c r="J4" s="554"/>
+      <c r="K4" s="554"/>
+      <c r="L4" s="554"/>
       <c r="M4" s="556"/>
-      <c r="N4" s="555" t="s">
+      <c r="N4" s="554" t="s">
         <v>768</v>
       </c>
-      <c r="O4" s="555"/>
-      <c r="P4" s="555"/>
-      <c r="Q4" s="555"/>
+      <c r="O4" s="554"/>
+      <c r="P4" s="554"/>
+      <c r="Q4" s="554"/>
       <c r="R4" s="556"/>
-      <c r="S4" s="555" t="s">
+      <c r="S4" s="554" t="s">
         <v>769</v>
       </c>
-      <c r="T4" s="555"/>
-      <c r="U4" s="555"/>
-      <c r="V4" s="555"/>
+      <c r="T4" s="554"/>
+      <c r="U4" s="554"/>
+      <c r="V4" s="554"/>
       <c r="W4" s="556"/>
-      <c r="X4" s="555" t="s">
+      <c r="X4" s="554" t="s">
         <v>770</v>
       </c>
-      <c r="Y4" s="555"/>
-      <c r="Z4" s="555"/>
-      <c r="AA4" s="555"/>
+      <c r="Y4" s="554"/>
+      <c r="Z4" s="554"/>
+      <c r="AA4" s="554"/>
       <c r="AB4" s="556"/>
-      <c r="AC4" s="555" t="s">
+      <c r="AC4" s="554" t="s">
         <v>771</v>
       </c>
-      <c r="AD4" s="555"/>
-      <c r="AE4" s="555"/>
-      <c r="AF4" s="555"/>
+      <c r="AD4" s="554"/>
+      <c r="AE4" s="554"/>
+      <c r="AF4" s="554"/>
       <c r="AG4" s="556"/>
-      <c r="AH4" s="555" t="s">
+      <c r="AH4" s="554" t="s">
         <v>772</v>
       </c>
-      <c r="AI4" s="555"/>
-      <c r="AJ4" s="555"/>
-      <c r="AK4" s="555"/>
+      <c r="AI4" s="554"/>
+      <c r="AJ4" s="554"/>
+      <c r="AK4" s="554"/>
       <c r="AL4" s="556"/>
-      <c r="AM4" s="555" t="s">
+      <c r="AM4" s="554" t="s">
         <v>773</v>
       </c>
-      <c r="AN4" s="555"/>
-      <c r="AO4" s="555"/>
-      <c r="AP4" s="555"/>
+      <c r="AN4" s="554"/>
+      <c r="AO4" s="554"/>
+      <c r="AP4" s="554"/>
       <c r="AQ4" s="556"/>
-      <c r="AR4" s="555" t="s">
+      <c r="AR4" s="554" t="s">
         <v>774</v>
       </c>
-      <c r="AS4" s="555"/>
-      <c r="AT4" s="555"/>
-      <c r="AU4" s="555"/>
+      <c r="AS4" s="554"/>
+      <c r="AT4" s="554"/>
+      <c r="AU4" s="554"/>
       <c r="AV4" s="556"/>
-      <c r="AW4" s="555" t="s">
+      <c r="AW4" s="554" t="s">
         <v>775</v>
       </c>
-      <c r="AX4" s="555"/>
-      <c r="AY4" s="555"/>
-      <c r="AZ4" s="555"/>
-      <c r="BA4" s="555"/>
-      <c r="BB4" s="554" t="s">
+      <c r="AX4" s="554"/>
+      <c r="AY4" s="554"/>
+      <c r="AZ4" s="554"/>
+      <c r="BA4" s="554"/>
+      <c r="BB4" s="555" t="s">
         <v>776</v>
       </c>
-      <c r="BC4" s="555"/>
-      <c r="BD4" s="555"/>
-      <c r="BE4" s="555"/>
+      <c r="BC4" s="554"/>
+      <c r="BD4" s="554"/>
+      <c r="BE4" s="554"/>
       <c r="BF4" s="556"/>
-      <c r="BG4" s="555" t="s">
+      <c r="BG4" s="554" t="s">
         <v>777</v>
       </c>
-      <c r="BH4" s="555"/>
-      <c r="BI4" s="555"/>
-      <c r="BJ4" s="555"/>
-      <c r="BK4" s="555"/>
-      <c r="BL4" s="554" t="s">
+      <c r="BH4" s="554"/>
+      <c r="BI4" s="554"/>
+      <c r="BJ4" s="554"/>
+      <c r="BK4" s="554"/>
+      <c r="BL4" s="555" t="s">
         <v>778</v>
       </c>
-      <c r="BM4" s="555"/>
-      <c r="BN4" s="555"/>
-      <c r="BO4" s="555"/>
-      <c r="BP4" s="555"/>
-      <c r="BQ4" s="554" t="s">
+      <c r="BM4" s="554"/>
+      <c r="BN4" s="554"/>
+      <c r="BO4" s="554"/>
+      <c r="BP4" s="554"/>
+      <c r="BQ4" s="555" t="s">
         <v>779</v>
       </c>
-      <c r="BR4" s="555"/>
-      <c r="BS4" s="555"/>
-      <c r="BT4" s="555"/>
+      <c r="BR4" s="554"/>
+      <c r="BS4" s="554"/>
+      <c r="BT4" s="554"/>
       <c r="BU4" s="556"/>
       <c r="BV4" s="357" t="s">
         <v>780</v>
@@ -62760,6 +62777,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="BL4:BP4"/>
+    <mergeCell ref="BQ4:BU4"/>
+    <mergeCell ref="BW4:CA4"/>
+    <mergeCell ref="CB4:CF4"/>
+    <mergeCell ref="CG4:CK4"/>
     <mergeCell ref="BG4:BK4"/>
     <mergeCell ref="D4:H4"/>
     <mergeCell ref="I4:M4"/>
@@ -62772,11 +62794,6 @@
     <mergeCell ref="AR4:AV4"/>
     <mergeCell ref="AW4:BA4"/>
     <mergeCell ref="BB4:BF4"/>
-    <mergeCell ref="BL4:BP4"/>
-    <mergeCell ref="BQ4:BU4"/>
-    <mergeCell ref="BW4:CA4"/>
-    <mergeCell ref="CB4:CF4"/>
-    <mergeCell ref="CG4:CK4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
Update Coal UP UC
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_RSD.xlsx
+++ b/SubRES_TMPL/SubRes_RSD.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E023D0F6-540C-4B76-A1D5-9E400FFAFA6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4B6CF27-F226-4261-8D3F-7C26435A26DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{34F9D92C-266F-476D-89E0-63153305AC39}"/>
   </bookViews>
@@ -14623,15 +14623,6 @@
     <xf numFmtId="0" fontId="53" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="23" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -14639,6 +14630,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -14650,17 +14650,26 @@
     <xf numFmtId="0" fontId="16" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="69" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="23" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -14671,19 +14680,10 @@
     <xf numFmtId="0" fontId="16" fillId="23" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="69" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="60" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="60" fillId="31" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="60" fillId="31" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -15814,10 +15814,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -25110,8 +25106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{104F8057-C735-4662-BAA6-EEDCF7B57273}">
   <dimension ref="A2:AQ166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C69" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="H105" sqref="H105:K106"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="C106" sqref="C106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -25297,12 +25293,12 @@
         <v>321</v>
       </c>
       <c r="U4" s="544"/>
-      <c r="V4" s="536" t="s">
+      <c r="V4" s="545" t="s">
         <v>322</v>
       </c>
-      <c r="W4" s="537"/>
-      <c r="X4" s="537"/>
-      <c r="Y4" s="538"/>
+      <c r="W4" s="546"/>
+      <c r="X4" s="546"/>
+      <c r="Y4" s="547"/>
       <c r="Z4" s="106"/>
       <c r="AA4" s="106"/>
       <c r="AB4" s="114" t="s">
@@ -25401,34 +25397,34 @@
       <c r="E6" s="84"/>
       <c r="F6" s="84"/>
       <c r="G6" s="85"/>
-      <c r="H6" s="539" t="s">
+      <c r="H6" s="536" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="540"/>
-      <c r="J6" s="540"/>
-      <c r="K6" s="541"/>
-      <c r="L6" s="540" t="s">
+      <c r="I6" s="537"/>
+      <c r="J6" s="537"/>
+      <c r="K6" s="538"/>
+      <c r="L6" s="537" t="s">
         <v>45</v>
       </c>
-      <c r="M6" s="540"/>
-      <c r="N6" s="540"/>
-      <c r="O6" s="541"/>
-      <c r="P6" s="539" t="s">
+      <c r="M6" s="537"/>
+      <c r="N6" s="537"/>
+      <c r="O6" s="538"/>
+      <c r="P6" s="536" t="s">
         <v>45</v>
       </c>
-      <c r="Q6" s="540"/>
-      <c r="R6" s="540"/>
-      <c r="S6" s="541"/>
-      <c r="T6" s="539" t="s">
+      <c r="Q6" s="537"/>
+      <c r="R6" s="537"/>
+      <c r="S6" s="538"/>
+      <c r="T6" s="536" t="s">
         <v>302</v>
       </c>
-      <c r="U6" s="541"/>
-      <c r="V6" s="539" t="s">
+      <c r="U6" s="538"/>
+      <c r="V6" s="536" t="s">
         <v>967</v>
       </c>
-      <c r="W6" s="540"/>
-      <c r="X6" s="540"/>
-      <c r="Y6" s="541"/>
+      <c r="W6" s="537"/>
+      <c r="X6" s="537"/>
+      <c r="Y6" s="538"/>
       <c r="Z6" s="107" t="s">
         <v>979</v>
       </c>
@@ -28362,12 +28358,12 @@
         <v>321</v>
       </c>
       <c r="U42" s="544"/>
-      <c r="V42" s="536" t="s">
+      <c r="V42" s="545" t="s">
         <v>322</v>
       </c>
-      <c r="W42" s="537"/>
-      <c r="X42" s="537"/>
-      <c r="Y42" s="538"/>
+      <c r="W42" s="546"/>
+      <c r="X42" s="546"/>
+      <c r="Y42" s="547"/>
       <c r="Z42" s="106"/>
       <c r="AA42" s="106"/>
       <c r="AB42" s="114" t="s">
@@ -28466,34 +28462,34 @@
       <c r="E44" s="84"/>
       <c r="F44" s="84"/>
       <c r="G44" s="85"/>
-      <c r="H44" s="539" t="s">
+      <c r="H44" s="536" t="s">
         <v>45</v>
       </c>
-      <c r="I44" s="540"/>
-      <c r="J44" s="540"/>
-      <c r="K44" s="541"/>
-      <c r="L44" s="540" t="s">
+      <c r="I44" s="537"/>
+      <c r="J44" s="537"/>
+      <c r="K44" s="538"/>
+      <c r="L44" s="537" t="s">
         <v>45</v>
       </c>
-      <c r="M44" s="540"/>
-      <c r="N44" s="540"/>
-      <c r="O44" s="541"/>
-      <c r="P44" s="539" t="s">
+      <c r="M44" s="537"/>
+      <c r="N44" s="537"/>
+      <c r="O44" s="538"/>
+      <c r="P44" s="536" t="s">
         <v>45</v>
       </c>
-      <c r="Q44" s="540"/>
-      <c r="R44" s="540"/>
-      <c r="S44" s="541"/>
-      <c r="T44" s="545" t="s">
+      <c r="Q44" s="537"/>
+      <c r="R44" s="537"/>
+      <c r="S44" s="538"/>
+      <c r="T44" s="539" t="s">
         <v>302</v>
       </c>
-      <c r="U44" s="546"/>
-      <c r="V44" s="545" t="s">
+      <c r="U44" s="540"/>
+      <c r="V44" s="539" t="s">
         <v>967</v>
       </c>
-      <c r="W44" s="547"/>
-      <c r="X44" s="547"/>
-      <c r="Y44" s="546"/>
+      <c r="W44" s="541"/>
+      <c r="X44" s="541"/>
+      <c r="Y44" s="540"/>
       <c r="Z44" s="450" t="s">
         <v>979</v>
       </c>
@@ -32284,12 +32280,12 @@
         <v>321</v>
       </c>
       <c r="U90" s="544"/>
-      <c r="V90" s="536" t="s">
+      <c r="V90" s="545" t="s">
         <v>322</v>
       </c>
-      <c r="W90" s="537"/>
-      <c r="X90" s="537"/>
-      <c r="Y90" s="538"/>
+      <c r="W90" s="546"/>
+      <c r="X90" s="546"/>
+      <c r="Y90" s="547"/>
       <c r="Z90" s="106"/>
       <c r="AA90" s="106"/>
       <c r="AB90" s="114" t="s">
@@ -32388,34 +32384,34 @@
       <c r="E92" s="84"/>
       <c r="F92" s="84"/>
       <c r="G92" s="85"/>
-      <c r="H92" s="539" t="s">
+      <c r="H92" s="536" t="s">
         <v>45</v>
       </c>
-      <c r="I92" s="540"/>
-      <c r="J92" s="540"/>
-      <c r="K92" s="541"/>
-      <c r="L92" s="540" t="s">
+      <c r="I92" s="537"/>
+      <c r="J92" s="537"/>
+      <c r="K92" s="538"/>
+      <c r="L92" s="537" t="s">
         <v>45</v>
       </c>
-      <c r="M92" s="540"/>
-      <c r="N92" s="540"/>
-      <c r="O92" s="541"/>
-      <c r="P92" s="539" t="s">
+      <c r="M92" s="537"/>
+      <c r="N92" s="537"/>
+      <c r="O92" s="538"/>
+      <c r="P92" s="536" t="s">
         <v>45</v>
       </c>
-      <c r="Q92" s="540"/>
-      <c r="R92" s="540"/>
-      <c r="S92" s="541"/>
-      <c r="T92" s="545" t="s">
+      <c r="Q92" s="537"/>
+      <c r="R92" s="537"/>
+      <c r="S92" s="538"/>
+      <c r="T92" s="539" t="s">
         <v>302</v>
       </c>
-      <c r="U92" s="546"/>
-      <c r="V92" s="545" t="s">
+      <c r="U92" s="540"/>
+      <c r="V92" s="539" t="s">
         <v>967</v>
       </c>
-      <c r="W92" s="547"/>
-      <c r="X92" s="547"/>
-      <c r="Y92" s="546"/>
+      <c r="W92" s="541"/>
+      <c r="X92" s="541"/>
+      <c r="Y92" s="540"/>
       <c r="Z92" s="450" t="s">
         <v>979</v>
       </c>
@@ -36346,26 +36342,6 @@
     <row r="166" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="H92:K92"/>
-    <mergeCell ref="L92:O92"/>
-    <mergeCell ref="P92:S92"/>
-    <mergeCell ref="T92:U92"/>
-    <mergeCell ref="V92:Y92"/>
-    <mergeCell ref="H90:K90"/>
-    <mergeCell ref="L90:O90"/>
-    <mergeCell ref="P90:S90"/>
-    <mergeCell ref="T90:U90"/>
-    <mergeCell ref="V90:Y90"/>
-    <mergeCell ref="H44:K44"/>
-    <mergeCell ref="L44:O44"/>
-    <mergeCell ref="P44:S44"/>
-    <mergeCell ref="T44:U44"/>
-    <mergeCell ref="V44:Y44"/>
-    <mergeCell ref="H42:K42"/>
-    <mergeCell ref="L42:O42"/>
-    <mergeCell ref="P42:S42"/>
-    <mergeCell ref="T42:U42"/>
-    <mergeCell ref="V42:Y42"/>
     <mergeCell ref="V4:Y4"/>
     <mergeCell ref="V6:Y6"/>
     <mergeCell ref="H4:K4"/>
@@ -36376,6 +36352,26 @@
     <mergeCell ref="P6:S6"/>
     <mergeCell ref="L6:O6"/>
     <mergeCell ref="H6:K6"/>
+    <mergeCell ref="H42:K42"/>
+    <mergeCell ref="L42:O42"/>
+    <mergeCell ref="P42:S42"/>
+    <mergeCell ref="T42:U42"/>
+    <mergeCell ref="V42:Y42"/>
+    <mergeCell ref="H44:K44"/>
+    <mergeCell ref="L44:O44"/>
+    <mergeCell ref="P44:S44"/>
+    <mergeCell ref="T44:U44"/>
+    <mergeCell ref="V44:Y44"/>
+    <mergeCell ref="H90:K90"/>
+    <mergeCell ref="L90:O90"/>
+    <mergeCell ref="P90:S90"/>
+    <mergeCell ref="T90:U90"/>
+    <mergeCell ref="V90:Y90"/>
+    <mergeCell ref="H92:K92"/>
+    <mergeCell ref="L92:O92"/>
+    <mergeCell ref="P92:S92"/>
+    <mergeCell ref="T92:U92"/>
+    <mergeCell ref="V92:Y92"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
@@ -36520,12 +36516,12 @@
       <c r="I5" s="173"/>
       <c r="J5" s="173"/>
       <c r="K5" s="173"/>
-      <c r="L5" s="536" t="s">
+      <c r="L5" s="545" t="s">
         <v>322</v>
       </c>
-      <c r="M5" s="537"/>
-      <c r="N5" s="537"/>
-      <c r="O5" s="538"/>
+      <c r="M5" s="546"/>
+      <c r="N5" s="546"/>
+      <c r="O5" s="547"/>
       <c r="P5" s="106"/>
       <c r="Q5" s="106" t="s">
         <v>323</v>
@@ -36556,12 +36552,12 @@
       <c r="I6" s="83"/>
       <c r="J6" s="83"/>
       <c r="K6" s="83"/>
-      <c r="L6" s="545" t="s">
+      <c r="L6" s="539" t="s">
         <v>967</v>
       </c>
-      <c r="M6" s="547"/>
-      <c r="N6" s="547"/>
-      <c r="O6" s="546"/>
+      <c r="M6" s="541"/>
+      <c r="N6" s="541"/>
+      <c r="O6" s="540"/>
       <c r="P6" s="450" t="s">
         <v>979</v>
       </c>
@@ -37479,23 +37475,23 @@
       <c r="K33" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="L33" s="536" t="s">
+      <c r="L33" s="545" t="s">
         <v>322</v>
       </c>
-      <c r="M33" s="537"/>
-      <c r="N33" s="537"/>
-      <c r="O33" s="538"/>
+      <c r="M33" s="546"/>
+      <c r="N33" s="546"/>
+      <c r="O33" s="547"/>
     </row>
     <row r="34" spans="8:15" x14ac:dyDescent="0.2">
       <c r="H34" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="L34" s="545" t="s">
+      <c r="L34" s="539" t="s">
         <v>327</v>
       </c>
-      <c r="M34" s="547"/>
-      <c r="N34" s="547"/>
-      <c r="O34" s="546"/>
+      <c r="M34" s="541"/>
+      <c r="N34" s="541"/>
+      <c r="O34" s="540"/>
     </row>
     <row r="35" spans="8:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H35" s="5" t="s">
@@ -37842,11 +37838,11 @@
       </c>
       <c r="I4" s="543"/>
       <c r="J4" s="544"/>
-      <c r="K4" s="536" t="s">
+      <c r="K4" s="545" t="s">
         <v>322</v>
       </c>
-      <c r="L4" s="537"/>
-      <c r="M4" s="538"/>
+      <c r="L4" s="546"/>
+      <c r="M4" s="547"/>
       <c r="N4" s="106"/>
       <c r="O4" s="106" t="s">
         <v>323</v>
@@ -37872,16 +37868,16 @@
       <c r="G5" s="458" t="s">
         <v>302</v>
       </c>
-      <c r="H5" s="549" t="s">
+      <c r="H5" s="552" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="550"/>
-      <c r="J5" s="551"/>
-      <c r="K5" s="549" t="s">
+      <c r="I5" s="553"/>
+      <c r="J5" s="554"/>
+      <c r="K5" s="552" t="s">
         <v>756</v>
       </c>
-      <c r="L5" s="550"/>
-      <c r="M5" s="551"/>
+      <c r="L5" s="553"/>
+      <c r="M5" s="554"/>
       <c r="N5" s="459" t="s">
         <v>328</v>
       </c>
@@ -37898,23 +37894,23 @@
         <v>626</v>
       </c>
       <c r="AA5" s="281"/>
-      <c r="AB5" s="552" t="s">
+      <c r="AB5" s="549" t="s">
         <v>1011</v>
       </c>
-      <c r="AC5" s="552"/>
+      <c r="AC5" s="549"/>
       <c r="AD5" s="461"/>
-      <c r="AE5" s="553" t="s">
+      <c r="AE5" s="550" t="s">
         <v>110</v>
       </c>
-      <c r="AF5" s="553"/>
-      <c r="AG5" s="553" t="s">
+      <c r="AF5" s="550"/>
+      <c r="AG5" s="550" t="s">
         <v>1012</v>
       </c>
-      <c r="AH5" s="553"/>
-      <c r="AI5" s="554" t="s">
+      <c r="AH5" s="550"/>
+      <c r="AI5" s="551" t="s">
         <v>1013</v>
       </c>
-      <c r="AJ5" s="554"/>
+      <c r="AJ5" s="551"/>
     </row>
     <row r="6" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C6" s="505" t="str">
@@ -38652,12 +38648,12 @@
       <c r="K27" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="L27" s="536" t="s">
+      <c r="L27" s="545" t="s">
         <v>322</v>
       </c>
-      <c r="M27" s="537"/>
-      <c r="N27" s="537"/>
-      <c r="O27" s="538"/>
+      <c r="M27" s="546"/>
+      <c r="N27" s="546"/>
+      <c r="O27" s="547"/>
       <c r="T27" s="283"/>
       <c r="U27" s="283"/>
     </row>
@@ -38665,12 +38661,12 @@
       <c r="J28" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="L28" s="539" t="s">
+      <c r="L28" s="536" t="s">
         <v>327</v>
       </c>
-      <c r="M28" s="540"/>
-      <c r="N28" s="540"/>
-      <c r="O28" s="541"/>
+      <c r="M28" s="537"/>
+      <c r="N28" s="537"/>
+      <c r="O28" s="538"/>
       <c r="T28" s="283"/>
       <c r="U28" s="283"/>
     </row>
@@ -40060,16 +40056,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="L28:O28"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="K5:M5"/>
     <mergeCell ref="AB5:AC5"/>
     <mergeCell ref="AE5:AF5"/>
     <mergeCell ref="AG5:AH5"/>
     <mergeCell ref="AI5:AJ5"/>
     <mergeCell ref="L27:O27"/>
-    <mergeCell ref="L28:O28"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="K5:M5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="S7" r:id="rId1" xr:uid="{B1EDD63D-40A5-4174-9D28-8666BD314B83}"/>
@@ -49099,103 +49095,103 @@
       <c r="C4" s="356" t="s">
         <v>765</v>
       </c>
-      <c r="D4" s="555" t="s">
+      <c r="D4" s="556" t="s">
         <v>766</v>
       </c>
-      <c r="E4" s="556"/>
-      <c r="F4" s="556"/>
-      <c r="G4" s="556"/>
+      <c r="E4" s="555"/>
+      <c r="F4" s="555"/>
+      <c r="G4" s="555"/>
       <c r="H4" s="557"/>
-      <c r="I4" s="556" t="s">
+      <c r="I4" s="555" t="s">
         <v>767</v>
       </c>
-      <c r="J4" s="556"/>
-      <c r="K4" s="556"/>
-      <c r="L4" s="556"/>
+      <c r="J4" s="555"/>
+      <c r="K4" s="555"/>
+      <c r="L4" s="555"/>
       <c r="M4" s="557"/>
-      <c r="N4" s="556" t="s">
+      <c r="N4" s="555" t="s">
         <v>768</v>
       </c>
-      <c r="O4" s="556"/>
-      <c r="P4" s="556"/>
-      <c r="Q4" s="556"/>
+      <c r="O4" s="555"/>
+      <c r="P4" s="555"/>
+      <c r="Q4" s="555"/>
       <c r="R4" s="557"/>
-      <c r="S4" s="556" t="s">
+      <c r="S4" s="555" t="s">
         <v>769</v>
       </c>
-      <c r="T4" s="556"/>
-      <c r="U4" s="556"/>
-      <c r="V4" s="556"/>
+      <c r="T4" s="555"/>
+      <c r="U4" s="555"/>
+      <c r="V4" s="555"/>
       <c r="W4" s="557"/>
-      <c r="X4" s="556" t="s">
+      <c r="X4" s="555" t="s">
         <v>770</v>
       </c>
-      <c r="Y4" s="556"/>
-      <c r="Z4" s="556"/>
-      <c r="AA4" s="556"/>
+      <c r="Y4" s="555"/>
+      <c r="Z4" s="555"/>
+      <c r="AA4" s="555"/>
       <c r="AB4" s="557"/>
-      <c r="AC4" s="556" t="s">
+      <c r="AC4" s="555" t="s">
         <v>771</v>
       </c>
-      <c r="AD4" s="556"/>
-      <c r="AE4" s="556"/>
-      <c r="AF4" s="556"/>
+      <c r="AD4" s="555"/>
+      <c r="AE4" s="555"/>
+      <c r="AF4" s="555"/>
       <c r="AG4" s="557"/>
-      <c r="AH4" s="556" t="s">
+      <c r="AH4" s="555" t="s">
         <v>772</v>
       </c>
-      <c r="AI4" s="556"/>
-      <c r="AJ4" s="556"/>
-      <c r="AK4" s="556"/>
+      <c r="AI4" s="555"/>
+      <c r="AJ4" s="555"/>
+      <c r="AK4" s="555"/>
       <c r="AL4" s="557"/>
-      <c r="AM4" s="556" t="s">
+      <c r="AM4" s="555" t="s">
         <v>773</v>
       </c>
-      <c r="AN4" s="556"/>
-      <c r="AO4" s="556"/>
-      <c r="AP4" s="556"/>
+      <c r="AN4" s="555"/>
+      <c r="AO4" s="555"/>
+      <c r="AP4" s="555"/>
       <c r="AQ4" s="557"/>
-      <c r="AR4" s="556" t="s">
+      <c r="AR4" s="555" t="s">
         <v>774</v>
       </c>
-      <c r="AS4" s="556"/>
-      <c r="AT4" s="556"/>
-      <c r="AU4" s="556"/>
+      <c r="AS4" s="555"/>
+      <c r="AT4" s="555"/>
+      <c r="AU4" s="555"/>
       <c r="AV4" s="557"/>
-      <c r="AW4" s="556" t="s">
+      <c r="AW4" s="555" t="s">
         <v>775</v>
       </c>
-      <c r="AX4" s="556"/>
-      <c r="AY4" s="556"/>
-      <c r="AZ4" s="556"/>
-      <c r="BA4" s="556"/>
-      <c r="BB4" s="555" t="s">
+      <c r="AX4" s="555"/>
+      <c r="AY4" s="555"/>
+      <c r="AZ4" s="555"/>
+      <c r="BA4" s="555"/>
+      <c r="BB4" s="556" t="s">
         <v>776</v>
       </c>
-      <c r="BC4" s="556"/>
-      <c r="BD4" s="556"/>
-      <c r="BE4" s="556"/>
+      <c r="BC4" s="555"/>
+      <c r="BD4" s="555"/>
+      <c r="BE4" s="555"/>
       <c r="BF4" s="557"/>
-      <c r="BG4" s="556" t="s">
+      <c r="BG4" s="555" t="s">
         <v>777</v>
       </c>
-      <c r="BH4" s="556"/>
-      <c r="BI4" s="556"/>
-      <c r="BJ4" s="556"/>
-      <c r="BK4" s="556"/>
-      <c r="BL4" s="555" t="s">
+      <c r="BH4" s="555"/>
+      <c r="BI4" s="555"/>
+      <c r="BJ4" s="555"/>
+      <c r="BK4" s="555"/>
+      <c r="BL4" s="556" t="s">
         <v>778</v>
       </c>
-      <c r="BM4" s="556"/>
-      <c r="BN4" s="556"/>
-      <c r="BO4" s="556"/>
-      <c r="BP4" s="556"/>
-      <c r="BQ4" s="555" t="s">
+      <c r="BM4" s="555"/>
+      <c r="BN4" s="555"/>
+      <c r="BO4" s="555"/>
+      <c r="BP4" s="555"/>
+      <c r="BQ4" s="556" t="s">
         <v>779</v>
       </c>
-      <c r="BR4" s="556"/>
-      <c r="BS4" s="556"/>
-      <c r="BT4" s="556"/>
+      <c r="BR4" s="555"/>
+      <c r="BS4" s="555"/>
+      <c r="BT4" s="555"/>
       <c r="BU4" s="557"/>
       <c r="BV4" s="357" t="s">
         <v>780</v>
@@ -62789,6 +62785,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="BL4:BP4"/>
+    <mergeCell ref="BQ4:BU4"/>
+    <mergeCell ref="BW4:CA4"/>
+    <mergeCell ref="CB4:CF4"/>
+    <mergeCell ref="CG4:CK4"/>
     <mergeCell ref="BG4:BK4"/>
     <mergeCell ref="D4:H4"/>
     <mergeCell ref="I4:M4"/>
@@ -62801,11 +62802,6 @@
     <mergeCell ref="AR4:AV4"/>
     <mergeCell ref="AW4:BA4"/>
     <mergeCell ref="BB4:BF4"/>
-    <mergeCell ref="BL4:BP4"/>
-    <mergeCell ref="BQ4:BU4"/>
-    <mergeCell ref="BW4:CA4"/>
-    <mergeCell ref="CB4:CF4"/>
-    <mergeCell ref="CG4:CK4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
Update Ambient Heat Changes for Water Heating
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_RSD.xlsx
+++ b/SubRES_TMPL/SubRes_RSD.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A65BFB2D-4258-47E7-8BCD-0B9DA8F90389}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31D8C5CE-366D-40AE-8F99-9C2422D783A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="9" xr2:uid="{34F9D92C-266F-476D-89E0-63153305AC39}"/>
   </bookViews>
@@ -15058,6 +15058,86 @@
     <xf numFmtId="0" fontId="41" fillId="21" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="17" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="15" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="80" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="80" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="16" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="17" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="12" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="86" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="86" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="6" borderId="1" xfId="15" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="1" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -15103,15 +15183,6 @@
     <xf numFmtId="0" fontId="54" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="23" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -15119,6 +15190,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -15130,17 +15210,26 @@
     <xf numFmtId="0" fontId="17" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="70" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="23" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -15151,19 +15240,10 @@
     <xf numFmtId="0" fontId="17" fillId="23" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="70" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="61" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="61" fillId="31" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="61" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="61" fillId="31" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -15178,15 +15258,19 @@
     <xf numFmtId="0" fontId="61" fillId="32" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="15" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="84" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="82" xfId="0" applyBorder="1" applyAlignment="1">
@@ -15198,90 +15282,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="84" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="80" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="80" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="16" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="17" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="12" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="86" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="86" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="6" borderId="1" xfId="15" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="1" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="18">
     <cellStyle name="20% - Colore 2" xfId="11" xr:uid="{3E3DAF22-4D86-48A9-B6EE-8D230C1E993C}"/>
@@ -16993,14 +16993,14 @@
       <c r="F16" s="211"/>
     </row>
     <row r="17" spans="1:14" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="522" t="s">
+      <c r="A17" s="562" t="s">
         <v>434</v>
       </c>
-      <c r="B17" s="522"/>
-      <c r="C17" s="522"/>
-      <c r="D17" s="522"/>
-      <c r="E17" s="522"/>
-      <c r="F17" s="522"/>
+      <c r="B17" s="562"/>
+      <c r="C17" s="562"/>
+      <c r="D17" s="562"/>
+      <c r="E17" s="562"/>
+      <c r="F17" s="562"/>
       <c r="G17" s="213"/>
       <c r="H17" s="213"/>
       <c r="I17" s="214"/>
@@ -17038,13 +17038,13 @@
       <c r="A20" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="523" t="s">
+      <c r="B20" s="563" t="s">
         <v>436</v>
       </c>
-      <c r="C20" s="523"/>
-      <c r="D20" s="523"/>
-      <c r="E20" s="523"/>
-      <c r="F20" s="523"/>
+      <c r="C20" s="563"/>
+      <c r="D20" s="563"/>
+      <c r="E20" s="563"/>
+      <c r="F20" s="563"/>
       <c r="G20" s="218"/>
       <c r="H20" s="218"/>
       <c r="I20" s="219"/>
@@ -17058,13 +17058,13 @@
       <c r="A21" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="524" t="s">
+      <c r="B21" s="564" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="524"/>
-      <c r="D21" s="524"/>
-      <c r="E21" s="524"/>
-      <c r="F21" s="524"/>
+      <c r="C21" s="564"/>
+      <c r="D21" s="564"/>
+      <c r="E21" s="564"/>
+      <c r="F21" s="564"/>
       <c r="G21" s="218"/>
       <c r="H21" s="218"/>
       <c r="I21" s="219"/>
@@ -17078,13 +17078,13 @@
       <c r="A22" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="524" t="s">
+      <c r="B22" s="564" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="524"/>
-      <c r="D22" s="524"/>
-      <c r="E22" s="524"/>
-      <c r="F22" s="524"/>
+      <c r="C22" s="564"/>
+      <c r="D22" s="564"/>
+      <c r="E22" s="564"/>
+      <c r="F22" s="564"/>
     </row>
     <row r="23" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
@@ -17113,22 +17113,22 @@
       <c r="H24" s="3"/>
     </row>
     <row r="25" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="525"/>
-      <c r="B25" s="525"/>
-      <c r="C25" s="525"/>
-      <c r="D25" s="525"/>
-      <c r="E25" s="525"/>
-      <c r="F25" s="525"/>
+      <c r="A25" s="565"/>
+      <c r="B25" s="565"/>
+      <c r="C25" s="565"/>
+      <c r="D25" s="565"/>
+      <c r="E25" s="565"/>
+      <c r="F25" s="565"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
     </row>
     <row r="26" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="521"/>
-      <c r="B26" s="521"/>
-      <c r="C26" s="521"/>
-      <c r="D26" s="521"/>
-      <c r="E26" s="521"/>
-      <c r="F26" s="521"/>
+      <c r="A26" s="561"/>
+      <c r="B26" s="561"/>
+      <c r="C26" s="561"/>
+      <c r="D26" s="561"/>
+      <c r="E26" s="561"/>
+      <c r="F26" s="561"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="211"/>
@@ -17293,8 +17293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC422C74-4930-4E02-A6A2-617D513D886A}">
   <dimension ref="A1:AD121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="AB52" sqref="AB52"/>
+    <sheetView tabSelected="1" topLeftCell="B25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="T38" sqref="T38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -17304,23 +17304,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" s="567" t="s">
+      <c r="A1" s="604" t="s">
         <v>1062</v>
       </c>
-      <c r="B1" s="568" t="s">
+      <c r="B1" s="606" t="s">
         <v>1063</v>
       </c>
-      <c r="C1" s="569"/>
-      <c r="D1" s="569"/>
-      <c r="E1" s="569"/>
-      <c r="F1" s="570"/>
-      <c r="G1" s="568" t="s">
+      <c r="C1" s="607"/>
+      <c r="D1" s="607"/>
+      <c r="E1" s="607"/>
+      <c r="F1" s="608"/>
+      <c r="G1" s="606" t="s">
         <v>1064</v>
       </c>
-      <c r="H1" s="569"/>
-      <c r="I1" s="569"/>
-      <c r="J1" s="569"/>
-      <c r="K1" s="570"/>
+      <c r="H1" s="607"/>
+      <c r="I1" s="607"/>
+      <c r="J1" s="607"/>
+      <c r="K1" s="608"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
@@ -17330,39 +17330,39 @@
       <c r="R1" s="5"/>
     </row>
     <row r="2" spans="1:18" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="571"/>
-      <c r="B2" s="572" t="s">
+      <c r="A2" s="605"/>
+      <c r="B2" s="527" t="s">
         <v>686</v>
       </c>
-      <c r="C2" s="573" t="s">
+      <c r="C2" s="528" t="s">
         <v>1065</v>
       </c>
-      <c r="D2" s="573" t="s">
+      <c r="D2" s="528" t="s">
         <v>1066</v>
       </c>
-      <c r="E2" s="573" t="s">
+      <c r="E2" s="528" t="s">
         <v>1067</v>
       </c>
-      <c r="F2" s="574" t="s">
+      <c r="F2" s="529" t="s">
         <v>1068</v>
       </c>
-      <c r="G2" s="572" t="s">
+      <c r="G2" s="527" t="s">
         <v>686</v>
       </c>
-      <c r="H2" s="573" t="s">
+      <c r="H2" s="528" t="s">
         <v>1065</v>
       </c>
-      <c r="I2" s="573" t="s">
+      <c r="I2" s="528" t="s">
         <v>1066</v>
       </c>
-      <c r="J2" s="573" t="s">
+      <c r="J2" s="528" t="s">
         <v>1067</v>
       </c>
-      <c r="K2" s="574" t="s">
+      <c r="K2" s="529" t="s">
         <v>1068</v>
       </c>
       <c r="L2" s="5"/>
-      <c r="M2" s="575"/>
+      <c r="M2" s="530"/>
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
@@ -17370,46 +17370,46 @@
       <c r="R2" s="5"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A3" s="576" t="s">
+      <c r="A3" s="531" t="s">
         <v>1069</v>
       </c>
-      <c r="B3" s="577">
+      <c r="B3" s="532">
         <f>SUM(C3:F3)</f>
         <v>113.577</v>
       </c>
-      <c r="C3" s="578">
+      <c r="C3" s="533">
         <v>94.888999999999996</v>
       </c>
-      <c r="D3" s="579">
+      <c r="D3" s="534">
         <v>2.831</v>
       </c>
-      <c r="E3" s="579"/>
-      <c r="F3" s="580">
+      <c r="E3" s="534"/>
+      <c r="F3" s="535">
         <v>15.856999999999999</v>
       </c>
-      <c r="G3" s="577">
+      <c r="G3" s="532">
         <f>B3/3.6</f>
         <v>31.549166666666665</v>
       </c>
-      <c r="H3" s="581">
+      <c r="H3" s="536">
         <f>C3/3.6</f>
         <v>26.358055555555552</v>
       </c>
-      <c r="I3" s="581">
+      <c r="I3" s="536">
         <f>D3/3.6</f>
         <v>0.7863888888888888</v>
       </c>
-      <c r="J3" s="581">
+      <c r="J3" s="536">
         <f>E3/3.6</f>
         <v>0</v>
       </c>
-      <c r="K3" s="582">
+      <c r="K3" s="537">
         <f>F3/3.6</f>
         <v>4.4047222222222215</v>
       </c>
       <c r="L3" s="5"/>
-      <c r="M3" s="583"/>
-      <c r="N3" s="584"/>
+      <c r="M3" s="538"/>
+      <c r="N3" s="539"/>
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
@@ -17476,12 +17476,12 @@
       <c r="R6" s="5"/>
     </row>
     <row r="7" spans="1:18" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="585" t="s">
+      <c r="A7" s="601" t="s">
         <v>1065</v>
       </c>
-      <c r="B7" s="585"/>
-      <c r="C7" s="585"/>
-      <c r="D7" s="585"/>
+      <c r="B7" s="601"/>
+      <c r="C7" s="601"/>
+      <c r="D7" s="601"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
@@ -17498,16 +17498,16 @@
       <c r="R7" s="5"/>
     </row>
     <row r="8" spans="1:18" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="586" t="s">
+      <c r="A8" s="540" t="s">
         <v>1070</v>
       </c>
-      <c r="B8" s="586">
+      <c r="B8" s="540">
         <v>2015</v>
       </c>
-      <c r="C8" s="586">
+      <c r="C8" s="540">
         <v>2020</v>
       </c>
-      <c r="D8" s="586">
+      <c r="D8" s="540">
         <v>2030</v>
       </c>
       <c r="E8" s="5"/>
@@ -17664,11 +17664,11 @@
         <v>1076</v>
       </c>
       <c r="B14" s="5"/>
-      <c r="C14" s="587">
+      <c r="C14" s="541">
         <f>(C11/C12)*C13</f>
         <v>15.311999999999998</v>
       </c>
-      <c r="D14" s="587">
+      <c r="D14" s="541">
         <f>(D11/D12)*D13</f>
         <v>8.7120000000000015</v>
       </c>
@@ -17719,15 +17719,15 @@
       <c r="A16" s="5" t="s">
         <v>1078</v>
       </c>
-      <c r="B16" s="587">
+      <c r="B16" s="541">
         <f>C3</f>
         <v>94.888999999999996</v>
       </c>
-      <c r="C16" s="587">
+      <c r="C16" s="541">
         <f>C15/1000</f>
         <v>55.12319999999999</v>
       </c>
-      <c r="D16" s="603">
+      <c r="D16" s="557">
         <f>D15/1000</f>
         <v>31.363200000000003</v>
       </c>
@@ -17748,9 +17748,9 @@
     </row>
     <row r="17" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A17" s="5"/>
-      <c r="B17" s="587"/>
-      <c r="C17" s="587"/>
-      <c r="D17" s="587"/>
+      <c r="B17" s="541"/>
+      <c r="C17" s="541"/>
+      <c r="D17" s="541"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
@@ -17767,12 +17767,12 @@
       <c r="R17" s="5"/>
     </row>
     <row r="18" spans="1:30" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="585" t="s">
+      <c r="A18" s="601" t="s">
         <v>1079</v>
       </c>
-      <c r="B18" s="585"/>
-      <c r="C18" s="585"/>
-      <c r="D18" s="585"/>
+      <c r="B18" s="601"/>
+      <c r="C18" s="601"/>
+      <c r="D18" s="601"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
@@ -17789,14 +17789,14 @@
       <c r="R18" s="5"/>
     </row>
     <row r="19" spans="1:30" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="586" t="s">
+      <c r="A19" s="540" t="s">
         <v>1070</v>
       </c>
-      <c r="B19" s="586"/>
-      <c r="C19" s="586">
+      <c r="B19" s="540"/>
+      <c r="C19" s="540">
         <v>2020</v>
       </c>
-      <c r="D19" s="586">
+      <c r="D19" s="540">
         <v>2030</v>
       </c>
       <c r="E19" s="5"/>
@@ -17847,10 +17847,10 @@
         <v>1081</v>
       </c>
       <c r="B21" s="5"/>
-      <c r="C21" s="588">
+      <c r="C21" s="542">
         <v>0.127</v>
       </c>
-      <c r="D21" s="589">
+      <c r="D21" s="543">
         <v>0.1</v>
       </c>
       <c r="E21" s="5"/>
@@ -17901,7 +17901,7 @@
         <v>1083</v>
       </c>
       <c r="B23" s="5"/>
-      <c r="C23" s="566">
+      <c r="C23" s="526">
         <v>3</v>
       </c>
       <c r="D23" s="5">
@@ -17955,11 +17955,11 @@
         <v>1085</v>
       </c>
       <c r="B25" s="5"/>
-      <c r="C25" s="566">
+      <c r="C25" s="526">
         <f>C24*3600</f>
         <v>20047.670103092783</v>
       </c>
-      <c r="D25" s="566">
+      <c r="D25" s="526">
         <f>D24*3600</f>
         <v>30491.999999999996</v>
       </c>
@@ -17983,11 +17983,11 @@
         <v>1086</v>
       </c>
       <c r="B26" s="5"/>
-      <c r="C26" s="587">
+      <c r="C26" s="541">
         <f>C25/1000</f>
         <v>20.047670103092784</v>
       </c>
-      <c r="D26" s="603">
+      <c r="D26" s="557">
         <f>D25/1000</f>
         <v>30.491999999999997</v>
       </c>
@@ -18027,12 +18027,12 @@
       <c r="R27" s="5"/>
     </row>
     <row r="28" spans="1:30" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="585" t="s">
+      <c r="A28" s="601" t="s">
         <v>1087</v>
       </c>
-      <c r="B28" s="585"/>
-      <c r="C28" s="585"/>
-      <c r="D28" s="585"/>
+      <c r="B28" s="601"/>
+      <c r="C28" s="601"/>
+      <c r="D28" s="601"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
@@ -18048,17 +18048,17 @@
       <c r="Q28" s="5"/>
       <c r="R28" s="5"/>
     </row>
-    <row r="29" spans="1:30" ht="60" x14ac:dyDescent="0.25">
-      <c r="A29" s="586" t="s">
+    <row r="29" spans="1:30" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="540" t="s">
         <v>1070</v>
       </c>
-      <c r="B29" s="586">
+      <c r="B29" s="540">
         <v>2015</v>
       </c>
-      <c r="C29" s="586">
+      <c r="C29" s="540">
         <v>2020</v>
       </c>
-      <c r="D29" s="586">
+      <c r="D29" s="540">
         <v>2030</v>
       </c>
       <c r="E29" s="5"/>
@@ -18075,18 +18075,18 @@
       <c r="P29" s="5"/>
       <c r="Q29" s="5"/>
       <c r="R29" s="5"/>
-      <c r="T29" s="561"/>
-      <c r="U29" s="562"/>
-      <c r="V29" s="563" t="s">
+      <c r="T29" s="521"/>
+      <c r="U29" s="522"/>
+      <c r="V29" s="523" t="s">
         <v>1048</v>
       </c>
-      <c r="W29" s="563" t="s">
+      <c r="W29" s="523" t="s">
         <v>1049</v>
       </c>
-      <c r="X29" s="563" t="s">
+      <c r="X29" s="523" t="s">
         <v>1050</v>
       </c>
-      <c r="Y29" s="563" t="s">
+      <c r="Y29" s="523" t="s">
         <v>1051</v>
       </c>
     </row>
@@ -18119,20 +18119,20 @@
       <c r="P30" s="5"/>
       <c r="Q30" s="5"/>
       <c r="R30" s="5"/>
-      <c r="T30" s="561"/>
-      <c r="U30" s="561" t="s">
+      <c r="T30" s="521"/>
+      <c r="U30" s="521" t="s">
         <v>1052</v>
       </c>
-      <c r="V30" s="561" t="s">
+      <c r="V30" s="521" t="s">
         <v>1053</v>
       </c>
-      <c r="W30" s="561" t="s">
+      <c r="W30" s="521" t="s">
         <v>1054</v>
       </c>
-      <c r="X30" s="561" t="s">
+      <c r="X30" s="521" t="s">
         <v>1055</v>
       </c>
-      <c r="Y30" s="561" t="s">
+      <c r="Y30" s="521" t="s">
         <v>1056</v>
       </c>
     </row>
@@ -18165,22 +18165,22 @@
       <c r="P31" s="5"/>
       <c r="Q31" s="5"/>
       <c r="R31" s="5"/>
-      <c r="T31" s="562" t="s">
+      <c r="T31" s="522" t="s">
         <v>1057</v>
       </c>
-      <c r="U31" s="561">
+      <c r="U31" s="521">
         <v>311.65399600000001</v>
       </c>
-      <c r="V31" s="561">
+      <c r="V31" s="521">
         <v>8845.3479520000001</v>
       </c>
-      <c r="W31" s="561">
+      <c r="W31" s="521">
         <v>22461.807872000001</v>
       </c>
-      <c r="X31" s="561">
+      <c r="X31" s="521">
         <v>28682.778717000001</v>
       </c>
-      <c r="Y31" s="561">
+      <c r="Y31" s="521">
         <v>8653.6989190000004</v>
       </c>
     </row>
@@ -18188,15 +18188,15 @@
       <c r="A32" s="5" t="s">
         <v>1090</v>
       </c>
-      <c r="B32" s="566">
+      <c r="B32" s="526">
         <f>B30/B31</f>
         <v>72</v>
       </c>
-      <c r="C32" s="566">
+      <c r="C32" s="526">
         <f>C30/C31</f>
         <v>312</v>
       </c>
-      <c r="D32" s="566">
+      <c r="D32" s="526">
         <f>D30/D31</f>
         <v>386</v>
       </c>
@@ -18214,25 +18214,25 @@
       <c r="P32" s="5"/>
       <c r="Q32" s="5"/>
       <c r="R32" s="5"/>
-      <c r="T32" s="562" t="s">
+      <c r="T32" s="522" t="s">
         <v>1058</v>
       </c>
-      <c r="U32" s="564">
+      <c r="U32" s="524">
         <v>2.9555506715861044E-3</v>
       </c>
-      <c r="V32" s="601">
+      <c r="V32" s="555">
         <v>8.3884289678565108E-2</v>
       </c>
-      <c r="W32" s="601">
+      <c r="W32" s="555">
         <v>0.21301511353355998</v>
       </c>
-      <c r="X32" s="601">
+      <c r="X32" s="555">
         <v>0.2720112913295839</v>
       </c>
-      <c r="Y32" s="601">
+      <c r="Y32" s="555">
         <v>8.2066798372623442E-2</v>
       </c>
-      <c r="AA32" s="602">
+      <c r="AA32" s="556">
         <f>SUM(V32:Y32)</f>
         <v>0.65097749291433249</v>
       </c>
@@ -18269,20 +18269,20 @@
       <c r="P33" s="5"/>
       <c r="Q33" s="5"/>
       <c r="R33" s="5"/>
-      <c r="T33" s="562" t="s">
+      <c r="T33" s="522" t="s">
         <v>329</v>
       </c>
-      <c r="U33" s="565"/>
-      <c r="V33" s="565">
+      <c r="U33" s="525"/>
+      <c r="V33" s="525">
         <v>8</v>
       </c>
-      <c r="W33" s="565">
+      <c r="W33" s="525">
         <v>6</v>
       </c>
-      <c r="X33" s="565">
+      <c r="X33" s="525">
         <v>3.7</v>
       </c>
-      <c r="Y33" s="565">
+      <c r="Y33" s="525">
         <v>1.9</v>
       </c>
       <c r="AD33" s="471">
@@ -18318,20 +18318,20 @@
       <c r="P34" s="5"/>
       <c r="Q34" s="5"/>
       <c r="R34" s="5"/>
-      <c r="T34" s="562" t="s">
+      <c r="T34" s="522" t="s">
         <v>1059</v>
       </c>
-      <c r="U34" s="561"/>
-      <c r="V34" s="561">
+      <c r="U34" s="521"/>
+      <c r="V34" s="521">
         <v>1387</v>
       </c>
-      <c r="W34" s="561">
+      <c r="W34" s="521">
         <v>2642</v>
       </c>
-      <c r="X34" s="561">
+      <c r="X34" s="521">
         <v>2080</v>
       </c>
-      <c r="Y34" s="561">
+      <c r="Y34" s="521">
         <v>322</v>
       </c>
     </row>
@@ -18339,15 +18339,15 @@
       <c r="A35" s="5" t="s">
         <v>1093</v>
       </c>
-      <c r="B35" s="566">
+      <c r="B35" s="526">
         <f>(B32*8760*B33*B34)</f>
         <v>353203.19999999995</v>
       </c>
-      <c r="C35" s="566">
+      <c r="C35" s="526">
         <f>(C32*8760*C33*C34)</f>
         <v>1530547.2</v>
       </c>
-      <c r="D35" s="566">
+      <c r="D35" s="526">
         <f>(D32*8760*D33*D34)</f>
         <v>1893561.5999999999</v>
       </c>
@@ -18365,23 +18365,23 @@
       <c r="P35" s="5"/>
       <c r="Q35" s="5"/>
       <c r="R35" s="5"/>
-      <c r="T35" s="562" t="s">
+      <c r="T35" s="522" t="s">
         <v>1060</v>
       </c>
-      <c r="U35" s="561"/>
-      <c r="V35" s="600">
+      <c r="U35" s="521"/>
+      <c r="V35" s="554">
         <f t="shared" ref="V35:X35" si="0">V34*110%</f>
         <v>1525.7</v>
       </c>
-      <c r="W35" s="600">
+      <c r="W35" s="554">
         <f>W34*110%</f>
         <v>2906.2000000000003</v>
       </c>
-      <c r="X35" s="600">
+      <c r="X35" s="554">
         <f t="shared" si="0"/>
         <v>2288</v>
       </c>
-      <c r="Y35" s="600">
+      <c r="Y35" s="554">
         <f>Y34*110%</f>
         <v>354.20000000000005</v>
       </c>
@@ -18390,15 +18390,15 @@
       <c r="A36" s="5" t="s">
         <v>1064</v>
       </c>
-      <c r="B36" s="587">
+      <c r="B36" s="541">
         <f>B35/10^6</f>
         <v>0.35320319999999994</v>
       </c>
-      <c r="C36" s="587">
+      <c r="C36" s="541">
         <f>C35/10^6</f>
         <v>1.5305472</v>
       </c>
-      <c r="D36" s="587">
+      <c r="D36" s="541">
         <f>D35/10^6</f>
         <v>1.8935616</v>
       </c>
@@ -18416,26 +18416,26 @@
       <c r="P36" s="5"/>
       <c r="Q36" s="5"/>
       <c r="R36" s="5"/>
-      <c r="T36" s="566"/>
-      <c r="U36" s="566"/>
-      <c r="V36" s="566"/>
-      <c r="W36" s="566"/>
-      <c r="X36" s="566"/>
-      <c r="Y36" s="566"/>
+      <c r="T36" s="526"/>
+      <c r="U36" s="526"/>
+      <c r="V36" s="526"/>
+      <c r="W36" s="526"/>
+      <c r="X36" s="526"/>
+      <c r="Y36" s="526"/>
     </row>
     <row r="37" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
         <v>1094</v>
       </c>
-      <c r="B37" s="566">
+      <c r="B37" s="526">
         <f>B36*3600</f>
         <v>1271.5315199999998</v>
       </c>
-      <c r="C37" s="566">
+      <c r="C37" s="526">
         <f>C36*3600</f>
         <v>5509.9699199999995</v>
       </c>
-      <c r="D37" s="566">
+      <c r="D37" s="526">
         <f>D36*3600</f>
         <v>6816.8217599999998</v>
       </c>
@@ -18453,14 +18453,14 @@
       <c r="P37" s="5"/>
       <c r="Q37" s="5"/>
       <c r="R37" s="5"/>
-      <c r="T37" s="566" t="s">
+      <c r="T37" s="526" t="s">
         <v>1061</v>
       </c>
-      <c r="U37" s="566"/>
-      <c r="V37" s="566"/>
-      <c r="W37" s="566"/>
-      <c r="X37" s="566"/>
-      <c r="Y37" s="566"/>
+      <c r="U37" s="526"/>
+      <c r="V37" s="526"/>
+      <c r="W37" s="526"/>
+      <c r="X37" s="526"/>
+      <c r="Y37" s="526"/>
     </row>
     <row r="38" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
@@ -18474,7 +18474,7 @@
         <f>C37/1000</f>
         <v>5.5099699199999996</v>
       </c>
-      <c r="D38" s="604">
+      <c r="D38" s="558">
         <f>D37/1000</f>
         <v>6.8168217599999998</v>
       </c>
@@ -18520,12 +18520,12 @@
       </c>
     </row>
     <row r="40" spans="1:30" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="585" t="s">
+      <c r="A40" s="601" t="s">
         <v>1068</v>
       </c>
-      <c r="B40" s="585"/>
-      <c r="C40" s="585"/>
-      <c r="D40" s="585"/>
+      <c r="B40" s="601"/>
+      <c r="C40" s="601"/>
+      <c r="D40" s="601"/>
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
@@ -18563,14 +18563,14 @@
       </c>
     </row>
     <row r="41" spans="1:30" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="586" t="s">
+      <c r="A41" s="540" t="s">
         <v>1070</v>
       </c>
-      <c r="B41" s="586">
+      <c r="B41" s="540">
         <v>2015</v>
       </c>
       <c r="C41" s="5"/>
-      <c r="D41" s="586">
+      <c r="D41" s="540">
         <v>2030</v>
       </c>
       <c r="E41" s="5"/>
@@ -18619,7 +18619,7 @@
         <v>15.856999999999999</v>
       </c>
       <c r="C42" s="5"/>
-      <c r="D42" s="605">
+      <c r="D42" s="559">
         <f>B42</f>
         <v>15.856999999999999</v>
       </c>
@@ -18701,12 +18701,12 @@
       <c r="T44" s="5"/>
     </row>
     <row r="45" spans="1:30" ht="15" x14ac:dyDescent="0.25">
-      <c r="A45" s="585" t="s">
+      <c r="A45" s="601" t="s">
         <v>1096</v>
       </c>
-      <c r="B45" s="585"/>
-      <c r="C45" s="585"/>
-      <c r="D45" s="585"/>
+      <c r="B45" s="601"/>
+      <c r="C45" s="601"/>
+      <c r="D45" s="601"/>
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
       <c r="G45" s="5"/>
@@ -18725,20 +18725,20 @@
       <c r="T45" s="5"/>
     </row>
     <row r="46" spans="1:30" ht="15" x14ac:dyDescent="0.25">
-      <c r="A46" s="586" t="s">
+      <c r="A46" s="540" t="s">
         <v>1070</v>
       </c>
-      <c r="B46" s="586">
+      <c r="B46" s="540">
         <v>2018</v>
       </c>
-      <c r="C46" s="586">
+      <c r="C46" s="540">
         <v>2020</v>
       </c>
-      <c r="D46" s="586">
+      <c r="D46" s="540">
         <v>2030</v>
       </c>
       <c r="E46" s="5"/>
-      <c r="F46" s="586" t="s">
+      <c r="F46" s="540" t="s">
         <v>1097</v>
       </c>
       <c r="G46" s="5"/>
@@ -18790,17 +18790,17 @@
       </c>
     </row>
     <row r="48" spans="1:30" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="590" t="s">
+      <c r="A48" s="544" t="s">
         <v>1099</v>
       </c>
-      <c r="B48" s="591">
+      <c r="B48" s="545">
         <v>0.5</v>
       </c>
-      <c r="C48" s="591">
+      <c r="C48" s="545">
         <f>B48</f>
         <v>0.5</v>
       </c>
-      <c r="D48" s="591">
+      <c r="D48" s="545">
         <f>C48</f>
         <v>0.5</v>
       </c>
@@ -18823,11 +18823,11 @@
       <c r="Y48" t="s">
         <v>1113</v>
       </c>
-      <c r="Z48" s="606" t="s">
+      <c r="Z48" s="602" t="s">
         <v>1051</v>
       </c>
-      <c r="AA48" s="607"/>
-      <c r="AB48" s="607"/>
+      <c r="AA48" s="603"/>
+      <c r="AB48" s="603"/>
     </row>
     <row r="49" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
@@ -18961,15 +18961,15 @@
       <c r="A52" s="5" t="s">
         <v>1103</v>
       </c>
-      <c r="B52" s="587">
+      <c r="B52" s="541">
         <f>B51/10^6</f>
         <v>1.752</v>
       </c>
-      <c r="C52" s="587">
+      <c r="C52" s="541">
         <f>C51/10^6</f>
         <v>3.0659999999999998</v>
       </c>
-      <c r="D52" s="587">
+      <c r="D52" s="541">
         <f>D51/10^6</f>
         <v>6.1319999999999997</v>
       </c>
@@ -18993,7 +18993,7 @@
       <c r="V52" s="5"/>
       <c r="W52" s="5"/>
       <c r="X52" s="5"/>
-      <c r="Y52" s="608" t="s">
+      <c r="Y52" s="560" t="s">
         <v>1118</v>
       </c>
       <c r="Z52">
@@ -19009,15 +19009,15 @@
       <c r="A53" s="5" t="s">
         <v>1104</v>
       </c>
-      <c r="B53" s="566">
+      <c r="B53" s="526">
         <f>B52*3600</f>
         <v>6307.2</v>
       </c>
-      <c r="C53" s="566">
+      <c r="C53" s="526">
         <f>C52*3600</f>
         <v>11037.599999999999</v>
       </c>
-      <c r="D53" s="566">
+      <c r="D53" s="526">
         <f>D52*3600</f>
         <v>22075.199999999997</v>
       </c>
@@ -19044,11 +19044,11 @@
       <c r="Y53" t="s">
         <v>1115</v>
       </c>
-      <c r="Z53" s="606" t="s">
+      <c r="Z53" s="602" t="s">
         <v>1050</v>
       </c>
-      <c r="AA53" s="607"/>
-      <c r="AB53" s="607"/>
+      <c r="AA53" s="603"/>
+      <c r="AB53" s="603"/>
     </row>
     <row r="54" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A54" s="5" t="s">
@@ -19062,7 +19062,7 @@
         <f>C53/1000</f>
         <v>11.037599999999999</v>
       </c>
-      <c r="D54" s="604">
+      <c r="D54" s="558">
         <f>D53/1000</f>
         <v>22.075199999999999</v>
       </c>
@@ -19181,20 +19181,20 @@
       <c r="R57" s="5"/>
       <c r="S57" s="5"/>
       <c r="T57" s="5"/>
-      <c r="Y57" s="608" t="s">
+      <c r="Y57" s="560" t="s">
         <v>1118</v>
       </c>
       <c r="AA57" s="5"/>
     </row>
     <row r="58" spans="1:28" ht="15" x14ac:dyDescent="0.25">
-      <c r="A58" s="592" t="str">
+      <c r="A58" s="546" t="str">
         <f>A54</f>
         <v>Excess Heat Production (PJ)</v>
       </c>
-      <c r="B58" s="592">
+      <c r="B58" s="546">
         <v>2020</v>
       </c>
-      <c r="C58" s="592">
+      <c r="C58" s="546">
         <v>2030</v>
       </c>
       <c r="D58" s="5"/>
@@ -19216,15 +19216,15 @@
       <c r="T58" s="5"/>
     </row>
     <row r="59" spans="1:28" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="593" t="str">
+      <c r="A59" s="547" t="str">
         <f>A7</f>
         <v>Power Plants</v>
       </c>
-      <c r="B59" s="594">
+      <c r="B59" s="548">
         <f>C16</f>
         <v>55.12319999999999</v>
       </c>
-      <c r="C59" s="594">
+      <c r="C59" s="548">
         <f>D16</f>
         <v>31.363200000000003</v>
       </c>
@@ -19255,22 +19255,22 @@
       <c r="Y59" t="s">
         <v>1116</v>
       </c>
-      <c r="Z59" s="606" t="s">
+      <c r="Z59" s="602" t="s">
         <v>1117</v>
       </c>
-      <c r="AA59" s="607"/>
-      <c r="AB59" s="607"/>
+      <c r="AA59" s="603"/>
+      <c r="AB59" s="603"/>
     </row>
     <row r="60" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A60" s="593" t="str">
+      <c r="A60" s="547" t="str">
         <f>A18</f>
         <v>Excess Renewable Electricity via Heat Pump</v>
       </c>
-      <c r="B60" s="595">
+      <c r="B60" s="549">
         <f>C26</f>
         <v>20.047670103092784</v>
       </c>
-      <c r="C60" s="595">
+      <c r="C60" s="549">
         <f>D26</f>
         <v>30.491999999999997</v>
       </c>
@@ -19306,15 +19306,15 @@
       </c>
     </row>
     <row r="61" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A61" s="593" t="str">
+      <c r="A61" s="547" t="str">
         <f>A28</f>
         <v>Waste Incinteration</v>
       </c>
-      <c r="B61" s="594">
+      <c r="B61" s="548">
         <f>C38</f>
         <v>5.5099699199999996</v>
       </c>
-      <c r="C61" s="594">
+      <c r="C61" s="548">
         <f>D38</f>
         <v>6.8168217599999998</v>
       </c>
@@ -19350,15 +19350,15 @@
       </c>
     </row>
     <row r="62" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A62" s="593" t="str">
+      <c r="A62" s="547" t="str">
         <f>A40</f>
         <v>Industrial Excess Heat</v>
       </c>
-      <c r="B62" s="594">
+      <c r="B62" s="548">
         <f>B42</f>
         <v>15.856999999999999</v>
       </c>
-      <c r="C62" s="594">
+      <c r="C62" s="548">
         <f>D42</f>
         <v>15.856999999999999</v>
       </c>
@@ -19390,15 +19390,15 @@
       </c>
     </row>
     <row r="63" spans="1:28" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="596" t="str">
+      <c r="A63" s="550" t="str">
         <f>A45</f>
         <v>Data Centres</v>
       </c>
-      <c r="B63" s="597">
+      <c r="B63" s="551">
         <f>C54</f>
         <v>11.037599999999999</v>
       </c>
-      <c r="C63" s="597">
+      <c r="C63" s="551">
         <f>D54</f>
         <v>22.075199999999999</v>
       </c>
@@ -19422,19 +19422,19 @@
       <c r="U63" s="5">
         <v>18482</v>
       </c>
-      <c r="Y63" s="608" t="s">
+      <c r="Y63" s="560" t="s">
         <v>1118</v>
       </c>
     </row>
     <row r="64" spans="1:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="598" t="s">
+      <c r="A64" s="552" t="s">
         <v>686</v>
       </c>
-      <c r="B64" s="599">
+      <c r="B64" s="553">
         <f>SUM(B59:B63)</f>
         <v>107.57544002309277</v>
       </c>
-      <c r="C64" s="599">
+      <c r="C64" s="553">
         <f>SUM(C59:C63)</f>
         <v>106.60422175999999</v>
       </c>
@@ -20157,17 +20157,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A18:D18"/>
     <mergeCell ref="A40:D40"/>
     <mergeCell ref="A45:D45"/>
     <mergeCell ref="Z59:AB59"/>
     <mergeCell ref="Z53:AB53"/>
     <mergeCell ref="Z48:AB48"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="G1:K1"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="A28:D28"/>
   </mergeCells>
   <phoneticPr fontId="71" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -20202,16 +20202,16 @@
   <sheetData>
     <row r="1" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:20" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="526" t="s">
+      <c r="B2" s="566" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="527"/>
-      <c r="D2" s="527"/>
-      <c r="E2" s="528"/>
-      <c r="G2" s="526" t="s">
+      <c r="C2" s="567"/>
+      <c r="D2" s="567"/>
+      <c r="E2" s="568"/>
+      <c r="G2" s="566" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="528"/>
+      <c r="H2" s="568"/>
       <c r="I2" s="222"/>
       <c r="J2" s="222"/>
       <c r="K2" s="223"/>
@@ -20553,16 +20553,16 @@
     </row>
     <row r="19" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="2:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="529" t="s">
+      <c r="B20" s="569" t="s">
         <v>70</v>
       </c>
-      <c r="C20" s="530"/>
-      <c r="D20" s="530"/>
-      <c r="E20" s="531"/>
-      <c r="G20" s="526" t="s">
+      <c r="C20" s="570"/>
+      <c r="D20" s="570"/>
+      <c r="E20" s="571"/>
+      <c r="G20" s="566" t="s">
         <v>14</v>
       </c>
-      <c r="H20" s="528"/>
+      <c r="H20" s="568"/>
     </row>
     <row r="21" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="250" t="s">
@@ -20806,16 +20806,16 @@
     </row>
     <row r="37" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="38" spans="2:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="526" t="s">
+      <c r="B38" s="566" t="s">
         <v>78</v>
       </c>
-      <c r="C38" s="527"/>
-      <c r="D38" s="527"/>
-      <c r="E38" s="528"/>
-      <c r="G38" s="532" t="s">
+      <c r="C38" s="567"/>
+      <c r="D38" s="567"/>
+      <c r="E38" s="568"/>
+      <c r="G38" s="572" t="s">
         <v>72</v>
       </c>
-      <c r="H38" s="533"/>
+      <c r="H38" s="573"/>
     </row>
     <row r="39" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B39" s="271" t="s">
@@ -20984,13 +20984,13 @@
       <c r="M3" s="5" t="s">
         <v>390</v>
       </c>
-      <c r="S3" s="534" t="s">
+      <c r="S3" s="574" t="s">
         <v>680</v>
       </c>
-      <c r="T3" s="534"/>
-      <c r="U3" s="534"/>
-      <c r="V3" s="534"/>
-      <c r="W3" s="534"/>
+      <c r="T3" s="574"/>
+      <c r="U3" s="574"/>
+      <c r="V3" s="574"/>
+      <c r="W3" s="574"/>
     </row>
     <row r="4" spans="3:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C4" s="62" t="s">
@@ -21184,10 +21184,10 @@
         <v>5.6296955912135845E-4</v>
       </c>
       <c r="J9" s="103"/>
-      <c r="M9" s="535" t="s">
+      <c r="M9" s="575" t="s">
         <v>110</v>
       </c>
-      <c r="N9" s="535" t="s">
+      <c r="N9" s="575" t="s">
         <v>110</v>
       </c>
       <c r="S9" s="300" t="s">
@@ -28854,34 +28854,34 @@
       <c r="G4" s="62" t="s">
         <v>317</v>
       </c>
-      <c r="H4" s="542" t="s">
+      <c r="H4" s="582" t="s">
         <v>719</v>
       </c>
-      <c r="I4" s="543"/>
-      <c r="J4" s="543"/>
-      <c r="K4" s="544"/>
-      <c r="L4" s="542" t="s">
+      <c r="I4" s="583"/>
+      <c r="J4" s="583"/>
+      <c r="K4" s="584"/>
+      <c r="L4" s="582" t="s">
         <v>319</v>
       </c>
-      <c r="M4" s="543"/>
-      <c r="N4" s="543"/>
-      <c r="O4" s="544"/>
-      <c r="P4" s="542" t="s">
+      <c r="M4" s="583"/>
+      <c r="N4" s="583"/>
+      <c r="O4" s="584"/>
+      <c r="P4" s="582" t="s">
         <v>320</v>
       </c>
-      <c r="Q4" s="543"/>
-      <c r="R4" s="543"/>
-      <c r="S4" s="544"/>
-      <c r="T4" s="542" t="s">
+      <c r="Q4" s="583"/>
+      <c r="R4" s="583"/>
+      <c r="S4" s="584"/>
+      <c r="T4" s="582" t="s">
         <v>321</v>
       </c>
-      <c r="U4" s="544"/>
-      <c r="V4" s="536" t="s">
+      <c r="U4" s="584"/>
+      <c r="V4" s="585" t="s">
         <v>322</v>
       </c>
-      <c r="W4" s="537"/>
-      <c r="X4" s="537"/>
-      <c r="Y4" s="538"/>
+      <c r="W4" s="586"/>
+      <c r="X4" s="586"/>
+      <c r="Y4" s="587"/>
       <c r="Z4" s="106"/>
       <c r="AA4" s="106"/>
       <c r="AB4" s="114" t="s">
@@ -28980,34 +28980,34 @@
       <c r="E6" s="84"/>
       <c r="F6" s="84"/>
       <c r="G6" s="85"/>
-      <c r="H6" s="539" t="s">
+      <c r="H6" s="576" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="540"/>
-      <c r="J6" s="540"/>
-      <c r="K6" s="541"/>
-      <c r="L6" s="540" t="s">
+      <c r="I6" s="577"/>
+      <c r="J6" s="577"/>
+      <c r="K6" s="578"/>
+      <c r="L6" s="577" t="s">
         <v>45</v>
       </c>
-      <c r="M6" s="540"/>
-      <c r="N6" s="540"/>
-      <c r="O6" s="541"/>
-      <c r="P6" s="539" t="s">
+      <c r="M6" s="577"/>
+      <c r="N6" s="577"/>
+      <c r="O6" s="578"/>
+      <c r="P6" s="576" t="s">
         <v>45</v>
       </c>
-      <c r="Q6" s="540"/>
-      <c r="R6" s="540"/>
-      <c r="S6" s="541"/>
-      <c r="T6" s="539" t="s">
+      <c r="Q6" s="577"/>
+      <c r="R6" s="577"/>
+      <c r="S6" s="578"/>
+      <c r="T6" s="576" t="s">
         <v>302</v>
       </c>
-      <c r="U6" s="541"/>
-      <c r="V6" s="539" t="s">
+      <c r="U6" s="578"/>
+      <c r="V6" s="576" t="s">
         <v>967</v>
       </c>
-      <c r="W6" s="540"/>
-      <c r="X6" s="540"/>
-      <c r="Y6" s="541"/>
+      <c r="W6" s="577"/>
+      <c r="X6" s="577"/>
+      <c r="Y6" s="578"/>
       <c r="Z6" s="107" t="s">
         <v>979</v>
       </c>
@@ -31919,34 +31919,34 @@
       <c r="G42" s="62" t="s">
         <v>317</v>
       </c>
-      <c r="H42" s="542" t="s">
+      <c r="H42" s="582" t="s">
         <v>318</v>
       </c>
-      <c r="I42" s="543"/>
-      <c r="J42" s="543"/>
-      <c r="K42" s="544"/>
-      <c r="L42" s="542" t="s">
+      <c r="I42" s="583"/>
+      <c r="J42" s="583"/>
+      <c r="K42" s="584"/>
+      <c r="L42" s="582" t="s">
         <v>319</v>
       </c>
-      <c r="M42" s="543"/>
-      <c r="N42" s="543"/>
-      <c r="O42" s="544"/>
-      <c r="P42" s="542" t="s">
+      <c r="M42" s="583"/>
+      <c r="N42" s="583"/>
+      <c r="O42" s="584"/>
+      <c r="P42" s="582" t="s">
         <v>320</v>
       </c>
-      <c r="Q42" s="543"/>
-      <c r="R42" s="543"/>
-      <c r="S42" s="544"/>
-      <c r="T42" s="542" t="s">
+      <c r="Q42" s="583"/>
+      <c r="R42" s="583"/>
+      <c r="S42" s="584"/>
+      <c r="T42" s="582" t="s">
         <v>321</v>
       </c>
-      <c r="U42" s="544"/>
-      <c r="V42" s="536" t="s">
+      <c r="U42" s="584"/>
+      <c r="V42" s="585" t="s">
         <v>322</v>
       </c>
-      <c r="W42" s="537"/>
-      <c r="X42" s="537"/>
-      <c r="Y42" s="538"/>
+      <c r="W42" s="586"/>
+      <c r="X42" s="586"/>
+      <c r="Y42" s="587"/>
       <c r="Z42" s="106"/>
       <c r="AA42" s="106"/>
       <c r="AB42" s="114" t="s">
@@ -32045,34 +32045,34 @@
       <c r="E44" s="84"/>
       <c r="F44" s="84"/>
       <c r="G44" s="85"/>
-      <c r="H44" s="539" t="s">
+      <c r="H44" s="576" t="s">
         <v>45</v>
       </c>
-      <c r="I44" s="540"/>
-      <c r="J44" s="540"/>
-      <c r="K44" s="541"/>
-      <c r="L44" s="540" t="s">
+      <c r="I44" s="577"/>
+      <c r="J44" s="577"/>
+      <c r="K44" s="578"/>
+      <c r="L44" s="577" t="s">
         <v>45</v>
       </c>
-      <c r="M44" s="540"/>
-      <c r="N44" s="540"/>
-      <c r="O44" s="541"/>
-      <c r="P44" s="539" t="s">
+      <c r="M44" s="577"/>
+      <c r="N44" s="577"/>
+      <c r="O44" s="578"/>
+      <c r="P44" s="576" t="s">
         <v>45</v>
       </c>
-      <c r="Q44" s="540"/>
-      <c r="R44" s="540"/>
-      <c r="S44" s="541"/>
-      <c r="T44" s="545" t="s">
+      <c r="Q44" s="577"/>
+      <c r="R44" s="577"/>
+      <c r="S44" s="578"/>
+      <c r="T44" s="579" t="s">
         <v>302</v>
       </c>
-      <c r="U44" s="546"/>
-      <c r="V44" s="545" t="s">
+      <c r="U44" s="580"/>
+      <c r="V44" s="579" t="s">
         <v>967</v>
       </c>
-      <c r="W44" s="547"/>
-      <c r="X44" s="547"/>
-      <c r="Y44" s="546"/>
+      <c r="W44" s="581"/>
+      <c r="X44" s="581"/>
+      <c r="Y44" s="580"/>
       <c r="Z44" s="450" t="s">
         <v>979</v>
       </c>
@@ -35841,34 +35841,34 @@
       <c r="G90" s="62" t="s">
         <v>317</v>
       </c>
-      <c r="H90" s="542" t="s">
+      <c r="H90" s="582" t="s">
         <v>318</v>
       </c>
-      <c r="I90" s="543"/>
-      <c r="J90" s="543"/>
-      <c r="K90" s="544"/>
-      <c r="L90" s="542" t="s">
+      <c r="I90" s="583"/>
+      <c r="J90" s="583"/>
+      <c r="K90" s="584"/>
+      <c r="L90" s="582" t="s">
         <v>319</v>
       </c>
-      <c r="M90" s="543"/>
-      <c r="N90" s="543"/>
-      <c r="O90" s="544"/>
-      <c r="P90" s="542" t="s">
+      <c r="M90" s="583"/>
+      <c r="N90" s="583"/>
+      <c r="O90" s="584"/>
+      <c r="P90" s="582" t="s">
         <v>320</v>
       </c>
-      <c r="Q90" s="543"/>
-      <c r="R90" s="543"/>
-      <c r="S90" s="544"/>
-      <c r="T90" s="542" t="s">
+      <c r="Q90" s="583"/>
+      <c r="R90" s="583"/>
+      <c r="S90" s="584"/>
+      <c r="T90" s="582" t="s">
         <v>321</v>
       </c>
-      <c r="U90" s="544"/>
-      <c r="V90" s="536" t="s">
+      <c r="U90" s="584"/>
+      <c r="V90" s="585" t="s">
         <v>322</v>
       </c>
-      <c r="W90" s="537"/>
-      <c r="X90" s="537"/>
-      <c r="Y90" s="538"/>
+      <c r="W90" s="586"/>
+      <c r="X90" s="586"/>
+      <c r="Y90" s="587"/>
       <c r="Z90" s="106"/>
       <c r="AA90" s="106"/>
       <c r="AB90" s="114" t="s">
@@ -35967,34 +35967,34 @@
       <c r="E92" s="84"/>
       <c r="F92" s="84"/>
       <c r="G92" s="85"/>
-      <c r="H92" s="539" t="s">
+      <c r="H92" s="576" t="s">
         <v>45</v>
       </c>
-      <c r="I92" s="540"/>
-      <c r="J92" s="540"/>
-      <c r="K92" s="541"/>
-      <c r="L92" s="540" t="s">
+      <c r="I92" s="577"/>
+      <c r="J92" s="577"/>
+      <c r="K92" s="578"/>
+      <c r="L92" s="577" t="s">
         <v>45</v>
       </c>
-      <c r="M92" s="540"/>
-      <c r="N92" s="540"/>
-      <c r="O92" s="541"/>
-      <c r="P92" s="539" t="s">
+      <c r="M92" s="577"/>
+      <c r="N92" s="577"/>
+      <c r="O92" s="578"/>
+      <c r="P92" s="576" t="s">
         <v>45</v>
       </c>
-      <c r="Q92" s="540"/>
-      <c r="R92" s="540"/>
-      <c r="S92" s="541"/>
-      <c r="T92" s="545" t="s">
+      <c r="Q92" s="577"/>
+      <c r="R92" s="577"/>
+      <c r="S92" s="578"/>
+      <c r="T92" s="579" t="s">
         <v>302</v>
       </c>
-      <c r="U92" s="546"/>
-      <c r="V92" s="545" t="s">
+      <c r="U92" s="580"/>
+      <c r="V92" s="579" t="s">
         <v>967</v>
       </c>
-      <c r="W92" s="547"/>
-      <c r="X92" s="547"/>
-      <c r="Y92" s="546"/>
+      <c r="W92" s="581"/>
+      <c r="X92" s="581"/>
+      <c r="Y92" s="580"/>
       <c r="Z92" s="450" t="s">
         <v>979</v>
       </c>
@@ -39925,26 +39925,6 @@
     <row r="166" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="H92:K92"/>
-    <mergeCell ref="L92:O92"/>
-    <mergeCell ref="P92:S92"/>
-    <mergeCell ref="T92:U92"/>
-    <mergeCell ref="V92:Y92"/>
-    <mergeCell ref="H90:K90"/>
-    <mergeCell ref="L90:O90"/>
-    <mergeCell ref="P90:S90"/>
-    <mergeCell ref="T90:U90"/>
-    <mergeCell ref="V90:Y90"/>
-    <mergeCell ref="H44:K44"/>
-    <mergeCell ref="L44:O44"/>
-    <mergeCell ref="P44:S44"/>
-    <mergeCell ref="T44:U44"/>
-    <mergeCell ref="V44:Y44"/>
-    <mergeCell ref="H42:K42"/>
-    <mergeCell ref="L42:O42"/>
-    <mergeCell ref="P42:S42"/>
-    <mergeCell ref="T42:U42"/>
-    <mergeCell ref="V42:Y42"/>
     <mergeCell ref="V4:Y4"/>
     <mergeCell ref="V6:Y6"/>
     <mergeCell ref="H4:K4"/>
@@ -39955,6 +39935,26 @@
     <mergeCell ref="P6:S6"/>
     <mergeCell ref="L6:O6"/>
     <mergeCell ref="H6:K6"/>
+    <mergeCell ref="H42:K42"/>
+    <mergeCell ref="L42:O42"/>
+    <mergeCell ref="P42:S42"/>
+    <mergeCell ref="T42:U42"/>
+    <mergeCell ref="V42:Y42"/>
+    <mergeCell ref="H44:K44"/>
+    <mergeCell ref="L44:O44"/>
+    <mergeCell ref="P44:S44"/>
+    <mergeCell ref="T44:U44"/>
+    <mergeCell ref="V44:Y44"/>
+    <mergeCell ref="H90:K90"/>
+    <mergeCell ref="L90:O90"/>
+    <mergeCell ref="P90:S90"/>
+    <mergeCell ref="T90:U90"/>
+    <mergeCell ref="V90:Y90"/>
+    <mergeCell ref="H92:K92"/>
+    <mergeCell ref="L92:O92"/>
+    <mergeCell ref="P92:S92"/>
+    <mergeCell ref="T92:U92"/>
+    <mergeCell ref="V92:Y92"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>
@@ -40099,12 +40099,12 @@
       <c r="I5" s="173"/>
       <c r="J5" s="173"/>
       <c r="K5" s="173"/>
-      <c r="L5" s="536" t="s">
+      <c r="L5" s="585" t="s">
         <v>322</v>
       </c>
-      <c r="M5" s="537"/>
-      <c r="N5" s="537"/>
-      <c r="O5" s="538"/>
+      <c r="M5" s="586"/>
+      <c r="N5" s="586"/>
+      <c r="O5" s="587"/>
       <c r="P5" s="106"/>
       <c r="Q5" s="106" t="s">
         <v>323</v>
@@ -40135,12 +40135,12 @@
       <c r="I6" s="83"/>
       <c r="J6" s="83"/>
       <c r="K6" s="83"/>
-      <c r="L6" s="545" t="s">
+      <c r="L6" s="579" t="s">
         <v>967</v>
       </c>
-      <c r="M6" s="547"/>
-      <c r="N6" s="547"/>
-      <c r="O6" s="546"/>
+      <c r="M6" s="581"/>
+      <c r="N6" s="581"/>
+      <c r="O6" s="580"/>
       <c r="P6" s="450" t="s">
         <v>979</v>
       </c>
@@ -40766,10 +40766,10 @@
       <c r="C18" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="R18" s="548" t="s">
+      <c r="R18" s="588" t="s">
         <v>662</v>
       </c>
-      <c r="S18" s="548"/>
+      <c r="S18" s="588"/>
       <c r="U18" s="5" t="s">
         <v>860</v>
       </c>
@@ -40802,8 +40802,8 @@
       <c r="J19" s="195" t="s">
         <v>301</v>
       </c>
-      <c r="R19" s="548"/>
-      <c r="S19" s="548"/>
+      <c r="R19" s="588"/>
+      <c r="S19" s="588"/>
       <c r="V19" s="5" t="s">
         <v>1021</v>
       </c>
@@ -40829,8 +40829,8 @@
       <c r="J20" s="170" t="s">
         <v>1026</v>
       </c>
-      <c r="R20" s="548"/>
-      <c r="S20" s="548"/>
+      <c r="R20" s="588"/>
+      <c r="S20" s="588"/>
       <c r="V20" s="5" t="s">
         <v>1022</v>
       </c>
@@ -40857,8 +40857,8 @@
       <c r="J21" s="170" t="s">
         <v>1026</v>
       </c>
-      <c r="R21" s="548"/>
-      <c r="S21" s="548"/>
+      <c r="R21" s="588"/>
+      <c r="S21" s="588"/>
     </row>
     <row r="22" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C22" s="168" t="s">
@@ -40882,8 +40882,8 @@
       <c r="J22" s="170" t="s">
         <v>1026</v>
       </c>
-      <c r="R22" s="548"/>
-      <c r="S22" s="548"/>
+      <c r="R22" s="588"/>
+      <c r="S22" s="588"/>
     </row>
     <row r="23" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C23" s="168" t="s">
@@ -41058,23 +41058,23 @@
       <c r="K33" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="L33" s="536" t="s">
+      <c r="L33" s="585" t="s">
         <v>322</v>
       </c>
-      <c r="M33" s="537"/>
-      <c r="N33" s="537"/>
-      <c r="O33" s="538"/>
+      <c r="M33" s="586"/>
+      <c r="N33" s="586"/>
+      <c r="O33" s="587"/>
     </row>
     <row r="34" spans="8:15" x14ac:dyDescent="0.2">
       <c r="H34" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="L34" s="545" t="s">
+      <c r="L34" s="579" t="s">
         <v>327</v>
       </c>
-      <c r="M34" s="547"/>
-      <c r="N34" s="547"/>
-      <c r="O34" s="546"/>
+      <c r="M34" s="581"/>
+      <c r="N34" s="581"/>
+      <c r="O34" s="580"/>
     </row>
     <row r="35" spans="8:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H35" s="5" t="s">
@@ -41416,16 +41416,16 @@
       <c r="G4" s="173" t="s">
         <v>321</v>
       </c>
-      <c r="H4" s="542" t="s">
+      <c r="H4" s="582" t="s">
         <v>110</v>
       </c>
-      <c r="I4" s="543"/>
-      <c r="J4" s="544"/>
-      <c r="K4" s="536" t="s">
+      <c r="I4" s="583"/>
+      <c r="J4" s="584"/>
+      <c r="K4" s="585" t="s">
         <v>322</v>
       </c>
-      <c r="L4" s="537"/>
-      <c r="M4" s="538"/>
+      <c r="L4" s="586"/>
+      <c r="M4" s="587"/>
       <c r="N4" s="106"/>
       <c r="O4" s="106" t="s">
         <v>323</v>
@@ -41451,16 +41451,16 @@
       <c r="G5" s="458" t="s">
         <v>302</v>
       </c>
-      <c r="H5" s="549" t="s">
+      <c r="H5" s="592" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="550"/>
-      <c r="J5" s="551"/>
-      <c r="K5" s="549" t="s">
+      <c r="I5" s="593"/>
+      <c r="J5" s="594"/>
+      <c r="K5" s="592" t="s">
         <v>756</v>
       </c>
-      <c r="L5" s="550"/>
-      <c r="M5" s="551"/>
+      <c r="L5" s="593"/>
+      <c r="M5" s="594"/>
       <c r="N5" s="459" t="s">
         <v>328</v>
       </c>
@@ -41477,23 +41477,23 @@
         <v>626</v>
       </c>
       <c r="AA5" s="281"/>
-      <c r="AB5" s="552" t="s">
+      <c r="AB5" s="589" t="s">
         <v>1011</v>
       </c>
-      <c r="AC5" s="552"/>
+      <c r="AC5" s="589"/>
       <c r="AD5" s="461"/>
-      <c r="AE5" s="553" t="s">
+      <c r="AE5" s="590" t="s">
         <v>110</v>
       </c>
-      <c r="AF5" s="553"/>
-      <c r="AG5" s="553" t="s">
+      <c r="AF5" s="590"/>
+      <c r="AG5" s="590" t="s">
         <v>1012</v>
       </c>
-      <c r="AH5" s="553"/>
-      <c r="AI5" s="554" t="s">
+      <c r="AH5" s="590"/>
+      <c r="AI5" s="591" t="s">
         <v>1013</v>
       </c>
-      <c r="AJ5" s="554"/>
+      <c r="AJ5" s="591"/>
     </row>
     <row r="6" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C6" s="505" t="str">
@@ -42231,12 +42231,12 @@
       <c r="K27" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="L27" s="536" t="s">
+      <c r="L27" s="585" t="s">
         <v>322</v>
       </c>
-      <c r="M27" s="537"/>
-      <c r="N27" s="537"/>
-      <c r="O27" s="538"/>
+      <c r="M27" s="586"/>
+      <c r="N27" s="586"/>
+      <c r="O27" s="587"/>
       <c r="T27" s="283"/>
       <c r="U27" s="283"/>
     </row>
@@ -42244,12 +42244,12 @@
       <c r="J28" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="L28" s="539" t="s">
+      <c r="L28" s="576" t="s">
         <v>327</v>
       </c>
-      <c r="M28" s="540"/>
-      <c r="N28" s="540"/>
-      <c r="O28" s="541"/>
+      <c r="M28" s="577"/>
+      <c r="N28" s="577"/>
+      <c r="O28" s="578"/>
       <c r="T28" s="283"/>
       <c r="U28" s="283"/>
     </row>
@@ -43639,16 +43639,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="L28:O28"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="K5:M5"/>
     <mergeCell ref="AB5:AC5"/>
     <mergeCell ref="AE5:AF5"/>
     <mergeCell ref="AG5:AH5"/>
     <mergeCell ref="AI5:AJ5"/>
     <mergeCell ref="L27:O27"/>
-    <mergeCell ref="L28:O28"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="K5:M5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="S7" r:id="rId1" xr:uid="{B1EDD63D-40A5-4174-9D28-8666BD314B83}"/>
@@ -52678,128 +52678,128 @@
       <c r="C4" s="356" t="s">
         <v>765</v>
       </c>
-      <c r="D4" s="555" t="s">
+      <c r="D4" s="596" t="s">
         <v>766</v>
       </c>
-      <c r="E4" s="556"/>
-      <c r="F4" s="556"/>
-      <c r="G4" s="556"/>
-      <c r="H4" s="557"/>
-      <c r="I4" s="556" t="s">
+      <c r="E4" s="595"/>
+      <c r="F4" s="595"/>
+      <c r="G4" s="595"/>
+      <c r="H4" s="597"/>
+      <c r="I4" s="595" t="s">
         <v>767</v>
       </c>
-      <c r="J4" s="556"/>
-      <c r="K4" s="556"/>
-      <c r="L4" s="556"/>
-      <c r="M4" s="557"/>
-      <c r="N4" s="556" t="s">
+      <c r="J4" s="595"/>
+      <c r="K4" s="595"/>
+      <c r="L4" s="595"/>
+      <c r="M4" s="597"/>
+      <c r="N4" s="595" t="s">
         <v>768</v>
       </c>
-      <c r="O4" s="556"/>
-      <c r="P4" s="556"/>
-      <c r="Q4" s="556"/>
-      <c r="R4" s="557"/>
-      <c r="S4" s="556" t="s">
+      <c r="O4" s="595"/>
+      <c r="P4" s="595"/>
+      <c r="Q4" s="595"/>
+      <c r="R4" s="597"/>
+      <c r="S4" s="595" t="s">
         <v>769</v>
       </c>
-      <c r="T4" s="556"/>
-      <c r="U4" s="556"/>
-      <c r="V4" s="556"/>
-      <c r="W4" s="557"/>
-      <c r="X4" s="556" t="s">
+      <c r="T4" s="595"/>
+      <c r="U4" s="595"/>
+      <c r="V4" s="595"/>
+      <c r="W4" s="597"/>
+      <c r="X4" s="595" t="s">
         <v>770</v>
       </c>
-      <c r="Y4" s="556"/>
-      <c r="Z4" s="556"/>
-      <c r="AA4" s="556"/>
-      <c r="AB4" s="557"/>
-      <c r="AC4" s="556" t="s">
+      <c r="Y4" s="595"/>
+      <c r="Z4" s="595"/>
+      <c r="AA4" s="595"/>
+      <c r="AB4" s="597"/>
+      <c r="AC4" s="595" t="s">
         <v>771</v>
       </c>
-      <c r="AD4" s="556"/>
-      <c r="AE4" s="556"/>
-      <c r="AF4" s="556"/>
-      <c r="AG4" s="557"/>
-      <c r="AH4" s="556" t="s">
+      <c r="AD4" s="595"/>
+      <c r="AE4" s="595"/>
+      <c r="AF4" s="595"/>
+      <c r="AG4" s="597"/>
+      <c r="AH4" s="595" t="s">
         <v>772</v>
       </c>
-      <c r="AI4" s="556"/>
-      <c r="AJ4" s="556"/>
-      <c r="AK4" s="556"/>
-      <c r="AL4" s="557"/>
-      <c r="AM4" s="556" t="s">
+      <c r="AI4" s="595"/>
+      <c r="AJ4" s="595"/>
+      <c r="AK4" s="595"/>
+      <c r="AL4" s="597"/>
+      <c r="AM4" s="595" t="s">
         <v>773</v>
       </c>
-      <c r="AN4" s="556"/>
-      <c r="AO4" s="556"/>
-      <c r="AP4" s="556"/>
-      <c r="AQ4" s="557"/>
-      <c r="AR4" s="556" t="s">
+      <c r="AN4" s="595"/>
+      <c r="AO4" s="595"/>
+      <c r="AP4" s="595"/>
+      <c r="AQ4" s="597"/>
+      <c r="AR4" s="595" t="s">
         <v>774</v>
       </c>
-      <c r="AS4" s="556"/>
-      <c r="AT4" s="556"/>
-      <c r="AU4" s="556"/>
-      <c r="AV4" s="557"/>
-      <c r="AW4" s="556" t="s">
+      <c r="AS4" s="595"/>
+      <c r="AT4" s="595"/>
+      <c r="AU4" s="595"/>
+      <c r="AV4" s="597"/>
+      <c r="AW4" s="595" t="s">
         <v>775</v>
       </c>
-      <c r="AX4" s="556"/>
-      <c r="AY4" s="556"/>
-      <c r="AZ4" s="556"/>
-      <c r="BA4" s="556"/>
-      <c r="BB4" s="555" t="s">
+      <c r="AX4" s="595"/>
+      <c r="AY4" s="595"/>
+      <c r="AZ4" s="595"/>
+      <c r="BA4" s="595"/>
+      <c r="BB4" s="596" t="s">
         <v>776</v>
       </c>
-      <c r="BC4" s="556"/>
-      <c r="BD4" s="556"/>
-      <c r="BE4" s="556"/>
-      <c r="BF4" s="557"/>
-      <c r="BG4" s="556" t="s">
+      <c r="BC4" s="595"/>
+      <c r="BD4" s="595"/>
+      <c r="BE4" s="595"/>
+      <c r="BF4" s="597"/>
+      <c r="BG4" s="595" t="s">
         <v>777</v>
       </c>
-      <c r="BH4" s="556"/>
-      <c r="BI4" s="556"/>
-      <c r="BJ4" s="556"/>
-      <c r="BK4" s="556"/>
-      <c r="BL4" s="555" t="s">
+      <c r="BH4" s="595"/>
+      <c r="BI4" s="595"/>
+      <c r="BJ4" s="595"/>
+      <c r="BK4" s="595"/>
+      <c r="BL4" s="596" t="s">
         <v>778</v>
       </c>
-      <c r="BM4" s="556"/>
-      <c r="BN4" s="556"/>
-      <c r="BO4" s="556"/>
-      <c r="BP4" s="556"/>
-      <c r="BQ4" s="555" t="s">
+      <c r="BM4" s="595"/>
+      <c r="BN4" s="595"/>
+      <c r="BO4" s="595"/>
+      <c r="BP4" s="595"/>
+      <c r="BQ4" s="596" t="s">
         <v>779</v>
       </c>
-      <c r="BR4" s="556"/>
-      <c r="BS4" s="556"/>
-      <c r="BT4" s="556"/>
-      <c r="BU4" s="557"/>
+      <c r="BR4" s="595"/>
+      <c r="BS4" s="595"/>
+      <c r="BT4" s="595"/>
+      <c r="BU4" s="597"/>
       <c r="BV4" s="357" t="s">
         <v>780</v>
       </c>
-      <c r="BW4" s="558" t="s">
+      <c r="BW4" s="598" t="s">
         <v>781</v>
       </c>
-      <c r="BX4" s="559"/>
-      <c r="BY4" s="559"/>
-      <c r="BZ4" s="559"/>
-      <c r="CA4" s="560"/>
-      <c r="CB4" s="558" t="s">
+      <c r="BX4" s="599"/>
+      <c r="BY4" s="599"/>
+      <c r="BZ4" s="599"/>
+      <c r="CA4" s="600"/>
+      <c r="CB4" s="598" t="s">
         <v>782</v>
       </c>
-      <c r="CC4" s="559"/>
-      <c r="CD4" s="559"/>
-      <c r="CE4" s="559"/>
-      <c r="CF4" s="560"/>
-      <c r="CG4" s="558" t="s">
+      <c r="CC4" s="599"/>
+      <c r="CD4" s="599"/>
+      <c r="CE4" s="599"/>
+      <c r="CF4" s="600"/>
+      <c r="CG4" s="598" t="s">
         <v>783</v>
       </c>
-      <c r="CH4" s="559"/>
-      <c r="CI4" s="559"/>
-      <c r="CJ4" s="559"/>
-      <c r="CK4" s="560"/>
+      <c r="CH4" s="599"/>
+      <c r="CI4" s="599"/>
+      <c r="CJ4" s="599"/>
+      <c r="CK4" s="600"/>
     </row>
     <row r="5" spans="1:89" x14ac:dyDescent="0.2">
       <c r="A5" s="359"/>
@@ -66368,6 +66368,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="BL4:BP4"/>
+    <mergeCell ref="BQ4:BU4"/>
+    <mergeCell ref="BW4:CA4"/>
+    <mergeCell ref="CB4:CF4"/>
+    <mergeCell ref="CG4:CK4"/>
     <mergeCell ref="BG4:BK4"/>
     <mergeCell ref="D4:H4"/>
     <mergeCell ref="I4:M4"/>
@@ -66380,11 +66385,6 @@
     <mergeCell ref="AR4:AV4"/>
     <mergeCell ref="AW4:BA4"/>
     <mergeCell ref="BB4:BF4"/>
-    <mergeCell ref="BL4:BP4"/>
-    <mergeCell ref="BQ4:BU4"/>
-    <mergeCell ref="BW4:CA4"/>
-    <mergeCell ref="CB4:CF4"/>
-    <mergeCell ref="CG4:CK4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
Account for ambient heat for water heating in RSD (new HPs)
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_RSD.xlsx
+++ b/SubRES_TMPL/SubRes_RSD.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31D8C5CE-366D-40AE-8F99-9C2422D783A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCFF2CD8-6F24-4D0D-A00A-C3DD5D1BE7CA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="9" xr2:uid="{34F9D92C-266F-476D-89E0-63153305AC39}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{34F9D92C-266F-476D-89E0-63153305AC39}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="34" r:id="rId1"/>
@@ -8866,7 +8866,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3617" uniqueCount="1120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3640" uniqueCount="1139">
   <si>
     <t>Document type:</t>
   </si>
@@ -12248,6 +12248,63 @@
   <si>
     <t>COM MAX</t>
   </si>
+  <si>
+    <t>~FI_COMM</t>
+  </si>
+  <si>
+    <t>Csets</t>
+  </si>
+  <si>
+    <t>CommName</t>
+  </si>
+  <si>
+    <t>CommDesc</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>LimType</t>
+  </si>
+  <si>
+    <t>CTSLvl</t>
+  </si>
+  <si>
+    <t>PeakTS</t>
+  </si>
+  <si>
+    <t>Ctype</t>
+  </si>
+  <si>
+    <t>* Set</t>
+  </si>
+  <si>
+    <t>Commodity Name</t>
+  </si>
+  <si>
+    <t>Commodity Description</t>
+  </si>
+  <si>
+    <t>Sense of the Balance EQ</t>
+  </si>
+  <si>
+    <t>Timeslice Level</t>
+  </si>
+  <si>
+    <t>Peak Monitoring</t>
+  </si>
+  <si>
+    <t>Electricity Indicator</t>
+  </si>
+  <si>
+    <t>RSDAHT2</t>
+  </si>
+  <si>
+    <t>Ambient Heat to Residential (2)</t>
+  </si>
+  <si>
+    <t>RSDAHT,RSDAHT2</t>
+  </si>
 </sst>
 </file>
 
@@ -12266,7 +12323,7 @@
     <numFmt numFmtId="172" formatCode="0.000"/>
     <numFmt numFmtId="173" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="72" x14ac:knownFonts="1">
+  <fonts count="74" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -12732,8 +12789,20 @@
       <sz val="8"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="38">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -12952,6 +13021,11 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
       </patternFill>
     </fill>
   </fills>
@@ -14034,7 +14108,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="18">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -14053,8 +14127,9 @@
     <xf numFmtId="9" fontId="55" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="72" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="609">
+  <cellXfs count="616">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -15183,6 +15258,15 @@
     <xf numFmtId="0" fontId="54" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="23" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -15190,15 +15274,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -15210,17 +15285,26 @@
     <xf numFmtId="0" fontId="17" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -15231,19 +15315,10 @@
     <xf numFmtId="0" fontId="70" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="61" fillId="31" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="61" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="61" fillId="31" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="61" fillId="31" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -15261,12 +15336,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -15282,9 +15351,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="72" fillId="38" borderId="0" xfId="18" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="72" fillId="38" borderId="0" xfId="18" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="72" fillId="38" borderId="0" xfId="18"/>
+    <xf numFmtId="166" fontId="73" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="73" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="18">
+  <cellStyles count="19">
     <cellStyle name="20% - Colore 2" xfId="11" xr:uid="{3E3DAF22-4D86-48A9-B6EE-8D230C1E993C}"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29"/>
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Comma 2" xfId="12" xr:uid="{0ABA8B51-FCCD-40DB-958F-AE78849A8FFE}"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -17293,8 +17380,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC422C74-4930-4E02-A6A2-617D513D886A}">
   <dimension ref="A1:AD121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="T38" sqref="T38"/>
+    <sheetView topLeftCell="B25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="T48" sqref="T48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -17304,23 +17391,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" s="604" t="s">
+      <c r="A1" s="602" t="s">
         <v>1062</v>
       </c>
-      <c r="B1" s="606" t="s">
+      <c r="B1" s="604" t="s">
         <v>1063</v>
       </c>
-      <c r="C1" s="607"/>
-      <c r="D1" s="607"/>
-      <c r="E1" s="607"/>
-      <c r="F1" s="608"/>
-      <c r="G1" s="606" t="s">
+      <c r="C1" s="605"/>
+      <c r="D1" s="605"/>
+      <c r="E1" s="605"/>
+      <c r="F1" s="606"/>
+      <c r="G1" s="604" t="s">
         <v>1064</v>
       </c>
-      <c r="H1" s="607"/>
-      <c r="I1" s="607"/>
-      <c r="J1" s="607"/>
-      <c r="K1" s="608"/>
+      <c r="H1" s="605"/>
+      <c r="I1" s="605"/>
+      <c r="J1" s="605"/>
+      <c r="K1" s="606"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
@@ -17330,7 +17417,7 @@
       <c r="R1" s="5"/>
     </row>
     <row r="2" spans="1:18" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="605"/>
+      <c r="A2" s="603"/>
       <c r="B2" s="527" t="s">
         <v>686</v>
       </c>
@@ -18823,11 +18910,11 @@
       <c r="Y48" t="s">
         <v>1113</v>
       </c>
-      <c r="Z48" s="602" t="s">
+      <c r="Z48" s="607" t="s">
         <v>1051</v>
       </c>
-      <c r="AA48" s="603"/>
-      <c r="AB48" s="603"/>
+      <c r="AA48" s="608"/>
+      <c r="AB48" s="608"/>
     </row>
     <row r="49" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
@@ -19044,11 +19131,11 @@
       <c r="Y53" t="s">
         <v>1115</v>
       </c>
-      <c r="Z53" s="602" t="s">
+      <c r="Z53" s="607" t="s">
         <v>1050</v>
       </c>
-      <c r="AA53" s="603"/>
-      <c r="AB53" s="603"/>
+      <c r="AA53" s="608"/>
+      <c r="AB53" s="608"/>
     </row>
     <row r="54" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A54" s="5" t="s">
@@ -19255,11 +19342,11 @@
       <c r="Y59" t="s">
         <v>1116</v>
       </c>
-      <c r="Z59" s="602" t="s">
+      <c r="Z59" s="607" t="s">
         <v>1117</v>
       </c>
-      <c r="AA59" s="603"/>
-      <c r="AB59" s="603"/>
+      <c r="AA59" s="608"/>
+      <c r="AB59" s="608"/>
     </row>
     <row r="60" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A60" s="547" t="str">
@@ -20157,17 +20244,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="Z59:AB59"/>
+    <mergeCell ref="Z53:AB53"/>
+    <mergeCell ref="Z48:AB48"/>
     <mergeCell ref="A28:D28"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="G1:K1"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="A18:D18"/>
-    <mergeCell ref="A40:D40"/>
-    <mergeCell ref="A45:D45"/>
-    <mergeCell ref="Z59:AB59"/>
-    <mergeCell ref="Z53:AB53"/>
-    <mergeCell ref="Z48:AB48"/>
   </mergeCells>
   <phoneticPr fontId="71" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -28687,10 +28774,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{104F8057-C735-4662-BAA6-EEDCF7B57273}">
-  <dimension ref="A2:AQ166"/>
+  <dimension ref="A2:AR166"/>
   <sheetViews>
-    <sheetView topLeftCell="A56" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="C106" sqref="C106"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -28876,12 +28963,12 @@
         <v>321</v>
       </c>
       <c r="U4" s="584"/>
-      <c r="V4" s="585" t="s">
+      <c r="V4" s="576" t="s">
         <v>322</v>
       </c>
-      <c r="W4" s="586"/>
-      <c r="X4" s="586"/>
-      <c r="Y4" s="587"/>
+      <c r="W4" s="577"/>
+      <c r="X4" s="577"/>
+      <c r="Y4" s="578"/>
       <c r="Z4" s="106"/>
       <c r="AA4" s="106"/>
       <c r="AB4" s="114" t="s">
@@ -28980,34 +29067,34 @@
       <c r="E6" s="84"/>
       <c r="F6" s="84"/>
       <c r="G6" s="85"/>
-      <c r="H6" s="576" t="s">
+      <c r="H6" s="579" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="577"/>
-      <c r="J6" s="577"/>
-      <c r="K6" s="578"/>
-      <c r="L6" s="577" t="s">
+      <c r="I6" s="580"/>
+      <c r="J6" s="580"/>
+      <c r="K6" s="581"/>
+      <c r="L6" s="580" t="s">
         <v>45</v>
       </c>
-      <c r="M6" s="577"/>
-      <c r="N6" s="577"/>
-      <c r="O6" s="578"/>
-      <c r="P6" s="576" t="s">
+      <c r="M6" s="580"/>
+      <c r="N6" s="580"/>
+      <c r="O6" s="581"/>
+      <c r="P6" s="579" t="s">
         <v>45</v>
       </c>
-      <c r="Q6" s="577"/>
-      <c r="R6" s="577"/>
-      <c r="S6" s="578"/>
-      <c r="T6" s="576" t="s">
+      <c r="Q6" s="580"/>
+      <c r="R6" s="580"/>
+      <c r="S6" s="581"/>
+      <c r="T6" s="579" t="s">
         <v>302</v>
       </c>
-      <c r="U6" s="578"/>
-      <c r="V6" s="576" t="s">
+      <c r="U6" s="581"/>
+      <c r="V6" s="579" t="s">
         <v>967</v>
       </c>
-      <c r="W6" s="577"/>
-      <c r="X6" s="577"/>
-      <c r="Y6" s="578"/>
+      <c r="W6" s="580"/>
+      <c r="X6" s="580"/>
+      <c r="Y6" s="581"/>
       <c r="Z6" s="107" t="s">
         <v>979</v>
       </c>
@@ -30398,7 +30485,7 @@
         <v>406</v>
       </c>
       <c r="F21" s="70" t="s">
-        <v>1033</v>
+        <v>1138</v>
       </c>
       <c r="G21" s="103" t="s">
         <v>713</v>
@@ -30779,7 +30866,7 @@
         <v>725</v>
       </c>
       <c r="F25" s="135" t="s">
-        <v>1033</v>
+        <v>1138</v>
       </c>
       <c r="G25" s="135" t="s">
         <v>713</v>
@@ -30892,7 +30979,7 @@
         <v>725</v>
       </c>
       <c r="F26" s="73" t="s">
-        <v>1033</v>
+        <v>1138</v>
       </c>
       <c r="G26" s="73" t="s">
         <v>713</v>
@@ -31061,7 +31148,7 @@
         <v>729</v>
       </c>
       <c r="F28" s="167" t="s">
-        <v>1033</v>
+        <v>1138</v>
       </c>
       <c r="G28" s="144" t="s">
         <v>713</v>
@@ -31448,7 +31535,7 @@
       <c r="AH32" s="80"/>
       <c r="AI32" s="80"/>
     </row>
-    <row r="33" spans="3:43" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:44" x14ac:dyDescent="0.2">
       <c r="C33" s="75" t="str">
         <f>"R-WH_Apt"&amp;"_"&amp;RIGHT(E33,3)&amp;"_N1"</f>
         <v>R-WH_Apt_ELC_N1</v>
@@ -31524,7 +31611,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="3:43" x14ac:dyDescent="0.2">
+    <row r="34" spans="3:44" x14ac:dyDescent="0.2">
       <c r="C34" s="69" t="str">
         <f>"R-WH_Apt"&amp;"_"&amp;RIGHT(E34,3)&amp;"_N1"</f>
         <v>R-WH_Apt_SOL_N1</v>
@@ -31602,7 +31689,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="3:43" x14ac:dyDescent="0.2">
+    <row r="35" spans="3:44" x14ac:dyDescent="0.2">
       <c r="C35" s="79" t="s">
         <v>740</v>
       </c>
@@ -31639,7 +31726,7 @@
       <c r="AH35" s="80"/>
       <c r="AI35" s="80"/>
     </row>
-    <row r="36" spans="3:43" x14ac:dyDescent="0.2">
+    <row r="36" spans="3:44" x14ac:dyDescent="0.2">
       <c r="C36" s="65" t="str">
         <f>"R-SC_Apt"&amp;"_"&amp;RIGHT(E36,3)&amp;"_N1"</f>
         <v>R-SC_Apt_ELC_N1</v>
@@ -31718,7 +31805,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="3:43" x14ac:dyDescent="0.2">
+    <row r="37" spans="3:44" ht="15" x14ac:dyDescent="0.25">
       <c r="C37" s="329" t="str">
         <f>"R-SC_Apt"&amp;"_"&amp;RIGHT(E37,3)&amp;"_N2"</f>
         <v>R-SC_Apt_ELC_N2</v>
@@ -31796,13 +31883,98 @@
       <c r="AI37" s="113">
         <v>5</v>
       </c>
-    </row>
-    <row r="40" spans="3:43" x14ac:dyDescent="0.2">
+      <c r="AK37" s="609" t="s">
+        <v>1120</v>
+      </c>
+      <c r="AL37" s="610"/>
+      <c r="AM37" s="610"/>
+      <c r="AN37" s="610"/>
+      <c r="AO37" s="610"/>
+      <c r="AP37" s="610"/>
+      <c r="AQ37" s="610"/>
+      <c r="AR37" s="611"/>
+    </row>
+    <row r="38" spans="3:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AK38" s="182" t="s">
+        <v>1121</v>
+      </c>
+      <c r="AL38" s="182" t="s">
+        <v>1122</v>
+      </c>
+      <c r="AM38" s="182" t="s">
+        <v>1123</v>
+      </c>
+      <c r="AN38" s="182" t="s">
+        <v>1124</v>
+      </c>
+      <c r="AO38" s="182" t="s">
+        <v>1125</v>
+      </c>
+      <c r="AP38" s="182" t="s">
+        <v>1126</v>
+      </c>
+      <c r="AQ38" s="182" t="s">
+        <v>1127</v>
+      </c>
+      <c r="AR38" s="182" t="s">
+        <v>1128</v>
+      </c>
+    </row>
+    <row r="39" spans="3:44" ht="48.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AK39" s="612" t="s">
+        <v>1129</v>
+      </c>
+      <c r="AL39" s="612" t="s">
+        <v>1130</v>
+      </c>
+      <c r="AM39" s="612" t="s">
+        <v>1131</v>
+      </c>
+      <c r="AN39" s="613" t="s">
+        <v>1124</v>
+      </c>
+      <c r="AO39" s="613" t="s">
+        <v>1132</v>
+      </c>
+      <c r="AP39" s="613" t="s">
+        <v>1133</v>
+      </c>
+      <c r="AQ39" s="613" t="s">
+        <v>1134</v>
+      </c>
+      <c r="AR39" s="613" t="s">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="40" spans="3:44" x14ac:dyDescent="0.2">
       <c r="H40" s="51" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="41" spans="3:43" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AK40" s="614" t="str">
+        <f>AI40&amp;"NRG"</f>
+        <v>NRG</v>
+      </c>
+      <c r="AL40" s="614" t="s">
+        <v>1136</v>
+      </c>
+      <c r="AM40" s="614" t="s">
+        <v>1137</v>
+      </c>
+      <c r="AN40" s="615" t="s">
+        <v>16</v>
+      </c>
+      <c r="AO40" s="614" t="s">
+        <v>914</v>
+      </c>
+      <c r="AP40" s="614"/>
+      <c r="AQ40" s="614" t="s">
+        <v>914</v>
+      </c>
+      <c r="AR40" s="614" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="41" spans="3:44" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C41" s="60" t="s">
         <v>28</v>
       </c>
@@ -31903,7 +32075,7 @@
         <v>1029</v>
       </c>
     </row>
-    <row r="42" spans="3:43" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="42" spans="3:44" ht="38.25" x14ac:dyDescent="0.2">
       <c r="C42" s="62" t="s">
         <v>315</v>
       </c>
@@ -31941,12 +32113,12 @@
         <v>321</v>
       </c>
       <c r="U42" s="584"/>
-      <c r="V42" s="585" t="s">
+      <c r="V42" s="576" t="s">
         <v>322</v>
       </c>
-      <c r="W42" s="586"/>
-      <c r="X42" s="586"/>
-      <c r="Y42" s="587"/>
+      <c r="W42" s="577"/>
+      <c r="X42" s="577"/>
+      <c r="Y42" s="578"/>
       <c r="Z42" s="106"/>
       <c r="AA42" s="106"/>
       <c r="AB42" s="114" t="s">
@@ -31979,7 +32151,7 @@
       <c r="AP42" s="57"/>
       <c r="AQ42" s="57"/>
     </row>
-    <row r="43" spans="3:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C43" s="60" t="s">
         <v>743</v>
       </c>
@@ -32037,7 +32209,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="44" spans="3:43" ht="33.75" x14ac:dyDescent="0.2">
+    <row r="44" spans="3:44" ht="33.75" x14ac:dyDescent="0.2">
       <c r="C44" s="83" t="s">
         <v>733</v>
       </c>
@@ -32045,34 +32217,34 @@
       <c r="E44" s="84"/>
       <c r="F44" s="84"/>
       <c r="G44" s="85"/>
-      <c r="H44" s="576" t="s">
+      <c r="H44" s="579" t="s">
         <v>45</v>
       </c>
-      <c r="I44" s="577"/>
-      <c r="J44" s="577"/>
-      <c r="K44" s="578"/>
-      <c r="L44" s="577" t="s">
+      <c r="I44" s="580"/>
+      <c r="J44" s="580"/>
+      <c r="K44" s="581"/>
+      <c r="L44" s="580" t="s">
         <v>45</v>
       </c>
-      <c r="M44" s="577"/>
-      <c r="N44" s="577"/>
-      <c r="O44" s="578"/>
-      <c r="P44" s="576" t="s">
+      <c r="M44" s="580"/>
+      <c r="N44" s="580"/>
+      <c r="O44" s="581"/>
+      <c r="P44" s="579" t="s">
         <v>45</v>
       </c>
-      <c r="Q44" s="577"/>
-      <c r="R44" s="577"/>
-      <c r="S44" s="578"/>
-      <c r="T44" s="579" t="s">
+      <c r="Q44" s="580"/>
+      <c r="R44" s="580"/>
+      <c r="S44" s="581"/>
+      <c r="T44" s="585" t="s">
         <v>302</v>
       </c>
-      <c r="U44" s="580"/>
-      <c r="V44" s="579" t="s">
+      <c r="U44" s="586"/>
+      <c r="V44" s="585" t="s">
         <v>967</v>
       </c>
-      <c r="W44" s="581"/>
-      <c r="X44" s="581"/>
-      <c r="Y44" s="580"/>
+      <c r="W44" s="587"/>
+      <c r="X44" s="587"/>
+      <c r="Y44" s="586"/>
       <c r="Z44" s="450" t="s">
         <v>979</v>
       </c>
@@ -32123,7 +32295,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="45" spans="3:43" ht="15" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:44" ht="15" x14ac:dyDescent="0.25">
       <c r="C45" s="65" t="str">
         <f>"R-SH_Att"&amp;"_"&amp;RIGHT(E45,3)&amp;"_N1"</f>
         <v>R-SH_Att_KER_N1</v>
@@ -32219,7 +32391,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="46" spans="3:43" ht="15" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:44" ht="15" x14ac:dyDescent="0.25">
       <c r="C46" s="68" t="str">
         <f>"R-SW_Att"&amp;"_"&amp;RIGHT(E46,3)&amp;"_N1"</f>
         <v>R-SW_Att_KER_N1</v>
@@ -32325,7 +32497,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="47" spans="3:43" ht="15" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:44" ht="15" x14ac:dyDescent="0.25">
       <c r="C47" s="86" t="str">
         <f>"R-SW_Att"&amp;"_"&amp;RIGHT(E47,3)&amp;"_N2"</f>
         <v>R-SW_Att_KER_N2</v>
@@ -32436,7 +32608,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="48" spans="3:43" ht="15" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:44" ht="15" x14ac:dyDescent="0.25">
       <c r="C48" s="68" t="str">
         <f>"R-SW_Att"&amp;"_"&amp;RIGHT(E48,3)&amp;"_N3"</f>
         <v>R-SW_Att_KER_N3</v>
@@ -34300,7 +34472,7 @@
         <v>406</v>
       </c>
       <c r="F67" s="70" t="s">
-        <v>1033</v>
+        <v>1138</v>
       </c>
       <c r="G67" s="103" t="s">
         <v>715</v>
@@ -34411,7 +34583,7 @@
         <v>1023</v>
       </c>
       <c r="F68" s="76" t="s">
-        <v>1033</v>
+        <v>1138</v>
       </c>
       <c r="G68" s="104" t="s">
         <v>715</v>
@@ -34794,7 +34966,7 @@
         <v>725</v>
       </c>
       <c r="F72" s="135" t="s">
-        <v>1033</v>
+        <v>1138</v>
       </c>
       <c r="G72" s="135" t="s">
         <v>715</v>
@@ -34907,7 +35079,7 @@
         <v>725</v>
       </c>
       <c r="F73" s="73" t="s">
-        <v>1033</v>
+        <v>1138</v>
       </c>
       <c r="G73" s="73" t="s">
         <v>715</v>
@@ -35076,7 +35248,7 @@
         <v>729</v>
       </c>
       <c r="F75" s="167" t="s">
-        <v>1033</v>
+        <v>1138</v>
       </c>
       <c r="G75" s="144" t="s">
         <v>715</v>
@@ -35863,12 +36035,12 @@
         <v>321</v>
       </c>
       <c r="U90" s="584"/>
-      <c r="V90" s="585" t="s">
+      <c r="V90" s="576" t="s">
         <v>322</v>
       </c>
-      <c r="W90" s="586"/>
-      <c r="X90" s="586"/>
-      <c r="Y90" s="587"/>
+      <c r="W90" s="577"/>
+      <c r="X90" s="577"/>
+      <c r="Y90" s="578"/>
       <c r="Z90" s="106"/>
       <c r="AA90" s="106"/>
       <c r="AB90" s="114" t="s">
@@ -35967,34 +36139,34 @@
       <c r="E92" s="84"/>
       <c r="F92" s="84"/>
       <c r="G92" s="85"/>
-      <c r="H92" s="576" t="s">
+      <c r="H92" s="579" t="s">
         <v>45</v>
       </c>
-      <c r="I92" s="577"/>
-      <c r="J92" s="577"/>
-      <c r="K92" s="578"/>
-      <c r="L92" s="577" t="s">
+      <c r="I92" s="580"/>
+      <c r="J92" s="580"/>
+      <c r="K92" s="581"/>
+      <c r="L92" s="580" t="s">
         <v>45</v>
       </c>
-      <c r="M92" s="577"/>
-      <c r="N92" s="577"/>
-      <c r="O92" s="578"/>
-      <c r="P92" s="576" t="s">
+      <c r="M92" s="580"/>
+      <c r="N92" s="580"/>
+      <c r="O92" s="581"/>
+      <c r="P92" s="579" t="s">
         <v>45</v>
       </c>
-      <c r="Q92" s="577"/>
-      <c r="R92" s="577"/>
-      <c r="S92" s="578"/>
-      <c r="T92" s="579" t="s">
+      <c r="Q92" s="580"/>
+      <c r="R92" s="580"/>
+      <c r="S92" s="581"/>
+      <c r="T92" s="585" t="s">
         <v>302</v>
       </c>
-      <c r="U92" s="580"/>
-      <c r="V92" s="579" t="s">
+      <c r="U92" s="586"/>
+      <c r="V92" s="585" t="s">
         <v>967</v>
       </c>
-      <c r="W92" s="581"/>
-      <c r="X92" s="581"/>
-      <c r="Y92" s="580"/>
+      <c r="W92" s="587"/>
+      <c r="X92" s="587"/>
+      <c r="Y92" s="586"/>
       <c r="Z92" s="450" t="s">
         <v>979</v>
       </c>
@@ -38210,7 +38382,7 @@
         <v>406</v>
       </c>
       <c r="F115" s="70" t="s">
-        <v>1033</v>
+        <v>1138</v>
       </c>
       <c r="G115" s="103" t="s">
         <v>717</v>
@@ -38318,7 +38490,7 @@
         <v>1023</v>
       </c>
       <c r="F116" s="76" t="s">
-        <v>1033</v>
+        <v>1138</v>
       </c>
       <c r="G116" s="104" t="s">
         <v>717</v>
@@ -38689,7 +38861,7 @@
         <v>725</v>
       </c>
       <c r="F120" s="135" t="s">
-        <v>1033</v>
+        <v>1138</v>
       </c>
       <c r="G120" s="135" t="s">
         <v>717</v>
@@ -38802,7 +38974,7 @@
         <v>725</v>
       </c>
       <c r="F121" s="73" t="s">
-        <v>1033</v>
+        <v>1138</v>
       </c>
       <c r="G121" s="73" t="s">
         <v>717</v>
@@ -38971,7 +39143,7 @@
         <v>729</v>
       </c>
       <c r="F123" s="167" t="s">
-        <v>1033</v>
+        <v>1138</v>
       </c>
       <c r="G123" s="144" t="s">
         <v>717</v>
@@ -39925,6 +40097,26 @@
     <row r="166" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="H92:K92"/>
+    <mergeCell ref="L92:O92"/>
+    <mergeCell ref="P92:S92"/>
+    <mergeCell ref="T92:U92"/>
+    <mergeCell ref="V92:Y92"/>
+    <mergeCell ref="H90:K90"/>
+    <mergeCell ref="L90:O90"/>
+    <mergeCell ref="P90:S90"/>
+    <mergeCell ref="T90:U90"/>
+    <mergeCell ref="V90:Y90"/>
+    <mergeCell ref="H44:K44"/>
+    <mergeCell ref="L44:O44"/>
+    <mergeCell ref="P44:S44"/>
+    <mergeCell ref="T44:U44"/>
+    <mergeCell ref="V44:Y44"/>
+    <mergeCell ref="H42:K42"/>
+    <mergeCell ref="L42:O42"/>
+    <mergeCell ref="P42:S42"/>
+    <mergeCell ref="T42:U42"/>
+    <mergeCell ref="V42:Y42"/>
     <mergeCell ref="V4:Y4"/>
     <mergeCell ref="V6:Y6"/>
     <mergeCell ref="H4:K4"/>
@@ -39935,26 +40127,6 @@
     <mergeCell ref="P6:S6"/>
     <mergeCell ref="L6:O6"/>
     <mergeCell ref="H6:K6"/>
-    <mergeCell ref="H42:K42"/>
-    <mergeCell ref="L42:O42"/>
-    <mergeCell ref="P42:S42"/>
-    <mergeCell ref="T42:U42"/>
-    <mergeCell ref="V42:Y42"/>
-    <mergeCell ref="H44:K44"/>
-    <mergeCell ref="L44:O44"/>
-    <mergeCell ref="P44:S44"/>
-    <mergeCell ref="T44:U44"/>
-    <mergeCell ref="V44:Y44"/>
-    <mergeCell ref="H90:K90"/>
-    <mergeCell ref="L90:O90"/>
-    <mergeCell ref="P90:S90"/>
-    <mergeCell ref="T90:U90"/>
-    <mergeCell ref="V90:Y90"/>
-    <mergeCell ref="H92:K92"/>
-    <mergeCell ref="L92:O92"/>
-    <mergeCell ref="P92:S92"/>
-    <mergeCell ref="T92:U92"/>
-    <mergeCell ref="V92:Y92"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>
@@ -40099,12 +40271,12 @@
       <c r="I5" s="173"/>
       <c r="J5" s="173"/>
       <c r="K5" s="173"/>
-      <c r="L5" s="585" t="s">
+      <c r="L5" s="576" t="s">
         <v>322</v>
       </c>
-      <c r="M5" s="586"/>
-      <c r="N5" s="586"/>
-      <c r="O5" s="587"/>
+      <c r="M5" s="577"/>
+      <c r="N5" s="577"/>
+      <c r="O5" s="578"/>
       <c r="P5" s="106"/>
       <c r="Q5" s="106" t="s">
         <v>323</v>
@@ -40135,12 +40307,12 @@
       <c r="I6" s="83"/>
       <c r="J6" s="83"/>
       <c r="K6" s="83"/>
-      <c r="L6" s="579" t="s">
+      <c r="L6" s="585" t="s">
         <v>967</v>
       </c>
-      <c r="M6" s="581"/>
-      <c r="N6" s="581"/>
-      <c r="O6" s="580"/>
+      <c r="M6" s="587"/>
+      <c r="N6" s="587"/>
+      <c r="O6" s="586"/>
       <c r="P6" s="450" t="s">
         <v>979</v>
       </c>
@@ -41058,23 +41230,23 @@
       <c r="K33" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="L33" s="585" t="s">
+      <c r="L33" s="576" t="s">
         <v>322</v>
       </c>
-      <c r="M33" s="586"/>
-      <c r="N33" s="586"/>
-      <c r="O33" s="587"/>
+      <c r="M33" s="577"/>
+      <c r="N33" s="577"/>
+      <c r="O33" s="578"/>
     </row>
     <row r="34" spans="8:15" x14ac:dyDescent="0.2">
       <c r="H34" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="L34" s="579" t="s">
+      <c r="L34" s="585" t="s">
         <v>327</v>
       </c>
-      <c r="M34" s="581"/>
-      <c r="N34" s="581"/>
-      <c r="O34" s="580"/>
+      <c r="M34" s="587"/>
+      <c r="N34" s="587"/>
+      <c r="O34" s="586"/>
     </row>
     <row r="35" spans="8:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H35" s="5" t="s">
@@ -41421,11 +41593,11 @@
       </c>
       <c r="I4" s="583"/>
       <c r="J4" s="584"/>
-      <c r="K4" s="585" t="s">
+      <c r="K4" s="576" t="s">
         <v>322</v>
       </c>
-      <c r="L4" s="586"/>
-      <c r="M4" s="587"/>
+      <c r="L4" s="577"/>
+      <c r="M4" s="578"/>
       <c r="N4" s="106"/>
       <c r="O4" s="106" t="s">
         <v>323</v>
@@ -41451,16 +41623,16 @@
       <c r="G5" s="458" t="s">
         <v>302</v>
       </c>
-      <c r="H5" s="592" t="s">
+      <c r="H5" s="589" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="593"/>
-      <c r="J5" s="594"/>
-      <c r="K5" s="592" t="s">
+      <c r="I5" s="590"/>
+      <c r="J5" s="591"/>
+      <c r="K5" s="589" t="s">
         <v>756</v>
       </c>
-      <c r="L5" s="593"/>
-      <c r="M5" s="594"/>
+      <c r="L5" s="590"/>
+      <c r="M5" s="591"/>
       <c r="N5" s="459" t="s">
         <v>328</v>
       </c>
@@ -41477,23 +41649,23 @@
         <v>626</v>
       </c>
       <c r="AA5" s="281"/>
-      <c r="AB5" s="589" t="s">
+      <c r="AB5" s="592" t="s">
         <v>1011</v>
       </c>
-      <c r="AC5" s="589"/>
+      <c r="AC5" s="592"/>
       <c r="AD5" s="461"/>
-      <c r="AE5" s="590" t="s">
+      <c r="AE5" s="593" t="s">
         <v>110</v>
       </c>
-      <c r="AF5" s="590"/>
-      <c r="AG5" s="590" t="s">
+      <c r="AF5" s="593"/>
+      <c r="AG5" s="593" t="s">
         <v>1012</v>
       </c>
-      <c r="AH5" s="590"/>
-      <c r="AI5" s="591" t="s">
+      <c r="AH5" s="593"/>
+      <c r="AI5" s="594" t="s">
         <v>1013</v>
       </c>
-      <c r="AJ5" s="591"/>
+      <c r="AJ5" s="594"/>
     </row>
     <row r="6" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C6" s="505" t="str">
@@ -42231,12 +42403,12 @@
       <c r="K27" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="L27" s="585" t="s">
+      <c r="L27" s="576" t="s">
         <v>322</v>
       </c>
-      <c r="M27" s="586"/>
-      <c r="N27" s="586"/>
-      <c r="O27" s="587"/>
+      <c r="M27" s="577"/>
+      <c r="N27" s="577"/>
+      <c r="O27" s="578"/>
       <c r="T27" s="283"/>
       <c r="U27" s="283"/>
     </row>
@@ -42244,12 +42416,12 @@
       <c r="J28" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="L28" s="576" t="s">
+      <c r="L28" s="579" t="s">
         <v>327</v>
       </c>
-      <c r="M28" s="577"/>
-      <c r="N28" s="577"/>
-      <c r="O28" s="578"/>
+      <c r="M28" s="580"/>
+      <c r="N28" s="580"/>
+      <c r="O28" s="581"/>
       <c r="T28" s="283"/>
       <c r="U28" s="283"/>
     </row>
@@ -43639,16 +43811,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="AB5:AC5"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AG5:AH5"/>
+    <mergeCell ref="AI5:AJ5"/>
+    <mergeCell ref="L27:O27"/>
     <mergeCell ref="L28:O28"/>
     <mergeCell ref="H4:J4"/>
     <mergeCell ref="K4:M4"/>
     <mergeCell ref="H5:J5"/>
     <mergeCell ref="K5:M5"/>
-    <mergeCell ref="AB5:AC5"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="AG5:AH5"/>
-    <mergeCell ref="AI5:AJ5"/>
-    <mergeCell ref="L27:O27"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="S7" r:id="rId1" xr:uid="{B1EDD63D-40A5-4174-9D28-8666BD314B83}"/>
@@ -52678,103 +52850,103 @@
       <c r="C4" s="356" t="s">
         <v>765</v>
       </c>
-      <c r="D4" s="596" t="s">
+      <c r="D4" s="595" t="s">
         <v>766</v>
       </c>
-      <c r="E4" s="595"/>
-      <c r="F4" s="595"/>
-      <c r="G4" s="595"/>
+      <c r="E4" s="596"/>
+      <c r="F4" s="596"/>
+      <c r="G4" s="596"/>
       <c r="H4" s="597"/>
-      <c r="I4" s="595" t="s">
+      <c r="I4" s="596" t="s">
         <v>767</v>
       </c>
-      <c r="J4" s="595"/>
-      <c r="K4" s="595"/>
-      <c r="L4" s="595"/>
+      <c r="J4" s="596"/>
+      <c r="K4" s="596"/>
+      <c r="L4" s="596"/>
       <c r="M4" s="597"/>
-      <c r="N4" s="595" t="s">
+      <c r="N4" s="596" t="s">
         <v>768</v>
       </c>
-      <c r="O4" s="595"/>
-      <c r="P4" s="595"/>
-      <c r="Q4" s="595"/>
+      <c r="O4" s="596"/>
+      <c r="P4" s="596"/>
+      <c r="Q4" s="596"/>
       <c r="R4" s="597"/>
-      <c r="S4" s="595" t="s">
+      <c r="S4" s="596" t="s">
         <v>769</v>
       </c>
-      <c r="T4" s="595"/>
-      <c r="U4" s="595"/>
-      <c r="V4" s="595"/>
+      <c r="T4" s="596"/>
+      <c r="U4" s="596"/>
+      <c r="V4" s="596"/>
       <c r="W4" s="597"/>
-      <c r="X4" s="595" t="s">
+      <c r="X4" s="596" t="s">
         <v>770</v>
       </c>
-      <c r="Y4" s="595"/>
-      <c r="Z4" s="595"/>
-      <c r="AA4" s="595"/>
+      <c r="Y4" s="596"/>
+      <c r="Z4" s="596"/>
+      <c r="AA4" s="596"/>
       <c r="AB4" s="597"/>
-      <c r="AC4" s="595" t="s">
+      <c r="AC4" s="596" t="s">
         <v>771</v>
       </c>
-      <c r="AD4" s="595"/>
-      <c r="AE4" s="595"/>
-      <c r="AF4" s="595"/>
+      <c r="AD4" s="596"/>
+      <c r="AE4" s="596"/>
+      <c r="AF4" s="596"/>
       <c r="AG4" s="597"/>
-      <c r="AH4" s="595" t="s">
+      <c r="AH4" s="596" t="s">
         <v>772</v>
       </c>
-      <c r="AI4" s="595"/>
-      <c r="AJ4" s="595"/>
-      <c r="AK4" s="595"/>
+      <c r="AI4" s="596"/>
+      <c r="AJ4" s="596"/>
+      <c r="AK4" s="596"/>
       <c r="AL4" s="597"/>
-      <c r="AM4" s="595" t="s">
+      <c r="AM4" s="596" t="s">
         <v>773</v>
       </c>
-      <c r="AN4" s="595"/>
-      <c r="AO4" s="595"/>
-      <c r="AP4" s="595"/>
+      <c r="AN4" s="596"/>
+      <c r="AO4" s="596"/>
+      <c r="AP4" s="596"/>
       <c r="AQ4" s="597"/>
-      <c r="AR4" s="595" t="s">
+      <c r="AR4" s="596" t="s">
         <v>774</v>
       </c>
-      <c r="AS4" s="595"/>
-      <c r="AT4" s="595"/>
-      <c r="AU4" s="595"/>
+      <c r="AS4" s="596"/>
+      <c r="AT4" s="596"/>
+      <c r="AU4" s="596"/>
       <c r="AV4" s="597"/>
-      <c r="AW4" s="595" t="s">
+      <c r="AW4" s="596" t="s">
         <v>775</v>
       </c>
-      <c r="AX4" s="595"/>
-      <c r="AY4" s="595"/>
-      <c r="AZ4" s="595"/>
-      <c r="BA4" s="595"/>
-      <c r="BB4" s="596" t="s">
+      <c r="AX4" s="596"/>
+      <c r="AY4" s="596"/>
+      <c r="AZ4" s="596"/>
+      <c r="BA4" s="596"/>
+      <c r="BB4" s="595" t="s">
         <v>776</v>
       </c>
-      <c r="BC4" s="595"/>
-      <c r="BD4" s="595"/>
-      <c r="BE4" s="595"/>
+      <c r="BC4" s="596"/>
+      <c r="BD4" s="596"/>
+      <c r="BE4" s="596"/>
       <c r="BF4" s="597"/>
-      <c r="BG4" s="595" t="s">
+      <c r="BG4" s="596" t="s">
         <v>777</v>
       </c>
-      <c r="BH4" s="595"/>
-      <c r="BI4" s="595"/>
-      <c r="BJ4" s="595"/>
-      <c r="BK4" s="595"/>
-      <c r="BL4" s="596" t="s">
+      <c r="BH4" s="596"/>
+      <c r="BI4" s="596"/>
+      <c r="BJ4" s="596"/>
+      <c r="BK4" s="596"/>
+      <c r="BL4" s="595" t="s">
         <v>778</v>
       </c>
-      <c r="BM4" s="595"/>
-      <c r="BN4" s="595"/>
-      <c r="BO4" s="595"/>
-      <c r="BP4" s="595"/>
-      <c r="BQ4" s="596" t="s">
+      <c r="BM4" s="596"/>
+      <c r="BN4" s="596"/>
+      <c r="BO4" s="596"/>
+      <c r="BP4" s="596"/>
+      <c r="BQ4" s="595" t="s">
         <v>779</v>
       </c>
-      <c r="BR4" s="595"/>
-      <c r="BS4" s="595"/>
-      <c r="BT4" s="595"/>
+      <c r="BR4" s="596"/>
+      <c r="BS4" s="596"/>
+      <c r="BT4" s="596"/>
       <c r="BU4" s="597"/>
       <c r="BV4" s="357" t="s">
         <v>780</v>
@@ -66368,11 +66540,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="BL4:BP4"/>
-    <mergeCell ref="BQ4:BU4"/>
-    <mergeCell ref="BW4:CA4"/>
-    <mergeCell ref="CB4:CF4"/>
-    <mergeCell ref="CG4:CK4"/>
     <mergeCell ref="BG4:BK4"/>
     <mergeCell ref="D4:H4"/>
     <mergeCell ref="I4:M4"/>
@@ -66385,6 +66552,11 @@
     <mergeCell ref="AR4:AV4"/>
     <mergeCell ref="AW4:BA4"/>
     <mergeCell ref="BB4:BF4"/>
+    <mergeCell ref="BL4:BP4"/>
+    <mergeCell ref="BQ4:BU4"/>
+    <mergeCell ref="BW4:CA4"/>
+    <mergeCell ref="CB4:CF4"/>
+    <mergeCell ref="CG4:CK4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>